<commit_message>
Boat Enabled - India TV
Boat Enabled - India TV

BoardRw_Wbt :- 1
</commit_message>
<xml_diff>
--- a/System_2.1.5.xlsx
+++ b/System_2.1.5.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Work\Work_For_\Work\Running AppS\System_Work_RW\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1CAD6A1-14FF-4215-A114-764E51A23A06}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DDDD0170-174B-4852-83CE-C36478C627D2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="BoardRW" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1071" uniqueCount="609">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1074" uniqueCount="610">
   <si>
     <t>Zone</t>
   </si>
@@ -1866,6 +1866,9 @@
   </si>
   <si>
     <t>No NICURD</t>
+  </si>
+  <si>
+    <t>X-Trophy-X</t>
   </si>
 </sst>
 </file>
@@ -3446,7 +3449,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="738">
+  <cellXfs count="737">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
@@ -4633,7 +4636,6 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -4754,6 +4756,9 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="54" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -4802,6 +4807,36 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="255" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="39" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="39" fillId="6" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="18" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="18" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="18" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255"/>
+    </xf>
     <xf numFmtId="0" fontId="32" fillId="27" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -4859,34 +4894,139 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="39" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="39" fillId="6" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="18" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="19" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="19" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="3" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="19" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="19" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="38" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="38" fillId="7" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="255"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="18" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="255"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="18" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="33" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="33" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="33" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="52" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="54" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="16" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="16" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="3" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="18" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="18" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="18" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="49" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="49" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="49" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="255"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
@@ -4961,140 +5101,62 @@
     <xf numFmtId="0" fontId="3" fillId="11" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="3" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="18" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="18" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="18" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="49" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="49" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="49" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="52" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="54" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="16" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="16" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="19" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="19" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="3" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="19" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="19" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="38" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="38" fillId="7" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="33" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="33" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="33" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="3" fillId="43" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="43" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="43" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="18" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="18" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="18" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="40" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="40" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="40" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="7" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="32" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="32" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="52" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="52" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="35" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="255" wrapText="1"/>
@@ -5105,63 +5167,6 @@
     <xf numFmtId="0" fontId="3" fillId="35" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="255" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="43" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="43" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="43" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="18" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="18" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="18" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="40" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="40" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="40" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="7" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="32" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="32" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="52" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="52" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -5180,46 +5185,25 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="30" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="30" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="30" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="24" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="24" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="24" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="18" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -5297,29 +5281,47 @@
     <xf numFmtId="0" fontId="3" fillId="21" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="30" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="30" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="30" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="24" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="24" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="24" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -5613,7 +5615,7 @@
   <dimension ref="B1:W28"/>
   <sheetViews>
     <sheetView topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="U18" sqref="U18"/>
+      <selection activeCell="Q24" sqref="Q24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5645,7 +5647,7 @@
       <c r="B2" s="1" t="s">
         <v>375</v>
       </c>
-      <c r="C2" s="509" t="s">
+      <c r="C2" s="508" t="s">
         <v>0</v>
       </c>
       <c r="D2" s="409" t="s">
@@ -5797,7 +5799,7 @@
       <c r="N5" s="377" t="s">
         <v>522</v>
       </c>
-      <c r="P5" s="506"/>
+      <c r="P5" s="505"/>
       <c r="T5" s="563"/>
       <c r="U5" s="209" t="s">
         <v>228</v>
@@ -5834,7 +5836,7 @@
       <c r="N6" s="381" t="s">
         <v>522</v>
       </c>
-      <c r="P6" s="506"/>
+      <c r="P6" s="505"/>
       <c r="Q6" s="16"/>
       <c r="R6" s="6"/>
       <c r="T6" s="563"/>
@@ -5865,7 +5867,7 @@
       <c r="N7" s="61" t="s">
         <v>18</v>
       </c>
-      <c r="P7" s="506"/>
+      <c r="P7" s="505"/>
       <c r="Q7" s="16"/>
       <c r="R7" s="6"/>
       <c r="T7" s="563"/>
@@ -5894,7 +5896,7 @@
       <c r="N8" s="61" t="s">
         <v>18</v>
       </c>
-      <c r="P8" s="506"/>
+      <c r="P8" s="505"/>
       <c r="Q8" s="16"/>
       <c r="R8" s="6"/>
       <c r="T8" s="563"/>
@@ -5927,10 +5929,10 @@
         <v>45275</v>
       </c>
       <c r="N9" s="349"/>
-      <c r="O9" s="504" t="s">
+      <c r="O9" s="503" t="s">
         <v>44</v>
       </c>
-      <c r="P9" s="506"/>
+      <c r="P9" s="505"/>
       <c r="T9" s="563"/>
     </row>
     <row r="10" spans="2:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -5960,7 +5962,7 @@
       <c r="N10" s="377" t="s">
         <v>522</v>
       </c>
-      <c r="P10" s="506"/>
+      <c r="P10" s="505"/>
       <c r="T10" s="563"/>
     </row>
     <row r="11" spans="2:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -5993,7 +5995,7 @@
       <c r="N11" s="373" t="s">
         <v>18</v>
       </c>
-      <c r="P11" s="506"/>
+      <c r="P11" s="505"/>
       <c r="Q11" s="16"/>
       <c r="R11" s="142"/>
       <c r="T11" s="563"/>
@@ -6026,7 +6028,7 @@
       <c r="N12" s="374" t="s">
         <v>26</v>
       </c>
-      <c r="P12" s="506"/>
+      <c r="P12" s="505"/>
       <c r="Q12" s="16"/>
       <c r="R12" s="142"/>
       <c r="T12" s="563"/>
@@ -6063,18 +6065,18 @@
       <c r="N13" s="378" t="s">
         <v>522</v>
       </c>
-      <c r="P13" s="506"/>
+      <c r="P13" s="505"/>
       <c r="T13" s="563"/>
     </row>
     <row r="14" spans="2:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="P14" s="506"/>
+      <c r="P14" s="505"/>
       <c r="T14" s="563"/>
     </row>
     <row r="15" spans="2:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B15" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="C15" s="510" t="s">
+      <c r="C15" s="509" t="s">
         <v>20</v>
       </c>
       <c r="D15" s="61"/>
@@ -6100,10 +6102,10 @@
       <c r="N15" s="554" t="s">
         <v>22</v>
       </c>
-      <c r="O15" s="504" t="s">
+      <c r="O15" s="503" t="s">
         <v>44</v>
       </c>
-      <c r="P15" s="506"/>
+      <c r="P15" s="505"/>
       <c r="S15" s="6"/>
       <c r="T15" s="563"/>
     </row>
@@ -6111,7 +6113,7 @@
       <c r="B16" s="487" t="s">
         <v>377</v>
       </c>
-      <c r="C16" s="511" t="s">
+      <c r="C16" s="510" t="s">
         <v>11</v>
       </c>
       <c r="D16" s="384"/>
@@ -6133,14 +6135,14 @@
       </c>
       <c r="M16" s="552"/>
       <c r="N16" s="555"/>
-      <c r="P16" s="506"/>
+      <c r="P16" s="505"/>
       <c r="T16" s="563"/>
     </row>
     <row r="17" spans="2:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B17" s="2" t="s">
         <v>224</v>
       </c>
-      <c r="C17" s="510" t="s">
+      <c r="C17" s="509" t="s">
         <v>23</v>
       </c>
       <c r="D17" s="61"/>
@@ -6164,7 +6166,7 @@
       </c>
       <c r="M17" s="553"/>
       <c r="N17" s="556"/>
-      <c r="O17" s="504" t="s">
+      <c r="O17" s="503" t="s">
         <v>44</v>
       </c>
       <c r="P17" s="321">
@@ -6182,7 +6184,7 @@
       <c r="T17" s="563"/>
     </row>
     <row r="18" spans="2:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="P18" s="506"/>
+      <c r="P18" s="505"/>
       <c r="T18" s="563"/>
     </row>
     <row r="19" spans="2:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -6217,7 +6219,7 @@
       <c r="N19" s="415" t="s">
         <v>522</v>
       </c>
-      <c r="P19" s="506"/>
+      <c r="P19" s="505"/>
       <c r="T19" s="563"/>
     </row>
     <row r="20" spans="2:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -6248,7 +6250,7 @@
       <c r="N20" s="404" t="s">
         <v>26</v>
       </c>
-      <c r="P20" s="506"/>
+      <c r="P20" s="505"/>
       <c r="T20" s="563"/>
     </row>
     <row r="21" spans="2:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -6279,7 +6281,7 @@
       <c r="N21" s="404" t="s">
         <v>18</v>
       </c>
-      <c r="P21" s="506"/>
+      <c r="P21" s="505"/>
       <c r="T21" s="563"/>
       <c r="U21" s="549" t="s">
         <v>226</v>
@@ -6314,7 +6316,7 @@
       <c r="N22" s="384" t="s">
         <v>26</v>
       </c>
-      <c r="P22" s="506"/>
+      <c r="P22" s="505"/>
       <c r="T22" s="563"/>
     </row>
     <row r="23" spans="2:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -6345,7 +6347,7 @@
       <c r="N23" s="61" t="s">
         <v>523</v>
       </c>
-      <c r="P23" s="506"/>
+      <c r="P23" s="505"/>
       <c r="T23" s="563"/>
     </row>
     <row r="24" spans="2:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -6376,10 +6378,10 @@
       <c r="N24" s="61" t="s">
         <v>26</v>
       </c>
-      <c r="O24" s="505" t="s">
+      <c r="O24" s="504" t="s">
         <v>44</v>
       </c>
-      <c r="P24" s="507"/>
+      <c r="P24" s="506"/>
       <c r="S24" s="16"/>
       <c r="T24" s="563"/>
     </row>
@@ -6413,7 +6415,7 @@
       <c r="N25" s="61" t="s">
         <v>26</v>
       </c>
-      <c r="P25" s="506">
+      <c r="P25" s="505">
         <v>1</v>
       </c>
       <c r="Q25" s="2" t="s">
@@ -6458,7 +6460,7 @@
       <c r="N26" s="61" t="s">
         <v>524</v>
       </c>
-      <c r="P26" s="506"/>
+      <c r="P26" s="505"/>
       <c r="T26" s="563"/>
       <c r="W26" s="2" t="s">
         <v>607</v>
@@ -6507,7 +6509,7 @@
       <c r="B28" s="261" t="s">
         <v>406</v>
       </c>
-      <c r="C28" s="503" t="s">
+      <c r="C28" s="502" t="s">
         <v>16</v>
       </c>
       <c r="D28" s="61" t="s">
@@ -6533,7 +6535,7 @@
       <c r="N28" s="61" t="s">
         <v>524</v>
       </c>
-      <c r="P28" s="508">
+      <c r="P28" s="507">
         <v>1</v>
       </c>
       <c r="Q28" s="2" t="s">
@@ -6566,8 +6568,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AB54FD83-008D-4F8B-87AC-83E7F70047CB}">
   <dimension ref="A1:AA32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
-      <selection activeCell="Z13" sqref="Z13"/>
+    <sheetView topLeftCell="H1" workbookViewId="0">
+      <selection activeCell="V3" sqref="V3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6624,7 +6626,7 @@
       <c r="P1" s="423" t="s">
         <v>408</v>
       </c>
-      <c r="Q1" s="584" t="s">
+      <c r="Q1" s="565" t="s">
         <v>181</v>
       </c>
       <c r="R1" s="100" t="s">
@@ -6644,32 +6646,32 @@
       </c>
     </row>
     <row r="2" spans="1:27" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="568">
+      <c r="A2" s="578">
         <f ca="1">TODAY()</f>
         <v>45279</v>
       </c>
-      <c r="B2" s="570" t="s">
+      <c r="B2" s="580" t="s">
         <v>389</v>
       </c>
-      <c r="C2" s="582" t="s">
+      <c r="C2" s="592" t="s">
         <v>365</v>
       </c>
-      <c r="D2" s="572" t="s">
+      <c r="D2" s="582" t="s">
         <v>103</v>
       </c>
-      <c r="E2" s="574" t="s">
+      <c r="E2" s="584" t="s">
         <v>65</v>
       </c>
       <c r="F2" s="196" t="s">
         <v>220</v>
       </c>
-      <c r="G2" s="580" t="s">
+      <c r="G2" s="590" t="s">
         <v>381</v>
       </c>
       <c r="H2" s="211" t="s">
         <v>220</v>
       </c>
-      <c r="I2" s="591" t="s">
+      <c r="I2" s="572" t="s">
         <v>103</v>
       </c>
       <c r="J2" s="421" t="s">
@@ -6693,18 +6695,18 @@
       <c r="P2" s="424">
         <v>40</v>
       </c>
-      <c r="Q2" s="585"/>
+      <c r="Q2" s="566"/>
       <c r="R2" s="21">
         <f>R7+R18</f>
         <v>6</v>
       </c>
       <c r="S2" s="21">
         <f>S7+S18</f>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="T2" s="176">
         <f>SUM(T4:T16)</f>
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="U2" s="6"/>
       <c r="V2" s="496"/>
@@ -6715,18 +6717,18 @@
       </c>
       <c r="AA2" s="68">
         <f>Z2+T2</f>
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="3" spans="1:27" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="569"/>
-      <c r="B3" s="571"/>
-      <c r="C3" s="583"/>
-      <c r="D3" s="573"/>
-      <c r="E3" s="575"/>
-      <c r="G3" s="581"/>
+      <c r="A3" s="579"/>
+      <c r="B3" s="581"/>
+      <c r="C3" s="593"/>
+      <c r="D3" s="583"/>
+      <c r="E3" s="585"/>
+      <c r="G3" s="591"/>
       <c r="H3" s="6"/>
-      <c r="I3" s="592"/>
+      <c r="I3" s="573"/>
       <c r="K3" s="24">
         <v>2</v>
       </c>
@@ -6738,7 +6740,12 @@
         <v>5</v>
       </c>
       <c r="U3" s="6"/>
-      <c r="V3" s="497"/>
+      <c r="V3" s="497">
+        <v>1</v>
+      </c>
+      <c r="W3" s="6" t="s">
+        <v>252</v>
+      </c>
       <c r="X3" s="497"/>
     </row>
     <row r="4" spans="1:27" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -6746,16 +6753,16 @@
         <v>390</v>
       </c>
       <c r="B4" s="248"/>
-      <c r="C4" s="576" t="s">
+      <c r="C4" s="586" t="s">
         <v>178</v>
       </c>
-      <c r="I4" s="592"/>
+      <c r="I4" s="573"/>
       <c r="R4" s="499" t="s">
         <v>580</v>
       </c>
       <c r="T4" s="24">
         <f>IF((R7-SUM(V2:V10)&lt;0),R7-SUM(V2:V10),0)</f>
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="U4" s="6" t="s">
         <v>518</v>
@@ -6777,7 +6784,7 @@
       <c r="B5" s="100" t="s">
         <v>365</v>
       </c>
-      <c r="C5" s="577"/>
+      <c r="C5" s="587"/>
       <c r="D5" s="227" t="s">
         <v>103</v>
       </c>
@@ -6793,7 +6800,7 @@
       <c r="H5" s="211" t="s">
         <v>220</v>
       </c>
-      <c r="I5" s="592"/>
+      <c r="I5" s="573"/>
       <c r="J5" s="422" t="s">
         <v>273</v>
       </c>
@@ -6824,22 +6831,22 @@
       <c r="X5" s="495"/>
     </row>
     <row r="6" spans="1:27" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="565" t="s">
+      <c r="A6" s="575" t="s">
         <v>290</v>
       </c>
       <c r="B6" s="105" t="s">
         <v>199</v>
       </c>
-      <c r="C6" s="578"/>
-      <c r="D6" s="579"/>
+      <c r="C6" s="588"/>
+      <c r="D6" s="589"/>
       <c r="E6" s="96">
         <v>1</v>
       </c>
       <c r="G6" s="555"/>
-      <c r="I6" s="592"/>
+      <c r="I6" s="573"/>
     </row>
     <row r="7" spans="1:27" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="566"/>
+      <c r="A7" s="576"/>
       <c r="B7" s="100" t="s">
         <v>155</v>
       </c>
@@ -6850,7 +6857,7 @@
         <v>136</v>
       </c>
       <c r="G7" s="555"/>
-      <c r="I7" s="592"/>
+      <c r="I7" s="573"/>
       <c r="M7" s="16" t="s">
         <v>354</v>
       </c>
@@ -6886,7 +6893,7 @@
       </c>
     </row>
     <row r="8" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="567"/>
+      <c r="A8" s="577"/>
       <c r="B8" s="217" t="s">
         <v>28</v>
       </c>
@@ -6895,7 +6902,7 @@
         <v>3</v>
       </c>
       <c r="G8" s="555"/>
-      <c r="I8" s="592"/>
+      <c r="I8" s="573"/>
       <c r="N8" s="80"/>
       <c r="U8" s="6" t="s">
         <v>466</v>
@@ -6919,7 +6926,7 @@
       </c>
       <c r="G9" s="555"/>
       <c r="H9" s="6"/>
-      <c r="I9" s="592"/>
+      <c r="I9" s="573"/>
       <c r="M9" s="19" t="s">
         <v>547</v>
       </c>
@@ -6946,7 +6953,7 @@
         <v>42</v>
       </c>
       <c r="G10" s="555"/>
-      <c r="I10" s="592"/>
+      <c r="I10" s="573"/>
       <c r="J10" s="24" t="s">
         <v>381</v>
       </c>
@@ -6980,7 +6987,7 @@
         <v>270</v>
       </c>
       <c r="G11" s="555"/>
-      <c r="I11" s="592"/>
+      <c r="I11" s="573"/>
       <c r="J11" s="24" t="s">
         <v>195</v>
       </c>
@@ -7006,12 +7013,12 @@
       <c r="S11" s="24">
         <v>1</v>
       </c>
-      <c r="U11" s="586" t="s">
+      <c r="U11" s="567" t="s">
         <v>583</v>
       </c>
-      <c r="V11" s="587"/>
-      <c r="W11" s="587"/>
-      <c r="X11" s="588"/>
+      <c r="V11" s="568"/>
+      <c r="W11" s="568"/>
+      <c r="X11" s="569"/>
     </row>
     <row r="12" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="232" t="s">
@@ -7022,7 +7029,7 @@
         <v>3</v>
       </c>
       <c r="G12" s="555"/>
-      <c r="I12" s="592"/>
+      <c r="I12" s="573"/>
       <c r="J12" s="24" t="s">
         <v>538</v>
       </c>
@@ -7055,7 +7062,7 @@
       </c>
       <c r="D13" s="20"/>
       <c r="G13" s="555"/>
-      <c r="I13" s="592"/>
+      <c r="I13" s="573"/>
       <c r="J13" s="108" t="s">
         <v>572</v>
       </c>
@@ -7096,7 +7103,7 @@
       <c r="H14" s="211" t="s">
         <v>220</v>
       </c>
-      <c r="I14" s="592"/>
+      <c r="I14" s="573"/>
       <c r="U14" s="6"/>
       <c r="V14" s="112"/>
       <c r="W14" s="6"/>
@@ -7114,7 +7121,7 @@
       <c r="H15" s="277">
         <v>0</v>
       </c>
-      <c r="I15" s="592"/>
+      <c r="I15" s="573"/>
       <c r="J15" s="108" t="s">
         <v>154</v>
       </c>
@@ -7145,7 +7152,7 @@
       <c r="D16" s="2" t="s">
         <v>510</v>
       </c>
-      <c r="I16" s="592"/>
+      <c r="I16" s="573"/>
       <c r="K16" s="100" t="s">
         <v>44</v>
       </c>
@@ -7179,7 +7186,7 @@
       <c r="G17" s="2" t="s">
         <v>441</v>
       </c>
-      <c r="I17" s="592"/>
+      <c r="I17" s="573"/>
       <c r="L17" s="2" t="s">
         <v>444</v>
       </c>
@@ -7191,13 +7198,13 @@
     </row>
     <row r="18" spans="1:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="G18" s="16"/>
-      <c r="I18" s="592"/>
+      <c r="I18" s="573"/>
       <c r="L18" s="16"/>
       <c r="M18" s="21"/>
-      <c r="O18" s="589" t="s">
+      <c r="O18" s="570" t="s">
         <v>539</v>
       </c>
-      <c r="P18" s="590"/>
+      <c r="P18" s="571"/>
       <c r="Q18" s="127" t="s">
         <v>44</v>
       </c>
@@ -7207,7 +7214,7 @@
       </c>
       <c r="S18" s="24">
         <f>5-S26</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="U18" s="6" t="s">
         <v>479</v>
@@ -7223,7 +7230,7 @@
       </c>
     </row>
     <row r="19" spans="1:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="I19" s="592"/>
+      <c r="I19" s="573"/>
       <c r="M19" s="21" t="s">
         <v>443</v>
       </c>
@@ -7251,7 +7258,7 @@
       <c r="G20" s="2" t="s">
         <v>441</v>
       </c>
-      <c r="I20" s="592"/>
+      <c r="I20" s="573"/>
       <c r="K20" s="19" t="s">
         <v>440</v>
       </c>
@@ -7267,12 +7274,16 @@
       <c r="V20" s="24">
         <v>1</v>
       </c>
-      <c r="W20" s="6"/>
-      <c r="X20" s="497"/>
+      <c r="W20" s="6" t="s">
+        <v>352</v>
+      </c>
+      <c r="X20" s="497">
+        <v>1</v>
+      </c>
       <c r="Z20" s="112"/>
     </row>
     <row r="21" spans="1:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="I21" s="592"/>
+      <c r="I21" s="573"/>
       <c r="M21" s="221" t="s">
         <v>422</v>
       </c>
@@ -7304,7 +7315,7 @@
       <c r="G22" s="2" t="s">
         <v>441</v>
       </c>
-      <c r="I22" s="592"/>
+      <c r="I22" s="573"/>
       <c r="U22" s="6"/>
       <c r="V22" s="495"/>
       <c r="W22" s="6" t="s">
@@ -7324,13 +7335,13 @@
       <c r="E23" s="289" t="s">
         <v>44</v>
       </c>
-      <c r="I23" s="592"/>
+      <c r="I23" s="573"/>
       <c r="U23" s="6"/>
       <c r="V23" s="24"/>
       <c r="W23" s="6"/>
     </row>
     <row r="24" spans="1:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="I24" s="592"/>
+      <c r="I24" s="573"/>
       <c r="U24" s="354"/>
       <c r="V24" s="498">
         <v>-1</v>
@@ -7358,7 +7369,7 @@
       <c r="H25" s="196" t="s">
         <v>271</v>
       </c>
-      <c r="I25" s="592"/>
+      <c r="I25" s="573"/>
       <c r="J25" s="422" t="s">
         <v>274</v>
       </c>
@@ -7403,7 +7414,7 @@
       <c r="H26" s="19" t="s">
         <v>220</v>
       </c>
-      <c r="I26" s="592"/>
+      <c r="I26" s="573"/>
       <c r="K26" s="24">
         <v>15</v>
       </c>
@@ -7421,7 +7432,7 @@
         <v>2</v>
       </c>
       <c r="S26" s="24">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="T26" s="61" t="s">
         <v>581</v>
@@ -7438,7 +7449,7 @@
       </c>
     </row>
     <row r="27" spans="1:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="I27" s="592"/>
+      <c r="I27" s="573"/>
       <c r="O27" s="2" t="s">
         <v>99</v>
       </c>
@@ -7465,7 +7476,7 @@
       <c r="E28" s="220">
         <v>2</v>
       </c>
-      <c r="I28" s="592"/>
+      <c r="I28" s="573"/>
       <c r="Q28" s="6"/>
       <c r="R28" s="112"/>
       <c r="T28" s="142"/>
@@ -7487,7 +7498,7 @@
       <c r="H29" s="196" t="s">
         <v>272</v>
       </c>
-      <c r="I29" s="593"/>
+      <c r="I29" s="574"/>
       <c r="J29" s="333"/>
       <c r="L29" s="96" t="s">
         <v>278</v>
@@ -7516,21 +7527,23 @@
       <c r="B30" s="2" t="s">
         <v>415</v>
       </c>
-      <c r="U30" s="500" t="s">
+      <c r="U30" s="25" t="s">
         <v>582</v>
       </c>
-      <c r="V30" s="501">
+      <c r="V30" s="500">
         <v>0</v>
       </c>
       <c r="W30" s="19" t="s">
         <v>516</v>
       </c>
-      <c r="X30" s="502">
+      <c r="X30" s="501">
         <v>1</v>
       </c>
     </row>
     <row r="31" spans="1:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="U31" s="354"/>
+      <c r="U31" s="25" t="s">
+        <v>609</v>
+      </c>
       <c r="V31" s="335">
         <v>0</v>
       </c>
@@ -7542,8 +7555,8 @@
       </c>
     </row>
     <row r="32" spans="1:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="U32" s="516"/>
-      <c r="V32" s="502">
+      <c r="U32" s="515"/>
+      <c r="V32" s="501">
         <v>-1</v>
       </c>
       <c r="W32" s="19" t="s">
@@ -7555,11 +7568,6 @@
     </row>
   </sheetData>
   <mergeCells count="16">
-    <mergeCell ref="Q1:Q2"/>
-    <mergeCell ref="U11:X11"/>
-    <mergeCell ref="O18:P18"/>
-    <mergeCell ref="I2:I29"/>
-    <mergeCell ref="C13:C14"/>
     <mergeCell ref="A6:A8"/>
     <mergeCell ref="G5:G14"/>
     <mergeCell ref="A2:A3"/>
@@ -7571,6 +7579,11 @@
     <mergeCell ref="B11:B12"/>
     <mergeCell ref="G2:G3"/>
     <mergeCell ref="C2:C3"/>
+    <mergeCell ref="Q1:Q2"/>
+    <mergeCell ref="U11:X11"/>
+    <mergeCell ref="O18:P18"/>
+    <mergeCell ref="I2:I29"/>
+    <mergeCell ref="C13:C14"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -7646,7 +7659,7 @@
       <c r="H1" s="97" t="s">
         <v>350</v>
       </c>
-      <c r="I1" s="580" t="s">
+      <c r="I1" s="590" t="s">
         <v>378</v>
       </c>
       <c r="J1" s="2" t="s">
@@ -7707,7 +7720,7 @@
         <v>517</v>
       </c>
       <c r="AM1" s="427"/>
-      <c r="AN1" s="618"/>
+      <c r="AN1" s="621"/>
       <c r="AO1" s="350" t="s">
         <v>487</v>
       </c>
@@ -7716,23 +7729,23 @@
       </c>
     </row>
     <row r="2" spans="1:43" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="600">
+      <c r="A2" s="645">
         <f ca="1">TODAY()</f>
         <v>45279</v>
       </c>
-      <c r="B2" s="602" t="s">
+      <c r="B2" s="647" t="s">
         <v>379</v>
       </c>
-      <c r="C2" s="582" t="s">
+      <c r="C2" s="592" t="s">
         <v>365</v>
       </c>
-      <c r="D2" s="604" t="s">
+      <c r="D2" s="649" t="s">
         <v>362</v>
       </c>
-      <c r="E2" s="648" t="s">
+      <c r="E2" s="594" t="s">
         <v>65</v>
       </c>
-      <c r="F2" s="623" t="s">
+      <c r="F2" s="602" t="s">
         <v>103</v>
       </c>
       <c r="G2" s="418" t="s">
@@ -7741,31 +7754,31 @@
       <c r="H2" s="80" t="s">
         <v>33</v>
       </c>
-      <c r="I2" s="581"/>
+      <c r="I2" s="591"/>
       <c r="J2" s="81" t="s">
         <v>77</v>
       </c>
-      <c r="K2" s="650" t="s">
+      <c r="K2" s="596" t="s">
         <v>349</v>
       </c>
-      <c r="L2" s="651"/>
-      <c r="M2" s="623" t="s">
+      <c r="L2" s="597"/>
+      <c r="M2" s="602" t="s">
         <v>103</v>
       </c>
       <c r="N2" s="69" t="s">
         <v>28</v>
       </c>
-      <c r="O2" s="627" t="s">
+      <c r="O2" s="628" t="s">
         <v>103</v>
       </c>
       <c r="P2" s="85" t="s">
         <v>148</v>
       </c>
-      <c r="Q2" s="582" t="s">
+      <c r="Q2" s="592" t="s">
         <v>144</v>
       </c>
       <c r="R2" s="554"/>
-      <c r="S2" s="640" t="s">
+      <c r="S2" s="615" t="s">
         <v>149</v>
       </c>
       <c r="T2" s="89"/>
@@ -7798,15 +7811,15 @@
         <v>481</v>
       </c>
       <c r="AM2" s="453"/>
-      <c r="AN2" s="619"/>
+      <c r="AN2" s="622"/>
     </row>
     <row r="3" spans="1:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="601"/>
-      <c r="B3" s="603"/>
-      <c r="C3" s="583"/>
-      <c r="D3" s="605"/>
-      <c r="E3" s="649"/>
-      <c r="F3" s="624"/>
+      <c r="A3" s="646"/>
+      <c r="B3" s="648"/>
+      <c r="C3" s="593"/>
+      <c r="D3" s="650"/>
+      <c r="E3" s="595"/>
+      <c r="F3" s="603"/>
       <c r="G3" s="419" t="s">
         <v>28</v>
       </c>
@@ -7825,17 +7838,17 @@
       <c r="L3" s="206" t="s">
         <v>108</v>
       </c>
-      <c r="M3" s="624"/>
+      <c r="M3" s="603"/>
       <c r="N3" s="69" t="s">
         <v>147</v>
       </c>
-      <c r="O3" s="628"/>
+      <c r="O3" s="629"/>
       <c r="P3" s="2" t="s">
         <v>155</v>
       </c>
-      <c r="Q3" s="583"/>
+      <c r="Q3" s="593"/>
       <c r="R3" s="556"/>
-      <c r="S3" s="641"/>
+      <c r="S3" s="617"/>
       <c r="T3" s="89"/>
       <c r="U3" s="124"/>
       <c r="V3" s="120"/>
@@ -7852,7 +7865,7 @@
       <c r="AC3" s="100" t="s">
         <v>498</v>
       </c>
-      <c r="AD3" s="639" t="s">
+      <c r="AD3" s="612" t="s">
         <v>473</v>
       </c>
       <c r="AE3" s="262"/>
@@ -7864,16 +7877,16 @@
       <c r="AK3" s="262"/>
       <c r="AL3" s="16"/>
       <c r="AM3" s="453"/>
-      <c r="AN3" s="619"/>
+      <c r="AN3" s="622"/>
     </row>
     <row r="4" spans="1:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="243" t="s">
         <v>184</v>
       </c>
-      <c r="B4" s="616" t="s">
+      <c r="B4" s="661" t="s">
         <v>382</v>
       </c>
-      <c r="C4" s="582" t="s">
+      <c r="C4" s="592" t="s">
         <v>155</v>
       </c>
       <c r="D4" s="359" t="s">
@@ -7882,7 +7895,7 @@
       <c r="E4" s="396">
         <v>2</v>
       </c>
-      <c r="F4" s="624"/>
+      <c r="F4" s="603"/>
       <c r="G4" s="400" t="s">
         <v>203</v>
       </c>
@@ -7899,11 +7912,11 @@
         <v>151</v>
       </c>
       <c r="L4" s="209"/>
-      <c r="M4" s="624"/>
+      <c r="M4" s="603"/>
       <c r="N4" s="178" t="s">
         <v>70</v>
       </c>
-      <c r="O4" s="628"/>
+      <c r="O4" s="629"/>
       <c r="P4" s="2" t="s">
         <v>192</v>
       </c>
@@ -7930,7 +7943,7 @@
       <c r="AA4" s="313"/>
       <c r="AB4" s="214"/>
       <c r="AC4" s="16"/>
-      <c r="AD4" s="639"/>
+      <c r="AD4" s="612"/>
       <c r="AE4" s="262"/>
       <c r="AF4" s="262"/>
       <c r="AG4" s="16"/>
@@ -7940,37 +7953,37 @@
       <c r="AK4" s="262"/>
       <c r="AL4" s="16"/>
       <c r="AM4" s="453"/>
-      <c r="AN4" s="619"/>
+      <c r="AN4" s="622"/>
       <c r="AO4" s="350" t="s">
         <v>91</v>
       </c>
     </row>
     <row r="5" spans="1:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="580" t="s">
+      <c r="A5" s="590" t="s">
         <v>435</v>
       </c>
-      <c r="B5" s="617"/>
-      <c r="C5" s="583"/>
+      <c r="B5" s="662"/>
+      <c r="C5" s="593"/>
       <c r="D5" s="61" t="s">
         <v>154</v>
       </c>
       <c r="E5" s="397">
         <v>1</v>
       </c>
-      <c r="F5" s="624"/>
-      <c r="G5" s="608" t="s">
+      <c r="F5" s="603"/>
+      <c r="G5" s="653" t="s">
         <v>193</v>
       </c>
-      <c r="H5" s="608"/>
-      <c r="I5" s="608"/>
-      <c r="J5" s="608"/>
-      <c r="K5" s="608"/>
-      <c r="L5" s="609"/>
-      <c r="M5" s="624"/>
+      <c r="H5" s="653"/>
+      <c r="I5" s="653"/>
+      <c r="J5" s="653"/>
+      <c r="K5" s="653"/>
+      <c r="L5" s="654"/>
+      <c r="M5" s="603"/>
       <c r="N5" s="21">
         <v>8</v>
       </c>
-      <c r="O5" s="628"/>
+      <c r="O5" s="629"/>
       <c r="T5" s="89"/>
       <c r="U5" s="124"/>
       <c r="V5" s="120"/>
@@ -8001,24 +8014,24 @@
       <c r="AK5" s="262"/>
       <c r="AL5" s="80"/>
       <c r="AM5" s="453"/>
-      <c r="AN5" s="619"/>
+      <c r="AN5" s="622"/>
     </row>
     <row r="6" spans="1:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="581"/>
-      <c r="B6" s="614" t="s">
+      <c r="A6" s="591"/>
+      <c r="B6" s="659" t="s">
         <v>178</v>
       </c>
-      <c r="C6" s="578"/>
-      <c r="D6" s="579"/>
-      <c r="F6" s="624"/>
-      <c r="G6" s="610"/>
-      <c r="H6" s="610"/>
-      <c r="I6" s="610"/>
-      <c r="J6" s="610"/>
-      <c r="K6" s="610"/>
-      <c r="L6" s="611"/>
-      <c r="M6" s="624"/>
-      <c r="O6" s="628"/>
+      <c r="C6" s="588"/>
+      <c r="D6" s="589"/>
+      <c r="F6" s="603"/>
+      <c r="G6" s="655"/>
+      <c r="H6" s="655"/>
+      <c r="I6" s="655"/>
+      <c r="J6" s="655"/>
+      <c r="K6" s="655"/>
+      <c r="L6" s="656"/>
+      <c r="M6" s="603"/>
+      <c r="O6" s="629"/>
       <c r="T6" s="89"/>
       <c r="U6" s="124"/>
       <c r="V6" s="98" t="s">
@@ -8042,16 +8055,16 @@
       <c r="AF6" s="262"/>
       <c r="AG6" s="262"/>
       <c r="AH6" s="262"/>
-      <c r="AI6" s="633"/>
+      <c r="AI6" s="611"/>
       <c r="AJ6" s="466" t="s">
         <v>476</v>
       </c>
-      <c r="AK6" s="633" t="s">
+      <c r="AK6" s="611" t="s">
         <v>256</v>
       </c>
       <c r="AL6" s="262"/>
       <c r="AM6" s="453"/>
-      <c r="AN6" s="619"/>
+      <c r="AN6" s="622"/>
       <c r="AO6" s="350" t="s">
         <v>488</v>
       </c>
@@ -8060,7 +8073,7 @@
       <c r="A7" s="237" t="s">
         <v>598</v>
       </c>
-      <c r="B7" s="615"/>
+      <c r="B7" s="660"/>
       <c r="C7" s="207" t="s">
         <v>383</v>
       </c>
@@ -8070,7 +8083,7 @@
       <c r="E7" s="271">
         <v>3</v>
       </c>
-      <c r="F7" s="624"/>
+      <c r="F7" s="603"/>
       <c r="G7" s="420">
         <v>0</v>
       </c>
@@ -8089,8 +8102,8 @@
       <c r="L7" s="217">
         <v>0</v>
       </c>
-      <c r="M7" s="624"/>
-      <c r="O7" s="628"/>
+      <c r="M7" s="603"/>
+      <c r="O7" s="629"/>
       <c r="R7" s="99" t="s">
         <v>44</v>
       </c>
@@ -8114,18 +8127,18 @@
       <c r="AD7" s="16"/>
       <c r="AE7" s="262"/>
       <c r="AF7" s="262"/>
-      <c r="AG7" s="639" t="s">
+      <c r="AG7" s="612" t="s">
         <v>472</v>
       </c>
       <c r="AH7" s="262"/>
-      <c r="AI7" s="633"/>
+      <c r="AI7" s="611"/>
       <c r="AJ7" s="262"/>
-      <c r="AK7" s="633"/>
+      <c r="AK7" s="611"/>
       <c r="AL7" s="80" t="s">
         <v>515</v>
       </c>
       <c r="AM7" s="453"/>
-      <c r="AN7" s="619"/>
+      <c r="AN7" s="622"/>
       <c r="AP7" s="76" t="s">
         <v>489</v>
       </c>
@@ -8142,27 +8155,27 @@
         <f>SUM(G7:N9)</f>
         <v>15</v>
       </c>
-      <c r="F8" s="624"/>
-      <c r="G8" s="609">
-        <v>0</v>
-      </c>
-      <c r="H8" s="606" t="s">
+      <c r="F8" s="603"/>
+      <c r="G8" s="654">
+        <v>0</v>
+      </c>
+      <c r="H8" s="651" t="s">
         <v>105</v>
       </c>
       <c r="I8" s="554">
         <v>0</v>
       </c>
-      <c r="J8" s="606" t="s">
+      <c r="J8" s="651" t="s">
         <v>105</v>
       </c>
-      <c r="K8" s="612"/>
-      <c r="L8" s="642"/>
-      <c r="M8" s="625"/>
-      <c r="N8" s="645">
+      <c r="K8" s="657"/>
+      <c r="L8" s="613"/>
+      <c r="M8" s="626"/>
+      <c r="N8" s="618">
         <f>N5+N11</f>
         <v>15</v>
       </c>
-      <c r="O8" s="628"/>
+      <c r="O8" s="629"/>
       <c r="T8" s="103" t="s">
         <v>44</v>
       </c>
@@ -8180,14 +8193,14 @@
       <c r="AD8" s="16"/>
       <c r="AE8" s="262"/>
       <c r="AF8" s="262"/>
-      <c r="AG8" s="639"/>
+      <c r="AG8" s="612"/>
       <c r="AH8" s="262"/>
-      <c r="AI8" s="633"/>
+      <c r="AI8" s="611"/>
       <c r="AJ8" s="262"/>
       <c r="AK8" s="262"/>
       <c r="AL8" s="262"/>
       <c r="AM8" s="453"/>
-      <c r="AN8" s="619"/>
+      <c r="AN8" s="622"/>
     </row>
     <row r="9" spans="1:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="237" t="s">
@@ -8202,17 +8215,17 @@
       <c r="D9" s="360" t="s">
         <v>286</v>
       </c>
-      <c r="F9" s="624"/>
-      <c r="G9" s="611"/>
-      <c r="H9" s="607"/>
+      <c r="F9" s="603"/>
+      <c r="G9" s="656"/>
+      <c r="H9" s="652"/>
       <c r="I9" s="556"/>
-      <c r="J9" s="607"/>
-      <c r="K9" s="613"/>
-      <c r="L9" s="643"/>
-      <c r="M9" s="626"/>
-      <c r="N9" s="646"/>
-      <c r="O9" s="629"/>
-      <c r="S9" s="640" t="s">
+      <c r="J9" s="652"/>
+      <c r="K9" s="658"/>
+      <c r="L9" s="614"/>
+      <c r="M9" s="627"/>
+      <c r="N9" s="619"/>
+      <c r="O9" s="630"/>
+      <c r="S9" s="615" t="s">
         <v>62</v>
       </c>
       <c r="T9" s="89"/>
@@ -8234,16 +8247,16 @@
       </c>
       <c r="AE9" s="262"/>
       <c r="AF9" s="262"/>
-      <c r="AG9" s="639"/>
+      <c r="AG9" s="612"/>
       <c r="AH9" s="262"/>
-      <c r="AI9" s="633"/>
+      <c r="AI9" s="611"/>
       <c r="AJ9" s="80"/>
-      <c r="AK9" s="633" t="s">
+      <c r="AK9" s="611" t="s">
         <v>256</v>
       </c>
       <c r="AL9" s="262"/>
       <c r="AM9" s="453"/>
-      <c r="AN9" s="619"/>
+      <c r="AN9" s="622"/>
       <c r="AP9" s="2" t="s">
         <v>527</v>
       </c>
@@ -8260,20 +8273,20 @@
         <f>Boat!U8</f>
         <v>42</v>
       </c>
-      <c r="F10" s="624"/>
+      <c r="F10" s="603"/>
       <c r="N10" s="443" t="s">
         <v>407</v>
       </c>
-      <c r="O10" s="657" t="s">
+      <c r="O10" s="605" t="s">
         <v>103</v>
       </c>
-      <c r="P10" s="630" t="s">
+      <c r="P10" s="631" t="s">
         <v>411</v>
       </c>
       <c r="R10" s="74" t="s">
         <v>44</v>
       </c>
-      <c r="S10" s="644"/>
+      <c r="S10" s="616"/>
       <c r="T10" s="89"/>
       <c r="U10" s="123" t="s">
         <v>177</v>
@@ -8303,16 +8316,16 @@
       <c r="AF10" s="243" t="s">
         <v>318</v>
       </c>
-      <c r="AG10" s="639"/>
+      <c r="AG10" s="612"/>
       <c r="AH10" s="80"/>
-      <c r="AI10" s="633"/>
+      <c r="AI10" s="611"/>
       <c r="AJ10" s="262"/>
-      <c r="AK10" s="633"/>
+      <c r="AK10" s="611"/>
       <c r="AL10" s="262"/>
       <c r="AM10" s="467" t="s">
         <v>325</v>
       </c>
-      <c r="AN10" s="619"/>
+      <c r="AN10" s="622"/>
       <c r="AO10" s="209" t="s">
         <v>95</v>
       </c>
@@ -8330,18 +8343,18 @@
       <c r="D11" s="174" t="s">
         <v>362</v>
       </c>
-      <c r="F11" s="624"/>
+      <c r="F11" s="603"/>
       <c r="M11" s="6"/>
       <c r="N11" s="117">
         <v>7</v>
       </c>
-      <c r="O11" s="658"/>
-      <c r="P11" s="631"/>
+      <c r="O11" s="606"/>
+      <c r="P11" s="632"/>
       <c r="Q11" s="65"/>
       <c r="R11" s="120" t="s">
         <v>222</v>
       </c>
-      <c r="S11" s="644"/>
+      <c r="S11" s="616"/>
       <c r="T11" s="102" t="s">
         <v>44</v>
       </c>
@@ -8365,14 +8378,14 @@
       <c r="AF11" s="262" t="s">
         <v>494</v>
       </c>
-      <c r="AG11" s="639"/>
+      <c r="AG11" s="612"/>
       <c r="AH11" s="262"/>
       <c r="AI11" s="70"/>
       <c r="AJ11" s="262"/>
       <c r="AK11" s="262"/>
       <c r="AL11" s="262"/>
       <c r="AM11" s="453"/>
-      <c r="AN11" s="619"/>
+      <c r="AN11" s="622"/>
       <c r="AP11" s="76" t="s">
         <v>502</v>
       </c>
@@ -8391,7 +8404,7 @@
       <c r="E12" s="229">
         <v>3</v>
       </c>
-      <c r="F12" s="624"/>
+      <c r="F12" s="603"/>
       <c r="G12" s="349" t="s">
         <v>411</v>
       </c>
@@ -8400,16 +8413,16 @@
       </c>
       <c r="I12" s="561"/>
       <c r="J12" s="561"/>
-      <c r="K12" s="662"/>
+      <c r="K12" s="610"/>
       <c r="L12" s="208"/>
       <c r="M12" s="208"/>
       <c r="N12" s="208"/>
-      <c r="O12" s="658"/>
-      <c r="P12" s="631"/>
+      <c r="O12" s="606"/>
+      <c r="P12" s="632"/>
       <c r="R12" s="122" t="s">
         <v>181</v>
       </c>
-      <c r="S12" s="641"/>
+      <c r="S12" s="617"/>
       <c r="T12" s="101" t="s">
         <v>44</v>
       </c>
@@ -8430,16 +8443,16 @@
       <c r="AC12" s="100" t="s">
         <v>499</v>
       </c>
-      <c r="AD12" s="647" t="s">
+      <c r="AD12" s="620" t="s">
         <v>245</v>
       </c>
       <c r="AE12" s="466" t="s">
         <v>244</v>
       </c>
-      <c r="AF12" s="639" t="s">
+      <c r="AF12" s="612" t="s">
         <v>231</v>
       </c>
-      <c r="AG12" s="639"/>
+      <c r="AG12" s="612"/>
       <c r="AH12" s="243" t="s">
         <v>264</v>
       </c>
@@ -8452,7 +8465,7 @@
       <c r="AM12" s="634" t="s">
         <v>254</v>
       </c>
-      <c r="AN12" s="619"/>
+      <c r="AN12" s="622"/>
       <c r="AO12" s="350" t="s">
         <v>97</v>
       </c>
@@ -8464,17 +8477,17 @@
       <c r="E13" s="473">
         <v>-3</v>
       </c>
-      <c r="F13" s="624"/>
+      <c r="F13" s="603"/>
       <c r="G13" s="561" t="s">
         <v>448</v>
       </c>
       <c r="H13" s="561"/>
       <c r="I13" s="561"/>
-      <c r="J13" s="662"/>
+      <c r="J13" s="610"/>
       <c r="M13" s="6"/>
       <c r="N13" s="6"/>
-      <c r="O13" s="658"/>
-      <c r="P13" s="632"/>
+      <c r="O13" s="606"/>
+      <c r="P13" s="633"/>
       <c r="T13" s="105" t="s">
         <v>44</v>
       </c>
@@ -8495,8 +8508,8 @@
         <v>519</v>
       </c>
       <c r="AC13" s="16"/>
-      <c r="AD13" s="647"/>
-      <c r="AF13" s="639"/>
+      <c r="AD13" s="620"/>
+      <c r="AF13" s="612"/>
       <c r="AG13" s="80"/>
       <c r="AH13" s="243" t="s">
         <v>314</v>
@@ -8508,7 +8521,7 @@
       <c r="AK13" s="262"/>
       <c r="AL13" s="262"/>
       <c r="AM13" s="634"/>
-      <c r="AN13" s="619"/>
+      <c r="AN13" s="622"/>
     </row>
     <row r="14" spans="1:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="475"/>
@@ -8516,18 +8529,18 @@
       <c r="C14" s="484"/>
       <c r="D14" s="477"/>
       <c r="E14" s="478"/>
-      <c r="F14" s="624"/>
+      <c r="F14" s="603"/>
       <c r="G14" s="561" t="s">
         <v>447</v>
       </c>
       <c r="H14" s="561"/>
       <c r="I14" s="561"/>
-      <c r="J14" s="662"/>
+      <c r="J14" s="610"/>
       <c r="K14" s="2">
         <v>12</v>
       </c>
       <c r="N14" s="6"/>
-      <c r="O14" s="658"/>
+      <c r="O14" s="606"/>
       <c r="Q14" s="61" t="s">
         <v>555</v>
       </c>
@@ -8548,9 +8561,9 @@
       <c r="AA14" s="313"/>
       <c r="AB14" s="214"/>
       <c r="AC14" s="16"/>
-      <c r="AD14" s="647"/>
+      <c r="AD14" s="620"/>
       <c r="AE14" s="262"/>
-      <c r="AF14" s="639"/>
+      <c r="AF14" s="612"/>
       <c r="AG14" s="262"/>
       <c r="AH14" s="262"/>
       <c r="AI14" s="70"/>
@@ -8558,7 +8571,7 @@
       <c r="AK14" s="262"/>
       <c r="AL14" s="262"/>
       <c r="AM14" s="634"/>
-      <c r="AN14" s="619"/>
+      <c r="AN14" s="622"/>
     </row>
     <row r="15" spans="1:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="474" t="s">
@@ -8567,8 +8580,8 @@
       <c r="C15" s="554" t="s">
         <v>382</v>
       </c>
-      <c r="F15" s="624"/>
-      <c r="O15" s="658"/>
+      <c r="F15" s="603"/>
+      <c r="O15" s="606"/>
       <c r="R15" s="99" t="s">
         <v>44</v>
       </c>
@@ -8590,8 +8603,8 @@
       <c r="AC15" s="76" t="s">
         <v>497</v>
       </c>
-      <c r="AD15" s="647"/>
-      <c r="AF15" s="639"/>
+      <c r="AD15" s="620"/>
+      <c r="AF15" s="612"/>
       <c r="AG15" s="80"/>
       <c r="AH15" s="243" t="s">
         <v>466</v>
@@ -8605,7 +8618,7 @@
       <c r="AK15" s="262"/>
       <c r="AL15" s="262"/>
       <c r="AM15" s="634"/>
-      <c r="AN15" s="619"/>
+      <c r="AN15" s="622"/>
       <c r="AP15" s="76" t="s">
         <v>74</v>
       </c>
@@ -8627,13 +8640,13 @@
       <c r="E16" s="229">
         <v>1</v>
       </c>
-      <c r="F16" s="624"/>
+      <c r="F16" s="603"/>
       <c r="G16" s="349" t="s">
         <v>506</v>
       </c>
       <c r="I16" s="496"/>
       <c r="J16" s="20"/>
-      <c r="O16" s="658"/>
+      <c r="O16" s="606"/>
       <c r="R16" s="460" t="s">
         <v>185</v>
       </c>
@@ -8665,18 +8678,18 @@
       <c r="AM16" s="453" t="s">
         <v>324</v>
       </c>
-      <c r="AN16" s="619"/>
+      <c r="AN16" s="622"/>
       <c r="AP16" s="76" t="s">
         <v>235</v>
       </c>
     </row>
     <row r="17" spans="1:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B17" s="80"/>
-      <c r="F17" s="624"/>
+      <c r="F17" s="603"/>
       <c r="I17" s="497"/>
       <c r="J17" s="20"/>
       <c r="N17" s="6"/>
-      <c r="O17" s="658"/>
+      <c r="O17" s="606"/>
       <c r="Q17" s="21" t="s">
         <v>553</v>
       </c>
@@ -8721,7 +8734,7 @@
       <c r="AK17" s="262"/>
       <c r="AL17" s="80"/>
       <c r="AM17" s="453"/>
-      <c r="AN17" s="619"/>
+      <c r="AN17" s="622"/>
       <c r="AO17" s="209" t="s">
         <v>516</v>
       </c>
@@ -8745,21 +8758,21 @@
       <c r="E18" s="99" t="s">
         <v>44</v>
       </c>
-      <c r="F18" s="624"/>
+      <c r="F18" s="603"/>
       <c r="G18" s="349" t="s">
         <v>550</v>
       </c>
       <c r="I18" s="24"/>
       <c r="J18" s="20"/>
-      <c r="O18" s="658"/>
+      <c r="O18" s="606"/>
       <c r="Q18" s="112"/>
-      <c r="R18" s="652" t="s">
+      <c r="R18" s="598" t="s">
         <v>558</v>
       </c>
       <c r="T18" s="100" t="s">
         <v>44</v>
       </c>
-      <c r="U18" s="597" t="s">
+      <c r="U18" s="642" t="s">
         <v>44</v>
       </c>
       <c r="V18" s="120"/>
@@ -8780,7 +8793,7 @@
       <c r="AC18" s="16"/>
       <c r="AD18" s="16"/>
       <c r="AE18" s="262"/>
-      <c r="AF18" s="633" t="s">
+      <c r="AF18" s="611" t="s">
         <v>493</v>
       </c>
       <c r="AG18" s="262"/>
@@ -8792,20 +8805,20 @@
       <c r="AK18" s="262"/>
       <c r="AL18" s="80"/>
       <c r="AM18" s="453"/>
-      <c r="AN18" s="619"/>
+      <c r="AN18" s="622"/>
       <c r="AP18" s="76" t="s">
         <v>88</v>
       </c>
     </row>
     <row r="19" spans="1:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="F19" s="624"/>
+      <c r="F19" s="603"/>
       <c r="I19" s="224"/>
-      <c r="O19" s="658"/>
-      <c r="R19" s="653"/>
+      <c r="O19" s="606"/>
+      <c r="R19" s="599"/>
       <c r="S19" s="30" t="s">
         <v>556</v>
       </c>
-      <c r="U19" s="598"/>
+      <c r="U19" s="643"/>
       <c r="V19" s="146"/>
       <c r="W19" s="146"/>
       <c r="X19" s="456" t="s">
@@ -8820,7 +8833,7 @@
       <c r="AC19" s="16"/>
       <c r="AD19" s="16"/>
       <c r="AE19" s="262"/>
-      <c r="AF19" s="633"/>
+      <c r="AF19" s="611"/>
       <c r="AG19" s="262"/>
       <c r="AH19" s="262"/>
       <c r="AI19" s="70"/>
@@ -8830,7 +8843,7 @@
       </c>
       <c r="AL19" s="80"/>
       <c r="AM19" s="453"/>
-      <c r="AN19" s="619"/>
+      <c r="AN19" s="622"/>
       <c r="AP19" s="76" t="s">
         <v>486</v>
       </c>
@@ -8851,19 +8864,19 @@
       <c r="E20" s="462">
         <v>-1</v>
       </c>
-      <c r="F20" s="624"/>
+      <c r="F20" s="603"/>
       <c r="G20" s="349" t="s">
         <v>509</v>
       </c>
       <c r="I20" s="224"/>
-      <c r="O20" s="658"/>
-      <c r="Q20" s="660" t="s">
+      <c r="O20" s="606"/>
+      <c r="Q20" s="608" t="s">
         <v>48</v>
       </c>
       <c r="T20" s="429" t="s">
         <v>44</v>
       </c>
-      <c r="U20" s="599"/>
+      <c r="U20" s="644"/>
       <c r="W20" s="430"/>
       <c r="X20" s="457" t="s">
         <v>175</v>
@@ -8893,7 +8906,7 @@
       <c r="AM20" s="400" t="s">
         <v>254</v>
       </c>
-      <c r="AN20" s="619"/>
+      <c r="AN20" s="622"/>
       <c r="AO20" s="350" t="s">
         <v>478</v>
       </c>
@@ -8914,13 +8927,13 @@
       <c r="E21" s="271">
         <v>0</v>
       </c>
-      <c r="F21" s="624"/>
+      <c r="F21" s="603"/>
       <c r="I21" s="224"/>
-      <c r="O21" s="658"/>
-      <c r="Q21" s="661"/>
+      <c r="O21" s="606"/>
+      <c r="Q21" s="609"/>
       <c r="T21" s="447"/>
       <c r="U21" s="14"/>
-      <c r="V21" s="594"/>
+      <c r="V21" s="639"/>
       <c r="W21" s="451" t="s">
         <v>176</v>
       </c>
@@ -8958,15 +8971,15 @@
       <c r="AM21" s="453" t="s">
         <v>567</v>
       </c>
-      <c r="AN21" s="619"/>
+      <c r="AN21" s="622"/>
     </row>
     <row r="22" spans="1:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="F22" s="624"/>
+      <c r="F22" s="603"/>
       <c r="G22" s="349" t="s">
         <v>507</v>
       </c>
       <c r="I22" s="224"/>
-      <c r="O22" s="658"/>
+      <c r="O22" s="606"/>
       <c r="R22" s="459" t="s">
         <v>44</v>
       </c>
@@ -8974,7 +8987,7 @@
         <v>44</v>
       </c>
       <c r="U22" s="15"/>
-      <c r="V22" s="595"/>
+      <c r="V22" s="640"/>
       <c r="W22" s="451" t="s">
         <v>176</v>
       </c>
@@ -8992,7 +9005,7 @@
       <c r="AG22" s="6"/>
       <c r="AH22" s="6"/>
       <c r="AI22" s="6"/>
-      <c r="AJ22" s="633" t="s">
+      <c r="AJ22" s="611" t="s">
         <v>490</v>
       </c>
       <c r="AK22" s="262"/>
@@ -9000,7 +9013,7 @@
         <v>496</v>
       </c>
       <c r="AM22" s="306"/>
-      <c r="AN22" s="619"/>
+      <c r="AN22" s="622"/>
     </row>
     <row r="23" spans="1:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="236" t="s">
@@ -9018,17 +9031,17 @@
       <c r="E23" s="230">
         <v>1</v>
       </c>
-      <c r="F23" s="624"/>
+      <c r="F23" s="603"/>
       <c r="I23" s="224"/>
-      <c r="O23" s="658"/>
-      <c r="Q23" s="660" t="s">
+      <c r="O23" s="606"/>
+      <c r="Q23" s="608" t="s">
         <v>145</v>
       </c>
       <c r="T23" s="17"/>
       <c r="U23" s="445" t="s">
         <v>44</v>
       </c>
-      <c r="V23" s="595"/>
+      <c r="V23" s="640"/>
       <c r="W23" s="148"/>
       <c r="X23" s="454" t="s">
         <v>189</v>
@@ -9044,13 +9057,13 @@
       <c r="AG23" s="6"/>
       <c r="AH23" s="6"/>
       <c r="AI23" s="6"/>
-      <c r="AJ23" s="633"/>
+      <c r="AJ23" s="611"/>
       <c r="AK23" s="262"/>
       <c r="AL23" s="80" t="s">
         <v>526</v>
       </c>
       <c r="AM23" s="306"/>
-      <c r="AN23" s="619"/>
+      <c r="AN23" s="622"/>
     </row>
     <row r="24" spans="1:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="465" t="s">
@@ -9068,18 +9081,18 @@
       <c r="E24" s="461">
         <v>1</v>
       </c>
-      <c r="F24" s="624"/>
+      <c r="F24" s="603"/>
       <c r="G24" s="61" t="s">
         <v>508</v>
       </c>
       <c r="I24" s="224"/>
-      <c r="O24" s="658"/>
-      <c r="Q24" s="661"/>
+      <c r="O24" s="606"/>
+      <c r="Q24" s="609"/>
       <c r="T24" s="17"/>
       <c r="U24" s="232" t="s">
         <v>44</v>
       </c>
-      <c r="V24" s="595"/>
+      <c r="V24" s="640"/>
       <c r="W24" s="148"/>
       <c r="X24" s="454" t="s">
         <v>186</v>
@@ -9103,12 +9116,12 @@
         <v>481</v>
       </c>
       <c r="AM24" s="306"/>
-      <c r="AN24" s="619"/>
+      <c r="AN24" s="622"/>
     </row>
     <row r="25" spans="1:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="F25" s="624"/>
+      <c r="F25" s="603"/>
       <c r="I25" s="224"/>
-      <c r="O25" s="658"/>
+      <c r="O25" s="606"/>
       <c r="P25" s="209" t="s">
         <v>285</v>
       </c>
@@ -9121,7 +9134,7 @@
       <c r="U25" s="425" t="s">
         <v>44</v>
       </c>
-      <c r="V25" s="596"/>
+      <c r="V25" s="641"/>
       <c r="W25" s="148"/>
       <c r="X25" s="454" t="s">
         <v>190</v>
@@ -9143,7 +9156,7 @@
       <c r="AK25" s="142"/>
       <c r="AL25" s="6"/>
       <c r="AM25" s="306"/>
-      <c r="AN25" s="619"/>
+      <c r="AN25" s="622"/>
     </row>
     <row r="26" spans="1:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="236" t="s">
@@ -9161,17 +9174,17 @@
       <c r="E26" s="398">
         <v>1</v>
       </c>
-      <c r="F26" s="624"/>
+      <c r="F26" s="603"/>
       <c r="G26" s="349" t="s">
         <v>505</v>
       </c>
       <c r="I26" s="224"/>
-      <c r="O26" s="658"/>
-      <c r="P26" s="621" t="s">
+      <c r="O26" s="606"/>
+      <c r="P26" s="624" t="s">
         <v>548</v>
       </c>
-      <c r="Q26" s="622"/>
-      <c r="R26" s="654" t="s">
+      <c r="Q26" s="625"/>
+      <c r="R26" s="600" t="s">
         <v>557</v>
       </c>
       <c r="T26" s="182"/>
@@ -9210,7 +9223,7 @@
       <c r="AM26" s="467" t="s">
         <v>474</v>
       </c>
-      <c r="AN26" s="619"/>
+      <c r="AN26" s="622"/>
     </row>
     <row r="27" spans="1:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B27" s="21" t="s">
@@ -9222,13 +9235,13 @@
       <c r="E27" s="271" t="s">
         <v>44</v>
       </c>
-      <c r="F27" s="656"/>
+      <c r="F27" s="604"/>
       <c r="G27" s="61" t="s">
         <v>566</v>
       </c>
       <c r="I27" s="225"/>
-      <c r="O27" s="659"/>
-      <c r="R27" s="655"/>
+      <c r="O27" s="607"/>
+      <c r="R27" s="601"/>
       <c r="S27" s="446" t="s">
         <v>54</v>
       </c>
@@ -9258,32 +9271,26 @@
       <c r="AM27" s="400" t="s">
         <v>326</v>
       </c>
-      <c r="AN27" s="620"/>
+      <c r="AN27" s="623"/>
     </row>
   </sheetData>
   <mergeCells count="54">
-    <mergeCell ref="E2:E3"/>
-    <mergeCell ref="K2:L2"/>
-    <mergeCell ref="I1:I2"/>
-    <mergeCell ref="R18:R19"/>
-    <mergeCell ref="R26:R27"/>
-    <mergeCell ref="F2:F27"/>
-    <mergeCell ref="O10:O27"/>
-    <mergeCell ref="Q20:Q21"/>
-    <mergeCell ref="Q23:Q24"/>
-    <mergeCell ref="G14:J14"/>
-    <mergeCell ref="G13:J13"/>
-    <mergeCell ref="H12:K12"/>
-    <mergeCell ref="A5:A6"/>
-    <mergeCell ref="C6:D6"/>
-    <mergeCell ref="AI6:AI10"/>
-    <mergeCell ref="AF12:AF15"/>
-    <mergeCell ref="AG7:AG12"/>
-    <mergeCell ref="L8:L9"/>
-    <mergeCell ref="S9:S12"/>
-    <mergeCell ref="N8:N9"/>
-    <mergeCell ref="AD12:AD15"/>
-    <mergeCell ref="C15:C16"/>
+    <mergeCell ref="V21:V25"/>
+    <mergeCell ref="U18:U20"/>
+    <mergeCell ref="C2:C3"/>
+    <mergeCell ref="C4:C5"/>
+    <mergeCell ref="A2:A3"/>
+    <mergeCell ref="B2:B3"/>
+    <mergeCell ref="D2:D3"/>
+    <mergeCell ref="J8:J9"/>
+    <mergeCell ref="G5:L6"/>
+    <mergeCell ref="I8:I9"/>
+    <mergeCell ref="K7:K9"/>
+    <mergeCell ref="H8:H9"/>
+    <mergeCell ref="G8:G9"/>
+    <mergeCell ref="B11:B12"/>
+    <mergeCell ref="B6:B7"/>
+    <mergeCell ref="B4:B5"/>
     <mergeCell ref="AN1:AN27"/>
     <mergeCell ref="P26:Q26"/>
     <mergeCell ref="Q2:Q3"/>
@@ -9300,22 +9307,28 @@
     <mergeCell ref="AD3:AD4"/>
     <mergeCell ref="S2:S3"/>
     <mergeCell ref="R2:R3"/>
-    <mergeCell ref="V21:V25"/>
-    <mergeCell ref="U18:U20"/>
-    <mergeCell ref="C2:C3"/>
-    <mergeCell ref="C4:C5"/>
-    <mergeCell ref="A2:A3"/>
-    <mergeCell ref="B2:B3"/>
-    <mergeCell ref="D2:D3"/>
-    <mergeCell ref="J8:J9"/>
-    <mergeCell ref="G5:L6"/>
-    <mergeCell ref="I8:I9"/>
-    <mergeCell ref="K7:K9"/>
-    <mergeCell ref="H8:H9"/>
-    <mergeCell ref="G8:G9"/>
-    <mergeCell ref="B11:B12"/>
-    <mergeCell ref="B6:B7"/>
-    <mergeCell ref="B4:B5"/>
+    <mergeCell ref="A5:A6"/>
+    <mergeCell ref="C6:D6"/>
+    <mergeCell ref="AI6:AI10"/>
+    <mergeCell ref="AF12:AF15"/>
+    <mergeCell ref="AG7:AG12"/>
+    <mergeCell ref="L8:L9"/>
+    <mergeCell ref="S9:S12"/>
+    <mergeCell ref="N8:N9"/>
+    <mergeCell ref="AD12:AD15"/>
+    <mergeCell ref="C15:C16"/>
+    <mergeCell ref="E2:E3"/>
+    <mergeCell ref="K2:L2"/>
+    <mergeCell ref="I1:I2"/>
+    <mergeCell ref="R18:R19"/>
+    <mergeCell ref="R26:R27"/>
+    <mergeCell ref="F2:F27"/>
+    <mergeCell ref="O10:O27"/>
+    <mergeCell ref="Q20:Q21"/>
+    <mergeCell ref="Q23:Q24"/>
+    <mergeCell ref="G14:J14"/>
+    <mergeCell ref="G13:J13"/>
+    <mergeCell ref="H12:K12"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -9325,8 +9338,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2029A93E-B53C-4201-9F17-439C144F3CF1}">
   <dimension ref="A1:AN37"/>
   <sheetViews>
-    <sheetView topLeftCell="A18" workbookViewId="0">
-      <selection activeCell="I22" sqref="I22"/>
+    <sheetView tabSelected="1" topLeftCell="N1" workbookViewId="0">
+      <selection activeCell="W25" sqref="W25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9421,17 +9434,17 @@
       <c r="S1" s="142"/>
       <c r="T1" s="142"/>
       <c r="U1" s="6"/>
-      <c r="V1" s="669" t="s">
+      <c r="V1" s="666" t="s">
         <v>459</v>
       </c>
-      <c r="W1" s="670"/>
+      <c r="W1" s="667"/>
       <c r="X1" s="312">
         <f>68-(U8+W3+V3+S3)</f>
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="Y1" s="102">
         <f>X1+X3</f>
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="Z1" s="102" t="s">
         <v>458</v>
@@ -9440,28 +9453,28 @@
       <c r="AB1" s="308" t="s">
         <v>44</v>
       </c>
-      <c r="AC1" s="671" t="s">
+      <c r="AC1" s="668" t="s">
         <v>191</v>
       </c>
-      <c r="AD1" s="672"/>
-      <c r="AE1" s="673"/>
-      <c r="AF1" s="674" t="s">
+      <c r="AD1" s="669"/>
+      <c r="AE1" s="670"/>
+      <c r="AF1" s="671" t="s">
         <v>298</v>
       </c>
-      <c r="AG1" s="675"/>
-      <c r="AH1" s="676"/>
-      <c r="AI1" s="666" t="s">
+      <c r="AG1" s="672"/>
+      <c r="AH1" s="673"/>
+      <c r="AI1" s="663" t="s">
         <v>462</v>
       </c>
-      <c r="AJ1" s="667"/>
-      <c r="AK1" s="668"/>
+      <c r="AJ1" s="664"/>
+      <c r="AK1" s="665"/>
       <c r="AN1" s="142"/>
     </row>
     <row r="2" spans="1:40" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="F2" s="22" t="s">
         <v>44</v>
       </c>
-      <c r="H2" s="544">
+      <c r="H2" s="543">
         <f>SUM(H4:H37)</f>
         <v>-8</v>
       </c>
@@ -9471,19 +9484,19 @@
       <c r="K2" s="327">
         <v>-3</v>
       </c>
-      <c r="L2" s="677">
+      <c r="L2" s="674">
         <f>SUM(L5:L30)</f>
-        <v>1</v>
-      </c>
-      <c r="M2" s="679">
+        <v>2</v>
+      </c>
+      <c r="M2" s="676">
         <f>SUM(M4:M29)</f>
         <v>6</v>
       </c>
-      <c r="N2" s="681">
+      <c r="N2" s="678">
         <f>SUM(N4:N29)</f>
         <v>5</v>
       </c>
-      <c r="O2" s="645">
+      <c r="O2" s="618">
         <f>SUM(M30:M37)* (-1)</f>
         <v>-1</v>
       </c>
@@ -9496,19 +9509,19 @@
       <c r="R2" s="2" t="s">
         <v>205</v>
       </c>
-      <c r="S2" s="517" t="s">
+      <c r="S2" s="516" t="s">
         <v>267</v>
       </c>
-      <c r="T2" s="518" t="s">
+      <c r="T2" s="517" t="s">
         <v>221</v>
       </c>
-      <c r="U2" s="683" t="s">
+      <c r="U2" s="680" t="s">
         <v>239</v>
       </c>
-      <c r="V2" s="519" t="s">
+      <c r="V2" s="518" t="s">
         <v>456</v>
       </c>
-      <c r="W2" s="517" t="s">
+      <c r="W2" s="516" t="s">
         <v>258</v>
       </c>
       <c r="X2" s="61" t="s">
@@ -9569,12 +9582,12 @@
       </c>
       <c r="K3" s="319">
         <f>T3+V3+W3+S3</f>
-        <v>69</v>
-      </c>
-      <c r="L3" s="678"/>
-      <c r="M3" s="680"/>
-      <c r="N3" s="682"/>
-      <c r="O3" s="646"/>
+        <v>68</v>
+      </c>
+      <c r="L3" s="675"/>
+      <c r="M3" s="677"/>
+      <c r="N3" s="679"/>
+      <c r="O3" s="619"/>
       <c r="P3" s="176">
         <f>(L2+M2)-W3</f>
         <v>0</v>
@@ -9582,22 +9595,22 @@
       <c r="R3" s="161" t="s">
         <v>249</v>
       </c>
-      <c r="S3" s="520">
+      <c r="S3" s="519">
         <f>SUM(S4:S29)</f>
         <v>12</v>
       </c>
-      <c r="T3" s="521">
+      <c r="T3" s="520">
         <f>SUM(T4:T29)</f>
         <v>42</v>
       </c>
-      <c r="U3" s="684"/>
-      <c r="V3" s="522">
+      <c r="U3" s="681"/>
+      <c r="V3" s="521">
         <f t="shared" ref="V3:AA3" si="0">SUM(V4:V29)</f>
+        <v>6</v>
+      </c>
+      <c r="W3" s="521">
+        <f t="shared" si="0"/>
         <v>8</v>
-      </c>
-      <c r="W3" s="522">
-        <f t="shared" si="0"/>
-        <v>7</v>
       </c>
       <c r="X3" s="59">
         <f t="shared" si="0"/>
@@ -9609,7 +9622,7 @@
       </c>
       <c r="Z3" s="66">
         <f t="shared" si="0"/>
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="AA3" s="66">
         <f t="shared" si="0"/>
@@ -9689,7 +9702,7 @@
         <f>AA4</f>
         <v>0</v>
       </c>
-      <c r="O4" s="663" t="s">
+      <c r="O4" s="682" t="s">
         <v>200</v>
       </c>
       <c r="P4" s="20"/>
@@ -9699,15 +9712,15 @@
       <c r="R4" s="320" t="s">
         <v>204</v>
       </c>
-      <c r="S4" s="523"/>
-      <c r="T4" s="524">
+      <c r="S4" s="522"/>
+      <c r="T4" s="523">
         <v>2</v>
       </c>
-      <c r="U4" s="525">
+      <c r="U4" s="524">
         <v>-2</v>
       </c>
-      <c r="V4" s="526"/>
-      <c r="W4" s="527">
+      <c r="V4" s="525"/>
+      <c r="W4" s="526">
         <f t="shared" ref="W4:W37" si="2">SUM(L4:M4)</f>
         <v>0</v>
       </c>
@@ -9750,7 +9763,7 @@
         <f>IF((AI4-AJ4)&gt;AJ4,(AI4-AJ4),AJ4)</f>
         <v>0</v>
       </c>
-      <c r="AL4" s="545" t="s">
+      <c r="AL4" s="544" t="s">
         <v>204</v>
       </c>
       <c r="AM4" s="320"/>
@@ -9768,7 +9781,7 @@
         <f>AA5</f>
         <v>0</v>
       </c>
-      <c r="O5" s="664"/>
+      <c r="O5" s="683"/>
       <c r="P5" s="20"/>
       <c r="Q5" s="2" t="s">
         <v>347</v>
@@ -9776,15 +9789,15 @@
       <c r="R5" s="321" t="s">
         <v>244</v>
       </c>
-      <c r="S5" s="528"/>
-      <c r="T5" s="529">
+      <c r="S5" s="527"/>
+      <c r="T5" s="528">
         <v>2</v>
       </c>
-      <c r="U5" s="530">
+      <c r="U5" s="529">
         <v>-2</v>
       </c>
-      <c r="V5" s="531"/>
-      <c r="W5" s="527">
+      <c r="V5" s="530"/>
+      <c r="W5" s="526">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
@@ -9856,26 +9869,26 @@
         <f>AA6</f>
         <v>0</v>
       </c>
-      <c r="O6" s="664"/>
+      <c r="O6" s="683"/>
       <c r="P6" s="19" t="s">
         <v>342</v>
       </c>
       <c r="R6" s="321" t="s">
         <v>231</v>
       </c>
-      <c r="S6" s="532">
+      <c r="S6" s="531">
         <v>2</v>
       </c>
-      <c r="T6" s="533">
+      <c r="T6" s="532">
         <v>2</v>
       </c>
-      <c r="U6" s="530">
+      <c r="U6" s="529">
         <v>-2</v>
       </c>
-      <c r="V6" s="534">
+      <c r="V6" s="533">
         <v>2</v>
       </c>
-      <c r="W6" s="527">
+      <c r="W6" s="526">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
@@ -9948,7 +9961,7 @@
         <f t="shared" ref="N7:N37" si="10">AA7</f>
         <v>0</v>
       </c>
-      <c r="O7" s="664"/>
+      <c r="O7" s="683"/>
       <c r="P7" s="20"/>
       <c r="Q7" s="2" t="s">
         <v>342</v>
@@ -9956,19 +9969,19 @@
       <c r="R7" s="321" t="s">
         <v>245</v>
       </c>
-      <c r="S7" s="535">
-        <v>1</v>
-      </c>
-      <c r="T7" s="536">
+      <c r="S7" s="534">
+        <v>1</v>
+      </c>
+      <c r="T7" s="535">
         <v>2</v>
       </c>
-      <c r="U7" s="537">
+      <c r="U7" s="536">
         <v>-2</v>
       </c>
-      <c r="V7" s="534">
+      <c r="V7" s="533">
         <v>2</v>
       </c>
-      <c r="W7" s="527">
+      <c r="W7" s="526">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
@@ -10054,7 +10067,7 @@
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
-      <c r="O8" s="664"/>
+      <c r="O8" s="683"/>
       <c r="P8" s="21" t="s">
         <v>238</v>
       </c>
@@ -10064,7 +10077,7 @@
       <c r="R8" s="322" t="s">
         <v>202</v>
       </c>
-      <c r="S8" s="538">
+      <c r="S8" s="537">
         <v>0</v>
       </c>
       <c r="T8" s="26">
@@ -10074,10 +10087,10 @@
         <f>T3</f>
         <v>42</v>
       </c>
-      <c r="V8" s="534">
-        <v>0</v>
-      </c>
-      <c r="W8" s="527">
+      <c r="V8" s="533">
+        <v>0</v>
+      </c>
+      <c r="W8" s="526">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
@@ -10138,22 +10151,22 @@
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
-      <c r="O9" s="664"/>
+      <c r="O9" s="683"/>
       <c r="P9" s="21" t="s">
         <v>342</v>
       </c>
       <c r="R9" s="322" t="s">
         <v>264</v>
       </c>
-      <c r="S9" s="539"/>
-      <c r="T9" s="540">
+      <c r="S9" s="538"/>
+      <c r="T9" s="539">
         <v>2</v>
       </c>
-      <c r="U9" s="525">
+      <c r="U9" s="524">
         <v>-2</v>
       </c>
-      <c r="V9" s="541"/>
-      <c r="W9" s="527">
+      <c r="V9" s="540"/>
+      <c r="W9" s="526">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
@@ -10234,7 +10247,7 @@
         <f t="shared" si="10"/>
         <v>1</v>
       </c>
-      <c r="O10" s="664"/>
+      <c r="O10" s="683"/>
       <c r="P10" s="20"/>
       <c r="Q10" s="2" t="s">
         <v>347</v>
@@ -10242,17 +10255,17 @@
       <c r="R10" s="321" t="s">
         <v>74</v>
       </c>
-      <c r="S10" s="542">
-        <v>0</v>
-      </c>
-      <c r="T10" s="529">
-        <v>1</v>
-      </c>
-      <c r="U10" s="530">
+      <c r="S10" s="541">
+        <v>0</v>
+      </c>
+      <c r="T10" s="528">
+        <v>1</v>
+      </c>
+      <c r="U10" s="529">
         <v>-2</v>
       </c>
-      <c r="V10" s="533"/>
-      <c r="W10" s="527">
+      <c r="V10" s="532"/>
+      <c r="W10" s="526">
         <f t="shared" si="2"/>
         <v>2</v>
       </c>
@@ -10315,7 +10328,7 @@
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
-      <c r="O11" s="664"/>
+      <c r="O11" s="683"/>
       <c r="P11" s="21" t="s">
         <v>342</v>
       </c>
@@ -10323,15 +10336,15 @@
       <c r="R11" s="321" t="s">
         <v>241</v>
       </c>
-      <c r="S11" s="542"/>
-      <c r="T11" s="529">
+      <c r="S11" s="541"/>
+      <c r="T11" s="528">
         <v>2</v>
       </c>
-      <c r="U11" s="530">
+      <c r="U11" s="529">
         <v>-2</v>
       </c>
-      <c r="V11" s="533"/>
-      <c r="W11" s="527">
+      <c r="V11" s="532"/>
+      <c r="W11" s="526">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
@@ -10375,7 +10388,7 @@
       <c r="AN11" s="142"/>
     </row>
     <row r="12" spans="1:40" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="609" t="s">
+      <c r="A12" s="654" t="s">
         <v>55</v>
       </c>
       <c r="B12" s="30">
@@ -10384,11 +10397,11 @@
       <c r="C12" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="E12" s="660" t="s">
+      <c r="E12" s="608" t="s">
         <v>57</v>
       </c>
       <c r="G12" s="267"/>
-      <c r="H12" s="512"/>
+      <c r="H12" s="511"/>
       <c r="I12" s="61" t="s">
         <v>568</v>
       </c>
@@ -10403,7 +10416,7 @@
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
-      <c r="O12" s="664"/>
+      <c r="O12" s="683"/>
       <c r="P12" s="21" t="s">
         <v>342</v>
       </c>
@@ -10411,15 +10424,15 @@
       <c r="R12" s="321" t="s">
         <v>240</v>
       </c>
-      <c r="S12" s="542"/>
-      <c r="T12" s="529">
+      <c r="S12" s="541"/>
+      <c r="T12" s="528">
         <v>2</v>
       </c>
-      <c r="U12" s="530">
+      <c r="U12" s="529">
         <v>-2</v>
       </c>
-      <c r="V12" s="533"/>
-      <c r="W12" s="527">
+      <c r="V12" s="532"/>
+      <c r="W12" s="526">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
@@ -10471,14 +10484,14 @@
       </c>
     </row>
     <row r="13" spans="1:40" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="611"/>
+      <c r="A13" s="656"/>
       <c r="B13" s="153">
         <v>12</v>
       </c>
       <c r="C13" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="E13" s="661"/>
+      <c r="E13" s="609"/>
       <c r="F13" s="176">
         <v>0</v>
       </c>
@@ -10501,7 +10514,7 @@
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
-      <c r="O13" s="664"/>
+      <c r="O13" s="683"/>
       <c r="P13" s="21" t="s">
         <v>342</v>
       </c>
@@ -10509,15 +10522,15 @@
       <c r="R13" s="321" t="s">
         <v>234</v>
       </c>
-      <c r="S13" s="542"/>
-      <c r="T13" s="529">
+      <c r="S13" s="541"/>
+      <c r="T13" s="528">
         <v>2</v>
       </c>
-      <c r="U13" s="530">
+      <c r="U13" s="529">
         <v>-2</v>
       </c>
-      <c r="V13" s="533"/>
-      <c r="W13" s="527">
+      <c r="V13" s="532"/>
+      <c r="W13" s="526">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
@@ -10574,7 +10587,7 @@
         <f t="shared" si="10"/>
         <v>1</v>
       </c>
-      <c r="O14" s="664"/>
+      <c r="O14" s="683"/>
       <c r="P14" s="20"/>
       <c r="Q14" s="205" t="s">
         <v>346</v>
@@ -10582,15 +10595,15 @@
       <c r="R14" s="321" t="s">
         <v>246</v>
       </c>
-      <c r="S14" s="542"/>
-      <c r="T14" s="529">
-        <v>0</v>
-      </c>
-      <c r="U14" s="530">
+      <c r="S14" s="541"/>
+      <c r="T14" s="528">
+        <v>0</v>
+      </c>
+      <c r="U14" s="529">
         <v>-1</v>
       </c>
-      <c r="V14" s="533"/>
-      <c r="W14" s="527">
+      <c r="V14" s="532"/>
+      <c r="W14" s="526">
         <f t="shared" si="2"/>
         <v>1</v>
       </c>
@@ -10638,7 +10651,7 @@
       <c r="AL14" s="6" t="s">
         <v>584</v>
       </c>
-      <c r="AM14" s="546" t="s">
+      <c r="AM14" s="545" t="s">
         <v>587</v>
       </c>
       <c r="AN14" s="142" t="s">
@@ -10655,7 +10668,7 @@
       <c r="G15" s="266" t="s">
         <v>44</v>
       </c>
-      <c r="H15" s="514">
+      <c r="H15" s="513">
         <v>-1</v>
       </c>
       <c r="I15" s="277"/>
@@ -10671,7 +10684,7 @@
         <f t="shared" si="10"/>
         <v>1</v>
       </c>
-      <c r="O15" s="664"/>
+      <c r="O15" s="683"/>
       <c r="P15" s="20"/>
       <c r="Q15" s="205" t="s">
         <v>346</v>
@@ -10679,15 +10692,15 @@
       <c r="R15" s="321" t="s">
         <v>232</v>
       </c>
-      <c r="S15" s="542"/>
-      <c r="T15" s="529">
-        <v>1</v>
-      </c>
-      <c r="U15" s="530">
+      <c r="S15" s="541"/>
+      <c r="T15" s="528">
+        <v>1</v>
+      </c>
+      <c r="U15" s="529">
         <v>-2</v>
       </c>
-      <c r="V15" s="541"/>
-      <c r="W15" s="527">
+      <c r="V15" s="540"/>
+      <c r="W15" s="526">
         <f t="shared" si="2"/>
         <v>1</v>
       </c>
@@ -10758,7 +10771,7 @@
         <f t="shared" si="10"/>
         <v>1</v>
       </c>
-      <c r="O16" s="664"/>
+      <c r="O16" s="683"/>
       <c r="P16" s="21" t="s">
         <v>342</v>
       </c>
@@ -10768,15 +10781,15 @@
       <c r="R16" s="321" t="s">
         <v>235</v>
       </c>
-      <c r="S16" s="542"/>
-      <c r="T16" s="529">
+      <c r="S16" s="541"/>
+      <c r="T16" s="528">
         <v>2</v>
       </c>
-      <c r="U16" s="530">
+      <c r="U16" s="529">
         <v>-3</v>
       </c>
-      <c r="V16" s="541"/>
-      <c r="W16" s="527">
+      <c r="V16" s="540"/>
+      <c r="W16" s="526">
         <f t="shared" si="2"/>
         <v>1</v>
       </c>
@@ -10826,7 +10839,7 @@
       <c r="AL16" s="6" t="s">
         <v>235</v>
       </c>
-      <c r="AM16" s="547" t="s">
+      <c r="AM16" s="546" t="s">
         <v>579</v>
       </c>
       <c r="AN16" s="107" t="s">
@@ -10854,7 +10867,7 @@
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
-      <c r="O17" s="664"/>
+      <c r="O17" s="683"/>
       <c r="P17" s="20"/>
       <c r="Q17" s="2" t="s">
         <v>348</v>
@@ -10862,17 +10875,17 @@
       <c r="R17" s="321" t="s">
         <v>97</v>
       </c>
-      <c r="S17" s="542">
-        <v>1</v>
-      </c>
-      <c r="T17" s="529">
-        <v>1</v>
-      </c>
-      <c r="U17" s="530">
+      <c r="S17" s="541">
+        <v>1</v>
+      </c>
+      <c r="T17" s="528">
+        <v>1</v>
+      </c>
+      <c r="U17" s="529">
         <v>-1</v>
       </c>
-      <c r="V17" s="533"/>
-      <c r="W17" s="527">
+      <c r="V17" s="532"/>
+      <c r="W17" s="526">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
@@ -10911,7 +10924,7 @@
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
-      <c r="AM17" s="506"/>
+      <c r="AM17" s="505"/>
       <c r="AN17" s="142"/>
     </row>
     <row r="18" spans="1:40" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -10938,7 +10951,7 @@
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
-      <c r="O18" s="664"/>
+      <c r="O18" s="683"/>
       <c r="P18" s="21" t="s">
         <v>342</v>
       </c>
@@ -10946,15 +10959,15 @@
       <c r="R18" s="321" t="s">
         <v>248</v>
       </c>
-      <c r="S18" s="542"/>
-      <c r="T18" s="529">
+      <c r="S18" s="541"/>
+      <c r="T18" s="528">
         <v>3</v>
       </c>
-      <c r="U18" s="530">
+      <c r="U18" s="529">
         <v>-3</v>
       </c>
-      <c r="V18" s="531"/>
-      <c r="W18" s="527">
+      <c r="V18" s="530"/>
+      <c r="W18" s="526">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
@@ -10998,7 +11011,7 @@
         <v>0</v>
       </c>
       <c r="AL18" s="6"/>
-      <c r="AM18" s="506"/>
+      <c r="AM18" s="505"/>
       <c r="AN18" s="142"/>
     </row>
     <row r="19" spans="1:40" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -11021,7 +11034,7 @@
         <f t="shared" si="10"/>
         <v>1</v>
       </c>
-      <c r="O19" s="664"/>
+      <c r="O19" s="683"/>
       <c r="P19" s="20"/>
       <c r="Q19" s="2" t="s">
         <v>341</v>
@@ -11029,17 +11042,17 @@
       <c r="R19" s="321" t="s">
         <v>247</v>
       </c>
-      <c r="S19" s="542"/>
-      <c r="T19" s="529">
-        <v>1</v>
-      </c>
-      <c r="U19" s="530">
+      <c r="S19" s="541"/>
+      <c r="T19" s="528">
+        <v>1</v>
+      </c>
+      <c r="U19" s="529">
         <v>-1</v>
       </c>
-      <c r="V19" s="532">
-        <v>2</v>
-      </c>
-      <c r="W19" s="527">
+      <c r="V19" s="531">
+        <v>1</v>
+      </c>
+      <c r="W19" s="526">
         <f t="shared" si="2"/>
         <v>1</v>
       </c>
@@ -11117,23 +11130,23 @@
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
-      <c r="O20" s="665"/>
+      <c r="O20" s="684"/>
       <c r="P20" s="559" t="s">
         <v>342</v>
       </c>
-      <c r="Q20" s="662"/>
+      <c r="Q20" s="610"/>
       <c r="R20" s="321" t="s">
         <v>86</v>
       </c>
-      <c r="S20" s="542"/>
-      <c r="T20" s="529">
+      <c r="S20" s="541"/>
+      <c r="T20" s="528">
         <v>3</v>
       </c>
-      <c r="U20" s="530">
+      <c r="U20" s="529">
         <v>-3</v>
       </c>
-      <c r="V20" s="543"/>
-      <c r="W20" s="527">
+      <c r="V20" s="542"/>
+      <c r="W20" s="526">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
@@ -11217,17 +11230,17 @@
       <c r="R21" s="321" t="s">
         <v>250</v>
       </c>
-      <c r="S21" s="542">
-        <v>1</v>
-      </c>
-      <c r="T21" s="529">
-        <v>1</v>
-      </c>
-      <c r="U21" s="530">
+      <c r="S21" s="541">
+        <v>1</v>
+      </c>
+      <c r="T21" s="528">
+        <v>1</v>
+      </c>
+      <c r="U21" s="529">
         <v>-1</v>
       </c>
-      <c r="V21" s="531"/>
-      <c r="W21" s="527">
+      <c r="V21" s="530"/>
+      <c r="W21" s="526">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
@@ -11300,15 +11313,15 @@
       <c r="R22" s="321" t="s">
         <v>265</v>
       </c>
-      <c r="S22" s="542"/>
-      <c r="T22" s="529">
+      <c r="S22" s="541"/>
+      <c r="T22" s="528">
         <v>2</v>
       </c>
-      <c r="U22" s="530">
+      <c r="U22" s="529">
         <v>-2</v>
       </c>
-      <c r="V22" s="543"/>
-      <c r="W22" s="527">
+      <c r="V22" s="542"/>
+      <c r="W22" s="526">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
@@ -11352,19 +11365,22 @@
         <v>0</v>
       </c>
       <c r="AL22" s="16"/>
-      <c r="AM22" s="506"/>
+      <c r="AM22" s="505"/>
       <c r="AN22" s="142"/>
     </row>
     <row r="23" spans="1:40" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E23" s="616" t="s">
+      <c r="E23" s="661" t="s">
         <v>294</v>
       </c>
       <c r="F23" s="184"/>
+      <c r="H23" s="274">
+        <v>-1</v>
+      </c>
       <c r="K23" s="403" t="s">
         <v>263</v>
       </c>
       <c r="L23" s="336">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M23" s="107">
         <v>1</v>
@@ -11377,19 +11393,19 @@
       <c r="R23" s="321" t="s">
         <v>252</v>
       </c>
-      <c r="S23" s="542"/>
-      <c r="T23" s="529">
-        <v>0</v>
-      </c>
-      <c r="U23" s="530">
+      <c r="S23" s="541"/>
+      <c r="T23" s="528">
+        <v>0</v>
+      </c>
+      <c r="U23" s="529">
         <v>-1</v>
       </c>
-      <c r="V23" s="534">
-        <v>1</v>
-      </c>
-      <c r="W23" s="527">
+      <c r="V23" s="533">
+        <v>0</v>
+      </c>
+      <c r="W23" s="526">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="X23" s="302"/>
       <c r="Y23" s="117">
@@ -11398,7 +11414,7 @@
       </c>
       <c r="Z23" s="296">
         <f t="shared" si="6"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AA23" s="296">
         <v>0</v>
@@ -11446,7 +11462,7 @@
       <c r="C24" s="2" t="s">
         <v>260</v>
       </c>
-      <c r="E24" s="617"/>
+      <c r="E24" s="662"/>
       <c r="F24" s="176"/>
       <c r="K24" s="403" t="s">
         <v>301</v>
@@ -11464,21 +11480,21 @@
       <c r="P24" s="559" t="s">
         <v>342</v>
       </c>
-      <c r="Q24" s="662"/>
+      <c r="Q24" s="610"/>
       <c r="R24" s="321" t="s">
         <v>254</v>
       </c>
-      <c r="S24" s="542">
+      <c r="S24" s="541">
         <v>2</v>
       </c>
-      <c r="T24" s="529">
+      <c r="T24" s="528">
         <v>2</v>
       </c>
-      <c r="U24" s="530">
+      <c r="U24" s="529">
         <v>-2</v>
       </c>
-      <c r="V24" s="541"/>
-      <c r="W24" s="527">
+      <c r="V24" s="540"/>
+      <c r="W24" s="526">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
@@ -11554,17 +11570,17 @@
       <c r="R25" s="321" t="s">
         <v>255</v>
       </c>
-      <c r="S25" s="542">
+      <c r="S25" s="541">
         <v>2</v>
       </c>
-      <c r="T25" s="529">
+      <c r="T25" s="528">
         <v>2</v>
       </c>
-      <c r="U25" s="530">
+      <c r="U25" s="529">
         <v>-2</v>
       </c>
-      <c r="V25" s="543"/>
-      <c r="W25" s="527">
+      <c r="V25" s="542"/>
+      <c r="W25" s="526">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
@@ -11639,19 +11655,19 @@
       <c r="R26" s="321" t="s">
         <v>256</v>
       </c>
-      <c r="S26" s="542">
-        <v>1</v>
-      </c>
-      <c r="T26" s="529">
-        <v>1</v>
-      </c>
-      <c r="U26" s="530">
+      <c r="S26" s="541">
+        <v>1</v>
+      </c>
+      <c r="T26" s="528">
+        <v>1</v>
+      </c>
+      <c r="U26" s="529">
         <v>-2</v>
       </c>
-      <c r="V26" s="534">
-        <v>1</v>
-      </c>
-      <c r="W26" s="527">
+      <c r="V26" s="533">
+        <v>1</v>
+      </c>
+      <c r="W26" s="526">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
@@ -11722,17 +11738,17 @@
       <c r="R27" s="321" t="s">
         <v>257</v>
       </c>
-      <c r="S27" s="542">
+      <c r="S27" s="541">
         <v>2</v>
       </c>
-      <c r="T27" s="529">
+      <c r="T27" s="528">
         <v>2</v>
       </c>
-      <c r="U27" s="530">
+      <c r="U27" s="529">
         <v>-2</v>
       </c>
-      <c r="V27" s="541"/>
-      <c r="W27" s="527">
+      <c r="V27" s="540"/>
+      <c r="W27" s="526">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
@@ -11772,7 +11788,7 @@
         <v>0</v>
       </c>
       <c r="AL27" s="16"/>
-      <c r="AM27" s="506"/>
+      <c r="AM27" s="505"/>
       <c r="AN27" s="142"/>
     </row>
     <row r="28" spans="1:40" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -11791,15 +11807,15 @@
       <c r="R28" s="321" t="s">
         <v>253</v>
       </c>
-      <c r="S28" s="542"/>
-      <c r="T28" s="529">
-        <v>1</v>
-      </c>
-      <c r="U28" s="530">
+      <c r="S28" s="541"/>
+      <c r="T28" s="528">
+        <v>1</v>
+      </c>
+      <c r="U28" s="529">
         <v>-1</v>
       </c>
-      <c r="V28" s="541"/>
-      <c r="W28" s="527">
+      <c r="V28" s="540"/>
+      <c r="W28" s="526">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
@@ -11838,7 +11854,7 @@
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
-      <c r="AM28" s="506"/>
+      <c r="AM28" s="505"/>
       <c r="AN28" s="142"/>
     </row>
     <row r="29" spans="1:40" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -11867,15 +11883,15 @@
       <c r="R29" s="323" t="s">
         <v>266</v>
       </c>
-      <c r="S29" s="528"/>
-      <c r="T29" s="536">
+      <c r="S29" s="527"/>
+      <c r="T29" s="535">
         <v>2</v>
       </c>
-      <c r="U29" s="537">
+      <c r="U29" s="536">
         <v>-2</v>
       </c>
-      <c r="V29" s="531"/>
-      <c r="W29" s="527">
+      <c r="V29" s="530"/>
+      <c r="W29" s="526">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
@@ -11918,7 +11934,7 @@
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
-      <c r="AM29" s="506"/>
+      <c r="AM29" s="505"/>
       <c r="AN29" s="142"/>
     </row>
     <row r="30" spans="1:40" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -11978,7 +11994,7 @@
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
-      <c r="AM30" s="506"/>
+      <c r="AM30" s="505"/>
       <c r="AN30" s="142"/>
     </row>
     <row r="31" spans="1:40" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -11992,7 +12008,7 @@
         <v>-1</v>
       </c>
       <c r="H31" s="42">
-        <v>-3</v>
+        <v>-2</v>
       </c>
       <c r="I31" s="21" t="s">
         <v>436</v>
@@ -12049,11 +12065,11 @@
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
-      <c r="AM31" s="506"/>
+      <c r="AM31" s="505"/>
       <c r="AN31" s="142"/>
     </row>
     <row r="32" spans="1:40" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="H32" s="737">
+      <c r="H32" s="548">
         <v>-1</v>
       </c>
       <c r="I32" s="221" t="s">
@@ -12118,7 +12134,9 @@
       <c r="AG32" s="348">
         <v>0</v>
       </c>
-      <c r="AH32" s="326"/>
+      <c r="AH32" s="326">
+        <v>1</v>
+      </c>
       <c r="AI32" s="347">
         <f t="shared" si="7"/>
         <v>1</v>
@@ -12142,7 +12160,7 @@
       </c>
     </row>
     <row r="33" spans="3:40" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="G33" s="513"/>
+      <c r="G33" s="512"/>
       <c r="H33" s="42">
         <v>-1</v>
       </c>
@@ -12202,7 +12220,7 @@
         <v>0</v>
       </c>
       <c r="AL33" s="6"/>
-      <c r="AM33" s="506"/>
+      <c r="AM33" s="505"/>
       <c r="AN33" s="142"/>
     </row>
     <row r="34" spans="3:40" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -12347,7 +12365,7 @@
         <v>0</v>
       </c>
       <c r="AG35" s="348"/>
-      <c r="AH35" s="515">
+      <c r="AH35" s="514">
         <v>0</v>
       </c>
       <c r="AI35" s="347">
@@ -12443,13 +12461,13 @@
       <c r="AL36" s="6" t="s">
         <v>313</v>
       </c>
-      <c r="AM36" s="506"/>
+      <c r="AM36" s="505"/>
       <c r="AN36" s="142" t="s">
         <v>591</v>
       </c>
     </row>
     <row r="37" spans="3:40" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="H37" s="544">
+      <c r="H37" s="543">
         <v>-1</v>
       </c>
       <c r="K37" s="407"/>
@@ -12525,7 +12543,7 @@
       <c r="AL37" s="6" t="s">
         <v>486</v>
       </c>
-      <c r="AM37" s="548" t="s">
+      <c r="AM37" s="547" t="s">
         <v>589</v>
       </c>
       <c r="AN37" s="107" t="s">
@@ -12534,6 +12552,12 @@
     </row>
   </sheetData>
   <mergeCells count="15">
+    <mergeCell ref="A12:A13"/>
+    <mergeCell ref="E12:E13"/>
+    <mergeCell ref="P20:Q20"/>
+    <mergeCell ref="E23:E24"/>
+    <mergeCell ref="P24:Q24"/>
+    <mergeCell ref="O4:O20"/>
     <mergeCell ref="AI1:AK1"/>
     <mergeCell ref="V1:W1"/>
     <mergeCell ref="AC1:AE1"/>
@@ -12543,12 +12567,6 @@
     <mergeCell ref="N2:N3"/>
     <mergeCell ref="O2:O3"/>
     <mergeCell ref="U2:U3"/>
-    <mergeCell ref="A12:A13"/>
-    <mergeCell ref="E12:E13"/>
-    <mergeCell ref="P20:Q20"/>
-    <mergeCell ref="E23:E24"/>
-    <mergeCell ref="P24:Q24"/>
-    <mergeCell ref="O4:O20"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -12585,12 +12603,12 @@
       <c r="B1" s="559" t="s">
         <v>317</v>
       </c>
-      <c r="C1" s="662"/>
+      <c r="C1" s="610"/>
       <c r="D1" s="209"/>
       <c r="J1" s="559" t="s">
         <v>70</v>
       </c>
-      <c r="K1" s="662"/>
+      <c r="K1" s="610"/>
       <c r="L1" s="200" t="s">
         <v>337</v>
       </c>
@@ -12981,7 +12999,7 @@
       <c r="V1" s="559" t="s">
         <v>71</v>
       </c>
-      <c r="W1" s="662"/>
+      <c r="W1" s="610"/>
       <c r="X1" s="62" t="s">
         <v>102</v>
       </c>
@@ -13000,7 +13018,7 @@
       <c r="AC1" s="116" t="s">
         <v>191</v>
       </c>
-      <c r="AD1" s="705" t="s">
+      <c r="AD1" s="698" t="s">
         <v>213</v>
       </c>
       <c r="AE1" s="116" t="s">
@@ -13017,10 +13035,10 @@
       <c r="E2" s="39" t="s">
         <v>74</v>
       </c>
-      <c r="F2" s="736" t="s">
+      <c r="F2" s="697" t="s">
         <v>75</v>
       </c>
-      <c r="G2" s="693" t="s">
+      <c r="G2" s="725" t="s">
         <v>44</v>
       </c>
       <c r="H2" s="40" t="s">
@@ -13048,10 +13066,10 @@
       <c r="U2" s="60" t="s">
         <v>106</v>
       </c>
-      <c r="V2" s="669" t="s">
+      <c r="V2" s="666" t="s">
         <v>121</v>
       </c>
-      <c r="W2" s="670"/>
+      <c r="W2" s="667"/>
       <c r="X2" s="64" t="s">
         <v>110</v>
       </c>
@@ -13070,7 +13088,7 @@
       <c r="AC2" s="117" t="s">
         <v>99</v>
       </c>
-      <c r="AD2" s="706"/>
+      <c r="AD2" s="699"/>
       <c r="AE2" s="64" t="s">
         <v>99</v>
       </c>
@@ -13089,8 +13107,8 @@
       <c r="E3" s="39" t="s">
         <v>80</v>
       </c>
-      <c r="F3" s="613"/>
-      <c r="G3" s="694"/>
+      <c r="F3" s="658"/>
+      <c r="G3" s="726"/>
       <c r="H3" s="40" t="s">
         <v>81</v>
       </c>
@@ -13101,13 +13119,13 @@
         <v>82</v>
       </c>
       <c r="N3" s="44"/>
-      <c r="O3" s="703" t="s">
+      <c r="O3" s="735" t="s">
         <v>44</v>
       </c>
-      <c r="P3" s="724" t="s">
+      <c r="P3" s="717" t="s">
         <v>219</v>
       </c>
-      <c r="Q3" s="725"/>
+      <c r="Q3" s="718"/>
       <c r="S3" s="57" t="s">
         <v>220</v>
       </c>
@@ -13117,15 +13135,15 @@
       <c r="W3" s="59" t="s">
         <v>105</v>
       </c>
-      <c r="AD3" s="706"/>
+      <c r="AD3" s="699"/>
     </row>
     <row r="4" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="G4" s="694"/>
+      <c r="G4" s="726"/>
       <c r="H4" s="6"/>
       <c r="L4" s="688" t="s">
         <v>83</v>
       </c>
-      <c r="O4" s="704"/>
+      <c r="O4" s="736"/>
       <c r="T4" s="55" t="s">
         <v>98</v>
       </c>
@@ -13139,8 +13157,8 @@
         <v>195</v>
       </c>
       <c r="Z4" s="561"/>
-      <c r="AA4" s="662"/>
-      <c r="AD4" s="706"/>
+      <c r="AA4" s="610"/>
+      <c r="AD4" s="699"/>
     </row>
     <row r="5" spans="1:31" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C5" s="52" t="s">
@@ -13155,21 +13173,21 @@
       <c r="F5" s="66" t="s">
         <v>85</v>
       </c>
-      <c r="G5" s="694"/>
+      <c r="G5" s="726"/>
       <c r="H5" s="46" t="s">
         <v>76</v>
       </c>
-      <c r="K5" s="711" t="s">
+      <c r="K5" s="704" t="s">
         <v>217</v>
       </c>
-      <c r="L5" s="726"/>
+      <c r="L5" s="719"/>
       <c r="M5" s="2" t="s">
         <v>215</v>
       </c>
       <c r="N5" s="61" t="s">
         <v>214</v>
       </c>
-      <c r="O5" s="704"/>
+      <c r="O5" s="736"/>
       <c r="P5" s="108" t="s">
         <v>216</v>
       </c>
@@ -13185,11 +13203,11 @@
       <c r="U5" s="19" t="s">
         <v>99</v>
       </c>
-      <c r="Y5" s="714" t="s">
+      <c r="Y5" s="707" t="s">
         <v>287</v>
       </c>
-      <c r="Z5" s="715"/>
-      <c r="AD5" s="706"/>
+      <c r="Z5" s="708"/>
+      <c r="AD5" s="699"/>
     </row>
     <row r="6" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C6" s="109"/>
@@ -13199,16 +13217,16 @@
       <c r="E6" s="45" t="s">
         <v>86</v>
       </c>
-      <c r="G6" s="694"/>
+      <c r="G6" s="726"/>
       <c r="H6" s="46" t="s">
         <v>81</v>
       </c>
       <c r="I6" s="23">
         <v>15</v>
       </c>
-      <c r="K6" s="712"/>
-      <c r="L6" s="726"/>
-      <c r="O6" s="704"/>
+      <c r="K6" s="705"/>
+      <c r="L6" s="719"/>
+      <c r="O6" s="736"/>
       <c r="T6" s="2" t="s">
         <v>101</v>
       </c>
@@ -13218,23 +13236,23 @@
       <c r="V6" s="21">
         <v>-1</v>
       </c>
-      <c r="AD6" s="706"/>
+      <c r="AD6" s="699"/>
     </row>
     <row r="7" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C7" s="110"/>
-      <c r="G7" s="694"/>
+      <c r="G7" s="726"/>
       <c r="H7" s="6"/>
-      <c r="K7" s="712"/>
-      <c r="L7" s="726"/>
+      <c r="K7" s="705"/>
+      <c r="L7" s="719"/>
       <c r="N7" s="21" t="s">
         <v>120</v>
       </c>
-      <c r="O7" s="704"/>
+      <c r="O7" s="736"/>
       <c r="P7" s="73"/>
       <c r="U7" s="104" t="s">
         <v>20</v>
       </c>
-      <c r="AD7" s="706"/>
+      <c r="AD7" s="699"/>
     </row>
     <row r="8" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C8" s="130"/>
@@ -13247,7 +13265,7 @@
       <c r="F8" s="66" t="s">
         <v>87</v>
       </c>
-      <c r="G8" s="694"/>
+      <c r="G8" s="726"/>
       <c r="H8" s="50" t="s">
         <v>76</v>
       </c>
@@ -13257,41 +13275,41 @@
       <c r="J8" s="111">
         <v>115</v>
       </c>
-      <c r="K8" s="712"/>
-      <c r="L8" s="726"/>
-      <c r="O8" s="704"/>
+      <c r="K8" s="705"/>
+      <c r="L8" s="719"/>
+      <c r="O8" s="736"/>
       <c r="P8" s="49"/>
-      <c r="S8" s="708" t="s">
+      <c r="S8" s="701" t="s">
         <v>212</v>
       </c>
-      <c r="T8" s="709"/>
-      <c r="U8" s="709"/>
-      <c r="V8" s="709"/>
-      <c r="W8" s="709"/>
-      <c r="X8" s="709"/>
-      <c r="Y8" s="709"/>
-      <c r="Z8" s="709"/>
-      <c r="AA8" s="709"/>
-      <c r="AB8" s="709"/>
-      <c r="AC8" s="710"/>
-      <c r="AD8" s="706"/>
+      <c r="T8" s="702"/>
+      <c r="U8" s="702"/>
+      <c r="V8" s="702"/>
+      <c r="W8" s="702"/>
+      <c r="X8" s="702"/>
+      <c r="Y8" s="702"/>
+      <c r="Z8" s="702"/>
+      <c r="AA8" s="702"/>
+      <c r="AB8" s="702"/>
+      <c r="AC8" s="703"/>
+      <c r="AD8" s="699"/>
     </row>
     <row r="9" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C9" s="730"/>
-      <c r="G9" s="694"/>
+      <c r="C9" s="691"/>
+      <c r="G9" s="726"/>
       <c r="H9" s="6"/>
-      <c r="K9" s="712"/>
-      <c r="L9" s="697" t="s">
+      <c r="K9" s="705"/>
+      <c r="L9" s="729" t="s">
         <v>218</v>
       </c>
-      <c r="M9" s="698"/>
-      <c r="N9" s="699"/>
-      <c r="O9" s="704"/>
+      <c r="M9" s="730"/>
+      <c r="N9" s="731"/>
+      <c r="O9" s="736"/>
       <c r="P9" s="75"/>
-      <c r="AD9" s="706"/>
+      <c r="AD9" s="699"/>
     </row>
     <row r="10" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C10" s="731"/>
+      <c r="C10" s="692"/>
       <c r="D10" s="23"/>
       <c r="E10" s="45" t="s">
         <v>88</v>
@@ -13299,7 +13317,7 @@
       <c r="F10" s="66" t="s">
         <v>89</v>
       </c>
-      <c r="G10" s="694"/>
+      <c r="G10" s="726"/>
       <c r="H10" s="51"/>
       <c r="I10" s="21" t="s">
         <v>81</v>
@@ -13307,33 +13325,33 @@
       <c r="J10" s="3">
         <v>15</v>
       </c>
-      <c r="K10" s="712"/>
-      <c r="M10" s="733" t="s">
+      <c r="K10" s="705"/>
+      <c r="M10" s="694" t="s">
         <v>90</v>
       </c>
-      <c r="N10" s="734"/>
-      <c r="O10" s="734"/>
-      <c r="P10" s="734"/>
-      <c r="Q10" s="734"/>
-      <c r="R10" s="734"/>
-      <c r="S10" s="734"/>
-      <c r="T10" s="734"/>
-      <c r="U10" s="734"/>
-      <c r="V10" s="734"/>
-      <c r="W10" s="734"/>
-      <c r="X10" s="734"/>
-      <c r="Y10" s="734"/>
-      <c r="Z10" s="734"/>
-      <c r="AA10" s="734"/>
-      <c r="AB10" s="734"/>
-      <c r="AC10" s="735"/>
-      <c r="AD10" s="706"/>
+      <c r="N10" s="695"/>
+      <c r="O10" s="695"/>
+      <c r="P10" s="695"/>
+      <c r="Q10" s="695"/>
+      <c r="R10" s="695"/>
+      <c r="S10" s="695"/>
+      <c r="T10" s="695"/>
+      <c r="U10" s="695"/>
+      <c r="V10" s="695"/>
+      <c r="W10" s="695"/>
+      <c r="X10" s="695"/>
+      <c r="Y10" s="695"/>
+      <c r="Z10" s="695"/>
+      <c r="AA10" s="695"/>
+      <c r="AB10" s="695"/>
+      <c r="AC10" s="696"/>
+      <c r="AD10" s="699"/>
     </row>
     <row r="11" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C11" s="732"/>
-      <c r="G11" s="694"/>
+      <c r="C11" s="693"/>
+      <c r="G11" s="726"/>
       <c r="H11" s="6"/>
-      <c r="K11" s="712"/>
+      <c r="K11" s="705"/>
       <c r="R11" s="52" t="s">
         <v>44</v>
       </c>
@@ -13341,17 +13359,17 @@
       <c r="Y11" s="68" t="s">
         <v>121</v>
       </c>
-      <c r="Z11" s="722" t="s">
+      <c r="Z11" s="715" t="s">
         <v>121</v>
       </c>
-      <c r="AA11" s="723"/>
+      <c r="AA11" s="716"/>
       <c r="AB11" s="52" t="s">
         <v>44</v>
       </c>
       <c r="AC11" s="118" t="s">
         <v>121</v>
       </c>
-      <c r="AD11" s="706"/>
+      <c r="AD11" s="699"/>
     </row>
     <row r="12" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C12" s="129"/>
@@ -13364,7 +13382,7 @@
       <c r="F12" s="66" t="s">
         <v>92</v>
       </c>
-      <c r="G12" s="694"/>
+      <c r="G12" s="726"/>
       <c r="H12" s="128"/>
       <c r="I12" s="19" t="s">
         <v>81</v>
@@ -13372,8 +13390,8 @@
       <c r="J12" s="3">
         <v>15</v>
       </c>
-      <c r="K12" s="712"/>
-      <c r="L12" s="727" t="s">
+      <c r="K12" s="705"/>
+      <c r="L12" s="720" t="s">
         <v>93</v>
       </c>
       <c r="M12" s="21" t="s">
@@ -13404,25 +13422,25 @@
         <v>116</v>
       </c>
       <c r="Y12" s="6"/>
-      <c r="AA12" s="716" t="s">
+      <c r="AA12" s="709" t="s">
         <v>126</v>
       </c>
-      <c r="AB12" s="717"/>
+      <c r="AB12" s="710"/>
       <c r="AC12" s="21" t="s">
         <v>233</v>
       </c>
-      <c r="AD12" s="706"/>
+      <c r="AD12" s="699"/>
     </row>
     <row r="13" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C13" s="730"/>
-      <c r="G13" s="694"/>
-      <c r="K13" s="712"/>
-      <c r="L13" s="728"/>
+      <c r="C13" s="691"/>
+      <c r="G13" s="726"/>
+      <c r="K13" s="705"/>
+      <c r="L13" s="721"/>
       <c r="M13" s="47"/>
-      <c r="Q13" s="696" t="s">
+      <c r="Q13" s="728" t="s">
         <v>210</v>
       </c>
-      <c r="R13" s="622"/>
+      <c r="R13" s="625"/>
       <c r="S13" s="555"/>
       <c r="T13" s="6"/>
       <c r="U13" s="96" t="s">
@@ -13431,17 +13449,17 @@
       <c r="X13" s="2" t="s">
         <v>123</v>
       </c>
-      <c r="AA13" s="718"/>
-      <c r="AB13" s="719"/>
-      <c r="AD13" s="706"/>
+      <c r="AA13" s="711"/>
+      <c r="AB13" s="712"/>
+      <c r="AD13" s="699"/>
     </row>
     <row r="14" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B14" s="2" t="s">
         <v>339</v>
       </c>
-      <c r="C14" s="732"/>
+      <c r="C14" s="693"/>
       <c r="D14" s="23"/>
-      <c r="G14" s="694"/>
+      <c r="G14" s="726"/>
       <c r="H14" s="125"/>
       <c r="I14" s="99" t="s">
         <v>44</v>
@@ -13449,8 +13467,8 @@
       <c r="J14" s="111">
         <v>115</v>
       </c>
-      <c r="K14" s="712"/>
-      <c r="L14" s="728"/>
+      <c r="K14" s="705"/>
+      <c r="L14" s="721"/>
       <c r="M14" s="21" t="s">
         <v>111</v>
       </c>
@@ -13471,9 +13489,9 @@
       <c r="Y14" s="21" t="s">
         <v>73</v>
       </c>
-      <c r="AA14" s="718"/>
-      <c r="AB14" s="719"/>
-      <c r="AD14" s="706"/>
+      <c r="AA14" s="711"/>
+      <c r="AB14" s="712"/>
+      <c r="AD14" s="699"/>
     </row>
     <row r="15" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C15" s="130" t="s">
@@ -13488,19 +13506,19 @@
       <c r="F15" s="66" t="s">
         <v>94</v>
       </c>
-      <c r="G15" s="694"/>
+      <c r="G15" s="726"/>
       <c r="H15" s="2" t="s">
         <v>81</v>
       </c>
       <c r="I15" s="53" t="s">
         <v>81</v>
       </c>
-      <c r="K15" s="712"/>
-      <c r="L15" s="729"/>
-      <c r="Q15" s="696" t="s">
+      <c r="K15" s="705"/>
+      <c r="L15" s="722"/>
+      <c r="Q15" s="728" t="s">
         <v>211</v>
       </c>
-      <c r="R15" s="622"/>
+      <c r="R15" s="625"/>
       <c r="S15" s="555"/>
       <c r="T15" s="6"/>
       <c r="V15" s="68" t="s">
@@ -13509,14 +13527,14 @@
       <c r="X15" s="2" t="s">
         <v>128</v>
       </c>
-      <c r="AA15" s="718"/>
-      <c r="AB15" s="719"/>
-      <c r="AD15" s="706"/>
+      <c r="AA15" s="711"/>
+      <c r="AB15" s="712"/>
+      <c r="AD15" s="699"/>
     </row>
     <row r="16" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C16" s="132"/>
-      <c r="G16" s="694"/>
-      <c r="K16" s="712"/>
+      <c r="G16" s="726"/>
+      <c r="K16" s="705"/>
       <c r="N16" s="47"/>
       <c r="O16" s="61" t="s">
         <v>109</v>
@@ -13535,24 +13553,24 @@
       <c r="Z16" s="76" t="s">
         <v>127</v>
       </c>
-      <c r="AA16" s="718"/>
-      <c r="AB16" s="719"/>
-      <c r="AD16" s="706"/>
+      <c r="AA16" s="711"/>
+      <c r="AB16" s="712"/>
+      <c r="AD16" s="699"/>
     </row>
     <row r="17" spans="3:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C17" s="109"/>
       <c r="E17" s="6" t="s">
         <v>95</v>
       </c>
-      <c r="F17" s="691" t="s">
+      <c r="F17" s="723" t="s">
         <v>96</v>
       </c>
-      <c r="G17" s="694"/>
+      <c r="G17" s="726"/>
       <c r="H17" s="54"/>
       <c r="I17" s="133" t="s">
         <v>81</v>
       </c>
-      <c r="K17" s="712"/>
+      <c r="K17" s="705"/>
       <c r="S17" s="555"/>
       <c r="V17" s="68" t="s">
         <v>44</v>
@@ -13560,9 +13578,9 @@
       <c r="X17" s="2" t="s">
         <v>118</v>
       </c>
-      <c r="AA17" s="718"/>
-      <c r="AB17" s="719"/>
-      <c r="AD17" s="706"/>
+      <c r="AA17" s="711"/>
+      <c r="AB17" s="712"/>
+      <c r="AD17" s="699"/>
     </row>
     <row r="18" spans="3:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C18" s="130"/>
@@ -13572,15 +13590,15 @@
       <c r="E18" s="6" t="s">
         <v>97</v>
       </c>
-      <c r="F18" s="692"/>
-      <c r="G18" s="694"/>
+      <c r="F18" s="724"/>
+      <c r="G18" s="726"/>
       <c r="H18" s="108" t="s">
         <v>76</v>
       </c>
       <c r="I18" s="21" t="s">
         <v>81</v>
       </c>
-      <c r="K18" s="712"/>
+      <c r="K18" s="705"/>
       <c r="O18" s="64" t="s">
         <v>115</v>
       </c>
@@ -13591,39 +13609,42 @@
       <c r="X18" s="2" t="s">
         <v>117</v>
       </c>
-      <c r="AA18" s="720"/>
-      <c r="AB18" s="721"/>
-      <c r="AD18" s="706"/>
+      <c r="AA18" s="713"/>
+      <c r="AB18" s="714"/>
+      <c r="AD18" s="699"/>
     </row>
     <row r="19" spans="3:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="F19" s="64" t="s">
         <v>209</v>
       </c>
-      <c r="G19" s="695"/>
-      <c r="K19" s="713"/>
+      <c r="G19" s="727"/>
+      <c r="K19" s="706"/>
       <c r="Q19" s="68" t="s">
         <v>44</v>
       </c>
-      <c r="R19" s="700" t="s">
+      <c r="R19" s="732" t="s">
         <v>124</v>
       </c>
-      <c r="S19" s="701"/>
-      <c r="T19" s="702"/>
+      <c r="S19" s="733"/>
+      <c r="T19" s="734"/>
       <c r="V19" s="77" t="s">
         <v>115</v>
       </c>
       <c r="Y19" s="19" t="s">
         <v>125</v>
       </c>
-      <c r="AD19" s="707"/>
+      <c r="AD19" s="700"/>
     </row>
   </sheetData>
   <mergeCells count="24">
-    <mergeCell ref="C9:C11"/>
-    <mergeCell ref="C13:C14"/>
-    <mergeCell ref="V2:W2"/>
-    <mergeCell ref="M10:AC10"/>
-    <mergeCell ref="F2:F3"/>
+    <mergeCell ref="F17:F18"/>
+    <mergeCell ref="G2:G19"/>
+    <mergeCell ref="Q13:R13"/>
+    <mergeCell ref="Q15:R15"/>
+    <mergeCell ref="L9:N9"/>
+    <mergeCell ref="R19:T19"/>
+    <mergeCell ref="S12:S18"/>
+    <mergeCell ref="O3:O9"/>
     <mergeCell ref="AD1:AD19"/>
     <mergeCell ref="S8:AC8"/>
     <mergeCell ref="K5:K19"/>
@@ -13635,14 +13656,11 @@
     <mergeCell ref="P3:Q3"/>
     <mergeCell ref="L4:L8"/>
     <mergeCell ref="L12:L15"/>
-    <mergeCell ref="F17:F18"/>
-    <mergeCell ref="G2:G19"/>
-    <mergeCell ref="Q13:R13"/>
-    <mergeCell ref="Q15:R15"/>
-    <mergeCell ref="L9:N9"/>
-    <mergeCell ref="R19:T19"/>
-    <mergeCell ref="S12:S18"/>
-    <mergeCell ref="O3:O9"/>
+    <mergeCell ref="C9:C11"/>
+    <mergeCell ref="C13:C14"/>
+    <mergeCell ref="V2:W2"/>
+    <mergeCell ref="M10:AC10"/>
+    <mergeCell ref="F2:F3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Rw Updates - Error Eradicated
Rw Updates - Error Eradicated
</commit_message>
<xml_diff>
--- a/System_2.1.5.xlsx
+++ b/System_2.1.5.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Work\Work_For_\Work\Running AppS\System_Work_RW\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DDDD0170-174B-4852-83CE-C36478C627D2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA4CE41D-7E92-464C-B43E-4BFA563D2AE3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -4807,6 +4807,63 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="255" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="32" fillId="27" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="27" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="27" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="13" fillId="27" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="13" fillId="27" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="27" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="27" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="27" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="27" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="19" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="19" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="36" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="36" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="39" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -4837,62 +4894,167 @@
     <xf numFmtId="0" fontId="6" fillId="18" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="255"/>
     </xf>
-    <xf numFmtId="0" fontId="32" fillId="27" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="73" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="57" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="11" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="11" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="13" fillId="27" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="13" fillId="27" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="27" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="27" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="27" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="27" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="36" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="36" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="3" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="18" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="18" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="18" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="32" fillId="27" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="32" fillId="27" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="14" fontId="13" fillId="27" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="49" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="49" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="49" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="14" fontId="13" fillId="27" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="32" fillId="27" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="27" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="27" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="27" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="19" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="19" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="36" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="36" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="52" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="54" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="16" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="16" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="19" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -4918,12 +5080,6 @@
     <xf numFmtId="0" fontId="38" fillId="7" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255"/>
-    </xf>
     <xf numFmtId="0" fontId="17" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="255"/>
     </xf>
@@ -4945,161 +5101,14 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="52" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="54" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="16" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="16" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="3" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="18" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="18" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="18" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="49" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="49" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="49" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="73" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="57" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="11" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="11" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="13" fillId="27" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="13" fillId="27" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="27" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="27" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="27" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="27" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="36" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="36" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="11" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="3" fillId="35" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="35" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="35" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="43" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -5158,15 +5167,6 @@
     <xf numFmtId="0" fontId="6" fillId="52" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="35" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="35" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="35" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -5185,25 +5185,46 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="30" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="30" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="30" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="24" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="24" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="24" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="18" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -5281,46 +5302,25 @@
     <xf numFmtId="0" fontId="3" fillId="21" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="30" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="30" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="30" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="24" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="24" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="24" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -5615,7 +5615,7 @@
   <dimension ref="B1:W28"/>
   <sheetViews>
     <sheetView topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="Q24" sqref="Q24"/>
+      <selection activeCell="V15" sqref="V15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6569,7 +6569,7 @@
   <dimension ref="A1:AA32"/>
   <sheetViews>
     <sheetView topLeftCell="H1" workbookViewId="0">
-      <selection activeCell="V3" sqref="V3"/>
+      <selection activeCell="W15" sqref="W15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6626,7 +6626,7 @@
       <c r="P1" s="423" t="s">
         <v>408</v>
       </c>
-      <c r="Q1" s="565" t="s">
+      <c r="Q1" s="584" t="s">
         <v>181</v>
       </c>
       <c r="R1" s="100" t="s">
@@ -6646,32 +6646,32 @@
       </c>
     </row>
     <row r="2" spans="1:27" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="578">
+      <c r="A2" s="568">
         <f ca="1">TODAY()</f>
         <v>45279</v>
       </c>
-      <c r="B2" s="580" t="s">
+      <c r="B2" s="570" t="s">
         <v>389</v>
       </c>
-      <c r="C2" s="592" t="s">
+      <c r="C2" s="582" t="s">
         <v>365</v>
       </c>
-      <c r="D2" s="582" t="s">
+      <c r="D2" s="572" t="s">
         <v>103</v>
       </c>
-      <c r="E2" s="584" t="s">
+      <c r="E2" s="574" t="s">
         <v>65</v>
       </c>
       <c r="F2" s="196" t="s">
         <v>220</v>
       </c>
-      <c r="G2" s="590" t="s">
+      <c r="G2" s="580" t="s">
         <v>381</v>
       </c>
       <c r="H2" s="211" t="s">
         <v>220</v>
       </c>
-      <c r="I2" s="572" t="s">
+      <c r="I2" s="591" t="s">
         <v>103</v>
       </c>
       <c r="J2" s="421" t="s">
@@ -6695,7 +6695,7 @@
       <c r="P2" s="424">
         <v>40</v>
       </c>
-      <c r="Q2" s="566"/>
+      <c r="Q2" s="585"/>
       <c r="R2" s="21">
         <f>R7+R18</f>
         <v>6</v>
@@ -6706,7 +6706,7 @@
       </c>
       <c r="T2" s="176">
         <f>SUM(T4:T16)</f>
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="U2" s="6"/>
       <c r="V2" s="496"/>
@@ -6717,18 +6717,18 @@
       </c>
       <c r="AA2" s="68">
         <f>Z2+T2</f>
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:27" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="579"/>
-      <c r="B3" s="581"/>
-      <c r="C3" s="593"/>
-      <c r="D3" s="583"/>
-      <c r="E3" s="585"/>
-      <c r="G3" s="591"/>
+      <c r="A3" s="569"/>
+      <c r="B3" s="571"/>
+      <c r="C3" s="583"/>
+      <c r="D3" s="573"/>
+      <c r="E3" s="575"/>
+      <c r="G3" s="581"/>
       <c r="H3" s="6"/>
-      <c r="I3" s="573"/>
+      <c r="I3" s="592"/>
       <c r="K3" s="24">
         <v>2</v>
       </c>
@@ -6740,9 +6740,7 @@
         <v>5</v>
       </c>
       <c r="U3" s="6"/>
-      <c r="V3" s="497">
-        <v>1</v>
-      </c>
+      <c r="V3" s="497"/>
       <c r="W3" s="6" t="s">
         <v>252</v>
       </c>
@@ -6753,16 +6751,16 @@
         <v>390</v>
       </c>
       <c r="B4" s="248"/>
-      <c r="C4" s="586" t="s">
+      <c r="C4" s="576" t="s">
         <v>178</v>
       </c>
-      <c r="I4" s="573"/>
+      <c r="I4" s="592"/>
       <c r="R4" s="499" t="s">
         <v>580</v>
       </c>
       <c r="T4" s="24">
         <f>IF((R7-SUM(V2:V10)&lt;0),R7-SUM(V2:V10),0)</f>
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="U4" s="6" t="s">
         <v>518</v>
@@ -6784,7 +6782,7 @@
       <c r="B5" s="100" t="s">
         <v>365</v>
       </c>
-      <c r="C5" s="587"/>
+      <c r="C5" s="577"/>
       <c r="D5" s="227" t="s">
         <v>103</v>
       </c>
@@ -6800,7 +6798,7 @@
       <c r="H5" s="211" t="s">
         <v>220</v>
       </c>
-      <c r="I5" s="573"/>
+      <c r="I5" s="592"/>
       <c r="J5" s="422" t="s">
         <v>273</v>
       </c>
@@ -6831,22 +6829,22 @@
       <c r="X5" s="495"/>
     </row>
     <row r="6" spans="1:27" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="575" t="s">
+      <c r="A6" s="565" t="s">
         <v>290</v>
       </c>
       <c r="B6" s="105" t="s">
         <v>199</v>
       </c>
-      <c r="C6" s="588"/>
-      <c r="D6" s="589"/>
+      <c r="C6" s="578"/>
+      <c r="D6" s="579"/>
       <c r="E6" s="96">
         <v>1</v>
       </c>
       <c r="G6" s="555"/>
-      <c r="I6" s="573"/>
+      <c r="I6" s="592"/>
     </row>
     <row r="7" spans="1:27" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="576"/>
+      <c r="A7" s="566"/>
       <c r="B7" s="100" t="s">
         <v>155</v>
       </c>
@@ -6857,7 +6855,7 @@
         <v>136</v>
       </c>
       <c r="G7" s="555"/>
-      <c r="I7" s="573"/>
+      <c r="I7" s="592"/>
       <c r="M7" s="16" t="s">
         <v>354</v>
       </c>
@@ -6893,7 +6891,7 @@
       </c>
     </row>
     <row r="8" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="577"/>
+      <c r="A8" s="567"/>
       <c r="B8" s="217" t="s">
         <v>28</v>
       </c>
@@ -6902,7 +6900,7 @@
         <v>3</v>
       </c>
       <c r="G8" s="555"/>
-      <c r="I8" s="573"/>
+      <c r="I8" s="592"/>
       <c r="N8" s="80"/>
       <c r="U8" s="6" t="s">
         <v>466</v>
@@ -6926,7 +6924,7 @@
       </c>
       <c r="G9" s="555"/>
       <c r="H9" s="6"/>
-      <c r="I9" s="573"/>
+      <c r="I9" s="592"/>
       <c r="M9" s="19" t="s">
         <v>547</v>
       </c>
@@ -6953,7 +6951,7 @@
         <v>42</v>
       </c>
       <c r="G10" s="555"/>
-      <c r="I10" s="573"/>
+      <c r="I10" s="592"/>
       <c r="J10" s="24" t="s">
         <v>381</v>
       </c>
@@ -6987,7 +6985,7 @@
         <v>270</v>
       </c>
       <c r="G11" s="555"/>
-      <c r="I11" s="573"/>
+      <c r="I11" s="592"/>
       <c r="J11" s="24" t="s">
         <v>195</v>
       </c>
@@ -7013,12 +7011,12 @@
       <c r="S11" s="24">
         <v>1</v>
       </c>
-      <c r="U11" s="567" t="s">
+      <c r="U11" s="586" t="s">
         <v>583</v>
       </c>
-      <c r="V11" s="568"/>
-      <c r="W11" s="568"/>
-      <c r="X11" s="569"/>
+      <c r="V11" s="587"/>
+      <c r="W11" s="587"/>
+      <c r="X11" s="588"/>
     </row>
     <row r="12" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="232" t="s">
@@ -7029,7 +7027,7 @@
         <v>3</v>
       </c>
       <c r="G12" s="555"/>
-      <c r="I12" s="573"/>
+      <c r="I12" s="592"/>
       <c r="J12" s="24" t="s">
         <v>538</v>
       </c>
@@ -7062,7 +7060,7 @@
       </c>
       <c r="D13" s="20"/>
       <c r="G13" s="555"/>
-      <c r="I13" s="573"/>
+      <c r="I13" s="592"/>
       <c r="J13" s="108" t="s">
         <v>572</v>
       </c>
@@ -7103,7 +7101,7 @@
       <c r="H14" s="211" t="s">
         <v>220</v>
       </c>
-      <c r="I14" s="573"/>
+      <c r="I14" s="592"/>
       <c r="U14" s="6"/>
       <c r="V14" s="112"/>
       <c r="W14" s="6"/>
@@ -7121,7 +7119,7 @@
       <c r="H15" s="277">
         <v>0</v>
       </c>
-      <c r="I15" s="573"/>
+      <c r="I15" s="592"/>
       <c r="J15" s="108" t="s">
         <v>154</v>
       </c>
@@ -7152,7 +7150,7 @@
       <c r="D16" s="2" t="s">
         <v>510</v>
       </c>
-      <c r="I16" s="573"/>
+      <c r="I16" s="592"/>
       <c r="K16" s="100" t="s">
         <v>44</v>
       </c>
@@ -7186,7 +7184,7 @@
       <c r="G17" s="2" t="s">
         <v>441</v>
       </c>
-      <c r="I17" s="573"/>
+      <c r="I17" s="592"/>
       <c r="L17" s="2" t="s">
         <v>444</v>
       </c>
@@ -7198,13 +7196,13 @@
     </row>
     <row r="18" spans="1:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="G18" s="16"/>
-      <c r="I18" s="573"/>
+      <c r="I18" s="592"/>
       <c r="L18" s="16"/>
       <c r="M18" s="21"/>
-      <c r="O18" s="570" t="s">
+      <c r="O18" s="589" t="s">
         <v>539</v>
       </c>
-      <c r="P18" s="571"/>
+      <c r="P18" s="590"/>
       <c r="Q18" s="127" t="s">
         <v>44</v>
       </c>
@@ -7230,7 +7228,7 @@
       </c>
     </row>
     <row r="19" spans="1:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="I19" s="573"/>
+      <c r="I19" s="592"/>
       <c r="M19" s="21" t="s">
         <v>443</v>
       </c>
@@ -7258,7 +7256,7 @@
       <c r="G20" s="2" t="s">
         <v>441</v>
       </c>
-      <c r="I20" s="573"/>
+      <c r="I20" s="592"/>
       <c r="K20" s="19" t="s">
         <v>440</v>
       </c>
@@ -7283,7 +7281,7 @@
       <c r="Z20" s="112"/>
     </row>
     <row r="21" spans="1:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="I21" s="573"/>
+      <c r="I21" s="592"/>
       <c r="M21" s="221" t="s">
         <v>422</v>
       </c>
@@ -7315,7 +7313,7 @@
       <c r="G22" s="2" t="s">
         <v>441</v>
       </c>
-      <c r="I22" s="573"/>
+      <c r="I22" s="592"/>
       <c r="U22" s="6"/>
       <c r="V22" s="495"/>
       <c r="W22" s="6" t="s">
@@ -7335,13 +7333,13 @@
       <c r="E23" s="289" t="s">
         <v>44</v>
       </c>
-      <c r="I23" s="573"/>
+      <c r="I23" s="592"/>
       <c r="U23" s="6"/>
       <c r="V23" s="24"/>
       <c r="W23" s="6"/>
     </row>
     <row r="24" spans="1:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="I24" s="573"/>
+      <c r="I24" s="592"/>
       <c r="U24" s="354"/>
       <c r="V24" s="498">
         <v>-1</v>
@@ -7369,7 +7367,7 @@
       <c r="H25" s="196" t="s">
         <v>271</v>
       </c>
-      <c r="I25" s="573"/>
+      <c r="I25" s="592"/>
       <c r="J25" s="422" t="s">
         <v>274</v>
       </c>
@@ -7414,7 +7412,7 @@
       <c r="H26" s="19" t="s">
         <v>220</v>
       </c>
-      <c r="I26" s="573"/>
+      <c r="I26" s="592"/>
       <c r="K26" s="24">
         <v>15</v>
       </c>
@@ -7449,7 +7447,7 @@
       </c>
     </row>
     <row r="27" spans="1:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="I27" s="573"/>
+      <c r="I27" s="592"/>
       <c r="O27" s="2" t="s">
         <v>99</v>
       </c>
@@ -7476,7 +7474,7 @@
       <c r="E28" s="220">
         <v>2</v>
       </c>
-      <c r="I28" s="573"/>
+      <c r="I28" s="592"/>
       <c r="Q28" s="6"/>
       <c r="R28" s="112"/>
       <c r="T28" s="142"/>
@@ -7498,7 +7496,7 @@
       <c r="H29" s="196" t="s">
         <v>272</v>
       </c>
-      <c r="I29" s="574"/>
+      <c r="I29" s="593"/>
       <c r="J29" s="333"/>
       <c r="L29" s="96" t="s">
         <v>278</v>
@@ -7568,6 +7566,11 @@
     </row>
   </sheetData>
   <mergeCells count="16">
+    <mergeCell ref="Q1:Q2"/>
+    <mergeCell ref="U11:X11"/>
+    <mergeCell ref="O18:P18"/>
+    <mergeCell ref="I2:I29"/>
+    <mergeCell ref="C13:C14"/>
     <mergeCell ref="A6:A8"/>
     <mergeCell ref="G5:G14"/>
     <mergeCell ref="A2:A3"/>
@@ -7579,11 +7582,6 @@
     <mergeCell ref="B11:B12"/>
     <mergeCell ref="G2:G3"/>
     <mergeCell ref="C2:C3"/>
-    <mergeCell ref="Q1:Q2"/>
-    <mergeCell ref="U11:X11"/>
-    <mergeCell ref="O18:P18"/>
-    <mergeCell ref="I2:I29"/>
-    <mergeCell ref="C13:C14"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -7659,7 +7657,7 @@
       <c r="H1" s="97" t="s">
         <v>350</v>
       </c>
-      <c r="I1" s="590" t="s">
+      <c r="I1" s="580" t="s">
         <v>378</v>
       </c>
       <c r="J1" s="2" t="s">
@@ -7720,7 +7718,7 @@
         <v>517</v>
       </c>
       <c r="AM1" s="427"/>
-      <c r="AN1" s="621"/>
+      <c r="AN1" s="618"/>
       <c r="AO1" s="350" t="s">
         <v>487</v>
       </c>
@@ -7729,23 +7727,23 @@
       </c>
     </row>
     <row r="2" spans="1:43" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="645">
+      <c r="A2" s="600">
         <f ca="1">TODAY()</f>
         <v>45279</v>
       </c>
-      <c r="B2" s="647" t="s">
+      <c r="B2" s="602" t="s">
         <v>379</v>
       </c>
-      <c r="C2" s="592" t="s">
+      <c r="C2" s="582" t="s">
         <v>365</v>
       </c>
-      <c r="D2" s="649" t="s">
+      <c r="D2" s="604" t="s">
         <v>362</v>
       </c>
-      <c r="E2" s="594" t="s">
+      <c r="E2" s="648" t="s">
         <v>65</v>
       </c>
-      <c r="F2" s="602" t="s">
+      <c r="F2" s="623" t="s">
         <v>103</v>
       </c>
       <c r="G2" s="418" t="s">
@@ -7754,31 +7752,31 @@
       <c r="H2" s="80" t="s">
         <v>33</v>
       </c>
-      <c r="I2" s="591"/>
+      <c r="I2" s="581"/>
       <c r="J2" s="81" t="s">
         <v>77</v>
       </c>
-      <c r="K2" s="596" t="s">
+      <c r="K2" s="650" t="s">
         <v>349</v>
       </c>
-      <c r="L2" s="597"/>
-      <c r="M2" s="602" t="s">
+      <c r="L2" s="651"/>
+      <c r="M2" s="623" t="s">
         <v>103</v>
       </c>
       <c r="N2" s="69" t="s">
         <v>28</v>
       </c>
-      <c r="O2" s="628" t="s">
+      <c r="O2" s="627" t="s">
         <v>103</v>
       </c>
       <c r="P2" s="85" t="s">
         <v>148</v>
       </c>
-      <c r="Q2" s="592" t="s">
+      <c r="Q2" s="582" t="s">
         <v>144</v>
       </c>
       <c r="R2" s="554"/>
-      <c r="S2" s="615" t="s">
+      <c r="S2" s="640" t="s">
         <v>149</v>
       </c>
       <c r="T2" s="89"/>
@@ -7811,15 +7809,15 @@
         <v>481</v>
       </c>
       <c r="AM2" s="453"/>
-      <c r="AN2" s="622"/>
+      <c r="AN2" s="619"/>
     </row>
     <row r="3" spans="1:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="646"/>
-      <c r="B3" s="648"/>
-      <c r="C3" s="593"/>
-      <c r="D3" s="650"/>
-      <c r="E3" s="595"/>
-      <c r="F3" s="603"/>
+      <c r="A3" s="601"/>
+      <c r="B3" s="603"/>
+      <c r="C3" s="583"/>
+      <c r="D3" s="605"/>
+      <c r="E3" s="649"/>
+      <c r="F3" s="624"/>
       <c r="G3" s="419" t="s">
         <v>28</v>
       </c>
@@ -7838,17 +7836,17 @@
       <c r="L3" s="206" t="s">
         <v>108</v>
       </c>
-      <c r="M3" s="603"/>
+      <c r="M3" s="624"/>
       <c r="N3" s="69" t="s">
         <v>147</v>
       </c>
-      <c r="O3" s="629"/>
+      <c r="O3" s="628"/>
       <c r="P3" s="2" t="s">
         <v>155</v>
       </c>
-      <c r="Q3" s="593"/>
+      <c r="Q3" s="583"/>
       <c r="R3" s="556"/>
-      <c r="S3" s="617"/>
+      <c r="S3" s="641"/>
       <c r="T3" s="89"/>
       <c r="U3" s="124"/>
       <c r="V3" s="120"/>
@@ -7865,7 +7863,7 @@
       <c r="AC3" s="100" t="s">
         <v>498</v>
       </c>
-      <c r="AD3" s="612" t="s">
+      <c r="AD3" s="639" t="s">
         <v>473</v>
       </c>
       <c r="AE3" s="262"/>
@@ -7877,16 +7875,16 @@
       <c r="AK3" s="262"/>
       <c r="AL3" s="16"/>
       <c r="AM3" s="453"/>
-      <c r="AN3" s="622"/>
+      <c r="AN3" s="619"/>
     </row>
     <row r="4" spans="1:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="243" t="s">
         <v>184</v>
       </c>
-      <c r="B4" s="661" t="s">
+      <c r="B4" s="616" t="s">
         <v>382</v>
       </c>
-      <c r="C4" s="592" t="s">
+      <c r="C4" s="582" t="s">
         <v>155</v>
       </c>
       <c r="D4" s="359" t="s">
@@ -7895,7 +7893,7 @@
       <c r="E4" s="396">
         <v>2</v>
       </c>
-      <c r="F4" s="603"/>
+      <c r="F4" s="624"/>
       <c r="G4" s="400" t="s">
         <v>203</v>
       </c>
@@ -7912,11 +7910,11 @@
         <v>151</v>
       </c>
       <c r="L4" s="209"/>
-      <c r="M4" s="603"/>
+      <c r="M4" s="624"/>
       <c r="N4" s="178" t="s">
         <v>70</v>
       </c>
-      <c r="O4" s="629"/>
+      <c r="O4" s="628"/>
       <c r="P4" s="2" t="s">
         <v>192</v>
       </c>
@@ -7943,7 +7941,7 @@
       <c r="AA4" s="313"/>
       <c r="AB4" s="214"/>
       <c r="AC4" s="16"/>
-      <c r="AD4" s="612"/>
+      <c r="AD4" s="639"/>
       <c r="AE4" s="262"/>
       <c r="AF4" s="262"/>
       <c r="AG4" s="16"/>
@@ -7953,37 +7951,37 @@
       <c r="AK4" s="262"/>
       <c r="AL4" s="16"/>
       <c r="AM4" s="453"/>
-      <c r="AN4" s="622"/>
+      <c r="AN4" s="619"/>
       <c r="AO4" s="350" t="s">
         <v>91</v>
       </c>
     </row>
     <row r="5" spans="1:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="590" t="s">
+      <c r="A5" s="580" t="s">
         <v>435</v>
       </c>
-      <c r="B5" s="662"/>
-      <c r="C5" s="593"/>
+      <c r="B5" s="617"/>
+      <c r="C5" s="583"/>
       <c r="D5" s="61" t="s">
         <v>154</v>
       </c>
       <c r="E5" s="397">
         <v>1</v>
       </c>
-      <c r="F5" s="603"/>
-      <c r="G5" s="653" t="s">
+      <c r="F5" s="624"/>
+      <c r="G5" s="608" t="s">
         <v>193</v>
       </c>
-      <c r="H5" s="653"/>
-      <c r="I5" s="653"/>
-      <c r="J5" s="653"/>
-      <c r="K5" s="653"/>
-      <c r="L5" s="654"/>
-      <c r="M5" s="603"/>
+      <c r="H5" s="608"/>
+      <c r="I5" s="608"/>
+      <c r="J5" s="608"/>
+      <c r="K5" s="608"/>
+      <c r="L5" s="609"/>
+      <c r="M5" s="624"/>
       <c r="N5" s="21">
         <v>8</v>
       </c>
-      <c r="O5" s="629"/>
+      <c r="O5" s="628"/>
       <c r="T5" s="89"/>
       <c r="U5" s="124"/>
       <c r="V5" s="120"/>
@@ -8014,24 +8012,24 @@
       <c r="AK5" s="262"/>
       <c r="AL5" s="80"/>
       <c r="AM5" s="453"/>
-      <c r="AN5" s="622"/>
+      <c r="AN5" s="619"/>
     </row>
     <row r="6" spans="1:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="591"/>
-      <c r="B6" s="659" t="s">
+      <c r="A6" s="581"/>
+      <c r="B6" s="614" t="s">
         <v>178</v>
       </c>
-      <c r="C6" s="588"/>
-      <c r="D6" s="589"/>
-      <c r="F6" s="603"/>
-      <c r="G6" s="655"/>
-      <c r="H6" s="655"/>
-      <c r="I6" s="655"/>
-      <c r="J6" s="655"/>
-      <c r="K6" s="655"/>
-      <c r="L6" s="656"/>
-      <c r="M6" s="603"/>
-      <c r="O6" s="629"/>
+      <c r="C6" s="578"/>
+      <c r="D6" s="579"/>
+      <c r="F6" s="624"/>
+      <c r="G6" s="610"/>
+      <c r="H6" s="610"/>
+      <c r="I6" s="610"/>
+      <c r="J6" s="610"/>
+      <c r="K6" s="610"/>
+      <c r="L6" s="611"/>
+      <c r="M6" s="624"/>
+      <c r="O6" s="628"/>
       <c r="T6" s="89"/>
       <c r="U6" s="124"/>
       <c r="V6" s="98" t="s">
@@ -8055,16 +8053,16 @@
       <c r="AF6" s="262"/>
       <c r="AG6" s="262"/>
       <c r="AH6" s="262"/>
-      <c r="AI6" s="611"/>
+      <c r="AI6" s="633"/>
       <c r="AJ6" s="466" t="s">
         <v>476</v>
       </c>
-      <c r="AK6" s="611" t="s">
+      <c r="AK6" s="633" t="s">
         <v>256</v>
       </c>
       <c r="AL6" s="262"/>
       <c r="AM6" s="453"/>
-      <c r="AN6" s="622"/>
+      <c r="AN6" s="619"/>
       <c r="AO6" s="350" t="s">
         <v>488</v>
       </c>
@@ -8073,7 +8071,7 @@
       <c r="A7" s="237" t="s">
         <v>598</v>
       </c>
-      <c r="B7" s="660"/>
+      <c r="B7" s="615"/>
       <c r="C7" s="207" t="s">
         <v>383</v>
       </c>
@@ -8083,7 +8081,7 @@
       <c r="E7" s="271">
         <v>3</v>
       </c>
-      <c r="F7" s="603"/>
+      <c r="F7" s="624"/>
       <c r="G7" s="420">
         <v>0</v>
       </c>
@@ -8102,8 +8100,8 @@
       <c r="L7" s="217">
         <v>0</v>
       </c>
-      <c r="M7" s="603"/>
-      <c r="O7" s="629"/>
+      <c r="M7" s="624"/>
+      <c r="O7" s="628"/>
       <c r="R7" s="99" t="s">
         <v>44</v>
       </c>
@@ -8127,18 +8125,18 @@
       <c r="AD7" s="16"/>
       <c r="AE7" s="262"/>
       <c r="AF7" s="262"/>
-      <c r="AG7" s="612" t="s">
+      <c r="AG7" s="639" t="s">
         <v>472</v>
       </c>
       <c r="AH7" s="262"/>
-      <c r="AI7" s="611"/>
+      <c r="AI7" s="633"/>
       <c r="AJ7" s="262"/>
-      <c r="AK7" s="611"/>
+      <c r="AK7" s="633"/>
       <c r="AL7" s="80" t="s">
         <v>515</v>
       </c>
       <c r="AM7" s="453"/>
-      <c r="AN7" s="622"/>
+      <c r="AN7" s="619"/>
       <c r="AP7" s="76" t="s">
         <v>489</v>
       </c>
@@ -8155,27 +8153,27 @@
         <f>SUM(G7:N9)</f>
         <v>15</v>
       </c>
-      <c r="F8" s="603"/>
-      <c r="G8" s="654">
-        <v>0</v>
-      </c>
-      <c r="H8" s="651" t="s">
+      <c r="F8" s="624"/>
+      <c r="G8" s="609">
+        <v>0</v>
+      </c>
+      <c r="H8" s="606" t="s">
         <v>105</v>
       </c>
       <c r="I8" s="554">
         <v>0</v>
       </c>
-      <c r="J8" s="651" t="s">
+      <c r="J8" s="606" t="s">
         <v>105</v>
       </c>
-      <c r="K8" s="657"/>
-      <c r="L8" s="613"/>
-      <c r="M8" s="626"/>
-      <c r="N8" s="618">
+      <c r="K8" s="612"/>
+      <c r="L8" s="642"/>
+      <c r="M8" s="625"/>
+      <c r="N8" s="645">
         <f>N5+N11</f>
         <v>15</v>
       </c>
-      <c r="O8" s="629"/>
+      <c r="O8" s="628"/>
       <c r="T8" s="103" t="s">
         <v>44</v>
       </c>
@@ -8193,14 +8191,14 @@
       <c r="AD8" s="16"/>
       <c r="AE8" s="262"/>
       <c r="AF8" s="262"/>
-      <c r="AG8" s="612"/>
+      <c r="AG8" s="639"/>
       <c r="AH8" s="262"/>
-      <c r="AI8" s="611"/>
+      <c r="AI8" s="633"/>
       <c r="AJ8" s="262"/>
       <c r="AK8" s="262"/>
       <c r="AL8" s="262"/>
       <c r="AM8" s="453"/>
-      <c r="AN8" s="622"/>
+      <c r="AN8" s="619"/>
     </row>
     <row r="9" spans="1:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="237" t="s">
@@ -8215,17 +8213,17 @@
       <c r="D9" s="360" t="s">
         <v>286</v>
       </c>
-      <c r="F9" s="603"/>
-      <c r="G9" s="656"/>
-      <c r="H9" s="652"/>
+      <c r="F9" s="624"/>
+      <c r="G9" s="611"/>
+      <c r="H9" s="607"/>
       <c r="I9" s="556"/>
-      <c r="J9" s="652"/>
-      <c r="K9" s="658"/>
-      <c r="L9" s="614"/>
-      <c r="M9" s="627"/>
-      <c r="N9" s="619"/>
-      <c r="O9" s="630"/>
-      <c r="S9" s="615" t="s">
+      <c r="J9" s="607"/>
+      <c r="K9" s="613"/>
+      <c r="L9" s="643"/>
+      <c r="M9" s="626"/>
+      <c r="N9" s="646"/>
+      <c r="O9" s="629"/>
+      <c r="S9" s="640" t="s">
         <v>62</v>
       </c>
       <c r="T9" s="89"/>
@@ -8247,16 +8245,16 @@
       </c>
       <c r="AE9" s="262"/>
       <c r="AF9" s="262"/>
-      <c r="AG9" s="612"/>
+      <c r="AG9" s="639"/>
       <c r="AH9" s="262"/>
-      <c r="AI9" s="611"/>
+      <c r="AI9" s="633"/>
       <c r="AJ9" s="80"/>
-      <c r="AK9" s="611" t="s">
+      <c r="AK9" s="633" t="s">
         <v>256</v>
       </c>
       <c r="AL9" s="262"/>
       <c r="AM9" s="453"/>
-      <c r="AN9" s="622"/>
+      <c r="AN9" s="619"/>
       <c r="AP9" s="2" t="s">
         <v>527</v>
       </c>
@@ -8273,20 +8271,20 @@
         <f>Boat!U8</f>
         <v>42</v>
       </c>
-      <c r="F10" s="603"/>
+      <c r="F10" s="624"/>
       <c r="N10" s="443" t="s">
         <v>407</v>
       </c>
-      <c r="O10" s="605" t="s">
+      <c r="O10" s="657" t="s">
         <v>103</v>
       </c>
-      <c r="P10" s="631" t="s">
+      <c r="P10" s="630" t="s">
         <v>411</v>
       </c>
       <c r="R10" s="74" t="s">
         <v>44</v>
       </c>
-      <c r="S10" s="616"/>
+      <c r="S10" s="644"/>
       <c r="T10" s="89"/>
       <c r="U10" s="123" t="s">
         <v>177</v>
@@ -8316,16 +8314,16 @@
       <c r="AF10" s="243" t="s">
         <v>318</v>
       </c>
-      <c r="AG10" s="612"/>
+      <c r="AG10" s="639"/>
       <c r="AH10" s="80"/>
-      <c r="AI10" s="611"/>
+      <c r="AI10" s="633"/>
       <c r="AJ10" s="262"/>
-      <c r="AK10" s="611"/>
+      <c r="AK10" s="633"/>
       <c r="AL10" s="262"/>
       <c r="AM10" s="467" t="s">
         <v>325</v>
       </c>
-      <c r="AN10" s="622"/>
+      <c r="AN10" s="619"/>
       <c r="AO10" s="209" t="s">
         <v>95</v>
       </c>
@@ -8343,18 +8341,18 @@
       <c r="D11" s="174" t="s">
         <v>362</v>
       </c>
-      <c r="F11" s="603"/>
+      <c r="F11" s="624"/>
       <c r="M11" s="6"/>
       <c r="N11" s="117">
         <v>7</v>
       </c>
-      <c r="O11" s="606"/>
-      <c r="P11" s="632"/>
+      <c r="O11" s="658"/>
+      <c r="P11" s="631"/>
       <c r="Q11" s="65"/>
       <c r="R11" s="120" t="s">
         <v>222</v>
       </c>
-      <c r="S11" s="616"/>
+      <c r="S11" s="644"/>
       <c r="T11" s="102" t="s">
         <v>44</v>
       </c>
@@ -8378,14 +8376,14 @@
       <c r="AF11" s="262" t="s">
         <v>494</v>
       </c>
-      <c r="AG11" s="612"/>
+      <c r="AG11" s="639"/>
       <c r="AH11" s="262"/>
       <c r="AI11" s="70"/>
       <c r="AJ11" s="262"/>
       <c r="AK11" s="262"/>
       <c r="AL11" s="262"/>
       <c r="AM11" s="453"/>
-      <c r="AN11" s="622"/>
+      <c r="AN11" s="619"/>
       <c r="AP11" s="76" t="s">
         <v>502</v>
       </c>
@@ -8404,7 +8402,7 @@
       <c r="E12" s="229">
         <v>3</v>
       </c>
-      <c r="F12" s="603"/>
+      <c r="F12" s="624"/>
       <c r="G12" s="349" t="s">
         <v>411</v>
       </c>
@@ -8413,16 +8411,16 @@
       </c>
       <c r="I12" s="561"/>
       <c r="J12" s="561"/>
-      <c r="K12" s="610"/>
+      <c r="K12" s="662"/>
       <c r="L12" s="208"/>
       <c r="M12" s="208"/>
       <c r="N12" s="208"/>
-      <c r="O12" s="606"/>
-      <c r="P12" s="632"/>
+      <c r="O12" s="658"/>
+      <c r="P12" s="631"/>
       <c r="R12" s="122" t="s">
         <v>181</v>
       </c>
-      <c r="S12" s="617"/>
+      <c r="S12" s="641"/>
       <c r="T12" s="101" t="s">
         <v>44</v>
       </c>
@@ -8443,16 +8441,16 @@
       <c r="AC12" s="100" t="s">
         <v>499</v>
       </c>
-      <c r="AD12" s="620" t="s">
+      <c r="AD12" s="647" t="s">
         <v>245</v>
       </c>
       <c r="AE12" s="466" t="s">
         <v>244</v>
       </c>
-      <c r="AF12" s="612" t="s">
+      <c r="AF12" s="639" t="s">
         <v>231</v>
       </c>
-      <c r="AG12" s="612"/>
+      <c r="AG12" s="639"/>
       <c r="AH12" s="243" t="s">
         <v>264</v>
       </c>
@@ -8465,7 +8463,7 @@
       <c r="AM12" s="634" t="s">
         <v>254</v>
       </c>
-      <c r="AN12" s="622"/>
+      <c r="AN12" s="619"/>
       <c r="AO12" s="350" t="s">
         <v>97</v>
       </c>
@@ -8477,17 +8475,17 @@
       <c r="E13" s="473">
         <v>-3</v>
       </c>
-      <c r="F13" s="603"/>
+      <c r="F13" s="624"/>
       <c r="G13" s="561" t="s">
         <v>448</v>
       </c>
       <c r="H13" s="561"/>
       <c r="I13" s="561"/>
-      <c r="J13" s="610"/>
+      <c r="J13" s="662"/>
       <c r="M13" s="6"/>
       <c r="N13" s="6"/>
-      <c r="O13" s="606"/>
-      <c r="P13" s="633"/>
+      <c r="O13" s="658"/>
+      <c r="P13" s="632"/>
       <c r="T13" s="105" t="s">
         <v>44</v>
       </c>
@@ -8508,8 +8506,8 @@
         <v>519</v>
       </c>
       <c r="AC13" s="16"/>
-      <c r="AD13" s="620"/>
-      <c r="AF13" s="612"/>
+      <c r="AD13" s="647"/>
+      <c r="AF13" s="639"/>
       <c r="AG13" s="80"/>
       <c r="AH13" s="243" t="s">
         <v>314</v>
@@ -8521,7 +8519,7 @@
       <c r="AK13" s="262"/>
       <c r="AL13" s="262"/>
       <c r="AM13" s="634"/>
-      <c r="AN13" s="622"/>
+      <c r="AN13" s="619"/>
     </row>
     <row r="14" spans="1:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="475"/>
@@ -8529,18 +8527,18 @@
       <c r="C14" s="484"/>
       <c r="D14" s="477"/>
       <c r="E14" s="478"/>
-      <c r="F14" s="603"/>
+      <c r="F14" s="624"/>
       <c r="G14" s="561" t="s">
         <v>447</v>
       </c>
       <c r="H14" s="561"/>
       <c r="I14" s="561"/>
-      <c r="J14" s="610"/>
+      <c r="J14" s="662"/>
       <c r="K14" s="2">
         <v>12</v>
       </c>
       <c r="N14" s="6"/>
-      <c r="O14" s="606"/>
+      <c r="O14" s="658"/>
       <c r="Q14" s="61" t="s">
         <v>555</v>
       </c>
@@ -8561,9 +8559,9 @@
       <c r="AA14" s="313"/>
       <c r="AB14" s="214"/>
       <c r="AC14" s="16"/>
-      <c r="AD14" s="620"/>
+      <c r="AD14" s="647"/>
       <c r="AE14" s="262"/>
-      <c r="AF14" s="612"/>
+      <c r="AF14" s="639"/>
       <c r="AG14" s="262"/>
       <c r="AH14" s="262"/>
       <c r="AI14" s="70"/>
@@ -8571,7 +8569,7 @@
       <c r="AK14" s="262"/>
       <c r="AL14" s="262"/>
       <c r="AM14" s="634"/>
-      <c r="AN14" s="622"/>
+      <c r="AN14" s="619"/>
     </row>
     <row r="15" spans="1:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="474" t="s">
@@ -8580,8 +8578,8 @@
       <c r="C15" s="554" t="s">
         <v>382</v>
       </c>
-      <c r="F15" s="603"/>
-      <c r="O15" s="606"/>
+      <c r="F15" s="624"/>
+      <c r="O15" s="658"/>
       <c r="R15" s="99" t="s">
         <v>44</v>
       </c>
@@ -8603,8 +8601,8 @@
       <c r="AC15" s="76" t="s">
         <v>497</v>
       </c>
-      <c r="AD15" s="620"/>
-      <c r="AF15" s="612"/>
+      <c r="AD15" s="647"/>
+      <c r="AF15" s="639"/>
       <c r="AG15" s="80"/>
       <c r="AH15" s="243" t="s">
         <v>466</v>
@@ -8618,7 +8616,7 @@
       <c r="AK15" s="262"/>
       <c r="AL15" s="262"/>
       <c r="AM15" s="634"/>
-      <c r="AN15" s="622"/>
+      <c r="AN15" s="619"/>
       <c r="AP15" s="76" t="s">
         <v>74</v>
       </c>
@@ -8640,13 +8638,13 @@
       <c r="E16" s="229">
         <v>1</v>
       </c>
-      <c r="F16" s="603"/>
+      <c r="F16" s="624"/>
       <c r="G16" s="349" t="s">
         <v>506</v>
       </c>
       <c r="I16" s="496"/>
       <c r="J16" s="20"/>
-      <c r="O16" s="606"/>
+      <c r="O16" s="658"/>
       <c r="R16" s="460" t="s">
         <v>185</v>
       </c>
@@ -8678,18 +8676,18 @@
       <c r="AM16" s="453" t="s">
         <v>324</v>
       </c>
-      <c r="AN16" s="622"/>
+      <c r="AN16" s="619"/>
       <c r="AP16" s="76" t="s">
         <v>235</v>
       </c>
     </row>
     <row r="17" spans="1:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B17" s="80"/>
-      <c r="F17" s="603"/>
+      <c r="F17" s="624"/>
       <c r="I17" s="497"/>
       <c r="J17" s="20"/>
       <c r="N17" s="6"/>
-      <c r="O17" s="606"/>
+      <c r="O17" s="658"/>
       <c r="Q17" s="21" t="s">
         <v>553</v>
       </c>
@@ -8734,7 +8732,7 @@
       <c r="AK17" s="262"/>
       <c r="AL17" s="80"/>
       <c r="AM17" s="453"/>
-      <c r="AN17" s="622"/>
+      <c r="AN17" s="619"/>
       <c r="AO17" s="209" t="s">
         <v>516</v>
       </c>
@@ -8758,21 +8756,21 @@
       <c r="E18" s="99" t="s">
         <v>44</v>
       </c>
-      <c r="F18" s="603"/>
+      <c r="F18" s="624"/>
       <c r="G18" s="349" t="s">
         <v>550</v>
       </c>
       <c r="I18" s="24"/>
       <c r="J18" s="20"/>
-      <c r="O18" s="606"/>
+      <c r="O18" s="658"/>
       <c r="Q18" s="112"/>
-      <c r="R18" s="598" t="s">
+      <c r="R18" s="652" t="s">
         <v>558</v>
       </c>
       <c r="T18" s="100" t="s">
         <v>44</v>
       </c>
-      <c r="U18" s="642" t="s">
+      <c r="U18" s="597" t="s">
         <v>44</v>
       </c>
       <c r="V18" s="120"/>
@@ -8793,7 +8791,7 @@
       <c r="AC18" s="16"/>
       <c r="AD18" s="16"/>
       <c r="AE18" s="262"/>
-      <c r="AF18" s="611" t="s">
+      <c r="AF18" s="633" t="s">
         <v>493</v>
       </c>
       <c r="AG18" s="262"/>
@@ -8805,20 +8803,20 @@
       <c r="AK18" s="262"/>
       <c r="AL18" s="80"/>
       <c r="AM18" s="453"/>
-      <c r="AN18" s="622"/>
+      <c r="AN18" s="619"/>
       <c r="AP18" s="76" t="s">
         <v>88</v>
       </c>
     </row>
     <row r="19" spans="1:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="F19" s="603"/>
+      <c r="F19" s="624"/>
       <c r="I19" s="224"/>
-      <c r="O19" s="606"/>
-      <c r="R19" s="599"/>
+      <c r="O19" s="658"/>
+      <c r="R19" s="653"/>
       <c r="S19" s="30" t="s">
         <v>556</v>
       </c>
-      <c r="U19" s="643"/>
+      <c r="U19" s="598"/>
       <c r="V19" s="146"/>
       <c r="W19" s="146"/>
       <c r="X19" s="456" t="s">
@@ -8833,7 +8831,7 @@
       <c r="AC19" s="16"/>
       <c r="AD19" s="16"/>
       <c r="AE19" s="262"/>
-      <c r="AF19" s="611"/>
+      <c r="AF19" s="633"/>
       <c r="AG19" s="262"/>
       <c r="AH19" s="262"/>
       <c r="AI19" s="70"/>
@@ -8843,7 +8841,7 @@
       </c>
       <c r="AL19" s="80"/>
       <c r="AM19" s="453"/>
-      <c r="AN19" s="622"/>
+      <c r="AN19" s="619"/>
       <c r="AP19" s="76" t="s">
         <v>486</v>
       </c>
@@ -8864,19 +8862,19 @@
       <c r="E20" s="462">
         <v>-1</v>
       </c>
-      <c r="F20" s="603"/>
+      <c r="F20" s="624"/>
       <c r="G20" s="349" t="s">
         <v>509</v>
       </c>
       <c r="I20" s="224"/>
-      <c r="O20" s="606"/>
-      <c r="Q20" s="608" t="s">
+      <c r="O20" s="658"/>
+      <c r="Q20" s="660" t="s">
         <v>48</v>
       </c>
       <c r="T20" s="429" t="s">
         <v>44</v>
       </c>
-      <c r="U20" s="644"/>
+      <c r="U20" s="599"/>
       <c r="W20" s="430"/>
       <c r="X20" s="457" t="s">
         <v>175</v>
@@ -8906,7 +8904,7 @@
       <c r="AM20" s="400" t="s">
         <v>254</v>
       </c>
-      <c r="AN20" s="622"/>
+      <c r="AN20" s="619"/>
       <c r="AO20" s="350" t="s">
         <v>478</v>
       </c>
@@ -8927,13 +8925,13 @@
       <c r="E21" s="271">
         <v>0</v>
       </c>
-      <c r="F21" s="603"/>
+      <c r="F21" s="624"/>
       <c r="I21" s="224"/>
-      <c r="O21" s="606"/>
-      <c r="Q21" s="609"/>
+      <c r="O21" s="658"/>
+      <c r="Q21" s="661"/>
       <c r="T21" s="447"/>
       <c r="U21" s="14"/>
-      <c r="V21" s="639"/>
+      <c r="V21" s="594"/>
       <c r="W21" s="451" t="s">
         <v>176</v>
       </c>
@@ -8971,15 +8969,15 @@
       <c r="AM21" s="453" t="s">
         <v>567</v>
       </c>
-      <c r="AN21" s="622"/>
+      <c r="AN21" s="619"/>
     </row>
     <row r="22" spans="1:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="F22" s="603"/>
+      <c r="F22" s="624"/>
       <c r="G22" s="349" t="s">
         <v>507</v>
       </c>
       <c r="I22" s="224"/>
-      <c r="O22" s="606"/>
+      <c r="O22" s="658"/>
       <c r="R22" s="459" t="s">
         <v>44</v>
       </c>
@@ -8987,7 +8985,7 @@
         <v>44</v>
       </c>
       <c r="U22" s="15"/>
-      <c r="V22" s="640"/>
+      <c r="V22" s="595"/>
       <c r="W22" s="451" t="s">
         <v>176</v>
       </c>
@@ -9005,7 +9003,7 @@
       <c r="AG22" s="6"/>
       <c r="AH22" s="6"/>
       <c r="AI22" s="6"/>
-      <c r="AJ22" s="611" t="s">
+      <c r="AJ22" s="633" t="s">
         <v>490</v>
       </c>
       <c r="AK22" s="262"/>
@@ -9013,7 +9011,7 @@
         <v>496</v>
       </c>
       <c r="AM22" s="306"/>
-      <c r="AN22" s="622"/>
+      <c r="AN22" s="619"/>
     </row>
     <row r="23" spans="1:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="236" t="s">
@@ -9031,17 +9029,17 @@
       <c r="E23" s="230">
         <v>1</v>
       </c>
-      <c r="F23" s="603"/>
+      <c r="F23" s="624"/>
       <c r="I23" s="224"/>
-      <c r="O23" s="606"/>
-      <c r="Q23" s="608" t="s">
+      <c r="O23" s="658"/>
+      <c r="Q23" s="660" t="s">
         <v>145</v>
       </c>
       <c r="T23" s="17"/>
       <c r="U23" s="445" t="s">
         <v>44</v>
       </c>
-      <c r="V23" s="640"/>
+      <c r="V23" s="595"/>
       <c r="W23" s="148"/>
       <c r="X23" s="454" t="s">
         <v>189</v>
@@ -9057,13 +9055,13 @@
       <c r="AG23" s="6"/>
       <c r="AH23" s="6"/>
       <c r="AI23" s="6"/>
-      <c r="AJ23" s="611"/>
+      <c r="AJ23" s="633"/>
       <c r="AK23" s="262"/>
       <c r="AL23" s="80" t="s">
         <v>526</v>
       </c>
       <c r="AM23" s="306"/>
-      <c r="AN23" s="622"/>
+      <c r="AN23" s="619"/>
     </row>
     <row r="24" spans="1:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="465" t="s">
@@ -9081,18 +9079,18 @@
       <c r="E24" s="461">
         <v>1</v>
       </c>
-      <c r="F24" s="603"/>
+      <c r="F24" s="624"/>
       <c r="G24" s="61" t="s">
         <v>508</v>
       </c>
       <c r="I24" s="224"/>
-      <c r="O24" s="606"/>
-      <c r="Q24" s="609"/>
+      <c r="O24" s="658"/>
+      <c r="Q24" s="661"/>
       <c r="T24" s="17"/>
       <c r="U24" s="232" t="s">
         <v>44</v>
       </c>
-      <c r="V24" s="640"/>
+      <c r="V24" s="595"/>
       <c r="W24" s="148"/>
       <c r="X24" s="454" t="s">
         <v>186</v>
@@ -9116,12 +9114,12 @@
         <v>481</v>
       </c>
       <c r="AM24" s="306"/>
-      <c r="AN24" s="622"/>
+      <c r="AN24" s="619"/>
     </row>
     <row r="25" spans="1:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="F25" s="603"/>
+      <c r="F25" s="624"/>
       <c r="I25" s="224"/>
-      <c r="O25" s="606"/>
+      <c r="O25" s="658"/>
       <c r="P25" s="209" t="s">
         <v>285</v>
       </c>
@@ -9134,7 +9132,7 @@
       <c r="U25" s="425" t="s">
         <v>44</v>
       </c>
-      <c r="V25" s="641"/>
+      <c r="V25" s="596"/>
       <c r="W25" s="148"/>
       <c r="X25" s="454" t="s">
         <v>190</v>
@@ -9156,7 +9154,7 @@
       <c r="AK25" s="142"/>
       <c r="AL25" s="6"/>
       <c r="AM25" s="306"/>
-      <c r="AN25" s="622"/>
+      <c r="AN25" s="619"/>
     </row>
     <row r="26" spans="1:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="236" t="s">
@@ -9174,17 +9172,17 @@
       <c r="E26" s="398">
         <v>1</v>
       </c>
-      <c r="F26" s="603"/>
+      <c r="F26" s="624"/>
       <c r="G26" s="349" t="s">
         <v>505</v>
       </c>
       <c r="I26" s="224"/>
-      <c r="O26" s="606"/>
-      <c r="P26" s="624" t="s">
+      <c r="O26" s="658"/>
+      <c r="P26" s="621" t="s">
         <v>548</v>
       </c>
-      <c r="Q26" s="625"/>
-      <c r="R26" s="600" t="s">
+      <c r="Q26" s="622"/>
+      <c r="R26" s="654" t="s">
         <v>557</v>
       </c>
       <c r="T26" s="182"/>
@@ -9223,7 +9221,7 @@
       <c r="AM26" s="467" t="s">
         <v>474</v>
       </c>
-      <c r="AN26" s="622"/>
+      <c r="AN26" s="619"/>
     </row>
     <row r="27" spans="1:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B27" s="21" t="s">
@@ -9235,13 +9233,13 @@
       <c r="E27" s="271" t="s">
         <v>44</v>
       </c>
-      <c r="F27" s="604"/>
+      <c r="F27" s="656"/>
       <c r="G27" s="61" t="s">
         <v>566</v>
       </c>
       <c r="I27" s="225"/>
-      <c r="O27" s="607"/>
-      <c r="R27" s="601"/>
+      <c r="O27" s="659"/>
+      <c r="R27" s="655"/>
       <c r="S27" s="446" t="s">
         <v>54</v>
       </c>
@@ -9271,10 +9269,48 @@
       <c r="AM27" s="400" t="s">
         <v>326</v>
       </c>
-      <c r="AN27" s="623"/>
+      <c r="AN27" s="620"/>
     </row>
   </sheetData>
   <mergeCells count="54">
+    <mergeCell ref="E2:E3"/>
+    <mergeCell ref="K2:L2"/>
+    <mergeCell ref="I1:I2"/>
+    <mergeCell ref="R18:R19"/>
+    <mergeCell ref="R26:R27"/>
+    <mergeCell ref="F2:F27"/>
+    <mergeCell ref="O10:O27"/>
+    <mergeCell ref="Q20:Q21"/>
+    <mergeCell ref="Q23:Q24"/>
+    <mergeCell ref="G14:J14"/>
+    <mergeCell ref="G13:J13"/>
+    <mergeCell ref="H12:K12"/>
+    <mergeCell ref="A5:A6"/>
+    <mergeCell ref="C6:D6"/>
+    <mergeCell ref="AI6:AI10"/>
+    <mergeCell ref="AF12:AF15"/>
+    <mergeCell ref="AG7:AG12"/>
+    <mergeCell ref="L8:L9"/>
+    <mergeCell ref="S9:S12"/>
+    <mergeCell ref="N8:N9"/>
+    <mergeCell ref="AD12:AD15"/>
+    <mergeCell ref="C15:C16"/>
+    <mergeCell ref="AN1:AN27"/>
+    <mergeCell ref="P26:Q26"/>
+    <mergeCell ref="Q2:Q3"/>
+    <mergeCell ref="M2:M9"/>
+    <mergeCell ref="O2:O9"/>
+    <mergeCell ref="P10:P13"/>
+    <mergeCell ref="AK6:AK7"/>
+    <mergeCell ref="AM12:AM15"/>
+    <mergeCell ref="AF18:AF19"/>
+    <mergeCell ref="AJ18:AJ19"/>
+    <mergeCell ref="Y1:Y27"/>
+    <mergeCell ref="AJ22:AJ23"/>
+    <mergeCell ref="AK9:AK10"/>
+    <mergeCell ref="AD3:AD4"/>
+    <mergeCell ref="S2:S3"/>
+    <mergeCell ref="R2:R3"/>
     <mergeCell ref="V21:V25"/>
     <mergeCell ref="U18:U20"/>
     <mergeCell ref="C2:C3"/>
@@ -9291,44 +9327,6 @@
     <mergeCell ref="B11:B12"/>
     <mergeCell ref="B6:B7"/>
     <mergeCell ref="B4:B5"/>
-    <mergeCell ref="AN1:AN27"/>
-    <mergeCell ref="P26:Q26"/>
-    <mergeCell ref="Q2:Q3"/>
-    <mergeCell ref="M2:M9"/>
-    <mergeCell ref="O2:O9"/>
-    <mergeCell ref="P10:P13"/>
-    <mergeCell ref="AK6:AK7"/>
-    <mergeCell ref="AM12:AM15"/>
-    <mergeCell ref="AF18:AF19"/>
-    <mergeCell ref="AJ18:AJ19"/>
-    <mergeCell ref="Y1:Y27"/>
-    <mergeCell ref="AJ22:AJ23"/>
-    <mergeCell ref="AK9:AK10"/>
-    <mergeCell ref="AD3:AD4"/>
-    <mergeCell ref="S2:S3"/>
-    <mergeCell ref="R2:R3"/>
-    <mergeCell ref="A5:A6"/>
-    <mergeCell ref="C6:D6"/>
-    <mergeCell ref="AI6:AI10"/>
-    <mergeCell ref="AF12:AF15"/>
-    <mergeCell ref="AG7:AG12"/>
-    <mergeCell ref="L8:L9"/>
-    <mergeCell ref="S9:S12"/>
-    <mergeCell ref="N8:N9"/>
-    <mergeCell ref="AD12:AD15"/>
-    <mergeCell ref="C15:C16"/>
-    <mergeCell ref="E2:E3"/>
-    <mergeCell ref="K2:L2"/>
-    <mergeCell ref="I1:I2"/>
-    <mergeCell ref="R18:R19"/>
-    <mergeCell ref="R26:R27"/>
-    <mergeCell ref="F2:F27"/>
-    <mergeCell ref="O10:O27"/>
-    <mergeCell ref="Q20:Q21"/>
-    <mergeCell ref="Q23:Q24"/>
-    <mergeCell ref="G14:J14"/>
-    <mergeCell ref="G13:J13"/>
-    <mergeCell ref="H12:K12"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -9338,7 +9336,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2029A93E-B53C-4201-9F17-439C144F3CF1}">
   <dimension ref="A1:AN37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="N1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="D14" workbookViewId="0">
       <selection activeCell="W25" sqref="W25"/>
     </sheetView>
   </sheetViews>
@@ -9434,10 +9432,10 @@
       <c r="S1" s="142"/>
       <c r="T1" s="142"/>
       <c r="U1" s="6"/>
-      <c r="V1" s="666" t="s">
+      <c r="V1" s="669" t="s">
         <v>459</v>
       </c>
-      <c r="W1" s="667"/>
+      <c r="W1" s="670"/>
       <c r="X1" s="312">
         <f>68-(U8+W3+V3+S3)</f>
         <v>0</v>
@@ -9453,21 +9451,21 @@
       <c r="AB1" s="308" t="s">
         <v>44</v>
       </c>
-      <c r="AC1" s="668" t="s">
+      <c r="AC1" s="671" t="s">
         <v>191</v>
       </c>
-      <c r="AD1" s="669"/>
-      <c r="AE1" s="670"/>
-      <c r="AF1" s="671" t="s">
+      <c r="AD1" s="672"/>
+      <c r="AE1" s="673"/>
+      <c r="AF1" s="674" t="s">
         <v>298</v>
       </c>
-      <c r="AG1" s="672"/>
-      <c r="AH1" s="673"/>
-      <c r="AI1" s="663" t="s">
+      <c r="AG1" s="675"/>
+      <c r="AH1" s="676"/>
+      <c r="AI1" s="666" t="s">
         <v>462</v>
       </c>
-      <c r="AJ1" s="664"/>
-      <c r="AK1" s="665"/>
+      <c r="AJ1" s="667"/>
+      <c r="AK1" s="668"/>
       <c r="AN1" s="142"/>
     </row>
     <row r="2" spans="1:40" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -9484,19 +9482,19 @@
       <c r="K2" s="327">
         <v>-3</v>
       </c>
-      <c r="L2" s="674">
+      <c r="L2" s="677">
         <f>SUM(L5:L30)</f>
         <v>2</v>
       </c>
-      <c r="M2" s="676">
+      <c r="M2" s="679">
         <f>SUM(M4:M29)</f>
         <v>6</v>
       </c>
-      <c r="N2" s="678">
+      <c r="N2" s="681">
         <f>SUM(N4:N29)</f>
         <v>5</v>
       </c>
-      <c r="O2" s="618">
+      <c r="O2" s="645">
         <f>SUM(M30:M37)* (-1)</f>
         <v>-1</v>
       </c>
@@ -9515,7 +9513,7 @@
       <c r="T2" s="517" t="s">
         <v>221</v>
       </c>
-      <c r="U2" s="680" t="s">
+      <c r="U2" s="683" t="s">
         <v>239</v>
       </c>
       <c r="V2" s="518" t="s">
@@ -9584,10 +9582,10 @@
         <f>T3+V3+W3+S3</f>
         <v>68</v>
       </c>
-      <c r="L3" s="675"/>
-      <c r="M3" s="677"/>
-      <c r="N3" s="679"/>
-      <c r="O3" s="619"/>
+      <c r="L3" s="678"/>
+      <c r="M3" s="680"/>
+      <c r="N3" s="682"/>
+      <c r="O3" s="646"/>
       <c r="P3" s="176">
         <f>(L2+M2)-W3</f>
         <v>0</v>
@@ -9603,7 +9601,7 @@
         <f>SUM(T4:T29)</f>
         <v>42</v>
       </c>
-      <c r="U3" s="681"/>
+      <c r="U3" s="684"/>
       <c r="V3" s="521">
         <f t="shared" ref="V3:AA3" si="0">SUM(V4:V29)</f>
         <v>6</v>
@@ -9702,7 +9700,7 @@
         <f>AA4</f>
         <v>0</v>
       </c>
-      <c r="O4" s="682" t="s">
+      <c r="O4" s="663" t="s">
         <v>200</v>
       </c>
       <c r="P4" s="20"/>
@@ -9781,7 +9779,7 @@
         <f>AA5</f>
         <v>0</v>
       </c>
-      <c r="O5" s="683"/>
+      <c r="O5" s="664"/>
       <c r="P5" s="20"/>
       <c r="Q5" s="2" t="s">
         <v>347</v>
@@ -9869,7 +9867,7 @@
         <f>AA6</f>
         <v>0</v>
       </c>
-      <c r="O6" s="683"/>
+      <c r="O6" s="664"/>
       <c r="P6" s="19" t="s">
         <v>342</v>
       </c>
@@ -9961,7 +9959,7 @@
         <f t="shared" ref="N7:N37" si="10">AA7</f>
         <v>0</v>
       </c>
-      <c r="O7" s="683"/>
+      <c r="O7" s="664"/>
       <c r="P7" s="20"/>
       <c r="Q7" s="2" t="s">
         <v>342</v>
@@ -10067,7 +10065,7 @@
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
-      <c r="O8" s="683"/>
+      <c r="O8" s="664"/>
       <c r="P8" s="21" t="s">
         <v>238</v>
       </c>
@@ -10151,7 +10149,7 @@
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
-      <c r="O9" s="683"/>
+      <c r="O9" s="664"/>
       <c r="P9" s="21" t="s">
         <v>342</v>
       </c>
@@ -10247,7 +10245,7 @@
         <f t="shared" si="10"/>
         <v>1</v>
       </c>
-      <c r="O10" s="683"/>
+      <c r="O10" s="664"/>
       <c r="P10" s="20"/>
       <c r="Q10" s="2" t="s">
         <v>347</v>
@@ -10328,7 +10326,7 @@
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
-      <c r="O11" s="683"/>
+      <c r="O11" s="664"/>
       <c r="P11" s="21" t="s">
         <v>342</v>
       </c>
@@ -10388,7 +10386,7 @@
       <c r="AN11" s="142"/>
     </row>
     <row r="12" spans="1:40" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="654" t="s">
+      <c r="A12" s="609" t="s">
         <v>55</v>
       </c>
       <c r="B12" s="30">
@@ -10397,7 +10395,7 @@
       <c r="C12" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="E12" s="608" t="s">
+      <c r="E12" s="660" t="s">
         <v>57</v>
       </c>
       <c r="G12" s="267"/>
@@ -10416,7 +10414,7 @@
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
-      <c r="O12" s="683"/>
+      <c r="O12" s="664"/>
       <c r="P12" s="21" t="s">
         <v>342</v>
       </c>
@@ -10484,14 +10482,14 @@
       </c>
     </row>
     <row r="13" spans="1:40" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="656"/>
+      <c r="A13" s="611"/>
       <c r="B13" s="153">
         <v>12</v>
       </c>
       <c r="C13" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="E13" s="609"/>
+      <c r="E13" s="661"/>
       <c r="F13" s="176">
         <v>0</v>
       </c>
@@ -10514,7 +10512,7 @@
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
-      <c r="O13" s="683"/>
+      <c r="O13" s="664"/>
       <c r="P13" s="21" t="s">
         <v>342</v>
       </c>
@@ -10587,7 +10585,7 @@
         <f t="shared" si="10"/>
         <v>1</v>
       </c>
-      <c r="O14" s="683"/>
+      <c r="O14" s="664"/>
       <c r="P14" s="20"/>
       <c r="Q14" s="205" t="s">
         <v>346</v>
@@ -10684,7 +10682,7 @@
         <f t="shared" si="10"/>
         <v>1</v>
       </c>
-      <c r="O15" s="683"/>
+      <c r="O15" s="664"/>
       <c r="P15" s="20"/>
       <c r="Q15" s="205" t="s">
         <v>346</v>
@@ -10771,7 +10769,7 @@
         <f t="shared" si="10"/>
         <v>1</v>
       </c>
-      <c r="O16" s="683"/>
+      <c r="O16" s="664"/>
       <c r="P16" s="21" t="s">
         <v>342</v>
       </c>
@@ -10867,7 +10865,7 @@
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
-      <c r="O17" s="683"/>
+      <c r="O17" s="664"/>
       <c r="P17" s="20"/>
       <c r="Q17" s="2" t="s">
         <v>348</v>
@@ -10951,7 +10949,7 @@
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
-      <c r="O18" s="683"/>
+      <c r="O18" s="664"/>
       <c r="P18" s="21" t="s">
         <v>342</v>
       </c>
@@ -11034,7 +11032,7 @@
         <f t="shared" si="10"/>
         <v>1</v>
       </c>
-      <c r="O19" s="683"/>
+      <c r="O19" s="664"/>
       <c r="P19" s="20"/>
       <c r="Q19" s="2" t="s">
         <v>341</v>
@@ -11130,11 +11128,11 @@
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
-      <c r="O20" s="684"/>
+      <c r="O20" s="665"/>
       <c r="P20" s="559" t="s">
         <v>342</v>
       </c>
-      <c r="Q20" s="610"/>
+      <c r="Q20" s="662"/>
       <c r="R20" s="321" t="s">
         <v>86</v>
       </c>
@@ -11369,7 +11367,7 @@
       <c r="AN22" s="142"/>
     </row>
     <row r="23" spans="1:40" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E23" s="661" t="s">
+      <c r="E23" s="616" t="s">
         <v>294</v>
       </c>
       <c r="F23" s="184"/>
@@ -11462,7 +11460,7 @@
       <c r="C24" s="2" t="s">
         <v>260</v>
       </c>
-      <c r="E24" s="662"/>
+      <c r="E24" s="617"/>
       <c r="F24" s="176"/>
       <c r="K24" s="403" t="s">
         <v>301</v>
@@ -11480,7 +11478,7 @@
       <c r="P24" s="559" t="s">
         <v>342</v>
       </c>
-      <c r="Q24" s="610"/>
+      <c r="Q24" s="662"/>
       <c r="R24" s="321" t="s">
         <v>254</v>
       </c>
@@ -12552,12 +12550,6 @@
     </row>
   </sheetData>
   <mergeCells count="15">
-    <mergeCell ref="A12:A13"/>
-    <mergeCell ref="E12:E13"/>
-    <mergeCell ref="P20:Q20"/>
-    <mergeCell ref="E23:E24"/>
-    <mergeCell ref="P24:Q24"/>
-    <mergeCell ref="O4:O20"/>
     <mergeCell ref="AI1:AK1"/>
     <mergeCell ref="V1:W1"/>
     <mergeCell ref="AC1:AE1"/>
@@ -12567,6 +12559,12 @@
     <mergeCell ref="N2:N3"/>
     <mergeCell ref="O2:O3"/>
     <mergeCell ref="U2:U3"/>
+    <mergeCell ref="A12:A13"/>
+    <mergeCell ref="E12:E13"/>
+    <mergeCell ref="P20:Q20"/>
+    <mergeCell ref="E23:E24"/>
+    <mergeCell ref="P24:Q24"/>
+    <mergeCell ref="O4:O20"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -12603,12 +12601,12 @@
       <c r="B1" s="559" t="s">
         <v>317</v>
       </c>
-      <c r="C1" s="610"/>
+      <c r="C1" s="662"/>
       <c r="D1" s="209"/>
       <c r="J1" s="559" t="s">
         <v>70</v>
       </c>
-      <c r="K1" s="610"/>
+      <c r="K1" s="662"/>
       <c r="L1" s="200" t="s">
         <v>337</v>
       </c>
@@ -12999,7 +12997,7 @@
       <c r="V1" s="559" t="s">
         <v>71</v>
       </c>
-      <c r="W1" s="610"/>
+      <c r="W1" s="662"/>
       <c r="X1" s="62" t="s">
         <v>102</v>
       </c>
@@ -13018,7 +13016,7 @@
       <c r="AC1" s="116" t="s">
         <v>191</v>
       </c>
-      <c r="AD1" s="698" t="s">
+      <c r="AD1" s="705" t="s">
         <v>213</v>
       </c>
       <c r="AE1" s="116" t="s">
@@ -13035,10 +13033,10 @@
       <c r="E2" s="39" t="s">
         <v>74</v>
       </c>
-      <c r="F2" s="697" t="s">
+      <c r="F2" s="736" t="s">
         <v>75</v>
       </c>
-      <c r="G2" s="725" t="s">
+      <c r="G2" s="693" t="s">
         <v>44</v>
       </c>
       <c r="H2" s="40" t="s">
@@ -13066,10 +13064,10 @@
       <c r="U2" s="60" t="s">
         <v>106</v>
       </c>
-      <c r="V2" s="666" t="s">
+      <c r="V2" s="669" t="s">
         <v>121</v>
       </c>
-      <c r="W2" s="667"/>
+      <c r="W2" s="670"/>
       <c r="X2" s="64" t="s">
         <v>110</v>
       </c>
@@ -13088,7 +13086,7 @@
       <c r="AC2" s="117" t="s">
         <v>99</v>
       </c>
-      <c r="AD2" s="699"/>
+      <c r="AD2" s="706"/>
       <c r="AE2" s="64" t="s">
         <v>99</v>
       </c>
@@ -13107,8 +13105,8 @@
       <c r="E3" s="39" t="s">
         <v>80</v>
       </c>
-      <c r="F3" s="658"/>
-      <c r="G3" s="726"/>
+      <c r="F3" s="613"/>
+      <c r="G3" s="694"/>
       <c r="H3" s="40" t="s">
         <v>81</v>
       </c>
@@ -13119,13 +13117,13 @@
         <v>82</v>
       </c>
       <c r="N3" s="44"/>
-      <c r="O3" s="735" t="s">
+      <c r="O3" s="703" t="s">
         <v>44</v>
       </c>
-      <c r="P3" s="717" t="s">
+      <c r="P3" s="724" t="s">
         <v>219</v>
       </c>
-      <c r="Q3" s="718"/>
+      <c r="Q3" s="725"/>
       <c r="S3" s="57" t="s">
         <v>220</v>
       </c>
@@ -13135,15 +13133,15 @@
       <c r="W3" s="59" t="s">
         <v>105</v>
       </c>
-      <c r="AD3" s="699"/>
+      <c r="AD3" s="706"/>
     </row>
     <row r="4" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="G4" s="726"/>
+      <c r="G4" s="694"/>
       <c r="H4" s="6"/>
       <c r="L4" s="688" t="s">
         <v>83</v>
       </c>
-      <c r="O4" s="736"/>
+      <c r="O4" s="704"/>
       <c r="T4" s="55" t="s">
         <v>98</v>
       </c>
@@ -13157,8 +13155,8 @@
         <v>195</v>
       </c>
       <c r="Z4" s="561"/>
-      <c r="AA4" s="610"/>
-      <c r="AD4" s="699"/>
+      <c r="AA4" s="662"/>
+      <c r="AD4" s="706"/>
     </row>
     <row r="5" spans="1:31" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C5" s="52" t="s">
@@ -13173,21 +13171,21 @@
       <c r="F5" s="66" t="s">
         <v>85</v>
       </c>
-      <c r="G5" s="726"/>
+      <c r="G5" s="694"/>
       <c r="H5" s="46" t="s">
         <v>76</v>
       </c>
-      <c r="K5" s="704" t="s">
+      <c r="K5" s="711" t="s">
         <v>217</v>
       </c>
-      <c r="L5" s="719"/>
+      <c r="L5" s="726"/>
       <c r="M5" s="2" t="s">
         <v>215</v>
       </c>
       <c r="N5" s="61" t="s">
         <v>214</v>
       </c>
-      <c r="O5" s="736"/>
+      <c r="O5" s="704"/>
       <c r="P5" s="108" t="s">
         <v>216</v>
       </c>
@@ -13203,11 +13201,11 @@
       <c r="U5" s="19" t="s">
         <v>99</v>
       </c>
-      <c r="Y5" s="707" t="s">
+      <c r="Y5" s="714" t="s">
         <v>287</v>
       </c>
-      <c r="Z5" s="708"/>
-      <c r="AD5" s="699"/>
+      <c r="Z5" s="715"/>
+      <c r="AD5" s="706"/>
     </row>
     <row r="6" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C6" s="109"/>
@@ -13217,16 +13215,16 @@
       <c r="E6" s="45" t="s">
         <v>86</v>
       </c>
-      <c r="G6" s="726"/>
+      <c r="G6" s="694"/>
       <c r="H6" s="46" t="s">
         <v>81</v>
       </c>
       <c r="I6" s="23">
         <v>15</v>
       </c>
-      <c r="K6" s="705"/>
-      <c r="L6" s="719"/>
-      <c r="O6" s="736"/>
+      <c r="K6" s="712"/>
+      <c r="L6" s="726"/>
+      <c r="O6" s="704"/>
       <c r="T6" s="2" t="s">
         <v>101</v>
       </c>
@@ -13236,23 +13234,23 @@
       <c r="V6" s="21">
         <v>-1</v>
       </c>
-      <c r="AD6" s="699"/>
+      <c r="AD6" s="706"/>
     </row>
     <row r="7" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C7" s="110"/>
-      <c r="G7" s="726"/>
+      <c r="G7" s="694"/>
       <c r="H7" s="6"/>
-      <c r="K7" s="705"/>
-      <c r="L7" s="719"/>
+      <c r="K7" s="712"/>
+      <c r="L7" s="726"/>
       <c r="N7" s="21" t="s">
         <v>120</v>
       </c>
-      <c r="O7" s="736"/>
+      <c r="O7" s="704"/>
       <c r="P7" s="73"/>
       <c r="U7" s="104" t="s">
         <v>20</v>
       </c>
-      <c r="AD7" s="699"/>
+      <c r="AD7" s="706"/>
     </row>
     <row r="8" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C8" s="130"/>
@@ -13265,7 +13263,7 @@
       <c r="F8" s="66" t="s">
         <v>87</v>
       </c>
-      <c r="G8" s="726"/>
+      <c r="G8" s="694"/>
       <c r="H8" s="50" t="s">
         <v>76</v>
       </c>
@@ -13275,41 +13273,41 @@
       <c r="J8" s="111">
         <v>115</v>
       </c>
-      <c r="K8" s="705"/>
-      <c r="L8" s="719"/>
-      <c r="O8" s="736"/>
+      <c r="K8" s="712"/>
+      <c r="L8" s="726"/>
+      <c r="O8" s="704"/>
       <c r="P8" s="49"/>
-      <c r="S8" s="701" t="s">
+      <c r="S8" s="708" t="s">
         <v>212</v>
       </c>
-      <c r="T8" s="702"/>
-      <c r="U8" s="702"/>
-      <c r="V8" s="702"/>
-      <c r="W8" s="702"/>
-      <c r="X8" s="702"/>
-      <c r="Y8" s="702"/>
-      <c r="Z8" s="702"/>
-      <c r="AA8" s="702"/>
-      <c r="AB8" s="702"/>
-      <c r="AC8" s="703"/>
-      <c r="AD8" s="699"/>
+      <c r="T8" s="709"/>
+      <c r="U8" s="709"/>
+      <c r="V8" s="709"/>
+      <c r="W8" s="709"/>
+      <c r="X8" s="709"/>
+      <c r="Y8" s="709"/>
+      <c r="Z8" s="709"/>
+      <c r="AA8" s="709"/>
+      <c r="AB8" s="709"/>
+      <c r="AC8" s="710"/>
+      <c r="AD8" s="706"/>
     </row>
     <row r="9" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C9" s="691"/>
-      <c r="G9" s="726"/>
+      <c r="C9" s="730"/>
+      <c r="G9" s="694"/>
       <c r="H9" s="6"/>
-      <c r="K9" s="705"/>
-      <c r="L9" s="729" t="s">
+      <c r="K9" s="712"/>
+      <c r="L9" s="697" t="s">
         <v>218</v>
       </c>
-      <c r="M9" s="730"/>
-      <c r="N9" s="731"/>
-      <c r="O9" s="736"/>
+      <c r="M9" s="698"/>
+      <c r="N9" s="699"/>
+      <c r="O9" s="704"/>
       <c r="P9" s="75"/>
-      <c r="AD9" s="699"/>
+      <c r="AD9" s="706"/>
     </row>
     <row r="10" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C10" s="692"/>
+      <c r="C10" s="731"/>
       <c r="D10" s="23"/>
       <c r="E10" s="45" t="s">
         <v>88</v>
@@ -13317,7 +13315,7 @@
       <c r="F10" s="66" t="s">
         <v>89</v>
       </c>
-      <c r="G10" s="726"/>
+      <c r="G10" s="694"/>
       <c r="H10" s="51"/>
       <c r="I10" s="21" t="s">
         <v>81</v>
@@ -13325,33 +13323,33 @@
       <c r="J10" s="3">
         <v>15</v>
       </c>
-      <c r="K10" s="705"/>
-      <c r="M10" s="694" t="s">
+      <c r="K10" s="712"/>
+      <c r="M10" s="733" t="s">
         <v>90</v>
       </c>
-      <c r="N10" s="695"/>
-      <c r="O10" s="695"/>
-      <c r="P10" s="695"/>
-      <c r="Q10" s="695"/>
-      <c r="R10" s="695"/>
-      <c r="S10" s="695"/>
-      <c r="T10" s="695"/>
-      <c r="U10" s="695"/>
-      <c r="V10" s="695"/>
-      <c r="W10" s="695"/>
-      <c r="X10" s="695"/>
-      <c r="Y10" s="695"/>
-      <c r="Z10" s="695"/>
-      <c r="AA10" s="695"/>
-      <c r="AB10" s="695"/>
-      <c r="AC10" s="696"/>
-      <c r="AD10" s="699"/>
+      <c r="N10" s="734"/>
+      <c r="O10" s="734"/>
+      <c r="P10" s="734"/>
+      <c r="Q10" s="734"/>
+      <c r="R10" s="734"/>
+      <c r="S10" s="734"/>
+      <c r="T10" s="734"/>
+      <c r="U10" s="734"/>
+      <c r="V10" s="734"/>
+      <c r="W10" s="734"/>
+      <c r="X10" s="734"/>
+      <c r="Y10" s="734"/>
+      <c r="Z10" s="734"/>
+      <c r="AA10" s="734"/>
+      <c r="AB10" s="734"/>
+      <c r="AC10" s="735"/>
+      <c r="AD10" s="706"/>
     </row>
     <row r="11" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C11" s="693"/>
-      <c r="G11" s="726"/>
+      <c r="C11" s="732"/>
+      <c r="G11" s="694"/>
       <c r="H11" s="6"/>
-      <c r="K11" s="705"/>
+      <c r="K11" s="712"/>
       <c r="R11" s="52" t="s">
         <v>44</v>
       </c>
@@ -13359,17 +13357,17 @@
       <c r="Y11" s="68" t="s">
         <v>121</v>
       </c>
-      <c r="Z11" s="715" t="s">
+      <c r="Z11" s="722" t="s">
         <v>121</v>
       </c>
-      <c r="AA11" s="716"/>
+      <c r="AA11" s="723"/>
       <c r="AB11" s="52" t="s">
         <v>44</v>
       </c>
       <c r="AC11" s="118" t="s">
         <v>121</v>
       </c>
-      <c r="AD11" s="699"/>
+      <c r="AD11" s="706"/>
     </row>
     <row r="12" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C12" s="129"/>
@@ -13382,7 +13380,7 @@
       <c r="F12" s="66" t="s">
         <v>92</v>
       </c>
-      <c r="G12" s="726"/>
+      <c r="G12" s="694"/>
       <c r="H12" s="128"/>
       <c r="I12" s="19" t="s">
         <v>81</v>
@@ -13390,8 +13388,8 @@
       <c r="J12" s="3">
         <v>15</v>
       </c>
-      <c r="K12" s="705"/>
-      <c r="L12" s="720" t="s">
+      <c r="K12" s="712"/>
+      <c r="L12" s="727" t="s">
         <v>93</v>
       </c>
       <c r="M12" s="21" t="s">
@@ -13422,25 +13420,25 @@
         <v>116</v>
       </c>
       <c r="Y12" s="6"/>
-      <c r="AA12" s="709" t="s">
+      <c r="AA12" s="716" t="s">
         <v>126</v>
       </c>
-      <c r="AB12" s="710"/>
+      <c r="AB12" s="717"/>
       <c r="AC12" s="21" t="s">
         <v>233</v>
       </c>
-      <c r="AD12" s="699"/>
+      <c r="AD12" s="706"/>
     </row>
     <row r="13" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C13" s="691"/>
-      <c r="G13" s="726"/>
-      <c r="K13" s="705"/>
-      <c r="L13" s="721"/>
+      <c r="C13" s="730"/>
+      <c r="G13" s="694"/>
+      <c r="K13" s="712"/>
+      <c r="L13" s="728"/>
       <c r="M13" s="47"/>
-      <c r="Q13" s="728" t="s">
+      <c r="Q13" s="696" t="s">
         <v>210</v>
       </c>
-      <c r="R13" s="625"/>
+      <c r="R13" s="622"/>
       <c r="S13" s="555"/>
       <c r="T13" s="6"/>
       <c r="U13" s="96" t="s">
@@ -13449,17 +13447,17 @@
       <c r="X13" s="2" t="s">
         <v>123</v>
       </c>
-      <c r="AA13" s="711"/>
-      <c r="AB13" s="712"/>
-      <c r="AD13" s="699"/>
+      <c r="AA13" s="718"/>
+      <c r="AB13" s="719"/>
+      <c r="AD13" s="706"/>
     </row>
     <row r="14" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B14" s="2" t="s">
         <v>339</v>
       </c>
-      <c r="C14" s="693"/>
+      <c r="C14" s="732"/>
       <c r="D14" s="23"/>
-      <c r="G14" s="726"/>
+      <c r="G14" s="694"/>
       <c r="H14" s="125"/>
       <c r="I14" s="99" t="s">
         <v>44</v>
@@ -13467,8 +13465,8 @@
       <c r="J14" s="111">
         <v>115</v>
       </c>
-      <c r="K14" s="705"/>
-      <c r="L14" s="721"/>
+      <c r="K14" s="712"/>
+      <c r="L14" s="728"/>
       <c r="M14" s="21" t="s">
         <v>111</v>
       </c>
@@ -13489,9 +13487,9 @@
       <c r="Y14" s="21" t="s">
         <v>73</v>
       </c>
-      <c r="AA14" s="711"/>
-      <c r="AB14" s="712"/>
-      <c r="AD14" s="699"/>
+      <c r="AA14" s="718"/>
+      <c r="AB14" s="719"/>
+      <c r="AD14" s="706"/>
     </row>
     <row r="15" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C15" s="130" t="s">
@@ -13506,19 +13504,19 @@
       <c r="F15" s="66" t="s">
         <v>94</v>
       </c>
-      <c r="G15" s="726"/>
+      <c r="G15" s="694"/>
       <c r="H15" s="2" t="s">
         <v>81</v>
       </c>
       <c r="I15" s="53" t="s">
         <v>81</v>
       </c>
-      <c r="K15" s="705"/>
-      <c r="L15" s="722"/>
-      <c r="Q15" s="728" t="s">
+      <c r="K15" s="712"/>
+      <c r="L15" s="729"/>
+      <c r="Q15" s="696" t="s">
         <v>211</v>
       </c>
-      <c r="R15" s="625"/>
+      <c r="R15" s="622"/>
       <c r="S15" s="555"/>
       <c r="T15" s="6"/>
       <c r="V15" s="68" t="s">
@@ -13527,14 +13525,14 @@
       <c r="X15" s="2" t="s">
         <v>128</v>
       </c>
-      <c r="AA15" s="711"/>
-      <c r="AB15" s="712"/>
-      <c r="AD15" s="699"/>
+      <c r="AA15" s="718"/>
+      <c r="AB15" s="719"/>
+      <c r="AD15" s="706"/>
     </row>
     <row r="16" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C16" s="132"/>
-      <c r="G16" s="726"/>
-      <c r="K16" s="705"/>
+      <c r="G16" s="694"/>
+      <c r="K16" s="712"/>
       <c r="N16" s="47"/>
       <c r="O16" s="61" t="s">
         <v>109</v>
@@ -13553,24 +13551,24 @@
       <c r="Z16" s="76" t="s">
         <v>127</v>
       </c>
-      <c r="AA16" s="711"/>
-      <c r="AB16" s="712"/>
-      <c r="AD16" s="699"/>
+      <c r="AA16" s="718"/>
+      <c r="AB16" s="719"/>
+      <c r="AD16" s="706"/>
     </row>
     <row r="17" spans="3:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C17" s="109"/>
       <c r="E17" s="6" t="s">
         <v>95</v>
       </c>
-      <c r="F17" s="723" t="s">
+      <c r="F17" s="691" t="s">
         <v>96</v>
       </c>
-      <c r="G17" s="726"/>
+      <c r="G17" s="694"/>
       <c r="H17" s="54"/>
       <c r="I17" s="133" t="s">
         <v>81</v>
       </c>
-      <c r="K17" s="705"/>
+      <c r="K17" s="712"/>
       <c r="S17" s="555"/>
       <c r="V17" s="68" t="s">
         <v>44</v>
@@ -13578,9 +13576,9 @@
       <c r="X17" s="2" t="s">
         <v>118</v>
       </c>
-      <c r="AA17" s="711"/>
-      <c r="AB17" s="712"/>
-      <c r="AD17" s="699"/>
+      <c r="AA17" s="718"/>
+      <c r="AB17" s="719"/>
+      <c r="AD17" s="706"/>
     </row>
     <row r="18" spans="3:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C18" s="130"/>
@@ -13590,15 +13588,15 @@
       <c r="E18" s="6" t="s">
         <v>97</v>
       </c>
-      <c r="F18" s="724"/>
-      <c r="G18" s="726"/>
+      <c r="F18" s="692"/>
+      <c r="G18" s="694"/>
       <c r="H18" s="108" t="s">
         <v>76</v>
       </c>
       <c r="I18" s="21" t="s">
         <v>81</v>
       </c>
-      <c r="K18" s="705"/>
+      <c r="K18" s="712"/>
       <c r="O18" s="64" t="s">
         <v>115</v>
       </c>
@@ -13609,42 +13607,39 @@
       <c r="X18" s="2" t="s">
         <v>117</v>
       </c>
-      <c r="AA18" s="713"/>
-      <c r="AB18" s="714"/>
-      <c r="AD18" s="699"/>
+      <c r="AA18" s="720"/>
+      <c r="AB18" s="721"/>
+      <c r="AD18" s="706"/>
     </row>
     <row r="19" spans="3:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="F19" s="64" t="s">
         <v>209</v>
       </c>
-      <c r="G19" s="727"/>
-      <c r="K19" s="706"/>
+      <c r="G19" s="695"/>
+      <c r="K19" s="713"/>
       <c r="Q19" s="68" t="s">
         <v>44</v>
       </c>
-      <c r="R19" s="732" t="s">
+      <c r="R19" s="700" t="s">
         <v>124</v>
       </c>
-      <c r="S19" s="733"/>
-      <c r="T19" s="734"/>
+      <c r="S19" s="701"/>
+      <c r="T19" s="702"/>
       <c r="V19" s="77" t="s">
         <v>115</v>
       </c>
       <c r="Y19" s="19" t="s">
         <v>125</v>
       </c>
-      <c r="AD19" s="700"/>
+      <c r="AD19" s="707"/>
     </row>
   </sheetData>
   <mergeCells count="24">
-    <mergeCell ref="F17:F18"/>
-    <mergeCell ref="G2:G19"/>
-    <mergeCell ref="Q13:R13"/>
-    <mergeCell ref="Q15:R15"/>
-    <mergeCell ref="L9:N9"/>
-    <mergeCell ref="R19:T19"/>
-    <mergeCell ref="S12:S18"/>
-    <mergeCell ref="O3:O9"/>
+    <mergeCell ref="C9:C11"/>
+    <mergeCell ref="C13:C14"/>
+    <mergeCell ref="V2:W2"/>
+    <mergeCell ref="M10:AC10"/>
+    <mergeCell ref="F2:F3"/>
     <mergeCell ref="AD1:AD19"/>
     <mergeCell ref="S8:AC8"/>
     <mergeCell ref="K5:K19"/>
@@ -13656,11 +13651,14 @@
     <mergeCell ref="P3:Q3"/>
     <mergeCell ref="L4:L8"/>
     <mergeCell ref="L12:L15"/>
-    <mergeCell ref="C9:C11"/>
-    <mergeCell ref="C13:C14"/>
-    <mergeCell ref="V2:W2"/>
-    <mergeCell ref="M10:AC10"/>
-    <mergeCell ref="F2:F3"/>
+    <mergeCell ref="F17:F18"/>
+    <mergeCell ref="G2:G19"/>
+    <mergeCell ref="Q13:R13"/>
+    <mergeCell ref="Q15:R15"/>
+    <mergeCell ref="L9:N9"/>
+    <mergeCell ref="R19:T19"/>
+    <mergeCell ref="S12:S18"/>
+    <mergeCell ref="O3:O9"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Boat Node Enabled - CNA
Boat Node Enabled - CNA

Boat Node - Enabled
</commit_message>
<xml_diff>
--- a/System_2.1.5.xlsx
+++ b/System_2.1.5.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Work\Work_For_\Work\Running AppS\System_Work_RW\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C136A8A2-048A-4016-AD26-A3AA438E4A5A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48A570F9-FB8E-4DC4-8524-7FE9F362FC19}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1077" uniqueCount="610">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1078" uniqueCount="610">
   <si>
     <t>Zone</t>
   </si>
@@ -3449,7 +3449,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="737">
+  <cellXfs count="736">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
@@ -4804,6 +4804,63 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="255" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="32" fillId="27" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="27" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="27" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="13" fillId="27" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="13" fillId="27" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="27" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="27" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="27" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="27" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="19" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="19" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="36" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="36" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="39" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -4834,62 +4891,167 @@
     <xf numFmtId="0" fontId="6" fillId="18" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="255"/>
     </xf>
-    <xf numFmtId="0" fontId="32" fillId="27" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="73" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="57" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="11" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="11" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="13" fillId="27" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="13" fillId="27" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="27" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="27" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="27" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="27" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="36" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="36" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="3" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="18" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="18" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="18" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="32" fillId="27" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="32" fillId="27" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="14" fontId="13" fillId="27" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="49" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="49" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="49" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="14" fontId="13" fillId="27" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="32" fillId="27" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="27" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="27" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="27" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="19" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="19" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="36" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="36" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="52" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="54" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="16" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="16" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="19" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -4915,12 +5077,6 @@
     <xf numFmtId="0" fontId="38" fillId="7" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255"/>
-    </xf>
     <xf numFmtId="0" fontId="17" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="255"/>
     </xf>
@@ -4942,161 +5098,14 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="52" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="54" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="16" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="16" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="3" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="18" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="18" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="18" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="49" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="49" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="49" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="73" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="57" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="11" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="11" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="13" fillId="27" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="13" fillId="27" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="27" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="27" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="27" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="27" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="36" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="36" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="11" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="3" fillId="35" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="35" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="35" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="43" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -5155,15 +5164,6 @@
     <xf numFmtId="0" fontId="6" fillId="52" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="35" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="35" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="35" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -5182,25 +5182,46 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="30" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="30" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="30" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="24" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="24" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="24" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="18" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -5278,49 +5299,27 @@
     <xf numFmtId="0" fontId="3" fillId="21" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="30" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="30" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="30" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="24" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="24" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="24" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="53" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -6566,8 +6565,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AB54FD83-008D-4F8B-87AC-83E7F70047CB}">
   <dimension ref="A1:AA32"/>
   <sheetViews>
-    <sheetView topLeftCell="H1" workbookViewId="0">
-      <selection activeCell="Z5" sqref="Z5"/>
+    <sheetView topLeftCell="H13" workbookViewId="0">
+      <selection activeCell="AA28" sqref="AA28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6624,7 +6623,7 @@
       <c r="P1" s="423" t="s">
         <v>408</v>
       </c>
-      <c r="Q1" s="564" t="s">
+      <c r="Q1" s="583" t="s">
         <v>181</v>
       </c>
       <c r="R1" s="100" t="s">
@@ -6644,32 +6643,32 @@
       </c>
     </row>
     <row r="2" spans="1:27" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="577">
+      <c r="A2" s="567">
         <f ca="1">TODAY()</f>
         <v>45279</v>
       </c>
-      <c r="B2" s="579" t="s">
+      <c r="B2" s="569" t="s">
         <v>389</v>
       </c>
-      <c r="C2" s="591" t="s">
+      <c r="C2" s="581" t="s">
         <v>365</v>
       </c>
-      <c r="D2" s="581" t="s">
+      <c r="D2" s="571" t="s">
         <v>103</v>
       </c>
-      <c r="E2" s="583" t="s">
+      <c r="E2" s="573" t="s">
         <v>65</v>
       </c>
       <c r="F2" s="196" t="s">
         <v>220</v>
       </c>
-      <c r="G2" s="589" t="s">
+      <c r="G2" s="579" t="s">
         <v>381</v>
       </c>
       <c r="H2" s="211" t="s">
         <v>220</v>
       </c>
-      <c r="I2" s="571" t="s">
+      <c r="I2" s="590" t="s">
         <v>103</v>
       </c>
       <c r="J2" s="421" t="s">
@@ -6693,14 +6692,14 @@
       <c r="P2" s="424">
         <v>40</v>
       </c>
-      <c r="Q2" s="565"/>
+      <c r="Q2" s="584"/>
       <c r="R2" s="21">
         <f>R7+R18</f>
         <v>6</v>
       </c>
       <c r="S2" s="21">
         <f>S7+S18</f>
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="T2" s="176">
         <f>SUM(T4:T16)</f>
@@ -6719,14 +6718,14 @@
       </c>
     </row>
     <row r="3" spans="1:27" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="578"/>
-      <c r="B3" s="580"/>
-      <c r="C3" s="592"/>
-      <c r="D3" s="582"/>
-      <c r="E3" s="584"/>
-      <c r="G3" s="590"/>
+      <c r="A3" s="568"/>
+      <c r="B3" s="570"/>
+      <c r="C3" s="582"/>
+      <c r="D3" s="572"/>
+      <c r="E3" s="574"/>
+      <c r="G3" s="580"/>
       <c r="H3" s="6"/>
-      <c r="I3" s="572"/>
+      <c r="I3" s="591"/>
       <c r="K3" s="24">
         <v>2</v>
       </c>
@@ -6735,7 +6734,7 @@
       </c>
       <c r="Q3" s="499">
         <f>SUM(X24:X32)</f>
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="U3" s="6"/>
       <c r="V3" s="497"/>
@@ -6751,10 +6750,10 @@
         <v>390</v>
       </c>
       <c r="B4" s="248"/>
-      <c r="C4" s="585" t="s">
+      <c r="C4" s="575" t="s">
         <v>178</v>
       </c>
-      <c r="I4" s="572"/>
+      <c r="I4" s="591"/>
       <c r="R4" s="499" t="s">
         <v>580</v>
       </c>
@@ -6778,7 +6777,7 @@
       <c r="B5" s="100" t="s">
         <v>365</v>
       </c>
-      <c r="C5" s="586"/>
+      <c r="C5" s="576"/>
       <c r="D5" s="227" t="s">
         <v>103</v>
       </c>
@@ -6794,7 +6793,7 @@
       <c r="H5" s="211" t="s">
         <v>220</v>
       </c>
-      <c r="I5" s="572"/>
+      <c r="I5" s="591"/>
       <c r="J5" s="422" t="s">
         <v>273</v>
       </c>
@@ -6825,22 +6824,22 @@
       <c r="X5" s="495"/>
     </row>
     <row r="6" spans="1:27" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="574" t="s">
+      <c r="A6" s="564" t="s">
         <v>290</v>
       </c>
       <c r="B6" s="105" t="s">
         <v>199</v>
       </c>
-      <c r="C6" s="587"/>
-      <c r="D6" s="588"/>
+      <c r="C6" s="577"/>
+      <c r="D6" s="578"/>
       <c r="E6" s="96">
         <v>1</v>
       </c>
       <c r="G6" s="554"/>
-      <c r="I6" s="572"/>
+      <c r="I6" s="591"/>
     </row>
     <row r="7" spans="1:27" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="575"/>
+      <c r="A7" s="565"/>
       <c r="B7" s="100" t="s">
         <v>155</v>
       </c>
@@ -6851,7 +6850,7 @@
         <v>136</v>
       </c>
       <c r="G7" s="554"/>
-      <c r="I7" s="572"/>
+      <c r="I7" s="591"/>
       <c r="M7" s="16" t="s">
         <v>354</v>
       </c>
@@ -6887,7 +6886,7 @@
       </c>
     </row>
     <row r="8" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="576"/>
+      <c r="A8" s="566"/>
       <c r="B8" s="217" t="s">
         <v>28</v>
       </c>
@@ -6896,7 +6895,7 @@
         <v>3</v>
       </c>
       <c r="G8" s="554"/>
-      <c r="I8" s="572"/>
+      <c r="I8" s="591"/>
       <c r="N8" s="80"/>
       <c r="U8" s="6" t="s">
         <v>466</v>
@@ -6920,7 +6919,7 @@
       </c>
       <c r="G9" s="554"/>
       <c r="H9" s="6"/>
-      <c r="I9" s="572"/>
+      <c r="I9" s="591"/>
       <c r="M9" s="19" t="s">
         <v>547</v>
       </c>
@@ -6947,7 +6946,7 @@
         <v>41</v>
       </c>
       <c r="G10" s="554"/>
-      <c r="I10" s="572"/>
+      <c r="I10" s="591"/>
       <c r="J10" s="24" t="s">
         <v>381</v>
       </c>
@@ -6981,7 +6980,7 @@
         <v>270</v>
       </c>
       <c r="G11" s="554"/>
-      <c r="I11" s="572"/>
+      <c r="I11" s="591"/>
       <c r="J11" s="24" t="s">
         <v>195</v>
       </c>
@@ -7007,12 +7006,12 @@
       <c r="S11" s="24">
         <v>1</v>
       </c>
-      <c r="U11" s="566" t="s">
+      <c r="U11" s="585" t="s">
         <v>583</v>
       </c>
-      <c r="V11" s="567"/>
-      <c r="W11" s="567"/>
-      <c r="X11" s="568"/>
+      <c r="V11" s="586"/>
+      <c r="W11" s="586"/>
+      <c r="X11" s="587"/>
     </row>
     <row r="12" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="232" t="s">
@@ -7023,7 +7022,7 @@
         <v>3</v>
       </c>
       <c r="G12" s="554"/>
-      <c r="I12" s="572"/>
+      <c r="I12" s="591"/>
       <c r="J12" s="24" t="s">
         <v>538</v>
       </c>
@@ -7056,7 +7055,7 @@
       </c>
       <c r="D13" s="20"/>
       <c r="G13" s="554"/>
-      <c r="I13" s="572"/>
+      <c r="I13" s="591"/>
       <c r="J13" s="108" t="s">
         <v>572</v>
       </c>
@@ -7097,7 +7096,7 @@
       <c r="H14" s="211" t="s">
         <v>220</v>
       </c>
-      <c r="I14" s="572"/>
+      <c r="I14" s="591"/>
       <c r="U14" s="6"/>
       <c r="V14" s="112"/>
       <c r="W14" s="6"/>
@@ -7115,7 +7114,7 @@
       <c r="H15" s="277">
         <v>0</v>
       </c>
-      <c r="I15" s="572"/>
+      <c r="I15" s="591"/>
       <c r="J15" s="108" t="s">
         <v>154</v>
       </c>
@@ -7146,7 +7145,7 @@
       <c r="D16" s="2" t="s">
         <v>510</v>
       </c>
-      <c r="I16" s="572"/>
+      <c r="I16" s="591"/>
       <c r="K16" s="100" t="s">
         <v>44</v>
       </c>
@@ -7180,7 +7179,7 @@
       <c r="G17" s="2" t="s">
         <v>441</v>
       </c>
-      <c r="I17" s="572"/>
+      <c r="I17" s="591"/>
       <c r="L17" s="2" t="s">
         <v>444</v>
       </c>
@@ -7192,13 +7191,13 @@
     </row>
     <row r="18" spans="1:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="G18" s="16"/>
-      <c r="I18" s="572"/>
+      <c r="I18" s="591"/>
       <c r="L18" s="16"/>
       <c r="M18" s="21"/>
-      <c r="O18" s="569" t="s">
+      <c r="O18" s="588" t="s">
         <v>539</v>
       </c>
-      <c r="P18" s="570"/>
+      <c r="P18" s="589"/>
       <c r="Q18" s="127" t="s">
         <v>44</v>
       </c>
@@ -7208,7 +7207,7 @@
       </c>
       <c r="S18" s="24">
         <f>5-S26</f>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="U18" s="6" t="s">
         <v>479</v>
@@ -7224,7 +7223,7 @@
       </c>
     </row>
     <row r="19" spans="1:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="I19" s="572"/>
+      <c r="I19" s="591"/>
       <c r="M19" s="21" t="s">
         <v>443</v>
       </c>
@@ -7256,7 +7255,7 @@
       <c r="G20" s="2" t="s">
         <v>441</v>
       </c>
-      <c r="I20" s="572"/>
+      <c r="I20" s="591"/>
       <c r="K20" s="19" t="s">
         <v>440</v>
       </c>
@@ -7281,7 +7280,7 @@
       <c r="Z20" s="112"/>
     </row>
     <row r="21" spans="1:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="I21" s="572"/>
+      <c r="I21" s="591"/>
       <c r="M21" s="221" t="s">
         <v>422</v>
       </c>
@@ -7291,8 +7290,12 @@
       <c r="V21" s="24">
         <v>1</v>
       </c>
-      <c r="W21" s="6"/>
-      <c r="X21" s="497"/>
+      <c r="W21" s="6" t="s">
+        <v>486</v>
+      </c>
+      <c r="X21" s="497">
+        <v>1</v>
+      </c>
     </row>
     <row r="22" spans="1:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="236" t="s">
@@ -7313,7 +7316,7 @@
       <c r="G22" s="2" t="s">
         <v>441</v>
       </c>
-      <c r="I22" s="572"/>
+      <c r="I22" s="591"/>
       <c r="U22" s="6"/>
       <c r="V22" s="495"/>
       <c r="W22" s="6" t="s">
@@ -7333,13 +7336,13 @@
       <c r="E23" s="289" t="s">
         <v>44</v>
       </c>
-      <c r="I23" s="572"/>
+      <c r="I23" s="591"/>
       <c r="U23" s="6"/>
       <c r="V23" s="24"/>
       <c r="W23" s="6"/>
     </row>
     <row r="24" spans="1:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="I24" s="572"/>
+      <c r="I24" s="591"/>
       <c r="U24" s="354"/>
       <c r="V24" s="498">
         <v>-1</v>
@@ -7367,7 +7370,7 @@
       <c r="H25" s="196" t="s">
         <v>271</v>
       </c>
-      <c r="I25" s="572"/>
+      <c r="I25" s="591"/>
       <c r="J25" s="422" t="s">
         <v>274</v>
       </c>
@@ -7412,7 +7415,7 @@
       <c r="H26" s="19" t="s">
         <v>220</v>
       </c>
-      <c r="I26" s="572"/>
+      <c r="I26" s="591"/>
       <c r="K26" s="24">
         <v>15</v>
       </c>
@@ -7430,7 +7433,7 @@
         <v>2</v>
       </c>
       <c r="S26" s="24">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="T26" s="61" t="s">
         <v>581</v>
@@ -7447,7 +7450,7 @@
       </c>
     </row>
     <row r="27" spans="1:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="I27" s="572"/>
+      <c r="I27" s="591"/>
       <c r="O27" s="2" t="s">
         <v>99</v>
       </c>
@@ -7474,7 +7477,7 @@
       <c r="E28" s="220">
         <v>2</v>
       </c>
-      <c r="I28" s="572"/>
+      <c r="I28" s="591"/>
       <c r="Q28" s="6"/>
       <c r="R28" s="112"/>
       <c r="T28" s="142"/>
@@ -7496,7 +7499,7 @@
       <c r="H29" s="196" t="s">
         <v>272</v>
       </c>
-      <c r="I29" s="573"/>
+      <c r="I29" s="592"/>
       <c r="J29" s="333"/>
       <c r="L29" s="96" t="s">
         <v>278</v>
@@ -7555,17 +7558,22 @@
     <row r="32" spans="1:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="U32" s="514"/>
       <c r="V32" s="501">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="W32" s="19" t="s">
         <v>486</v>
       </c>
       <c r="X32" s="24">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="16">
+    <mergeCell ref="Q1:Q2"/>
+    <mergeCell ref="U11:X11"/>
+    <mergeCell ref="O18:P18"/>
+    <mergeCell ref="I2:I29"/>
+    <mergeCell ref="C13:C14"/>
     <mergeCell ref="A6:A8"/>
     <mergeCell ref="G5:G14"/>
     <mergeCell ref="A2:A3"/>
@@ -7577,11 +7585,6 @@
     <mergeCell ref="B11:B12"/>
     <mergeCell ref="G2:G3"/>
     <mergeCell ref="C2:C3"/>
-    <mergeCell ref="Q1:Q2"/>
-    <mergeCell ref="U11:X11"/>
-    <mergeCell ref="O18:P18"/>
-    <mergeCell ref="I2:I29"/>
-    <mergeCell ref="C13:C14"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -7591,7 +7594,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A8CFE6D2-5300-4D31-9A66-EC93F2A54B69}">
   <dimension ref="A1:AQ27"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A9" workbookViewId="0">
       <selection activeCell="N16" sqref="N16"/>
     </sheetView>
   </sheetViews>
@@ -7657,7 +7660,7 @@
       <c r="H1" s="97" t="s">
         <v>350</v>
       </c>
-      <c r="I1" s="589" t="s">
+      <c r="I1" s="579" t="s">
         <v>378</v>
       </c>
       <c r="J1" s="2" t="s">
@@ -7718,7 +7721,7 @@
         <v>517</v>
       </c>
       <c r="AM1" s="427"/>
-      <c r="AN1" s="620"/>
+      <c r="AN1" s="617"/>
       <c r="AO1" s="350" t="s">
         <v>487</v>
       </c>
@@ -7727,23 +7730,23 @@
       </c>
     </row>
     <row r="2" spans="1:43" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="644">
+      <c r="A2" s="599">
         <f ca="1">TODAY()</f>
         <v>45279</v>
       </c>
-      <c r="B2" s="646" t="s">
+      <c r="B2" s="601" t="s">
         <v>379</v>
       </c>
-      <c r="C2" s="591" t="s">
+      <c r="C2" s="581" t="s">
         <v>365</v>
       </c>
-      <c r="D2" s="648" t="s">
+      <c r="D2" s="603" t="s">
         <v>362</v>
       </c>
-      <c r="E2" s="593" t="s">
+      <c r="E2" s="647" t="s">
         <v>65</v>
       </c>
-      <c r="F2" s="601" t="s">
+      <c r="F2" s="622" t="s">
         <v>103</v>
       </c>
       <c r="G2" s="418" t="s">
@@ -7752,31 +7755,31 @@
       <c r="H2" s="80" t="s">
         <v>33</v>
       </c>
-      <c r="I2" s="590"/>
+      <c r="I2" s="580"/>
       <c r="J2" s="81" t="s">
         <v>77</v>
       </c>
-      <c r="K2" s="595" t="s">
+      <c r="K2" s="649" t="s">
         <v>349</v>
       </c>
-      <c r="L2" s="596"/>
-      <c r="M2" s="601" t="s">
+      <c r="L2" s="650"/>
+      <c r="M2" s="622" t="s">
         <v>103</v>
       </c>
       <c r="N2" s="69" t="s">
         <v>28</v>
       </c>
-      <c r="O2" s="627" t="s">
+      <c r="O2" s="626" t="s">
         <v>103</v>
       </c>
       <c r="P2" s="85" t="s">
         <v>148</v>
       </c>
-      <c r="Q2" s="591" t="s">
+      <c r="Q2" s="581" t="s">
         <v>144</v>
       </c>
       <c r="R2" s="553"/>
-      <c r="S2" s="614" t="s">
+      <c r="S2" s="639" t="s">
         <v>149</v>
       </c>
       <c r="T2" s="89"/>
@@ -7809,15 +7812,15 @@
         <v>481</v>
       </c>
       <c r="AM2" s="453"/>
-      <c r="AN2" s="621"/>
+      <c r="AN2" s="618"/>
     </row>
     <row r="3" spans="1:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="645"/>
-      <c r="B3" s="647"/>
-      <c r="C3" s="592"/>
-      <c r="D3" s="649"/>
-      <c r="E3" s="594"/>
-      <c r="F3" s="602"/>
+      <c r="A3" s="600"/>
+      <c r="B3" s="602"/>
+      <c r="C3" s="582"/>
+      <c r="D3" s="604"/>
+      <c r="E3" s="648"/>
+      <c r="F3" s="623"/>
       <c r="G3" s="419" t="s">
         <v>28</v>
       </c>
@@ -7836,17 +7839,17 @@
       <c r="L3" s="206" t="s">
         <v>108</v>
       </c>
-      <c r="M3" s="602"/>
+      <c r="M3" s="623"/>
       <c r="N3" s="69" t="s">
         <v>147</v>
       </c>
-      <c r="O3" s="628"/>
+      <c r="O3" s="627"/>
       <c r="P3" s="2" t="s">
         <v>155</v>
       </c>
-      <c r="Q3" s="592"/>
+      <c r="Q3" s="582"/>
       <c r="R3" s="555"/>
-      <c r="S3" s="616"/>
+      <c r="S3" s="640"/>
       <c r="T3" s="89"/>
       <c r="U3" s="124"/>
       <c r="V3" s="120"/>
@@ -7863,7 +7866,7 @@
       <c r="AC3" s="100" t="s">
         <v>498</v>
       </c>
-      <c r="AD3" s="611" t="s">
+      <c r="AD3" s="638" t="s">
         <v>473</v>
       </c>
       <c r="AE3" s="262"/>
@@ -7875,16 +7878,16 @@
       <c r="AK3" s="262"/>
       <c r="AL3" s="16"/>
       <c r="AM3" s="453"/>
-      <c r="AN3" s="621"/>
+      <c r="AN3" s="618"/>
     </row>
     <row r="4" spans="1:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="243" t="s">
         <v>184</v>
       </c>
-      <c r="B4" s="660" t="s">
+      <c r="B4" s="615" t="s">
         <v>382</v>
       </c>
-      <c r="C4" s="591" t="s">
+      <c r="C4" s="581" t="s">
         <v>155</v>
       </c>
       <c r="D4" s="359" t="s">
@@ -7893,7 +7896,7 @@
       <c r="E4" s="396">
         <v>2</v>
       </c>
-      <c r="F4" s="602"/>
+      <c r="F4" s="623"/>
       <c r="G4" s="400" t="s">
         <v>203</v>
       </c>
@@ -7910,11 +7913,11 @@
         <v>151</v>
       </c>
       <c r="L4" s="209"/>
-      <c r="M4" s="602"/>
+      <c r="M4" s="623"/>
       <c r="N4" s="178" t="s">
         <v>70</v>
       </c>
-      <c r="O4" s="628"/>
+      <c r="O4" s="627"/>
       <c r="P4" s="2" t="s">
         <v>192</v>
       </c>
@@ -7941,7 +7944,7 @@
       <c r="AA4" s="313"/>
       <c r="AB4" s="214"/>
       <c r="AC4" s="16"/>
-      <c r="AD4" s="611"/>
+      <c r="AD4" s="638"/>
       <c r="AE4" s="262"/>
       <c r="AF4" s="262"/>
       <c r="AG4" s="16"/>
@@ -7951,37 +7954,37 @@
       <c r="AK4" s="262"/>
       <c r="AL4" s="16"/>
       <c r="AM4" s="453"/>
-      <c r="AN4" s="621"/>
+      <c r="AN4" s="618"/>
       <c r="AO4" s="350" t="s">
         <v>91</v>
       </c>
     </row>
     <row r="5" spans="1:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="589" t="s">
+      <c r="A5" s="579" t="s">
         <v>435</v>
       </c>
-      <c r="B5" s="661"/>
-      <c r="C5" s="592"/>
+      <c r="B5" s="616"/>
+      <c r="C5" s="582"/>
       <c r="D5" s="61" t="s">
         <v>154</v>
       </c>
       <c r="E5" s="397">
         <v>1</v>
       </c>
-      <c r="F5" s="602"/>
-      <c r="G5" s="652" t="s">
+      <c r="F5" s="623"/>
+      <c r="G5" s="607" t="s">
         <v>193</v>
       </c>
-      <c r="H5" s="652"/>
-      <c r="I5" s="652"/>
-      <c r="J5" s="652"/>
-      <c r="K5" s="652"/>
-      <c r="L5" s="653"/>
-      <c r="M5" s="602"/>
+      <c r="H5" s="607"/>
+      <c r="I5" s="607"/>
+      <c r="J5" s="607"/>
+      <c r="K5" s="607"/>
+      <c r="L5" s="608"/>
+      <c r="M5" s="623"/>
       <c r="N5" s="21">
         <v>8</v>
       </c>
-      <c r="O5" s="628"/>
+      <c r="O5" s="627"/>
       <c r="T5" s="89"/>
       <c r="U5" s="124"/>
       <c r="V5" s="120"/>
@@ -8012,24 +8015,24 @@
       <c r="AK5" s="262"/>
       <c r="AL5" s="80"/>
       <c r="AM5" s="453"/>
-      <c r="AN5" s="621"/>
+      <c r="AN5" s="618"/>
     </row>
     <row r="6" spans="1:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="590"/>
-      <c r="B6" s="658" t="s">
+      <c r="A6" s="580"/>
+      <c r="B6" s="613" t="s">
         <v>178</v>
       </c>
-      <c r="C6" s="587"/>
-      <c r="D6" s="588"/>
-      <c r="F6" s="602"/>
-      <c r="G6" s="654"/>
-      <c r="H6" s="654"/>
-      <c r="I6" s="654"/>
-      <c r="J6" s="654"/>
-      <c r="K6" s="654"/>
-      <c r="L6" s="655"/>
-      <c r="M6" s="602"/>
-      <c r="O6" s="628"/>
+      <c r="C6" s="577"/>
+      <c r="D6" s="578"/>
+      <c r="F6" s="623"/>
+      <c r="G6" s="609"/>
+      <c r="H6" s="609"/>
+      <c r="I6" s="609"/>
+      <c r="J6" s="609"/>
+      <c r="K6" s="609"/>
+      <c r="L6" s="610"/>
+      <c r="M6" s="623"/>
+      <c r="O6" s="627"/>
       <c r="T6" s="89"/>
       <c r="U6" s="124"/>
       <c r="V6" s="98" t="s">
@@ -8053,16 +8056,16 @@
       <c r="AF6" s="262"/>
       <c r="AG6" s="262"/>
       <c r="AH6" s="262"/>
-      <c r="AI6" s="610"/>
+      <c r="AI6" s="632"/>
       <c r="AJ6" s="466" t="s">
         <v>476</v>
       </c>
-      <c r="AK6" s="610" t="s">
+      <c r="AK6" s="632" t="s">
         <v>256</v>
       </c>
       <c r="AL6" s="262"/>
       <c r="AM6" s="453"/>
-      <c r="AN6" s="621"/>
+      <c r="AN6" s="618"/>
       <c r="AO6" s="350" t="s">
         <v>488</v>
       </c>
@@ -8071,7 +8074,7 @@
       <c r="A7" s="237" t="s">
         <v>598</v>
       </c>
-      <c r="B7" s="659"/>
+      <c r="B7" s="614"/>
       <c r="C7" s="207" t="s">
         <v>383</v>
       </c>
@@ -8081,7 +8084,7 @@
       <c r="E7" s="271">
         <v>3</v>
       </c>
-      <c r="F7" s="602"/>
+      <c r="F7" s="623"/>
       <c r="G7" s="420">
         <v>0</v>
       </c>
@@ -8100,8 +8103,8 @@
       <c r="L7" s="217">
         <v>0</v>
       </c>
-      <c r="M7" s="602"/>
-      <c r="O7" s="628"/>
+      <c r="M7" s="623"/>
+      <c r="O7" s="627"/>
       <c r="R7" s="99" t="s">
         <v>44</v>
       </c>
@@ -8125,18 +8128,18 @@
       <c r="AD7" s="16"/>
       <c r="AE7" s="262"/>
       <c r="AF7" s="262"/>
-      <c r="AG7" s="611" t="s">
+      <c r="AG7" s="638" t="s">
         <v>472</v>
       </c>
       <c r="AH7" s="262"/>
-      <c r="AI7" s="610"/>
+      <c r="AI7" s="632"/>
       <c r="AJ7" s="262"/>
-      <c r="AK7" s="610"/>
+      <c r="AK7" s="632"/>
       <c r="AL7" s="80" t="s">
         <v>515</v>
       </c>
       <c r="AM7" s="453"/>
-      <c r="AN7" s="621"/>
+      <c r="AN7" s="618"/>
       <c r="AP7" s="76" t="s">
         <v>489</v>
       </c>
@@ -8153,27 +8156,27 @@
         <f>SUM(G7:N9)</f>
         <v>15</v>
       </c>
-      <c r="F8" s="602"/>
-      <c r="G8" s="653">
-        <v>0</v>
-      </c>
-      <c r="H8" s="650" t="s">
+      <c r="F8" s="623"/>
+      <c r="G8" s="608">
+        <v>0</v>
+      </c>
+      <c r="H8" s="605" t="s">
         <v>105</v>
       </c>
       <c r="I8" s="553">
         <v>0</v>
       </c>
-      <c r="J8" s="650" t="s">
+      <c r="J8" s="605" t="s">
         <v>105</v>
       </c>
-      <c r="K8" s="656"/>
-      <c r="L8" s="612"/>
-      <c r="M8" s="625"/>
-      <c r="N8" s="617">
+      <c r="K8" s="611"/>
+      <c r="L8" s="641"/>
+      <c r="M8" s="624"/>
+      <c r="N8" s="644">
         <f>N5+N11</f>
         <v>15</v>
       </c>
-      <c r="O8" s="628"/>
+      <c r="O8" s="627"/>
       <c r="T8" s="103" t="s">
         <v>44</v>
       </c>
@@ -8191,14 +8194,14 @@
       <c r="AD8" s="16"/>
       <c r="AE8" s="262"/>
       <c r="AF8" s="262"/>
-      <c r="AG8" s="611"/>
+      <c r="AG8" s="638"/>
       <c r="AH8" s="262"/>
-      <c r="AI8" s="610"/>
+      <c r="AI8" s="632"/>
       <c r="AJ8" s="262"/>
       <c r="AK8" s="262"/>
       <c r="AL8" s="262"/>
       <c r="AM8" s="453"/>
-      <c r="AN8" s="621"/>
+      <c r="AN8" s="618"/>
     </row>
     <row r="9" spans="1:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="237" t="s">
@@ -8213,17 +8216,17 @@
       <c r="D9" s="360" t="s">
         <v>286</v>
       </c>
-      <c r="F9" s="602"/>
-      <c r="G9" s="655"/>
-      <c r="H9" s="651"/>
+      <c r="F9" s="623"/>
+      <c r="G9" s="610"/>
+      <c r="H9" s="606"/>
       <c r="I9" s="555"/>
-      <c r="J9" s="651"/>
-      <c r="K9" s="657"/>
-      <c r="L9" s="613"/>
-      <c r="M9" s="626"/>
-      <c r="N9" s="618"/>
-      <c r="O9" s="629"/>
-      <c r="S9" s="614" t="s">
+      <c r="J9" s="606"/>
+      <c r="K9" s="612"/>
+      <c r="L9" s="642"/>
+      <c r="M9" s="625"/>
+      <c r="N9" s="645"/>
+      <c r="O9" s="628"/>
+      <c r="S9" s="639" t="s">
         <v>62</v>
       </c>
       <c r="T9" s="89"/>
@@ -8245,16 +8248,16 @@
       </c>
       <c r="AE9" s="262"/>
       <c r="AF9" s="262"/>
-      <c r="AG9" s="611"/>
+      <c r="AG9" s="638"/>
       <c r="AH9" s="262"/>
-      <c r="AI9" s="610"/>
+      <c r="AI9" s="632"/>
       <c r="AJ9" s="80"/>
-      <c r="AK9" s="610" t="s">
+      <c r="AK9" s="632" t="s">
         <v>256</v>
       </c>
       <c r="AL9" s="262"/>
       <c r="AM9" s="453"/>
-      <c r="AN9" s="621"/>
+      <c r="AN9" s="618"/>
       <c r="AP9" s="2" t="s">
         <v>527</v>
       </c>
@@ -8271,20 +8274,20 @@
         <f>Boat!U8</f>
         <v>41</v>
       </c>
-      <c r="F10" s="602"/>
+      <c r="F10" s="623"/>
       <c r="N10" s="443" t="s">
         <v>407</v>
       </c>
-      <c r="O10" s="604" t="s">
+      <c r="O10" s="656" t="s">
         <v>103</v>
       </c>
-      <c r="P10" s="630" t="s">
+      <c r="P10" s="629" t="s">
         <v>411</v>
       </c>
       <c r="R10" s="74" t="s">
         <v>44</v>
       </c>
-      <c r="S10" s="615"/>
+      <c r="S10" s="643"/>
       <c r="T10" s="89"/>
       <c r="U10" s="123" t="s">
         <v>177</v>
@@ -8314,16 +8317,16 @@
       <c r="AF10" s="243" t="s">
         <v>318</v>
       </c>
-      <c r="AG10" s="611"/>
+      <c r="AG10" s="638"/>
       <c r="AH10" s="80"/>
-      <c r="AI10" s="610"/>
+      <c r="AI10" s="632"/>
       <c r="AJ10" s="262"/>
-      <c r="AK10" s="610"/>
+      <c r="AK10" s="632"/>
       <c r="AL10" s="262"/>
       <c r="AM10" s="467" t="s">
         <v>325</v>
       </c>
-      <c r="AN10" s="621"/>
+      <c r="AN10" s="618"/>
       <c r="AO10" s="209" t="s">
         <v>95</v>
       </c>
@@ -8341,18 +8344,18 @@
       <c r="D11" s="174" t="s">
         <v>362</v>
       </c>
-      <c r="F11" s="602"/>
+      <c r="F11" s="623"/>
       <c r="M11" s="6"/>
       <c r="N11" s="117">
         <v>7</v>
       </c>
-      <c r="O11" s="605"/>
-      <c r="P11" s="631"/>
+      <c r="O11" s="657"/>
+      <c r="P11" s="630"/>
       <c r="Q11" s="65"/>
       <c r="R11" s="120" t="s">
         <v>222</v>
       </c>
-      <c r="S11" s="615"/>
+      <c r="S11" s="643"/>
       <c r="T11" s="102" t="s">
         <v>44</v>
       </c>
@@ -8376,14 +8379,14 @@
       <c r="AF11" s="262" t="s">
         <v>494</v>
       </c>
-      <c r="AG11" s="611"/>
+      <c r="AG11" s="638"/>
       <c r="AH11" s="262"/>
       <c r="AI11" s="70"/>
       <c r="AJ11" s="262"/>
       <c r="AK11" s="262"/>
       <c r="AL11" s="262"/>
       <c r="AM11" s="453"/>
-      <c r="AN11" s="621"/>
+      <c r="AN11" s="618"/>
       <c r="AP11" s="76" t="s">
         <v>502</v>
       </c>
@@ -8402,7 +8405,7 @@
       <c r="E12" s="229">
         <v>3</v>
       </c>
-      <c r="F12" s="602"/>
+      <c r="F12" s="623"/>
       <c r="G12" s="349" t="s">
         <v>411</v>
       </c>
@@ -8411,16 +8414,16 @@
       </c>
       <c r="I12" s="560"/>
       <c r="J12" s="560"/>
-      <c r="K12" s="609"/>
+      <c r="K12" s="661"/>
       <c r="L12" s="208"/>
       <c r="M12" s="208"/>
       <c r="N12" s="208"/>
-      <c r="O12" s="605"/>
-      <c r="P12" s="631"/>
+      <c r="O12" s="657"/>
+      <c r="P12" s="630"/>
       <c r="R12" s="122" t="s">
         <v>181</v>
       </c>
-      <c r="S12" s="616"/>
+      <c r="S12" s="640"/>
       <c r="T12" s="101" t="s">
         <v>44</v>
       </c>
@@ -8441,16 +8444,16 @@
       <c r="AC12" s="100" t="s">
         <v>499</v>
       </c>
-      <c r="AD12" s="619" t="s">
+      <c r="AD12" s="646" t="s">
         <v>245</v>
       </c>
       <c r="AE12" s="466" t="s">
         <v>244</v>
       </c>
-      <c r="AF12" s="611" t="s">
+      <c r="AF12" s="638" t="s">
         <v>231</v>
       </c>
-      <c r="AG12" s="611"/>
+      <c r="AG12" s="638"/>
       <c r="AH12" s="243" t="s">
         <v>264</v>
       </c>
@@ -8463,7 +8466,7 @@
       <c r="AM12" s="633" t="s">
         <v>254</v>
       </c>
-      <c r="AN12" s="621"/>
+      <c r="AN12" s="618"/>
       <c r="AO12" s="350" t="s">
         <v>97</v>
       </c>
@@ -8475,17 +8478,17 @@
       <c r="E13" s="473">
         <v>-3</v>
       </c>
-      <c r="F13" s="602"/>
+      <c r="F13" s="623"/>
       <c r="G13" s="560" t="s">
         <v>448</v>
       </c>
       <c r="H13" s="560"/>
       <c r="I13" s="560"/>
-      <c r="J13" s="609"/>
+      <c r="J13" s="661"/>
       <c r="M13" s="6"/>
       <c r="N13" s="6"/>
-      <c r="O13" s="605"/>
-      <c r="P13" s="632"/>
+      <c r="O13" s="657"/>
+      <c r="P13" s="631"/>
       <c r="T13" s="105" t="s">
         <v>44</v>
       </c>
@@ -8506,8 +8509,8 @@
         <v>519</v>
       </c>
       <c r="AC13" s="16"/>
-      <c r="AD13" s="619"/>
-      <c r="AF13" s="611"/>
+      <c r="AD13" s="646"/>
+      <c r="AF13" s="638"/>
       <c r="AG13" s="80"/>
       <c r="AH13" s="243" t="s">
         <v>314</v>
@@ -8519,7 +8522,7 @@
       <c r="AK13" s="262"/>
       <c r="AL13" s="262"/>
       <c r="AM13" s="633"/>
-      <c r="AN13" s="621"/>
+      <c r="AN13" s="618"/>
     </row>
     <row r="14" spans="1:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="475"/>
@@ -8527,18 +8530,18 @@
       <c r="C14" s="484"/>
       <c r="D14" s="477"/>
       <c r="E14" s="478"/>
-      <c r="F14" s="602"/>
+      <c r="F14" s="623"/>
       <c r="G14" s="560" t="s">
         <v>447</v>
       </c>
       <c r="H14" s="560"/>
       <c r="I14" s="560"/>
-      <c r="J14" s="609"/>
+      <c r="J14" s="661"/>
       <c r="K14" s="2">
         <v>12</v>
       </c>
       <c r="N14" s="6"/>
-      <c r="O14" s="605"/>
+      <c r="O14" s="657"/>
       <c r="Q14" s="61" t="s">
         <v>555</v>
       </c>
@@ -8559,9 +8562,9 @@
       <c r="AA14" s="313"/>
       <c r="AB14" s="214"/>
       <c r="AC14" s="16"/>
-      <c r="AD14" s="619"/>
+      <c r="AD14" s="646"/>
       <c r="AE14" s="262"/>
-      <c r="AF14" s="611"/>
+      <c r="AF14" s="638"/>
       <c r="AG14" s="262"/>
       <c r="AH14" s="262"/>
       <c r="AI14" s="70"/>
@@ -8569,7 +8572,7 @@
       <c r="AK14" s="262"/>
       <c r="AL14" s="262"/>
       <c r="AM14" s="633"/>
-      <c r="AN14" s="621"/>
+      <c r="AN14" s="618"/>
     </row>
     <row r="15" spans="1:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="474" t="s">
@@ -8578,8 +8581,8 @@
       <c r="C15" s="553" t="s">
         <v>382</v>
       </c>
-      <c r="F15" s="602"/>
-      <c r="O15" s="605"/>
+      <c r="F15" s="623"/>
+      <c r="O15" s="657"/>
       <c r="R15" s="99" t="s">
         <v>44</v>
       </c>
@@ -8601,8 +8604,8 @@
       <c r="AC15" s="76" t="s">
         <v>497</v>
       </c>
-      <c r="AD15" s="619"/>
-      <c r="AF15" s="611"/>
+      <c r="AD15" s="646"/>
+      <c r="AF15" s="638"/>
       <c r="AG15" s="80"/>
       <c r="AH15" s="243" t="s">
         <v>466</v>
@@ -8616,7 +8619,7 @@
       <c r="AK15" s="262"/>
       <c r="AL15" s="262"/>
       <c r="AM15" s="633"/>
-      <c r="AN15" s="621"/>
+      <c r="AN15" s="618"/>
       <c r="AP15" s="76" t="s">
         <v>74</v>
       </c>
@@ -8638,13 +8641,13 @@
       <c r="E16" s="229">
         <v>1</v>
       </c>
-      <c r="F16" s="602"/>
+      <c r="F16" s="623"/>
       <c r="G16" s="349" t="s">
         <v>506</v>
       </c>
       <c r="I16" s="496"/>
       <c r="J16" s="20"/>
-      <c r="O16" s="605"/>
+      <c r="O16" s="657"/>
       <c r="R16" s="460" t="s">
         <v>185</v>
       </c>
@@ -8676,18 +8679,18 @@
       <c r="AM16" s="453" t="s">
         <v>324</v>
       </c>
-      <c r="AN16" s="621"/>
+      <c r="AN16" s="618"/>
       <c r="AP16" s="76" t="s">
         <v>235</v>
       </c>
     </row>
     <row r="17" spans="1:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B17" s="80"/>
-      <c r="F17" s="602"/>
+      <c r="F17" s="623"/>
       <c r="I17" s="497"/>
       <c r="J17" s="20"/>
       <c r="N17" s="6"/>
-      <c r="O17" s="605"/>
+      <c r="O17" s="657"/>
       <c r="Q17" s="21" t="s">
         <v>553</v>
       </c>
@@ -8732,7 +8735,7 @@
       <c r="AK17" s="262"/>
       <c r="AL17" s="80"/>
       <c r="AM17" s="453"/>
-      <c r="AN17" s="621"/>
+      <c r="AN17" s="618"/>
       <c r="AO17" s="209" t="s">
         <v>516</v>
       </c>
@@ -8756,21 +8759,21 @@
       <c r="E18" s="99" t="s">
         <v>44</v>
       </c>
-      <c r="F18" s="602"/>
+      <c r="F18" s="623"/>
       <c r="G18" s="349" t="s">
         <v>550</v>
       </c>
       <c r="I18" s="24"/>
       <c r="J18" s="20"/>
-      <c r="O18" s="605"/>
+      <c r="O18" s="657"/>
       <c r="Q18" s="112"/>
-      <c r="R18" s="597" t="s">
+      <c r="R18" s="651" t="s">
         <v>558</v>
       </c>
       <c r="T18" s="100" t="s">
         <v>44</v>
       </c>
-      <c r="U18" s="641" t="s">
+      <c r="U18" s="596" t="s">
         <v>44</v>
       </c>
       <c r="V18" s="120"/>
@@ -8791,7 +8794,7 @@
       <c r="AC18" s="16"/>
       <c r="AD18" s="16"/>
       <c r="AE18" s="262"/>
-      <c r="AF18" s="610" t="s">
+      <c r="AF18" s="632" t="s">
         <v>493</v>
       </c>
       <c r="AG18" s="262"/>
@@ -8803,20 +8806,20 @@
       <c r="AK18" s="262"/>
       <c r="AL18" s="80"/>
       <c r="AM18" s="453"/>
-      <c r="AN18" s="621"/>
+      <c r="AN18" s="618"/>
       <c r="AP18" s="76" t="s">
         <v>88</v>
       </c>
     </row>
     <row r="19" spans="1:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="F19" s="602"/>
+      <c r="F19" s="623"/>
       <c r="I19" s="224"/>
-      <c r="O19" s="605"/>
-      <c r="R19" s="598"/>
+      <c r="O19" s="657"/>
+      <c r="R19" s="652"/>
       <c r="S19" s="30" t="s">
         <v>556</v>
       </c>
-      <c r="U19" s="642"/>
+      <c r="U19" s="597"/>
       <c r="V19" s="146"/>
       <c r="W19" s="146"/>
       <c r="X19" s="456" t="s">
@@ -8831,7 +8834,7 @@
       <c r="AC19" s="16"/>
       <c r="AD19" s="16"/>
       <c r="AE19" s="262"/>
-      <c r="AF19" s="610"/>
+      <c r="AF19" s="632"/>
       <c r="AG19" s="262"/>
       <c r="AH19" s="262"/>
       <c r="AI19" s="70"/>
@@ -8841,7 +8844,7 @@
       </c>
       <c r="AL19" s="80"/>
       <c r="AM19" s="453"/>
-      <c r="AN19" s="621"/>
+      <c r="AN19" s="618"/>
       <c r="AP19" s="76" t="s">
         <v>486</v>
       </c>
@@ -8862,19 +8865,19 @@
       <c r="E20" s="462">
         <v>-1</v>
       </c>
-      <c r="F20" s="602"/>
+      <c r="F20" s="623"/>
       <c r="G20" s="349" t="s">
         <v>509</v>
       </c>
       <c r="I20" s="224"/>
-      <c r="O20" s="605"/>
-      <c r="Q20" s="607" t="s">
+      <c r="O20" s="657"/>
+      <c r="Q20" s="659" t="s">
         <v>48</v>
       </c>
       <c r="T20" s="429" t="s">
         <v>44</v>
       </c>
-      <c r="U20" s="643"/>
+      <c r="U20" s="598"/>
       <c r="W20" s="430"/>
       <c r="X20" s="457" t="s">
         <v>175</v>
@@ -8904,7 +8907,7 @@
       <c r="AM20" s="400" t="s">
         <v>254</v>
       </c>
-      <c r="AN20" s="621"/>
+      <c r="AN20" s="618"/>
       <c r="AO20" s="350" t="s">
         <v>478</v>
       </c>
@@ -8925,13 +8928,13 @@
       <c r="E21" s="271">
         <v>0</v>
       </c>
-      <c r="F21" s="602"/>
+      <c r="F21" s="623"/>
       <c r="I21" s="224"/>
-      <c r="O21" s="605"/>
-      <c r="Q21" s="608"/>
+      <c r="O21" s="657"/>
+      <c r="Q21" s="660"/>
       <c r="T21" s="447"/>
       <c r="U21" s="14"/>
-      <c r="V21" s="638"/>
+      <c r="V21" s="593"/>
       <c r="W21" s="451" t="s">
         <v>176</v>
       </c>
@@ -8969,15 +8972,15 @@
       <c r="AM21" s="453" t="s">
         <v>567</v>
       </c>
-      <c r="AN21" s="621"/>
+      <c r="AN21" s="618"/>
     </row>
     <row r="22" spans="1:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="F22" s="602"/>
+      <c r="F22" s="623"/>
       <c r="G22" s="349" t="s">
         <v>507</v>
       </c>
       <c r="I22" s="224"/>
-      <c r="O22" s="605"/>
+      <c r="O22" s="657"/>
       <c r="R22" s="459" t="s">
         <v>44</v>
       </c>
@@ -8985,7 +8988,7 @@
         <v>44</v>
       </c>
       <c r="U22" s="15"/>
-      <c r="V22" s="639"/>
+      <c r="V22" s="594"/>
       <c r="W22" s="451" t="s">
         <v>176</v>
       </c>
@@ -9003,7 +9006,7 @@
       <c r="AG22" s="6"/>
       <c r="AH22" s="6"/>
       <c r="AI22" s="6"/>
-      <c r="AJ22" s="610" t="s">
+      <c r="AJ22" s="632" t="s">
         <v>490</v>
       </c>
       <c r="AK22" s="262"/>
@@ -9011,7 +9014,7 @@
         <v>496</v>
       </c>
       <c r="AM22" s="306"/>
-      <c r="AN22" s="621"/>
+      <c r="AN22" s="618"/>
     </row>
     <row r="23" spans="1:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="236" t="s">
@@ -9029,17 +9032,17 @@
       <c r="E23" s="230">
         <v>1</v>
       </c>
-      <c r="F23" s="602"/>
+      <c r="F23" s="623"/>
       <c r="I23" s="224"/>
-      <c r="O23" s="605"/>
-      <c r="Q23" s="607" t="s">
+      <c r="O23" s="657"/>
+      <c r="Q23" s="659" t="s">
         <v>145</v>
       </c>
       <c r="T23" s="17"/>
       <c r="U23" s="445" t="s">
         <v>44</v>
       </c>
-      <c r="V23" s="639"/>
+      <c r="V23" s="594"/>
       <c r="W23" s="148"/>
       <c r="X23" s="454" t="s">
         <v>189</v>
@@ -9055,13 +9058,13 @@
       <c r="AG23" s="6"/>
       <c r="AH23" s="6"/>
       <c r="AI23" s="6"/>
-      <c r="AJ23" s="610"/>
+      <c r="AJ23" s="632"/>
       <c r="AK23" s="262"/>
       <c r="AL23" s="80" t="s">
         <v>526</v>
       </c>
       <c r="AM23" s="306"/>
-      <c r="AN23" s="621"/>
+      <c r="AN23" s="618"/>
     </row>
     <row r="24" spans="1:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="465" t="s">
@@ -9079,18 +9082,18 @@
       <c r="E24" s="461">
         <v>1</v>
       </c>
-      <c r="F24" s="602"/>
+      <c r="F24" s="623"/>
       <c r="G24" s="61" t="s">
         <v>508</v>
       </c>
       <c r="I24" s="224"/>
-      <c r="O24" s="605"/>
-      <c r="Q24" s="608"/>
+      <c r="O24" s="657"/>
+      <c r="Q24" s="660"/>
       <c r="T24" s="17"/>
       <c r="U24" s="232" t="s">
         <v>44</v>
       </c>
-      <c r="V24" s="639"/>
+      <c r="V24" s="594"/>
       <c r="W24" s="148"/>
       <c r="X24" s="454" t="s">
         <v>186</v>
@@ -9114,12 +9117,12 @@
         <v>481</v>
       </c>
       <c r="AM24" s="306"/>
-      <c r="AN24" s="621"/>
+      <c r="AN24" s="618"/>
     </row>
     <row r="25" spans="1:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="F25" s="602"/>
+      <c r="F25" s="623"/>
       <c r="I25" s="224"/>
-      <c r="O25" s="605"/>
+      <c r="O25" s="657"/>
       <c r="P25" s="209" t="s">
         <v>285</v>
       </c>
@@ -9132,7 +9135,7 @@
       <c r="U25" s="425" t="s">
         <v>44</v>
       </c>
-      <c r="V25" s="640"/>
+      <c r="V25" s="595"/>
       <c r="W25" s="148"/>
       <c r="X25" s="454" t="s">
         <v>190</v>
@@ -9154,7 +9157,7 @@
       <c r="AK25" s="142"/>
       <c r="AL25" s="6"/>
       <c r="AM25" s="306"/>
-      <c r="AN25" s="621"/>
+      <c r="AN25" s="618"/>
     </row>
     <row r="26" spans="1:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="236" t="s">
@@ -9172,17 +9175,17 @@
       <c r="E26" s="398">
         <v>1</v>
       </c>
-      <c r="F26" s="602"/>
+      <c r="F26" s="623"/>
       <c r="G26" s="349" t="s">
         <v>505</v>
       </c>
       <c r="I26" s="224"/>
-      <c r="O26" s="605"/>
-      <c r="P26" s="623" t="s">
+      <c r="O26" s="657"/>
+      <c r="P26" s="620" t="s">
         <v>548</v>
       </c>
-      <c r="Q26" s="624"/>
-      <c r="R26" s="599" t="s">
+      <c r="Q26" s="621"/>
+      <c r="R26" s="653" t="s">
         <v>557</v>
       </c>
       <c r="T26" s="182"/>
@@ -9221,7 +9224,7 @@
       <c r="AM26" s="467" t="s">
         <v>474</v>
       </c>
-      <c r="AN26" s="621"/>
+      <c r="AN26" s="618"/>
     </row>
     <row r="27" spans="1:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B27" s="21" t="s">
@@ -9233,13 +9236,13 @@
       <c r="E27" s="271" t="s">
         <v>44</v>
       </c>
-      <c r="F27" s="603"/>
+      <c r="F27" s="655"/>
       <c r="G27" s="61" t="s">
         <v>566</v>
       </c>
       <c r="I27" s="225"/>
-      <c r="O27" s="606"/>
-      <c r="R27" s="600"/>
+      <c r="O27" s="658"/>
+      <c r="R27" s="654"/>
       <c r="S27" s="446" t="s">
         <v>54</v>
       </c>
@@ -9269,10 +9272,48 @@
       <c r="AM27" s="400" t="s">
         <v>326</v>
       </c>
-      <c r="AN27" s="622"/>
+      <c r="AN27" s="619"/>
     </row>
   </sheetData>
   <mergeCells count="54">
+    <mergeCell ref="E2:E3"/>
+    <mergeCell ref="K2:L2"/>
+    <mergeCell ref="I1:I2"/>
+    <mergeCell ref="R18:R19"/>
+    <mergeCell ref="R26:R27"/>
+    <mergeCell ref="F2:F27"/>
+    <mergeCell ref="O10:O27"/>
+    <mergeCell ref="Q20:Q21"/>
+    <mergeCell ref="Q23:Q24"/>
+    <mergeCell ref="G14:J14"/>
+    <mergeCell ref="G13:J13"/>
+    <mergeCell ref="H12:K12"/>
+    <mergeCell ref="A5:A6"/>
+    <mergeCell ref="C6:D6"/>
+    <mergeCell ref="AI6:AI10"/>
+    <mergeCell ref="AF12:AF15"/>
+    <mergeCell ref="AG7:AG12"/>
+    <mergeCell ref="L8:L9"/>
+    <mergeCell ref="S9:S12"/>
+    <mergeCell ref="N8:N9"/>
+    <mergeCell ref="AD12:AD15"/>
+    <mergeCell ref="C15:C16"/>
+    <mergeCell ref="AN1:AN27"/>
+    <mergeCell ref="P26:Q26"/>
+    <mergeCell ref="Q2:Q3"/>
+    <mergeCell ref="M2:M9"/>
+    <mergeCell ref="O2:O9"/>
+    <mergeCell ref="P10:P13"/>
+    <mergeCell ref="AK6:AK7"/>
+    <mergeCell ref="AM12:AM15"/>
+    <mergeCell ref="AF18:AF19"/>
+    <mergeCell ref="AJ18:AJ19"/>
+    <mergeCell ref="Y1:Y27"/>
+    <mergeCell ref="AJ22:AJ23"/>
+    <mergeCell ref="AK9:AK10"/>
+    <mergeCell ref="AD3:AD4"/>
+    <mergeCell ref="S2:S3"/>
+    <mergeCell ref="R2:R3"/>
     <mergeCell ref="V21:V25"/>
     <mergeCell ref="U18:U20"/>
     <mergeCell ref="C2:C3"/>
@@ -9289,44 +9330,6 @@
     <mergeCell ref="B11:B12"/>
     <mergeCell ref="B6:B7"/>
     <mergeCell ref="B4:B5"/>
-    <mergeCell ref="AN1:AN27"/>
-    <mergeCell ref="P26:Q26"/>
-    <mergeCell ref="Q2:Q3"/>
-    <mergeCell ref="M2:M9"/>
-    <mergeCell ref="O2:O9"/>
-    <mergeCell ref="P10:P13"/>
-    <mergeCell ref="AK6:AK7"/>
-    <mergeCell ref="AM12:AM15"/>
-    <mergeCell ref="AF18:AF19"/>
-    <mergeCell ref="AJ18:AJ19"/>
-    <mergeCell ref="Y1:Y27"/>
-    <mergeCell ref="AJ22:AJ23"/>
-    <mergeCell ref="AK9:AK10"/>
-    <mergeCell ref="AD3:AD4"/>
-    <mergeCell ref="S2:S3"/>
-    <mergeCell ref="R2:R3"/>
-    <mergeCell ref="A5:A6"/>
-    <mergeCell ref="C6:D6"/>
-    <mergeCell ref="AI6:AI10"/>
-    <mergeCell ref="AF12:AF15"/>
-    <mergeCell ref="AG7:AG12"/>
-    <mergeCell ref="L8:L9"/>
-    <mergeCell ref="S9:S12"/>
-    <mergeCell ref="N8:N9"/>
-    <mergeCell ref="AD12:AD15"/>
-    <mergeCell ref="C15:C16"/>
-    <mergeCell ref="E2:E3"/>
-    <mergeCell ref="K2:L2"/>
-    <mergeCell ref="I1:I2"/>
-    <mergeCell ref="R18:R19"/>
-    <mergeCell ref="R26:R27"/>
-    <mergeCell ref="F2:F27"/>
-    <mergeCell ref="O10:O27"/>
-    <mergeCell ref="Q20:Q21"/>
-    <mergeCell ref="Q23:Q24"/>
-    <mergeCell ref="G14:J14"/>
-    <mergeCell ref="G13:J13"/>
-    <mergeCell ref="H12:K12"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -9336,8 +9339,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2029A93E-B53C-4201-9F17-439C144F3CF1}">
   <dimension ref="A1:AN37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="N7" workbookViewId="0">
-      <selection activeCell="AL11" sqref="AL11"/>
+    <sheetView tabSelected="1" topLeftCell="M1" workbookViewId="0">
+      <selection activeCell="AH31" sqref="AH31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9432,10 +9435,10 @@
       <c r="S1" s="142"/>
       <c r="T1" s="142"/>
       <c r="U1" s="6"/>
-      <c r="V1" s="665" t="s">
+      <c r="V1" s="668" t="s">
         <v>459</v>
       </c>
-      <c r="W1" s="666"/>
+      <c r="W1" s="669"/>
       <c r="X1" s="312">
         <f>68-(U8+W3+V3+S3)</f>
         <v>0</v>
@@ -9451,21 +9454,21 @@
       <c r="AB1" s="308" t="s">
         <v>44</v>
       </c>
-      <c r="AC1" s="667" t="s">
+      <c r="AC1" s="670" t="s">
         <v>191</v>
       </c>
-      <c r="AD1" s="668"/>
-      <c r="AE1" s="669"/>
-      <c r="AF1" s="670" t="s">
+      <c r="AD1" s="671"/>
+      <c r="AE1" s="672"/>
+      <c r="AF1" s="673" t="s">
         <v>298</v>
       </c>
-      <c r="AG1" s="671"/>
-      <c r="AH1" s="672"/>
-      <c r="AI1" s="662" t="s">
+      <c r="AG1" s="674"/>
+      <c r="AH1" s="675"/>
+      <c r="AI1" s="665" t="s">
         <v>462</v>
       </c>
-      <c r="AJ1" s="663"/>
-      <c r="AK1" s="664"/>
+      <c r="AJ1" s="666"/>
+      <c r="AK1" s="667"/>
       <c r="AN1" s="142"/>
     </row>
     <row r="2" spans="1:40" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -9482,21 +9485,21 @@
       <c r="K2" s="327">
         <v>-3</v>
       </c>
-      <c r="L2" s="673">
+      <c r="L2" s="676">
         <f>SUM(L5:L30)</f>
         <v>2</v>
       </c>
-      <c r="M2" s="675">
+      <c r="M2" s="678">
         <f>SUM(M4:M29)</f>
         <v>7</v>
       </c>
-      <c r="N2" s="677">
+      <c r="N2" s="680">
         <f>SUM(N4:N29)</f>
         <v>6</v>
       </c>
-      <c r="O2" s="617">
+      <c r="O2" s="644">
         <f>SUM(M30:M37)* (-1)</f>
-        <v>-1</v>
+        <v>-3</v>
       </c>
       <c r="P2" s="275" t="s">
         <v>243</v>
@@ -9513,7 +9516,7 @@
       <c r="T2" s="516" t="s">
         <v>221</v>
       </c>
-      <c r="U2" s="679" t="s">
+      <c r="U2" s="682" t="s">
         <v>239</v>
       </c>
       <c r="V2" s="517" t="s">
@@ -9582,10 +9585,10 @@
         <f>T3+V3+W3+S3</f>
         <v>68</v>
       </c>
-      <c r="L3" s="674"/>
-      <c r="M3" s="676"/>
-      <c r="N3" s="678"/>
-      <c r="O3" s="618"/>
+      <c r="L3" s="677"/>
+      <c r="M3" s="679"/>
+      <c r="N3" s="681"/>
+      <c r="O3" s="645"/>
       <c r="P3" s="176">
         <f>(L2+M2)-W3</f>
         <v>0</v>
@@ -9601,7 +9604,7 @@
         <f>SUM(T4:T29)</f>
         <v>41</v>
       </c>
-      <c r="U3" s="680"/>
+      <c r="U3" s="683"/>
       <c r="V3" s="520">
         <f t="shared" ref="V3:AA3" si="0">SUM(V4:V29)</f>
         <v>6</v>
@@ -9700,7 +9703,7 @@
         <f>AA4</f>
         <v>0</v>
       </c>
-      <c r="O4" s="681" t="s">
+      <c r="O4" s="662" t="s">
         <v>200</v>
       </c>
       <c r="P4" s="20"/>
@@ -9779,7 +9782,7 @@
         <f>AA5</f>
         <v>0</v>
       </c>
-      <c r="O5" s="682"/>
+      <c r="O5" s="663"/>
       <c r="P5" s="20"/>
       <c r="Q5" s="2" t="s">
         <v>347</v>
@@ -9867,7 +9870,7 @@
         <f>AA6</f>
         <v>0</v>
       </c>
-      <c r="O6" s="682"/>
+      <c r="O6" s="663"/>
       <c r="P6" s="19" t="s">
         <v>342</v>
       </c>
@@ -9958,7 +9961,7 @@
         <f t="shared" ref="N7:N37" si="10">AA7</f>
         <v>0</v>
       </c>
-      <c r="O7" s="682"/>
+      <c r="O7" s="663"/>
       <c r="P7" s="20"/>
       <c r="Q7" s="2" t="s">
         <v>342</v>
@@ -10064,7 +10067,7 @@
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
-      <c r="O8" s="682"/>
+      <c r="O8" s="663"/>
       <c r="P8" s="21" t="s">
         <v>238</v>
       </c>
@@ -10148,7 +10151,7 @@
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
-      <c r="O9" s="682"/>
+      <c r="O9" s="663"/>
       <c r="P9" s="21" t="s">
         <v>342</v>
       </c>
@@ -10244,7 +10247,7 @@
         <f t="shared" si="10"/>
         <v>1</v>
       </c>
-      <c r="O10" s="682"/>
+      <c r="O10" s="663"/>
       <c r="P10" s="20"/>
       <c r="Q10" s="2" t="s">
         <v>347</v>
@@ -10325,7 +10328,7 @@
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
-      <c r="O11" s="682"/>
+      <c r="O11" s="663"/>
       <c r="P11" s="21" t="s">
         <v>342</v>
       </c>
@@ -10385,7 +10388,7 @@
       <c r="AN11" s="142"/>
     </row>
     <row r="12" spans="1:40" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="653" t="s">
+      <c r="A12" s="608" t="s">
         <v>55</v>
       </c>
       <c r="B12" s="30">
@@ -10394,7 +10397,7 @@
       <c r="C12" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="E12" s="607" t="s">
+      <c r="E12" s="659" t="s">
         <v>57</v>
       </c>
       <c r="G12" s="267"/>
@@ -10412,7 +10415,7 @@
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
-      <c r="O12" s="682"/>
+      <c r="O12" s="663"/>
       <c r="P12" s="21" t="s">
         <v>342</v>
       </c>
@@ -10480,14 +10483,14 @@
       </c>
     </row>
     <row r="13" spans="1:40" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="655"/>
+      <c r="A13" s="610"/>
       <c r="B13" s="153">
         <v>12</v>
       </c>
       <c r="C13" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="E13" s="608"/>
+      <c r="E13" s="660"/>
       <c r="F13" s="176">
         <v>0</v>
       </c>
@@ -10510,7 +10513,7 @@
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
-      <c r="O13" s="682"/>
+      <c r="O13" s="663"/>
       <c r="P13" s="21" t="s">
         <v>342</v>
       </c>
@@ -10583,7 +10586,7 @@
         <f t="shared" si="10"/>
         <v>1</v>
       </c>
-      <c r="O14" s="682"/>
+      <c r="O14" s="663"/>
       <c r="P14" s="20"/>
       <c r="Q14" s="205" t="s">
         <v>346</v>
@@ -10680,7 +10683,7 @@
         <f t="shared" si="10"/>
         <v>1</v>
       </c>
-      <c r="O15" s="682"/>
+      <c r="O15" s="663"/>
       <c r="P15" s="20"/>
       <c r="Q15" s="205" t="s">
         <v>346</v>
@@ -10767,7 +10770,7 @@
         <f t="shared" si="10"/>
         <v>1</v>
       </c>
-      <c r="O16" s="682"/>
+      <c r="O16" s="663"/>
       <c r="P16" s="21" t="s">
         <v>342</v>
       </c>
@@ -10865,7 +10868,7 @@
         <f t="shared" si="10"/>
         <v>1</v>
       </c>
-      <c r="O17" s="682"/>
+      <c r="O17" s="663"/>
       <c r="P17" s="20"/>
       <c r="Q17" s="2" t="s">
         <v>348</v>
@@ -10929,8 +10932,8 @@
       <c r="AL17" s="6" t="s">
         <v>97</v>
       </c>
-      <c r="AM17" s="736" t="s">
-        <v>468</v>
+      <c r="AM17" s="546" t="s">
+        <v>589</v>
       </c>
       <c r="AN17" s="64" t="s">
         <v>95</v>
@@ -10960,7 +10963,7 @@
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
-      <c r="O18" s="682"/>
+      <c r="O18" s="663"/>
       <c r="P18" s="21" t="s">
         <v>342</v>
       </c>
@@ -11043,7 +11046,7 @@
         <f t="shared" si="10"/>
         <v>1</v>
       </c>
-      <c r="O19" s="682"/>
+      <c r="O19" s="663"/>
       <c r="P19" s="20"/>
       <c r="Q19" s="2" t="s">
         <v>341</v>
@@ -11139,11 +11142,11 @@
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
-      <c r="O20" s="683"/>
+      <c r="O20" s="664"/>
       <c r="P20" s="558" t="s">
         <v>342</v>
       </c>
-      <c r="Q20" s="609"/>
+      <c r="Q20" s="661"/>
       <c r="R20" s="321" t="s">
         <v>86</v>
       </c>
@@ -11378,7 +11381,7 @@
       <c r="AN22" s="142"/>
     </row>
     <row r="23" spans="1:40" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E23" s="660" t="s">
+      <c r="E23" s="615" t="s">
         <v>294</v>
       </c>
       <c r="F23" s="184"/>
@@ -11471,7 +11474,7 @@
       <c r="C24" s="2" t="s">
         <v>260</v>
       </c>
-      <c r="E24" s="661"/>
+      <c r="E24" s="616"/>
       <c r="F24" s="176"/>
       <c r="K24" s="403" t="s">
         <v>301</v>
@@ -11489,7 +11492,7 @@
       <c r="P24" s="558" t="s">
         <v>342</v>
       </c>
-      <c r="Q24" s="609"/>
+      <c r="Q24" s="661"/>
       <c r="R24" s="321" t="s">
         <v>254</v>
       </c>
@@ -12482,21 +12485,21 @@
       <c r="K37" s="407"/>
       <c r="L37" s="346"/>
       <c r="M37" s="254">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="N37" s="299">
         <f t="shared" si="10"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P37" s="20"/>
       <c r="R37" s="256" t="s">
         <v>486</v>
       </c>
       <c r="S37" s="257">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="T37" s="197">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U37" s="225">
         <v>-1</v>
@@ -12504,50 +12507,50 @@
       <c r="V37" s="197"/>
       <c r="W37" s="24">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="X37" s="65"/>
       <c r="Y37" s="117">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Z37" s="64">
         <f t="shared" si="6"/>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="AA37" s="64">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AB37" s="307">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="AC37" s="362">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AD37" s="368"/>
       <c r="AE37" s="369"/>
       <c r="AF37" s="363">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AG37" s="390">
         <v>0</v>
       </c>
       <c r="AH37" s="329">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AI37" s="347">
         <f t="shared" si="7"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AJ37" s="315">
         <f t="shared" si="8"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AK37" s="316">
         <f t="shared" si="9"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AL37" s="6" t="s">
         <v>486</v>
@@ -12561,12 +12564,6 @@
     </row>
   </sheetData>
   <mergeCells count="15">
-    <mergeCell ref="A12:A13"/>
-    <mergeCell ref="E12:E13"/>
-    <mergeCell ref="P20:Q20"/>
-    <mergeCell ref="E23:E24"/>
-    <mergeCell ref="P24:Q24"/>
-    <mergeCell ref="O4:O20"/>
     <mergeCell ref="AI1:AK1"/>
     <mergeCell ref="V1:W1"/>
     <mergeCell ref="AC1:AE1"/>
@@ -12576,6 +12573,12 @@
     <mergeCell ref="N2:N3"/>
     <mergeCell ref="O2:O3"/>
     <mergeCell ref="U2:U3"/>
+    <mergeCell ref="A12:A13"/>
+    <mergeCell ref="E12:E13"/>
+    <mergeCell ref="P20:Q20"/>
+    <mergeCell ref="E23:E24"/>
+    <mergeCell ref="P24:Q24"/>
+    <mergeCell ref="O4:O20"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -12612,12 +12615,12 @@
       <c r="B1" s="558" t="s">
         <v>317</v>
       </c>
-      <c r="C1" s="609"/>
+      <c r="C1" s="661"/>
       <c r="D1" s="209"/>
       <c r="J1" s="558" t="s">
         <v>70</v>
       </c>
-      <c r="K1" s="609"/>
+      <c r="K1" s="661"/>
       <c r="L1" s="200" t="s">
         <v>337</v>
       </c>
@@ -13008,7 +13011,7 @@
       <c r="V1" s="558" t="s">
         <v>71</v>
       </c>
-      <c r="W1" s="609"/>
+      <c r="W1" s="661"/>
       <c r="X1" s="62" t="s">
         <v>102</v>
       </c>
@@ -13027,7 +13030,7 @@
       <c r="AC1" s="116" t="s">
         <v>191</v>
       </c>
-      <c r="AD1" s="697" t="s">
+      <c r="AD1" s="704" t="s">
         <v>213</v>
       </c>
       <c r="AE1" s="116" t="s">
@@ -13044,10 +13047,10 @@
       <c r="E2" s="39" t="s">
         <v>74</v>
       </c>
-      <c r="F2" s="696" t="s">
+      <c r="F2" s="735" t="s">
         <v>75</v>
       </c>
-      <c r="G2" s="724" t="s">
+      <c r="G2" s="692" t="s">
         <v>44</v>
       </c>
       <c r="H2" s="40" t="s">
@@ -13075,10 +13078,10 @@
       <c r="U2" s="60" t="s">
         <v>106</v>
       </c>
-      <c r="V2" s="665" t="s">
+      <c r="V2" s="668" t="s">
         <v>121</v>
       </c>
-      <c r="W2" s="666"/>
+      <c r="W2" s="669"/>
       <c r="X2" s="64" t="s">
         <v>110</v>
       </c>
@@ -13097,7 +13100,7 @@
       <c r="AC2" s="117" t="s">
         <v>99</v>
       </c>
-      <c r="AD2" s="698"/>
+      <c r="AD2" s="705"/>
       <c r="AE2" s="64" t="s">
         <v>99</v>
       </c>
@@ -13116,8 +13119,8 @@
       <c r="E3" s="39" t="s">
         <v>80</v>
       </c>
-      <c r="F3" s="657"/>
-      <c r="G3" s="725"/>
+      <c r="F3" s="612"/>
+      <c r="G3" s="693"/>
       <c r="H3" s="40" t="s">
         <v>81</v>
       </c>
@@ -13128,13 +13131,13 @@
         <v>82</v>
       </c>
       <c r="N3" s="44"/>
-      <c r="O3" s="734" t="s">
+      <c r="O3" s="702" t="s">
         <v>44</v>
       </c>
-      <c r="P3" s="716" t="s">
+      <c r="P3" s="723" t="s">
         <v>219</v>
       </c>
-      <c r="Q3" s="717"/>
+      <c r="Q3" s="724"/>
       <c r="S3" s="57" t="s">
         <v>220</v>
       </c>
@@ -13144,15 +13147,15 @@
       <c r="W3" s="59" t="s">
         <v>105</v>
       </c>
-      <c r="AD3" s="698"/>
+      <c r="AD3" s="705"/>
     </row>
     <row r="4" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="G4" s="725"/>
+      <c r="G4" s="693"/>
       <c r="H4" s="6"/>
       <c r="L4" s="687" t="s">
         <v>83</v>
       </c>
-      <c r="O4" s="735"/>
+      <c r="O4" s="703"/>
       <c r="T4" s="55" t="s">
         <v>98</v>
       </c>
@@ -13166,8 +13169,8 @@
         <v>195</v>
       </c>
       <c r="Z4" s="560"/>
-      <c r="AA4" s="609"/>
-      <c r="AD4" s="698"/>
+      <c r="AA4" s="661"/>
+      <c r="AD4" s="705"/>
     </row>
     <row r="5" spans="1:31" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C5" s="52" t="s">
@@ -13182,21 +13185,21 @@
       <c r="F5" s="66" t="s">
         <v>85</v>
       </c>
-      <c r="G5" s="725"/>
+      <c r="G5" s="693"/>
       <c r="H5" s="46" t="s">
         <v>76</v>
       </c>
-      <c r="K5" s="703" t="s">
+      <c r="K5" s="710" t="s">
         <v>217</v>
       </c>
-      <c r="L5" s="718"/>
+      <c r="L5" s="725"/>
       <c r="M5" s="2" t="s">
         <v>215</v>
       </c>
       <c r="N5" s="61" t="s">
         <v>214</v>
       </c>
-      <c r="O5" s="735"/>
+      <c r="O5" s="703"/>
       <c r="P5" s="108" t="s">
         <v>216</v>
       </c>
@@ -13212,11 +13215,11 @@
       <c r="U5" s="19" t="s">
         <v>99</v>
       </c>
-      <c r="Y5" s="706" t="s">
+      <c r="Y5" s="713" t="s">
         <v>287</v>
       </c>
-      <c r="Z5" s="707"/>
-      <c r="AD5" s="698"/>
+      <c r="Z5" s="714"/>
+      <c r="AD5" s="705"/>
     </row>
     <row r="6" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C6" s="109"/>
@@ -13226,16 +13229,16 @@
       <c r="E6" s="45" t="s">
         <v>86</v>
       </c>
-      <c r="G6" s="725"/>
+      <c r="G6" s="693"/>
       <c r="H6" s="46" t="s">
         <v>81</v>
       </c>
       <c r="I6" s="23">
         <v>15</v>
       </c>
-      <c r="K6" s="704"/>
-      <c r="L6" s="718"/>
-      <c r="O6" s="735"/>
+      <c r="K6" s="711"/>
+      <c r="L6" s="725"/>
+      <c r="O6" s="703"/>
       <c r="T6" s="2" t="s">
         <v>101</v>
       </c>
@@ -13245,23 +13248,23 @@
       <c r="V6" s="21">
         <v>-1</v>
       </c>
-      <c r="AD6" s="698"/>
+      <c r="AD6" s="705"/>
     </row>
     <row r="7" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C7" s="110"/>
-      <c r="G7" s="725"/>
+      <c r="G7" s="693"/>
       <c r="H7" s="6"/>
-      <c r="K7" s="704"/>
-      <c r="L7" s="718"/>
+      <c r="K7" s="711"/>
+      <c r="L7" s="725"/>
       <c r="N7" s="21" t="s">
         <v>120</v>
       </c>
-      <c r="O7" s="735"/>
+      <c r="O7" s="703"/>
       <c r="P7" s="73"/>
       <c r="U7" s="104" t="s">
         <v>20</v>
       </c>
-      <c r="AD7" s="698"/>
+      <c r="AD7" s="705"/>
     </row>
     <row r="8" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C8" s="130"/>
@@ -13274,7 +13277,7 @@
       <c r="F8" s="66" t="s">
         <v>87</v>
       </c>
-      <c r="G8" s="725"/>
+      <c r="G8" s="693"/>
       <c r="H8" s="50" t="s">
         <v>76</v>
       </c>
@@ -13284,41 +13287,41 @@
       <c r="J8" s="111">
         <v>115</v>
       </c>
-      <c r="K8" s="704"/>
-      <c r="L8" s="718"/>
-      <c r="O8" s="735"/>
+      <c r="K8" s="711"/>
+      <c r="L8" s="725"/>
+      <c r="O8" s="703"/>
       <c r="P8" s="49"/>
-      <c r="S8" s="700" t="s">
+      <c r="S8" s="707" t="s">
         <v>212</v>
       </c>
-      <c r="T8" s="701"/>
-      <c r="U8" s="701"/>
-      <c r="V8" s="701"/>
-      <c r="W8" s="701"/>
-      <c r="X8" s="701"/>
-      <c r="Y8" s="701"/>
-      <c r="Z8" s="701"/>
-      <c r="AA8" s="701"/>
-      <c r="AB8" s="701"/>
-      <c r="AC8" s="702"/>
-      <c r="AD8" s="698"/>
+      <c r="T8" s="708"/>
+      <c r="U8" s="708"/>
+      <c r="V8" s="708"/>
+      <c r="W8" s="708"/>
+      <c r="X8" s="708"/>
+      <c r="Y8" s="708"/>
+      <c r="Z8" s="708"/>
+      <c r="AA8" s="708"/>
+      <c r="AB8" s="708"/>
+      <c r="AC8" s="709"/>
+      <c r="AD8" s="705"/>
     </row>
     <row r="9" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C9" s="690"/>
-      <c r="G9" s="725"/>
+      <c r="C9" s="729"/>
+      <c r="G9" s="693"/>
       <c r="H9" s="6"/>
-      <c r="K9" s="704"/>
-      <c r="L9" s="728" t="s">
+      <c r="K9" s="711"/>
+      <c r="L9" s="696" t="s">
         <v>218</v>
       </c>
-      <c r="M9" s="729"/>
-      <c r="N9" s="730"/>
-      <c r="O9" s="735"/>
+      <c r="M9" s="697"/>
+      <c r="N9" s="698"/>
+      <c r="O9" s="703"/>
       <c r="P9" s="75"/>
-      <c r="AD9" s="698"/>
+      <c r="AD9" s="705"/>
     </row>
     <row r="10" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C10" s="691"/>
+      <c r="C10" s="730"/>
       <c r="D10" s="23"/>
       <c r="E10" s="45" t="s">
         <v>88</v>
@@ -13326,7 +13329,7 @@
       <c r="F10" s="66" t="s">
         <v>89</v>
       </c>
-      <c r="G10" s="725"/>
+      <c r="G10" s="693"/>
       <c r="H10" s="51"/>
       <c r="I10" s="21" t="s">
         <v>81</v>
@@ -13334,33 +13337,33 @@
       <c r="J10" s="3">
         <v>15</v>
       </c>
-      <c r="K10" s="704"/>
-      <c r="M10" s="693" t="s">
+      <c r="K10" s="711"/>
+      <c r="M10" s="732" t="s">
         <v>90</v>
       </c>
-      <c r="N10" s="694"/>
-      <c r="O10" s="694"/>
-      <c r="P10" s="694"/>
-      <c r="Q10" s="694"/>
-      <c r="R10" s="694"/>
-      <c r="S10" s="694"/>
-      <c r="T10" s="694"/>
-      <c r="U10" s="694"/>
-      <c r="V10" s="694"/>
-      <c r="W10" s="694"/>
-      <c r="X10" s="694"/>
-      <c r="Y10" s="694"/>
-      <c r="Z10" s="694"/>
-      <c r="AA10" s="694"/>
-      <c r="AB10" s="694"/>
-      <c r="AC10" s="695"/>
-      <c r="AD10" s="698"/>
+      <c r="N10" s="733"/>
+      <c r="O10" s="733"/>
+      <c r="P10" s="733"/>
+      <c r="Q10" s="733"/>
+      <c r="R10" s="733"/>
+      <c r="S10" s="733"/>
+      <c r="T10" s="733"/>
+      <c r="U10" s="733"/>
+      <c r="V10" s="733"/>
+      <c r="W10" s="733"/>
+      <c r="X10" s="733"/>
+      <c r="Y10" s="733"/>
+      <c r="Z10" s="733"/>
+      <c r="AA10" s="733"/>
+      <c r="AB10" s="733"/>
+      <c r="AC10" s="734"/>
+      <c r="AD10" s="705"/>
     </row>
     <row r="11" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C11" s="692"/>
-      <c r="G11" s="725"/>
+      <c r="C11" s="731"/>
+      <c r="G11" s="693"/>
       <c r="H11" s="6"/>
-      <c r="K11" s="704"/>
+      <c r="K11" s="711"/>
       <c r="R11" s="52" t="s">
         <v>44</v>
       </c>
@@ -13368,17 +13371,17 @@
       <c r="Y11" s="68" t="s">
         <v>121</v>
       </c>
-      <c r="Z11" s="714" t="s">
+      <c r="Z11" s="721" t="s">
         <v>121</v>
       </c>
-      <c r="AA11" s="715"/>
+      <c r="AA11" s="722"/>
       <c r="AB11" s="52" t="s">
         <v>44</v>
       </c>
       <c r="AC11" s="118" t="s">
         <v>121</v>
       </c>
-      <c r="AD11" s="698"/>
+      <c r="AD11" s="705"/>
     </row>
     <row r="12" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C12" s="129"/>
@@ -13391,7 +13394,7 @@
       <c r="F12" s="66" t="s">
         <v>92</v>
       </c>
-      <c r="G12" s="725"/>
+      <c r="G12" s="693"/>
       <c r="H12" s="128"/>
       <c r="I12" s="19" t="s">
         <v>81</v>
@@ -13399,8 +13402,8 @@
       <c r="J12" s="3">
         <v>15</v>
       </c>
-      <c r="K12" s="704"/>
-      <c r="L12" s="719" t="s">
+      <c r="K12" s="711"/>
+      <c r="L12" s="726" t="s">
         <v>93</v>
       </c>
       <c r="M12" s="21" t="s">
@@ -13431,25 +13434,25 @@
         <v>116</v>
       </c>
       <c r="Y12" s="6"/>
-      <c r="AA12" s="708" t="s">
+      <c r="AA12" s="715" t="s">
         <v>126</v>
       </c>
-      <c r="AB12" s="709"/>
+      <c r="AB12" s="716"/>
       <c r="AC12" s="21" t="s">
         <v>233</v>
       </c>
-      <c r="AD12" s="698"/>
+      <c r="AD12" s="705"/>
     </row>
     <row r="13" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C13" s="690"/>
-      <c r="G13" s="725"/>
-      <c r="K13" s="704"/>
-      <c r="L13" s="720"/>
+      <c r="C13" s="729"/>
+      <c r="G13" s="693"/>
+      <c r="K13" s="711"/>
+      <c r="L13" s="727"/>
       <c r="M13" s="47"/>
-      <c r="Q13" s="727" t="s">
+      <c r="Q13" s="695" t="s">
         <v>210</v>
       </c>
-      <c r="R13" s="624"/>
+      <c r="R13" s="621"/>
       <c r="S13" s="554"/>
       <c r="T13" s="6"/>
       <c r="U13" s="96" t="s">
@@ -13458,17 +13461,17 @@
       <c r="X13" s="2" t="s">
         <v>123</v>
       </c>
-      <c r="AA13" s="710"/>
-      <c r="AB13" s="711"/>
-      <c r="AD13" s="698"/>
+      <c r="AA13" s="717"/>
+      <c r="AB13" s="718"/>
+      <c r="AD13" s="705"/>
     </row>
     <row r="14" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B14" s="2" t="s">
         <v>339</v>
       </c>
-      <c r="C14" s="692"/>
+      <c r="C14" s="731"/>
       <c r="D14" s="23"/>
-      <c r="G14" s="725"/>
+      <c r="G14" s="693"/>
       <c r="H14" s="125"/>
       <c r="I14" s="99" t="s">
         <v>44</v>
@@ -13476,8 +13479,8 @@
       <c r="J14" s="111">
         <v>115</v>
       </c>
-      <c r="K14" s="704"/>
-      <c r="L14" s="720"/>
+      <c r="K14" s="711"/>
+      <c r="L14" s="727"/>
       <c r="M14" s="21" t="s">
         <v>111</v>
       </c>
@@ -13498,9 +13501,9 @@
       <c r="Y14" s="21" t="s">
         <v>73</v>
       </c>
-      <c r="AA14" s="710"/>
-      <c r="AB14" s="711"/>
-      <c r="AD14" s="698"/>
+      <c r="AA14" s="717"/>
+      <c r="AB14" s="718"/>
+      <c r="AD14" s="705"/>
     </row>
     <row r="15" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C15" s="130" t="s">
@@ -13515,19 +13518,19 @@
       <c r="F15" s="66" t="s">
         <v>94</v>
       </c>
-      <c r="G15" s="725"/>
+      <c r="G15" s="693"/>
       <c r="H15" s="2" t="s">
         <v>81</v>
       </c>
       <c r="I15" s="53" t="s">
         <v>81</v>
       </c>
-      <c r="K15" s="704"/>
-      <c r="L15" s="721"/>
-      <c r="Q15" s="727" t="s">
+      <c r="K15" s="711"/>
+      <c r="L15" s="728"/>
+      <c r="Q15" s="695" t="s">
         <v>211</v>
       </c>
-      <c r="R15" s="624"/>
+      <c r="R15" s="621"/>
       <c r="S15" s="554"/>
       <c r="T15" s="6"/>
       <c r="V15" s="68" t="s">
@@ -13536,14 +13539,14 @@
       <c r="X15" s="2" t="s">
         <v>128</v>
       </c>
-      <c r="AA15" s="710"/>
-      <c r="AB15" s="711"/>
-      <c r="AD15" s="698"/>
+      <c r="AA15" s="717"/>
+      <c r="AB15" s="718"/>
+      <c r="AD15" s="705"/>
     </row>
     <row r="16" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C16" s="132"/>
-      <c r="G16" s="725"/>
-      <c r="K16" s="704"/>
+      <c r="G16" s="693"/>
+      <c r="K16" s="711"/>
       <c r="N16" s="47"/>
       <c r="O16" s="61" t="s">
         <v>109</v>
@@ -13562,24 +13565,24 @@
       <c r="Z16" s="76" t="s">
         <v>127</v>
       </c>
-      <c r="AA16" s="710"/>
-      <c r="AB16" s="711"/>
-      <c r="AD16" s="698"/>
+      <c r="AA16" s="717"/>
+      <c r="AB16" s="718"/>
+      <c r="AD16" s="705"/>
     </row>
     <row r="17" spans="3:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C17" s="109"/>
       <c r="E17" s="6" t="s">
         <v>95</v>
       </c>
-      <c r="F17" s="722" t="s">
+      <c r="F17" s="690" t="s">
         <v>96</v>
       </c>
-      <c r="G17" s="725"/>
+      <c r="G17" s="693"/>
       <c r="H17" s="54"/>
       <c r="I17" s="133" t="s">
         <v>81</v>
       </c>
-      <c r="K17" s="704"/>
+      <c r="K17" s="711"/>
       <c r="S17" s="554"/>
       <c r="V17" s="68" t="s">
         <v>44</v>
@@ -13587,9 +13590,9 @@
       <c r="X17" s="2" t="s">
         <v>118</v>
       </c>
-      <c r="AA17" s="710"/>
-      <c r="AB17" s="711"/>
-      <c r="AD17" s="698"/>
+      <c r="AA17" s="717"/>
+      <c r="AB17" s="718"/>
+      <c r="AD17" s="705"/>
     </row>
     <row r="18" spans="3:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C18" s="130"/>
@@ -13599,15 +13602,15 @@
       <c r="E18" s="6" t="s">
         <v>97</v>
       </c>
-      <c r="F18" s="723"/>
-      <c r="G18" s="725"/>
+      <c r="F18" s="691"/>
+      <c r="G18" s="693"/>
       <c r="H18" s="108" t="s">
         <v>76</v>
       </c>
       <c r="I18" s="21" t="s">
         <v>81</v>
       </c>
-      <c r="K18" s="704"/>
+      <c r="K18" s="711"/>
       <c r="O18" s="64" t="s">
         <v>115</v>
       </c>
@@ -13618,42 +13621,39 @@
       <c r="X18" s="2" t="s">
         <v>117</v>
       </c>
-      <c r="AA18" s="712"/>
-      <c r="AB18" s="713"/>
-      <c r="AD18" s="698"/>
+      <c r="AA18" s="719"/>
+      <c r="AB18" s="720"/>
+      <c r="AD18" s="705"/>
     </row>
     <row r="19" spans="3:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="F19" s="64" t="s">
         <v>209</v>
       </c>
-      <c r="G19" s="726"/>
-      <c r="K19" s="705"/>
+      <c r="G19" s="694"/>
+      <c r="K19" s="712"/>
       <c r="Q19" s="68" t="s">
         <v>44</v>
       </c>
-      <c r="R19" s="731" t="s">
+      <c r="R19" s="699" t="s">
         <v>124</v>
       </c>
-      <c r="S19" s="732"/>
-      <c r="T19" s="733"/>
+      <c r="S19" s="700"/>
+      <c r="T19" s="701"/>
       <c r="V19" s="77" t="s">
         <v>115</v>
       </c>
       <c r="Y19" s="19" t="s">
         <v>125</v>
       </c>
-      <c r="AD19" s="699"/>
+      <c r="AD19" s="706"/>
     </row>
   </sheetData>
   <mergeCells count="24">
-    <mergeCell ref="F17:F18"/>
-    <mergeCell ref="G2:G19"/>
-    <mergeCell ref="Q13:R13"/>
-    <mergeCell ref="Q15:R15"/>
-    <mergeCell ref="L9:N9"/>
-    <mergeCell ref="R19:T19"/>
-    <mergeCell ref="S12:S18"/>
-    <mergeCell ref="O3:O9"/>
+    <mergeCell ref="C9:C11"/>
+    <mergeCell ref="C13:C14"/>
+    <mergeCell ref="V2:W2"/>
+    <mergeCell ref="M10:AC10"/>
+    <mergeCell ref="F2:F3"/>
     <mergeCell ref="AD1:AD19"/>
     <mergeCell ref="S8:AC8"/>
     <mergeCell ref="K5:K19"/>
@@ -13665,11 +13665,14 @@
     <mergeCell ref="P3:Q3"/>
     <mergeCell ref="L4:L8"/>
     <mergeCell ref="L12:L15"/>
-    <mergeCell ref="C9:C11"/>
-    <mergeCell ref="C13:C14"/>
-    <mergeCell ref="V2:W2"/>
-    <mergeCell ref="M10:AC10"/>
-    <mergeCell ref="F2:F3"/>
+    <mergeCell ref="F17:F18"/>
+    <mergeCell ref="G2:G19"/>
+    <mergeCell ref="Q13:R13"/>
+    <mergeCell ref="Q15:R15"/>
+    <mergeCell ref="L9:N9"/>
+    <mergeCell ref="R19:T19"/>
+    <mergeCell ref="S12:S18"/>
+    <mergeCell ref="O3:O9"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Boat Enabled - TBS
Boat Enabled - TBS
ShieldW Enabled
Alliance Partner - NTV Japan
</commit_message>
<xml_diff>
--- a/System_2.1.5.xlsx
+++ b/System_2.1.5.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Work\Work_For_\Work\Running AppS\System_Work_RW\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48A570F9-FB8E-4DC4-8524-7FE9F362FC19}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F059F8D-180C-4319-A4DB-2F832C53BEE3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="BoardRW" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1078" uniqueCount="610">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1079" uniqueCount="610">
   <si>
     <t>Zone</t>
   </si>
@@ -4804,6 +4804,36 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="255" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="39" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="39" fillId="6" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="18" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="18" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="18" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255"/>
+    </xf>
     <xf numFmtId="0" fontId="32" fillId="27" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -4861,34 +4891,139 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="39" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="39" fillId="6" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="18" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="19" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="19" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="3" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="19" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="19" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="38" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="38" fillId="7" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="255"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="18" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="255"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="18" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="33" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="33" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="33" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="52" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="54" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="16" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="16" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="3" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="18" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="18" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="18" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="49" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="49" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="49" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="255"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
@@ -4963,140 +5098,62 @@
     <xf numFmtId="0" fontId="3" fillId="11" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="3" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="18" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="18" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="18" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="49" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="49" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="49" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="52" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="54" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="16" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="16" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="19" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="19" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="3" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="19" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="19" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="38" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="38" fillId="7" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="33" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="33" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="33" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="3" fillId="43" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="43" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="43" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="18" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="18" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="18" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="40" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="40" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="40" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="7" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="32" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="32" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="52" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="52" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="35" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="255" wrapText="1"/>
@@ -5107,63 +5164,6 @@
     <xf numFmtId="0" fontId="3" fillId="35" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="255" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="43" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="43" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="43" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="18" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="18" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="18" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="40" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="40" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="40" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="7" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="32" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="32" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="52" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="52" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -5182,46 +5182,25 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="30" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="30" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="30" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="24" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="24" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="24" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="18" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -5299,25 +5278,46 @@
     <xf numFmtId="0" fontId="3" fillId="21" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="30" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="30" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="30" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="24" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="24" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="24" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -6565,8 +6565,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AB54FD83-008D-4F8B-87AC-83E7F70047CB}">
   <dimension ref="A1:AA32"/>
   <sheetViews>
-    <sheetView topLeftCell="H13" workbookViewId="0">
-      <selection activeCell="AA28" sqref="AA28"/>
+    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
+      <selection activeCell="V13" sqref="V13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6623,7 +6623,7 @@
       <c r="P1" s="423" t="s">
         <v>408</v>
       </c>
-      <c r="Q1" s="583" t="s">
+      <c r="Q1" s="564" t="s">
         <v>181</v>
       </c>
       <c r="R1" s="100" t="s">
@@ -6643,32 +6643,32 @@
       </c>
     </row>
     <row r="2" spans="1:27" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="567">
+      <c r="A2" s="577">
         <f ca="1">TODAY()</f>
         <v>45279</v>
       </c>
-      <c r="B2" s="569" t="s">
+      <c r="B2" s="579" t="s">
         <v>389</v>
       </c>
-      <c r="C2" s="581" t="s">
+      <c r="C2" s="591" t="s">
         <v>365</v>
       </c>
-      <c r="D2" s="571" t="s">
+      <c r="D2" s="581" t="s">
         <v>103</v>
       </c>
-      <c r="E2" s="573" t="s">
+      <c r="E2" s="583" t="s">
         <v>65</v>
       </c>
       <c r="F2" s="196" t="s">
         <v>220</v>
       </c>
-      <c r="G2" s="579" t="s">
+      <c r="G2" s="589" t="s">
         <v>381</v>
       </c>
       <c r="H2" s="211" t="s">
         <v>220</v>
       </c>
-      <c r="I2" s="590" t="s">
+      <c r="I2" s="571" t="s">
         <v>103</v>
       </c>
       <c r="J2" s="421" t="s">
@@ -6692,7 +6692,7 @@
       <c r="P2" s="424">
         <v>40</v>
       </c>
-      <c r="Q2" s="584"/>
+      <c r="Q2" s="565"/>
       <c r="R2" s="21">
         <f>R7+R18</f>
         <v>6</v>
@@ -6718,14 +6718,14 @@
       </c>
     </row>
     <row r="3" spans="1:27" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="568"/>
-      <c r="B3" s="570"/>
-      <c r="C3" s="582"/>
-      <c r="D3" s="572"/>
-      <c r="E3" s="574"/>
-      <c r="G3" s="580"/>
+      <c r="A3" s="578"/>
+      <c r="B3" s="580"/>
+      <c r="C3" s="592"/>
+      <c r="D3" s="582"/>
+      <c r="E3" s="584"/>
+      <c r="G3" s="590"/>
       <c r="H3" s="6"/>
-      <c r="I3" s="591"/>
+      <c r="I3" s="572"/>
       <c r="K3" s="24">
         <v>2</v>
       </c>
@@ -6734,7 +6734,7 @@
       </c>
       <c r="Q3" s="499">
         <f>SUM(X24:X32)</f>
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="U3" s="6"/>
       <c r="V3" s="497"/>
@@ -6750,10 +6750,10 @@
         <v>390</v>
       </c>
       <c r="B4" s="248"/>
-      <c r="C4" s="575" t="s">
+      <c r="C4" s="585" t="s">
         <v>178</v>
       </c>
-      <c r="I4" s="591"/>
+      <c r="I4" s="572"/>
       <c r="R4" s="499" t="s">
         <v>580</v>
       </c>
@@ -6777,7 +6777,7 @@
       <c r="B5" s="100" t="s">
         <v>365</v>
       </c>
-      <c r="C5" s="576"/>
+      <c r="C5" s="586"/>
       <c r="D5" s="227" t="s">
         <v>103</v>
       </c>
@@ -6793,7 +6793,7 @@
       <c r="H5" s="211" t="s">
         <v>220</v>
       </c>
-      <c r="I5" s="591"/>
+      <c r="I5" s="572"/>
       <c r="J5" s="422" t="s">
         <v>273</v>
       </c>
@@ -6824,22 +6824,22 @@
       <c r="X5" s="495"/>
     </row>
     <row r="6" spans="1:27" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="564" t="s">
+      <c r="A6" s="574" t="s">
         <v>290</v>
       </c>
       <c r="B6" s="105" t="s">
         <v>199</v>
       </c>
-      <c r="C6" s="577"/>
-      <c r="D6" s="578"/>
+      <c r="C6" s="587"/>
+      <c r="D6" s="588"/>
       <c r="E6" s="96">
         <v>1</v>
       </c>
       <c r="G6" s="554"/>
-      <c r="I6" s="591"/>
+      <c r="I6" s="572"/>
     </row>
     <row r="7" spans="1:27" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="565"/>
+      <c r="A7" s="575"/>
       <c r="B7" s="100" t="s">
         <v>155</v>
       </c>
@@ -6850,7 +6850,7 @@
         <v>136</v>
       </c>
       <c r="G7" s="554"/>
-      <c r="I7" s="591"/>
+      <c r="I7" s="572"/>
       <c r="M7" s="16" t="s">
         <v>354</v>
       </c>
@@ -6886,7 +6886,7 @@
       </c>
     </row>
     <row r="8" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="566"/>
+      <c r="A8" s="576"/>
       <c r="B8" s="217" t="s">
         <v>28</v>
       </c>
@@ -6895,7 +6895,7 @@
         <v>3</v>
       </c>
       <c r="G8" s="554"/>
-      <c r="I8" s="591"/>
+      <c r="I8" s="572"/>
       <c r="N8" s="80"/>
       <c r="U8" s="6" t="s">
         <v>466</v>
@@ -6919,7 +6919,7 @@
       </c>
       <c r="G9" s="554"/>
       <c r="H9" s="6"/>
-      <c r="I9" s="591"/>
+      <c r="I9" s="572"/>
       <c r="M9" s="19" t="s">
         <v>547</v>
       </c>
@@ -6943,10 +6943,10 @@
       <c r="D10" s="108"/>
       <c r="E10" s="68">
         <f>Boat!U8</f>
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="G10" s="554"/>
-      <c r="I10" s="591"/>
+      <c r="I10" s="572"/>
       <c r="J10" s="24" t="s">
         <v>381</v>
       </c>
@@ -6980,7 +6980,7 @@
         <v>270</v>
       </c>
       <c r="G11" s="554"/>
-      <c r="I11" s="591"/>
+      <c r="I11" s="572"/>
       <c r="J11" s="24" t="s">
         <v>195</v>
       </c>
@@ -7006,12 +7006,12 @@
       <c r="S11" s="24">
         <v>1</v>
       </c>
-      <c r="U11" s="585" t="s">
+      <c r="U11" s="566" t="s">
         <v>583</v>
       </c>
-      <c r="V11" s="586"/>
-      <c r="W11" s="586"/>
-      <c r="X11" s="587"/>
+      <c r="V11" s="567"/>
+      <c r="W11" s="567"/>
+      <c r="X11" s="568"/>
     </row>
     <row r="12" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="232" t="s">
@@ -7022,7 +7022,7 @@
         <v>3</v>
       </c>
       <c r="G12" s="554"/>
-      <c r="I12" s="591"/>
+      <c r="I12" s="572"/>
       <c r="J12" s="24" t="s">
         <v>538</v>
       </c>
@@ -7055,7 +7055,7 @@
       </c>
       <c r="D13" s="20"/>
       <c r="G13" s="554"/>
-      <c r="I13" s="591"/>
+      <c r="I13" s="572"/>
       <c r="J13" s="108" t="s">
         <v>572</v>
       </c>
@@ -7096,7 +7096,7 @@
       <c r="H14" s="211" t="s">
         <v>220</v>
       </c>
-      <c r="I14" s="591"/>
+      <c r="I14" s="572"/>
       <c r="U14" s="6"/>
       <c r="V14" s="112"/>
       <c r="W14" s="6"/>
@@ -7114,7 +7114,7 @@
       <c r="H15" s="277">
         <v>0</v>
       </c>
-      <c r="I15" s="591"/>
+      <c r="I15" s="572"/>
       <c r="J15" s="108" t="s">
         <v>154</v>
       </c>
@@ -7145,7 +7145,7 @@
       <c r="D16" s="2" t="s">
         <v>510</v>
       </c>
-      <c r="I16" s="591"/>
+      <c r="I16" s="572"/>
       <c r="K16" s="100" t="s">
         <v>44</v>
       </c>
@@ -7179,7 +7179,7 @@
       <c r="G17" s="2" t="s">
         <v>441</v>
       </c>
-      <c r="I17" s="591"/>
+      <c r="I17" s="572"/>
       <c r="L17" s="2" t="s">
         <v>444</v>
       </c>
@@ -7191,13 +7191,13 @@
     </row>
     <row r="18" spans="1:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="G18" s="16"/>
-      <c r="I18" s="591"/>
+      <c r="I18" s="572"/>
       <c r="L18" s="16"/>
       <c r="M18" s="21"/>
-      <c r="O18" s="588" t="s">
+      <c r="O18" s="569" t="s">
         <v>539</v>
       </c>
-      <c r="P18" s="589"/>
+      <c r="P18" s="570"/>
       <c r="Q18" s="127" t="s">
         <v>44</v>
       </c>
@@ -7223,7 +7223,7 @@
       </c>
     </row>
     <row r="19" spans="1:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="I19" s="591"/>
+      <c r="I19" s="572"/>
       <c r="M19" s="21" t="s">
         <v>443</v>
       </c>
@@ -7255,7 +7255,7 @@
       <c r="G20" s="2" t="s">
         <v>441</v>
       </c>
-      <c r="I20" s="591"/>
+      <c r="I20" s="572"/>
       <c r="K20" s="19" t="s">
         <v>440</v>
       </c>
@@ -7280,7 +7280,7 @@
       <c r="Z20" s="112"/>
     </row>
     <row r="21" spans="1:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="I21" s="591"/>
+      <c r="I21" s="572"/>
       <c r="M21" s="221" t="s">
         <v>422</v>
       </c>
@@ -7316,7 +7316,7 @@
       <c r="G22" s="2" t="s">
         <v>441</v>
       </c>
-      <c r="I22" s="591"/>
+      <c r="I22" s="572"/>
       <c r="U22" s="6"/>
       <c r="V22" s="495"/>
       <c r="W22" s="6" t="s">
@@ -7336,22 +7336,22 @@
       <c r="E23" s="289" t="s">
         <v>44</v>
       </c>
-      <c r="I23" s="591"/>
+      <c r="I23" s="572"/>
       <c r="U23" s="6"/>
       <c r="V23" s="24"/>
       <c r="W23" s="6"/>
     </row>
     <row r="24" spans="1:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="I24" s="591"/>
+      <c r="I24" s="572"/>
       <c r="U24" s="354"/>
       <c r="V24" s="498">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="W24" s="19" t="s">
         <v>513</v>
       </c>
       <c r="X24" s="24">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="25" spans="1:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -7370,7 +7370,7 @@
       <c r="H25" s="196" t="s">
         <v>271</v>
       </c>
-      <c r="I25" s="591"/>
+      <c r="I25" s="572"/>
       <c r="J25" s="422" t="s">
         <v>274</v>
       </c>
@@ -7415,7 +7415,7 @@
       <c r="H26" s="19" t="s">
         <v>220</v>
       </c>
-      <c r="I26" s="591"/>
+      <c r="I26" s="572"/>
       <c r="K26" s="24">
         <v>15</v>
       </c>
@@ -7450,7 +7450,7 @@
       </c>
     </row>
     <row r="27" spans="1:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="I27" s="591"/>
+      <c r="I27" s="572"/>
       <c r="O27" s="2" t="s">
         <v>99</v>
       </c>
@@ -7477,7 +7477,7 @@
       <c r="E28" s="220">
         <v>2</v>
       </c>
-      <c r="I28" s="591"/>
+      <c r="I28" s="572"/>
       <c r="Q28" s="6"/>
       <c r="R28" s="112"/>
       <c r="T28" s="142"/>
@@ -7499,7 +7499,7 @@
       <c r="H29" s="196" t="s">
         <v>272</v>
       </c>
-      <c r="I29" s="592"/>
+      <c r="I29" s="573"/>
       <c r="J29" s="333"/>
       <c r="L29" s="96" t="s">
         <v>278</v>
@@ -7569,11 +7569,6 @@
     </row>
   </sheetData>
   <mergeCells count="16">
-    <mergeCell ref="Q1:Q2"/>
-    <mergeCell ref="U11:X11"/>
-    <mergeCell ref="O18:P18"/>
-    <mergeCell ref="I2:I29"/>
-    <mergeCell ref="C13:C14"/>
     <mergeCell ref="A6:A8"/>
     <mergeCell ref="G5:G14"/>
     <mergeCell ref="A2:A3"/>
@@ -7585,6 +7580,11 @@
     <mergeCell ref="B11:B12"/>
     <mergeCell ref="G2:G3"/>
     <mergeCell ref="C2:C3"/>
+    <mergeCell ref="Q1:Q2"/>
+    <mergeCell ref="U11:X11"/>
+    <mergeCell ref="O18:P18"/>
+    <mergeCell ref="I2:I29"/>
+    <mergeCell ref="C13:C14"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -7660,7 +7660,7 @@
       <c r="H1" s="97" t="s">
         <v>350</v>
       </c>
-      <c r="I1" s="579" t="s">
+      <c r="I1" s="589" t="s">
         <v>378</v>
       </c>
       <c r="J1" s="2" t="s">
@@ -7721,7 +7721,7 @@
         <v>517</v>
       </c>
       <c r="AM1" s="427"/>
-      <c r="AN1" s="617"/>
+      <c r="AN1" s="620"/>
       <c r="AO1" s="350" t="s">
         <v>487</v>
       </c>
@@ -7730,23 +7730,23 @@
       </c>
     </row>
     <row r="2" spans="1:43" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="599">
+      <c r="A2" s="644">
         <f ca="1">TODAY()</f>
         <v>45279</v>
       </c>
-      <c r="B2" s="601" t="s">
+      <c r="B2" s="646" t="s">
         <v>379</v>
       </c>
-      <c r="C2" s="581" t="s">
+      <c r="C2" s="591" t="s">
         <v>365</v>
       </c>
-      <c r="D2" s="603" t="s">
+      <c r="D2" s="648" t="s">
         <v>362</v>
       </c>
-      <c r="E2" s="647" t="s">
+      <c r="E2" s="593" t="s">
         <v>65</v>
       </c>
-      <c r="F2" s="622" t="s">
+      <c r="F2" s="601" t="s">
         <v>103</v>
       </c>
       <c r="G2" s="418" t="s">
@@ -7755,31 +7755,31 @@
       <c r="H2" s="80" t="s">
         <v>33</v>
       </c>
-      <c r="I2" s="580"/>
+      <c r="I2" s="590"/>
       <c r="J2" s="81" t="s">
         <v>77</v>
       </c>
-      <c r="K2" s="649" t="s">
+      <c r="K2" s="595" t="s">
         <v>349</v>
       </c>
-      <c r="L2" s="650"/>
-      <c r="M2" s="622" t="s">
+      <c r="L2" s="596"/>
+      <c r="M2" s="601" t="s">
         <v>103</v>
       </c>
       <c r="N2" s="69" t="s">
         <v>28</v>
       </c>
-      <c r="O2" s="626" t="s">
+      <c r="O2" s="627" t="s">
         <v>103</v>
       </c>
       <c r="P2" s="85" t="s">
         <v>148</v>
       </c>
-      <c r="Q2" s="581" t="s">
+      <c r="Q2" s="591" t="s">
         <v>144</v>
       </c>
       <c r="R2" s="553"/>
-      <c r="S2" s="639" t="s">
+      <c r="S2" s="614" t="s">
         <v>149</v>
       </c>
       <c r="T2" s="89"/>
@@ -7812,15 +7812,15 @@
         <v>481</v>
       </c>
       <c r="AM2" s="453"/>
-      <c r="AN2" s="618"/>
+      <c r="AN2" s="621"/>
     </row>
     <row r="3" spans="1:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="600"/>
-      <c r="B3" s="602"/>
-      <c r="C3" s="582"/>
-      <c r="D3" s="604"/>
-      <c r="E3" s="648"/>
-      <c r="F3" s="623"/>
+      <c r="A3" s="645"/>
+      <c r="B3" s="647"/>
+      <c r="C3" s="592"/>
+      <c r="D3" s="649"/>
+      <c r="E3" s="594"/>
+      <c r="F3" s="602"/>
       <c r="G3" s="419" t="s">
         <v>28</v>
       </c>
@@ -7839,17 +7839,17 @@
       <c r="L3" s="206" t="s">
         <v>108</v>
       </c>
-      <c r="M3" s="623"/>
+      <c r="M3" s="602"/>
       <c r="N3" s="69" t="s">
         <v>147</v>
       </c>
-      <c r="O3" s="627"/>
+      <c r="O3" s="628"/>
       <c r="P3" s="2" t="s">
         <v>155</v>
       </c>
-      <c r="Q3" s="582"/>
+      <c r="Q3" s="592"/>
       <c r="R3" s="555"/>
-      <c r="S3" s="640"/>
+      <c r="S3" s="616"/>
       <c r="T3" s="89"/>
       <c r="U3" s="124"/>
       <c r="V3" s="120"/>
@@ -7866,7 +7866,7 @@
       <c r="AC3" s="100" t="s">
         <v>498</v>
       </c>
-      <c r="AD3" s="638" t="s">
+      <c r="AD3" s="611" t="s">
         <v>473</v>
       </c>
       <c r="AE3" s="262"/>
@@ -7878,16 +7878,16 @@
       <c r="AK3" s="262"/>
       <c r="AL3" s="16"/>
       <c r="AM3" s="453"/>
-      <c r="AN3" s="618"/>
+      <c r="AN3" s="621"/>
     </row>
     <row r="4" spans="1:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="243" t="s">
         <v>184</v>
       </c>
-      <c r="B4" s="615" t="s">
+      <c r="B4" s="660" t="s">
         <v>382</v>
       </c>
-      <c r="C4" s="581" t="s">
+      <c r="C4" s="591" t="s">
         <v>155</v>
       </c>
       <c r="D4" s="359" t="s">
@@ -7896,7 +7896,7 @@
       <c r="E4" s="396">
         <v>2</v>
       </c>
-      <c r="F4" s="623"/>
+      <c r="F4" s="602"/>
       <c r="G4" s="400" t="s">
         <v>203</v>
       </c>
@@ -7913,11 +7913,11 @@
         <v>151</v>
       </c>
       <c r="L4" s="209"/>
-      <c r="M4" s="623"/>
+      <c r="M4" s="602"/>
       <c r="N4" s="178" t="s">
         <v>70</v>
       </c>
-      <c r="O4" s="627"/>
+      <c r="O4" s="628"/>
       <c r="P4" s="2" t="s">
         <v>192</v>
       </c>
@@ -7944,7 +7944,7 @@
       <c r="AA4" s="313"/>
       <c r="AB4" s="214"/>
       <c r="AC4" s="16"/>
-      <c r="AD4" s="638"/>
+      <c r="AD4" s="611"/>
       <c r="AE4" s="262"/>
       <c r="AF4" s="262"/>
       <c r="AG4" s="16"/>
@@ -7954,37 +7954,37 @@
       <c r="AK4" s="262"/>
       <c r="AL4" s="16"/>
       <c r="AM4" s="453"/>
-      <c r="AN4" s="618"/>
+      <c r="AN4" s="621"/>
       <c r="AO4" s="350" t="s">
         <v>91</v>
       </c>
     </row>
     <row r="5" spans="1:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="579" t="s">
+      <c r="A5" s="589" t="s">
         <v>435</v>
       </c>
-      <c r="B5" s="616"/>
-      <c r="C5" s="582"/>
+      <c r="B5" s="661"/>
+      <c r="C5" s="592"/>
       <c r="D5" s="61" t="s">
         <v>154</v>
       </c>
       <c r="E5" s="397">
         <v>1</v>
       </c>
-      <c r="F5" s="623"/>
-      <c r="G5" s="607" t="s">
+      <c r="F5" s="602"/>
+      <c r="G5" s="652" t="s">
         <v>193</v>
       </c>
-      <c r="H5" s="607"/>
-      <c r="I5" s="607"/>
-      <c r="J5" s="607"/>
-      <c r="K5" s="607"/>
-      <c r="L5" s="608"/>
-      <c r="M5" s="623"/>
+      <c r="H5" s="652"/>
+      <c r="I5" s="652"/>
+      <c r="J5" s="652"/>
+      <c r="K5" s="652"/>
+      <c r="L5" s="653"/>
+      <c r="M5" s="602"/>
       <c r="N5" s="21">
         <v>8</v>
       </c>
-      <c r="O5" s="627"/>
+      <c r="O5" s="628"/>
       <c r="T5" s="89"/>
       <c r="U5" s="124"/>
       <c r="V5" s="120"/>
@@ -8015,24 +8015,24 @@
       <c r="AK5" s="262"/>
       <c r="AL5" s="80"/>
       <c r="AM5" s="453"/>
-      <c r="AN5" s="618"/>
+      <c r="AN5" s="621"/>
     </row>
     <row r="6" spans="1:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="580"/>
-      <c r="B6" s="613" t="s">
+      <c r="A6" s="590"/>
+      <c r="B6" s="658" t="s">
         <v>178</v>
       </c>
-      <c r="C6" s="577"/>
-      <c r="D6" s="578"/>
-      <c r="F6" s="623"/>
-      <c r="G6" s="609"/>
-      <c r="H6" s="609"/>
-      <c r="I6" s="609"/>
-      <c r="J6" s="609"/>
-      <c r="K6" s="609"/>
-      <c r="L6" s="610"/>
-      <c r="M6" s="623"/>
-      <c r="O6" s="627"/>
+      <c r="C6" s="587"/>
+      <c r="D6" s="588"/>
+      <c r="F6" s="602"/>
+      <c r="G6" s="654"/>
+      <c r="H6" s="654"/>
+      <c r="I6" s="654"/>
+      <c r="J6" s="654"/>
+      <c r="K6" s="654"/>
+      <c r="L6" s="655"/>
+      <c r="M6" s="602"/>
+      <c r="O6" s="628"/>
       <c r="T6" s="89"/>
       <c r="U6" s="124"/>
       <c r="V6" s="98" t="s">
@@ -8056,16 +8056,16 @@
       <c r="AF6" s="262"/>
       <c r="AG6" s="262"/>
       <c r="AH6" s="262"/>
-      <c r="AI6" s="632"/>
+      <c r="AI6" s="610"/>
       <c r="AJ6" s="466" t="s">
         <v>476</v>
       </c>
-      <c r="AK6" s="632" t="s">
+      <c r="AK6" s="610" t="s">
         <v>256</v>
       </c>
       <c r="AL6" s="262"/>
       <c r="AM6" s="453"/>
-      <c r="AN6" s="618"/>
+      <c r="AN6" s="621"/>
       <c r="AO6" s="350" t="s">
         <v>488</v>
       </c>
@@ -8074,7 +8074,7 @@
       <c r="A7" s="237" t="s">
         <v>598</v>
       </c>
-      <c r="B7" s="614"/>
+      <c r="B7" s="659"/>
       <c r="C7" s="207" t="s">
         <v>383</v>
       </c>
@@ -8084,7 +8084,7 @@
       <c r="E7" s="271">
         <v>3</v>
       </c>
-      <c r="F7" s="623"/>
+      <c r="F7" s="602"/>
       <c r="G7" s="420">
         <v>0</v>
       </c>
@@ -8103,8 +8103,8 @@
       <c r="L7" s="217">
         <v>0</v>
       </c>
-      <c r="M7" s="623"/>
-      <c r="O7" s="627"/>
+      <c r="M7" s="602"/>
+      <c r="O7" s="628"/>
       <c r="R7" s="99" t="s">
         <v>44</v>
       </c>
@@ -8128,18 +8128,18 @@
       <c r="AD7" s="16"/>
       <c r="AE7" s="262"/>
       <c r="AF7" s="262"/>
-      <c r="AG7" s="638" t="s">
+      <c r="AG7" s="611" t="s">
         <v>472</v>
       </c>
       <c r="AH7" s="262"/>
-      <c r="AI7" s="632"/>
+      <c r="AI7" s="610"/>
       <c r="AJ7" s="262"/>
-      <c r="AK7" s="632"/>
+      <c r="AK7" s="610"/>
       <c r="AL7" s="80" t="s">
         <v>515</v>
       </c>
       <c r="AM7" s="453"/>
-      <c r="AN7" s="618"/>
+      <c r="AN7" s="621"/>
       <c r="AP7" s="76" t="s">
         <v>489</v>
       </c>
@@ -8156,27 +8156,27 @@
         <f>SUM(G7:N9)</f>
         <v>15</v>
       </c>
-      <c r="F8" s="623"/>
-      <c r="G8" s="608">
-        <v>0</v>
-      </c>
-      <c r="H8" s="605" t="s">
+      <c r="F8" s="602"/>
+      <c r="G8" s="653">
+        <v>0</v>
+      </c>
+      <c r="H8" s="650" t="s">
         <v>105</v>
       </c>
       <c r="I8" s="553">
         <v>0</v>
       </c>
-      <c r="J8" s="605" t="s">
+      <c r="J8" s="650" t="s">
         <v>105</v>
       </c>
-      <c r="K8" s="611"/>
-      <c r="L8" s="641"/>
-      <c r="M8" s="624"/>
-      <c r="N8" s="644">
+      <c r="K8" s="656"/>
+      <c r="L8" s="612"/>
+      <c r="M8" s="625"/>
+      <c r="N8" s="617">
         <f>N5+N11</f>
         <v>15</v>
       </c>
-      <c r="O8" s="627"/>
+      <c r="O8" s="628"/>
       <c r="T8" s="103" t="s">
         <v>44</v>
       </c>
@@ -8194,14 +8194,14 @@
       <c r="AD8" s="16"/>
       <c r="AE8" s="262"/>
       <c r="AF8" s="262"/>
-      <c r="AG8" s="638"/>
+      <c r="AG8" s="611"/>
       <c r="AH8" s="262"/>
-      <c r="AI8" s="632"/>
+      <c r="AI8" s="610"/>
       <c r="AJ8" s="262"/>
       <c r="AK8" s="262"/>
       <c r="AL8" s="262"/>
       <c r="AM8" s="453"/>
-      <c r="AN8" s="618"/>
+      <c r="AN8" s="621"/>
     </row>
     <row r="9" spans="1:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="237" t="s">
@@ -8216,17 +8216,17 @@
       <c r="D9" s="360" t="s">
         <v>286</v>
       </c>
-      <c r="F9" s="623"/>
-      <c r="G9" s="610"/>
-      <c r="H9" s="606"/>
+      <c r="F9" s="602"/>
+      <c r="G9" s="655"/>
+      <c r="H9" s="651"/>
       <c r="I9" s="555"/>
-      <c r="J9" s="606"/>
-      <c r="K9" s="612"/>
-      <c r="L9" s="642"/>
-      <c r="M9" s="625"/>
-      <c r="N9" s="645"/>
-      <c r="O9" s="628"/>
-      <c r="S9" s="639" t="s">
+      <c r="J9" s="651"/>
+      <c r="K9" s="657"/>
+      <c r="L9" s="613"/>
+      <c r="M9" s="626"/>
+      <c r="N9" s="618"/>
+      <c r="O9" s="629"/>
+      <c r="S9" s="614" t="s">
         <v>62</v>
       </c>
       <c r="T9" s="89"/>
@@ -8248,16 +8248,16 @@
       </c>
       <c r="AE9" s="262"/>
       <c r="AF9" s="262"/>
-      <c r="AG9" s="638"/>
+      <c r="AG9" s="611"/>
       <c r="AH9" s="262"/>
-      <c r="AI9" s="632"/>
+      <c r="AI9" s="610"/>
       <c r="AJ9" s="80"/>
-      <c r="AK9" s="632" t="s">
+      <c r="AK9" s="610" t="s">
         <v>256</v>
       </c>
       <c r="AL9" s="262"/>
       <c r="AM9" s="453"/>
-      <c r="AN9" s="618"/>
+      <c r="AN9" s="621"/>
       <c r="AP9" s="2" t="s">
         <v>527</v>
       </c>
@@ -8272,22 +8272,22 @@
       <c r="D10" s="142"/>
       <c r="E10" s="242">
         <f>Boat!U8</f>
-        <v>41</v>
-      </c>
-      <c r="F10" s="623"/>
+        <v>40</v>
+      </c>
+      <c r="F10" s="602"/>
       <c r="N10" s="443" t="s">
         <v>407</v>
       </c>
-      <c r="O10" s="656" t="s">
+      <c r="O10" s="604" t="s">
         <v>103</v>
       </c>
-      <c r="P10" s="629" t="s">
+      <c r="P10" s="630" t="s">
         <v>411</v>
       </c>
       <c r="R10" s="74" t="s">
         <v>44</v>
       </c>
-      <c r="S10" s="643"/>
+      <c r="S10" s="615"/>
       <c r="T10" s="89"/>
       <c r="U10" s="123" t="s">
         <v>177</v>
@@ -8317,16 +8317,16 @@
       <c r="AF10" s="243" t="s">
         <v>318</v>
       </c>
-      <c r="AG10" s="638"/>
+      <c r="AG10" s="611"/>
       <c r="AH10" s="80"/>
-      <c r="AI10" s="632"/>
+      <c r="AI10" s="610"/>
       <c r="AJ10" s="262"/>
-      <c r="AK10" s="632"/>
+      <c r="AK10" s="610"/>
       <c r="AL10" s="262"/>
       <c r="AM10" s="467" t="s">
         <v>325</v>
       </c>
-      <c r="AN10" s="618"/>
+      <c r="AN10" s="621"/>
       <c r="AO10" s="209" t="s">
         <v>95</v>
       </c>
@@ -8344,18 +8344,18 @@
       <c r="D11" s="174" t="s">
         <v>362</v>
       </c>
-      <c r="F11" s="623"/>
+      <c r="F11" s="602"/>
       <c r="M11" s="6"/>
       <c r="N11" s="117">
         <v>7</v>
       </c>
-      <c r="O11" s="657"/>
-      <c r="P11" s="630"/>
+      <c r="O11" s="605"/>
+      <c r="P11" s="631"/>
       <c r="Q11" s="65"/>
       <c r="R11" s="120" t="s">
         <v>222</v>
       </c>
-      <c r="S11" s="643"/>
+      <c r="S11" s="615"/>
       <c r="T11" s="102" t="s">
         <v>44</v>
       </c>
@@ -8379,14 +8379,14 @@
       <c r="AF11" s="262" t="s">
         <v>494</v>
       </c>
-      <c r="AG11" s="638"/>
+      <c r="AG11" s="611"/>
       <c r="AH11" s="262"/>
       <c r="AI11" s="70"/>
       <c r="AJ11" s="262"/>
       <c r="AK11" s="262"/>
       <c r="AL11" s="262"/>
       <c r="AM11" s="453"/>
-      <c r="AN11" s="618"/>
+      <c r="AN11" s="621"/>
       <c r="AP11" s="76" t="s">
         <v>502</v>
       </c>
@@ -8405,7 +8405,7 @@
       <c r="E12" s="229">
         <v>3</v>
       </c>
-      <c r="F12" s="623"/>
+      <c r="F12" s="602"/>
       <c r="G12" s="349" t="s">
         <v>411</v>
       </c>
@@ -8414,16 +8414,16 @@
       </c>
       <c r="I12" s="560"/>
       <c r="J12" s="560"/>
-      <c r="K12" s="661"/>
+      <c r="K12" s="609"/>
       <c r="L12" s="208"/>
       <c r="M12" s="208"/>
       <c r="N12" s="208"/>
-      <c r="O12" s="657"/>
-      <c r="P12" s="630"/>
+      <c r="O12" s="605"/>
+      <c r="P12" s="631"/>
       <c r="R12" s="122" t="s">
         <v>181</v>
       </c>
-      <c r="S12" s="640"/>
+      <c r="S12" s="616"/>
       <c r="T12" s="101" t="s">
         <v>44</v>
       </c>
@@ -8444,16 +8444,16 @@
       <c r="AC12" s="100" t="s">
         <v>499</v>
       </c>
-      <c r="AD12" s="646" t="s">
+      <c r="AD12" s="619" t="s">
         <v>245</v>
       </c>
       <c r="AE12" s="466" t="s">
         <v>244</v>
       </c>
-      <c r="AF12" s="638" t="s">
+      <c r="AF12" s="611" t="s">
         <v>231</v>
       </c>
-      <c r="AG12" s="638"/>
+      <c r="AG12" s="611"/>
       <c r="AH12" s="243" t="s">
         <v>264</v>
       </c>
@@ -8466,7 +8466,7 @@
       <c r="AM12" s="633" t="s">
         <v>254</v>
       </c>
-      <c r="AN12" s="618"/>
+      <c r="AN12" s="621"/>
       <c r="AO12" s="350" t="s">
         <v>97</v>
       </c>
@@ -8478,17 +8478,17 @@
       <c r="E13" s="473">
         <v>-3</v>
       </c>
-      <c r="F13" s="623"/>
+      <c r="F13" s="602"/>
       <c r="G13" s="560" t="s">
         <v>448</v>
       </c>
       <c r="H13" s="560"/>
       <c r="I13" s="560"/>
-      <c r="J13" s="661"/>
+      <c r="J13" s="609"/>
       <c r="M13" s="6"/>
       <c r="N13" s="6"/>
-      <c r="O13" s="657"/>
-      <c r="P13" s="631"/>
+      <c r="O13" s="605"/>
+      <c r="P13" s="632"/>
       <c r="T13" s="105" t="s">
         <v>44</v>
       </c>
@@ -8509,8 +8509,8 @@
         <v>519</v>
       </c>
       <c r="AC13" s="16"/>
-      <c r="AD13" s="646"/>
-      <c r="AF13" s="638"/>
+      <c r="AD13" s="619"/>
+      <c r="AF13" s="611"/>
       <c r="AG13" s="80"/>
       <c r="AH13" s="243" t="s">
         <v>314</v>
@@ -8522,7 +8522,7 @@
       <c r="AK13" s="262"/>
       <c r="AL13" s="262"/>
       <c r="AM13" s="633"/>
-      <c r="AN13" s="618"/>
+      <c r="AN13" s="621"/>
     </row>
     <row r="14" spans="1:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="475"/>
@@ -8530,18 +8530,18 @@
       <c r="C14" s="484"/>
       <c r="D14" s="477"/>
       <c r="E14" s="478"/>
-      <c r="F14" s="623"/>
+      <c r="F14" s="602"/>
       <c r="G14" s="560" t="s">
         <v>447</v>
       </c>
       <c r="H14" s="560"/>
       <c r="I14" s="560"/>
-      <c r="J14" s="661"/>
+      <c r="J14" s="609"/>
       <c r="K14" s="2">
         <v>12</v>
       </c>
       <c r="N14" s="6"/>
-      <c r="O14" s="657"/>
+      <c r="O14" s="605"/>
       <c r="Q14" s="61" t="s">
         <v>555</v>
       </c>
@@ -8562,9 +8562,9 @@
       <c r="AA14" s="313"/>
       <c r="AB14" s="214"/>
       <c r="AC14" s="16"/>
-      <c r="AD14" s="646"/>
+      <c r="AD14" s="619"/>
       <c r="AE14" s="262"/>
-      <c r="AF14" s="638"/>
+      <c r="AF14" s="611"/>
       <c r="AG14" s="262"/>
       <c r="AH14" s="262"/>
       <c r="AI14" s="70"/>
@@ -8572,7 +8572,7 @@
       <c r="AK14" s="262"/>
       <c r="AL14" s="262"/>
       <c r="AM14" s="633"/>
-      <c r="AN14" s="618"/>
+      <c r="AN14" s="621"/>
     </row>
     <row r="15" spans="1:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="474" t="s">
@@ -8581,8 +8581,8 @@
       <c r="C15" s="553" t="s">
         <v>382</v>
       </c>
-      <c r="F15" s="623"/>
-      <c r="O15" s="657"/>
+      <c r="F15" s="602"/>
+      <c r="O15" s="605"/>
       <c r="R15" s="99" t="s">
         <v>44</v>
       </c>
@@ -8604,8 +8604,8 @@
       <c r="AC15" s="76" t="s">
         <v>497</v>
       </c>
-      <c r="AD15" s="646"/>
-      <c r="AF15" s="638"/>
+      <c r="AD15" s="619"/>
+      <c r="AF15" s="611"/>
       <c r="AG15" s="80"/>
       <c r="AH15" s="243" t="s">
         <v>466</v>
@@ -8619,7 +8619,7 @@
       <c r="AK15" s="262"/>
       <c r="AL15" s="262"/>
       <c r="AM15" s="633"/>
-      <c r="AN15" s="618"/>
+      <c r="AN15" s="621"/>
       <c r="AP15" s="76" t="s">
         <v>74</v>
       </c>
@@ -8641,13 +8641,13 @@
       <c r="E16" s="229">
         <v>1</v>
       </c>
-      <c r="F16" s="623"/>
+      <c r="F16" s="602"/>
       <c r="G16" s="349" t="s">
         <v>506</v>
       </c>
       <c r="I16" s="496"/>
       <c r="J16" s="20"/>
-      <c r="O16" s="657"/>
+      <c r="O16" s="605"/>
       <c r="R16" s="460" t="s">
         <v>185</v>
       </c>
@@ -8679,18 +8679,18 @@
       <c r="AM16" s="453" t="s">
         <v>324</v>
       </c>
-      <c r="AN16" s="618"/>
+      <c r="AN16" s="621"/>
       <c r="AP16" s="76" t="s">
         <v>235</v>
       </c>
     </row>
     <row r="17" spans="1:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B17" s="80"/>
-      <c r="F17" s="623"/>
+      <c r="F17" s="602"/>
       <c r="I17" s="497"/>
       <c r="J17" s="20"/>
       <c r="N17" s="6"/>
-      <c r="O17" s="657"/>
+      <c r="O17" s="605"/>
       <c r="Q17" s="21" t="s">
         <v>553</v>
       </c>
@@ -8735,7 +8735,7 @@
       <c r="AK17" s="262"/>
       <c r="AL17" s="80"/>
       <c r="AM17" s="453"/>
-      <c r="AN17" s="618"/>
+      <c r="AN17" s="621"/>
       <c r="AO17" s="209" t="s">
         <v>516</v>
       </c>
@@ -8759,21 +8759,21 @@
       <c r="E18" s="99" t="s">
         <v>44</v>
       </c>
-      <c r="F18" s="623"/>
+      <c r="F18" s="602"/>
       <c r="G18" s="349" t="s">
         <v>550</v>
       </c>
       <c r="I18" s="24"/>
       <c r="J18" s="20"/>
-      <c r="O18" s="657"/>
+      <c r="O18" s="605"/>
       <c r="Q18" s="112"/>
-      <c r="R18" s="651" t="s">
+      <c r="R18" s="597" t="s">
         <v>558</v>
       </c>
       <c r="T18" s="100" t="s">
         <v>44</v>
       </c>
-      <c r="U18" s="596" t="s">
+      <c r="U18" s="641" t="s">
         <v>44</v>
       </c>
       <c r="V18" s="120"/>
@@ -8794,7 +8794,7 @@
       <c r="AC18" s="16"/>
       <c r="AD18" s="16"/>
       <c r="AE18" s="262"/>
-      <c r="AF18" s="632" t="s">
+      <c r="AF18" s="610" t="s">
         <v>493</v>
       </c>
       <c r="AG18" s="262"/>
@@ -8806,20 +8806,20 @@
       <c r="AK18" s="262"/>
       <c r="AL18" s="80"/>
       <c r="AM18" s="453"/>
-      <c r="AN18" s="618"/>
+      <c r="AN18" s="621"/>
       <c r="AP18" s="76" t="s">
         <v>88</v>
       </c>
     </row>
     <row r="19" spans="1:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="F19" s="623"/>
+      <c r="F19" s="602"/>
       <c r="I19" s="224"/>
-      <c r="O19" s="657"/>
-      <c r="R19" s="652"/>
+      <c r="O19" s="605"/>
+      <c r="R19" s="598"/>
       <c r="S19" s="30" t="s">
         <v>556</v>
       </c>
-      <c r="U19" s="597"/>
+      <c r="U19" s="642"/>
       <c r="V19" s="146"/>
       <c r="W19" s="146"/>
       <c r="X19" s="456" t="s">
@@ -8834,7 +8834,7 @@
       <c r="AC19" s="16"/>
       <c r="AD19" s="16"/>
       <c r="AE19" s="262"/>
-      <c r="AF19" s="632"/>
+      <c r="AF19" s="610"/>
       <c r="AG19" s="262"/>
       <c r="AH19" s="262"/>
       <c r="AI19" s="70"/>
@@ -8844,7 +8844,7 @@
       </c>
       <c r="AL19" s="80"/>
       <c r="AM19" s="453"/>
-      <c r="AN19" s="618"/>
+      <c r="AN19" s="621"/>
       <c r="AP19" s="76" t="s">
         <v>486</v>
       </c>
@@ -8865,19 +8865,19 @@
       <c r="E20" s="462">
         <v>-1</v>
       </c>
-      <c r="F20" s="623"/>
+      <c r="F20" s="602"/>
       <c r="G20" s="349" t="s">
         <v>509</v>
       </c>
       <c r="I20" s="224"/>
-      <c r="O20" s="657"/>
-      <c r="Q20" s="659" t="s">
+      <c r="O20" s="605"/>
+      <c r="Q20" s="607" t="s">
         <v>48</v>
       </c>
       <c r="T20" s="429" t="s">
         <v>44</v>
       </c>
-      <c r="U20" s="598"/>
+      <c r="U20" s="643"/>
       <c r="W20" s="430"/>
       <c r="X20" s="457" t="s">
         <v>175</v>
@@ -8907,7 +8907,7 @@
       <c r="AM20" s="400" t="s">
         <v>254</v>
       </c>
-      <c r="AN20" s="618"/>
+      <c r="AN20" s="621"/>
       <c r="AO20" s="350" t="s">
         <v>478</v>
       </c>
@@ -8928,13 +8928,13 @@
       <c r="E21" s="271">
         <v>0</v>
       </c>
-      <c r="F21" s="623"/>
+      <c r="F21" s="602"/>
       <c r="I21" s="224"/>
-      <c r="O21" s="657"/>
-      <c r="Q21" s="660"/>
+      <c r="O21" s="605"/>
+      <c r="Q21" s="608"/>
       <c r="T21" s="447"/>
       <c r="U21" s="14"/>
-      <c r="V21" s="593"/>
+      <c r="V21" s="638"/>
       <c r="W21" s="451" t="s">
         <v>176</v>
       </c>
@@ -8972,15 +8972,15 @@
       <c r="AM21" s="453" t="s">
         <v>567</v>
       </c>
-      <c r="AN21" s="618"/>
+      <c r="AN21" s="621"/>
     </row>
     <row r="22" spans="1:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="F22" s="623"/>
+      <c r="F22" s="602"/>
       <c r="G22" s="349" t="s">
         <v>507</v>
       </c>
       <c r="I22" s="224"/>
-      <c r="O22" s="657"/>
+      <c r="O22" s="605"/>
       <c r="R22" s="459" t="s">
         <v>44</v>
       </c>
@@ -8988,7 +8988,7 @@
         <v>44</v>
       </c>
       <c r="U22" s="15"/>
-      <c r="V22" s="594"/>
+      <c r="V22" s="639"/>
       <c r="W22" s="451" t="s">
         <v>176</v>
       </c>
@@ -9006,7 +9006,7 @@
       <c r="AG22" s="6"/>
       <c r="AH22" s="6"/>
       <c r="AI22" s="6"/>
-      <c r="AJ22" s="632" t="s">
+      <c r="AJ22" s="610" t="s">
         <v>490</v>
       </c>
       <c r="AK22" s="262"/>
@@ -9014,7 +9014,7 @@
         <v>496</v>
       </c>
       <c r="AM22" s="306"/>
-      <c r="AN22" s="618"/>
+      <c r="AN22" s="621"/>
     </row>
     <row r="23" spans="1:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="236" t="s">
@@ -9032,17 +9032,17 @@
       <c r="E23" s="230">
         <v>1</v>
       </c>
-      <c r="F23" s="623"/>
+      <c r="F23" s="602"/>
       <c r="I23" s="224"/>
-      <c r="O23" s="657"/>
-      <c r="Q23" s="659" t="s">
+      <c r="O23" s="605"/>
+      <c r="Q23" s="607" t="s">
         <v>145</v>
       </c>
       <c r="T23" s="17"/>
       <c r="U23" s="445" t="s">
         <v>44</v>
       </c>
-      <c r="V23" s="594"/>
+      <c r="V23" s="639"/>
       <c r="W23" s="148"/>
       <c r="X23" s="454" t="s">
         <v>189</v>
@@ -9058,13 +9058,13 @@
       <c r="AG23" s="6"/>
       <c r="AH23" s="6"/>
       <c r="AI23" s="6"/>
-      <c r="AJ23" s="632"/>
+      <c r="AJ23" s="610"/>
       <c r="AK23" s="262"/>
       <c r="AL23" s="80" t="s">
         <v>526</v>
       </c>
       <c r="AM23" s="306"/>
-      <c r="AN23" s="618"/>
+      <c r="AN23" s="621"/>
     </row>
     <row r="24" spans="1:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="465" t="s">
@@ -9082,18 +9082,18 @@
       <c r="E24" s="461">
         <v>1</v>
       </c>
-      <c r="F24" s="623"/>
+      <c r="F24" s="602"/>
       <c r="G24" s="61" t="s">
         <v>508</v>
       </c>
       <c r="I24" s="224"/>
-      <c r="O24" s="657"/>
-      <c r="Q24" s="660"/>
+      <c r="O24" s="605"/>
+      <c r="Q24" s="608"/>
       <c r="T24" s="17"/>
       <c r="U24" s="232" t="s">
         <v>44</v>
       </c>
-      <c r="V24" s="594"/>
+      <c r="V24" s="639"/>
       <c r="W24" s="148"/>
       <c r="X24" s="454" t="s">
         <v>186</v>
@@ -9117,12 +9117,12 @@
         <v>481</v>
       </c>
       <c r="AM24" s="306"/>
-      <c r="AN24" s="618"/>
+      <c r="AN24" s="621"/>
     </row>
     <row r="25" spans="1:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="F25" s="623"/>
+      <c r="F25" s="602"/>
       <c r="I25" s="224"/>
-      <c r="O25" s="657"/>
+      <c r="O25" s="605"/>
       <c r="P25" s="209" t="s">
         <v>285</v>
       </c>
@@ -9135,7 +9135,7 @@
       <c r="U25" s="425" t="s">
         <v>44</v>
       </c>
-      <c r="V25" s="595"/>
+      <c r="V25" s="640"/>
       <c r="W25" s="148"/>
       <c r="X25" s="454" t="s">
         <v>190</v>
@@ -9157,7 +9157,7 @@
       <c r="AK25" s="142"/>
       <c r="AL25" s="6"/>
       <c r="AM25" s="306"/>
-      <c r="AN25" s="618"/>
+      <c r="AN25" s="621"/>
     </row>
     <row r="26" spans="1:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="236" t="s">
@@ -9175,17 +9175,17 @@
       <c r="E26" s="398">
         <v>1</v>
       </c>
-      <c r="F26" s="623"/>
+      <c r="F26" s="602"/>
       <c r="G26" s="349" t="s">
         <v>505</v>
       </c>
       <c r="I26" s="224"/>
-      <c r="O26" s="657"/>
-      <c r="P26" s="620" t="s">
+      <c r="O26" s="605"/>
+      <c r="P26" s="623" t="s">
         <v>548</v>
       </c>
-      <c r="Q26" s="621"/>
-      <c r="R26" s="653" t="s">
+      <c r="Q26" s="624"/>
+      <c r="R26" s="599" t="s">
         <v>557</v>
       </c>
       <c r="T26" s="182"/>
@@ -9224,7 +9224,7 @@
       <c r="AM26" s="467" t="s">
         <v>474</v>
       </c>
-      <c r="AN26" s="618"/>
+      <c r="AN26" s="621"/>
     </row>
     <row r="27" spans="1:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B27" s="21" t="s">
@@ -9236,13 +9236,13 @@
       <c r="E27" s="271" t="s">
         <v>44</v>
       </c>
-      <c r="F27" s="655"/>
+      <c r="F27" s="603"/>
       <c r="G27" s="61" t="s">
         <v>566</v>
       </c>
       <c r="I27" s="225"/>
-      <c r="O27" s="658"/>
-      <c r="R27" s="654"/>
+      <c r="O27" s="606"/>
+      <c r="R27" s="600"/>
       <c r="S27" s="446" t="s">
         <v>54</v>
       </c>
@@ -9272,32 +9272,26 @@
       <c r="AM27" s="400" t="s">
         <v>326</v>
       </c>
-      <c r="AN27" s="619"/>
+      <c r="AN27" s="622"/>
     </row>
   </sheetData>
   <mergeCells count="54">
-    <mergeCell ref="E2:E3"/>
-    <mergeCell ref="K2:L2"/>
-    <mergeCell ref="I1:I2"/>
-    <mergeCell ref="R18:R19"/>
-    <mergeCell ref="R26:R27"/>
-    <mergeCell ref="F2:F27"/>
-    <mergeCell ref="O10:O27"/>
-    <mergeCell ref="Q20:Q21"/>
-    <mergeCell ref="Q23:Q24"/>
-    <mergeCell ref="G14:J14"/>
-    <mergeCell ref="G13:J13"/>
-    <mergeCell ref="H12:K12"/>
-    <mergeCell ref="A5:A6"/>
-    <mergeCell ref="C6:D6"/>
-    <mergeCell ref="AI6:AI10"/>
-    <mergeCell ref="AF12:AF15"/>
-    <mergeCell ref="AG7:AG12"/>
-    <mergeCell ref="L8:L9"/>
-    <mergeCell ref="S9:S12"/>
-    <mergeCell ref="N8:N9"/>
-    <mergeCell ref="AD12:AD15"/>
-    <mergeCell ref="C15:C16"/>
+    <mergeCell ref="V21:V25"/>
+    <mergeCell ref="U18:U20"/>
+    <mergeCell ref="C2:C3"/>
+    <mergeCell ref="C4:C5"/>
+    <mergeCell ref="A2:A3"/>
+    <mergeCell ref="B2:B3"/>
+    <mergeCell ref="D2:D3"/>
+    <mergeCell ref="J8:J9"/>
+    <mergeCell ref="G5:L6"/>
+    <mergeCell ref="I8:I9"/>
+    <mergeCell ref="K7:K9"/>
+    <mergeCell ref="H8:H9"/>
+    <mergeCell ref="G8:G9"/>
+    <mergeCell ref="B11:B12"/>
+    <mergeCell ref="B6:B7"/>
+    <mergeCell ref="B4:B5"/>
     <mergeCell ref="AN1:AN27"/>
     <mergeCell ref="P26:Q26"/>
     <mergeCell ref="Q2:Q3"/>
@@ -9314,22 +9308,28 @@
     <mergeCell ref="AD3:AD4"/>
     <mergeCell ref="S2:S3"/>
     <mergeCell ref="R2:R3"/>
-    <mergeCell ref="V21:V25"/>
-    <mergeCell ref="U18:U20"/>
-    <mergeCell ref="C2:C3"/>
-    <mergeCell ref="C4:C5"/>
-    <mergeCell ref="A2:A3"/>
-    <mergeCell ref="B2:B3"/>
-    <mergeCell ref="D2:D3"/>
-    <mergeCell ref="J8:J9"/>
-    <mergeCell ref="G5:L6"/>
-    <mergeCell ref="I8:I9"/>
-    <mergeCell ref="K7:K9"/>
-    <mergeCell ref="H8:H9"/>
-    <mergeCell ref="G8:G9"/>
-    <mergeCell ref="B11:B12"/>
-    <mergeCell ref="B6:B7"/>
-    <mergeCell ref="B4:B5"/>
+    <mergeCell ref="A5:A6"/>
+    <mergeCell ref="C6:D6"/>
+    <mergeCell ref="AI6:AI10"/>
+    <mergeCell ref="AF12:AF15"/>
+    <mergeCell ref="AG7:AG12"/>
+    <mergeCell ref="L8:L9"/>
+    <mergeCell ref="S9:S12"/>
+    <mergeCell ref="N8:N9"/>
+    <mergeCell ref="AD12:AD15"/>
+    <mergeCell ref="C15:C16"/>
+    <mergeCell ref="E2:E3"/>
+    <mergeCell ref="K2:L2"/>
+    <mergeCell ref="I1:I2"/>
+    <mergeCell ref="R18:R19"/>
+    <mergeCell ref="R26:R27"/>
+    <mergeCell ref="F2:F27"/>
+    <mergeCell ref="O10:O27"/>
+    <mergeCell ref="Q20:Q21"/>
+    <mergeCell ref="Q23:Q24"/>
+    <mergeCell ref="G14:J14"/>
+    <mergeCell ref="G13:J13"/>
+    <mergeCell ref="H12:K12"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -9339,8 +9339,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2029A93E-B53C-4201-9F17-439C144F3CF1}">
   <dimension ref="A1:AN37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="M1" workbookViewId="0">
-      <selection activeCell="AH31" sqref="AH31"/>
+    <sheetView topLeftCell="N1" workbookViewId="0">
+      <selection activeCell="AG12" sqref="AG12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9435,10 +9435,10 @@
       <c r="S1" s="142"/>
       <c r="T1" s="142"/>
       <c r="U1" s="6"/>
-      <c r="V1" s="668" t="s">
+      <c r="V1" s="665" t="s">
         <v>459</v>
       </c>
-      <c r="W1" s="669"/>
+      <c r="W1" s="666"/>
       <c r="X1" s="312">
         <f>68-(U8+W3+V3+S3)</f>
         <v>0</v>
@@ -9454,21 +9454,21 @@
       <c r="AB1" s="308" t="s">
         <v>44</v>
       </c>
-      <c r="AC1" s="670" t="s">
+      <c r="AC1" s="667" t="s">
         <v>191</v>
       </c>
-      <c r="AD1" s="671"/>
-      <c r="AE1" s="672"/>
-      <c r="AF1" s="673" t="s">
+      <c r="AD1" s="668"/>
+      <c r="AE1" s="669"/>
+      <c r="AF1" s="670" t="s">
         <v>298</v>
       </c>
-      <c r="AG1" s="674"/>
-      <c r="AH1" s="675"/>
-      <c r="AI1" s="665" t="s">
+      <c r="AG1" s="671"/>
+      <c r="AH1" s="672"/>
+      <c r="AI1" s="662" t="s">
         <v>462</v>
       </c>
-      <c r="AJ1" s="666"/>
-      <c r="AK1" s="667"/>
+      <c r="AJ1" s="663"/>
+      <c r="AK1" s="664"/>
       <c r="AN1" s="142"/>
     </row>
     <row r="2" spans="1:40" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -9485,19 +9485,19 @@
       <c r="K2" s="327">
         <v>-3</v>
       </c>
-      <c r="L2" s="676">
+      <c r="L2" s="673">
         <f>SUM(L5:L30)</f>
-        <v>2</v>
-      </c>
-      <c r="M2" s="678">
+        <v>4</v>
+      </c>
+      <c r="M2" s="675">
         <f>SUM(M4:M29)</f>
+        <v>6</v>
+      </c>
+      <c r="N2" s="677">
+        <f>SUM(N4:N29)</f>
         <v>7</v>
       </c>
-      <c r="N2" s="680">
-        <f>SUM(N4:N29)</f>
-        <v>6</v>
-      </c>
-      <c r="O2" s="644">
+      <c r="O2" s="617">
         <f>SUM(M30:M37)* (-1)</f>
         <v>-3</v>
       </c>
@@ -9516,7 +9516,7 @@
       <c r="T2" s="516" t="s">
         <v>221</v>
       </c>
-      <c r="U2" s="682" t="s">
+      <c r="U2" s="679" t="s">
         <v>239</v>
       </c>
       <c r="V2" s="517" t="s">
@@ -9585,10 +9585,10 @@
         <f>T3+V3+W3+S3</f>
         <v>68</v>
       </c>
-      <c r="L3" s="677"/>
-      <c r="M3" s="679"/>
-      <c r="N3" s="681"/>
-      <c r="O3" s="645"/>
+      <c r="L3" s="674"/>
+      <c r="M3" s="676"/>
+      <c r="N3" s="678"/>
+      <c r="O3" s="618"/>
       <c r="P3" s="176">
         <f>(L2+M2)-W3</f>
         <v>0</v>
@@ -9602,16 +9602,16 @@
       </c>
       <c r="T3" s="519">
         <f>SUM(T4:T29)</f>
-        <v>41</v>
-      </c>
-      <c r="U3" s="683"/>
+        <v>40</v>
+      </c>
+      <c r="U3" s="680"/>
       <c r="V3" s="520">
         <f t="shared" ref="V3:AA3" si="0">SUM(V4:V29)</f>
         <v>6</v>
       </c>
       <c r="W3" s="520">
         <f t="shared" si="0"/>
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="X3" s="59">
         <f t="shared" si="0"/>
@@ -9619,15 +9619,15 @@
       </c>
       <c r="Y3" s="66">
         <f t="shared" si="0"/>
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="Z3" s="66">
         <f t="shared" si="0"/>
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="AA3" s="66">
         <f t="shared" si="0"/>
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="AB3" s="66">
         <f t="shared" ref="AB3:AK3" si="1">SUM(AB4:AB29)</f>
@@ -9635,7 +9635,7 @@
       </c>
       <c r="AC3" s="66">
         <f t="shared" si="1"/>
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="AD3" s="66">
         <f t="shared" si="1"/>
@@ -9647,7 +9647,7 @@
       </c>
       <c r="AF3" s="66">
         <f>SUM(AF4:AF29)</f>
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="AG3" s="386">
         <f t="shared" si="1"/>
@@ -9659,15 +9659,15 @@
       </c>
       <c r="AI3" s="100">
         <f t="shared" si="1"/>
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="AJ3" s="317">
         <f t="shared" si="1"/>
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="AK3" s="318">
         <f t="shared" si="1"/>
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="AN3" s="142"/>
     </row>
@@ -9703,7 +9703,7 @@
         <f>AA4</f>
         <v>0</v>
       </c>
-      <c r="O4" s="662" t="s">
+      <c r="O4" s="681" t="s">
         <v>200</v>
       </c>
       <c r="P4" s="20"/>
@@ -9782,7 +9782,7 @@
         <f>AA5</f>
         <v>0</v>
       </c>
-      <c r="O5" s="663"/>
+      <c r="O5" s="682"/>
       <c r="P5" s="20"/>
       <c r="Q5" s="2" t="s">
         <v>347</v>
@@ -9870,7 +9870,7 @@
         <f>AA6</f>
         <v>0</v>
       </c>
-      <c r="O6" s="663"/>
+      <c r="O6" s="682"/>
       <c r="P6" s="19" t="s">
         <v>342</v>
       </c>
@@ -9961,7 +9961,7 @@
         <f t="shared" ref="N7:N37" si="10">AA7</f>
         <v>0</v>
       </c>
-      <c r="O7" s="663"/>
+      <c r="O7" s="682"/>
       <c r="P7" s="20"/>
       <c r="Q7" s="2" t="s">
         <v>342</v>
@@ -10067,7 +10067,7 @@
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
-      <c r="O8" s="663"/>
+      <c r="O8" s="682"/>
       <c r="P8" s="21" t="s">
         <v>238</v>
       </c>
@@ -10085,7 +10085,7 @@
       </c>
       <c r="U8" s="29">
         <f>T3</f>
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="V8" s="532">
         <v>0</v>
@@ -10151,7 +10151,7 @@
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
-      <c r="O9" s="663"/>
+      <c r="O9" s="682"/>
       <c r="P9" s="21" t="s">
         <v>342</v>
       </c>
@@ -10239,15 +10239,17 @@
       <c r="K10" s="403" t="s">
         <v>363</v>
       </c>
-      <c r="L10" s="338"/>
+      <c r="L10" s="338">
+        <v>2</v>
+      </c>
       <c r="M10" s="107">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="N10" s="299">
         <f t="shared" si="10"/>
-        <v>1</v>
-      </c>
-      <c r="O10" s="663"/>
+        <v>2</v>
+      </c>
+      <c r="O10" s="682"/>
       <c r="P10" s="20"/>
       <c r="Q10" s="2" t="s">
         <v>347</v>
@@ -10259,7 +10261,7 @@
         <v>0</v>
       </c>
       <c r="T10" s="527">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U10" s="528">
         <v>-2</v>
@@ -10267,53 +10269,55 @@
       <c r="V10" s="531"/>
       <c r="W10" s="525">
         <f t="shared" si="2"/>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="X10" s="302"/>
       <c r="Y10" s="117">
         <f t="shared" si="3"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="Z10" s="296">
         <f t="shared" si="6"/>
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="AA10" s="296">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AB10" s="296">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="AC10" s="300">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AD10" s="306"/>
       <c r="AE10" s="302"/>
       <c r="AF10" s="302">
         <f t="shared" si="5"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AG10" s="348"/>
       <c r="AH10" s="158"/>
       <c r="AI10" s="314">
         <f t="shared" si="7"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AJ10" s="315">
         <f t="shared" si="8"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AK10" s="316">
         <f t="shared" si="9"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AL10" s="6" t="s">
         <v>74</v>
       </c>
-      <c r="AM10" s="321"/>
+      <c r="AM10" s="546" t="s">
+        <v>589</v>
+      </c>
       <c r="AN10" s="262" t="s">
-        <v>591</v>
+        <v>513</v>
       </c>
     </row>
     <row r="11" spans="1:40" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -10328,7 +10332,7 @@
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
-      <c r="O11" s="663"/>
+      <c r="O11" s="682"/>
       <c r="P11" s="21" t="s">
         <v>342</v>
       </c>
@@ -10388,7 +10392,7 @@
       <c r="AN11" s="142"/>
     </row>
     <row r="12" spans="1:40" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="608" t="s">
+      <c r="A12" s="653" t="s">
         <v>55</v>
       </c>
       <c r="B12" s="30">
@@ -10397,7 +10401,7 @@
       <c r="C12" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="E12" s="659" t="s">
+      <c r="E12" s="607" t="s">
         <v>57</v>
       </c>
       <c r="G12" s="267"/>
@@ -10415,7 +10419,7 @@
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
-      <c r="O12" s="663"/>
+      <c r="O12" s="682"/>
       <c r="P12" s="21" t="s">
         <v>342</v>
       </c>
@@ -10483,14 +10487,14 @@
       </c>
     </row>
     <row r="13" spans="1:40" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="610"/>
+      <c r="A13" s="655"/>
       <c r="B13" s="153">
         <v>12</v>
       </c>
       <c r="C13" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="E13" s="660"/>
+      <c r="E13" s="608"/>
       <c r="F13" s="176">
         <v>0</v>
       </c>
@@ -10513,7 +10517,7 @@
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
-      <c r="O13" s="663"/>
+      <c r="O13" s="682"/>
       <c r="P13" s="21" t="s">
         <v>342</v>
       </c>
@@ -10586,7 +10590,7 @@
         <f t="shared" si="10"/>
         <v>1</v>
       </c>
-      <c r="O14" s="663"/>
+      <c r="O14" s="682"/>
       <c r="P14" s="20"/>
       <c r="Q14" s="205" t="s">
         <v>346</v>
@@ -10683,7 +10687,7 @@
         <f t="shared" si="10"/>
         <v>1</v>
       </c>
-      <c r="O15" s="663"/>
+      <c r="O15" s="682"/>
       <c r="P15" s="20"/>
       <c r="Q15" s="205" t="s">
         <v>346</v>
@@ -10770,7 +10774,7 @@
         <f t="shared" si="10"/>
         <v>1</v>
       </c>
-      <c r="O16" s="663"/>
+      <c r="O16" s="682"/>
       <c r="P16" s="21" t="s">
         <v>342</v>
       </c>
@@ -10868,7 +10872,7 @@
         <f t="shared" si="10"/>
         <v>1</v>
       </c>
-      <c r="O17" s="663"/>
+      <c r="O17" s="682"/>
       <c r="P17" s="20"/>
       <c r="Q17" s="2" t="s">
         <v>348</v>
@@ -10963,7 +10967,7 @@
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
-      <c r="O18" s="663"/>
+      <c r="O18" s="682"/>
       <c r="P18" s="21" t="s">
         <v>342</v>
       </c>
@@ -11046,7 +11050,7 @@
         <f t="shared" si="10"/>
         <v>1</v>
       </c>
-      <c r="O19" s="663"/>
+      <c r="O19" s="682"/>
       <c r="P19" s="20"/>
       <c r="Q19" s="2" t="s">
         <v>341</v>
@@ -11142,11 +11146,11 @@
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
-      <c r="O20" s="664"/>
+      <c r="O20" s="683"/>
       <c r="P20" s="558" t="s">
         <v>342</v>
       </c>
-      <c r="Q20" s="661"/>
+      <c r="Q20" s="609"/>
       <c r="R20" s="321" t="s">
         <v>86</v>
       </c>
@@ -11381,7 +11385,7 @@
       <c r="AN22" s="142"/>
     </row>
     <row r="23" spans="1:40" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E23" s="615" t="s">
+      <c r="E23" s="660" t="s">
         <v>294</v>
       </c>
       <c r="F23" s="184"/>
@@ -11474,7 +11478,7 @@
       <c r="C24" s="2" t="s">
         <v>260</v>
       </c>
-      <c r="E24" s="616"/>
+      <c r="E24" s="661"/>
       <c r="F24" s="176"/>
       <c r="K24" s="403" t="s">
         <v>301</v>
@@ -11492,7 +11496,7 @@
       <c r="P24" s="558" t="s">
         <v>342</v>
       </c>
-      <c r="Q24" s="661"/>
+      <c r="Q24" s="609"/>
       <c r="R24" s="321" t="s">
         <v>254</v>
       </c>
@@ -12564,6 +12568,12 @@
     </row>
   </sheetData>
   <mergeCells count="15">
+    <mergeCell ref="A12:A13"/>
+    <mergeCell ref="E12:E13"/>
+    <mergeCell ref="P20:Q20"/>
+    <mergeCell ref="E23:E24"/>
+    <mergeCell ref="P24:Q24"/>
+    <mergeCell ref="O4:O20"/>
     <mergeCell ref="AI1:AK1"/>
     <mergeCell ref="V1:W1"/>
     <mergeCell ref="AC1:AE1"/>
@@ -12573,12 +12583,6 @@
     <mergeCell ref="N2:N3"/>
     <mergeCell ref="O2:O3"/>
     <mergeCell ref="U2:U3"/>
-    <mergeCell ref="A12:A13"/>
-    <mergeCell ref="E12:E13"/>
-    <mergeCell ref="P20:Q20"/>
-    <mergeCell ref="E23:E24"/>
-    <mergeCell ref="P24:Q24"/>
-    <mergeCell ref="O4:O20"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -12615,12 +12619,12 @@
       <c r="B1" s="558" t="s">
         <v>317</v>
       </c>
-      <c r="C1" s="661"/>
+      <c r="C1" s="609"/>
       <c r="D1" s="209"/>
       <c r="J1" s="558" t="s">
         <v>70</v>
       </c>
-      <c r="K1" s="661"/>
+      <c r="K1" s="609"/>
       <c r="L1" s="200" t="s">
         <v>337</v>
       </c>
@@ -13011,7 +13015,7 @@
       <c r="V1" s="558" t="s">
         <v>71</v>
       </c>
-      <c r="W1" s="661"/>
+      <c r="W1" s="609"/>
       <c r="X1" s="62" t="s">
         <v>102</v>
       </c>
@@ -13030,7 +13034,7 @@
       <c r="AC1" s="116" t="s">
         <v>191</v>
       </c>
-      <c r="AD1" s="704" t="s">
+      <c r="AD1" s="697" t="s">
         <v>213</v>
       </c>
       <c r="AE1" s="116" t="s">
@@ -13047,10 +13051,10 @@
       <c r="E2" s="39" t="s">
         <v>74</v>
       </c>
-      <c r="F2" s="735" t="s">
+      <c r="F2" s="696" t="s">
         <v>75</v>
       </c>
-      <c r="G2" s="692" t="s">
+      <c r="G2" s="724" t="s">
         <v>44</v>
       </c>
       <c r="H2" s="40" t="s">
@@ -13078,10 +13082,10 @@
       <c r="U2" s="60" t="s">
         <v>106</v>
       </c>
-      <c r="V2" s="668" t="s">
+      <c r="V2" s="665" t="s">
         <v>121</v>
       </c>
-      <c r="W2" s="669"/>
+      <c r="W2" s="666"/>
       <c r="X2" s="64" t="s">
         <v>110</v>
       </c>
@@ -13100,7 +13104,7 @@
       <c r="AC2" s="117" t="s">
         <v>99</v>
       </c>
-      <c r="AD2" s="705"/>
+      <c r="AD2" s="698"/>
       <c r="AE2" s="64" t="s">
         <v>99</v>
       </c>
@@ -13119,8 +13123,8 @@
       <c r="E3" s="39" t="s">
         <v>80</v>
       </c>
-      <c r="F3" s="612"/>
-      <c r="G3" s="693"/>
+      <c r="F3" s="657"/>
+      <c r="G3" s="725"/>
       <c r="H3" s="40" t="s">
         <v>81</v>
       </c>
@@ -13131,13 +13135,13 @@
         <v>82</v>
       </c>
       <c r="N3" s="44"/>
-      <c r="O3" s="702" t="s">
+      <c r="O3" s="734" t="s">
         <v>44</v>
       </c>
-      <c r="P3" s="723" t="s">
+      <c r="P3" s="716" t="s">
         <v>219</v>
       </c>
-      <c r="Q3" s="724"/>
+      <c r="Q3" s="717"/>
       <c r="S3" s="57" t="s">
         <v>220</v>
       </c>
@@ -13147,15 +13151,15 @@
       <c r="W3" s="59" t="s">
         <v>105</v>
       </c>
-      <c r="AD3" s="705"/>
+      <c r="AD3" s="698"/>
     </row>
     <row r="4" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="G4" s="693"/>
+      <c r="G4" s="725"/>
       <c r="H4" s="6"/>
       <c r="L4" s="687" t="s">
         <v>83</v>
       </c>
-      <c r="O4" s="703"/>
+      <c r="O4" s="735"/>
       <c r="T4" s="55" t="s">
         <v>98</v>
       </c>
@@ -13169,8 +13173,8 @@
         <v>195</v>
       </c>
       <c r="Z4" s="560"/>
-      <c r="AA4" s="661"/>
-      <c r="AD4" s="705"/>
+      <c r="AA4" s="609"/>
+      <c r="AD4" s="698"/>
     </row>
     <row r="5" spans="1:31" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C5" s="52" t="s">
@@ -13185,21 +13189,21 @@
       <c r="F5" s="66" t="s">
         <v>85</v>
       </c>
-      <c r="G5" s="693"/>
+      <c r="G5" s="725"/>
       <c r="H5" s="46" t="s">
         <v>76</v>
       </c>
-      <c r="K5" s="710" t="s">
+      <c r="K5" s="703" t="s">
         <v>217</v>
       </c>
-      <c r="L5" s="725"/>
+      <c r="L5" s="718"/>
       <c r="M5" s="2" t="s">
         <v>215</v>
       </c>
       <c r="N5" s="61" t="s">
         <v>214</v>
       </c>
-      <c r="O5" s="703"/>
+      <c r="O5" s="735"/>
       <c r="P5" s="108" t="s">
         <v>216</v>
       </c>
@@ -13215,11 +13219,11 @@
       <c r="U5" s="19" t="s">
         <v>99</v>
       </c>
-      <c r="Y5" s="713" t="s">
+      <c r="Y5" s="706" t="s">
         <v>287</v>
       </c>
-      <c r="Z5" s="714"/>
-      <c r="AD5" s="705"/>
+      <c r="Z5" s="707"/>
+      <c r="AD5" s="698"/>
     </row>
     <row r="6" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C6" s="109"/>
@@ -13229,16 +13233,16 @@
       <c r="E6" s="45" t="s">
         <v>86</v>
       </c>
-      <c r="G6" s="693"/>
+      <c r="G6" s="725"/>
       <c r="H6" s="46" t="s">
         <v>81</v>
       </c>
       <c r="I6" s="23">
         <v>15</v>
       </c>
-      <c r="K6" s="711"/>
-      <c r="L6" s="725"/>
-      <c r="O6" s="703"/>
+      <c r="K6" s="704"/>
+      <c r="L6" s="718"/>
+      <c r="O6" s="735"/>
       <c r="T6" s="2" t="s">
         <v>101</v>
       </c>
@@ -13248,23 +13252,23 @@
       <c r="V6" s="21">
         <v>-1</v>
       </c>
-      <c r="AD6" s="705"/>
+      <c r="AD6" s="698"/>
     </row>
     <row r="7" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C7" s="110"/>
-      <c r="G7" s="693"/>
+      <c r="G7" s="725"/>
       <c r="H7" s="6"/>
-      <c r="K7" s="711"/>
-      <c r="L7" s="725"/>
+      <c r="K7" s="704"/>
+      <c r="L7" s="718"/>
       <c r="N7" s="21" t="s">
         <v>120</v>
       </c>
-      <c r="O7" s="703"/>
+      <c r="O7" s="735"/>
       <c r="P7" s="73"/>
       <c r="U7" s="104" t="s">
         <v>20</v>
       </c>
-      <c r="AD7" s="705"/>
+      <c r="AD7" s="698"/>
     </row>
     <row r="8" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C8" s="130"/>
@@ -13277,7 +13281,7 @@
       <c r="F8" s="66" t="s">
         <v>87</v>
       </c>
-      <c r="G8" s="693"/>
+      <c r="G8" s="725"/>
       <c r="H8" s="50" t="s">
         <v>76</v>
       </c>
@@ -13287,41 +13291,41 @@
       <c r="J8" s="111">
         <v>115</v>
       </c>
-      <c r="K8" s="711"/>
-      <c r="L8" s="725"/>
-      <c r="O8" s="703"/>
+      <c r="K8" s="704"/>
+      <c r="L8" s="718"/>
+      <c r="O8" s="735"/>
       <c r="P8" s="49"/>
-      <c r="S8" s="707" t="s">
+      <c r="S8" s="700" t="s">
         <v>212</v>
       </c>
-      <c r="T8" s="708"/>
-      <c r="U8" s="708"/>
-      <c r="V8" s="708"/>
-      <c r="W8" s="708"/>
-      <c r="X8" s="708"/>
-      <c r="Y8" s="708"/>
-      <c r="Z8" s="708"/>
-      <c r="AA8" s="708"/>
-      <c r="AB8" s="708"/>
-      <c r="AC8" s="709"/>
-      <c r="AD8" s="705"/>
+      <c r="T8" s="701"/>
+      <c r="U8" s="701"/>
+      <c r="V8" s="701"/>
+      <c r="W8" s="701"/>
+      <c r="X8" s="701"/>
+      <c r="Y8" s="701"/>
+      <c r="Z8" s="701"/>
+      <c r="AA8" s="701"/>
+      <c r="AB8" s="701"/>
+      <c r="AC8" s="702"/>
+      <c r="AD8" s="698"/>
     </row>
     <row r="9" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C9" s="729"/>
-      <c r="G9" s="693"/>
+      <c r="C9" s="690"/>
+      <c r="G9" s="725"/>
       <c r="H9" s="6"/>
-      <c r="K9" s="711"/>
-      <c r="L9" s="696" t="s">
+      <c r="K9" s="704"/>
+      <c r="L9" s="728" t="s">
         <v>218</v>
       </c>
-      <c r="M9" s="697"/>
-      <c r="N9" s="698"/>
-      <c r="O9" s="703"/>
+      <c r="M9" s="729"/>
+      <c r="N9" s="730"/>
+      <c r="O9" s="735"/>
       <c r="P9" s="75"/>
-      <c r="AD9" s="705"/>
+      <c r="AD9" s="698"/>
     </row>
     <row r="10" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C10" s="730"/>
+      <c r="C10" s="691"/>
       <c r="D10" s="23"/>
       <c r="E10" s="45" t="s">
         <v>88</v>
@@ -13329,7 +13333,7 @@
       <c r="F10" s="66" t="s">
         <v>89</v>
       </c>
-      <c r="G10" s="693"/>
+      <c r="G10" s="725"/>
       <c r="H10" s="51"/>
       <c r="I10" s="21" t="s">
         <v>81</v>
@@ -13337,33 +13341,33 @@
       <c r="J10" s="3">
         <v>15</v>
       </c>
-      <c r="K10" s="711"/>
-      <c r="M10" s="732" t="s">
+      <c r="K10" s="704"/>
+      <c r="M10" s="693" t="s">
         <v>90</v>
       </c>
-      <c r="N10" s="733"/>
-      <c r="O10" s="733"/>
-      <c r="P10" s="733"/>
-      <c r="Q10" s="733"/>
-      <c r="R10" s="733"/>
-      <c r="S10" s="733"/>
-      <c r="T10" s="733"/>
-      <c r="U10" s="733"/>
-      <c r="V10" s="733"/>
-      <c r="W10" s="733"/>
-      <c r="X10" s="733"/>
-      <c r="Y10" s="733"/>
-      <c r="Z10" s="733"/>
-      <c r="AA10" s="733"/>
-      <c r="AB10" s="733"/>
-      <c r="AC10" s="734"/>
-      <c r="AD10" s="705"/>
+      <c r="N10" s="694"/>
+      <c r="O10" s="694"/>
+      <c r="P10" s="694"/>
+      <c r="Q10" s="694"/>
+      <c r="R10" s="694"/>
+      <c r="S10" s="694"/>
+      <c r="T10" s="694"/>
+      <c r="U10" s="694"/>
+      <c r="V10" s="694"/>
+      <c r="W10" s="694"/>
+      <c r="X10" s="694"/>
+      <c r="Y10" s="694"/>
+      <c r="Z10" s="694"/>
+      <c r="AA10" s="694"/>
+      <c r="AB10" s="694"/>
+      <c r="AC10" s="695"/>
+      <c r="AD10" s="698"/>
     </row>
     <row r="11" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C11" s="731"/>
-      <c r="G11" s="693"/>
+      <c r="C11" s="692"/>
+      <c r="G11" s="725"/>
       <c r="H11" s="6"/>
-      <c r="K11" s="711"/>
+      <c r="K11" s="704"/>
       <c r="R11" s="52" t="s">
         <v>44</v>
       </c>
@@ -13371,17 +13375,17 @@
       <c r="Y11" s="68" t="s">
         <v>121</v>
       </c>
-      <c r="Z11" s="721" t="s">
+      <c r="Z11" s="714" t="s">
         <v>121</v>
       </c>
-      <c r="AA11" s="722"/>
+      <c r="AA11" s="715"/>
       <c r="AB11" s="52" t="s">
         <v>44</v>
       </c>
       <c r="AC11" s="118" t="s">
         <v>121</v>
       </c>
-      <c r="AD11" s="705"/>
+      <c r="AD11" s="698"/>
     </row>
     <row r="12" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C12" s="129"/>
@@ -13394,7 +13398,7 @@
       <c r="F12" s="66" t="s">
         <v>92</v>
       </c>
-      <c r="G12" s="693"/>
+      <c r="G12" s="725"/>
       <c r="H12" s="128"/>
       <c r="I12" s="19" t="s">
         <v>81</v>
@@ -13402,8 +13406,8 @@
       <c r="J12" s="3">
         <v>15</v>
       </c>
-      <c r="K12" s="711"/>
-      <c r="L12" s="726" t="s">
+      <c r="K12" s="704"/>
+      <c r="L12" s="719" t="s">
         <v>93</v>
       </c>
       <c r="M12" s="21" t="s">
@@ -13434,25 +13438,25 @@
         <v>116</v>
       </c>
       <c r="Y12" s="6"/>
-      <c r="AA12" s="715" t="s">
+      <c r="AA12" s="708" t="s">
         <v>126</v>
       </c>
-      <c r="AB12" s="716"/>
+      <c r="AB12" s="709"/>
       <c r="AC12" s="21" t="s">
         <v>233</v>
       </c>
-      <c r="AD12" s="705"/>
+      <c r="AD12" s="698"/>
     </row>
     <row r="13" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C13" s="729"/>
-      <c r="G13" s="693"/>
-      <c r="K13" s="711"/>
-      <c r="L13" s="727"/>
+      <c r="C13" s="690"/>
+      <c r="G13" s="725"/>
+      <c r="K13" s="704"/>
+      <c r="L13" s="720"/>
       <c r="M13" s="47"/>
-      <c r="Q13" s="695" t="s">
+      <c r="Q13" s="727" t="s">
         <v>210</v>
       </c>
-      <c r="R13" s="621"/>
+      <c r="R13" s="624"/>
       <c r="S13" s="554"/>
       <c r="T13" s="6"/>
       <c r="U13" s="96" t="s">
@@ -13461,17 +13465,17 @@
       <c r="X13" s="2" t="s">
         <v>123</v>
       </c>
-      <c r="AA13" s="717"/>
-      <c r="AB13" s="718"/>
-      <c r="AD13" s="705"/>
+      <c r="AA13" s="710"/>
+      <c r="AB13" s="711"/>
+      <c r="AD13" s="698"/>
     </row>
     <row r="14" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B14" s="2" t="s">
         <v>339</v>
       </c>
-      <c r="C14" s="731"/>
+      <c r="C14" s="692"/>
       <c r="D14" s="23"/>
-      <c r="G14" s="693"/>
+      <c r="G14" s="725"/>
       <c r="H14" s="125"/>
       <c r="I14" s="99" t="s">
         <v>44</v>
@@ -13479,8 +13483,8 @@
       <c r="J14" s="111">
         <v>115</v>
       </c>
-      <c r="K14" s="711"/>
-      <c r="L14" s="727"/>
+      <c r="K14" s="704"/>
+      <c r="L14" s="720"/>
       <c r="M14" s="21" t="s">
         <v>111</v>
       </c>
@@ -13501,9 +13505,9 @@
       <c r="Y14" s="21" t="s">
         <v>73</v>
       </c>
-      <c r="AA14" s="717"/>
-      <c r="AB14" s="718"/>
-      <c r="AD14" s="705"/>
+      <c r="AA14" s="710"/>
+      <c r="AB14" s="711"/>
+      <c r="AD14" s="698"/>
     </row>
     <row r="15" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C15" s="130" t="s">
@@ -13518,19 +13522,19 @@
       <c r="F15" s="66" t="s">
         <v>94</v>
       </c>
-      <c r="G15" s="693"/>
+      <c r="G15" s="725"/>
       <c r="H15" s="2" t="s">
         <v>81</v>
       </c>
       <c r="I15" s="53" t="s">
         <v>81</v>
       </c>
-      <c r="K15" s="711"/>
-      <c r="L15" s="728"/>
-      <c r="Q15" s="695" t="s">
+      <c r="K15" s="704"/>
+      <c r="L15" s="721"/>
+      <c r="Q15" s="727" t="s">
         <v>211</v>
       </c>
-      <c r="R15" s="621"/>
+      <c r="R15" s="624"/>
       <c r="S15" s="554"/>
       <c r="T15" s="6"/>
       <c r="V15" s="68" t="s">
@@ -13539,14 +13543,14 @@
       <c r="X15" s="2" t="s">
         <v>128</v>
       </c>
-      <c r="AA15" s="717"/>
-      <c r="AB15" s="718"/>
-      <c r="AD15" s="705"/>
+      <c r="AA15" s="710"/>
+      <c r="AB15" s="711"/>
+      <c r="AD15" s="698"/>
     </row>
     <row r="16" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C16" s="132"/>
-      <c r="G16" s="693"/>
-      <c r="K16" s="711"/>
+      <c r="G16" s="725"/>
+      <c r="K16" s="704"/>
       <c r="N16" s="47"/>
       <c r="O16" s="61" t="s">
         <v>109</v>
@@ -13565,24 +13569,24 @@
       <c r="Z16" s="76" t="s">
         <v>127</v>
       </c>
-      <c r="AA16" s="717"/>
-      <c r="AB16" s="718"/>
-      <c r="AD16" s="705"/>
+      <c r="AA16" s="710"/>
+      <c r="AB16" s="711"/>
+      <c r="AD16" s="698"/>
     </row>
     <row r="17" spans="3:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C17" s="109"/>
       <c r="E17" s="6" t="s">
         <v>95</v>
       </c>
-      <c r="F17" s="690" t="s">
+      <c r="F17" s="722" t="s">
         <v>96</v>
       </c>
-      <c r="G17" s="693"/>
+      <c r="G17" s="725"/>
       <c r="H17" s="54"/>
       <c r="I17" s="133" t="s">
         <v>81</v>
       </c>
-      <c r="K17" s="711"/>
+      <c r="K17" s="704"/>
       <c r="S17" s="554"/>
       <c r="V17" s="68" t="s">
         <v>44</v>
@@ -13590,9 +13594,9 @@
       <c r="X17" s="2" t="s">
         <v>118</v>
       </c>
-      <c r="AA17" s="717"/>
-      <c r="AB17" s="718"/>
-      <c r="AD17" s="705"/>
+      <c r="AA17" s="710"/>
+      <c r="AB17" s="711"/>
+      <c r="AD17" s="698"/>
     </row>
     <row r="18" spans="3:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C18" s="130"/>
@@ -13602,15 +13606,15 @@
       <c r="E18" s="6" t="s">
         <v>97</v>
       </c>
-      <c r="F18" s="691"/>
-      <c r="G18" s="693"/>
+      <c r="F18" s="723"/>
+      <c r="G18" s="725"/>
       <c r="H18" s="108" t="s">
         <v>76</v>
       </c>
       <c r="I18" s="21" t="s">
         <v>81</v>
       </c>
-      <c r="K18" s="711"/>
+      <c r="K18" s="704"/>
       <c r="O18" s="64" t="s">
         <v>115</v>
       </c>
@@ -13621,39 +13625,42 @@
       <c r="X18" s="2" t="s">
         <v>117</v>
       </c>
-      <c r="AA18" s="719"/>
-      <c r="AB18" s="720"/>
-      <c r="AD18" s="705"/>
+      <c r="AA18" s="712"/>
+      <c r="AB18" s="713"/>
+      <c r="AD18" s="698"/>
     </row>
     <row r="19" spans="3:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="F19" s="64" t="s">
         <v>209</v>
       </c>
-      <c r="G19" s="694"/>
-      <c r="K19" s="712"/>
+      <c r="G19" s="726"/>
+      <c r="K19" s="705"/>
       <c r="Q19" s="68" t="s">
         <v>44</v>
       </c>
-      <c r="R19" s="699" t="s">
+      <c r="R19" s="731" t="s">
         <v>124</v>
       </c>
-      <c r="S19" s="700"/>
-      <c r="T19" s="701"/>
+      <c r="S19" s="732"/>
+      <c r="T19" s="733"/>
       <c r="V19" s="77" t="s">
         <v>115</v>
       </c>
       <c r="Y19" s="19" t="s">
         <v>125</v>
       </c>
-      <c r="AD19" s="706"/>
+      <c r="AD19" s="699"/>
     </row>
   </sheetData>
   <mergeCells count="24">
-    <mergeCell ref="C9:C11"/>
-    <mergeCell ref="C13:C14"/>
-    <mergeCell ref="V2:W2"/>
-    <mergeCell ref="M10:AC10"/>
-    <mergeCell ref="F2:F3"/>
+    <mergeCell ref="F17:F18"/>
+    <mergeCell ref="G2:G19"/>
+    <mergeCell ref="Q13:R13"/>
+    <mergeCell ref="Q15:R15"/>
+    <mergeCell ref="L9:N9"/>
+    <mergeCell ref="R19:T19"/>
+    <mergeCell ref="S12:S18"/>
+    <mergeCell ref="O3:O9"/>
     <mergeCell ref="AD1:AD19"/>
     <mergeCell ref="S8:AC8"/>
     <mergeCell ref="K5:K19"/>
@@ -13665,14 +13672,11 @@
     <mergeCell ref="P3:Q3"/>
     <mergeCell ref="L4:L8"/>
     <mergeCell ref="L12:L15"/>
-    <mergeCell ref="F17:F18"/>
-    <mergeCell ref="G2:G19"/>
-    <mergeCell ref="Q13:R13"/>
-    <mergeCell ref="Q15:R15"/>
-    <mergeCell ref="L9:N9"/>
-    <mergeCell ref="R19:T19"/>
-    <mergeCell ref="S12:S18"/>
-    <mergeCell ref="O3:O9"/>
+    <mergeCell ref="C9:C11"/>
+    <mergeCell ref="C13:C14"/>
+    <mergeCell ref="V2:W2"/>
+    <mergeCell ref="M10:AC10"/>
+    <mergeCell ref="F2:F3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Boat Reconfigured - TBS
Shield CoHost - NTv Japan ReMapped
</commit_message>
<xml_diff>
--- a/System_2.1.5.xlsx
+++ b/System_2.1.5.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Work\Work_For_\Work\Running AppS\System_Work_RW\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD8481AC-BED1-40A1-A587-F93B75F11985}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0EBD1751-D9A9-4DE6-8DAF-9F1C6D5B8AE1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1080" uniqueCount="610">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1080" uniqueCount="611">
   <si>
     <t>Zone</t>
   </si>
@@ -1869,6 +1869,9 @@
   </si>
   <si>
     <t>Shield CoHost</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Boat Node </t>
   </si>
 </sst>
 </file>
@@ -2512,7 +2515,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="75">
+  <borders count="76">
     <border>
       <left/>
       <right/>
@@ -3438,11 +3441,24 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="735">
+  <cellXfs count="739">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
@@ -4733,7 +4749,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="61" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="53" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="53" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -4741,6 +4756,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -4791,6 +4809,36 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="255" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="39" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="39" fillId="6" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="18" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="18" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="18" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255"/>
+    </xf>
     <xf numFmtId="0" fontId="32" fillId="27" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -4848,34 +4896,139 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="39" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="39" fillId="6" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="18" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="19" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="19" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="3" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="19" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="19" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="38" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="38" fillId="7" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="255"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="18" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="255"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="18" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="33" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="33" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="33" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="52" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="54" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="16" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="16" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="3" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="18" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="18" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="18" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="49" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="49" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="49" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="255"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
@@ -4950,140 +5103,62 @@
     <xf numFmtId="0" fontId="3" fillId="11" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="3" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="18" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="18" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="18" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="49" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="49" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="49" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="52" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="54" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="16" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="16" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="19" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="19" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="3" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="19" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="19" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="38" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="38" fillId="7" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="33" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="33" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="33" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="3" fillId="43" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="43" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="43" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="18" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="18" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="18" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="40" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="40" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="40" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="7" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="32" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="32" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="52" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="52" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="35" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="255" wrapText="1"/>
@@ -5094,63 +5169,6 @@
     <xf numFmtId="0" fontId="3" fillId="35" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="255" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="43" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="43" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="43" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="18" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="18" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="18" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="40" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="40" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="40" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="7" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="32" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="32" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="52" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="52" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -5169,46 +5187,25 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="30" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="30" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="30" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="24" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="24" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="24" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="18" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -5286,28 +5283,61 @@
     <xf numFmtId="0" fontId="3" fillId="21" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="30" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="30" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="30" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="24" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="24" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="24" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="53" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="53" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="75" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="53" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="53" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -6555,8 +6585,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AB54FD83-008D-4F8B-87AC-83E7F70047CB}">
   <dimension ref="A1:AA32"/>
   <sheetViews>
-    <sheetView topLeftCell="H1" workbookViewId="0">
-      <selection activeCell="Y16" sqref="Y16"/>
+    <sheetView topLeftCell="H13" workbookViewId="0">
+      <selection activeCell="Z19" sqref="Z19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6613,7 +6643,7 @@
       <c r="P1" s="422" t="s">
         <v>407</v>
       </c>
-      <c r="Q1" s="581" t="s">
+      <c r="Q1" s="562" t="s">
         <v>181</v>
       </c>
       <c r="R1" s="100" t="s">
@@ -6633,32 +6663,32 @@
       </c>
     </row>
     <row r="2" spans="1:27" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="565">
+      <c r="A2" s="575">
         <f ca="1">TODAY()</f>
         <v>45279</v>
       </c>
-      <c r="B2" s="567" t="s">
+      <c r="B2" s="577" t="s">
         <v>388</v>
       </c>
-      <c r="C2" s="579" t="s">
+      <c r="C2" s="589" t="s">
         <v>364</v>
       </c>
-      <c r="D2" s="569" t="s">
+      <c r="D2" s="579" t="s">
         <v>103</v>
       </c>
-      <c r="E2" s="571" t="s">
+      <c r="E2" s="581" t="s">
         <v>65</v>
       </c>
       <c r="F2" s="196" t="s">
         <v>220</v>
       </c>
-      <c r="G2" s="577" t="s">
+      <c r="G2" s="587" t="s">
         <v>380</v>
       </c>
       <c r="H2" s="211" t="s">
         <v>220</v>
       </c>
-      <c r="I2" s="588" t="s">
+      <c r="I2" s="569" t="s">
         <v>103</v>
       </c>
       <c r="J2" s="420" t="s">
@@ -6682,7 +6712,7 @@
       <c r="P2" s="423">
         <v>40</v>
       </c>
-      <c r="Q2" s="582"/>
+      <c r="Q2" s="563"/>
       <c r="R2" s="21">
         <f>R7+R18</f>
         <v>6</v>
@@ -6708,14 +6738,14 @@
       </c>
     </row>
     <row r="3" spans="1:27" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="566"/>
-      <c r="B3" s="568"/>
-      <c r="C3" s="580"/>
-      <c r="D3" s="570"/>
-      <c r="E3" s="572"/>
-      <c r="G3" s="578"/>
+      <c r="A3" s="576"/>
+      <c r="B3" s="578"/>
+      <c r="C3" s="590"/>
+      <c r="D3" s="580"/>
+      <c r="E3" s="582"/>
+      <c r="G3" s="588"/>
       <c r="H3" s="6"/>
-      <c r="I3" s="589"/>
+      <c r="I3" s="570"/>
       <c r="K3" s="24">
         <v>2</v>
       </c>
@@ -6740,10 +6770,10 @@
         <v>389</v>
       </c>
       <c r="B4" s="248"/>
-      <c r="C4" s="573" t="s">
+      <c r="C4" s="583" t="s">
         <v>178</v>
       </c>
-      <c r="I4" s="589"/>
+      <c r="I4" s="570"/>
       <c r="R4" s="498" t="s">
         <v>579</v>
       </c>
@@ -6767,7 +6797,7 @@
       <c r="B5" s="100" t="s">
         <v>364</v>
       </c>
-      <c r="C5" s="574"/>
+      <c r="C5" s="584"/>
       <c r="D5" s="227" t="s">
         <v>103</v>
       </c>
@@ -6783,7 +6813,7 @@
       <c r="H5" s="211" t="s">
         <v>220</v>
       </c>
-      <c r="I5" s="589"/>
+      <c r="I5" s="570"/>
       <c r="J5" s="421" t="s">
         <v>273</v>
       </c>
@@ -6814,22 +6844,22 @@
       <c r="X5" s="494"/>
     </row>
     <row r="6" spans="1:27" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="562" t="s">
+      <c r="A6" s="572" t="s">
         <v>290</v>
       </c>
       <c r="B6" s="105" t="s">
         <v>199</v>
       </c>
-      <c r="C6" s="575"/>
-      <c r="D6" s="576"/>
+      <c r="C6" s="585"/>
+      <c r="D6" s="586"/>
       <c r="E6" s="96">
         <v>1</v>
       </c>
       <c r="G6" s="552"/>
-      <c r="I6" s="589"/>
+      <c r="I6" s="570"/>
     </row>
     <row r="7" spans="1:27" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="563"/>
+      <c r="A7" s="573"/>
       <c r="B7" s="100" t="s">
         <v>155</v>
       </c>
@@ -6840,7 +6870,7 @@
         <v>136</v>
       </c>
       <c r="G7" s="552"/>
-      <c r="I7" s="589"/>
+      <c r="I7" s="570"/>
       <c r="M7" s="16" t="s">
         <v>354</v>
       </c>
@@ -6876,7 +6906,7 @@
       </c>
     </row>
     <row r="8" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="564"/>
+      <c r="A8" s="574"/>
       <c r="B8" s="217" t="s">
         <v>28</v>
       </c>
@@ -6885,7 +6915,7 @@
         <v>3</v>
       </c>
       <c r="G8" s="552"/>
-      <c r="I8" s="589"/>
+      <c r="I8" s="570"/>
       <c r="N8" s="80"/>
       <c r="U8" s="6" t="s">
         <v>465</v>
@@ -6909,7 +6939,7 @@
       </c>
       <c r="G9" s="552"/>
       <c r="H9" s="6"/>
-      <c r="I9" s="589"/>
+      <c r="I9" s="570"/>
       <c r="M9" s="19" t="s">
         <v>546</v>
       </c>
@@ -6936,7 +6966,7 @@
         <v>41</v>
       </c>
       <c r="G10" s="552"/>
-      <c r="I10" s="589"/>
+      <c r="I10" s="570"/>
       <c r="J10" s="24" t="s">
         <v>380</v>
       </c>
@@ -6970,7 +7000,7 @@
         <v>270</v>
       </c>
       <c r="G11" s="552"/>
-      <c r="I11" s="589"/>
+      <c r="I11" s="570"/>
       <c r="J11" s="24" t="s">
         <v>195</v>
       </c>
@@ -6996,12 +7026,12 @@
       <c r="S11" s="24">
         <v>1</v>
       </c>
-      <c r="U11" s="583" t="s">
+      <c r="U11" s="564" t="s">
         <v>582</v>
       </c>
-      <c r="V11" s="584"/>
-      <c r="W11" s="584"/>
-      <c r="X11" s="585"/>
+      <c r="V11" s="565"/>
+      <c r="W11" s="565"/>
+      <c r="X11" s="566"/>
     </row>
     <row r="12" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="232" t="s">
@@ -7012,7 +7042,7 @@
         <v>3</v>
       </c>
       <c r="G12" s="552"/>
-      <c r="I12" s="589"/>
+      <c r="I12" s="570"/>
       <c r="J12" s="24" t="s">
         <v>537</v>
       </c>
@@ -7045,7 +7075,7 @@
       </c>
       <c r="D13" s="20"/>
       <c r="G13" s="552"/>
-      <c r="I13" s="589"/>
+      <c r="I13" s="570"/>
       <c r="J13" s="108" t="s">
         <v>571</v>
       </c>
@@ -7086,7 +7116,7 @@
       <c r="H14" s="211" t="s">
         <v>220</v>
       </c>
-      <c r="I14" s="589"/>
+      <c r="I14" s="570"/>
       <c r="U14" s="6"/>
       <c r="V14" s="112"/>
       <c r="W14" s="6"/>
@@ -7104,7 +7134,7 @@
       <c r="H15" s="277">
         <v>0</v>
       </c>
-      <c r="I15" s="589"/>
+      <c r="I15" s="570"/>
       <c r="J15" s="108" t="s">
         <v>154</v>
       </c>
@@ -7135,7 +7165,7 @@
       <c r="D16" s="2" t="s">
         <v>509</v>
       </c>
-      <c r="I16" s="589"/>
+      <c r="I16" s="570"/>
       <c r="K16" s="100" t="s">
         <v>44</v>
       </c>
@@ -7169,7 +7199,7 @@
       <c r="G17" s="2" t="s">
         <v>440</v>
       </c>
-      <c r="I17" s="589"/>
+      <c r="I17" s="570"/>
       <c r="L17" s="2" t="s">
         <v>443</v>
       </c>
@@ -7181,13 +7211,13 @@
     </row>
     <row r="18" spans="1:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="G18" s="16"/>
-      <c r="I18" s="589"/>
+      <c r="I18" s="570"/>
       <c r="L18" s="16"/>
       <c r="M18" s="21"/>
-      <c r="O18" s="586" t="s">
+      <c r="O18" s="567" t="s">
         <v>538</v>
       </c>
-      <c r="P18" s="587"/>
+      <c r="P18" s="568"/>
       <c r="Q18" s="127" t="s">
         <v>44</v>
       </c>
@@ -7213,7 +7243,7 @@
       </c>
     </row>
     <row r="19" spans="1:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="I19" s="589"/>
+      <c r="I19" s="570"/>
       <c r="M19" s="21" t="s">
         <v>442</v>
       </c>
@@ -7245,7 +7275,7 @@
       <c r="G20" s="2" t="s">
         <v>440</v>
       </c>
-      <c r="I20" s="589"/>
+      <c r="I20" s="570"/>
       <c r="K20" s="19" t="s">
         <v>439</v>
       </c>
@@ -7270,7 +7300,7 @@
       <c r="Z20" s="112"/>
     </row>
     <row r="21" spans="1:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="I21" s="589"/>
+      <c r="I21" s="570"/>
       <c r="M21" s="221" t="s">
         <v>421</v>
       </c>
@@ -7306,7 +7336,7 @@
       <c r="G22" s="2" t="s">
         <v>440</v>
       </c>
-      <c r="I22" s="589"/>
+      <c r="I22" s="570"/>
       <c r="U22" s="6"/>
       <c r="V22" s="494"/>
       <c r="W22" s="6" t="s">
@@ -7326,13 +7356,13 @@
       <c r="E23" s="289" t="s">
         <v>44</v>
       </c>
-      <c r="I23" s="589"/>
+      <c r="I23" s="570"/>
       <c r="U23" s="6"/>
       <c r="V23" s="24"/>
       <c r="W23" s="6"/>
     </row>
     <row r="24" spans="1:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="I24" s="589"/>
+      <c r="I24" s="570"/>
       <c r="U24" s="354"/>
       <c r="V24" s="497">
         <v>0</v>
@@ -7360,7 +7390,7 @@
       <c r="H25" s="196" t="s">
         <v>271</v>
       </c>
-      <c r="I25" s="589"/>
+      <c r="I25" s="570"/>
       <c r="J25" s="421" t="s">
         <v>274</v>
       </c>
@@ -7405,7 +7435,7 @@
       <c r="H26" s="19" t="s">
         <v>220</v>
       </c>
-      <c r="I26" s="589"/>
+      <c r="I26" s="570"/>
       <c r="K26" s="24">
         <v>15</v>
       </c>
@@ -7440,7 +7470,7 @@
       </c>
     </row>
     <row r="27" spans="1:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="I27" s="589"/>
+      <c r="I27" s="570"/>
       <c r="O27" s="2" t="s">
         <v>99</v>
       </c>
@@ -7467,7 +7497,7 @@
       <c r="E28" s="220">
         <v>2</v>
       </c>
-      <c r="I28" s="589"/>
+      <c r="I28" s="570"/>
       <c r="Q28" s="6"/>
       <c r="R28" s="112"/>
       <c r="T28" s="142"/>
@@ -7489,7 +7519,7 @@
       <c r="H29" s="196" t="s">
         <v>272</v>
       </c>
-      <c r="I29" s="590"/>
+      <c r="I29" s="571"/>
       <c r="J29" s="333"/>
       <c r="L29" s="96" t="s">
         <v>278</v>
@@ -7559,11 +7589,6 @@
     </row>
   </sheetData>
   <mergeCells count="16">
-    <mergeCell ref="Q1:Q2"/>
-    <mergeCell ref="U11:X11"/>
-    <mergeCell ref="O18:P18"/>
-    <mergeCell ref="I2:I29"/>
-    <mergeCell ref="C13:C14"/>
     <mergeCell ref="A6:A8"/>
     <mergeCell ref="G5:G14"/>
     <mergeCell ref="A2:A3"/>
@@ -7575,6 +7600,11 @@
     <mergeCell ref="B11:B12"/>
     <mergeCell ref="G2:G3"/>
     <mergeCell ref="C2:C3"/>
+    <mergeCell ref="Q1:Q2"/>
+    <mergeCell ref="U11:X11"/>
+    <mergeCell ref="O18:P18"/>
+    <mergeCell ref="I2:I29"/>
+    <mergeCell ref="C13:C14"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -7650,7 +7680,7 @@
       <c r="H1" s="97" t="s">
         <v>350</v>
       </c>
-      <c r="I1" s="577" t="s">
+      <c r="I1" s="587" t="s">
         <v>377</v>
       </c>
       <c r="J1" s="2" t="s">
@@ -7711,7 +7741,7 @@
         <v>516</v>
       </c>
       <c r="AM1" s="426"/>
-      <c r="AN1" s="615"/>
+      <c r="AN1" s="618"/>
       <c r="AO1" s="350" t="s">
         <v>486</v>
       </c>
@@ -7720,23 +7750,23 @@
       </c>
     </row>
     <row r="2" spans="1:43" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="597">
+      <c r="A2" s="642">
         <f ca="1">TODAY()</f>
         <v>45279</v>
       </c>
-      <c r="B2" s="599" t="s">
+      <c r="B2" s="644" t="s">
         <v>378</v>
       </c>
-      <c r="C2" s="579" t="s">
+      <c r="C2" s="589" t="s">
         <v>364</v>
       </c>
-      <c r="D2" s="601" t="s">
+      <c r="D2" s="646" t="s">
         <v>362</v>
       </c>
-      <c r="E2" s="645" t="s">
+      <c r="E2" s="591" t="s">
         <v>65</v>
       </c>
-      <c r="F2" s="620" t="s">
+      <c r="F2" s="599" t="s">
         <v>103</v>
       </c>
       <c r="G2" s="417" t="s">
@@ -7745,31 +7775,31 @@
       <c r="H2" s="80" t="s">
         <v>33</v>
       </c>
-      <c r="I2" s="578"/>
+      <c r="I2" s="588"/>
       <c r="J2" s="81" t="s">
         <v>77</v>
       </c>
-      <c r="K2" s="647" t="s">
+      <c r="K2" s="593" t="s">
         <v>349</v>
       </c>
-      <c r="L2" s="648"/>
-      <c r="M2" s="620" t="s">
+      <c r="L2" s="594"/>
+      <c r="M2" s="599" t="s">
         <v>103</v>
       </c>
       <c r="N2" s="69" t="s">
         <v>28</v>
       </c>
-      <c r="O2" s="624" t="s">
+      <c r="O2" s="625" t="s">
         <v>103</v>
       </c>
       <c r="P2" s="85" t="s">
         <v>148</v>
       </c>
-      <c r="Q2" s="579" t="s">
+      <c r="Q2" s="589" t="s">
         <v>144</v>
       </c>
       <c r="R2" s="551"/>
-      <c r="S2" s="637" t="s">
+      <c r="S2" s="612" t="s">
         <v>149</v>
       </c>
       <c r="T2" s="89"/>
@@ -7802,15 +7832,15 @@
         <v>480</v>
       </c>
       <c r="AM2" s="452"/>
-      <c r="AN2" s="616"/>
+      <c r="AN2" s="619"/>
     </row>
     <row r="3" spans="1:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="598"/>
-      <c r="B3" s="600"/>
-      <c r="C3" s="580"/>
-      <c r="D3" s="602"/>
-      <c r="E3" s="646"/>
-      <c r="F3" s="621"/>
+      <c r="A3" s="643"/>
+      <c r="B3" s="645"/>
+      <c r="C3" s="590"/>
+      <c r="D3" s="647"/>
+      <c r="E3" s="592"/>
+      <c r="F3" s="600"/>
       <c r="G3" s="418" t="s">
         <v>28</v>
       </c>
@@ -7829,17 +7859,17 @@
       <c r="L3" s="206" t="s">
         <v>108</v>
       </c>
-      <c r="M3" s="621"/>
+      <c r="M3" s="600"/>
       <c r="N3" s="69" t="s">
         <v>147</v>
       </c>
-      <c r="O3" s="625"/>
+      <c r="O3" s="626"/>
       <c r="P3" s="2" t="s">
         <v>155</v>
       </c>
-      <c r="Q3" s="580"/>
+      <c r="Q3" s="590"/>
       <c r="R3" s="553"/>
-      <c r="S3" s="638"/>
+      <c r="S3" s="614"/>
       <c r="T3" s="89"/>
       <c r="U3" s="124"/>
       <c r="V3" s="120"/>
@@ -7856,7 +7886,7 @@
       <c r="AC3" s="100" t="s">
         <v>497</v>
       </c>
-      <c r="AD3" s="636" t="s">
+      <c r="AD3" s="609" t="s">
         <v>472</v>
       </c>
       <c r="AE3" s="262"/>
@@ -7868,16 +7898,16 @@
       <c r="AK3" s="262"/>
       <c r="AL3" s="16"/>
       <c r="AM3" s="452"/>
-      <c r="AN3" s="616"/>
+      <c r="AN3" s="619"/>
     </row>
     <row r="4" spans="1:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="243" t="s">
         <v>184</v>
       </c>
-      <c r="B4" s="613" t="s">
+      <c r="B4" s="658" t="s">
         <v>381</v>
       </c>
-      <c r="C4" s="579" t="s">
+      <c r="C4" s="589" t="s">
         <v>155</v>
       </c>
       <c r="D4" s="359" t="s">
@@ -7886,7 +7916,7 @@
       <c r="E4" s="396">
         <v>2</v>
       </c>
-      <c r="F4" s="621"/>
+      <c r="F4" s="600"/>
       <c r="G4" s="400" t="s">
         <v>203</v>
       </c>
@@ -7903,11 +7933,11 @@
         <v>151</v>
       </c>
       <c r="L4" s="209"/>
-      <c r="M4" s="621"/>
+      <c r="M4" s="600"/>
       <c r="N4" s="178" t="s">
         <v>70</v>
       </c>
-      <c r="O4" s="625"/>
+      <c r="O4" s="626"/>
       <c r="P4" s="2" t="s">
         <v>192</v>
       </c>
@@ -7934,7 +7964,7 @@
       <c r="AA4" s="313"/>
       <c r="AB4" s="214"/>
       <c r="AC4" s="16"/>
-      <c r="AD4" s="636"/>
+      <c r="AD4" s="609"/>
       <c r="AE4" s="262"/>
       <c r="AF4" s="262"/>
       <c r="AG4" s="16"/>
@@ -7944,37 +7974,37 @@
       <c r="AK4" s="262"/>
       <c r="AL4" s="16"/>
       <c r="AM4" s="452"/>
-      <c r="AN4" s="616"/>
+      <c r="AN4" s="619"/>
       <c r="AO4" s="350" t="s">
         <v>91</v>
       </c>
     </row>
     <row r="5" spans="1:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="577" t="s">
+      <c r="A5" s="587" t="s">
         <v>434</v>
       </c>
-      <c r="B5" s="614"/>
-      <c r="C5" s="580"/>
+      <c r="B5" s="659"/>
+      <c r="C5" s="590"/>
       <c r="D5" s="61" t="s">
         <v>154</v>
       </c>
       <c r="E5" s="397">
         <v>1</v>
       </c>
-      <c r="F5" s="621"/>
-      <c r="G5" s="605" t="s">
+      <c r="F5" s="600"/>
+      <c r="G5" s="650" t="s">
         <v>193</v>
       </c>
-      <c r="H5" s="605"/>
-      <c r="I5" s="605"/>
-      <c r="J5" s="605"/>
-      <c r="K5" s="605"/>
-      <c r="L5" s="606"/>
-      <c r="M5" s="621"/>
+      <c r="H5" s="650"/>
+      <c r="I5" s="650"/>
+      <c r="J5" s="650"/>
+      <c r="K5" s="650"/>
+      <c r="L5" s="651"/>
+      <c r="M5" s="600"/>
       <c r="N5" s="21">
         <v>8</v>
       </c>
-      <c r="O5" s="625"/>
+      <c r="O5" s="626"/>
       <c r="T5" s="89"/>
       <c r="U5" s="124"/>
       <c r="V5" s="120"/>
@@ -8005,24 +8035,24 @@
       <c r="AK5" s="262"/>
       <c r="AL5" s="80"/>
       <c r="AM5" s="452"/>
-      <c r="AN5" s="616"/>
+      <c r="AN5" s="619"/>
     </row>
     <row r="6" spans="1:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="578"/>
-      <c r="B6" s="611" t="s">
+      <c r="A6" s="588"/>
+      <c r="B6" s="656" t="s">
         <v>178</v>
       </c>
-      <c r="C6" s="575"/>
-      <c r="D6" s="576"/>
-      <c r="F6" s="621"/>
-      <c r="G6" s="607"/>
-      <c r="H6" s="607"/>
-      <c r="I6" s="607"/>
-      <c r="J6" s="607"/>
-      <c r="K6" s="607"/>
-      <c r="L6" s="608"/>
-      <c r="M6" s="621"/>
-      <c r="O6" s="625"/>
+      <c r="C6" s="585"/>
+      <c r="D6" s="586"/>
+      <c r="F6" s="600"/>
+      <c r="G6" s="652"/>
+      <c r="H6" s="652"/>
+      <c r="I6" s="652"/>
+      <c r="J6" s="652"/>
+      <c r="K6" s="652"/>
+      <c r="L6" s="653"/>
+      <c r="M6" s="600"/>
+      <c r="O6" s="626"/>
       <c r="T6" s="89"/>
       <c r="U6" s="124"/>
       <c r="V6" s="98" t="s">
@@ -8046,16 +8076,16 @@
       <c r="AF6" s="262"/>
       <c r="AG6" s="262"/>
       <c r="AH6" s="262"/>
-      <c r="AI6" s="630"/>
+      <c r="AI6" s="608"/>
       <c r="AJ6" s="465" t="s">
         <v>475</v>
       </c>
-      <c r="AK6" s="630" t="s">
+      <c r="AK6" s="608" t="s">
         <v>256</v>
       </c>
       <c r="AL6" s="262"/>
       <c r="AM6" s="452"/>
-      <c r="AN6" s="616"/>
+      <c r="AN6" s="619"/>
       <c r="AO6" s="350" t="s">
         <v>487</v>
       </c>
@@ -8064,7 +8094,7 @@
       <c r="A7" s="237" t="s">
         <v>597</v>
       </c>
-      <c r="B7" s="612"/>
+      <c r="B7" s="657"/>
       <c r="C7" s="207" t="s">
         <v>382</v>
       </c>
@@ -8074,7 +8104,7 @@
       <c r="E7" s="271">
         <v>3</v>
       </c>
-      <c r="F7" s="621"/>
+      <c r="F7" s="600"/>
       <c r="G7" s="419">
         <v>0</v>
       </c>
@@ -8093,8 +8123,8 @@
       <c r="L7" s="217">
         <v>0</v>
       </c>
-      <c r="M7" s="621"/>
-      <c r="O7" s="625"/>
+      <c r="M7" s="600"/>
+      <c r="O7" s="626"/>
       <c r="R7" s="99" t="s">
         <v>44</v>
       </c>
@@ -8118,18 +8148,18 @@
       <c r="AD7" s="16"/>
       <c r="AE7" s="262"/>
       <c r="AF7" s="262"/>
-      <c r="AG7" s="636" t="s">
+      <c r="AG7" s="609" t="s">
         <v>471</v>
       </c>
       <c r="AH7" s="262"/>
-      <c r="AI7" s="630"/>
+      <c r="AI7" s="608"/>
       <c r="AJ7" s="262"/>
-      <c r="AK7" s="630"/>
+      <c r="AK7" s="608"/>
       <c r="AL7" s="80" t="s">
         <v>514</v>
       </c>
       <c r="AM7" s="452"/>
-      <c r="AN7" s="616"/>
+      <c r="AN7" s="619"/>
       <c r="AP7" s="76" t="s">
         <v>488</v>
       </c>
@@ -8146,27 +8176,27 @@
         <f>SUM(G7:N9)</f>
         <v>15</v>
       </c>
-      <c r="F8" s="621"/>
-      <c r="G8" s="606">
-        <v>0</v>
-      </c>
-      <c r="H8" s="603" t="s">
+      <c r="F8" s="600"/>
+      <c r="G8" s="651">
+        <v>0</v>
+      </c>
+      <c r="H8" s="648" t="s">
         <v>105</v>
       </c>
       <c r="I8" s="551">
         <v>0</v>
       </c>
-      <c r="J8" s="603" t="s">
+      <c r="J8" s="648" t="s">
         <v>105</v>
       </c>
-      <c r="K8" s="609"/>
-      <c r="L8" s="639"/>
-      <c r="M8" s="622"/>
-      <c r="N8" s="642">
+      <c r="K8" s="654"/>
+      <c r="L8" s="610"/>
+      <c r="M8" s="623"/>
+      <c r="N8" s="615">
         <f>N5+N11</f>
         <v>15</v>
       </c>
-      <c r="O8" s="625"/>
+      <c r="O8" s="626"/>
       <c r="T8" s="103" t="s">
         <v>44</v>
       </c>
@@ -8184,14 +8214,14 @@
       <c r="AD8" s="16"/>
       <c r="AE8" s="262"/>
       <c r="AF8" s="262"/>
-      <c r="AG8" s="636"/>
+      <c r="AG8" s="609"/>
       <c r="AH8" s="262"/>
-      <c r="AI8" s="630"/>
+      <c r="AI8" s="608"/>
       <c r="AJ8" s="262"/>
       <c r="AK8" s="262"/>
       <c r="AL8" s="262"/>
       <c r="AM8" s="452"/>
-      <c r="AN8" s="616"/>
+      <c r="AN8" s="619"/>
     </row>
     <row r="9" spans="1:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="237" t="s">
@@ -8206,17 +8236,17 @@
       <c r="D9" s="360" t="s">
         <v>286</v>
       </c>
-      <c r="F9" s="621"/>
-      <c r="G9" s="608"/>
-      <c r="H9" s="604"/>
+      <c r="F9" s="600"/>
+      <c r="G9" s="653"/>
+      <c r="H9" s="649"/>
       <c r="I9" s="553"/>
-      <c r="J9" s="604"/>
-      <c r="K9" s="610"/>
-      <c r="L9" s="640"/>
-      <c r="M9" s="623"/>
-      <c r="N9" s="643"/>
-      <c r="O9" s="626"/>
-      <c r="S9" s="637" t="s">
+      <c r="J9" s="649"/>
+      <c r="K9" s="655"/>
+      <c r="L9" s="611"/>
+      <c r="M9" s="624"/>
+      <c r="N9" s="616"/>
+      <c r="O9" s="627"/>
+      <c r="S9" s="612" t="s">
         <v>62</v>
       </c>
       <c r="T9" s="89"/>
@@ -8238,16 +8268,16 @@
       </c>
       <c r="AE9" s="262"/>
       <c r="AF9" s="262"/>
-      <c r="AG9" s="636"/>
+      <c r="AG9" s="609"/>
       <c r="AH9" s="262"/>
-      <c r="AI9" s="630"/>
+      <c r="AI9" s="608"/>
       <c r="AJ9" s="80"/>
-      <c r="AK9" s="630" t="s">
+      <c r="AK9" s="608" t="s">
         <v>256</v>
       </c>
       <c r="AL9" s="262"/>
       <c r="AM9" s="452"/>
-      <c r="AN9" s="616"/>
+      <c r="AN9" s="619"/>
       <c r="AP9" s="2" t="s">
         <v>526</v>
       </c>
@@ -8264,20 +8294,20 @@
         <f>Boat!U8</f>
         <v>41</v>
       </c>
-      <c r="F10" s="621"/>
+      <c r="F10" s="600"/>
       <c r="N10" s="442" t="s">
         <v>406</v>
       </c>
-      <c r="O10" s="654" t="s">
+      <c r="O10" s="602" t="s">
         <v>103</v>
       </c>
-      <c r="P10" s="627" t="s">
+      <c r="P10" s="628" t="s">
         <v>410</v>
       </c>
       <c r="R10" s="74" t="s">
         <v>44</v>
       </c>
-      <c r="S10" s="641"/>
+      <c r="S10" s="613"/>
       <c r="T10" s="89"/>
       <c r="U10" s="123" t="s">
         <v>177</v>
@@ -8307,16 +8337,16 @@
       <c r="AF10" s="243" t="s">
         <v>318</v>
       </c>
-      <c r="AG10" s="636"/>
+      <c r="AG10" s="609"/>
       <c r="AH10" s="80"/>
-      <c r="AI10" s="630"/>
+      <c r="AI10" s="608"/>
       <c r="AJ10" s="262"/>
-      <c r="AK10" s="630"/>
+      <c r="AK10" s="608"/>
       <c r="AL10" s="262"/>
       <c r="AM10" s="466" t="s">
         <v>325</v>
       </c>
-      <c r="AN10" s="616"/>
+      <c r="AN10" s="619"/>
       <c r="AO10" s="209" t="s">
         <v>95</v>
       </c>
@@ -8334,18 +8364,18 @@
       <c r="D11" s="174" t="s">
         <v>362</v>
       </c>
-      <c r="F11" s="621"/>
+      <c r="F11" s="600"/>
       <c r="M11" s="6"/>
       <c r="N11" s="117">
         <v>7</v>
       </c>
-      <c r="O11" s="655"/>
-      <c r="P11" s="628"/>
+      <c r="O11" s="603"/>
+      <c r="P11" s="629"/>
       <c r="Q11" s="65"/>
       <c r="R11" s="120" t="s">
         <v>222</v>
       </c>
-      <c r="S11" s="641"/>
+      <c r="S11" s="613"/>
       <c r="T11" s="102" t="s">
         <v>44</v>
       </c>
@@ -8369,14 +8399,14 @@
       <c r="AF11" s="262" t="s">
         <v>493</v>
       </c>
-      <c r="AG11" s="636"/>
+      <c r="AG11" s="609"/>
       <c r="AH11" s="262"/>
       <c r="AI11" s="70"/>
       <c r="AJ11" s="262"/>
       <c r="AK11" s="262"/>
       <c r="AL11" s="262"/>
       <c r="AM11" s="452"/>
-      <c r="AN11" s="616"/>
+      <c r="AN11" s="619"/>
       <c r="AP11" s="76" t="s">
         <v>501</v>
       </c>
@@ -8395,7 +8425,7 @@
       <c r="E12" s="229">
         <v>3</v>
       </c>
-      <c r="F12" s="621"/>
+      <c r="F12" s="600"/>
       <c r="G12" s="349" t="s">
         <v>410</v>
       </c>
@@ -8404,16 +8434,16 @@
       </c>
       <c r="I12" s="558"/>
       <c r="J12" s="558"/>
-      <c r="K12" s="659"/>
+      <c r="K12" s="607"/>
       <c r="L12" s="208"/>
       <c r="M12" s="208"/>
       <c r="N12" s="208"/>
-      <c r="O12" s="655"/>
-      <c r="P12" s="628"/>
+      <c r="O12" s="603"/>
+      <c r="P12" s="629"/>
       <c r="R12" s="122" t="s">
         <v>181</v>
       </c>
-      <c r="S12" s="638"/>
+      <c r="S12" s="614"/>
       <c r="T12" s="101" t="s">
         <v>44</v>
       </c>
@@ -8434,16 +8464,16 @@
       <c r="AC12" s="100" t="s">
         <v>498</v>
       </c>
-      <c r="AD12" s="644" t="s">
+      <c r="AD12" s="617" t="s">
         <v>245</v>
       </c>
       <c r="AE12" s="465" t="s">
         <v>244</v>
       </c>
-      <c r="AF12" s="636" t="s">
+      <c r="AF12" s="609" t="s">
         <v>231</v>
       </c>
-      <c r="AG12" s="636"/>
+      <c r="AG12" s="609"/>
       <c r="AH12" s="243" t="s">
         <v>264</v>
       </c>
@@ -8456,7 +8486,7 @@
       <c r="AM12" s="631" t="s">
         <v>254</v>
       </c>
-      <c r="AN12" s="616"/>
+      <c r="AN12" s="619"/>
       <c r="AO12" s="350" t="s">
         <v>97</v>
       </c>
@@ -8468,17 +8498,17 @@
       <c r="E13" s="472">
         <v>-3</v>
       </c>
-      <c r="F13" s="621"/>
+      <c r="F13" s="600"/>
       <c r="G13" s="558" t="s">
         <v>447</v>
       </c>
       <c r="H13" s="558"/>
       <c r="I13" s="558"/>
-      <c r="J13" s="659"/>
+      <c r="J13" s="607"/>
       <c r="M13" s="6"/>
       <c r="N13" s="6"/>
-      <c r="O13" s="655"/>
-      <c r="P13" s="629"/>
+      <c r="O13" s="603"/>
+      <c r="P13" s="630"/>
       <c r="T13" s="105" t="s">
         <v>44</v>
       </c>
@@ -8499,8 +8529,8 @@
         <v>518</v>
       </c>
       <c r="AC13" s="16"/>
-      <c r="AD13" s="644"/>
-      <c r="AF13" s="636"/>
+      <c r="AD13" s="617"/>
+      <c r="AF13" s="609"/>
       <c r="AG13" s="80"/>
       <c r="AH13" s="243" t="s">
         <v>314</v>
@@ -8512,7 +8542,7 @@
       <c r="AK13" s="262"/>
       <c r="AL13" s="262"/>
       <c r="AM13" s="631"/>
-      <c r="AN13" s="616"/>
+      <c r="AN13" s="619"/>
     </row>
     <row r="14" spans="1:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="474"/>
@@ -8520,18 +8550,18 @@
       <c r="C14" s="483"/>
       <c r="D14" s="476"/>
       <c r="E14" s="477"/>
-      <c r="F14" s="621"/>
+      <c r="F14" s="600"/>
       <c r="G14" s="558" t="s">
         <v>446</v>
       </c>
       <c r="H14" s="558"/>
       <c r="I14" s="558"/>
-      <c r="J14" s="659"/>
+      <c r="J14" s="607"/>
       <c r="K14" s="2">
         <v>12</v>
       </c>
       <c r="N14" s="6"/>
-      <c r="O14" s="655"/>
+      <c r="O14" s="603"/>
       <c r="Q14" s="61" t="s">
         <v>554</v>
       </c>
@@ -8552,9 +8582,9 @@
       <c r="AA14" s="313"/>
       <c r="AB14" s="214"/>
       <c r="AC14" s="16"/>
-      <c r="AD14" s="644"/>
+      <c r="AD14" s="617"/>
       <c r="AE14" s="262"/>
-      <c r="AF14" s="636"/>
+      <c r="AF14" s="609"/>
       <c r="AG14" s="262"/>
       <c r="AH14" s="262"/>
       <c r="AI14" s="70"/>
@@ -8562,7 +8592,7 @@
       <c r="AK14" s="262"/>
       <c r="AL14" s="262"/>
       <c r="AM14" s="631"/>
-      <c r="AN14" s="616"/>
+      <c r="AN14" s="619"/>
     </row>
     <row r="15" spans="1:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="473" t="s">
@@ -8571,8 +8601,8 @@
       <c r="C15" s="551" t="s">
         <v>381</v>
       </c>
-      <c r="F15" s="621"/>
-      <c r="O15" s="655"/>
+      <c r="F15" s="600"/>
+      <c r="O15" s="603"/>
       <c r="R15" s="99" t="s">
         <v>44</v>
       </c>
@@ -8594,8 +8624,8 @@
       <c r="AC15" s="76" t="s">
         <v>496</v>
       </c>
-      <c r="AD15" s="644"/>
-      <c r="AF15" s="636"/>
+      <c r="AD15" s="617"/>
+      <c r="AF15" s="609"/>
       <c r="AG15" s="80"/>
       <c r="AH15" s="243" t="s">
         <v>465</v>
@@ -8609,7 +8639,7 @@
       <c r="AK15" s="262"/>
       <c r="AL15" s="262"/>
       <c r="AM15" s="631"/>
-      <c r="AN15" s="616"/>
+      <c r="AN15" s="619"/>
       <c r="AP15" s="76" t="s">
         <v>74</v>
       </c>
@@ -8631,13 +8661,13 @@
       <c r="E16" s="229">
         <v>1</v>
       </c>
-      <c r="F16" s="621"/>
+      <c r="F16" s="600"/>
       <c r="G16" s="349" t="s">
         <v>505</v>
       </c>
       <c r="I16" s="495"/>
       <c r="J16" s="20"/>
-      <c r="O16" s="655"/>
+      <c r="O16" s="603"/>
       <c r="R16" s="459" t="s">
         <v>185</v>
       </c>
@@ -8669,18 +8699,18 @@
       <c r="AM16" s="452" t="s">
         <v>324</v>
       </c>
-      <c r="AN16" s="616"/>
+      <c r="AN16" s="619"/>
       <c r="AP16" s="76" t="s">
         <v>235</v>
       </c>
     </row>
     <row r="17" spans="1:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B17" s="80"/>
-      <c r="F17" s="621"/>
+      <c r="F17" s="600"/>
       <c r="I17" s="496"/>
       <c r="J17" s="20"/>
       <c r="N17" s="6"/>
-      <c r="O17" s="655"/>
+      <c r="O17" s="603"/>
       <c r="Q17" s="21" t="s">
         <v>552</v>
       </c>
@@ -8725,7 +8755,7 @@
       <c r="AK17" s="262"/>
       <c r="AL17" s="80"/>
       <c r="AM17" s="452"/>
-      <c r="AN17" s="616"/>
+      <c r="AN17" s="619"/>
       <c r="AO17" s="209" t="s">
         <v>515</v>
       </c>
@@ -8749,21 +8779,21 @@
       <c r="E18" s="99" t="s">
         <v>44</v>
       </c>
-      <c r="F18" s="621"/>
+      <c r="F18" s="600"/>
       <c r="G18" s="349" t="s">
         <v>549</v>
       </c>
       <c r="I18" s="24"/>
       <c r="J18" s="20"/>
-      <c r="O18" s="655"/>
+      <c r="O18" s="603"/>
       <c r="Q18" s="112"/>
-      <c r="R18" s="649" t="s">
+      <c r="R18" s="595" t="s">
         <v>557</v>
       </c>
       <c r="T18" s="100" t="s">
         <v>44</v>
       </c>
-      <c r="U18" s="594" t="s">
+      <c r="U18" s="639" t="s">
         <v>44</v>
       </c>
       <c r="V18" s="120"/>
@@ -8784,7 +8814,7 @@
       <c r="AC18" s="16"/>
       <c r="AD18" s="16"/>
       <c r="AE18" s="262"/>
-      <c r="AF18" s="630" t="s">
+      <c r="AF18" s="608" t="s">
         <v>492</v>
       </c>
       <c r="AG18" s="262"/>
@@ -8796,20 +8826,20 @@
       <c r="AK18" s="262"/>
       <c r="AL18" s="80"/>
       <c r="AM18" s="452"/>
-      <c r="AN18" s="616"/>
+      <c r="AN18" s="619"/>
       <c r="AP18" s="76" t="s">
         <v>88</v>
       </c>
     </row>
     <row r="19" spans="1:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="F19" s="621"/>
+      <c r="F19" s="600"/>
       <c r="I19" s="224"/>
-      <c r="O19" s="655"/>
-      <c r="R19" s="650"/>
+      <c r="O19" s="603"/>
+      <c r="R19" s="596"/>
       <c r="S19" s="30" t="s">
         <v>555</v>
       </c>
-      <c r="U19" s="595"/>
+      <c r="U19" s="640"/>
       <c r="V19" s="146"/>
       <c r="W19" s="146"/>
       <c r="X19" s="455" t="s">
@@ -8824,7 +8854,7 @@
       <c r="AC19" s="16"/>
       <c r="AD19" s="16"/>
       <c r="AE19" s="262"/>
-      <c r="AF19" s="630"/>
+      <c r="AF19" s="608"/>
       <c r="AG19" s="262"/>
       <c r="AH19" s="262"/>
       <c r="AI19" s="70"/>
@@ -8834,7 +8864,7 @@
       </c>
       <c r="AL19" s="80"/>
       <c r="AM19" s="452"/>
-      <c r="AN19" s="616"/>
+      <c r="AN19" s="619"/>
       <c r="AP19" s="76" t="s">
         <v>485</v>
       </c>
@@ -8855,19 +8885,19 @@
       <c r="E20" s="461">
         <v>-1</v>
       </c>
-      <c r="F20" s="621"/>
+      <c r="F20" s="600"/>
       <c r="G20" s="349" t="s">
         <v>508</v>
       </c>
       <c r="I20" s="224"/>
-      <c r="O20" s="655"/>
-      <c r="Q20" s="657" t="s">
+      <c r="O20" s="603"/>
+      <c r="Q20" s="605" t="s">
         <v>48</v>
       </c>
       <c r="T20" s="428" t="s">
         <v>44</v>
       </c>
-      <c r="U20" s="596"/>
+      <c r="U20" s="641"/>
       <c r="W20" s="429"/>
       <c r="X20" s="456" t="s">
         <v>175</v>
@@ -8897,7 +8927,7 @@
       <c r="AM20" s="400" t="s">
         <v>254</v>
       </c>
-      <c r="AN20" s="616"/>
+      <c r="AN20" s="619"/>
       <c r="AO20" s="350" t="s">
         <v>477</v>
       </c>
@@ -8918,13 +8948,13 @@
       <c r="E21" s="271">
         <v>0</v>
       </c>
-      <c r="F21" s="621"/>
+      <c r="F21" s="600"/>
       <c r="I21" s="224"/>
-      <c r="O21" s="655"/>
-      <c r="Q21" s="658"/>
+      <c r="O21" s="603"/>
+      <c r="Q21" s="606"/>
       <c r="T21" s="446"/>
       <c r="U21" s="14"/>
-      <c r="V21" s="591"/>
+      <c r="V21" s="636"/>
       <c r="W21" s="450" t="s">
         <v>176</v>
       </c>
@@ -8962,15 +8992,15 @@
       <c r="AM21" s="452" t="s">
         <v>566</v>
       </c>
-      <c r="AN21" s="616"/>
+      <c r="AN21" s="619"/>
     </row>
     <row r="22" spans="1:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="F22" s="621"/>
+      <c r="F22" s="600"/>
       <c r="G22" s="349" t="s">
         <v>506</v>
       </c>
       <c r="I22" s="224"/>
-      <c r="O22" s="655"/>
+      <c r="O22" s="603"/>
       <c r="R22" s="458" t="s">
         <v>44</v>
       </c>
@@ -8978,7 +9008,7 @@
         <v>44</v>
       </c>
       <c r="U22" s="15"/>
-      <c r="V22" s="592"/>
+      <c r="V22" s="637"/>
       <c r="W22" s="450" t="s">
         <v>176</v>
       </c>
@@ -8996,7 +9026,7 @@
       <c r="AG22" s="6"/>
       <c r="AH22" s="6"/>
       <c r="AI22" s="6"/>
-      <c r="AJ22" s="630" t="s">
+      <c r="AJ22" s="608" t="s">
         <v>489</v>
       </c>
       <c r="AK22" s="262"/>
@@ -9004,7 +9034,7 @@
         <v>495</v>
       </c>
       <c r="AM22" s="306"/>
-      <c r="AN22" s="616"/>
+      <c r="AN22" s="619"/>
     </row>
     <row r="23" spans="1:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="236" t="s">
@@ -9022,17 +9052,17 @@
       <c r="E23" s="230">
         <v>1</v>
       </c>
-      <c r="F23" s="621"/>
+      <c r="F23" s="600"/>
       <c r="I23" s="224"/>
-      <c r="O23" s="655"/>
-      <c r="Q23" s="657" t="s">
+      <c r="O23" s="603"/>
+      <c r="Q23" s="605" t="s">
         <v>145</v>
       </c>
       <c r="T23" s="17"/>
       <c r="U23" s="444" t="s">
         <v>44</v>
       </c>
-      <c r="V23" s="592"/>
+      <c r="V23" s="637"/>
       <c r="W23" s="148"/>
       <c r="X23" s="453" t="s">
         <v>189</v>
@@ -9048,13 +9078,13 @@
       <c r="AG23" s="6"/>
       <c r="AH23" s="6"/>
       <c r="AI23" s="6"/>
-      <c r="AJ23" s="630"/>
+      <c r="AJ23" s="608"/>
       <c r="AK23" s="262"/>
       <c r="AL23" s="80" t="s">
         <v>525</v>
       </c>
       <c r="AM23" s="306"/>
-      <c r="AN23" s="616"/>
+      <c r="AN23" s="619"/>
     </row>
     <row r="24" spans="1:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="464" t="s">
@@ -9072,18 +9102,18 @@
       <c r="E24" s="460">
         <v>1</v>
       </c>
-      <c r="F24" s="621"/>
+      <c r="F24" s="600"/>
       <c r="G24" s="61" t="s">
         <v>507</v>
       </c>
       <c r="I24" s="224"/>
-      <c r="O24" s="655"/>
-      <c r="Q24" s="658"/>
+      <c r="O24" s="603"/>
+      <c r="Q24" s="606"/>
       <c r="T24" s="17"/>
       <c r="U24" s="232" t="s">
         <v>44</v>
       </c>
-      <c r="V24" s="592"/>
+      <c r="V24" s="637"/>
       <c r="W24" s="148"/>
       <c r="X24" s="453" t="s">
         <v>186</v>
@@ -9107,12 +9137,12 @@
         <v>480</v>
       </c>
       <c r="AM24" s="306"/>
-      <c r="AN24" s="616"/>
+      <c r="AN24" s="619"/>
     </row>
     <row r="25" spans="1:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="F25" s="621"/>
+      <c r="F25" s="600"/>
       <c r="I25" s="224"/>
-      <c r="O25" s="655"/>
+      <c r="O25" s="603"/>
       <c r="P25" s="209" t="s">
         <v>285</v>
       </c>
@@ -9125,7 +9155,7 @@
       <c r="U25" s="424" t="s">
         <v>44</v>
       </c>
-      <c r="V25" s="593"/>
+      <c r="V25" s="638"/>
       <c r="W25" s="148"/>
       <c r="X25" s="453" t="s">
         <v>190</v>
@@ -9147,7 +9177,7 @@
       <c r="AK25" s="142"/>
       <c r="AL25" s="6"/>
       <c r="AM25" s="306"/>
-      <c r="AN25" s="616"/>
+      <c r="AN25" s="619"/>
     </row>
     <row r="26" spans="1:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="236" t="s">
@@ -9165,17 +9195,17 @@
       <c r="E26" s="398">
         <v>1</v>
       </c>
-      <c r="F26" s="621"/>
+      <c r="F26" s="600"/>
       <c r="G26" s="349" t="s">
         <v>504</v>
       </c>
       <c r="I26" s="224"/>
-      <c r="O26" s="655"/>
-      <c r="P26" s="618" t="s">
+      <c r="O26" s="603"/>
+      <c r="P26" s="621" t="s">
         <v>547</v>
       </c>
-      <c r="Q26" s="619"/>
-      <c r="R26" s="651" t="s">
+      <c r="Q26" s="622"/>
+      <c r="R26" s="597" t="s">
         <v>556</v>
       </c>
       <c r="T26" s="182"/>
@@ -9214,7 +9244,7 @@
       <c r="AM26" s="466" t="s">
         <v>473</v>
       </c>
-      <c r="AN26" s="616"/>
+      <c r="AN26" s="619"/>
     </row>
     <row r="27" spans="1:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B27" s="21" t="s">
@@ -9226,13 +9256,13 @@
       <c r="E27" s="271" t="s">
         <v>44</v>
       </c>
-      <c r="F27" s="653"/>
+      <c r="F27" s="601"/>
       <c r="G27" s="61" t="s">
         <v>565</v>
       </c>
       <c r="I27" s="225"/>
-      <c r="O27" s="656"/>
-      <c r="R27" s="652"/>
+      <c r="O27" s="604"/>
+      <c r="R27" s="598"/>
       <c r="S27" s="445" t="s">
         <v>54</v>
       </c>
@@ -9262,32 +9292,26 @@
       <c r="AM27" s="400" t="s">
         <v>326</v>
       </c>
-      <c r="AN27" s="617"/>
+      <c r="AN27" s="620"/>
     </row>
   </sheetData>
   <mergeCells count="54">
-    <mergeCell ref="E2:E3"/>
-    <mergeCell ref="K2:L2"/>
-    <mergeCell ref="I1:I2"/>
-    <mergeCell ref="R18:R19"/>
-    <mergeCell ref="R26:R27"/>
-    <mergeCell ref="F2:F27"/>
-    <mergeCell ref="O10:O27"/>
-    <mergeCell ref="Q20:Q21"/>
-    <mergeCell ref="Q23:Q24"/>
-    <mergeCell ref="G14:J14"/>
-    <mergeCell ref="G13:J13"/>
-    <mergeCell ref="H12:K12"/>
-    <mergeCell ref="A5:A6"/>
-    <mergeCell ref="C6:D6"/>
-    <mergeCell ref="AI6:AI10"/>
-    <mergeCell ref="AF12:AF15"/>
-    <mergeCell ref="AG7:AG12"/>
-    <mergeCell ref="L8:L9"/>
-    <mergeCell ref="S9:S12"/>
-    <mergeCell ref="N8:N9"/>
-    <mergeCell ref="AD12:AD15"/>
-    <mergeCell ref="C15:C16"/>
+    <mergeCell ref="V21:V25"/>
+    <mergeCell ref="U18:U20"/>
+    <mergeCell ref="C2:C3"/>
+    <mergeCell ref="C4:C5"/>
+    <mergeCell ref="A2:A3"/>
+    <mergeCell ref="B2:B3"/>
+    <mergeCell ref="D2:D3"/>
+    <mergeCell ref="J8:J9"/>
+    <mergeCell ref="G5:L6"/>
+    <mergeCell ref="I8:I9"/>
+    <mergeCell ref="K7:K9"/>
+    <mergeCell ref="H8:H9"/>
+    <mergeCell ref="G8:G9"/>
+    <mergeCell ref="B11:B12"/>
+    <mergeCell ref="B6:B7"/>
+    <mergeCell ref="B4:B5"/>
     <mergeCell ref="AN1:AN27"/>
     <mergeCell ref="P26:Q26"/>
     <mergeCell ref="Q2:Q3"/>
@@ -9304,22 +9328,28 @@
     <mergeCell ref="AD3:AD4"/>
     <mergeCell ref="S2:S3"/>
     <mergeCell ref="R2:R3"/>
-    <mergeCell ref="V21:V25"/>
-    <mergeCell ref="U18:U20"/>
-    <mergeCell ref="C2:C3"/>
-    <mergeCell ref="C4:C5"/>
-    <mergeCell ref="A2:A3"/>
-    <mergeCell ref="B2:B3"/>
-    <mergeCell ref="D2:D3"/>
-    <mergeCell ref="J8:J9"/>
-    <mergeCell ref="G5:L6"/>
-    <mergeCell ref="I8:I9"/>
-    <mergeCell ref="K7:K9"/>
-    <mergeCell ref="H8:H9"/>
-    <mergeCell ref="G8:G9"/>
-    <mergeCell ref="B11:B12"/>
-    <mergeCell ref="B6:B7"/>
-    <mergeCell ref="B4:B5"/>
+    <mergeCell ref="A5:A6"/>
+    <mergeCell ref="C6:D6"/>
+    <mergeCell ref="AI6:AI10"/>
+    <mergeCell ref="AF12:AF15"/>
+    <mergeCell ref="AG7:AG12"/>
+    <mergeCell ref="L8:L9"/>
+    <mergeCell ref="S9:S12"/>
+    <mergeCell ref="N8:N9"/>
+    <mergeCell ref="AD12:AD15"/>
+    <mergeCell ref="C15:C16"/>
+    <mergeCell ref="E2:E3"/>
+    <mergeCell ref="K2:L2"/>
+    <mergeCell ref="I1:I2"/>
+    <mergeCell ref="R18:R19"/>
+    <mergeCell ref="R26:R27"/>
+    <mergeCell ref="F2:F27"/>
+    <mergeCell ref="O10:O27"/>
+    <mergeCell ref="Q20:Q21"/>
+    <mergeCell ref="Q23:Q24"/>
+    <mergeCell ref="G14:J14"/>
+    <mergeCell ref="G13:J13"/>
+    <mergeCell ref="H12:K12"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -9329,8 +9359,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2029A93E-B53C-4201-9F17-439C144F3CF1}">
   <dimension ref="A1:AN37"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q36" sqref="Q36"/>
+    <sheetView tabSelected="1" topLeftCell="N1" workbookViewId="0">
+      <selection activeCell="AL8" sqref="AL8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9368,7 +9398,7 @@
     <col min="36" max="36" width="3.140625" bestFit="1" customWidth="1"/>
     <col min="37" max="37" width="4.42578125" bestFit="1" customWidth="1"/>
     <col min="38" max="38" width="15.28515625" bestFit="1" customWidth="1"/>
-    <col min="39" max="39" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="11.7109375" style="20" bestFit="1" customWidth="1"/>
     <col min="40" max="40" width="11.7109375" style="65" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -9425,10 +9455,10 @@
       <c r="S1" s="142"/>
       <c r="T1" s="142"/>
       <c r="U1" s="6"/>
-      <c r="V1" s="666" t="s">
+      <c r="V1" s="663" t="s">
         <v>458</v>
       </c>
-      <c r="W1" s="667"/>
+      <c r="W1" s="664"/>
       <c r="X1" s="312">
         <f>68-(U8+W3+V3+S3)</f>
         <v>0</v>
@@ -9444,28 +9474,28 @@
       <c r="AB1" s="308" t="s">
         <v>44</v>
       </c>
-      <c r="AC1" s="668" t="s">
+      <c r="AC1" s="665" t="s">
         <v>191</v>
       </c>
-      <c r="AD1" s="669"/>
-      <c r="AE1" s="670"/>
-      <c r="AF1" s="671" t="s">
+      <c r="AD1" s="666"/>
+      <c r="AE1" s="667"/>
+      <c r="AF1" s="668" t="s">
         <v>298</v>
       </c>
-      <c r="AG1" s="672"/>
-      <c r="AH1" s="673"/>
-      <c r="AI1" s="663" t="s">
+      <c r="AG1" s="669"/>
+      <c r="AH1" s="670"/>
+      <c r="AI1" s="660" t="s">
         <v>461</v>
       </c>
-      <c r="AJ1" s="664"/>
-      <c r="AK1" s="665"/>
+      <c r="AJ1" s="661"/>
+      <c r="AK1" s="662"/>
       <c r="AN1" s="142"/>
     </row>
     <row r="2" spans="1:40" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="F2" s="22" t="s">
         <v>44</v>
       </c>
-      <c r="H2" s="734">
+      <c r="H2" s="545">
         <f>SUM(H4:H37)</f>
         <v>-8</v>
       </c>
@@ -9475,19 +9505,19 @@
       <c r="K2" s="327">
         <v>-3</v>
       </c>
-      <c r="L2" s="674">
+      <c r="L2" s="671">
         <f>SUM(L5:L30)</f>
         <v>3</v>
       </c>
-      <c r="M2" s="676">
+      <c r="M2" s="673">
         <f>SUM(M4:M29)</f>
         <v>6</v>
       </c>
-      <c r="N2" s="678">
+      <c r="N2" s="675">
         <f>SUM(N4:N29)</f>
         <v>9</v>
       </c>
-      <c r="O2" s="642">
+      <c r="O2" s="615">
         <f>SUM(M30:M37)* (-1)</f>
         <v>-3</v>
       </c>
@@ -9506,7 +9536,7 @@
       <c r="T2" s="515" t="s">
         <v>221</v>
       </c>
-      <c r="U2" s="680" t="s">
+      <c r="U2" s="677" t="s">
         <v>239</v>
       </c>
       <c r="V2" s="516" t="s">
@@ -9560,7 +9590,7 @@
       <c r="AL2" s="181" t="s">
         <v>296</v>
       </c>
-      <c r="AM2" s="2" t="s">
+      <c r="AM2" s="21" t="s">
         <v>463</v>
       </c>
       <c r="AN2" s="61" t="s">
@@ -9575,10 +9605,10 @@
         <f>T3+V3+W3+S3</f>
         <v>68</v>
       </c>
-      <c r="L3" s="675"/>
-      <c r="M3" s="677"/>
-      <c r="N3" s="679"/>
-      <c r="O3" s="643"/>
+      <c r="L3" s="672"/>
+      <c r="M3" s="674"/>
+      <c r="N3" s="676"/>
+      <c r="O3" s="616"/>
       <c r="P3" s="176">
         <f>(L2+M2)-W3</f>
         <v>0</v>
@@ -9594,7 +9624,7 @@
         <f>SUM(T4:T29)</f>
         <v>41</v>
       </c>
-      <c r="U3" s="681"/>
+      <c r="U3" s="678"/>
       <c r="V3" s="519">
         <f t="shared" ref="V3:AA3" si="0">SUM(V4:V29)</f>
         <v>6</v>
@@ -9693,7 +9723,7 @@
         <f>AA4</f>
         <v>0</v>
       </c>
-      <c r="O4" s="660" t="s">
+      <c r="O4" s="679" t="s">
         <v>200</v>
       </c>
       <c r="P4" s="20"/>
@@ -9757,7 +9787,7 @@
       <c r="AL4" s="541" t="s">
         <v>204</v>
       </c>
-      <c r="AM4" s="320"/>
+      <c r="AM4" s="188"/>
       <c r="AN4" s="142" t="s">
         <v>577</v>
       </c>
@@ -9772,7 +9802,7 @@
         <f>AA5</f>
         <v>0</v>
       </c>
-      <c r="O5" s="661"/>
+      <c r="O5" s="680"/>
       <c r="P5" s="20"/>
       <c r="Q5" s="2" t="s">
         <v>347</v>
@@ -9830,7 +9860,7 @@
         <v>0</v>
       </c>
       <c r="AL5" s="6"/>
-      <c r="AM5" s="403"/>
+      <c r="AM5" s="734"/>
       <c r="AN5" s="142"/>
     </row>
     <row r="6" spans="1:40" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -9859,7 +9889,7 @@
         <f>AA6</f>
         <v>0</v>
       </c>
-      <c r="O6" s="661"/>
+      <c r="O6" s="680"/>
       <c r="P6" s="19" t="s">
         <v>342</v>
       </c>
@@ -9924,7 +9954,7 @@
         <v>0</v>
       </c>
       <c r="AL6" s="6"/>
-      <c r="AM6" s="321" t="s">
+      <c r="AM6" s="735" t="s">
         <v>584</v>
       </c>
       <c r="AN6" s="262"/>
@@ -9950,7 +9980,7 @@
         <f t="shared" ref="N7:N37" si="10">AA7</f>
         <v>0</v>
       </c>
-      <c r="O7" s="661"/>
+      <c r="O7" s="680"/>
       <c r="P7" s="20"/>
       <c r="Q7" s="2" t="s">
         <v>342</v>
@@ -10018,7 +10048,7 @@
         <v>0</v>
       </c>
       <c r="AL7" s="6"/>
-      <c r="AM7" s="321"/>
+      <c r="AM7" s="735"/>
       <c r="AN7" s="262"/>
     </row>
     <row r="8" spans="1:40" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -10056,7 +10086,7 @@
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
-      <c r="O8" s="661"/>
+      <c r="O8" s="680"/>
       <c r="P8" s="21" t="s">
         <v>238</v>
       </c>
@@ -10125,7 +10155,7 @@
         <v>0</v>
       </c>
       <c r="AL8" s="6"/>
-      <c r="AM8" s="321"/>
+      <c r="AM8" s="735"/>
       <c r="AN8" s="262"/>
     </row>
     <row r="9" spans="1:40" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -10140,7 +10170,7 @@
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
-      <c r="O9" s="661"/>
+      <c r="O9" s="680"/>
       <c r="P9" s="21" t="s">
         <v>342</v>
       </c>
@@ -10203,7 +10233,7 @@
         <v>0</v>
       </c>
       <c r="AL9" s="6"/>
-      <c r="AM9" s="321"/>
+      <c r="AM9" s="736"/>
       <c r="AN9" s="142"/>
     </row>
     <row r="10" spans="1:40" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -10238,7 +10268,7 @@
         <f t="shared" si="10"/>
         <v>2</v>
       </c>
-      <c r="O10" s="661"/>
+      <c r="O10" s="680"/>
       <c r="P10" s="20"/>
       <c r="Q10" s="2" t="s">
         <v>347</v>
@@ -10302,10 +10332,10 @@
       <c r="AL10" s="6" t="s">
         <v>74</v>
       </c>
-      <c r="AM10" s="544" t="s">
-        <v>588</v>
-      </c>
-      <c r="AN10" s="262" t="s">
+      <c r="AM10" s="24" t="s">
+        <v>610</v>
+      </c>
+      <c r="AN10" s="142" t="s">
         <v>512</v>
       </c>
     </row>
@@ -10321,7 +10351,7 @@
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
-      <c r="O11" s="661"/>
+      <c r="O11" s="680"/>
       <c r="P11" s="21" t="s">
         <v>342</v>
       </c>
@@ -10377,11 +10407,11 @@
         <v>0</v>
       </c>
       <c r="AL11" s="6"/>
-      <c r="AM11" s="321"/>
+      <c r="AM11" s="735"/>
       <c r="AN11" s="142"/>
     </row>
     <row r="12" spans="1:40" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="606" t="s">
+      <c r="A12" s="651" t="s">
         <v>55</v>
       </c>
       <c r="B12" s="30">
@@ -10390,7 +10420,7 @@
       <c r="C12" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="E12" s="657" t="s">
+      <c r="E12" s="605" t="s">
         <v>57</v>
       </c>
       <c r="G12" s="267"/>
@@ -10408,7 +10438,7 @@
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
-      <c r="O12" s="661"/>
+      <c r="O12" s="680"/>
       <c r="P12" s="21" t="s">
         <v>342</v>
       </c>
@@ -10468,7 +10498,7 @@
         <v>0</v>
       </c>
       <c r="AL12" s="6"/>
-      <c r="AM12" s="321" t="s">
+      <c r="AM12" s="735" t="s">
         <v>528</v>
       </c>
       <c r="AN12" s="301" t="s">
@@ -10476,14 +10506,14 @@
       </c>
     </row>
     <row r="13" spans="1:40" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="608"/>
+      <c r="A13" s="653"/>
       <c r="B13" s="153">
         <v>12</v>
       </c>
       <c r="C13" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="E13" s="658"/>
+      <c r="E13" s="606"/>
       <c r="F13" s="176">
         <v>0</v>
       </c>
@@ -10506,7 +10536,7 @@
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
-      <c r="O13" s="661"/>
+      <c r="O13" s="680"/>
       <c r="P13" s="21" t="s">
         <v>342</v>
       </c>
@@ -10562,7 +10592,7 @@
         <v>0</v>
       </c>
       <c r="AL13" s="16"/>
-      <c r="AM13" s="321"/>
+      <c r="AM13" s="735"/>
       <c r="AN13" s="142"/>
     </row>
     <row r="14" spans="1:40" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -10582,7 +10612,7 @@
         <f t="shared" si="10"/>
         <v>2</v>
       </c>
-      <c r="O14" s="661"/>
+      <c r="O14" s="680"/>
       <c r="P14" s="20"/>
       <c r="Q14" s="205" t="s">
         <v>346</v>
@@ -10644,7 +10674,7 @@
       <c r="AL14" s="6" t="s">
         <v>583</v>
       </c>
-      <c r="AM14" s="542" t="s">
+      <c r="AM14" s="737" t="s">
         <v>586</v>
       </c>
       <c r="AN14" s="142" t="s">
@@ -10677,7 +10707,7 @@
         <f t="shared" si="10"/>
         <v>1</v>
       </c>
-      <c r="O15" s="661"/>
+      <c r="O15" s="680"/>
       <c r="P15" s="20"/>
       <c r="Q15" s="205" t="s">
         <v>346</v>
@@ -10743,7 +10773,7 @@
       <c r="AL15" s="6" t="s">
         <v>232</v>
       </c>
-      <c r="AM15" s="321" t="s">
+      <c r="AM15" s="735" t="s">
         <v>468</v>
       </c>
       <c r="AN15" s="142"/>
@@ -10764,7 +10794,7 @@
         <f t="shared" si="10"/>
         <v>1</v>
       </c>
-      <c r="O16" s="661"/>
+      <c r="O16" s="680"/>
       <c r="P16" s="21" t="s">
         <v>342</v>
       </c>
@@ -10832,7 +10862,7 @@
       <c r="AL16" s="6" t="s">
         <v>235</v>
       </c>
-      <c r="AM16" s="543" t="s">
+      <c r="AM16" s="542" t="s">
         <v>578</v>
       </c>
       <c r="AN16" s="107" t="s">
@@ -10862,7 +10892,7 @@
         <f t="shared" si="10"/>
         <v>1</v>
       </c>
-      <c r="O17" s="661"/>
+      <c r="O17" s="680"/>
       <c r="P17" s="20"/>
       <c r="Q17" s="2" t="s">
         <v>348</v>
@@ -10926,7 +10956,7 @@
       <c r="AL17" s="6" t="s">
         <v>97</v>
       </c>
-      <c r="AM17" s="544" t="s">
+      <c r="AM17" s="543" t="s">
         <v>588</v>
       </c>
       <c r="AN17" s="64" t="s">
@@ -10957,7 +10987,7 @@
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
-      <c r="O18" s="661"/>
+      <c r="O18" s="680"/>
       <c r="P18" s="21" t="s">
         <v>342</v>
       </c>
@@ -11017,7 +11047,7 @@
         <v>0</v>
       </c>
       <c r="AL18" s="6"/>
-      <c r="AM18" s="504"/>
+      <c r="AM18" s="738"/>
       <c r="AN18" s="142"/>
     </row>
     <row r="19" spans="1:40" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -11040,7 +11070,7 @@
         <f t="shared" si="10"/>
         <v>1</v>
       </c>
-      <c r="O19" s="661"/>
+      <c r="O19" s="680"/>
       <c r="P19" s="20"/>
       <c r="Q19" s="2" t="s">
         <v>341</v>
@@ -11104,7 +11134,7 @@
       <c r="AL19" s="6" t="s">
         <v>574</v>
       </c>
-      <c r="AM19" s="321"/>
+      <c r="AM19" s="735"/>
       <c r="AN19" s="142"/>
     </row>
     <row r="20" spans="1:40" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -11136,11 +11166,11 @@
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
-      <c r="O20" s="662"/>
+      <c r="O20" s="681"/>
       <c r="P20" s="556" t="s">
         <v>342</v>
       </c>
-      <c r="Q20" s="659"/>
+      <c r="Q20" s="607"/>
       <c r="R20" s="321" t="s">
         <v>86</v>
       </c>
@@ -11198,7 +11228,7 @@
       <c r="AL20" s="6" t="s">
         <v>88</v>
       </c>
-      <c r="AM20" s="321" t="s">
+      <c r="AM20" s="735" t="s">
         <v>464</v>
       </c>
     </row>
@@ -11295,7 +11325,7 @@
       <c r="AL21" s="6" t="s">
         <v>84</v>
       </c>
-      <c r="AM21" s="321" t="s">
+      <c r="AM21" s="735" t="s">
         <v>464</v>
       </c>
       <c r="AN21" s="142"/>
@@ -11370,11 +11400,11 @@
         <v>0</v>
       </c>
       <c r="AL22" s="16"/>
-      <c r="AM22" s="504"/>
+      <c r="AM22" s="738"/>
       <c r="AN22" s="142"/>
     </row>
     <row r="23" spans="1:40" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E23" s="613" t="s">
+      <c r="E23" s="658" t="s">
         <v>294</v>
       </c>
       <c r="F23" s="184"/>
@@ -11454,7 +11484,7 @@
       <c r="AL23" s="6" t="s">
         <v>592</v>
       </c>
-      <c r="AM23" s="321" t="s">
+      <c r="AM23" s="735" t="s">
         <v>589</v>
       </c>
       <c r="AN23" s="142" t="s">
@@ -11465,7 +11495,7 @@
       <c r="C24" s="2" t="s">
         <v>260</v>
       </c>
-      <c r="E24" s="614"/>
+      <c r="E24" s="659"/>
       <c r="F24" s="176"/>
       <c r="K24" s="403" t="s">
         <v>301</v>
@@ -11483,7 +11513,7 @@
       <c r="P24" s="556" t="s">
         <v>342</v>
       </c>
-      <c r="Q24" s="659"/>
+      <c r="Q24" s="607"/>
       <c r="R24" s="321" t="s">
         <v>254</v>
       </c>
@@ -11549,7 +11579,7 @@
       <c r="AL24" s="6" t="s">
         <v>527</v>
       </c>
-      <c r="AM24" s="321"/>
+      <c r="AM24" s="735"/>
       <c r="AN24" s="142" t="s">
         <v>254</v>
       </c>
@@ -11625,7 +11655,7 @@
         <v>0</v>
       </c>
       <c r="AL25" s="16"/>
-      <c r="AM25" s="321" t="s">
+      <c r="AM25" s="735" t="s">
         <v>470</v>
       </c>
       <c r="AN25" s="142"/>
@@ -11714,7 +11744,7 @@
         <v>0</v>
       </c>
       <c r="AL26" s="493"/>
-      <c r="AM26" s="321"/>
+      <c r="AM26" s="735"/>
       <c r="AN26" s="142"/>
     </row>
     <row r="27" spans="1:40" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -11791,7 +11821,7 @@
         <v>0</v>
       </c>
       <c r="AL27" s="16"/>
-      <c r="AM27" s="504"/>
+      <c r="AM27" s="738"/>
       <c r="AN27" s="142"/>
     </row>
     <row r="28" spans="1:40" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -11857,7 +11887,7 @@
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
-      <c r="AM28" s="504"/>
+      <c r="AM28" s="738"/>
       <c r="AN28" s="142"/>
     </row>
     <row r="29" spans="1:40" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -11936,7 +11966,7 @@
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
-      <c r="AM29" s="504"/>
+      <c r="AM29" s="738"/>
       <c r="AN29" s="142"/>
     </row>
     <row r="30" spans="1:40" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -11996,7 +12026,7 @@
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
-      <c r="AM30" s="504"/>
+      <c r="AM30" s="738"/>
       <c r="AN30" s="142"/>
     </row>
     <row r="31" spans="1:40" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -12067,11 +12097,11 @@
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
-      <c r="AM31" s="504"/>
+      <c r="AM31" s="738"/>
       <c r="AN31" s="142"/>
     </row>
     <row r="32" spans="1:40" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="H32" s="545">
+      <c r="H32" s="544">
         <v>-1</v>
       </c>
       <c r="I32" s="221" t="s">
@@ -12154,7 +12184,7 @@
       <c r="AL32" s="6" t="s">
         <v>466</v>
       </c>
-      <c r="AM32" s="321" t="s">
+      <c r="AM32" s="735" t="s">
         <v>467</v>
       </c>
       <c r="AN32" s="107" t="s">
@@ -12222,7 +12252,7 @@
         <v>0</v>
       </c>
       <c r="AL33" s="6"/>
-      <c r="AM33" s="504"/>
+      <c r="AM33" s="738"/>
       <c r="AN33" s="142"/>
     </row>
     <row r="34" spans="3:40" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -12303,7 +12333,7 @@
         <v>1</v>
       </c>
       <c r="AL34" s="6"/>
-      <c r="AM34" s="321" t="s">
+      <c r="AM34" s="735" t="s">
         <v>589</v>
       </c>
       <c r="AN34" s="142" t="s">
@@ -12385,7 +12415,7 @@
       <c r="AL35" s="6" t="s">
         <v>314</v>
       </c>
-      <c r="AM35" s="321"/>
+      <c r="AM35" s="735"/>
       <c r="AN35" s="142"/>
     </row>
     <row r="36" spans="3:40" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -12462,13 +12492,13 @@
       <c r="AL36" s="6" t="s">
         <v>313</v>
       </c>
-      <c r="AM36" s="504"/>
+      <c r="AM36" s="738"/>
       <c r="AN36" s="142" t="s">
         <v>590</v>
       </c>
     </row>
     <row r="37" spans="3:40" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="H37" s="734">
+      <c r="H37" s="545">
         <v>-1</v>
       </c>
       <c r="K37" s="405" t="s">
@@ -12546,7 +12576,7 @@
       <c r="AL37" s="6" t="s">
         <v>485</v>
       </c>
-      <c r="AM37" s="544" t="s">
+      <c r="AM37" s="543" t="s">
         <v>588</v>
       </c>
       <c r="AN37" s="107" t="s">
@@ -12555,6 +12585,12 @@
     </row>
   </sheetData>
   <mergeCells count="15">
+    <mergeCell ref="A12:A13"/>
+    <mergeCell ref="E12:E13"/>
+    <mergeCell ref="P20:Q20"/>
+    <mergeCell ref="E23:E24"/>
+    <mergeCell ref="P24:Q24"/>
+    <mergeCell ref="O4:O20"/>
     <mergeCell ref="AI1:AK1"/>
     <mergeCell ref="V1:W1"/>
     <mergeCell ref="AC1:AE1"/>
@@ -12564,12 +12600,6 @@
     <mergeCell ref="N2:N3"/>
     <mergeCell ref="O2:O3"/>
     <mergeCell ref="U2:U3"/>
-    <mergeCell ref="A12:A13"/>
-    <mergeCell ref="E12:E13"/>
-    <mergeCell ref="P20:Q20"/>
-    <mergeCell ref="E23:E24"/>
-    <mergeCell ref="P24:Q24"/>
-    <mergeCell ref="O4:O20"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -12606,12 +12636,12 @@
       <c r="B1" s="556" t="s">
         <v>317</v>
       </c>
-      <c r="C1" s="659"/>
+      <c r="C1" s="607"/>
       <c r="D1" s="209"/>
       <c r="J1" s="556" t="s">
         <v>70</v>
       </c>
-      <c r="K1" s="659"/>
+      <c r="K1" s="607"/>
       <c r="L1" s="200" t="s">
         <v>337</v>
       </c>
@@ -13002,7 +13032,7 @@
       <c r="V1" s="556" t="s">
         <v>71</v>
       </c>
-      <c r="W1" s="659"/>
+      <c r="W1" s="607"/>
       <c r="X1" s="62" t="s">
         <v>102</v>
       </c>
@@ -13021,7 +13051,7 @@
       <c r="AC1" s="116" t="s">
         <v>191</v>
       </c>
-      <c r="AD1" s="702" t="s">
+      <c r="AD1" s="695" t="s">
         <v>213</v>
       </c>
       <c r="AE1" s="116" t="s">
@@ -13038,10 +13068,10 @@
       <c r="E2" s="39" t="s">
         <v>74</v>
       </c>
-      <c r="F2" s="733" t="s">
+      <c r="F2" s="694" t="s">
         <v>75</v>
       </c>
-      <c r="G2" s="690" t="s">
+      <c r="G2" s="722" t="s">
         <v>44</v>
       </c>
       <c r="H2" s="40" t="s">
@@ -13069,10 +13099,10 @@
       <c r="U2" s="60" t="s">
         <v>106</v>
       </c>
-      <c r="V2" s="666" t="s">
+      <c r="V2" s="663" t="s">
         <v>121</v>
       </c>
-      <c r="W2" s="667"/>
+      <c r="W2" s="664"/>
       <c r="X2" s="64" t="s">
         <v>110</v>
       </c>
@@ -13091,7 +13121,7 @@
       <c r="AC2" s="117" t="s">
         <v>99</v>
       </c>
-      <c r="AD2" s="703"/>
+      <c r="AD2" s="696"/>
       <c r="AE2" s="64" t="s">
         <v>99</v>
       </c>
@@ -13110,8 +13140,8 @@
       <c r="E3" s="39" t="s">
         <v>80</v>
       </c>
-      <c r="F3" s="610"/>
-      <c r="G3" s="691"/>
+      <c r="F3" s="655"/>
+      <c r="G3" s="723"/>
       <c r="H3" s="40" t="s">
         <v>81</v>
       </c>
@@ -13122,13 +13152,13 @@
         <v>82</v>
       </c>
       <c r="N3" s="44"/>
-      <c r="O3" s="700" t="s">
+      <c r="O3" s="732" t="s">
         <v>44</v>
       </c>
-      <c r="P3" s="721" t="s">
+      <c r="P3" s="714" t="s">
         <v>219</v>
       </c>
-      <c r="Q3" s="722"/>
+      <c r="Q3" s="715"/>
       <c r="S3" s="57" t="s">
         <v>220</v>
       </c>
@@ -13138,15 +13168,15 @@
       <c r="W3" s="59" t="s">
         <v>105</v>
       </c>
-      <c r="AD3" s="703"/>
+      <c r="AD3" s="696"/>
     </row>
     <row r="4" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="G4" s="691"/>
+      <c r="G4" s="723"/>
       <c r="H4" s="6"/>
       <c r="L4" s="685" t="s">
         <v>83</v>
       </c>
-      <c r="O4" s="701"/>
+      <c r="O4" s="733"/>
       <c r="T4" s="55" t="s">
         <v>98</v>
       </c>
@@ -13160,8 +13190,8 @@
         <v>195</v>
       </c>
       <c r="Z4" s="558"/>
-      <c r="AA4" s="659"/>
-      <c r="AD4" s="703"/>
+      <c r="AA4" s="607"/>
+      <c r="AD4" s="696"/>
     </row>
     <row r="5" spans="1:31" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C5" s="52" t="s">
@@ -13176,21 +13206,21 @@
       <c r="F5" s="66" t="s">
         <v>85</v>
       </c>
-      <c r="G5" s="691"/>
+      <c r="G5" s="723"/>
       <c r="H5" s="46" t="s">
         <v>76</v>
       </c>
-      <c r="K5" s="708" t="s">
+      <c r="K5" s="701" t="s">
         <v>217</v>
       </c>
-      <c r="L5" s="723"/>
+      <c r="L5" s="716"/>
       <c r="M5" s="2" t="s">
         <v>215</v>
       </c>
       <c r="N5" s="61" t="s">
         <v>214</v>
       </c>
-      <c r="O5" s="701"/>
+      <c r="O5" s="733"/>
       <c r="P5" s="108" t="s">
         <v>216</v>
       </c>
@@ -13206,11 +13236,11 @@
       <c r="U5" s="19" t="s">
         <v>99</v>
       </c>
-      <c r="Y5" s="711" t="s">
+      <c r="Y5" s="704" t="s">
         <v>287</v>
       </c>
-      <c r="Z5" s="712"/>
-      <c r="AD5" s="703"/>
+      <c r="Z5" s="705"/>
+      <c r="AD5" s="696"/>
     </row>
     <row r="6" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C6" s="109"/>
@@ -13220,16 +13250,16 @@
       <c r="E6" s="45" t="s">
         <v>86</v>
       </c>
-      <c r="G6" s="691"/>
+      <c r="G6" s="723"/>
       <c r="H6" s="46" t="s">
         <v>81</v>
       </c>
       <c r="I6" s="23">
         <v>15</v>
       </c>
-      <c r="K6" s="709"/>
-      <c r="L6" s="723"/>
-      <c r="O6" s="701"/>
+      <c r="K6" s="702"/>
+      <c r="L6" s="716"/>
+      <c r="O6" s="733"/>
       <c r="T6" s="2" t="s">
         <v>101</v>
       </c>
@@ -13239,23 +13269,23 @@
       <c r="V6" s="21">
         <v>-1</v>
       </c>
-      <c r="AD6" s="703"/>
+      <c r="AD6" s="696"/>
     </row>
     <row r="7" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C7" s="110"/>
-      <c r="G7" s="691"/>
+      <c r="G7" s="723"/>
       <c r="H7" s="6"/>
-      <c r="K7" s="709"/>
-      <c r="L7" s="723"/>
+      <c r="K7" s="702"/>
+      <c r="L7" s="716"/>
       <c r="N7" s="21" t="s">
         <v>120</v>
       </c>
-      <c r="O7" s="701"/>
+      <c r="O7" s="733"/>
       <c r="P7" s="73"/>
       <c r="U7" s="104" t="s">
         <v>20</v>
       </c>
-      <c r="AD7" s="703"/>
+      <c r="AD7" s="696"/>
     </row>
     <row r="8" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C8" s="130"/>
@@ -13268,7 +13298,7 @@
       <c r="F8" s="66" t="s">
         <v>87</v>
       </c>
-      <c r="G8" s="691"/>
+      <c r="G8" s="723"/>
       <c r="H8" s="50" t="s">
         <v>76</v>
       </c>
@@ -13278,41 +13308,41 @@
       <c r="J8" s="111">
         <v>115</v>
       </c>
-      <c r="K8" s="709"/>
-      <c r="L8" s="723"/>
-      <c r="O8" s="701"/>
+      <c r="K8" s="702"/>
+      <c r="L8" s="716"/>
+      <c r="O8" s="733"/>
       <c r="P8" s="49"/>
-      <c r="S8" s="705" t="s">
+      <c r="S8" s="698" t="s">
         <v>212</v>
       </c>
-      <c r="T8" s="706"/>
-      <c r="U8" s="706"/>
-      <c r="V8" s="706"/>
-      <c r="W8" s="706"/>
-      <c r="X8" s="706"/>
-      <c r="Y8" s="706"/>
-      <c r="Z8" s="706"/>
-      <c r="AA8" s="706"/>
-      <c r="AB8" s="706"/>
-      <c r="AC8" s="707"/>
-      <c r="AD8" s="703"/>
+      <c r="T8" s="699"/>
+      <c r="U8" s="699"/>
+      <c r="V8" s="699"/>
+      <c r="W8" s="699"/>
+      <c r="X8" s="699"/>
+      <c r="Y8" s="699"/>
+      <c r="Z8" s="699"/>
+      <c r="AA8" s="699"/>
+      <c r="AB8" s="699"/>
+      <c r="AC8" s="700"/>
+      <c r="AD8" s="696"/>
     </row>
     <row r="9" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C9" s="727"/>
-      <c r="G9" s="691"/>
+      <c r="C9" s="688"/>
+      <c r="G9" s="723"/>
       <c r="H9" s="6"/>
-      <c r="K9" s="709"/>
-      <c r="L9" s="694" t="s">
+      <c r="K9" s="702"/>
+      <c r="L9" s="726" t="s">
         <v>218</v>
       </c>
-      <c r="M9" s="695"/>
-      <c r="N9" s="696"/>
-      <c r="O9" s="701"/>
+      <c r="M9" s="727"/>
+      <c r="N9" s="728"/>
+      <c r="O9" s="733"/>
       <c r="P9" s="75"/>
-      <c r="AD9" s="703"/>
+      <c r="AD9" s="696"/>
     </row>
     <row r="10" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C10" s="728"/>
+      <c r="C10" s="689"/>
       <c r="D10" s="23"/>
       <c r="E10" s="45" t="s">
         <v>88</v>
@@ -13320,7 +13350,7 @@
       <c r="F10" s="66" t="s">
         <v>89</v>
       </c>
-      <c r="G10" s="691"/>
+      <c r="G10" s="723"/>
       <c r="H10" s="51"/>
       <c r="I10" s="21" t="s">
         <v>81</v>
@@ -13328,33 +13358,33 @@
       <c r="J10" s="3">
         <v>15</v>
       </c>
-      <c r="K10" s="709"/>
-      <c r="M10" s="730" t="s">
+      <c r="K10" s="702"/>
+      <c r="M10" s="691" t="s">
         <v>90</v>
       </c>
-      <c r="N10" s="731"/>
-      <c r="O10" s="731"/>
-      <c r="P10" s="731"/>
-      <c r="Q10" s="731"/>
-      <c r="R10" s="731"/>
-      <c r="S10" s="731"/>
-      <c r="T10" s="731"/>
-      <c r="U10" s="731"/>
-      <c r="V10" s="731"/>
-      <c r="W10" s="731"/>
-      <c r="X10" s="731"/>
-      <c r="Y10" s="731"/>
-      <c r="Z10" s="731"/>
-      <c r="AA10" s="731"/>
-      <c r="AB10" s="731"/>
-      <c r="AC10" s="732"/>
-      <c r="AD10" s="703"/>
+      <c r="N10" s="692"/>
+      <c r="O10" s="692"/>
+      <c r="P10" s="692"/>
+      <c r="Q10" s="692"/>
+      <c r="R10" s="692"/>
+      <c r="S10" s="692"/>
+      <c r="T10" s="692"/>
+      <c r="U10" s="692"/>
+      <c r="V10" s="692"/>
+      <c r="W10" s="692"/>
+      <c r="X10" s="692"/>
+      <c r="Y10" s="692"/>
+      <c r="Z10" s="692"/>
+      <c r="AA10" s="692"/>
+      <c r="AB10" s="692"/>
+      <c r="AC10" s="693"/>
+      <c r="AD10" s="696"/>
     </row>
     <row r="11" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C11" s="729"/>
-      <c r="G11" s="691"/>
+      <c r="C11" s="690"/>
+      <c r="G11" s="723"/>
       <c r="H11" s="6"/>
-      <c r="K11" s="709"/>
+      <c r="K11" s="702"/>
       <c r="R11" s="52" t="s">
         <v>44</v>
       </c>
@@ -13362,17 +13392,17 @@
       <c r="Y11" s="68" t="s">
         <v>121</v>
       </c>
-      <c r="Z11" s="719" t="s">
+      <c r="Z11" s="712" t="s">
         <v>121</v>
       </c>
-      <c r="AA11" s="720"/>
+      <c r="AA11" s="713"/>
       <c r="AB11" s="52" t="s">
         <v>44</v>
       </c>
       <c r="AC11" s="118" t="s">
         <v>121</v>
       </c>
-      <c r="AD11" s="703"/>
+      <c r="AD11" s="696"/>
     </row>
     <row r="12" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C12" s="129"/>
@@ -13385,7 +13415,7 @@
       <c r="F12" s="66" t="s">
         <v>92</v>
       </c>
-      <c r="G12" s="691"/>
+      <c r="G12" s="723"/>
       <c r="H12" s="128"/>
       <c r="I12" s="19" t="s">
         <v>81</v>
@@ -13393,8 +13423,8 @@
       <c r="J12" s="3">
         <v>15</v>
       </c>
-      <c r="K12" s="709"/>
-      <c r="L12" s="724" t="s">
+      <c r="K12" s="702"/>
+      <c r="L12" s="717" t="s">
         <v>93</v>
       </c>
       <c r="M12" s="21" t="s">
@@ -13425,25 +13455,25 @@
         <v>116</v>
       </c>
       <c r="Y12" s="6"/>
-      <c r="AA12" s="713" t="s">
+      <c r="AA12" s="706" t="s">
         <v>126</v>
       </c>
-      <c r="AB12" s="714"/>
+      <c r="AB12" s="707"/>
       <c r="AC12" s="21" t="s">
         <v>233</v>
       </c>
-      <c r="AD12" s="703"/>
+      <c r="AD12" s="696"/>
     </row>
     <row r="13" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C13" s="727"/>
-      <c r="G13" s="691"/>
-      <c r="K13" s="709"/>
-      <c r="L13" s="725"/>
+      <c r="C13" s="688"/>
+      <c r="G13" s="723"/>
+      <c r="K13" s="702"/>
+      <c r="L13" s="718"/>
       <c r="M13" s="47"/>
-      <c r="Q13" s="693" t="s">
+      <c r="Q13" s="725" t="s">
         <v>210</v>
       </c>
-      <c r="R13" s="619"/>
+      <c r="R13" s="622"/>
       <c r="S13" s="552"/>
       <c r="T13" s="6"/>
       <c r="U13" s="96" t="s">
@@ -13452,17 +13482,17 @@
       <c r="X13" s="2" t="s">
         <v>123</v>
       </c>
-      <c r="AA13" s="715"/>
-      <c r="AB13" s="716"/>
-      <c r="AD13" s="703"/>
+      <c r="AA13" s="708"/>
+      <c r="AB13" s="709"/>
+      <c r="AD13" s="696"/>
     </row>
     <row r="14" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B14" s="2" t="s">
         <v>339</v>
       </c>
-      <c r="C14" s="729"/>
+      <c r="C14" s="690"/>
       <c r="D14" s="23"/>
-      <c r="G14" s="691"/>
+      <c r="G14" s="723"/>
       <c r="H14" s="125"/>
       <c r="I14" s="99" t="s">
         <v>44</v>
@@ -13470,8 +13500,8 @@
       <c r="J14" s="111">
         <v>115</v>
       </c>
-      <c r="K14" s="709"/>
-      <c r="L14" s="725"/>
+      <c r="K14" s="702"/>
+      <c r="L14" s="718"/>
       <c r="M14" s="21" t="s">
         <v>111</v>
       </c>
@@ -13492,9 +13522,9 @@
       <c r="Y14" s="21" t="s">
         <v>73</v>
       </c>
-      <c r="AA14" s="715"/>
-      <c r="AB14" s="716"/>
-      <c r="AD14" s="703"/>
+      <c r="AA14" s="708"/>
+      <c r="AB14" s="709"/>
+      <c r="AD14" s="696"/>
     </row>
     <row r="15" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C15" s="130" t="s">
@@ -13509,19 +13539,19 @@
       <c r="F15" s="66" t="s">
         <v>94</v>
       </c>
-      <c r="G15" s="691"/>
+      <c r="G15" s="723"/>
       <c r="H15" s="2" t="s">
         <v>81</v>
       </c>
       <c r="I15" s="53" t="s">
         <v>81</v>
       </c>
-      <c r="K15" s="709"/>
-      <c r="L15" s="726"/>
-      <c r="Q15" s="693" t="s">
+      <c r="K15" s="702"/>
+      <c r="L15" s="719"/>
+      <c r="Q15" s="725" t="s">
         <v>211</v>
       </c>
-      <c r="R15" s="619"/>
+      <c r="R15" s="622"/>
       <c r="S15" s="552"/>
       <c r="T15" s="6"/>
       <c r="V15" s="68" t="s">
@@ -13530,14 +13560,14 @@
       <c r="X15" s="2" t="s">
         <v>128</v>
       </c>
-      <c r="AA15" s="715"/>
-      <c r="AB15" s="716"/>
-      <c r="AD15" s="703"/>
+      <c r="AA15" s="708"/>
+      <c r="AB15" s="709"/>
+      <c r="AD15" s="696"/>
     </row>
     <row r="16" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C16" s="132"/>
-      <c r="G16" s="691"/>
-      <c r="K16" s="709"/>
+      <c r="G16" s="723"/>
+      <c r="K16" s="702"/>
       <c r="N16" s="47"/>
       <c r="O16" s="61" t="s">
         <v>109</v>
@@ -13556,24 +13586,24 @@
       <c r="Z16" s="76" t="s">
         <v>127</v>
       </c>
-      <c r="AA16" s="715"/>
-      <c r="AB16" s="716"/>
-      <c r="AD16" s="703"/>
+      <c r="AA16" s="708"/>
+      <c r="AB16" s="709"/>
+      <c r="AD16" s="696"/>
     </row>
     <row r="17" spans="3:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C17" s="109"/>
       <c r="E17" s="6" t="s">
         <v>95</v>
       </c>
-      <c r="F17" s="688" t="s">
+      <c r="F17" s="720" t="s">
         <v>96</v>
       </c>
-      <c r="G17" s="691"/>
+      <c r="G17" s="723"/>
       <c r="H17" s="54"/>
       <c r="I17" s="133" t="s">
         <v>81</v>
       </c>
-      <c r="K17" s="709"/>
+      <c r="K17" s="702"/>
       <c r="S17" s="552"/>
       <c r="V17" s="68" t="s">
         <v>44</v>
@@ -13581,9 +13611,9 @@
       <c r="X17" s="2" t="s">
         <v>118</v>
       </c>
-      <c r="AA17" s="715"/>
-      <c r="AB17" s="716"/>
-      <c r="AD17" s="703"/>
+      <c r="AA17" s="708"/>
+      <c r="AB17" s="709"/>
+      <c r="AD17" s="696"/>
     </row>
     <row r="18" spans="3:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C18" s="130"/>
@@ -13593,15 +13623,15 @@
       <c r="E18" s="6" t="s">
         <v>97</v>
       </c>
-      <c r="F18" s="689"/>
-      <c r="G18" s="691"/>
+      <c r="F18" s="721"/>
+      <c r="G18" s="723"/>
       <c r="H18" s="108" t="s">
         <v>76</v>
       </c>
       <c r="I18" s="21" t="s">
         <v>81</v>
       </c>
-      <c r="K18" s="709"/>
+      <c r="K18" s="702"/>
       <c r="O18" s="64" t="s">
         <v>115</v>
       </c>
@@ -13612,39 +13642,42 @@
       <c r="X18" s="2" t="s">
         <v>117</v>
       </c>
-      <c r="AA18" s="717"/>
-      <c r="AB18" s="718"/>
-      <c r="AD18" s="703"/>
+      <c r="AA18" s="710"/>
+      <c r="AB18" s="711"/>
+      <c r="AD18" s="696"/>
     </row>
     <row r="19" spans="3:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="F19" s="64" t="s">
         <v>209</v>
       </c>
-      <c r="G19" s="692"/>
-      <c r="K19" s="710"/>
+      <c r="G19" s="724"/>
+      <c r="K19" s="703"/>
       <c r="Q19" s="68" t="s">
         <v>44</v>
       </c>
-      <c r="R19" s="697" t="s">
+      <c r="R19" s="729" t="s">
         <v>124</v>
       </c>
-      <c r="S19" s="698"/>
-      <c r="T19" s="699"/>
+      <c r="S19" s="730"/>
+      <c r="T19" s="731"/>
       <c r="V19" s="77" t="s">
         <v>115</v>
       </c>
       <c r="Y19" s="19" t="s">
         <v>125</v>
       </c>
-      <c r="AD19" s="704"/>
+      <c r="AD19" s="697"/>
     </row>
   </sheetData>
   <mergeCells count="24">
-    <mergeCell ref="C9:C11"/>
-    <mergeCell ref="C13:C14"/>
-    <mergeCell ref="V2:W2"/>
-    <mergeCell ref="M10:AC10"/>
-    <mergeCell ref="F2:F3"/>
+    <mergeCell ref="F17:F18"/>
+    <mergeCell ref="G2:G19"/>
+    <mergeCell ref="Q13:R13"/>
+    <mergeCell ref="Q15:R15"/>
+    <mergeCell ref="L9:N9"/>
+    <mergeCell ref="R19:T19"/>
+    <mergeCell ref="S12:S18"/>
+    <mergeCell ref="O3:O9"/>
     <mergeCell ref="AD1:AD19"/>
     <mergeCell ref="S8:AC8"/>
     <mergeCell ref="K5:K19"/>
@@ -13656,14 +13689,11 @@
     <mergeCell ref="P3:Q3"/>
     <mergeCell ref="L4:L8"/>
     <mergeCell ref="L12:L15"/>
-    <mergeCell ref="F17:F18"/>
-    <mergeCell ref="G2:G19"/>
-    <mergeCell ref="Q13:R13"/>
-    <mergeCell ref="Q15:R15"/>
-    <mergeCell ref="L9:N9"/>
-    <mergeCell ref="R19:T19"/>
-    <mergeCell ref="S12:S18"/>
-    <mergeCell ref="O3:O9"/>
+    <mergeCell ref="C9:C11"/>
+    <mergeCell ref="C13:C14"/>
+    <mergeCell ref="V2:W2"/>
+    <mergeCell ref="M10:AC10"/>
+    <mergeCell ref="F2:F3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Rw Usage Error Resolved
Rw Usage Error Resolved
</commit_message>
<xml_diff>
--- a/System_2.1.5.xlsx
+++ b/System_2.1.5.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Work\Work_For_\Work\Running AppS\System_Work_RW\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0EBD1751-D9A9-4DE6-8DAF-9F1C6D5B8AE1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4569098-7FAE-41E1-8561-514C4ED0CAD2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="BoardRW" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1080" uniqueCount="611">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1082" uniqueCount="613">
   <si>
     <t>Zone</t>
   </si>
@@ -1872,6 +1872,12 @@
   </si>
   <si>
     <t xml:space="preserve">Boat Node </t>
+  </si>
+  <si>
+    <t>Data</t>
+  </si>
+  <si>
+    <t>2 GB</t>
   </si>
 </sst>
 </file>
@@ -4761,6 +4767,21 @@
     <xf numFmtId="0" fontId="29" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="53" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="53" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="75" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="53" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="53" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -5324,21 +5345,6 @@
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="53" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="53" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="75" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="53" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="53" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -5631,8 +5637,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B1:W28"/>
   <sheetViews>
-    <sheetView topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="V15" sqref="V15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="W6" sqref="W6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5685,10 +5691,10 @@
       <c r="I2" s="415" t="s">
         <v>6</v>
       </c>
-      <c r="J2" s="554" t="s">
+      <c r="J2" s="559" t="s">
         <v>7</v>
       </c>
-      <c r="K2" s="555"/>
+      <c r="K2" s="560"/>
       <c r="L2" s="1" t="s">
         <v>8</v>
       </c>
@@ -5698,14 +5704,14 @@
       <c r="N2" s="361" t="s">
         <v>10</v>
       </c>
-      <c r="O2" s="556" t="s">
+      <c r="O2" s="561" t="s">
         <v>384</v>
       </c>
-      <c r="P2" s="557"/>
-      <c r="Q2" s="558"/>
-      <c r="R2" s="558"/>
-      <c r="S2" s="558"/>
-      <c r="T2" s="559" t="s">
+      <c r="P2" s="562"/>
+      <c r="Q2" s="563"/>
+      <c r="R2" s="563"/>
+      <c r="S2" s="563"/>
+      <c r="T2" s="564" t="s">
         <v>385</v>
       </c>
       <c r="V2" s="2" t="s">
@@ -5719,7 +5725,7 @@
       <c r="C3" s="168" t="s">
         <v>11</v>
       </c>
-      <c r="D3" s="551"/>
+      <c r="D3" s="556"/>
       <c r="E3" s="349"/>
       <c r="F3" s="271" t="s">
         <v>69</v>
@@ -5755,7 +5761,7 @@
       <c r="S3" s="176">
         <v>0</v>
       </c>
-      <c r="T3" s="560"/>
+      <c r="T3" s="565"/>
       <c r="U3" s="19" t="s">
         <v>590</v>
       </c>
@@ -5771,7 +5777,7 @@
       <c r="C4" s="168" t="s">
         <v>361</v>
       </c>
-      <c r="D4" s="552"/>
+      <c r="D4" s="557"/>
       <c r="E4" s="61"/>
       <c r="F4" s="371" t="s">
         <v>42</v>
@@ -5789,7 +5795,7 @@
       <c r="O4" s="6"/>
       <c r="P4" s="321"/>
       <c r="S4" s="6"/>
-      <c r="T4" s="560"/>
+      <c r="T4" s="565"/>
     </row>
     <row r="5" spans="2:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B5" s="2" t="s">
@@ -5798,7 +5804,7 @@
       <c r="C5" s="168" t="s">
         <v>16</v>
       </c>
-      <c r="D5" s="553"/>
+      <c r="D5" s="558"/>
       <c r="F5" s="375" t="s">
         <v>42</v>
       </c>
@@ -5817,12 +5823,12 @@
         <v>521</v>
       </c>
       <c r="P5" s="504"/>
-      <c r="T5" s="560"/>
+      <c r="T5" s="565"/>
       <c r="U5" s="209" t="s">
         <v>228</v>
       </c>
       <c r="V5" s="19">
-        <v>5760</v>
+        <v>5940</v>
       </c>
     </row>
     <row r="6" spans="2:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -5856,7 +5862,7 @@
       <c r="P6" s="504"/>
       <c r="Q6" s="16"/>
       <c r="R6" s="6"/>
-      <c r="T6" s="560"/>
+      <c r="T6" s="565"/>
     </row>
     <row r="7" spans="2:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B7" s="214" t="s">
@@ -5887,7 +5893,7 @@
       <c r="P7" s="504"/>
       <c r="Q7" s="16"/>
       <c r="R7" s="6"/>
-      <c r="T7" s="560"/>
+      <c r="T7" s="565"/>
     </row>
     <row r="8" spans="2:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B8" s="2" t="s">
@@ -5916,7 +5922,7 @@
       <c r="P8" s="504"/>
       <c r="Q8" s="16"/>
       <c r="R8" s="6"/>
-      <c r="T8" s="560"/>
+      <c r="T8" s="565"/>
     </row>
     <row r="9" spans="2:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B9" s="3" t="s">
@@ -5950,7 +5956,7 @@
         <v>44</v>
       </c>
       <c r="P9" s="504"/>
-      <c r="T9" s="560"/>
+      <c r="T9" s="565"/>
     </row>
     <row r="10" spans="2:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B10" s="2" t="s">
@@ -5980,7 +5986,7 @@
         <v>521</v>
       </c>
       <c r="P10" s="504"/>
-      <c r="T10" s="560"/>
+      <c r="T10" s="565"/>
     </row>
     <row r="11" spans="2:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B11" s="2" t="s">
@@ -6015,12 +6021,12 @@
       <c r="P11" s="504"/>
       <c r="Q11" s="16"/>
       <c r="R11" s="142"/>
-      <c r="T11" s="560"/>
+      <c r="T11" s="565"/>
       <c r="U11" s="209" t="s">
         <v>227</v>
       </c>
       <c r="V11" s="64">
-        <v>96</v>
+        <v>99</v>
       </c>
     </row>
     <row r="12" spans="2:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -6048,7 +6054,7 @@
       <c r="P12" s="504"/>
       <c r="Q12" s="16"/>
       <c r="R12" s="142"/>
-      <c r="T12" s="560"/>
+      <c r="T12" s="565"/>
     </row>
     <row r="13" spans="2:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B13" s="261" t="s">
@@ -6083,11 +6089,17 @@
         <v>521</v>
       </c>
       <c r="P13" s="504"/>
-      <c r="T13" s="560"/>
+      <c r="T13" s="565"/>
+      <c r="U13" s="2" t="s">
+        <v>611</v>
+      </c>
+      <c r="V13" s="24" t="s">
+        <v>612</v>
+      </c>
     </row>
     <row r="14" spans="2:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="P14" s="504"/>
-      <c r="T14" s="560"/>
+      <c r="T14" s="565"/>
     </row>
     <row r="15" spans="2:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B15" s="2" t="s">
@@ -6113,10 +6125,10 @@
       <c r="L15" s="137" t="s">
         <v>15</v>
       </c>
-      <c r="M15" s="548">
+      <c r="M15" s="553">
         <v>45275</v>
       </c>
-      <c r="N15" s="551" t="s">
+      <c r="N15" s="556" t="s">
         <v>22</v>
       </c>
       <c r="O15" s="502" t="s">
@@ -6124,7 +6136,7 @@
       </c>
       <c r="P15" s="504"/>
       <c r="S15" s="6"/>
-      <c r="T15" s="560"/>
+      <c r="T15" s="565"/>
     </row>
     <row r="16" spans="2:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B16" s="486" t="s">
@@ -6150,10 +6162,10 @@
       <c r="L16" s="199" t="s">
         <v>15</v>
       </c>
-      <c r="M16" s="549"/>
-      <c r="N16" s="552"/>
+      <c r="M16" s="554"/>
+      <c r="N16" s="557"/>
       <c r="P16" s="504"/>
-      <c r="T16" s="560"/>
+      <c r="T16" s="565"/>
     </row>
     <row r="17" spans="2:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B17" s="2" t="s">
@@ -6181,8 +6193,8 @@
       <c r="L17" s="135" t="s">
         <v>15</v>
       </c>
-      <c r="M17" s="550"/>
-      <c r="N17" s="553"/>
+      <c r="M17" s="555"/>
+      <c r="N17" s="558"/>
       <c r="O17" s="502" t="s">
         <v>44</v>
       </c>
@@ -6198,11 +6210,11 @@
       <c r="S17" s="176">
         <v>1</v>
       </c>
-      <c r="T17" s="560"/>
+      <c r="T17" s="565"/>
     </row>
     <row r="18" spans="2:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="P18" s="504"/>
-      <c r="T18" s="560"/>
+      <c r="T18" s="565"/>
     </row>
     <row r="19" spans="2:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B19" s="2" t="s">
@@ -6230,14 +6242,14 @@
       <c r="L19" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="M19" s="548">
+      <c r="M19" s="553">
         <v>45275</v>
       </c>
       <c r="N19" s="414" t="s">
         <v>521</v>
       </c>
       <c r="P19" s="504"/>
-      <c r="T19" s="560"/>
+      <c r="T19" s="565"/>
     </row>
     <row r="20" spans="2:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B20" s="246" t="s">
@@ -6263,12 +6275,12 @@
       <c r="L20" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="M20" s="549"/>
+      <c r="M20" s="554"/>
       <c r="N20" s="404" t="s">
         <v>26</v>
       </c>
       <c r="P20" s="504"/>
-      <c r="T20" s="560"/>
+      <c r="T20" s="565"/>
     </row>
     <row r="21" spans="2:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B21" s="246" t="s">
@@ -6294,16 +6306,16 @@
       <c r="L21" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="M21" s="549"/>
+      <c r="M21" s="554"/>
       <c r="N21" s="404" t="s">
         <v>18</v>
       </c>
       <c r="P21" s="504"/>
-      <c r="T21" s="560"/>
-      <c r="U21" s="546" t="s">
+      <c r="T21" s="565"/>
+      <c r="U21" s="551" t="s">
         <v>226</v>
       </c>
-      <c r="V21" s="547"/>
+      <c r="V21" s="552"/>
     </row>
     <row r="22" spans="2:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B22" s="276" t="s">
@@ -6329,12 +6341,12 @@
       <c r="L22" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="M22" s="549"/>
+      <c r="M22" s="554"/>
       <c r="N22" s="384" t="s">
         <v>26</v>
       </c>
       <c r="P22" s="504"/>
-      <c r="T22" s="560"/>
+      <c r="T22" s="565"/>
     </row>
     <row r="23" spans="2:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B23" s="2" t="s">
@@ -6360,12 +6372,12 @@
       <c r="L23" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="M23" s="549"/>
+      <c r="M23" s="554"/>
       <c r="N23" s="61" t="s">
         <v>522</v>
       </c>
       <c r="P23" s="504"/>
-      <c r="T23" s="560"/>
+      <c r="T23" s="565"/>
     </row>
     <row r="24" spans="2:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B24" s="3" t="s">
@@ -6391,7 +6403,7 @@
       <c r="L24" s="135" t="s">
         <v>32</v>
       </c>
-      <c r="M24" s="549"/>
+      <c r="M24" s="554"/>
       <c r="N24" s="61" t="s">
         <v>26</v>
       </c>
@@ -6400,7 +6412,7 @@
       </c>
       <c r="P24" s="505"/>
       <c r="S24" s="16"/>
-      <c r="T24" s="560"/>
+      <c r="T24" s="565"/>
     </row>
     <row r="25" spans="2:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B25" s="3" t="s">
@@ -6428,7 +6440,7 @@
       <c r="L25" s="135" t="s">
         <v>35</v>
       </c>
-      <c r="M25" s="549"/>
+      <c r="M25" s="554"/>
       <c r="N25" s="61" t="s">
         <v>26</v>
       </c>
@@ -6444,7 +6456,7 @@
       <c r="S25" s="21">
         <v>1</v>
       </c>
-      <c r="T25" s="560"/>
+      <c r="T25" s="565"/>
       <c r="V25" s="23" t="s">
         <v>605</v>
       </c>
@@ -6473,12 +6485,12 @@
       <c r="L26" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="M26" s="549"/>
+      <c r="M26" s="554"/>
       <c r="N26" s="61" t="s">
         <v>523</v>
       </c>
       <c r="P26" s="504"/>
-      <c r="T26" s="560"/>
+      <c r="T26" s="565"/>
       <c r="W26" s="2" t="s">
         <v>606</v>
       </c>
@@ -6503,7 +6515,7 @@
       <c r="J27" s="411"/>
       <c r="K27" s="412"/>
       <c r="L27" s="413"/>
-      <c r="M27" s="549"/>
+      <c r="M27" s="554"/>
       <c r="N27" s="61"/>
       <c r="P27" s="321">
         <v>1</v>
@@ -6517,7 +6529,7 @@
       <c r="S27" s="176">
         <v>1</v>
       </c>
-      <c r="T27" s="560"/>
+      <c r="T27" s="565"/>
       <c r="W27" s="2" t="s">
         <v>607</v>
       </c>
@@ -6548,7 +6560,7 @@
       <c r="L28" s="11" t="s">
         <v>37</v>
       </c>
-      <c r="M28" s="550"/>
+      <c r="M28" s="555"/>
       <c r="N28" s="61" t="s">
         <v>523</v>
       </c>
@@ -6564,7 +6576,7 @@
       <c r="S28" s="21">
         <v>1</v>
       </c>
-      <c r="T28" s="561"/>
+      <c r="T28" s="566"/>
     </row>
   </sheetData>
   <mergeCells count="8">
@@ -6643,7 +6655,7 @@
       <c r="P1" s="422" t="s">
         <v>407</v>
       </c>
-      <c r="Q1" s="562" t="s">
+      <c r="Q1" s="567" t="s">
         <v>181</v>
       </c>
       <c r="R1" s="100" t="s">
@@ -6663,32 +6675,32 @@
       </c>
     </row>
     <row r="2" spans="1:27" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="575">
+      <c r="A2" s="580">
         <f ca="1">TODAY()</f>
         <v>45279</v>
       </c>
-      <c r="B2" s="577" t="s">
+      <c r="B2" s="582" t="s">
         <v>388</v>
       </c>
-      <c r="C2" s="589" t="s">
+      <c r="C2" s="594" t="s">
         <v>364</v>
       </c>
-      <c r="D2" s="579" t="s">
+      <c r="D2" s="584" t="s">
         <v>103</v>
       </c>
-      <c r="E2" s="581" t="s">
+      <c r="E2" s="586" t="s">
         <v>65</v>
       </c>
       <c r="F2" s="196" t="s">
         <v>220</v>
       </c>
-      <c r="G2" s="587" t="s">
+      <c r="G2" s="592" t="s">
         <v>380</v>
       </c>
       <c r="H2" s="211" t="s">
         <v>220</v>
       </c>
-      <c r="I2" s="569" t="s">
+      <c r="I2" s="574" t="s">
         <v>103</v>
       </c>
       <c r="J2" s="420" t="s">
@@ -6712,7 +6724,7 @@
       <c r="P2" s="423">
         <v>40</v>
       </c>
-      <c r="Q2" s="563"/>
+      <c r="Q2" s="568"/>
       <c r="R2" s="21">
         <f>R7+R18</f>
         <v>6</v>
@@ -6738,14 +6750,14 @@
       </c>
     </row>
     <row r="3" spans="1:27" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="576"/>
-      <c r="B3" s="578"/>
-      <c r="C3" s="590"/>
-      <c r="D3" s="580"/>
-      <c r="E3" s="582"/>
-      <c r="G3" s="588"/>
+      <c r="A3" s="581"/>
+      <c r="B3" s="583"/>
+      <c r="C3" s="595"/>
+      <c r="D3" s="585"/>
+      <c r="E3" s="587"/>
+      <c r="G3" s="593"/>
       <c r="H3" s="6"/>
-      <c r="I3" s="570"/>
+      <c r="I3" s="575"/>
       <c r="K3" s="24">
         <v>2</v>
       </c>
@@ -6770,10 +6782,10 @@
         <v>389</v>
       </c>
       <c r="B4" s="248"/>
-      <c r="C4" s="583" t="s">
+      <c r="C4" s="588" t="s">
         <v>178</v>
       </c>
-      <c r="I4" s="570"/>
+      <c r="I4" s="575"/>
       <c r="R4" s="498" t="s">
         <v>579</v>
       </c>
@@ -6797,7 +6809,7 @@
       <c r="B5" s="100" t="s">
         <v>364</v>
       </c>
-      <c r="C5" s="584"/>
+      <c r="C5" s="589"/>
       <c r="D5" s="227" t="s">
         <v>103</v>
       </c>
@@ -6807,13 +6819,13 @@
       <c r="F5" s="211" t="s">
         <v>220</v>
       </c>
-      <c r="G5" s="551" t="s">
+      <c r="G5" s="556" t="s">
         <v>276</v>
       </c>
       <c r="H5" s="211" t="s">
         <v>220</v>
       </c>
-      <c r="I5" s="570"/>
+      <c r="I5" s="575"/>
       <c r="J5" s="421" t="s">
         <v>273</v>
       </c>
@@ -6844,22 +6856,22 @@
       <c r="X5" s="494"/>
     </row>
     <row r="6" spans="1:27" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="572" t="s">
+      <c r="A6" s="577" t="s">
         <v>290</v>
       </c>
       <c r="B6" s="105" t="s">
         <v>199</v>
       </c>
-      <c r="C6" s="585"/>
-      <c r="D6" s="586"/>
+      <c r="C6" s="590"/>
+      <c r="D6" s="591"/>
       <c r="E6" s="96">
         <v>1</v>
       </c>
-      <c r="G6" s="552"/>
-      <c r="I6" s="570"/>
+      <c r="G6" s="557"/>
+      <c r="I6" s="575"/>
     </row>
     <row r="7" spans="1:27" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="573"/>
+      <c r="A7" s="578"/>
       <c r="B7" s="100" t="s">
         <v>155</v>
       </c>
@@ -6869,8 +6881,8 @@
       <c r="D7" s="30" t="s">
         <v>136</v>
       </c>
-      <c r="G7" s="552"/>
-      <c r="I7" s="570"/>
+      <c r="G7" s="557"/>
+      <c r="I7" s="575"/>
       <c r="M7" s="16" t="s">
         <v>354</v>
       </c>
@@ -6906,7 +6918,7 @@
       </c>
     </row>
     <row r="8" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="574"/>
+      <c r="A8" s="579"/>
       <c r="B8" s="217" t="s">
         <v>28</v>
       </c>
@@ -6914,8 +6926,8 @@
       <c r="E8" s="30">
         <v>3</v>
       </c>
-      <c r="G8" s="552"/>
-      <c r="I8" s="570"/>
+      <c r="G8" s="557"/>
+      <c r="I8" s="575"/>
       <c r="N8" s="80"/>
       <c r="U8" s="6" t="s">
         <v>465</v>
@@ -6937,9 +6949,9 @@
       <c r="D9" s="2" t="s">
         <v>142</v>
       </c>
-      <c r="G9" s="552"/>
+      <c r="G9" s="557"/>
       <c r="H9" s="6"/>
-      <c r="I9" s="570"/>
+      <c r="I9" s="575"/>
       <c r="M9" s="19" t="s">
         <v>546</v>
       </c>
@@ -6965,8 +6977,8 @@
         <f>Boat!U8</f>
         <v>41</v>
       </c>
-      <c r="G10" s="552"/>
-      <c r="I10" s="570"/>
+      <c r="G10" s="557"/>
+      <c r="I10" s="575"/>
       <c r="J10" s="24" t="s">
         <v>380</v>
       </c>
@@ -6990,7 +7002,7 @@
       <c r="A11" s="99" t="s">
         <v>184</v>
       </c>
-      <c r="B11" s="551" t="s">
+      <c r="B11" s="556" t="s">
         <v>391</v>
       </c>
       <c r="C11" s="175" t="s">
@@ -6999,8 +7011,8 @@
       <c r="D11" s="222" t="s">
         <v>270</v>
       </c>
-      <c r="G11" s="552"/>
-      <c r="I11" s="570"/>
+      <c r="G11" s="557"/>
+      <c r="I11" s="575"/>
       <c r="J11" s="24" t="s">
         <v>195</v>
       </c>
@@ -7026,23 +7038,23 @@
       <c r="S11" s="24">
         <v>1</v>
       </c>
-      <c r="U11" s="564" t="s">
+      <c r="U11" s="569" t="s">
         <v>582</v>
       </c>
-      <c r="V11" s="565"/>
-      <c r="W11" s="565"/>
-      <c r="X11" s="566"/>
+      <c r="V11" s="570"/>
+      <c r="W11" s="570"/>
+      <c r="X11" s="571"/>
     </row>
     <row r="12" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="232" t="s">
         <v>392</v>
       </c>
-      <c r="B12" s="553"/>
+      <c r="B12" s="558"/>
       <c r="E12" s="234">
         <v>3</v>
       </c>
-      <c r="G12" s="552"/>
-      <c r="I12" s="570"/>
+      <c r="G12" s="557"/>
+      <c r="I12" s="575"/>
       <c r="J12" s="24" t="s">
         <v>537</v>
       </c>
@@ -7070,12 +7082,12 @@
       <c r="B13" s="221" t="s">
         <v>330</v>
       </c>
-      <c r="C13" s="551" t="s">
+      <c r="C13" s="556" t="s">
         <v>195</v>
       </c>
       <c r="D13" s="20"/>
-      <c r="G13" s="552"/>
-      <c r="I13" s="570"/>
+      <c r="G13" s="557"/>
+      <c r="I13" s="575"/>
       <c r="J13" s="108" t="s">
         <v>571</v>
       </c>
@@ -7102,7 +7114,7 @@
       <c r="B14" s="177" t="s">
         <v>150</v>
       </c>
-      <c r="C14" s="553"/>
+      <c r="C14" s="558"/>
       <c r="D14" s="209" t="s">
         <v>154</v>
       </c>
@@ -7112,11 +7124,11 @@
       <c r="F14" s="211" t="s">
         <v>220</v>
       </c>
-      <c r="G14" s="553"/>
+      <c r="G14" s="558"/>
       <c r="H14" s="211" t="s">
         <v>220</v>
       </c>
-      <c r="I14" s="570"/>
+      <c r="I14" s="575"/>
       <c r="U14" s="6"/>
       <c r="V14" s="112"/>
       <c r="W14" s="6"/>
@@ -7134,7 +7146,7 @@
       <c r="H15" s="277">
         <v>0</v>
       </c>
-      <c r="I15" s="570"/>
+      <c r="I15" s="575"/>
       <c r="J15" s="108" t="s">
         <v>154</v>
       </c>
@@ -7165,7 +7177,7 @@
       <c r="D16" s="2" t="s">
         <v>509</v>
       </c>
-      <c r="I16" s="570"/>
+      <c r="I16" s="575"/>
       <c r="K16" s="100" t="s">
         <v>44</v>
       </c>
@@ -7199,7 +7211,7 @@
       <c r="G17" s="2" t="s">
         <v>440</v>
       </c>
-      <c r="I17" s="570"/>
+      <c r="I17" s="575"/>
       <c r="L17" s="2" t="s">
         <v>443</v>
       </c>
@@ -7211,13 +7223,13 @@
     </row>
     <row r="18" spans="1:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="G18" s="16"/>
-      <c r="I18" s="570"/>
+      <c r="I18" s="575"/>
       <c r="L18" s="16"/>
       <c r="M18" s="21"/>
-      <c r="O18" s="567" t="s">
+      <c r="O18" s="572" t="s">
         <v>538</v>
       </c>
-      <c r="P18" s="568"/>
+      <c r="P18" s="573"/>
       <c r="Q18" s="127" t="s">
         <v>44</v>
       </c>
@@ -7243,7 +7255,7 @@
       </c>
     </row>
     <row r="19" spans="1:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="I19" s="570"/>
+      <c r="I19" s="575"/>
       <c r="M19" s="21" t="s">
         <v>442</v>
       </c>
@@ -7275,7 +7287,7 @@
       <c r="G20" s="2" t="s">
         <v>440</v>
       </c>
-      <c r="I20" s="570"/>
+      <c r="I20" s="575"/>
       <c r="K20" s="19" t="s">
         <v>439</v>
       </c>
@@ -7300,7 +7312,7 @@
       <c r="Z20" s="112"/>
     </row>
     <row r="21" spans="1:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="I21" s="570"/>
+      <c r="I21" s="575"/>
       <c r="M21" s="221" t="s">
         <v>421</v>
       </c>
@@ -7336,7 +7348,7 @@
       <c r="G22" s="2" t="s">
         <v>440</v>
       </c>
-      <c r="I22" s="570"/>
+      <c r="I22" s="575"/>
       <c r="U22" s="6"/>
       <c r="V22" s="494"/>
       <c r="W22" s="6" t="s">
@@ -7356,13 +7368,13 @@
       <c r="E23" s="289" t="s">
         <v>44</v>
       </c>
-      <c r="I23" s="570"/>
+      <c r="I23" s="575"/>
       <c r="U23" s="6"/>
       <c r="V23" s="24"/>
       <c r="W23" s="6"/>
     </row>
     <row r="24" spans="1:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="I24" s="570"/>
+      <c r="I24" s="575"/>
       <c r="U24" s="354"/>
       <c r="V24" s="497">
         <v>0</v>
@@ -7390,7 +7402,7 @@
       <c r="H25" s="196" t="s">
         <v>271</v>
       </c>
-      <c r="I25" s="570"/>
+      <c r="I25" s="575"/>
       <c r="J25" s="421" t="s">
         <v>274</v>
       </c>
@@ -7435,7 +7447,7 @@
       <c r="H26" s="19" t="s">
         <v>220</v>
       </c>
-      <c r="I26" s="570"/>
+      <c r="I26" s="575"/>
       <c r="K26" s="24">
         <v>15</v>
       </c>
@@ -7470,7 +7482,7 @@
       </c>
     </row>
     <row r="27" spans="1:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="I27" s="570"/>
+      <c r="I27" s="575"/>
       <c r="O27" s="2" t="s">
         <v>99</v>
       </c>
@@ -7497,7 +7509,7 @@
       <c r="E28" s="220">
         <v>2</v>
       </c>
-      <c r="I28" s="570"/>
+      <c r="I28" s="575"/>
       <c r="Q28" s="6"/>
       <c r="R28" s="112"/>
       <c r="T28" s="142"/>
@@ -7519,7 +7531,7 @@
       <c r="H29" s="196" t="s">
         <v>272</v>
       </c>
-      <c r="I29" s="571"/>
+      <c r="I29" s="576"/>
       <c r="J29" s="333"/>
       <c r="L29" s="96" t="s">
         <v>278</v>
@@ -7680,7 +7692,7 @@
       <c r="H1" s="97" t="s">
         <v>350</v>
       </c>
-      <c r="I1" s="587" t="s">
+      <c r="I1" s="592" t="s">
         <v>377</v>
       </c>
       <c r="J1" s="2" t="s">
@@ -7716,7 +7728,7 @@
       <c r="X1" s="454" t="s">
         <v>156</v>
       </c>
-      <c r="Y1" s="633" t="s">
+      <c r="Y1" s="638" t="s">
         <v>550</v>
       </c>
       <c r="Z1" s="430">
@@ -7741,7 +7753,7 @@
         <v>516</v>
       </c>
       <c r="AM1" s="426"/>
-      <c r="AN1" s="618"/>
+      <c r="AN1" s="623"/>
       <c r="AO1" s="350" t="s">
         <v>486</v>
       </c>
@@ -7750,23 +7762,23 @@
       </c>
     </row>
     <row r="2" spans="1:43" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="642">
+      <c r="A2" s="647">
         <f ca="1">TODAY()</f>
         <v>45279</v>
       </c>
-      <c r="B2" s="644" t="s">
+      <c r="B2" s="649" t="s">
         <v>378</v>
       </c>
-      <c r="C2" s="589" t="s">
+      <c r="C2" s="594" t="s">
         <v>364</v>
       </c>
-      <c r="D2" s="646" t="s">
+      <c r="D2" s="651" t="s">
         <v>362</v>
       </c>
-      <c r="E2" s="591" t="s">
+      <c r="E2" s="596" t="s">
         <v>65</v>
       </c>
-      <c r="F2" s="599" t="s">
+      <c r="F2" s="604" t="s">
         <v>103</v>
       </c>
       <c r="G2" s="417" t="s">
@@ -7775,31 +7787,31 @@
       <c r="H2" s="80" t="s">
         <v>33</v>
       </c>
-      <c r="I2" s="588"/>
+      <c r="I2" s="593"/>
       <c r="J2" s="81" t="s">
         <v>77</v>
       </c>
-      <c r="K2" s="593" t="s">
+      <c r="K2" s="598" t="s">
         <v>349</v>
       </c>
-      <c r="L2" s="594"/>
-      <c r="M2" s="599" t="s">
+      <c r="L2" s="599"/>
+      <c r="M2" s="604" t="s">
         <v>103</v>
       </c>
       <c r="N2" s="69" t="s">
         <v>28</v>
       </c>
-      <c r="O2" s="625" t="s">
+      <c r="O2" s="630" t="s">
         <v>103</v>
       </c>
       <c r="P2" s="85" t="s">
         <v>148</v>
       </c>
-      <c r="Q2" s="589" t="s">
+      <c r="Q2" s="594" t="s">
         <v>144</v>
       </c>
-      <c r="R2" s="551"/>
-      <c r="S2" s="612" t="s">
+      <c r="R2" s="556"/>
+      <c r="S2" s="617" t="s">
         <v>149</v>
       </c>
       <c r="T2" s="89"/>
@@ -7809,7 +7821,7 @@
       <c r="X2" s="455" t="s">
         <v>157</v>
       </c>
-      <c r="Y2" s="634"/>
+      <c r="Y2" s="639"/>
       <c r="Z2" s="431">
         <v>1</v>
       </c>
@@ -7832,15 +7844,15 @@
         <v>480</v>
       </c>
       <c r="AM2" s="452"/>
-      <c r="AN2" s="619"/>
+      <c r="AN2" s="624"/>
     </row>
     <row r="3" spans="1:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="643"/>
-      <c r="B3" s="645"/>
-      <c r="C3" s="590"/>
-      <c r="D3" s="647"/>
-      <c r="E3" s="592"/>
-      <c r="F3" s="600"/>
+      <c r="A3" s="648"/>
+      <c r="B3" s="650"/>
+      <c r="C3" s="595"/>
+      <c r="D3" s="652"/>
+      <c r="E3" s="597"/>
+      <c r="F3" s="605"/>
       <c r="G3" s="418" t="s">
         <v>28</v>
       </c>
@@ -7859,17 +7871,17 @@
       <c r="L3" s="206" t="s">
         <v>108</v>
       </c>
-      <c r="M3" s="600"/>
+      <c r="M3" s="605"/>
       <c r="N3" s="69" t="s">
         <v>147</v>
       </c>
-      <c r="O3" s="626"/>
+      <c r="O3" s="631"/>
       <c r="P3" s="2" t="s">
         <v>155</v>
       </c>
-      <c r="Q3" s="590"/>
-      <c r="R3" s="553"/>
-      <c r="S3" s="614"/>
+      <c r="Q3" s="595"/>
+      <c r="R3" s="558"/>
+      <c r="S3" s="619"/>
       <c r="T3" s="89"/>
       <c r="U3" s="124"/>
       <c r="V3" s="120"/>
@@ -7877,7 +7889,7 @@
       <c r="X3" s="455" t="s">
         <v>158</v>
       </c>
-      <c r="Y3" s="634"/>
+      <c r="Y3" s="639"/>
       <c r="Z3" s="432">
         <v>1</v>
       </c>
@@ -7886,7 +7898,7 @@
       <c r="AC3" s="100" t="s">
         <v>497</v>
       </c>
-      <c r="AD3" s="609" t="s">
+      <c r="AD3" s="614" t="s">
         <v>472</v>
       </c>
       <c r="AE3" s="262"/>
@@ -7898,16 +7910,16 @@
       <c r="AK3" s="262"/>
       <c r="AL3" s="16"/>
       <c r="AM3" s="452"/>
-      <c r="AN3" s="619"/>
+      <c r="AN3" s="624"/>
     </row>
     <row r="4" spans="1:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="243" t="s">
         <v>184</v>
       </c>
-      <c r="B4" s="658" t="s">
+      <c r="B4" s="663" t="s">
         <v>381</v>
       </c>
-      <c r="C4" s="589" t="s">
+      <c r="C4" s="594" t="s">
         <v>155</v>
       </c>
       <c r="D4" s="359" t="s">
@@ -7916,7 +7928,7 @@
       <c r="E4" s="396">
         <v>2</v>
       </c>
-      <c r="F4" s="600"/>
+      <c r="F4" s="605"/>
       <c r="G4" s="400" t="s">
         <v>203</v>
       </c>
@@ -7933,11 +7945,11 @@
         <v>151</v>
       </c>
       <c r="L4" s="209"/>
-      <c r="M4" s="600"/>
+      <c r="M4" s="605"/>
       <c r="N4" s="178" t="s">
         <v>70</v>
       </c>
-      <c r="O4" s="626"/>
+      <c r="O4" s="631"/>
       <c r="P4" s="2" t="s">
         <v>192</v>
       </c>
@@ -7959,12 +7971,12 @@
       <c r="X4" s="455" t="s">
         <v>159</v>
       </c>
-      <c r="Y4" s="634"/>
+      <c r="Y4" s="639"/>
       <c r="Z4" s="433"/>
       <c r="AA4" s="313"/>
       <c r="AB4" s="214"/>
       <c r="AC4" s="16"/>
-      <c r="AD4" s="609"/>
+      <c r="AD4" s="614"/>
       <c r="AE4" s="262"/>
       <c r="AF4" s="262"/>
       <c r="AG4" s="16"/>
@@ -7974,37 +7986,37 @@
       <c r="AK4" s="262"/>
       <c r="AL4" s="16"/>
       <c r="AM4" s="452"/>
-      <c r="AN4" s="619"/>
+      <c r="AN4" s="624"/>
       <c r="AO4" s="350" t="s">
         <v>91</v>
       </c>
     </row>
     <row r="5" spans="1:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="587" t="s">
+      <c r="A5" s="592" t="s">
         <v>434</v>
       </c>
-      <c r="B5" s="659"/>
-      <c r="C5" s="590"/>
+      <c r="B5" s="664"/>
+      <c r="C5" s="595"/>
       <c r="D5" s="61" t="s">
         <v>154</v>
       </c>
       <c r="E5" s="397">
         <v>1</v>
       </c>
-      <c r="F5" s="600"/>
-      <c r="G5" s="650" t="s">
+      <c r="F5" s="605"/>
+      <c r="G5" s="655" t="s">
         <v>193</v>
       </c>
-      <c r="H5" s="650"/>
-      <c r="I5" s="650"/>
-      <c r="J5" s="650"/>
-      <c r="K5" s="650"/>
-      <c r="L5" s="651"/>
-      <c r="M5" s="600"/>
+      <c r="H5" s="655"/>
+      <c r="I5" s="655"/>
+      <c r="J5" s="655"/>
+      <c r="K5" s="655"/>
+      <c r="L5" s="656"/>
+      <c r="M5" s="605"/>
       <c r="N5" s="21">
         <v>8</v>
       </c>
-      <c r="O5" s="626"/>
+      <c r="O5" s="631"/>
       <c r="T5" s="89"/>
       <c r="U5" s="124"/>
       <c r="V5" s="120"/>
@@ -8012,7 +8024,7 @@
       <c r="X5" s="455" t="s">
         <v>160</v>
       </c>
-      <c r="Y5" s="634"/>
+      <c r="Y5" s="639"/>
       <c r="Z5" s="433">
         <v>1</v>
       </c>
@@ -8035,24 +8047,24 @@
       <c r="AK5" s="262"/>
       <c r="AL5" s="80"/>
       <c r="AM5" s="452"/>
-      <c r="AN5" s="619"/>
+      <c r="AN5" s="624"/>
     </row>
     <row r="6" spans="1:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="588"/>
-      <c r="B6" s="656" t="s">
+      <c r="A6" s="593"/>
+      <c r="B6" s="661" t="s">
         <v>178</v>
       </c>
-      <c r="C6" s="585"/>
-      <c r="D6" s="586"/>
-      <c r="F6" s="600"/>
-      <c r="G6" s="652"/>
-      <c r="H6" s="652"/>
-      <c r="I6" s="652"/>
-      <c r="J6" s="652"/>
-      <c r="K6" s="652"/>
-      <c r="L6" s="653"/>
-      <c r="M6" s="600"/>
-      <c r="O6" s="626"/>
+      <c r="C6" s="590"/>
+      <c r="D6" s="591"/>
+      <c r="F6" s="605"/>
+      <c r="G6" s="657"/>
+      <c r="H6" s="657"/>
+      <c r="I6" s="657"/>
+      <c r="J6" s="657"/>
+      <c r="K6" s="657"/>
+      <c r="L6" s="658"/>
+      <c r="M6" s="605"/>
+      <c r="O6" s="631"/>
       <c r="T6" s="89"/>
       <c r="U6" s="124"/>
       <c r="V6" s="98" t="s">
@@ -8062,7 +8074,7 @@
       <c r="X6" s="455" t="s">
         <v>161</v>
       </c>
-      <c r="Y6" s="634"/>
+      <c r="Y6" s="639"/>
       <c r="Z6" s="431">
         <v>1</v>
       </c>
@@ -8076,16 +8088,16 @@
       <c r="AF6" s="262"/>
       <c r="AG6" s="262"/>
       <c r="AH6" s="262"/>
-      <c r="AI6" s="608"/>
+      <c r="AI6" s="613"/>
       <c r="AJ6" s="465" t="s">
         <v>475</v>
       </c>
-      <c r="AK6" s="608" t="s">
+      <c r="AK6" s="613" t="s">
         <v>256</v>
       </c>
       <c r="AL6" s="262"/>
       <c r="AM6" s="452"/>
-      <c r="AN6" s="619"/>
+      <c r="AN6" s="624"/>
       <c r="AO6" s="350" t="s">
         <v>487</v>
       </c>
@@ -8094,7 +8106,7 @@
       <c r="A7" s="237" t="s">
         <v>597</v>
       </c>
-      <c r="B7" s="657"/>
+      <c r="B7" s="662"/>
       <c r="C7" s="207" t="s">
         <v>382</v>
       </c>
@@ -8104,7 +8116,7 @@
       <c r="E7" s="271">
         <v>3</v>
       </c>
-      <c r="F7" s="600"/>
+      <c r="F7" s="605"/>
       <c r="G7" s="419">
         <v>0</v>
       </c>
@@ -8117,14 +8129,14 @@
       <c r="J7" s="30">
         <v>0</v>
       </c>
-      <c r="K7" s="551">
+      <c r="K7" s="556">
         <v>0</v>
       </c>
       <c r="L7" s="217">
         <v>0</v>
       </c>
-      <c r="M7" s="600"/>
-      <c r="O7" s="626"/>
+      <c r="M7" s="605"/>
+      <c r="O7" s="631"/>
       <c r="R7" s="99" t="s">
         <v>44</v>
       </c>
@@ -8138,7 +8150,7 @@
       <c r="X7" s="455" t="s">
         <v>162</v>
       </c>
-      <c r="Y7" s="634"/>
+      <c r="Y7" s="639"/>
       <c r="Z7" s="431">
         <v>1</v>
       </c>
@@ -8148,18 +8160,18 @@
       <c r="AD7" s="16"/>
       <c r="AE7" s="262"/>
       <c r="AF7" s="262"/>
-      <c r="AG7" s="609" t="s">
+      <c r="AG7" s="614" t="s">
         <v>471</v>
       </c>
       <c r="AH7" s="262"/>
-      <c r="AI7" s="608"/>
+      <c r="AI7" s="613"/>
       <c r="AJ7" s="262"/>
-      <c r="AK7" s="608"/>
+      <c r="AK7" s="613"/>
       <c r="AL7" s="80" t="s">
         <v>514</v>
       </c>
       <c r="AM7" s="452"/>
-      <c r="AN7" s="619"/>
+      <c r="AN7" s="624"/>
       <c r="AP7" s="76" t="s">
         <v>488</v>
       </c>
@@ -8176,27 +8188,27 @@
         <f>SUM(G7:N9)</f>
         <v>15</v>
       </c>
-      <c r="F8" s="600"/>
-      <c r="G8" s="651">
-        <v>0</v>
-      </c>
-      <c r="H8" s="648" t="s">
+      <c r="F8" s="605"/>
+      <c r="G8" s="656">
+        <v>0</v>
+      </c>
+      <c r="H8" s="653" t="s">
         <v>105</v>
       </c>
-      <c r="I8" s="551">
-        <v>0</v>
-      </c>
-      <c r="J8" s="648" t="s">
+      <c r="I8" s="556">
+        <v>0</v>
+      </c>
+      <c r="J8" s="653" t="s">
         <v>105</v>
       </c>
-      <c r="K8" s="654"/>
-      <c r="L8" s="610"/>
-      <c r="M8" s="623"/>
-      <c r="N8" s="615">
+      <c r="K8" s="659"/>
+      <c r="L8" s="615"/>
+      <c r="M8" s="628"/>
+      <c r="N8" s="620">
         <f>N5+N11</f>
         <v>15</v>
       </c>
-      <c r="O8" s="626"/>
+      <c r="O8" s="631"/>
       <c r="T8" s="103" t="s">
         <v>44</v>
       </c>
@@ -8206,7 +8218,7 @@
       <c r="X8" s="455" t="s">
         <v>163</v>
       </c>
-      <c r="Y8" s="634"/>
+      <c r="Y8" s="639"/>
       <c r="Z8" s="433"/>
       <c r="AA8" s="313"/>
       <c r="AB8" s="214"/>
@@ -8214,14 +8226,14 @@
       <c r="AD8" s="16"/>
       <c r="AE8" s="262"/>
       <c r="AF8" s="262"/>
-      <c r="AG8" s="609"/>
+      <c r="AG8" s="614"/>
       <c r="AH8" s="262"/>
-      <c r="AI8" s="608"/>
+      <c r="AI8" s="613"/>
       <c r="AJ8" s="262"/>
       <c r="AK8" s="262"/>
       <c r="AL8" s="262"/>
       <c r="AM8" s="452"/>
-      <c r="AN8" s="619"/>
+      <c r="AN8" s="624"/>
     </row>
     <row r="9" spans="1:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="237" t="s">
@@ -8236,17 +8248,17 @@
       <c r="D9" s="360" t="s">
         <v>286</v>
       </c>
-      <c r="F9" s="600"/>
-      <c r="G9" s="653"/>
-      <c r="H9" s="649"/>
-      <c r="I9" s="553"/>
-      <c r="J9" s="649"/>
-      <c r="K9" s="655"/>
-      <c r="L9" s="611"/>
-      <c r="M9" s="624"/>
-      <c r="N9" s="616"/>
-      <c r="O9" s="627"/>
-      <c r="S9" s="612" t="s">
+      <c r="F9" s="605"/>
+      <c r="G9" s="658"/>
+      <c r="H9" s="654"/>
+      <c r="I9" s="558"/>
+      <c r="J9" s="654"/>
+      <c r="K9" s="660"/>
+      <c r="L9" s="616"/>
+      <c r="M9" s="629"/>
+      <c r="N9" s="621"/>
+      <c r="O9" s="632"/>
+      <c r="S9" s="617" t="s">
         <v>62</v>
       </c>
       <c r="T9" s="89"/>
@@ -8258,7 +8270,7 @@
       <c r="X9" s="455" t="s">
         <v>164</v>
       </c>
-      <c r="Y9" s="634"/>
+      <c r="Y9" s="639"/>
       <c r="Z9" s="434"/>
       <c r="AA9" s="313"/>
       <c r="AB9" s="214"/>
@@ -8268,16 +8280,16 @@
       </c>
       <c r="AE9" s="262"/>
       <c r="AF9" s="262"/>
-      <c r="AG9" s="609"/>
+      <c r="AG9" s="614"/>
       <c r="AH9" s="262"/>
-      <c r="AI9" s="608"/>
+      <c r="AI9" s="613"/>
       <c r="AJ9" s="80"/>
-      <c r="AK9" s="608" t="s">
+      <c r="AK9" s="613" t="s">
         <v>256</v>
       </c>
       <c r="AL9" s="262"/>
       <c r="AM9" s="452"/>
-      <c r="AN9" s="619"/>
+      <c r="AN9" s="624"/>
       <c r="AP9" s="2" t="s">
         <v>526</v>
       </c>
@@ -8294,20 +8306,20 @@
         <f>Boat!U8</f>
         <v>41</v>
       </c>
-      <c r="F10" s="600"/>
+      <c r="F10" s="605"/>
       <c r="N10" s="442" t="s">
         <v>406</v>
       </c>
-      <c r="O10" s="602" t="s">
+      <c r="O10" s="607" t="s">
         <v>103</v>
       </c>
-      <c r="P10" s="628" t="s">
+      <c r="P10" s="633" t="s">
         <v>410</v>
       </c>
       <c r="R10" s="74" t="s">
         <v>44</v>
       </c>
-      <c r="S10" s="613"/>
+      <c r="S10" s="618"/>
       <c r="T10" s="89"/>
       <c r="U10" s="123" t="s">
         <v>177</v>
@@ -8319,7 +8331,7 @@
       <c r="X10" s="455" t="s">
         <v>165</v>
       </c>
-      <c r="Y10" s="634"/>
+      <c r="Y10" s="639"/>
       <c r="Z10" s="433">
         <v>0</v>
       </c>
@@ -8337,16 +8349,16 @@
       <c r="AF10" s="243" t="s">
         <v>318</v>
       </c>
-      <c r="AG10" s="609"/>
+      <c r="AG10" s="614"/>
       <c r="AH10" s="80"/>
-      <c r="AI10" s="608"/>
+      <c r="AI10" s="613"/>
       <c r="AJ10" s="262"/>
-      <c r="AK10" s="608"/>
+      <c r="AK10" s="613"/>
       <c r="AL10" s="262"/>
       <c r="AM10" s="466" t="s">
         <v>325</v>
       </c>
-      <c r="AN10" s="619"/>
+      <c r="AN10" s="624"/>
       <c r="AO10" s="209" t="s">
         <v>95</v>
       </c>
@@ -8355,7 +8367,7 @@
       <c r="A11" s="228" t="s">
         <v>290</v>
       </c>
-      <c r="B11" s="551" t="s">
+      <c r="B11" s="556" t="s">
         <v>288</v>
       </c>
       <c r="C11" s="481" t="s">
@@ -8364,18 +8376,18 @@
       <c r="D11" s="174" t="s">
         <v>362</v>
       </c>
-      <c r="F11" s="600"/>
+      <c r="F11" s="605"/>
       <c r="M11" s="6"/>
       <c r="N11" s="117">
         <v>7</v>
       </c>
-      <c r="O11" s="603"/>
-      <c r="P11" s="629"/>
+      <c r="O11" s="608"/>
+      <c r="P11" s="634"/>
       <c r="Q11" s="65"/>
       <c r="R11" s="120" t="s">
         <v>222</v>
       </c>
-      <c r="S11" s="613"/>
+      <c r="S11" s="618"/>
       <c r="T11" s="102" t="s">
         <v>44</v>
       </c>
@@ -8385,7 +8397,7 @@
       <c r="X11" s="455" t="s">
         <v>166</v>
       </c>
-      <c r="Y11" s="634"/>
+      <c r="Y11" s="639"/>
       <c r="Z11" s="433"/>
       <c r="AA11" s="313">
         <v>1</v>
@@ -8399,14 +8411,14 @@
       <c r="AF11" s="262" t="s">
         <v>493</v>
       </c>
-      <c r="AG11" s="609"/>
+      <c r="AG11" s="614"/>
       <c r="AH11" s="262"/>
       <c r="AI11" s="70"/>
       <c r="AJ11" s="262"/>
       <c r="AK11" s="262"/>
       <c r="AL11" s="262"/>
       <c r="AM11" s="452"/>
-      <c r="AN11" s="619"/>
+      <c r="AN11" s="624"/>
       <c r="AP11" s="76" t="s">
         <v>501</v>
       </c>
@@ -8415,7 +8427,7 @@
       <c r="A12" s="232" t="s">
         <v>392</v>
       </c>
-      <c r="B12" s="553"/>
+      <c r="B12" s="558"/>
       <c r="C12" s="482" t="s">
         <v>393</v>
       </c>
@@ -8425,25 +8437,25 @@
       <c r="E12" s="229">
         <v>3</v>
       </c>
-      <c r="F12" s="600"/>
+      <c r="F12" s="605"/>
       <c r="G12" s="349" t="s">
         <v>410</v>
       </c>
-      <c r="H12" s="556" t="s">
+      <c r="H12" s="561" t="s">
         <v>446</v>
       </c>
-      <c r="I12" s="558"/>
-      <c r="J12" s="558"/>
-      <c r="K12" s="607"/>
+      <c r="I12" s="563"/>
+      <c r="J12" s="563"/>
+      <c r="K12" s="612"/>
       <c r="L12" s="208"/>
       <c r="M12" s="208"/>
       <c r="N12" s="208"/>
-      <c r="O12" s="603"/>
-      <c r="P12" s="629"/>
+      <c r="O12" s="608"/>
+      <c r="P12" s="634"/>
       <c r="R12" s="122" t="s">
         <v>181</v>
       </c>
-      <c r="S12" s="614"/>
+      <c r="S12" s="619"/>
       <c r="T12" s="101" t="s">
         <v>44</v>
       </c>
@@ -8453,7 +8465,7 @@
       <c r="X12" s="455" t="s">
         <v>167</v>
       </c>
-      <c r="Y12" s="634"/>
+      <c r="Y12" s="639"/>
       <c r="Z12" s="431">
         <v>1</v>
       </c>
@@ -8464,16 +8476,16 @@
       <c r="AC12" s="100" t="s">
         <v>498</v>
       </c>
-      <c r="AD12" s="617" t="s">
+      <c r="AD12" s="622" t="s">
         <v>245</v>
       </c>
       <c r="AE12" s="465" t="s">
         <v>244</v>
       </c>
-      <c r="AF12" s="609" t="s">
+      <c r="AF12" s="614" t="s">
         <v>231</v>
       </c>
-      <c r="AG12" s="609"/>
+      <c r="AG12" s="614"/>
       <c r="AH12" s="243" t="s">
         <v>264</v>
       </c>
@@ -8483,10 +8495,10 @@
       <c r="AJ12" s="262"/>
       <c r="AK12" s="262"/>
       <c r="AL12" s="262"/>
-      <c r="AM12" s="631" t="s">
+      <c r="AM12" s="636" t="s">
         <v>254</v>
       </c>
-      <c r="AN12" s="619"/>
+      <c r="AN12" s="624"/>
       <c r="AO12" s="350" t="s">
         <v>97</v>
       </c>
@@ -8498,17 +8510,17 @@
       <c r="E13" s="472">
         <v>-3</v>
       </c>
-      <c r="F13" s="600"/>
-      <c r="G13" s="558" t="s">
+      <c r="F13" s="605"/>
+      <c r="G13" s="563" t="s">
         <v>447</v>
       </c>
-      <c r="H13" s="558"/>
-      <c r="I13" s="558"/>
-      <c r="J13" s="607"/>
+      <c r="H13" s="563"/>
+      <c r="I13" s="563"/>
+      <c r="J13" s="612"/>
       <c r="M13" s="6"/>
       <c r="N13" s="6"/>
-      <c r="O13" s="603"/>
-      <c r="P13" s="630"/>
+      <c r="O13" s="608"/>
+      <c r="P13" s="635"/>
       <c r="T13" s="105" t="s">
         <v>44</v>
       </c>
@@ -8518,7 +8530,7 @@
       <c r="X13" s="455" t="s">
         <v>168</v>
       </c>
-      <c r="Y13" s="634"/>
+      <c r="Y13" s="639"/>
       <c r="Z13" s="431">
         <v>1</v>
       </c>
@@ -8529,8 +8541,8 @@
         <v>518</v>
       </c>
       <c r="AC13" s="16"/>
-      <c r="AD13" s="617"/>
-      <c r="AF13" s="609"/>
+      <c r="AD13" s="622"/>
+      <c r="AF13" s="614"/>
       <c r="AG13" s="80"/>
       <c r="AH13" s="243" t="s">
         <v>314</v>
@@ -8541,8 +8553,8 @@
       <c r="AJ13" s="80"/>
       <c r="AK13" s="262"/>
       <c r="AL13" s="262"/>
-      <c r="AM13" s="631"/>
-      <c r="AN13" s="619"/>
+      <c r="AM13" s="636"/>
+      <c r="AN13" s="624"/>
     </row>
     <row r="14" spans="1:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="474"/>
@@ -8550,18 +8562,18 @@
       <c r="C14" s="483"/>
       <c r="D14" s="476"/>
       <c r="E14" s="477"/>
-      <c r="F14" s="600"/>
-      <c r="G14" s="558" t="s">
+      <c r="F14" s="605"/>
+      <c r="G14" s="563" t="s">
         <v>446</v>
       </c>
-      <c r="H14" s="558"/>
-      <c r="I14" s="558"/>
-      <c r="J14" s="607"/>
+      <c r="H14" s="563"/>
+      <c r="I14" s="563"/>
+      <c r="J14" s="612"/>
       <c r="K14" s="2">
         <v>12</v>
       </c>
       <c r="N14" s="6"/>
-      <c r="O14" s="603"/>
+      <c r="O14" s="608"/>
       <c r="Q14" s="61" t="s">
         <v>554</v>
       </c>
@@ -8575,34 +8587,34 @@
       <c r="X14" s="455" t="s">
         <v>169</v>
       </c>
-      <c r="Y14" s="634"/>
+      <c r="Y14" s="639"/>
       <c r="Z14" s="431">
         <v>1</v>
       </c>
       <c r="AA14" s="313"/>
       <c r="AB14" s="214"/>
       <c r="AC14" s="16"/>
-      <c r="AD14" s="617"/>
+      <c r="AD14" s="622"/>
       <c r="AE14" s="262"/>
-      <c r="AF14" s="609"/>
+      <c r="AF14" s="614"/>
       <c r="AG14" s="262"/>
       <c r="AH14" s="262"/>
       <c r="AI14" s="70"/>
       <c r="AJ14" s="262"/>
       <c r="AK14" s="262"/>
       <c r="AL14" s="262"/>
-      <c r="AM14" s="631"/>
-      <c r="AN14" s="619"/>
+      <c r="AM14" s="636"/>
+      <c r="AN14" s="624"/>
     </row>
     <row r="15" spans="1:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="473" t="s">
         <v>524</v>
       </c>
-      <c r="C15" s="551" t="s">
+      <c r="C15" s="556" t="s">
         <v>381</v>
       </c>
-      <c r="F15" s="600"/>
-      <c r="O15" s="603"/>
+      <c r="F15" s="605"/>
+      <c r="O15" s="608"/>
       <c r="R15" s="99" t="s">
         <v>44</v>
       </c>
@@ -8615,7 +8627,7 @@
       <c r="X15" s="455" t="s">
         <v>170</v>
       </c>
-      <c r="Y15" s="634"/>
+      <c r="Y15" s="639"/>
       <c r="Z15" s="433">
         <v>1</v>
       </c>
@@ -8624,8 +8636,8 @@
       <c r="AC15" s="76" t="s">
         <v>496</v>
       </c>
-      <c r="AD15" s="617"/>
-      <c r="AF15" s="609"/>
+      <c r="AD15" s="622"/>
+      <c r="AF15" s="614"/>
       <c r="AG15" s="80"/>
       <c r="AH15" s="243" t="s">
         <v>465</v>
@@ -8638,8 +8650,8 @@
       </c>
       <c r="AK15" s="262"/>
       <c r="AL15" s="262"/>
-      <c r="AM15" s="631"/>
-      <c r="AN15" s="619"/>
+      <c r="AM15" s="636"/>
+      <c r="AN15" s="624"/>
       <c r="AP15" s="76" t="s">
         <v>74</v>
       </c>
@@ -8654,20 +8666,20 @@
       <c r="B16" s="21" t="s">
         <v>416</v>
       </c>
-      <c r="C16" s="553"/>
+      <c r="C16" s="558"/>
       <c r="D16" s="61" t="s">
         <v>510</v>
       </c>
       <c r="E16" s="229">
         <v>1</v>
       </c>
-      <c r="F16" s="600"/>
+      <c r="F16" s="605"/>
       <c r="G16" s="349" t="s">
         <v>505</v>
       </c>
       <c r="I16" s="495"/>
       <c r="J16" s="20"/>
-      <c r="O16" s="603"/>
+      <c r="O16" s="608"/>
       <c r="R16" s="459" t="s">
         <v>185</v>
       </c>
@@ -8678,7 +8690,7 @@
       <c r="X16" s="455" t="s">
         <v>171</v>
       </c>
-      <c r="Y16" s="634"/>
+      <c r="Y16" s="639"/>
       <c r="Z16" s="431">
         <v>1</v>
       </c>
@@ -8699,18 +8711,18 @@
       <c r="AM16" s="452" t="s">
         <v>324</v>
       </c>
-      <c r="AN16" s="619"/>
+      <c r="AN16" s="624"/>
       <c r="AP16" s="76" t="s">
         <v>235</v>
       </c>
     </row>
     <row r="17" spans="1:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B17" s="80"/>
-      <c r="F17" s="600"/>
+      <c r="F17" s="605"/>
       <c r="I17" s="496"/>
       <c r="J17" s="20"/>
       <c r="N17" s="6"/>
-      <c r="O17" s="603"/>
+      <c r="O17" s="608"/>
       <c r="Q17" s="21" t="s">
         <v>552</v>
       </c>
@@ -8730,7 +8742,7 @@
       <c r="X17" s="455" t="s">
         <v>172</v>
       </c>
-      <c r="Y17" s="634"/>
+      <c r="Y17" s="639"/>
       <c r="Z17" s="433"/>
       <c r="AA17" s="313"/>
       <c r="AB17" s="214"/>
@@ -8755,7 +8767,7 @@
       <c r="AK17" s="262"/>
       <c r="AL17" s="80"/>
       <c r="AM17" s="452"/>
-      <c r="AN17" s="619"/>
+      <c r="AN17" s="624"/>
       <c r="AO17" s="209" t="s">
         <v>515</v>
       </c>
@@ -8779,21 +8791,21 @@
       <c r="E18" s="99" t="s">
         <v>44</v>
       </c>
-      <c r="F18" s="600"/>
+      <c r="F18" s="605"/>
       <c r="G18" s="349" t="s">
         <v>549</v>
       </c>
       <c r="I18" s="24"/>
       <c r="J18" s="20"/>
-      <c r="O18" s="603"/>
+      <c r="O18" s="608"/>
       <c r="Q18" s="112"/>
-      <c r="R18" s="595" t="s">
+      <c r="R18" s="600" t="s">
         <v>557</v>
       </c>
       <c r="T18" s="100" t="s">
         <v>44</v>
       </c>
-      <c r="U18" s="639" t="s">
+      <c r="U18" s="644" t="s">
         <v>44</v>
       </c>
       <c r="V18" s="120"/>
@@ -8803,7 +8815,7 @@
       <c r="X18" s="455" t="s">
         <v>173</v>
       </c>
-      <c r="Y18" s="634"/>
+      <c r="Y18" s="639"/>
       <c r="Z18" s="433">
         <v>1</v>
       </c>
@@ -8814,38 +8826,38 @@
       <c r="AC18" s="16"/>
       <c r="AD18" s="16"/>
       <c r="AE18" s="262"/>
-      <c r="AF18" s="608" t="s">
+      <c r="AF18" s="613" t="s">
         <v>492</v>
       </c>
       <c r="AG18" s="262"/>
       <c r="AH18" s="70"/>
       <c r="AI18" s="70"/>
-      <c r="AJ18" s="632" t="s">
+      <c r="AJ18" s="637" t="s">
         <v>322</v>
       </c>
       <c r="AK18" s="262"/>
       <c r="AL18" s="80"/>
       <c r="AM18" s="452"/>
-      <c r="AN18" s="619"/>
+      <c r="AN18" s="624"/>
       <c r="AP18" s="76" t="s">
         <v>88</v>
       </c>
     </row>
     <row r="19" spans="1:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="F19" s="600"/>
+      <c r="F19" s="605"/>
       <c r="I19" s="224"/>
-      <c r="O19" s="603"/>
-      <c r="R19" s="596"/>
+      <c r="O19" s="608"/>
+      <c r="R19" s="601"/>
       <c r="S19" s="30" t="s">
         <v>555</v>
       </c>
-      <c r="U19" s="640"/>
+      <c r="U19" s="645"/>
       <c r="V19" s="146"/>
       <c r="W19" s="146"/>
       <c r="X19" s="455" t="s">
         <v>174</v>
       </c>
-      <c r="Y19" s="634"/>
+      <c r="Y19" s="639"/>
       <c r="Z19" s="431">
         <v>1</v>
       </c>
@@ -8854,17 +8866,17 @@
       <c r="AC19" s="16"/>
       <c r="AD19" s="16"/>
       <c r="AE19" s="262"/>
-      <c r="AF19" s="608"/>
+      <c r="AF19" s="613"/>
       <c r="AG19" s="262"/>
       <c r="AH19" s="262"/>
       <c r="AI19" s="70"/>
-      <c r="AJ19" s="632"/>
+      <c r="AJ19" s="637"/>
       <c r="AK19" s="484" t="s">
         <v>256</v>
       </c>
       <c r="AL19" s="80"/>
       <c r="AM19" s="452"/>
-      <c r="AN19" s="619"/>
+      <c r="AN19" s="624"/>
       <c r="AP19" s="76" t="s">
         <v>485</v>
       </c>
@@ -8885,24 +8897,24 @@
       <c r="E20" s="461">
         <v>-1</v>
       </c>
-      <c r="F20" s="600"/>
+      <c r="F20" s="605"/>
       <c r="G20" s="349" t="s">
         <v>508</v>
       </c>
       <c r="I20" s="224"/>
-      <c r="O20" s="603"/>
-      <c r="Q20" s="605" t="s">
+      <c r="O20" s="608"/>
+      <c r="Q20" s="610" t="s">
         <v>48</v>
       </c>
       <c r="T20" s="428" t="s">
         <v>44</v>
       </c>
-      <c r="U20" s="641"/>
+      <c r="U20" s="646"/>
       <c r="W20" s="429"/>
       <c r="X20" s="456" t="s">
         <v>175</v>
       </c>
-      <c r="Y20" s="634"/>
+      <c r="Y20" s="639"/>
       <c r="Z20" s="435">
         <v>1</v>
       </c>
@@ -8927,7 +8939,7 @@
       <c r="AM20" s="400" t="s">
         <v>254</v>
       </c>
-      <c r="AN20" s="619"/>
+      <c r="AN20" s="624"/>
       <c r="AO20" s="350" t="s">
         <v>477</v>
       </c>
@@ -8948,20 +8960,20 @@
       <c r="E21" s="271">
         <v>0</v>
       </c>
-      <c r="F21" s="600"/>
+      <c r="F21" s="605"/>
       <c r="I21" s="224"/>
-      <c r="O21" s="603"/>
-      <c r="Q21" s="606"/>
+      <c r="O21" s="608"/>
+      <c r="Q21" s="611"/>
       <c r="T21" s="446"/>
       <c r="U21" s="14"/>
-      <c r="V21" s="636"/>
+      <c r="V21" s="641"/>
       <c r="W21" s="450" t="s">
         <v>176</v>
       </c>
       <c r="X21" s="453" t="s">
         <v>187</v>
       </c>
-      <c r="Y21" s="634"/>
+      <c r="Y21" s="639"/>
       <c r="Z21" s="469">
         <v>3</v>
       </c>
@@ -8992,15 +9004,15 @@
       <c r="AM21" s="452" t="s">
         <v>566</v>
       </c>
-      <c r="AN21" s="619"/>
+      <c r="AN21" s="624"/>
     </row>
     <row r="22" spans="1:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="F22" s="600"/>
+      <c r="F22" s="605"/>
       <c r="G22" s="349" t="s">
         <v>506</v>
       </c>
       <c r="I22" s="224"/>
-      <c r="O22" s="603"/>
+      <c r="O22" s="608"/>
       <c r="R22" s="458" t="s">
         <v>44</v>
       </c>
@@ -9008,14 +9020,14 @@
         <v>44</v>
       </c>
       <c r="U22" s="15"/>
-      <c r="V22" s="637"/>
+      <c r="V22" s="642"/>
       <c r="W22" s="450" t="s">
         <v>176</v>
       </c>
       <c r="X22" s="453" t="s">
         <v>188</v>
       </c>
-      <c r="Y22" s="634"/>
+      <c r="Y22" s="639"/>
       <c r="Z22" s="439"/>
       <c r="AA22" s="10"/>
       <c r="AB22" s="439"/>
@@ -9026,7 +9038,7 @@
       <c r="AG22" s="6"/>
       <c r="AH22" s="6"/>
       <c r="AI22" s="6"/>
-      <c r="AJ22" s="608" t="s">
+      <c r="AJ22" s="613" t="s">
         <v>489</v>
       </c>
       <c r="AK22" s="262"/>
@@ -9034,7 +9046,7 @@
         <v>495</v>
       </c>
       <c r="AM22" s="306"/>
-      <c r="AN22" s="619"/>
+      <c r="AN22" s="624"/>
     </row>
     <row r="23" spans="1:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="236" t="s">
@@ -9052,22 +9064,22 @@
       <c r="E23" s="230">
         <v>1</v>
       </c>
-      <c r="F23" s="600"/>
+      <c r="F23" s="605"/>
       <c r="I23" s="224"/>
-      <c r="O23" s="603"/>
-      <c r="Q23" s="605" t="s">
+      <c r="O23" s="608"/>
+      <c r="Q23" s="610" t="s">
         <v>145</v>
       </c>
       <c r="T23" s="17"/>
       <c r="U23" s="444" t="s">
         <v>44</v>
       </c>
-      <c r="V23" s="637"/>
+      <c r="V23" s="642"/>
       <c r="W23" s="148"/>
       <c r="X23" s="453" t="s">
         <v>189</v>
       </c>
-      <c r="Y23" s="634"/>
+      <c r="Y23" s="639"/>
       <c r="Z23" s="17"/>
       <c r="AA23" s="10"/>
       <c r="AB23" s="439"/>
@@ -9078,13 +9090,13 @@
       <c r="AG23" s="6"/>
       <c r="AH23" s="6"/>
       <c r="AI23" s="6"/>
-      <c r="AJ23" s="608"/>
+      <c r="AJ23" s="613"/>
       <c r="AK23" s="262"/>
       <c r="AL23" s="80" t="s">
         <v>525</v>
       </c>
       <c r="AM23" s="306"/>
-      <c r="AN23" s="619"/>
+      <c r="AN23" s="624"/>
     </row>
     <row r="24" spans="1:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="464" t="s">
@@ -9102,23 +9114,23 @@
       <c r="E24" s="460">
         <v>1</v>
       </c>
-      <c r="F24" s="600"/>
+      <c r="F24" s="605"/>
       <c r="G24" s="61" t="s">
         <v>507</v>
       </c>
       <c r="I24" s="224"/>
-      <c r="O24" s="603"/>
-      <c r="Q24" s="606"/>
+      <c r="O24" s="608"/>
+      <c r="Q24" s="611"/>
       <c r="T24" s="17"/>
       <c r="U24" s="232" t="s">
         <v>44</v>
       </c>
-      <c r="V24" s="637"/>
+      <c r="V24" s="642"/>
       <c r="W24" s="148"/>
       <c r="X24" s="453" t="s">
         <v>186</v>
       </c>
-      <c r="Y24" s="634"/>
+      <c r="Y24" s="639"/>
       <c r="Z24" s="17"/>
       <c r="AA24" s="10"/>
       <c r="AB24" s="439"/>
@@ -9137,12 +9149,12 @@
         <v>480</v>
       </c>
       <c r="AM24" s="306"/>
-      <c r="AN24" s="619"/>
+      <c r="AN24" s="624"/>
     </row>
     <row r="25" spans="1:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="F25" s="600"/>
+      <c r="F25" s="605"/>
       <c r="I25" s="224"/>
-      <c r="O25" s="603"/>
+      <c r="O25" s="608"/>
       <c r="P25" s="209" t="s">
         <v>285</v>
       </c>
@@ -9155,12 +9167,12 @@
       <c r="U25" s="424" t="s">
         <v>44</v>
       </c>
-      <c r="V25" s="638"/>
+      <c r="V25" s="643"/>
       <c r="W25" s="148"/>
       <c r="X25" s="453" t="s">
         <v>190</v>
       </c>
-      <c r="Y25" s="634"/>
+      <c r="Y25" s="639"/>
       <c r="Z25" s="17"/>
       <c r="AA25" s="10"/>
       <c r="AB25" s="439"/>
@@ -9177,7 +9189,7 @@
       <c r="AK25" s="142"/>
       <c r="AL25" s="6"/>
       <c r="AM25" s="306"/>
-      <c r="AN25" s="619"/>
+      <c r="AN25" s="624"/>
     </row>
     <row r="26" spans="1:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="236" t="s">
@@ -9195,17 +9207,17 @@
       <c r="E26" s="398">
         <v>1</v>
       </c>
-      <c r="F26" s="600"/>
+      <c r="F26" s="605"/>
       <c r="G26" s="349" t="s">
         <v>504</v>
       </c>
       <c r="I26" s="224"/>
-      <c r="O26" s="603"/>
-      <c r="P26" s="621" t="s">
+      <c r="O26" s="608"/>
+      <c r="P26" s="626" t="s">
         <v>547</v>
       </c>
-      <c r="Q26" s="622"/>
-      <c r="R26" s="597" t="s">
+      <c r="Q26" s="627"/>
+      <c r="R26" s="602" t="s">
         <v>556</v>
       </c>
       <c r="T26" s="182"/>
@@ -9217,7 +9229,7 @@
       <c r="X26" s="453" t="s">
         <v>182</v>
       </c>
-      <c r="Y26" s="634"/>
+      <c r="Y26" s="639"/>
       <c r="Z26" s="17"/>
       <c r="AA26" s="10"/>
       <c r="AB26" s="439"/>
@@ -9244,7 +9256,7 @@
       <c r="AM26" s="466" t="s">
         <v>473</v>
       </c>
-      <c r="AN26" s="619"/>
+      <c r="AN26" s="624"/>
     </row>
     <row r="27" spans="1:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B27" s="21" t="s">
@@ -9256,13 +9268,13 @@
       <c r="E27" s="271" t="s">
         <v>44</v>
       </c>
-      <c r="F27" s="601"/>
+      <c r="F27" s="606"/>
       <c r="G27" s="61" t="s">
         <v>565</v>
       </c>
       <c r="I27" s="225"/>
-      <c r="O27" s="604"/>
-      <c r="R27" s="598"/>
+      <c r="O27" s="609"/>
+      <c r="R27" s="603"/>
       <c r="S27" s="445" t="s">
         <v>54</v>
       </c>
@@ -9275,7 +9287,7 @@
       <c r="X27" s="453" t="s">
         <v>551</v>
       </c>
-      <c r="Y27" s="635"/>
+      <c r="Y27" s="640"/>
       <c r="Z27" s="163"/>
       <c r="AA27" s="13"/>
       <c r="AB27" s="440"/>
@@ -9292,7 +9304,7 @@
       <c r="AM27" s="400" t="s">
         <v>326</v>
       </c>
-      <c r="AN27" s="620"/>
+      <c r="AN27" s="625"/>
     </row>
   </sheetData>
   <mergeCells count="54">
@@ -9359,7 +9371,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2029A93E-B53C-4201-9F17-439C144F3CF1}">
   <dimension ref="A1:AN37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="N1" workbookViewId="0">
+    <sheetView topLeftCell="N1" workbookViewId="0">
       <selection activeCell="AL8" sqref="AL8"/>
     </sheetView>
   </sheetViews>
@@ -9455,10 +9467,10 @@
       <c r="S1" s="142"/>
       <c r="T1" s="142"/>
       <c r="U1" s="6"/>
-      <c r="V1" s="663" t="s">
+      <c r="V1" s="668" t="s">
         <v>458</v>
       </c>
-      <c r="W1" s="664"/>
+      <c r="W1" s="669"/>
       <c r="X1" s="312">
         <f>68-(U8+W3+V3+S3)</f>
         <v>0</v>
@@ -9474,21 +9486,21 @@
       <c r="AB1" s="308" t="s">
         <v>44</v>
       </c>
-      <c r="AC1" s="665" t="s">
+      <c r="AC1" s="670" t="s">
         <v>191</v>
       </c>
-      <c r="AD1" s="666"/>
-      <c r="AE1" s="667"/>
-      <c r="AF1" s="668" t="s">
+      <c r="AD1" s="671"/>
+      <c r="AE1" s="672"/>
+      <c r="AF1" s="673" t="s">
         <v>298</v>
       </c>
-      <c r="AG1" s="669"/>
-      <c r="AH1" s="670"/>
-      <c r="AI1" s="660" t="s">
+      <c r="AG1" s="674"/>
+      <c r="AH1" s="675"/>
+      <c r="AI1" s="665" t="s">
         <v>461</v>
       </c>
-      <c r="AJ1" s="661"/>
-      <c r="AK1" s="662"/>
+      <c r="AJ1" s="666"/>
+      <c r="AK1" s="667"/>
       <c r="AN1" s="142"/>
     </row>
     <row r="2" spans="1:40" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -9505,19 +9517,19 @@
       <c r="K2" s="327">
         <v>-3</v>
       </c>
-      <c r="L2" s="671">
+      <c r="L2" s="676">
         <f>SUM(L5:L30)</f>
         <v>3</v>
       </c>
-      <c r="M2" s="673">
+      <c r="M2" s="678">
         <f>SUM(M4:M29)</f>
         <v>6</v>
       </c>
-      <c r="N2" s="675">
+      <c r="N2" s="680">
         <f>SUM(N4:N29)</f>
         <v>9</v>
       </c>
-      <c r="O2" s="615">
+      <c r="O2" s="620">
         <f>SUM(M30:M37)* (-1)</f>
         <v>-3</v>
       </c>
@@ -9536,7 +9548,7 @@
       <c r="T2" s="515" t="s">
         <v>221</v>
       </c>
-      <c r="U2" s="677" t="s">
+      <c r="U2" s="682" t="s">
         <v>239</v>
       </c>
       <c r="V2" s="516" t="s">
@@ -9605,10 +9617,10 @@
         <f>T3+V3+W3+S3</f>
         <v>68</v>
       </c>
-      <c r="L3" s="672"/>
-      <c r="M3" s="674"/>
-      <c r="N3" s="676"/>
-      <c r="O3" s="616"/>
+      <c r="L3" s="677"/>
+      <c r="M3" s="679"/>
+      <c r="N3" s="681"/>
+      <c r="O3" s="621"/>
       <c r="P3" s="176">
         <f>(L2+M2)-W3</f>
         <v>0</v>
@@ -9624,7 +9636,7 @@
         <f>SUM(T4:T29)</f>
         <v>41</v>
       </c>
-      <c r="U3" s="678"/>
+      <c r="U3" s="683"/>
       <c r="V3" s="519">
         <f t="shared" ref="V3:AA3" si="0">SUM(V4:V29)</f>
         <v>6</v>
@@ -9723,7 +9735,7 @@
         <f>AA4</f>
         <v>0</v>
       </c>
-      <c r="O4" s="679" t="s">
+      <c r="O4" s="684" t="s">
         <v>200</v>
       </c>
       <c r="P4" s="20"/>
@@ -9802,7 +9814,7 @@
         <f>AA5</f>
         <v>0</v>
       </c>
-      <c r="O5" s="680"/>
+      <c r="O5" s="685"/>
       <c r="P5" s="20"/>
       <c r="Q5" s="2" t="s">
         <v>347</v>
@@ -9860,7 +9872,7 @@
         <v>0</v>
       </c>
       <c r="AL5" s="6"/>
-      <c r="AM5" s="734"/>
+      <c r="AM5" s="546"/>
       <c r="AN5" s="142"/>
     </row>
     <row r="6" spans="1:40" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -9889,7 +9901,7 @@
         <f>AA6</f>
         <v>0</v>
       </c>
-      <c r="O6" s="680"/>
+      <c r="O6" s="685"/>
       <c r="P6" s="19" t="s">
         <v>342</v>
       </c>
@@ -9954,7 +9966,7 @@
         <v>0</v>
       </c>
       <c r="AL6" s="6"/>
-      <c r="AM6" s="735" t="s">
+      <c r="AM6" s="547" t="s">
         <v>584</v>
       </c>
       <c r="AN6" s="262"/>
@@ -9980,7 +9992,7 @@
         <f t="shared" ref="N7:N37" si="10">AA7</f>
         <v>0</v>
       </c>
-      <c r="O7" s="680"/>
+      <c r="O7" s="685"/>
       <c r="P7" s="20"/>
       <c r="Q7" s="2" t="s">
         <v>342</v>
@@ -10048,7 +10060,7 @@
         <v>0</v>
       </c>
       <c r="AL7" s="6"/>
-      <c r="AM7" s="735"/>
+      <c r="AM7" s="547"/>
       <c r="AN7" s="262"/>
     </row>
     <row r="8" spans="1:40" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -10086,7 +10098,7 @@
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
-      <c r="O8" s="680"/>
+      <c r="O8" s="685"/>
       <c r="P8" s="21" t="s">
         <v>238</v>
       </c>
@@ -10155,7 +10167,7 @@
         <v>0</v>
       </c>
       <c r="AL8" s="6"/>
-      <c r="AM8" s="735"/>
+      <c r="AM8" s="547"/>
       <c r="AN8" s="262"/>
     </row>
     <row r="9" spans="1:40" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -10170,7 +10182,7 @@
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
-      <c r="O9" s="680"/>
+      <c r="O9" s="685"/>
       <c r="P9" s="21" t="s">
         <v>342</v>
       </c>
@@ -10233,7 +10245,7 @@
         <v>0</v>
       </c>
       <c r="AL9" s="6"/>
-      <c r="AM9" s="736"/>
+      <c r="AM9" s="548"/>
       <c r="AN9" s="142"/>
     </row>
     <row r="10" spans="1:40" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -10268,7 +10280,7 @@
         <f t="shared" si="10"/>
         <v>2</v>
       </c>
-      <c r="O10" s="680"/>
+      <c r="O10" s="685"/>
       <c r="P10" s="20"/>
       <c r="Q10" s="2" t="s">
         <v>347</v>
@@ -10351,7 +10363,7 @@
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
-      <c r="O11" s="680"/>
+      <c r="O11" s="685"/>
       <c r="P11" s="21" t="s">
         <v>342</v>
       </c>
@@ -10407,11 +10419,11 @@
         <v>0</v>
       </c>
       <c r="AL11" s="6"/>
-      <c r="AM11" s="735"/>
+      <c r="AM11" s="547"/>
       <c r="AN11" s="142"/>
     </row>
     <row r="12" spans="1:40" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="651" t="s">
+      <c r="A12" s="656" t="s">
         <v>55</v>
       </c>
       <c r="B12" s="30">
@@ -10420,7 +10432,7 @@
       <c r="C12" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="E12" s="605" t="s">
+      <c r="E12" s="610" t="s">
         <v>57</v>
       </c>
       <c r="G12" s="267"/>
@@ -10438,7 +10450,7 @@
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
-      <c r="O12" s="680"/>
+      <c r="O12" s="685"/>
       <c r="P12" s="21" t="s">
         <v>342</v>
       </c>
@@ -10498,7 +10510,7 @@
         <v>0</v>
       </c>
       <c r="AL12" s="6"/>
-      <c r="AM12" s="735" t="s">
+      <c r="AM12" s="547" t="s">
         <v>528</v>
       </c>
       <c r="AN12" s="301" t="s">
@@ -10506,14 +10518,14 @@
       </c>
     </row>
     <row r="13" spans="1:40" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="653"/>
+      <c r="A13" s="658"/>
       <c r="B13" s="153">
         <v>12</v>
       </c>
       <c r="C13" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="E13" s="606"/>
+      <c r="E13" s="611"/>
       <c r="F13" s="176">
         <v>0</v>
       </c>
@@ -10536,7 +10548,7 @@
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
-      <c r="O13" s="680"/>
+      <c r="O13" s="685"/>
       <c r="P13" s="21" t="s">
         <v>342</v>
       </c>
@@ -10592,7 +10604,7 @@
         <v>0</v>
       </c>
       <c r="AL13" s="16"/>
-      <c r="AM13" s="735"/>
+      <c r="AM13" s="547"/>
       <c r="AN13" s="142"/>
     </row>
     <row r="14" spans="1:40" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -10612,7 +10624,7 @@
         <f t="shared" si="10"/>
         <v>2</v>
       </c>
-      <c r="O14" s="680"/>
+      <c r="O14" s="685"/>
       <c r="P14" s="20"/>
       <c r="Q14" s="205" t="s">
         <v>346</v>
@@ -10674,7 +10686,7 @@
       <c r="AL14" s="6" t="s">
         <v>583</v>
       </c>
-      <c r="AM14" s="737" t="s">
+      <c r="AM14" s="549" t="s">
         <v>586</v>
       </c>
       <c r="AN14" s="142" t="s">
@@ -10707,7 +10719,7 @@
         <f t="shared" si="10"/>
         <v>1</v>
       </c>
-      <c r="O15" s="680"/>
+      <c r="O15" s="685"/>
       <c r="P15" s="20"/>
       <c r="Q15" s="205" t="s">
         <v>346</v>
@@ -10773,7 +10785,7 @@
       <c r="AL15" s="6" t="s">
         <v>232</v>
       </c>
-      <c r="AM15" s="735" t="s">
+      <c r="AM15" s="547" t="s">
         <v>468</v>
       </c>
       <c r="AN15" s="142"/>
@@ -10794,7 +10806,7 @@
         <f t="shared" si="10"/>
         <v>1</v>
       </c>
-      <c r="O16" s="680"/>
+      <c r="O16" s="685"/>
       <c r="P16" s="21" t="s">
         <v>342</v>
       </c>
@@ -10892,7 +10904,7 @@
         <f t="shared" si="10"/>
         <v>1</v>
       </c>
-      <c r="O17" s="680"/>
+      <c r="O17" s="685"/>
       <c r="P17" s="20"/>
       <c r="Q17" s="2" t="s">
         <v>348</v>
@@ -10987,7 +10999,7 @@
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
-      <c r="O18" s="680"/>
+      <c r="O18" s="685"/>
       <c r="P18" s="21" t="s">
         <v>342</v>
       </c>
@@ -11047,7 +11059,7 @@
         <v>0</v>
       </c>
       <c r="AL18" s="6"/>
-      <c r="AM18" s="738"/>
+      <c r="AM18" s="550"/>
       <c r="AN18" s="142"/>
     </row>
     <row r="19" spans="1:40" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -11070,7 +11082,7 @@
         <f t="shared" si="10"/>
         <v>1</v>
       </c>
-      <c r="O19" s="680"/>
+      <c r="O19" s="685"/>
       <c r="P19" s="20"/>
       <c r="Q19" s="2" t="s">
         <v>341</v>
@@ -11134,7 +11146,7 @@
       <c r="AL19" s="6" t="s">
         <v>574</v>
       </c>
-      <c r="AM19" s="735"/>
+      <c r="AM19" s="547"/>
       <c r="AN19" s="142"/>
     </row>
     <row r="20" spans="1:40" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -11166,11 +11178,11 @@
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
-      <c r="O20" s="681"/>
-      <c r="P20" s="556" t="s">
+      <c r="O20" s="686"/>
+      <c r="P20" s="561" t="s">
         <v>342</v>
       </c>
-      <c r="Q20" s="607"/>
+      <c r="Q20" s="612"/>
       <c r="R20" s="321" t="s">
         <v>86</v>
       </c>
@@ -11228,7 +11240,7 @@
       <c r="AL20" s="6" t="s">
         <v>88</v>
       </c>
-      <c r="AM20" s="735" t="s">
+      <c r="AM20" s="547" t="s">
         <v>464</v>
       </c>
     </row>
@@ -11325,7 +11337,7 @@
       <c r="AL21" s="6" t="s">
         <v>84</v>
       </c>
-      <c r="AM21" s="735" t="s">
+      <c r="AM21" s="547" t="s">
         <v>464</v>
       </c>
       <c r="AN21" s="142"/>
@@ -11400,11 +11412,11 @@
         <v>0</v>
       </c>
       <c r="AL22" s="16"/>
-      <c r="AM22" s="738"/>
+      <c r="AM22" s="550"/>
       <c r="AN22" s="142"/>
     </row>
     <row r="23" spans="1:40" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E23" s="658" t="s">
+      <c r="E23" s="663" t="s">
         <v>294</v>
       </c>
       <c r="F23" s="184"/>
@@ -11484,7 +11496,7 @@
       <c r="AL23" s="6" t="s">
         <v>592</v>
       </c>
-      <c r="AM23" s="735" t="s">
+      <c r="AM23" s="547" t="s">
         <v>589</v>
       </c>
       <c r="AN23" s="142" t="s">
@@ -11495,7 +11507,7 @@
       <c r="C24" s="2" t="s">
         <v>260</v>
       </c>
-      <c r="E24" s="659"/>
+      <c r="E24" s="664"/>
       <c r="F24" s="176"/>
       <c r="K24" s="403" t="s">
         <v>301</v>
@@ -11510,10 +11522,10 @@
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
-      <c r="P24" s="556" t="s">
+      <c r="P24" s="561" t="s">
         <v>342</v>
       </c>
-      <c r="Q24" s="607"/>
+      <c r="Q24" s="612"/>
       <c r="R24" s="321" t="s">
         <v>254</v>
       </c>
@@ -11579,7 +11591,7 @@
       <c r="AL24" s="6" t="s">
         <v>527</v>
       </c>
-      <c r="AM24" s="735"/>
+      <c r="AM24" s="547"/>
       <c r="AN24" s="142" t="s">
         <v>254</v>
       </c>
@@ -11655,7 +11667,7 @@
         <v>0</v>
       </c>
       <c r="AL25" s="16"/>
-      <c r="AM25" s="735" t="s">
+      <c r="AM25" s="547" t="s">
         <v>470</v>
       </c>
       <c r="AN25" s="142"/>
@@ -11744,7 +11756,7 @@
         <v>0</v>
       </c>
       <c r="AL26" s="493"/>
-      <c r="AM26" s="735"/>
+      <c r="AM26" s="547"/>
       <c r="AN26" s="142"/>
     </row>
     <row r="27" spans="1:40" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -11821,7 +11833,7 @@
         <v>0</v>
       </c>
       <c r="AL27" s="16"/>
-      <c r="AM27" s="738"/>
+      <c r="AM27" s="550"/>
       <c r="AN27" s="142"/>
     </row>
     <row r="28" spans="1:40" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -11887,7 +11899,7 @@
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
-      <c r="AM28" s="738"/>
+      <c r="AM28" s="550"/>
       <c r="AN28" s="142"/>
     </row>
     <row r="29" spans="1:40" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -11966,7 +11978,7 @@
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
-      <c r="AM29" s="738"/>
+      <c r="AM29" s="550"/>
       <c r="AN29" s="142"/>
     </row>
     <row r="30" spans="1:40" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -12026,7 +12038,7 @@
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
-      <c r="AM30" s="738"/>
+      <c r="AM30" s="550"/>
       <c r="AN30" s="142"/>
     </row>
     <row r="31" spans="1:40" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -12097,7 +12109,7 @@
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
-      <c r="AM31" s="738"/>
+      <c r="AM31" s="550"/>
       <c r="AN31" s="142"/>
     </row>
     <row r="32" spans="1:40" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -12184,7 +12196,7 @@
       <c r="AL32" s="6" t="s">
         <v>466</v>
       </c>
-      <c r="AM32" s="735" t="s">
+      <c r="AM32" s="547" t="s">
         <v>467</v>
       </c>
       <c r="AN32" s="107" t="s">
@@ -12252,7 +12264,7 @@
         <v>0</v>
       </c>
       <c r="AL33" s="6"/>
-      <c r="AM33" s="738"/>
+      <c r="AM33" s="550"/>
       <c r="AN33" s="142"/>
     </row>
     <row r="34" spans="3:40" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -12333,7 +12345,7 @@
         <v>1</v>
       </c>
       <c r="AL34" s="6"/>
-      <c r="AM34" s="735" t="s">
+      <c r="AM34" s="547" t="s">
         <v>589</v>
       </c>
       <c r="AN34" s="142" t="s">
@@ -12415,7 +12427,7 @@
       <c r="AL35" s="6" t="s">
         <v>314</v>
       </c>
-      <c r="AM35" s="735"/>
+      <c r="AM35" s="547"/>
       <c r="AN35" s="142"/>
     </row>
     <row r="36" spans="3:40" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -12492,7 +12504,7 @@
       <c r="AL36" s="6" t="s">
         <v>313</v>
       </c>
-      <c r="AM36" s="738"/>
+      <c r="AM36" s="550"/>
       <c r="AN36" s="142" t="s">
         <v>590</v>
       </c>
@@ -12633,15 +12645,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B1" s="556" t="s">
+      <c r="B1" s="561" t="s">
         <v>317</v>
       </c>
-      <c r="C1" s="607"/>
+      <c r="C1" s="612"/>
       <c r="D1" s="209"/>
-      <c r="J1" s="556" t="s">
+      <c r="J1" s="561" t="s">
         <v>70</v>
       </c>
-      <c r="K1" s="607"/>
+      <c r="K1" s="612"/>
       <c r="L1" s="200" t="s">
         <v>337</v>
       </c>
@@ -12679,13 +12691,13 @@
         <v>34</v>
       </c>
       <c r="L2" s="201"/>
-      <c r="M2" s="682"/>
+      <c r="M2" s="687"/>
       <c r="N2" s="154">
         <v>2</v>
       </c>
       <c r="O2" s="155"/>
       <c r="P2" s="5"/>
-      <c r="Q2" s="685" t="s">
+      <c r="Q2" s="690" t="s">
         <v>44</v>
       </c>
       <c r="R2" s="19">
@@ -12708,13 +12720,13 @@
       <c r="K3" s="6" t="s">
         <v>334</v>
       </c>
-      <c r="M3" s="683"/>
+      <c r="M3" s="688"/>
       <c r="N3" s="17">
         <v>1</v>
       </c>
       <c r="O3" s="15"/>
       <c r="P3" s="10"/>
-      <c r="Q3" s="686"/>
+      <c r="Q3" s="691"/>
       <c r="R3" s="224"/>
     </row>
     <row r="4" spans="2:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -12733,13 +12745,13 @@
       <c r="K4" s="6" t="s">
         <v>335</v>
       </c>
-      <c r="M4" s="683"/>
+      <c r="M4" s="688"/>
       <c r="N4" s="17"/>
       <c r="O4" s="15">
         <v>1</v>
       </c>
       <c r="P4" s="10"/>
-      <c r="Q4" s="686"/>
+      <c r="Q4" s="691"/>
       <c r="R4" s="224"/>
     </row>
     <row r="5" spans="2:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -12759,13 +12771,13 @@
         <v>13</v>
       </c>
       <c r="L5" s="201"/>
-      <c r="M5" s="683"/>
+      <c r="M5" s="688"/>
       <c r="N5" s="17">
         <v>1</v>
       </c>
       <c r="O5" s="15"/>
       <c r="P5" s="10"/>
-      <c r="Q5" s="686"/>
+      <c r="Q5" s="691"/>
       <c r="R5" s="19">
         <v>-1</v>
       </c>
@@ -12786,13 +12798,13 @@
       <c r="K6" s="6" t="s">
         <v>333</v>
       </c>
-      <c r="M6" s="683"/>
+      <c r="M6" s="688"/>
       <c r="N6" s="17">
         <v>1</v>
       </c>
       <c r="O6" s="15"/>
       <c r="P6" s="10"/>
-      <c r="Q6" s="686"/>
+      <c r="Q6" s="691"/>
       <c r="R6" s="224"/>
     </row>
     <row r="7" spans="2:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -12812,13 +12824,13 @@
         <v>334</v>
       </c>
       <c r="L7" s="203"/>
-      <c r="M7" s="683"/>
+      <c r="M7" s="688"/>
       <c r="N7" s="17">
         <v>1</v>
       </c>
       <c r="O7" s="15"/>
       <c r="P7" s="10"/>
-      <c r="Q7" s="686"/>
+      <c r="Q7" s="691"/>
       <c r="R7" s="19">
         <v>-1</v>
       </c>
@@ -12839,13 +12851,13 @@
       <c r="K8" s="6" t="s">
         <v>332</v>
       </c>
-      <c r="M8" s="683"/>
+      <c r="M8" s="688"/>
       <c r="N8" s="17">
         <v>1</v>
       </c>
       <c r="O8" s="15"/>
       <c r="P8" s="10"/>
-      <c r="Q8" s="686"/>
+      <c r="Q8" s="691"/>
       <c r="R8" s="224"/>
     </row>
     <row r="9" spans="2:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -12865,13 +12877,13 @@
         <v>336</v>
       </c>
       <c r="L9" s="185"/>
-      <c r="M9" s="684"/>
+      <c r="M9" s="689"/>
       <c r="N9" s="163"/>
       <c r="O9" s="18"/>
       <c r="P9" s="13">
         <v>1</v>
       </c>
-      <c r="Q9" s="687"/>
+      <c r="Q9" s="692"/>
       <c r="R9" s="225"/>
     </row>
     <row r="10" spans="2:18" x14ac:dyDescent="0.25">
@@ -13029,10 +13041,10 @@
         <f ca="1">TODAY()</f>
         <v>45279</v>
       </c>
-      <c r="V1" s="556" t="s">
+      <c r="V1" s="561" t="s">
         <v>71</v>
       </c>
-      <c r="W1" s="607"/>
+      <c r="W1" s="612"/>
       <c r="X1" s="62" t="s">
         <v>102</v>
       </c>
@@ -13051,7 +13063,7 @@
       <c r="AC1" s="116" t="s">
         <v>191</v>
       </c>
-      <c r="AD1" s="695" t="s">
+      <c r="AD1" s="700" t="s">
         <v>213</v>
       </c>
       <c r="AE1" s="116" t="s">
@@ -13068,10 +13080,10 @@
       <c r="E2" s="39" t="s">
         <v>74</v>
       </c>
-      <c r="F2" s="694" t="s">
+      <c r="F2" s="699" t="s">
         <v>75</v>
       </c>
-      <c r="G2" s="722" t="s">
+      <c r="G2" s="727" t="s">
         <v>44</v>
       </c>
       <c r="H2" s="40" t="s">
@@ -13099,10 +13111,10 @@
       <c r="U2" s="60" t="s">
         <v>106</v>
       </c>
-      <c r="V2" s="663" t="s">
+      <c r="V2" s="668" t="s">
         <v>121</v>
       </c>
-      <c r="W2" s="664"/>
+      <c r="W2" s="669"/>
       <c r="X2" s="64" t="s">
         <v>110</v>
       </c>
@@ -13121,7 +13133,7 @@
       <c r="AC2" s="117" t="s">
         <v>99</v>
       </c>
-      <c r="AD2" s="696"/>
+      <c r="AD2" s="701"/>
       <c r="AE2" s="64" t="s">
         <v>99</v>
       </c>
@@ -13140,8 +13152,8 @@
       <c r="E3" s="39" t="s">
         <v>80</v>
       </c>
-      <c r="F3" s="655"/>
-      <c r="G3" s="723"/>
+      <c r="F3" s="660"/>
+      <c r="G3" s="728"/>
       <c r="H3" s="40" t="s">
         <v>81</v>
       </c>
@@ -13152,13 +13164,13 @@
         <v>82</v>
       </c>
       <c r="N3" s="44"/>
-      <c r="O3" s="732" t="s">
+      <c r="O3" s="737" t="s">
         <v>44</v>
       </c>
-      <c r="P3" s="714" t="s">
+      <c r="P3" s="719" t="s">
         <v>219</v>
       </c>
-      <c r="Q3" s="715"/>
+      <c r="Q3" s="720"/>
       <c r="S3" s="57" t="s">
         <v>220</v>
       </c>
@@ -13168,15 +13180,15 @@
       <c r="W3" s="59" t="s">
         <v>105</v>
       </c>
-      <c r="AD3" s="696"/>
+      <c r="AD3" s="701"/>
     </row>
     <row r="4" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="G4" s="723"/>
+      <c r="G4" s="728"/>
       <c r="H4" s="6"/>
-      <c r="L4" s="685" t="s">
+      <c r="L4" s="690" t="s">
         <v>83</v>
       </c>
-      <c r="O4" s="733"/>
+      <c r="O4" s="738"/>
       <c r="T4" s="55" t="s">
         <v>98</v>
       </c>
@@ -13186,12 +13198,12 @@
       <c r="X4" s="67" t="s">
         <v>223</v>
       </c>
-      <c r="Y4" s="556" t="s">
+      <c r="Y4" s="561" t="s">
         <v>195</v>
       </c>
-      <c r="Z4" s="558"/>
-      <c r="AA4" s="607"/>
-      <c r="AD4" s="696"/>
+      <c r="Z4" s="563"/>
+      <c r="AA4" s="612"/>
+      <c r="AD4" s="701"/>
     </row>
     <row r="5" spans="1:31" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C5" s="52" t="s">
@@ -13206,21 +13218,21 @@
       <c r="F5" s="66" t="s">
         <v>85</v>
       </c>
-      <c r="G5" s="723"/>
+      <c r="G5" s="728"/>
       <c r="H5" s="46" t="s">
         <v>76</v>
       </c>
-      <c r="K5" s="701" t="s">
+      <c r="K5" s="706" t="s">
         <v>217</v>
       </c>
-      <c r="L5" s="716"/>
+      <c r="L5" s="721"/>
       <c r="M5" s="2" t="s">
         <v>215</v>
       </c>
       <c r="N5" s="61" t="s">
         <v>214</v>
       </c>
-      <c r="O5" s="733"/>
+      <c r="O5" s="738"/>
       <c r="P5" s="108" t="s">
         <v>216</v>
       </c>
@@ -13236,11 +13248,11 @@
       <c r="U5" s="19" t="s">
         <v>99</v>
       </c>
-      <c r="Y5" s="704" t="s">
+      <c r="Y5" s="709" t="s">
         <v>287</v>
       </c>
-      <c r="Z5" s="705"/>
-      <c r="AD5" s="696"/>
+      <c r="Z5" s="710"/>
+      <c r="AD5" s="701"/>
     </row>
     <row r="6" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C6" s="109"/>
@@ -13250,16 +13262,16 @@
       <c r="E6" s="45" t="s">
         <v>86</v>
       </c>
-      <c r="G6" s="723"/>
+      <c r="G6" s="728"/>
       <c r="H6" s="46" t="s">
         <v>81</v>
       </c>
       <c r="I6" s="23">
         <v>15</v>
       </c>
-      <c r="K6" s="702"/>
-      <c r="L6" s="716"/>
-      <c r="O6" s="733"/>
+      <c r="K6" s="707"/>
+      <c r="L6" s="721"/>
+      <c r="O6" s="738"/>
       <c r="T6" s="2" t="s">
         <v>101</v>
       </c>
@@ -13269,23 +13281,23 @@
       <c r="V6" s="21">
         <v>-1</v>
       </c>
-      <c r="AD6" s="696"/>
+      <c r="AD6" s="701"/>
     </row>
     <row r="7" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C7" s="110"/>
-      <c r="G7" s="723"/>
+      <c r="G7" s="728"/>
       <c r="H7" s="6"/>
-      <c r="K7" s="702"/>
-      <c r="L7" s="716"/>
+      <c r="K7" s="707"/>
+      <c r="L7" s="721"/>
       <c r="N7" s="21" t="s">
         <v>120</v>
       </c>
-      <c r="O7" s="733"/>
+      <c r="O7" s="738"/>
       <c r="P7" s="73"/>
       <c r="U7" s="104" t="s">
         <v>20</v>
       </c>
-      <c r="AD7" s="696"/>
+      <c r="AD7" s="701"/>
     </row>
     <row r="8" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C8" s="130"/>
@@ -13298,7 +13310,7 @@
       <c r="F8" s="66" t="s">
         <v>87</v>
       </c>
-      <c r="G8" s="723"/>
+      <c r="G8" s="728"/>
       <c r="H8" s="50" t="s">
         <v>76</v>
       </c>
@@ -13308,41 +13320,41 @@
       <c r="J8" s="111">
         <v>115</v>
       </c>
-      <c r="K8" s="702"/>
-      <c r="L8" s="716"/>
-      <c r="O8" s="733"/>
+      <c r="K8" s="707"/>
+      <c r="L8" s="721"/>
+      <c r="O8" s="738"/>
       <c r="P8" s="49"/>
-      <c r="S8" s="698" t="s">
+      <c r="S8" s="703" t="s">
         <v>212</v>
       </c>
-      <c r="T8" s="699"/>
-      <c r="U8" s="699"/>
-      <c r="V8" s="699"/>
-      <c r="W8" s="699"/>
-      <c r="X8" s="699"/>
-      <c r="Y8" s="699"/>
-      <c r="Z8" s="699"/>
-      <c r="AA8" s="699"/>
-      <c r="AB8" s="699"/>
-      <c r="AC8" s="700"/>
-      <c r="AD8" s="696"/>
+      <c r="T8" s="704"/>
+      <c r="U8" s="704"/>
+      <c r="V8" s="704"/>
+      <c r="W8" s="704"/>
+      <c r="X8" s="704"/>
+      <c r="Y8" s="704"/>
+      <c r="Z8" s="704"/>
+      <c r="AA8" s="704"/>
+      <c r="AB8" s="704"/>
+      <c r="AC8" s="705"/>
+      <c r="AD8" s="701"/>
     </row>
     <row r="9" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C9" s="688"/>
-      <c r="G9" s="723"/>
+      <c r="C9" s="693"/>
+      <c r="G9" s="728"/>
       <c r="H9" s="6"/>
-      <c r="K9" s="702"/>
-      <c r="L9" s="726" t="s">
+      <c r="K9" s="707"/>
+      <c r="L9" s="731" t="s">
         <v>218</v>
       </c>
-      <c r="M9" s="727"/>
-      <c r="N9" s="728"/>
-      <c r="O9" s="733"/>
+      <c r="M9" s="732"/>
+      <c r="N9" s="733"/>
+      <c r="O9" s="738"/>
       <c r="P9" s="75"/>
-      <c r="AD9" s="696"/>
+      <c r="AD9" s="701"/>
     </row>
     <row r="10" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C10" s="689"/>
+      <c r="C10" s="694"/>
       <c r="D10" s="23"/>
       <c r="E10" s="45" t="s">
         <v>88</v>
@@ -13350,7 +13362,7 @@
       <c r="F10" s="66" t="s">
         <v>89</v>
       </c>
-      <c r="G10" s="723"/>
+      <c r="G10" s="728"/>
       <c r="H10" s="51"/>
       <c r="I10" s="21" t="s">
         <v>81</v>
@@ -13358,33 +13370,33 @@
       <c r="J10" s="3">
         <v>15</v>
       </c>
-      <c r="K10" s="702"/>
-      <c r="M10" s="691" t="s">
+      <c r="K10" s="707"/>
+      <c r="M10" s="696" t="s">
         <v>90</v>
       </c>
-      <c r="N10" s="692"/>
-      <c r="O10" s="692"/>
-      <c r="P10" s="692"/>
-      <c r="Q10" s="692"/>
-      <c r="R10" s="692"/>
-      <c r="S10" s="692"/>
-      <c r="T10" s="692"/>
-      <c r="U10" s="692"/>
-      <c r="V10" s="692"/>
-      <c r="W10" s="692"/>
-      <c r="X10" s="692"/>
-      <c r="Y10" s="692"/>
-      <c r="Z10" s="692"/>
-      <c r="AA10" s="692"/>
-      <c r="AB10" s="692"/>
-      <c r="AC10" s="693"/>
-      <c r="AD10" s="696"/>
+      <c r="N10" s="697"/>
+      <c r="O10" s="697"/>
+      <c r="P10" s="697"/>
+      <c r="Q10" s="697"/>
+      <c r="R10" s="697"/>
+      <c r="S10" s="697"/>
+      <c r="T10" s="697"/>
+      <c r="U10" s="697"/>
+      <c r="V10" s="697"/>
+      <c r="W10" s="697"/>
+      <c r="X10" s="697"/>
+      <c r="Y10" s="697"/>
+      <c r="Z10" s="697"/>
+      <c r="AA10" s="697"/>
+      <c r="AB10" s="697"/>
+      <c r="AC10" s="698"/>
+      <c r="AD10" s="701"/>
     </row>
     <row r="11" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C11" s="690"/>
-      <c r="G11" s="723"/>
+      <c r="C11" s="695"/>
+      <c r="G11" s="728"/>
       <c r="H11" s="6"/>
-      <c r="K11" s="702"/>
+      <c r="K11" s="707"/>
       <c r="R11" s="52" t="s">
         <v>44</v>
       </c>
@@ -13392,17 +13404,17 @@
       <c r="Y11" s="68" t="s">
         <v>121</v>
       </c>
-      <c r="Z11" s="712" t="s">
+      <c r="Z11" s="717" t="s">
         <v>121</v>
       </c>
-      <c r="AA11" s="713"/>
+      <c r="AA11" s="718"/>
       <c r="AB11" s="52" t="s">
         <v>44</v>
       </c>
       <c r="AC11" s="118" t="s">
         <v>121</v>
       </c>
-      <c r="AD11" s="696"/>
+      <c r="AD11" s="701"/>
     </row>
     <row r="12" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C12" s="129"/>
@@ -13415,7 +13427,7 @@
       <c r="F12" s="66" t="s">
         <v>92</v>
       </c>
-      <c r="G12" s="723"/>
+      <c r="G12" s="728"/>
       <c r="H12" s="128"/>
       <c r="I12" s="19" t="s">
         <v>81</v>
@@ -13423,8 +13435,8 @@
       <c r="J12" s="3">
         <v>15</v>
       </c>
-      <c r="K12" s="702"/>
-      <c r="L12" s="717" t="s">
+      <c r="K12" s="707"/>
+      <c r="L12" s="722" t="s">
         <v>93</v>
       </c>
       <c r="M12" s="21" t="s">
@@ -13439,7 +13451,7 @@
       <c r="Q12" s="113" t="s">
         <v>44</v>
       </c>
-      <c r="S12" s="551" t="s">
+      <c r="S12" s="556" t="s">
         <v>107</v>
       </c>
       <c r="T12" s="2" t="s">
@@ -13455,26 +13467,26 @@
         <v>116</v>
       </c>
       <c r="Y12" s="6"/>
-      <c r="AA12" s="706" t="s">
+      <c r="AA12" s="711" t="s">
         <v>126</v>
       </c>
-      <c r="AB12" s="707"/>
+      <c r="AB12" s="712"/>
       <c r="AC12" s="21" t="s">
         <v>233</v>
       </c>
-      <c r="AD12" s="696"/>
+      <c r="AD12" s="701"/>
     </row>
     <row r="13" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C13" s="688"/>
-      <c r="G13" s="723"/>
-      <c r="K13" s="702"/>
-      <c r="L13" s="718"/>
+      <c r="C13" s="693"/>
+      <c r="G13" s="728"/>
+      <c r="K13" s="707"/>
+      <c r="L13" s="723"/>
       <c r="M13" s="47"/>
-      <c r="Q13" s="725" t="s">
+      <c r="Q13" s="730" t="s">
         <v>210</v>
       </c>
-      <c r="R13" s="622"/>
-      <c r="S13" s="552"/>
+      <c r="R13" s="627"/>
+      <c r="S13" s="557"/>
       <c r="T13" s="6"/>
       <c r="U13" s="96" t="s">
         <v>132</v>
@@ -13482,17 +13494,17 @@
       <c r="X13" s="2" t="s">
         <v>123</v>
       </c>
-      <c r="AA13" s="708"/>
-      <c r="AB13" s="709"/>
-      <c r="AD13" s="696"/>
+      <c r="AA13" s="713"/>
+      <c r="AB13" s="714"/>
+      <c r="AD13" s="701"/>
     </row>
     <row r="14" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B14" s="2" t="s">
         <v>339</v>
       </c>
-      <c r="C14" s="690"/>
+      <c r="C14" s="695"/>
       <c r="D14" s="23"/>
-      <c r="G14" s="723"/>
+      <c r="G14" s="728"/>
       <c r="H14" s="125"/>
       <c r="I14" s="99" t="s">
         <v>44</v>
@@ -13500,8 +13512,8 @@
       <c r="J14" s="111">
         <v>115</v>
       </c>
-      <c r="K14" s="702"/>
-      <c r="L14" s="718"/>
+      <c r="K14" s="707"/>
+      <c r="L14" s="723"/>
       <c r="M14" s="21" t="s">
         <v>111</v>
       </c>
@@ -13511,7 +13523,7 @@
       <c r="R14" s="115" t="s">
         <v>44</v>
       </c>
-      <c r="S14" s="552"/>
+      <c r="S14" s="557"/>
       <c r="T14" s="77" t="s">
         <v>130</v>
       </c>
@@ -13522,9 +13534,9 @@
       <c r="Y14" s="21" t="s">
         <v>73</v>
       </c>
-      <c r="AA14" s="708"/>
-      <c r="AB14" s="709"/>
-      <c r="AD14" s="696"/>
+      <c r="AA14" s="713"/>
+      <c r="AB14" s="714"/>
+      <c r="AD14" s="701"/>
     </row>
     <row r="15" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C15" s="130" t="s">
@@ -13539,20 +13551,20 @@
       <c r="F15" s="66" t="s">
         <v>94</v>
       </c>
-      <c r="G15" s="723"/>
+      <c r="G15" s="728"/>
       <c r="H15" s="2" t="s">
         <v>81</v>
       </c>
       <c r="I15" s="53" t="s">
         <v>81</v>
       </c>
-      <c r="K15" s="702"/>
-      <c r="L15" s="719"/>
-      <c r="Q15" s="725" t="s">
+      <c r="K15" s="707"/>
+      <c r="L15" s="724"/>
+      <c r="Q15" s="730" t="s">
         <v>211</v>
       </c>
-      <c r="R15" s="622"/>
-      <c r="S15" s="552"/>
+      <c r="R15" s="627"/>
+      <c r="S15" s="557"/>
       <c r="T15" s="6"/>
       <c r="V15" s="68" t="s">
         <v>44</v>
@@ -13560,14 +13572,14 @@
       <c r="X15" s="2" t="s">
         <v>128</v>
       </c>
-      <c r="AA15" s="708"/>
-      <c r="AB15" s="709"/>
-      <c r="AD15" s="696"/>
+      <c r="AA15" s="713"/>
+      <c r="AB15" s="714"/>
+      <c r="AD15" s="701"/>
     </row>
     <row r="16" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C16" s="132"/>
-      <c r="G16" s="723"/>
-      <c r="K16" s="702"/>
+      <c r="G16" s="728"/>
+      <c r="K16" s="707"/>
       <c r="N16" s="47"/>
       <c r="O16" s="61" t="s">
         <v>109</v>
@@ -13575,7 +13587,7 @@
       <c r="R16" s="114" t="s">
         <v>44</v>
       </c>
-      <c r="S16" s="552"/>
+      <c r="S16" s="557"/>
       <c r="T16" s="76" t="s">
         <v>129</v>
       </c>
@@ -13586,34 +13598,34 @@
       <c r="Z16" s="76" t="s">
         <v>127</v>
       </c>
-      <c r="AA16" s="708"/>
-      <c r="AB16" s="709"/>
-      <c r="AD16" s="696"/>
+      <c r="AA16" s="713"/>
+      <c r="AB16" s="714"/>
+      <c r="AD16" s="701"/>
     </row>
     <row r="17" spans="3:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C17" s="109"/>
       <c r="E17" s="6" t="s">
         <v>95</v>
       </c>
-      <c r="F17" s="720" t="s">
+      <c r="F17" s="725" t="s">
         <v>96</v>
       </c>
-      <c r="G17" s="723"/>
+      <c r="G17" s="728"/>
       <c r="H17" s="54"/>
       <c r="I17" s="133" t="s">
         <v>81</v>
       </c>
-      <c r="K17" s="702"/>
-      <c r="S17" s="552"/>
+      <c r="K17" s="707"/>
+      <c r="S17" s="557"/>
       <c r="V17" s="68" t="s">
         <v>44</v>
       </c>
       <c r="X17" s="2" t="s">
         <v>118</v>
       </c>
-      <c r="AA17" s="708"/>
-      <c r="AB17" s="709"/>
-      <c r="AD17" s="696"/>
+      <c r="AA17" s="713"/>
+      <c r="AB17" s="714"/>
+      <c r="AD17" s="701"/>
     </row>
     <row r="18" spans="3:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C18" s="130"/>
@@ -13623,50 +13635,50 @@
       <c r="E18" s="6" t="s">
         <v>97</v>
       </c>
-      <c r="F18" s="721"/>
-      <c r="G18" s="723"/>
+      <c r="F18" s="726"/>
+      <c r="G18" s="728"/>
       <c r="H18" s="108" t="s">
         <v>76</v>
       </c>
       <c r="I18" s="21" t="s">
         <v>81</v>
       </c>
-      <c r="K18" s="702"/>
+      <c r="K18" s="707"/>
       <c r="O18" s="64" t="s">
         <v>115</v>
       </c>
-      <c r="S18" s="552"/>
+      <c r="S18" s="557"/>
       <c r="U18" s="76" t="s">
         <v>133</v>
       </c>
       <c r="X18" s="2" t="s">
         <v>117</v>
       </c>
-      <c r="AA18" s="710"/>
-      <c r="AB18" s="711"/>
-      <c r="AD18" s="696"/>
+      <c r="AA18" s="715"/>
+      <c r="AB18" s="716"/>
+      <c r="AD18" s="701"/>
     </row>
     <row r="19" spans="3:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="F19" s="64" t="s">
         <v>209</v>
       </c>
-      <c r="G19" s="724"/>
-      <c r="K19" s="703"/>
+      <c r="G19" s="729"/>
+      <c r="K19" s="708"/>
       <c r="Q19" s="68" t="s">
         <v>44</v>
       </c>
-      <c r="R19" s="729" t="s">
+      <c r="R19" s="734" t="s">
         <v>124</v>
       </c>
-      <c r="S19" s="730"/>
-      <c r="T19" s="731"/>
+      <c r="S19" s="735"/>
+      <c r="T19" s="736"/>
       <c r="V19" s="77" t="s">
         <v>115</v>
       </c>
       <c r="Y19" s="19" t="s">
         <v>125</v>
       </c>
-      <c r="AD19" s="697"/>
+      <c r="AD19" s="702"/>
     </row>
   </sheetData>
   <mergeCells count="24">

</xml_diff>

<commit_message>
Boat Enabled - RBharat
Boat Enabled - RBharat
</commit_message>
<xml_diff>
--- a/System_2.1.5.xlsx
+++ b/System_2.1.5.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Work\Work_For_\Work\Running AppS\System_Work_RW\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4569098-7FAE-41E1-8561-514C4ED0CAD2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5063E981-829C-4FB7-8B45-B1FECF901B3C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="BoardRW" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1082" uniqueCount="613">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1083" uniqueCount="613">
   <si>
     <t>Zone</t>
   </si>
@@ -4830,6 +4830,63 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="255" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="32" fillId="27" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="27" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="27" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="13" fillId="27" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="13" fillId="27" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="27" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="27" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="27" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="27" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="19" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="19" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="36" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="36" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="39" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -4860,62 +4917,167 @@
     <xf numFmtId="0" fontId="6" fillId="18" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="255"/>
     </xf>
-    <xf numFmtId="0" fontId="32" fillId="27" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="73" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="57" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="11" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="11" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="13" fillId="27" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="13" fillId="27" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="27" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="27" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="27" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="27" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="36" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="36" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="3" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="18" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="18" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="18" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="32" fillId="27" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="32" fillId="27" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="14" fontId="13" fillId="27" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="49" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="49" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="49" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="14" fontId="13" fillId="27" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="32" fillId="27" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="27" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="27" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="27" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="19" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="19" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="36" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="36" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="52" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="54" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="16" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="16" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="19" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -4941,12 +5103,6 @@
     <xf numFmtId="0" fontId="38" fillId="7" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255"/>
-    </xf>
     <xf numFmtId="0" fontId="17" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="255"/>
     </xf>
@@ -4968,161 +5124,14 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="52" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="54" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="16" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="16" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="3" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="18" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="18" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="18" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="49" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="49" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="49" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="73" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="57" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="11" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="11" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="13" fillId="27" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="13" fillId="27" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="27" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="27" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="27" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="27" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="36" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="36" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="11" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="3" fillId="35" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="35" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="35" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="43" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -5181,15 +5190,6 @@
     <xf numFmtId="0" fontId="6" fillId="52" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="35" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="35" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="35" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -5208,25 +5208,46 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="30" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="30" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="30" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="24" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="24" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="24" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="18" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -5304,46 +5325,25 @@
     <xf numFmtId="0" fontId="3" fillId="21" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="30" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="30" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="30" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="24" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="24" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="24" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -5637,7 +5637,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B1:W28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="W6" sqref="W6"/>
     </sheetView>
   </sheetViews>
@@ -6597,8 +6597,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AB54FD83-008D-4F8B-87AC-83E7F70047CB}">
   <dimension ref="A1:AA32"/>
   <sheetViews>
-    <sheetView topLeftCell="H13" workbookViewId="0">
-      <selection activeCell="Z19" sqref="Z19"/>
+    <sheetView topLeftCell="H1" workbookViewId="0">
+      <selection activeCell="T14" sqref="T14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6655,7 +6655,7 @@
       <c r="P1" s="422" t="s">
         <v>407</v>
       </c>
-      <c r="Q1" s="567" t="s">
+      <c r="Q1" s="586" t="s">
         <v>181</v>
       </c>
       <c r="R1" s="100" t="s">
@@ -6675,32 +6675,32 @@
       </c>
     </row>
     <row r="2" spans="1:27" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="580">
+      <c r="A2" s="570">
         <f ca="1">TODAY()</f>
         <v>45279</v>
       </c>
-      <c r="B2" s="582" t="s">
+      <c r="B2" s="572" t="s">
         <v>388</v>
       </c>
-      <c r="C2" s="594" t="s">
+      <c r="C2" s="584" t="s">
         <v>364</v>
       </c>
-      <c r="D2" s="584" t="s">
+      <c r="D2" s="574" t="s">
         <v>103</v>
       </c>
-      <c r="E2" s="586" t="s">
+      <c r="E2" s="576" t="s">
         <v>65</v>
       </c>
       <c r="F2" s="196" t="s">
         <v>220</v>
       </c>
-      <c r="G2" s="592" t="s">
+      <c r="G2" s="582" t="s">
         <v>380</v>
       </c>
       <c r="H2" s="211" t="s">
         <v>220</v>
       </c>
-      <c r="I2" s="574" t="s">
+      <c r="I2" s="593" t="s">
         <v>103</v>
       </c>
       <c r="J2" s="420" t="s">
@@ -6724,7 +6724,7 @@
       <c r="P2" s="423">
         <v>40</v>
       </c>
-      <c r="Q2" s="568"/>
+      <c r="Q2" s="587"/>
       <c r="R2" s="21">
         <f>R7+R18</f>
         <v>6</v>
@@ -6750,14 +6750,14 @@
       </c>
     </row>
     <row r="3" spans="1:27" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="581"/>
-      <c r="B3" s="583"/>
-      <c r="C3" s="595"/>
-      <c r="D3" s="585"/>
-      <c r="E3" s="587"/>
-      <c r="G3" s="593"/>
+      <c r="A3" s="571"/>
+      <c r="B3" s="573"/>
+      <c r="C3" s="585"/>
+      <c r="D3" s="575"/>
+      <c r="E3" s="577"/>
+      <c r="G3" s="583"/>
       <c r="H3" s="6"/>
-      <c r="I3" s="575"/>
+      <c r="I3" s="594"/>
       <c r="K3" s="24">
         <v>2</v>
       </c>
@@ -6782,10 +6782,10 @@
         <v>389</v>
       </c>
       <c r="B4" s="248"/>
-      <c r="C4" s="588" t="s">
+      <c r="C4" s="578" t="s">
         <v>178</v>
       </c>
-      <c r="I4" s="575"/>
+      <c r="I4" s="594"/>
       <c r="R4" s="498" t="s">
         <v>579</v>
       </c>
@@ -6809,7 +6809,7 @@
       <c r="B5" s="100" t="s">
         <v>364</v>
       </c>
-      <c r="C5" s="589"/>
+      <c r="C5" s="579"/>
       <c r="D5" s="227" t="s">
         <v>103</v>
       </c>
@@ -6825,7 +6825,7 @@
       <c r="H5" s="211" t="s">
         <v>220</v>
       </c>
-      <c r="I5" s="575"/>
+      <c r="I5" s="594"/>
       <c r="J5" s="421" t="s">
         <v>273</v>
       </c>
@@ -6856,22 +6856,22 @@
       <c r="X5" s="494"/>
     </row>
     <row r="6" spans="1:27" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="577" t="s">
+      <c r="A6" s="567" t="s">
         <v>290</v>
       </c>
       <c r="B6" s="105" t="s">
         <v>199</v>
       </c>
-      <c r="C6" s="590"/>
-      <c r="D6" s="591"/>
+      <c r="C6" s="580"/>
+      <c r="D6" s="581"/>
       <c r="E6" s="96">
         <v>1</v>
       </c>
       <c r="G6" s="557"/>
-      <c r="I6" s="575"/>
+      <c r="I6" s="594"/>
     </row>
     <row r="7" spans="1:27" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="578"/>
+      <c r="A7" s="568"/>
       <c r="B7" s="100" t="s">
         <v>155</v>
       </c>
@@ -6882,7 +6882,7 @@
         <v>136</v>
       </c>
       <c r="G7" s="557"/>
-      <c r="I7" s="575"/>
+      <c r="I7" s="594"/>
       <c r="M7" s="16" t="s">
         <v>354</v>
       </c>
@@ -6918,7 +6918,7 @@
       </c>
     </row>
     <row r="8" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="579"/>
+      <c r="A8" s="569"/>
       <c r="B8" s="217" t="s">
         <v>28</v>
       </c>
@@ -6927,7 +6927,7 @@
         <v>3</v>
       </c>
       <c r="G8" s="557"/>
-      <c r="I8" s="575"/>
+      <c r="I8" s="594"/>
       <c r="N8" s="80"/>
       <c r="U8" s="6" t="s">
         <v>465</v>
@@ -6951,7 +6951,7 @@
       </c>
       <c r="G9" s="557"/>
       <c r="H9" s="6"/>
-      <c r="I9" s="575"/>
+      <c r="I9" s="594"/>
       <c r="M9" s="19" t="s">
         <v>546</v>
       </c>
@@ -6975,10 +6975,10 @@
       <c r="D10" s="108"/>
       <c r="E10" s="68">
         <f>Boat!U8</f>
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="G10" s="557"/>
-      <c r="I10" s="575"/>
+      <c r="I10" s="594"/>
       <c r="J10" s="24" t="s">
         <v>380</v>
       </c>
@@ -7012,7 +7012,7 @@
         <v>270</v>
       </c>
       <c r="G11" s="557"/>
-      <c r="I11" s="575"/>
+      <c r="I11" s="594"/>
       <c r="J11" s="24" t="s">
         <v>195</v>
       </c>
@@ -7038,12 +7038,12 @@
       <c r="S11" s="24">
         <v>1</v>
       </c>
-      <c r="U11" s="569" t="s">
+      <c r="U11" s="588" t="s">
         <v>582</v>
       </c>
-      <c r="V11" s="570"/>
-      <c r="W11" s="570"/>
-      <c r="X11" s="571"/>
+      <c r="V11" s="589"/>
+      <c r="W11" s="589"/>
+      <c r="X11" s="590"/>
     </row>
     <row r="12" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="232" t="s">
@@ -7054,7 +7054,7 @@
         <v>3</v>
       </c>
       <c r="G12" s="557"/>
-      <c r="I12" s="575"/>
+      <c r="I12" s="594"/>
       <c r="J12" s="24" t="s">
         <v>537</v>
       </c>
@@ -7087,7 +7087,7 @@
       </c>
       <c r="D13" s="20"/>
       <c r="G13" s="557"/>
-      <c r="I13" s="575"/>
+      <c r="I13" s="594"/>
       <c r="J13" s="108" t="s">
         <v>571</v>
       </c>
@@ -7128,7 +7128,7 @@
       <c r="H14" s="211" t="s">
         <v>220</v>
       </c>
-      <c r="I14" s="575"/>
+      <c r="I14" s="594"/>
       <c r="U14" s="6"/>
       <c r="V14" s="112"/>
       <c r="W14" s="6"/>
@@ -7146,7 +7146,7 @@
       <c r="H15" s="277">
         <v>0</v>
       </c>
-      <c r="I15" s="575"/>
+      <c r="I15" s="594"/>
       <c r="J15" s="108" t="s">
         <v>154</v>
       </c>
@@ -7177,7 +7177,7 @@
       <c r="D16" s="2" t="s">
         <v>509</v>
       </c>
-      <c r="I16" s="575"/>
+      <c r="I16" s="594"/>
       <c r="K16" s="100" t="s">
         <v>44</v>
       </c>
@@ -7211,7 +7211,7 @@
       <c r="G17" s="2" t="s">
         <v>440</v>
       </c>
-      <c r="I17" s="575"/>
+      <c r="I17" s="594"/>
       <c r="L17" s="2" t="s">
         <v>443</v>
       </c>
@@ -7223,13 +7223,13 @@
     </row>
     <row r="18" spans="1:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="G18" s="16"/>
-      <c r="I18" s="575"/>
+      <c r="I18" s="594"/>
       <c r="L18" s="16"/>
       <c r="M18" s="21"/>
-      <c r="O18" s="572" t="s">
+      <c r="O18" s="591" t="s">
         <v>538</v>
       </c>
-      <c r="P18" s="573"/>
+      <c r="P18" s="592"/>
       <c r="Q18" s="127" t="s">
         <v>44</v>
       </c>
@@ -7255,7 +7255,7 @@
       </c>
     </row>
     <row r="19" spans="1:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="I19" s="575"/>
+      <c r="I19" s="594"/>
       <c r="M19" s="21" t="s">
         <v>442</v>
       </c>
@@ -7287,7 +7287,7 @@
       <c r="G20" s="2" t="s">
         <v>440</v>
       </c>
-      <c r="I20" s="575"/>
+      <c r="I20" s="594"/>
       <c r="K20" s="19" t="s">
         <v>439</v>
       </c>
@@ -7312,7 +7312,7 @@
       <c r="Z20" s="112"/>
     </row>
     <row r="21" spans="1:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="I21" s="575"/>
+      <c r="I21" s="594"/>
       <c r="M21" s="221" t="s">
         <v>421</v>
       </c>
@@ -7348,7 +7348,7 @@
       <c r="G22" s="2" t="s">
         <v>440</v>
       </c>
-      <c r="I22" s="575"/>
+      <c r="I22" s="594"/>
       <c r="U22" s="6"/>
       <c r="V22" s="494"/>
       <c r="W22" s="6" t="s">
@@ -7368,13 +7368,13 @@
       <c r="E23" s="289" t="s">
         <v>44</v>
       </c>
-      <c r="I23" s="575"/>
+      <c r="I23" s="594"/>
       <c r="U23" s="6"/>
       <c r="V23" s="24"/>
       <c r="W23" s="6"/>
     </row>
     <row r="24" spans="1:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="I24" s="575"/>
+      <c r="I24" s="594"/>
       <c r="U24" s="354"/>
       <c r="V24" s="497">
         <v>0</v>
@@ -7402,7 +7402,7 @@
       <c r="H25" s="196" t="s">
         <v>271</v>
       </c>
-      <c r="I25" s="575"/>
+      <c r="I25" s="594"/>
       <c r="J25" s="421" t="s">
         <v>274</v>
       </c>
@@ -7447,7 +7447,7 @@
       <c r="H26" s="19" t="s">
         <v>220</v>
       </c>
-      <c r="I26" s="575"/>
+      <c r="I26" s="594"/>
       <c r="K26" s="24">
         <v>15</v>
       </c>
@@ -7482,7 +7482,7 @@
       </c>
     </row>
     <row r="27" spans="1:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="I27" s="575"/>
+      <c r="I27" s="594"/>
       <c r="O27" s="2" t="s">
         <v>99</v>
       </c>
@@ -7509,7 +7509,7 @@
       <c r="E28" s="220">
         <v>2</v>
       </c>
-      <c r="I28" s="575"/>
+      <c r="I28" s="594"/>
       <c r="Q28" s="6"/>
       <c r="R28" s="112"/>
       <c r="T28" s="142"/>
@@ -7531,7 +7531,7 @@
       <c r="H29" s="196" t="s">
         <v>272</v>
       </c>
-      <c r="I29" s="576"/>
+      <c r="I29" s="595"/>
       <c r="J29" s="333"/>
       <c r="L29" s="96" t="s">
         <v>278</v>
@@ -7601,6 +7601,11 @@
     </row>
   </sheetData>
   <mergeCells count="16">
+    <mergeCell ref="Q1:Q2"/>
+    <mergeCell ref="U11:X11"/>
+    <mergeCell ref="O18:P18"/>
+    <mergeCell ref="I2:I29"/>
+    <mergeCell ref="C13:C14"/>
     <mergeCell ref="A6:A8"/>
     <mergeCell ref="G5:G14"/>
     <mergeCell ref="A2:A3"/>
@@ -7612,11 +7617,6 @@
     <mergeCell ref="B11:B12"/>
     <mergeCell ref="G2:G3"/>
     <mergeCell ref="C2:C3"/>
-    <mergeCell ref="Q1:Q2"/>
-    <mergeCell ref="U11:X11"/>
-    <mergeCell ref="O18:P18"/>
-    <mergeCell ref="I2:I29"/>
-    <mergeCell ref="C13:C14"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -7692,7 +7692,7 @@
       <c r="H1" s="97" t="s">
         <v>350</v>
       </c>
-      <c r="I1" s="592" t="s">
+      <c r="I1" s="582" t="s">
         <v>377</v>
       </c>
       <c r="J1" s="2" t="s">
@@ -7753,7 +7753,7 @@
         <v>516</v>
       </c>
       <c r="AM1" s="426"/>
-      <c r="AN1" s="623"/>
+      <c r="AN1" s="620"/>
       <c r="AO1" s="350" t="s">
         <v>486</v>
       </c>
@@ -7762,23 +7762,23 @@
       </c>
     </row>
     <row r="2" spans="1:43" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="647">
+      <c r="A2" s="602">
         <f ca="1">TODAY()</f>
         <v>45279</v>
       </c>
-      <c r="B2" s="649" t="s">
+      <c r="B2" s="604" t="s">
         <v>378</v>
       </c>
-      <c r="C2" s="594" t="s">
+      <c r="C2" s="584" t="s">
         <v>364</v>
       </c>
-      <c r="D2" s="651" t="s">
+      <c r="D2" s="606" t="s">
         <v>362</v>
       </c>
-      <c r="E2" s="596" t="s">
+      <c r="E2" s="650" t="s">
         <v>65</v>
       </c>
-      <c r="F2" s="604" t="s">
+      <c r="F2" s="625" t="s">
         <v>103</v>
       </c>
       <c r="G2" s="417" t="s">
@@ -7787,31 +7787,31 @@
       <c r="H2" s="80" t="s">
         <v>33</v>
       </c>
-      <c r="I2" s="593"/>
+      <c r="I2" s="583"/>
       <c r="J2" s="81" t="s">
         <v>77</v>
       </c>
-      <c r="K2" s="598" t="s">
+      <c r="K2" s="652" t="s">
         <v>349</v>
       </c>
-      <c r="L2" s="599"/>
-      <c r="M2" s="604" t="s">
+      <c r="L2" s="653"/>
+      <c r="M2" s="625" t="s">
         <v>103</v>
       </c>
       <c r="N2" s="69" t="s">
         <v>28</v>
       </c>
-      <c r="O2" s="630" t="s">
+      <c r="O2" s="629" t="s">
         <v>103</v>
       </c>
       <c r="P2" s="85" t="s">
         <v>148</v>
       </c>
-      <c r="Q2" s="594" t="s">
+      <c r="Q2" s="584" t="s">
         <v>144</v>
       </c>
       <c r="R2" s="556"/>
-      <c r="S2" s="617" t="s">
+      <c r="S2" s="642" t="s">
         <v>149</v>
       </c>
       <c r="T2" s="89"/>
@@ -7844,15 +7844,15 @@
         <v>480</v>
       </c>
       <c r="AM2" s="452"/>
-      <c r="AN2" s="624"/>
+      <c r="AN2" s="621"/>
     </row>
     <row r="3" spans="1:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="648"/>
-      <c r="B3" s="650"/>
-      <c r="C3" s="595"/>
-      <c r="D3" s="652"/>
-      <c r="E3" s="597"/>
-      <c r="F3" s="605"/>
+      <c r="A3" s="603"/>
+      <c r="B3" s="605"/>
+      <c r="C3" s="585"/>
+      <c r="D3" s="607"/>
+      <c r="E3" s="651"/>
+      <c r="F3" s="626"/>
       <c r="G3" s="418" t="s">
         <v>28</v>
       </c>
@@ -7871,17 +7871,17 @@
       <c r="L3" s="206" t="s">
         <v>108</v>
       </c>
-      <c r="M3" s="605"/>
+      <c r="M3" s="626"/>
       <c r="N3" s="69" t="s">
         <v>147</v>
       </c>
-      <c r="O3" s="631"/>
+      <c r="O3" s="630"/>
       <c r="P3" s="2" t="s">
         <v>155</v>
       </c>
-      <c r="Q3" s="595"/>
+      <c r="Q3" s="585"/>
       <c r="R3" s="558"/>
-      <c r="S3" s="619"/>
+      <c r="S3" s="643"/>
       <c r="T3" s="89"/>
       <c r="U3" s="124"/>
       <c r="V3" s="120"/>
@@ -7898,7 +7898,7 @@
       <c r="AC3" s="100" t="s">
         <v>497</v>
       </c>
-      <c r="AD3" s="614" t="s">
+      <c r="AD3" s="641" t="s">
         <v>472</v>
       </c>
       <c r="AE3" s="262"/>
@@ -7910,16 +7910,16 @@
       <c r="AK3" s="262"/>
       <c r="AL3" s="16"/>
       <c r="AM3" s="452"/>
-      <c r="AN3" s="624"/>
+      <c r="AN3" s="621"/>
     </row>
     <row r="4" spans="1:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="243" t="s">
         <v>184</v>
       </c>
-      <c r="B4" s="663" t="s">
+      <c r="B4" s="618" t="s">
         <v>381</v>
       </c>
-      <c r="C4" s="594" t="s">
+      <c r="C4" s="584" t="s">
         <v>155</v>
       </c>
       <c r="D4" s="359" t="s">
@@ -7928,7 +7928,7 @@
       <c r="E4" s="396">
         <v>2</v>
       </c>
-      <c r="F4" s="605"/>
+      <c r="F4" s="626"/>
       <c r="G4" s="400" t="s">
         <v>203</v>
       </c>
@@ -7945,11 +7945,11 @@
         <v>151</v>
       </c>
       <c r="L4" s="209"/>
-      <c r="M4" s="605"/>
+      <c r="M4" s="626"/>
       <c r="N4" s="178" t="s">
         <v>70</v>
       </c>
-      <c r="O4" s="631"/>
+      <c r="O4" s="630"/>
       <c r="P4" s="2" t="s">
         <v>192</v>
       </c>
@@ -7976,7 +7976,7 @@
       <c r="AA4" s="313"/>
       <c r="AB4" s="214"/>
       <c r="AC4" s="16"/>
-      <c r="AD4" s="614"/>
+      <c r="AD4" s="641"/>
       <c r="AE4" s="262"/>
       <c r="AF4" s="262"/>
       <c r="AG4" s="16"/>
@@ -7986,37 +7986,37 @@
       <c r="AK4" s="262"/>
       <c r="AL4" s="16"/>
       <c r="AM4" s="452"/>
-      <c r="AN4" s="624"/>
+      <c r="AN4" s="621"/>
       <c r="AO4" s="350" t="s">
         <v>91</v>
       </c>
     </row>
     <row r="5" spans="1:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="592" t="s">
+      <c r="A5" s="582" t="s">
         <v>434</v>
       </c>
-      <c r="B5" s="664"/>
-      <c r="C5" s="595"/>
+      <c r="B5" s="619"/>
+      <c r="C5" s="585"/>
       <c r="D5" s="61" t="s">
         <v>154</v>
       </c>
       <c r="E5" s="397">
         <v>1</v>
       </c>
-      <c r="F5" s="605"/>
-      <c r="G5" s="655" t="s">
+      <c r="F5" s="626"/>
+      <c r="G5" s="610" t="s">
         <v>193</v>
       </c>
-      <c r="H5" s="655"/>
-      <c r="I5" s="655"/>
-      <c r="J5" s="655"/>
-      <c r="K5" s="655"/>
-      <c r="L5" s="656"/>
-      <c r="M5" s="605"/>
+      <c r="H5" s="610"/>
+      <c r="I5" s="610"/>
+      <c r="J5" s="610"/>
+      <c r="K5" s="610"/>
+      <c r="L5" s="611"/>
+      <c r="M5" s="626"/>
       <c r="N5" s="21">
         <v>8</v>
       </c>
-      <c r="O5" s="631"/>
+      <c r="O5" s="630"/>
       <c r="T5" s="89"/>
       <c r="U5" s="124"/>
       <c r="V5" s="120"/>
@@ -8047,24 +8047,24 @@
       <c r="AK5" s="262"/>
       <c r="AL5" s="80"/>
       <c r="AM5" s="452"/>
-      <c r="AN5" s="624"/>
+      <c r="AN5" s="621"/>
     </row>
     <row r="6" spans="1:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="593"/>
-      <c r="B6" s="661" t="s">
+      <c r="A6" s="583"/>
+      <c r="B6" s="616" t="s">
         <v>178</v>
       </c>
-      <c r="C6" s="590"/>
-      <c r="D6" s="591"/>
-      <c r="F6" s="605"/>
-      <c r="G6" s="657"/>
-      <c r="H6" s="657"/>
-      <c r="I6" s="657"/>
-      <c r="J6" s="657"/>
-      <c r="K6" s="657"/>
-      <c r="L6" s="658"/>
-      <c r="M6" s="605"/>
-      <c r="O6" s="631"/>
+      <c r="C6" s="580"/>
+      <c r="D6" s="581"/>
+      <c r="F6" s="626"/>
+      <c r="G6" s="612"/>
+      <c r="H6" s="612"/>
+      <c r="I6" s="612"/>
+      <c r="J6" s="612"/>
+      <c r="K6" s="612"/>
+      <c r="L6" s="613"/>
+      <c r="M6" s="626"/>
+      <c r="O6" s="630"/>
       <c r="T6" s="89"/>
       <c r="U6" s="124"/>
       <c r="V6" s="98" t="s">
@@ -8088,16 +8088,16 @@
       <c r="AF6" s="262"/>
       <c r="AG6" s="262"/>
       <c r="AH6" s="262"/>
-      <c r="AI6" s="613"/>
+      <c r="AI6" s="635"/>
       <c r="AJ6" s="465" t="s">
         <v>475</v>
       </c>
-      <c r="AK6" s="613" t="s">
+      <c r="AK6" s="635" t="s">
         <v>256</v>
       </c>
       <c r="AL6" s="262"/>
       <c r="AM6" s="452"/>
-      <c r="AN6" s="624"/>
+      <c r="AN6" s="621"/>
       <c r="AO6" s="350" t="s">
         <v>487</v>
       </c>
@@ -8106,7 +8106,7 @@
       <c r="A7" s="237" t="s">
         <v>597</v>
       </c>
-      <c r="B7" s="662"/>
+      <c r="B7" s="617"/>
       <c r="C7" s="207" t="s">
         <v>382</v>
       </c>
@@ -8116,7 +8116,7 @@
       <c r="E7" s="271">
         <v>3</v>
       </c>
-      <c r="F7" s="605"/>
+      <c r="F7" s="626"/>
       <c r="G7" s="419">
         <v>0</v>
       </c>
@@ -8135,8 +8135,8 @@
       <c r="L7" s="217">
         <v>0</v>
       </c>
-      <c r="M7" s="605"/>
-      <c r="O7" s="631"/>
+      <c r="M7" s="626"/>
+      <c r="O7" s="630"/>
       <c r="R7" s="99" t="s">
         <v>44</v>
       </c>
@@ -8160,18 +8160,18 @@
       <c r="AD7" s="16"/>
       <c r="AE7" s="262"/>
       <c r="AF7" s="262"/>
-      <c r="AG7" s="614" t="s">
+      <c r="AG7" s="641" t="s">
         <v>471</v>
       </c>
       <c r="AH7" s="262"/>
-      <c r="AI7" s="613"/>
+      <c r="AI7" s="635"/>
       <c r="AJ7" s="262"/>
-      <c r="AK7" s="613"/>
+      <c r="AK7" s="635"/>
       <c r="AL7" s="80" t="s">
         <v>514</v>
       </c>
       <c r="AM7" s="452"/>
-      <c r="AN7" s="624"/>
+      <c r="AN7" s="621"/>
       <c r="AP7" s="76" t="s">
         <v>488</v>
       </c>
@@ -8188,27 +8188,27 @@
         <f>SUM(G7:N9)</f>
         <v>15</v>
       </c>
-      <c r="F8" s="605"/>
-      <c r="G8" s="656">
-        <v>0</v>
-      </c>
-      <c r="H8" s="653" t="s">
+      <c r="F8" s="626"/>
+      <c r="G8" s="611">
+        <v>0</v>
+      </c>
+      <c r="H8" s="608" t="s">
         <v>105</v>
       </c>
       <c r="I8" s="556">
         <v>0</v>
       </c>
-      <c r="J8" s="653" t="s">
+      <c r="J8" s="608" t="s">
         <v>105</v>
       </c>
-      <c r="K8" s="659"/>
-      <c r="L8" s="615"/>
-      <c r="M8" s="628"/>
-      <c r="N8" s="620">
+      <c r="K8" s="614"/>
+      <c r="L8" s="644"/>
+      <c r="M8" s="627"/>
+      <c r="N8" s="647">
         <f>N5+N11</f>
         <v>15</v>
       </c>
-      <c r="O8" s="631"/>
+      <c r="O8" s="630"/>
       <c r="T8" s="103" t="s">
         <v>44</v>
       </c>
@@ -8226,14 +8226,14 @@
       <c r="AD8" s="16"/>
       <c r="AE8" s="262"/>
       <c r="AF8" s="262"/>
-      <c r="AG8" s="614"/>
+      <c r="AG8" s="641"/>
       <c r="AH8" s="262"/>
-      <c r="AI8" s="613"/>
+      <c r="AI8" s="635"/>
       <c r="AJ8" s="262"/>
       <c r="AK8" s="262"/>
       <c r="AL8" s="262"/>
       <c r="AM8" s="452"/>
-      <c r="AN8" s="624"/>
+      <c r="AN8" s="621"/>
     </row>
     <row r="9" spans="1:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="237" t="s">
@@ -8248,17 +8248,17 @@
       <c r="D9" s="360" t="s">
         <v>286</v>
       </c>
-      <c r="F9" s="605"/>
-      <c r="G9" s="658"/>
-      <c r="H9" s="654"/>
+      <c r="F9" s="626"/>
+      <c r="G9" s="613"/>
+      <c r="H9" s="609"/>
       <c r="I9" s="558"/>
-      <c r="J9" s="654"/>
-      <c r="K9" s="660"/>
-      <c r="L9" s="616"/>
-      <c r="M9" s="629"/>
-      <c r="N9" s="621"/>
-      <c r="O9" s="632"/>
-      <c r="S9" s="617" t="s">
+      <c r="J9" s="609"/>
+      <c r="K9" s="615"/>
+      <c r="L9" s="645"/>
+      <c r="M9" s="628"/>
+      <c r="N9" s="648"/>
+      <c r="O9" s="631"/>
+      <c r="S9" s="642" t="s">
         <v>62</v>
       </c>
       <c r="T9" s="89"/>
@@ -8280,16 +8280,16 @@
       </c>
       <c r="AE9" s="262"/>
       <c r="AF9" s="262"/>
-      <c r="AG9" s="614"/>
+      <c r="AG9" s="641"/>
       <c r="AH9" s="262"/>
-      <c r="AI9" s="613"/>
+      <c r="AI9" s="635"/>
       <c r="AJ9" s="80"/>
-      <c r="AK9" s="613" t="s">
+      <c r="AK9" s="635" t="s">
         <v>256</v>
       </c>
       <c r="AL9" s="262"/>
       <c r="AM9" s="452"/>
-      <c r="AN9" s="624"/>
+      <c r="AN9" s="621"/>
       <c r="AP9" s="2" t="s">
         <v>526</v>
       </c>
@@ -8304,22 +8304,22 @@
       <c r="D10" s="142"/>
       <c r="E10" s="242">
         <f>Boat!U8</f>
-        <v>41</v>
-      </c>
-      <c r="F10" s="605"/>
+        <v>40</v>
+      </c>
+      <c r="F10" s="626"/>
       <c r="N10" s="442" t="s">
         <v>406</v>
       </c>
-      <c r="O10" s="607" t="s">
+      <c r="O10" s="659" t="s">
         <v>103</v>
       </c>
-      <c r="P10" s="633" t="s">
+      <c r="P10" s="632" t="s">
         <v>410</v>
       </c>
       <c r="R10" s="74" t="s">
         <v>44</v>
       </c>
-      <c r="S10" s="618"/>
+      <c r="S10" s="646"/>
       <c r="T10" s="89"/>
       <c r="U10" s="123" t="s">
         <v>177</v>
@@ -8349,16 +8349,16 @@
       <c r="AF10" s="243" t="s">
         <v>318</v>
       </c>
-      <c r="AG10" s="614"/>
+      <c r="AG10" s="641"/>
       <c r="AH10" s="80"/>
-      <c r="AI10" s="613"/>
+      <c r="AI10" s="635"/>
       <c r="AJ10" s="262"/>
-      <c r="AK10" s="613"/>
+      <c r="AK10" s="635"/>
       <c r="AL10" s="262"/>
       <c r="AM10" s="466" t="s">
         <v>325</v>
       </c>
-      <c r="AN10" s="624"/>
+      <c r="AN10" s="621"/>
       <c r="AO10" s="209" t="s">
         <v>95</v>
       </c>
@@ -8376,18 +8376,18 @@
       <c r="D11" s="174" t="s">
         <v>362</v>
       </c>
-      <c r="F11" s="605"/>
+      <c r="F11" s="626"/>
       <c r="M11" s="6"/>
       <c r="N11" s="117">
         <v>7</v>
       </c>
-      <c r="O11" s="608"/>
-      <c r="P11" s="634"/>
+      <c r="O11" s="660"/>
+      <c r="P11" s="633"/>
       <c r="Q11" s="65"/>
       <c r="R11" s="120" t="s">
         <v>222</v>
       </c>
-      <c r="S11" s="618"/>
+      <c r="S11" s="646"/>
       <c r="T11" s="102" t="s">
         <v>44</v>
       </c>
@@ -8411,14 +8411,14 @@
       <c r="AF11" s="262" t="s">
         <v>493</v>
       </c>
-      <c r="AG11" s="614"/>
+      <c r="AG11" s="641"/>
       <c r="AH11" s="262"/>
       <c r="AI11" s="70"/>
       <c r="AJ11" s="262"/>
       <c r="AK11" s="262"/>
       <c r="AL11" s="262"/>
       <c r="AM11" s="452"/>
-      <c r="AN11" s="624"/>
+      <c r="AN11" s="621"/>
       <c r="AP11" s="76" t="s">
         <v>501</v>
       </c>
@@ -8437,7 +8437,7 @@
       <c r="E12" s="229">
         <v>3</v>
       </c>
-      <c r="F12" s="605"/>
+      <c r="F12" s="626"/>
       <c r="G12" s="349" t="s">
         <v>410</v>
       </c>
@@ -8446,16 +8446,16 @@
       </c>
       <c r="I12" s="563"/>
       <c r="J12" s="563"/>
-      <c r="K12" s="612"/>
+      <c r="K12" s="664"/>
       <c r="L12" s="208"/>
       <c r="M12" s="208"/>
       <c r="N12" s="208"/>
-      <c r="O12" s="608"/>
-      <c r="P12" s="634"/>
+      <c r="O12" s="660"/>
+      <c r="P12" s="633"/>
       <c r="R12" s="122" t="s">
         <v>181</v>
       </c>
-      <c r="S12" s="619"/>
+      <c r="S12" s="643"/>
       <c r="T12" s="101" t="s">
         <v>44</v>
       </c>
@@ -8476,16 +8476,16 @@
       <c r="AC12" s="100" t="s">
         <v>498</v>
       </c>
-      <c r="AD12" s="622" t="s">
+      <c r="AD12" s="649" t="s">
         <v>245</v>
       </c>
       <c r="AE12" s="465" t="s">
         <v>244</v>
       </c>
-      <c r="AF12" s="614" t="s">
+      <c r="AF12" s="641" t="s">
         <v>231</v>
       </c>
-      <c r="AG12" s="614"/>
+      <c r="AG12" s="641"/>
       <c r="AH12" s="243" t="s">
         <v>264</v>
       </c>
@@ -8498,7 +8498,7 @@
       <c r="AM12" s="636" t="s">
         <v>254</v>
       </c>
-      <c r="AN12" s="624"/>
+      <c r="AN12" s="621"/>
       <c r="AO12" s="350" t="s">
         <v>97</v>
       </c>
@@ -8510,17 +8510,17 @@
       <c r="E13" s="472">
         <v>-3</v>
       </c>
-      <c r="F13" s="605"/>
+      <c r="F13" s="626"/>
       <c r="G13" s="563" t="s">
         <v>447</v>
       </c>
       <c r="H13" s="563"/>
       <c r="I13" s="563"/>
-      <c r="J13" s="612"/>
+      <c r="J13" s="664"/>
       <c r="M13" s="6"/>
       <c r="N13" s="6"/>
-      <c r="O13" s="608"/>
-      <c r="P13" s="635"/>
+      <c r="O13" s="660"/>
+      <c r="P13" s="634"/>
       <c r="T13" s="105" t="s">
         <v>44</v>
       </c>
@@ -8541,8 +8541,8 @@
         <v>518</v>
       </c>
       <c r="AC13" s="16"/>
-      <c r="AD13" s="622"/>
-      <c r="AF13" s="614"/>
+      <c r="AD13" s="649"/>
+      <c r="AF13" s="641"/>
       <c r="AG13" s="80"/>
       <c r="AH13" s="243" t="s">
         <v>314</v>
@@ -8554,7 +8554,7 @@
       <c r="AK13" s="262"/>
       <c r="AL13" s="262"/>
       <c r="AM13" s="636"/>
-      <c r="AN13" s="624"/>
+      <c r="AN13" s="621"/>
     </row>
     <row r="14" spans="1:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="474"/>
@@ -8562,18 +8562,18 @@
       <c r="C14" s="483"/>
       <c r="D14" s="476"/>
       <c r="E14" s="477"/>
-      <c r="F14" s="605"/>
+      <c r="F14" s="626"/>
       <c r="G14" s="563" t="s">
         <v>446</v>
       </c>
       <c r="H14" s="563"/>
       <c r="I14" s="563"/>
-      <c r="J14" s="612"/>
+      <c r="J14" s="664"/>
       <c r="K14" s="2">
         <v>12</v>
       </c>
       <c r="N14" s="6"/>
-      <c r="O14" s="608"/>
+      <c r="O14" s="660"/>
       <c r="Q14" s="61" t="s">
         <v>554</v>
       </c>
@@ -8594,9 +8594,9 @@
       <c r="AA14" s="313"/>
       <c r="AB14" s="214"/>
       <c r="AC14" s="16"/>
-      <c r="AD14" s="622"/>
+      <c r="AD14" s="649"/>
       <c r="AE14" s="262"/>
-      <c r="AF14" s="614"/>
+      <c r="AF14" s="641"/>
       <c r="AG14" s="262"/>
       <c r="AH14" s="262"/>
       <c r="AI14" s="70"/>
@@ -8604,7 +8604,7 @@
       <c r="AK14" s="262"/>
       <c r="AL14" s="262"/>
       <c r="AM14" s="636"/>
-      <c r="AN14" s="624"/>
+      <c r="AN14" s="621"/>
     </row>
     <row r="15" spans="1:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="473" t="s">
@@ -8613,8 +8613,8 @@
       <c r="C15" s="556" t="s">
         <v>381</v>
       </c>
-      <c r="F15" s="605"/>
-      <c r="O15" s="608"/>
+      <c r="F15" s="626"/>
+      <c r="O15" s="660"/>
       <c r="R15" s="99" t="s">
         <v>44</v>
       </c>
@@ -8636,8 +8636,8 @@
       <c r="AC15" s="76" t="s">
         <v>496</v>
       </c>
-      <c r="AD15" s="622"/>
-      <c r="AF15" s="614"/>
+      <c r="AD15" s="649"/>
+      <c r="AF15" s="641"/>
       <c r="AG15" s="80"/>
       <c r="AH15" s="243" t="s">
         <v>465</v>
@@ -8651,7 +8651,7 @@
       <c r="AK15" s="262"/>
       <c r="AL15" s="262"/>
       <c r="AM15" s="636"/>
-      <c r="AN15" s="624"/>
+      <c r="AN15" s="621"/>
       <c r="AP15" s="76" t="s">
         <v>74</v>
       </c>
@@ -8673,13 +8673,13 @@
       <c r="E16" s="229">
         <v>1</v>
       </c>
-      <c r="F16" s="605"/>
+      <c r="F16" s="626"/>
       <c r="G16" s="349" t="s">
         <v>505</v>
       </c>
       <c r="I16" s="495"/>
       <c r="J16" s="20"/>
-      <c r="O16" s="608"/>
+      <c r="O16" s="660"/>
       <c r="R16" s="459" t="s">
         <v>185</v>
       </c>
@@ -8711,18 +8711,18 @@
       <c r="AM16" s="452" t="s">
         <v>324</v>
       </c>
-      <c r="AN16" s="624"/>
+      <c r="AN16" s="621"/>
       <c r="AP16" s="76" t="s">
         <v>235</v>
       </c>
     </row>
     <row r="17" spans="1:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B17" s="80"/>
-      <c r="F17" s="605"/>
+      <c r="F17" s="626"/>
       <c r="I17" s="496"/>
       <c r="J17" s="20"/>
       <c r="N17" s="6"/>
-      <c r="O17" s="608"/>
+      <c r="O17" s="660"/>
       <c r="Q17" s="21" t="s">
         <v>552</v>
       </c>
@@ -8767,7 +8767,7 @@
       <c r="AK17" s="262"/>
       <c r="AL17" s="80"/>
       <c r="AM17" s="452"/>
-      <c r="AN17" s="624"/>
+      <c r="AN17" s="621"/>
       <c r="AO17" s="209" t="s">
         <v>515</v>
       </c>
@@ -8791,21 +8791,21 @@
       <c r="E18" s="99" t="s">
         <v>44</v>
       </c>
-      <c r="F18" s="605"/>
+      <c r="F18" s="626"/>
       <c r="G18" s="349" t="s">
         <v>549</v>
       </c>
       <c r="I18" s="24"/>
       <c r="J18" s="20"/>
-      <c r="O18" s="608"/>
+      <c r="O18" s="660"/>
       <c r="Q18" s="112"/>
-      <c r="R18" s="600" t="s">
+      <c r="R18" s="654" t="s">
         <v>557</v>
       </c>
       <c r="T18" s="100" t="s">
         <v>44</v>
       </c>
-      <c r="U18" s="644" t="s">
+      <c r="U18" s="599" t="s">
         <v>44</v>
       </c>
       <c r="V18" s="120"/>
@@ -8826,7 +8826,7 @@
       <c r="AC18" s="16"/>
       <c r="AD18" s="16"/>
       <c r="AE18" s="262"/>
-      <c r="AF18" s="613" t="s">
+      <c r="AF18" s="635" t="s">
         <v>492</v>
       </c>
       <c r="AG18" s="262"/>
@@ -8838,20 +8838,20 @@
       <c r="AK18" s="262"/>
       <c r="AL18" s="80"/>
       <c r="AM18" s="452"/>
-      <c r="AN18" s="624"/>
+      <c r="AN18" s="621"/>
       <c r="AP18" s="76" t="s">
         <v>88</v>
       </c>
     </row>
     <row r="19" spans="1:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="F19" s="605"/>
+      <c r="F19" s="626"/>
       <c r="I19" s="224"/>
-      <c r="O19" s="608"/>
-      <c r="R19" s="601"/>
+      <c r="O19" s="660"/>
+      <c r="R19" s="655"/>
       <c r="S19" s="30" t="s">
         <v>555</v>
       </c>
-      <c r="U19" s="645"/>
+      <c r="U19" s="600"/>
       <c r="V19" s="146"/>
       <c r="W19" s="146"/>
       <c r="X19" s="455" t="s">
@@ -8866,7 +8866,7 @@
       <c r="AC19" s="16"/>
       <c r="AD19" s="16"/>
       <c r="AE19" s="262"/>
-      <c r="AF19" s="613"/>
+      <c r="AF19" s="635"/>
       <c r="AG19" s="262"/>
       <c r="AH19" s="262"/>
       <c r="AI19" s="70"/>
@@ -8876,7 +8876,7 @@
       </c>
       <c r="AL19" s="80"/>
       <c r="AM19" s="452"/>
-      <c r="AN19" s="624"/>
+      <c r="AN19" s="621"/>
       <c r="AP19" s="76" t="s">
         <v>485</v>
       </c>
@@ -8897,19 +8897,19 @@
       <c r="E20" s="461">
         <v>-1</v>
       </c>
-      <c r="F20" s="605"/>
+      <c r="F20" s="626"/>
       <c r="G20" s="349" t="s">
         <v>508</v>
       </c>
       <c r="I20" s="224"/>
-      <c r="O20" s="608"/>
-      <c r="Q20" s="610" t="s">
+      <c r="O20" s="660"/>
+      <c r="Q20" s="662" t="s">
         <v>48</v>
       </c>
       <c r="T20" s="428" t="s">
         <v>44</v>
       </c>
-      <c r="U20" s="646"/>
+      <c r="U20" s="601"/>
       <c r="W20" s="429"/>
       <c r="X20" s="456" t="s">
         <v>175</v>
@@ -8939,7 +8939,7 @@
       <c r="AM20" s="400" t="s">
         <v>254</v>
       </c>
-      <c r="AN20" s="624"/>
+      <c r="AN20" s="621"/>
       <c r="AO20" s="350" t="s">
         <v>477</v>
       </c>
@@ -8960,13 +8960,13 @@
       <c r="E21" s="271">
         <v>0</v>
       </c>
-      <c r="F21" s="605"/>
+      <c r="F21" s="626"/>
       <c r="I21" s="224"/>
-      <c r="O21" s="608"/>
-      <c r="Q21" s="611"/>
+      <c r="O21" s="660"/>
+      <c r="Q21" s="663"/>
       <c r="T21" s="446"/>
       <c r="U21" s="14"/>
-      <c r="V21" s="641"/>
+      <c r="V21" s="596"/>
       <c r="W21" s="450" t="s">
         <v>176</v>
       </c>
@@ -9004,15 +9004,15 @@
       <c r="AM21" s="452" t="s">
         <v>566</v>
       </c>
-      <c r="AN21" s="624"/>
+      <c r="AN21" s="621"/>
     </row>
     <row r="22" spans="1:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="F22" s="605"/>
+      <c r="F22" s="626"/>
       <c r="G22" s="349" t="s">
         <v>506</v>
       </c>
       <c r="I22" s="224"/>
-      <c r="O22" s="608"/>
+      <c r="O22" s="660"/>
       <c r="R22" s="458" t="s">
         <v>44</v>
       </c>
@@ -9020,7 +9020,7 @@
         <v>44</v>
       </c>
       <c r="U22" s="15"/>
-      <c r="V22" s="642"/>
+      <c r="V22" s="597"/>
       <c r="W22" s="450" t="s">
         <v>176</v>
       </c>
@@ -9038,7 +9038,7 @@
       <c r="AG22" s="6"/>
       <c r="AH22" s="6"/>
       <c r="AI22" s="6"/>
-      <c r="AJ22" s="613" t="s">
+      <c r="AJ22" s="635" t="s">
         <v>489</v>
       </c>
       <c r="AK22" s="262"/>
@@ -9046,7 +9046,7 @@
         <v>495</v>
       </c>
       <c r="AM22" s="306"/>
-      <c r="AN22" s="624"/>
+      <c r="AN22" s="621"/>
     </row>
     <row r="23" spans="1:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="236" t="s">
@@ -9064,17 +9064,17 @@
       <c r="E23" s="230">
         <v>1</v>
       </c>
-      <c r="F23" s="605"/>
+      <c r="F23" s="626"/>
       <c r="I23" s="224"/>
-      <c r="O23" s="608"/>
-      <c r="Q23" s="610" t="s">
+      <c r="O23" s="660"/>
+      <c r="Q23" s="662" t="s">
         <v>145</v>
       </c>
       <c r="T23" s="17"/>
       <c r="U23" s="444" t="s">
         <v>44</v>
       </c>
-      <c r="V23" s="642"/>
+      <c r="V23" s="597"/>
       <c r="W23" s="148"/>
       <c r="X23" s="453" t="s">
         <v>189</v>
@@ -9090,13 +9090,13 @@
       <c r="AG23" s="6"/>
       <c r="AH23" s="6"/>
       <c r="AI23" s="6"/>
-      <c r="AJ23" s="613"/>
+      <c r="AJ23" s="635"/>
       <c r="AK23" s="262"/>
       <c r="AL23" s="80" t="s">
         <v>525</v>
       </c>
       <c r="AM23" s="306"/>
-      <c r="AN23" s="624"/>
+      <c r="AN23" s="621"/>
     </row>
     <row r="24" spans="1:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="464" t="s">
@@ -9114,18 +9114,18 @@
       <c r="E24" s="460">
         <v>1</v>
       </c>
-      <c r="F24" s="605"/>
+      <c r="F24" s="626"/>
       <c r="G24" s="61" t="s">
         <v>507</v>
       </c>
       <c r="I24" s="224"/>
-      <c r="O24" s="608"/>
-      <c r="Q24" s="611"/>
+      <c r="O24" s="660"/>
+      <c r="Q24" s="663"/>
       <c r="T24" s="17"/>
       <c r="U24" s="232" t="s">
         <v>44</v>
       </c>
-      <c r="V24" s="642"/>
+      <c r="V24" s="597"/>
       <c r="W24" s="148"/>
       <c r="X24" s="453" t="s">
         <v>186</v>
@@ -9149,12 +9149,12 @@
         <v>480</v>
       </c>
       <c r="AM24" s="306"/>
-      <c r="AN24" s="624"/>
+      <c r="AN24" s="621"/>
     </row>
     <row r="25" spans="1:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="F25" s="605"/>
+      <c r="F25" s="626"/>
       <c r="I25" s="224"/>
-      <c r="O25" s="608"/>
+      <c r="O25" s="660"/>
       <c r="P25" s="209" t="s">
         <v>285</v>
       </c>
@@ -9167,7 +9167,7 @@
       <c r="U25" s="424" t="s">
         <v>44</v>
       </c>
-      <c r="V25" s="643"/>
+      <c r="V25" s="598"/>
       <c r="W25" s="148"/>
       <c r="X25" s="453" t="s">
         <v>190</v>
@@ -9189,7 +9189,7 @@
       <c r="AK25" s="142"/>
       <c r="AL25" s="6"/>
       <c r="AM25" s="306"/>
-      <c r="AN25" s="624"/>
+      <c r="AN25" s="621"/>
     </row>
     <row r="26" spans="1:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="236" t="s">
@@ -9207,17 +9207,17 @@
       <c r="E26" s="398">
         <v>1</v>
       </c>
-      <c r="F26" s="605"/>
+      <c r="F26" s="626"/>
       <c r="G26" s="349" t="s">
         <v>504</v>
       </c>
       <c r="I26" s="224"/>
-      <c r="O26" s="608"/>
-      <c r="P26" s="626" t="s">
+      <c r="O26" s="660"/>
+      <c r="P26" s="623" t="s">
         <v>547</v>
       </c>
-      <c r="Q26" s="627"/>
-      <c r="R26" s="602" t="s">
+      <c r="Q26" s="624"/>
+      <c r="R26" s="656" t="s">
         <v>556</v>
       </c>
       <c r="T26" s="182"/>
@@ -9256,7 +9256,7 @@
       <c r="AM26" s="466" t="s">
         <v>473</v>
       </c>
-      <c r="AN26" s="624"/>
+      <c r="AN26" s="621"/>
     </row>
     <row r="27" spans="1:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B27" s="21" t="s">
@@ -9268,13 +9268,13 @@
       <c r="E27" s="271" t="s">
         <v>44</v>
       </c>
-      <c r="F27" s="606"/>
+      <c r="F27" s="658"/>
       <c r="G27" s="61" t="s">
         <v>565</v>
       </c>
       <c r="I27" s="225"/>
-      <c r="O27" s="609"/>
-      <c r="R27" s="603"/>
+      <c r="O27" s="661"/>
+      <c r="R27" s="657"/>
       <c r="S27" s="445" t="s">
         <v>54</v>
       </c>
@@ -9304,10 +9304,48 @@
       <c r="AM27" s="400" t="s">
         <v>326</v>
       </c>
-      <c r="AN27" s="625"/>
+      <c r="AN27" s="622"/>
     </row>
   </sheetData>
   <mergeCells count="54">
+    <mergeCell ref="E2:E3"/>
+    <mergeCell ref="K2:L2"/>
+    <mergeCell ref="I1:I2"/>
+    <mergeCell ref="R18:R19"/>
+    <mergeCell ref="R26:R27"/>
+    <mergeCell ref="F2:F27"/>
+    <mergeCell ref="O10:O27"/>
+    <mergeCell ref="Q20:Q21"/>
+    <mergeCell ref="Q23:Q24"/>
+    <mergeCell ref="G14:J14"/>
+    <mergeCell ref="G13:J13"/>
+    <mergeCell ref="H12:K12"/>
+    <mergeCell ref="A5:A6"/>
+    <mergeCell ref="C6:D6"/>
+    <mergeCell ref="AI6:AI10"/>
+    <mergeCell ref="AF12:AF15"/>
+    <mergeCell ref="AG7:AG12"/>
+    <mergeCell ref="L8:L9"/>
+    <mergeCell ref="S9:S12"/>
+    <mergeCell ref="N8:N9"/>
+    <mergeCell ref="AD12:AD15"/>
+    <mergeCell ref="C15:C16"/>
+    <mergeCell ref="AN1:AN27"/>
+    <mergeCell ref="P26:Q26"/>
+    <mergeCell ref="Q2:Q3"/>
+    <mergeCell ref="M2:M9"/>
+    <mergeCell ref="O2:O9"/>
+    <mergeCell ref="P10:P13"/>
+    <mergeCell ref="AK6:AK7"/>
+    <mergeCell ref="AM12:AM15"/>
+    <mergeCell ref="AF18:AF19"/>
+    <mergeCell ref="AJ18:AJ19"/>
+    <mergeCell ref="Y1:Y27"/>
+    <mergeCell ref="AJ22:AJ23"/>
+    <mergeCell ref="AK9:AK10"/>
+    <mergeCell ref="AD3:AD4"/>
+    <mergeCell ref="S2:S3"/>
+    <mergeCell ref="R2:R3"/>
     <mergeCell ref="V21:V25"/>
     <mergeCell ref="U18:U20"/>
     <mergeCell ref="C2:C3"/>
@@ -9324,44 +9362,6 @@
     <mergeCell ref="B11:B12"/>
     <mergeCell ref="B6:B7"/>
     <mergeCell ref="B4:B5"/>
-    <mergeCell ref="AN1:AN27"/>
-    <mergeCell ref="P26:Q26"/>
-    <mergeCell ref="Q2:Q3"/>
-    <mergeCell ref="M2:M9"/>
-    <mergeCell ref="O2:O9"/>
-    <mergeCell ref="P10:P13"/>
-    <mergeCell ref="AK6:AK7"/>
-    <mergeCell ref="AM12:AM15"/>
-    <mergeCell ref="AF18:AF19"/>
-    <mergeCell ref="AJ18:AJ19"/>
-    <mergeCell ref="Y1:Y27"/>
-    <mergeCell ref="AJ22:AJ23"/>
-    <mergeCell ref="AK9:AK10"/>
-    <mergeCell ref="AD3:AD4"/>
-    <mergeCell ref="S2:S3"/>
-    <mergeCell ref="R2:R3"/>
-    <mergeCell ref="A5:A6"/>
-    <mergeCell ref="C6:D6"/>
-    <mergeCell ref="AI6:AI10"/>
-    <mergeCell ref="AF12:AF15"/>
-    <mergeCell ref="AG7:AG12"/>
-    <mergeCell ref="L8:L9"/>
-    <mergeCell ref="S9:S12"/>
-    <mergeCell ref="N8:N9"/>
-    <mergeCell ref="AD12:AD15"/>
-    <mergeCell ref="C15:C16"/>
-    <mergeCell ref="E2:E3"/>
-    <mergeCell ref="K2:L2"/>
-    <mergeCell ref="I1:I2"/>
-    <mergeCell ref="R18:R19"/>
-    <mergeCell ref="R26:R27"/>
-    <mergeCell ref="F2:F27"/>
-    <mergeCell ref="O10:O27"/>
-    <mergeCell ref="Q20:Q21"/>
-    <mergeCell ref="Q23:Q24"/>
-    <mergeCell ref="G14:J14"/>
-    <mergeCell ref="G13:J13"/>
-    <mergeCell ref="H12:K12"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -9371,8 +9371,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2029A93E-B53C-4201-9F17-439C144F3CF1}">
   <dimension ref="A1:AN37"/>
   <sheetViews>
-    <sheetView topLeftCell="N1" workbookViewId="0">
-      <selection activeCell="AL8" sqref="AL8"/>
+    <sheetView tabSelected="1" topLeftCell="I4" workbookViewId="0">
+      <selection activeCell="P16" sqref="P16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9467,10 +9467,10 @@
       <c r="S1" s="142"/>
       <c r="T1" s="142"/>
       <c r="U1" s="6"/>
-      <c r="V1" s="668" t="s">
+      <c r="V1" s="671" t="s">
         <v>458</v>
       </c>
-      <c r="W1" s="669"/>
+      <c r="W1" s="672"/>
       <c r="X1" s="312">
         <f>68-(U8+W3+V3+S3)</f>
         <v>0</v>
@@ -9486,21 +9486,21 @@
       <c r="AB1" s="308" t="s">
         <v>44</v>
       </c>
-      <c r="AC1" s="670" t="s">
+      <c r="AC1" s="673" t="s">
         <v>191</v>
       </c>
-      <c r="AD1" s="671"/>
-      <c r="AE1" s="672"/>
-      <c r="AF1" s="673" t="s">
+      <c r="AD1" s="674"/>
+      <c r="AE1" s="675"/>
+      <c r="AF1" s="676" t="s">
         <v>298</v>
       </c>
-      <c r="AG1" s="674"/>
-      <c r="AH1" s="675"/>
-      <c r="AI1" s="665" t="s">
+      <c r="AG1" s="677"/>
+      <c r="AH1" s="678"/>
+      <c r="AI1" s="668" t="s">
         <v>461</v>
       </c>
-      <c r="AJ1" s="666"/>
-      <c r="AK1" s="667"/>
+      <c r="AJ1" s="669"/>
+      <c r="AK1" s="670"/>
       <c r="AN1" s="142"/>
     </row>
     <row r="2" spans="1:40" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -9517,19 +9517,19 @@
       <c r="K2" s="327">
         <v>-3</v>
       </c>
-      <c r="L2" s="676">
+      <c r="L2" s="679">
         <f>SUM(L5:L30)</f>
         <v>3</v>
       </c>
-      <c r="M2" s="678">
+      <c r="M2" s="681">
         <f>SUM(M4:M29)</f>
-        <v>6</v>
-      </c>
-      <c r="N2" s="680">
+        <v>7</v>
+      </c>
+      <c r="N2" s="683">
         <f>SUM(N4:N29)</f>
         <v>9</v>
       </c>
-      <c r="O2" s="620">
+      <c r="O2" s="647">
         <f>SUM(M30:M37)* (-1)</f>
         <v>-3</v>
       </c>
@@ -9548,7 +9548,7 @@
       <c r="T2" s="515" t="s">
         <v>221</v>
       </c>
-      <c r="U2" s="682" t="s">
+      <c r="U2" s="685" t="s">
         <v>239</v>
       </c>
       <c r="V2" s="516" t="s">
@@ -9617,10 +9617,10 @@
         <f>T3+V3+W3+S3</f>
         <v>68</v>
       </c>
-      <c r="L3" s="677"/>
-      <c r="M3" s="679"/>
-      <c r="N3" s="681"/>
-      <c r="O3" s="621"/>
+      <c r="L3" s="680"/>
+      <c r="M3" s="682"/>
+      <c r="N3" s="684"/>
+      <c r="O3" s="648"/>
       <c r="P3" s="176">
         <f>(L2+M2)-W3</f>
         <v>0</v>
@@ -9634,16 +9634,16 @@
       </c>
       <c r="T3" s="518">
         <f>SUM(T4:T29)</f>
-        <v>41</v>
-      </c>
-      <c r="U3" s="683"/>
+        <v>40</v>
+      </c>
+      <c r="U3" s="686"/>
       <c r="V3" s="519">
         <f t="shared" ref="V3:AA3" si="0">SUM(V4:V29)</f>
         <v>6</v>
       </c>
       <c r="W3" s="519">
         <f t="shared" si="0"/>
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="X3" s="59">
         <f t="shared" si="0"/>
@@ -9655,7 +9655,7 @@
       </c>
       <c r="Z3" s="66">
         <f t="shared" si="0"/>
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="AA3" s="66">
         <f t="shared" si="0"/>
@@ -9687,7 +9687,7 @@
       </c>
       <c r="AH3" s="100">
         <f t="shared" si="1"/>
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="AI3" s="100">
         <f t="shared" si="1"/>
@@ -9735,7 +9735,7 @@
         <f>AA4</f>
         <v>0</v>
       </c>
-      <c r="O4" s="684" t="s">
+      <c r="O4" s="665" t="s">
         <v>200</v>
       </c>
       <c r="P4" s="20"/>
@@ -9814,7 +9814,7 @@
         <f>AA5</f>
         <v>0</v>
       </c>
-      <c r="O5" s="685"/>
+      <c r="O5" s="666"/>
       <c r="P5" s="20"/>
       <c r="Q5" s="2" t="s">
         <v>347</v>
@@ -9901,7 +9901,7 @@
         <f>AA6</f>
         <v>0</v>
       </c>
-      <c r="O6" s="685"/>
+      <c r="O6" s="666"/>
       <c r="P6" s="19" t="s">
         <v>342</v>
       </c>
@@ -9992,7 +9992,7 @@
         <f t="shared" ref="N7:N37" si="10">AA7</f>
         <v>0</v>
       </c>
-      <c r="O7" s="685"/>
+      <c r="O7" s="666"/>
       <c r="P7" s="20"/>
       <c r="Q7" s="2" t="s">
         <v>342</v>
@@ -10098,7 +10098,7 @@
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
-      <c r="O8" s="685"/>
+      <c r="O8" s="666"/>
       <c r="P8" s="21" t="s">
         <v>238</v>
       </c>
@@ -10116,7 +10116,7 @@
       </c>
       <c r="U8" s="29">
         <f>T3</f>
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="V8" s="531">
         <v>0</v>
@@ -10182,7 +10182,7 @@
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
-      <c r="O9" s="685"/>
+      <c r="O9" s="666"/>
       <c r="P9" s="21" t="s">
         <v>342</v>
       </c>
@@ -10280,7 +10280,7 @@
         <f t="shared" si="10"/>
         <v>2</v>
       </c>
-      <c r="O10" s="685"/>
+      <c r="O10" s="666"/>
       <c r="P10" s="20"/>
       <c r="Q10" s="2" t="s">
         <v>347</v>
@@ -10363,7 +10363,7 @@
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
-      <c r="O11" s="685"/>
+      <c r="O11" s="666"/>
       <c r="P11" s="21" t="s">
         <v>342</v>
       </c>
@@ -10423,7 +10423,7 @@
       <c r="AN11" s="142"/>
     </row>
     <row r="12" spans="1:40" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="656" t="s">
+      <c r="A12" s="611" t="s">
         <v>55</v>
       </c>
       <c r="B12" s="30">
@@ -10432,10 +10432,13 @@
       <c r="C12" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="E12" s="610" t="s">
+      <c r="E12" s="662" t="s">
         <v>57</v>
       </c>
       <c r="G12" s="267"/>
+      <c r="H12" s="545">
+        <v>-1</v>
+      </c>
       <c r="I12" s="61" t="s">
         <v>567</v>
       </c>
@@ -10444,13 +10447,13 @@
       </c>
       <c r="L12" s="338"/>
       <c r="M12" s="107">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N12" s="299">
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
-      <c r="O12" s="685"/>
+      <c r="O12" s="666"/>
       <c r="P12" s="21" t="s">
         <v>342</v>
       </c>
@@ -10460,7 +10463,7 @@
       </c>
       <c r="S12" s="539"/>
       <c r="T12" s="526">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="U12" s="527">
         <v>-2</v>
@@ -10468,7 +10471,7 @@
       <c r="V12" s="530"/>
       <c r="W12" s="524">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="X12" s="302"/>
       <c r="Y12" s="117">
@@ -10477,7 +10480,7 @@
       </c>
       <c r="Z12" s="296">
         <f t="shared" si="6"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AA12" s="296">
         <v>0</v>
@@ -10496,7 +10499,9 @@
         <v>0</v>
       </c>
       <c r="AG12" s="348"/>
-      <c r="AH12" s="158"/>
+      <c r="AH12" s="158">
+        <v>1</v>
+      </c>
       <c r="AI12" s="314">
         <f t="shared" si="7"/>
         <v>0</v>
@@ -10509,7 +10514,9 @@
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
-      <c r="AL12" s="6"/>
+      <c r="AL12" s="6" t="s">
+        <v>465</v>
+      </c>
       <c r="AM12" s="547" t="s">
         <v>528</v>
       </c>
@@ -10518,14 +10525,14 @@
       </c>
     </row>
     <row r="13" spans="1:40" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="658"/>
+      <c r="A13" s="613"/>
       <c r="B13" s="153">
         <v>12</v>
       </c>
       <c r="C13" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="E13" s="611"/>
+      <c r="E13" s="663"/>
       <c r="F13" s="176">
         <v>0</v>
       </c>
@@ -10548,7 +10555,7 @@
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
-      <c r="O13" s="685"/>
+      <c r="O13" s="666"/>
       <c r="P13" s="21" t="s">
         <v>342</v>
       </c>
@@ -10624,7 +10631,7 @@
         <f t="shared" si="10"/>
         <v>2</v>
       </c>
-      <c r="O14" s="685"/>
+      <c r="O14" s="666"/>
       <c r="P14" s="20"/>
       <c r="Q14" s="205" t="s">
         <v>346</v>
@@ -10719,7 +10726,7 @@
         <f t="shared" si="10"/>
         <v>1</v>
       </c>
-      <c r="O15" s="685"/>
+      <c r="O15" s="666"/>
       <c r="P15" s="20"/>
       <c r="Q15" s="205" t="s">
         <v>346</v>
@@ -10806,7 +10813,7 @@
         <f t="shared" si="10"/>
         <v>1</v>
       </c>
-      <c r="O16" s="685"/>
+      <c r="O16" s="666"/>
       <c r="P16" s="21" t="s">
         <v>342</v>
       </c>
@@ -10904,7 +10911,7 @@
         <f t="shared" si="10"/>
         <v>1</v>
       </c>
-      <c r="O17" s="685"/>
+      <c r="O17" s="666"/>
       <c r="P17" s="20"/>
       <c r="Q17" s="2" t="s">
         <v>348</v>
@@ -10999,7 +11006,7 @@
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
-      <c r="O18" s="685"/>
+      <c r="O18" s="666"/>
       <c r="P18" s="21" t="s">
         <v>342</v>
       </c>
@@ -11082,7 +11089,7 @@
         <f t="shared" si="10"/>
         <v>1</v>
       </c>
-      <c r="O19" s="685"/>
+      <c r="O19" s="666"/>
       <c r="P19" s="20"/>
       <c r="Q19" s="2" t="s">
         <v>341</v>
@@ -11178,11 +11185,11 @@
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
-      <c r="O20" s="686"/>
+      <c r="O20" s="667"/>
       <c r="P20" s="561" t="s">
         <v>342</v>
       </c>
-      <c r="Q20" s="612"/>
+      <c r="Q20" s="664"/>
       <c r="R20" s="321" t="s">
         <v>86</v>
       </c>
@@ -11416,7 +11423,7 @@
       <c r="AN22" s="142"/>
     </row>
     <row r="23" spans="1:40" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E23" s="663" t="s">
+      <c r="E23" s="618" t="s">
         <v>294</v>
       </c>
       <c r="F23" s="184"/>
@@ -11507,7 +11514,7 @@
       <c r="C24" s="2" t="s">
         <v>260</v>
       </c>
-      <c r="E24" s="664"/>
+      <c r="E24" s="619"/>
       <c r="F24" s="176"/>
       <c r="K24" s="403" t="s">
         <v>301</v>
@@ -11525,7 +11532,7 @@
       <c r="P24" s="561" t="s">
         <v>342</v>
       </c>
-      <c r="Q24" s="612"/>
+      <c r="Q24" s="664"/>
       <c r="R24" s="321" t="s">
         <v>254</v>
       </c>
@@ -12052,7 +12059,7 @@
         <v>-1</v>
       </c>
       <c r="H31" s="42">
-        <v>-2</v>
+        <v>-1</v>
       </c>
       <c r="I31" s="21" t="s">
         <v>435</v>
@@ -12597,12 +12604,6 @@
     </row>
   </sheetData>
   <mergeCells count="15">
-    <mergeCell ref="A12:A13"/>
-    <mergeCell ref="E12:E13"/>
-    <mergeCell ref="P20:Q20"/>
-    <mergeCell ref="E23:E24"/>
-    <mergeCell ref="P24:Q24"/>
-    <mergeCell ref="O4:O20"/>
     <mergeCell ref="AI1:AK1"/>
     <mergeCell ref="V1:W1"/>
     <mergeCell ref="AC1:AE1"/>
@@ -12612,8 +12613,15 @@
     <mergeCell ref="N2:N3"/>
     <mergeCell ref="O2:O3"/>
     <mergeCell ref="U2:U3"/>
+    <mergeCell ref="A12:A13"/>
+    <mergeCell ref="E12:E13"/>
+    <mergeCell ref="P20:Q20"/>
+    <mergeCell ref="E23:E24"/>
+    <mergeCell ref="P24:Q24"/>
+    <mergeCell ref="O4:O20"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -12648,12 +12656,12 @@
       <c r="B1" s="561" t="s">
         <v>317</v>
       </c>
-      <c r="C1" s="612"/>
+      <c r="C1" s="664"/>
       <c r="D1" s="209"/>
       <c r="J1" s="561" t="s">
         <v>70</v>
       </c>
-      <c r="K1" s="612"/>
+      <c r="K1" s="664"/>
       <c r="L1" s="200" t="s">
         <v>337</v>
       </c>
@@ -13044,7 +13052,7 @@
       <c r="V1" s="561" t="s">
         <v>71</v>
       </c>
-      <c r="W1" s="612"/>
+      <c r="W1" s="664"/>
       <c r="X1" s="62" t="s">
         <v>102</v>
       </c>
@@ -13063,7 +13071,7 @@
       <c r="AC1" s="116" t="s">
         <v>191</v>
       </c>
-      <c r="AD1" s="700" t="s">
+      <c r="AD1" s="707" t="s">
         <v>213</v>
       </c>
       <c r="AE1" s="116" t="s">
@@ -13080,10 +13088,10 @@
       <c r="E2" s="39" t="s">
         <v>74</v>
       </c>
-      <c r="F2" s="699" t="s">
+      <c r="F2" s="738" t="s">
         <v>75</v>
       </c>
-      <c r="G2" s="727" t="s">
+      <c r="G2" s="695" t="s">
         <v>44</v>
       </c>
       <c r="H2" s="40" t="s">
@@ -13111,10 +13119,10 @@
       <c r="U2" s="60" t="s">
         <v>106</v>
       </c>
-      <c r="V2" s="668" t="s">
+      <c r="V2" s="671" t="s">
         <v>121</v>
       </c>
-      <c r="W2" s="669"/>
+      <c r="W2" s="672"/>
       <c r="X2" s="64" t="s">
         <v>110</v>
       </c>
@@ -13133,7 +13141,7 @@
       <c r="AC2" s="117" t="s">
         <v>99</v>
       </c>
-      <c r="AD2" s="701"/>
+      <c r="AD2" s="708"/>
       <c r="AE2" s="64" t="s">
         <v>99</v>
       </c>
@@ -13152,8 +13160,8 @@
       <c r="E3" s="39" t="s">
         <v>80</v>
       </c>
-      <c r="F3" s="660"/>
-      <c r="G3" s="728"/>
+      <c r="F3" s="615"/>
+      <c r="G3" s="696"/>
       <c r="H3" s="40" t="s">
         <v>81</v>
       </c>
@@ -13164,13 +13172,13 @@
         <v>82</v>
       </c>
       <c r="N3" s="44"/>
-      <c r="O3" s="737" t="s">
+      <c r="O3" s="705" t="s">
         <v>44</v>
       </c>
-      <c r="P3" s="719" t="s">
+      <c r="P3" s="726" t="s">
         <v>219</v>
       </c>
-      <c r="Q3" s="720"/>
+      <c r="Q3" s="727"/>
       <c r="S3" s="57" t="s">
         <v>220</v>
       </c>
@@ -13180,15 +13188,15 @@
       <c r="W3" s="59" t="s">
         <v>105</v>
       </c>
-      <c r="AD3" s="701"/>
+      <c r="AD3" s="708"/>
     </row>
     <row r="4" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="G4" s="728"/>
+      <c r="G4" s="696"/>
       <c r="H4" s="6"/>
       <c r="L4" s="690" t="s">
         <v>83</v>
       </c>
-      <c r="O4" s="738"/>
+      <c r="O4" s="706"/>
       <c r="T4" s="55" t="s">
         <v>98</v>
       </c>
@@ -13202,8 +13210,8 @@
         <v>195</v>
       </c>
       <c r="Z4" s="563"/>
-      <c r="AA4" s="612"/>
-      <c r="AD4" s="701"/>
+      <c r="AA4" s="664"/>
+      <c r="AD4" s="708"/>
     </row>
     <row r="5" spans="1:31" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C5" s="52" t="s">
@@ -13218,21 +13226,21 @@
       <c r="F5" s="66" t="s">
         <v>85</v>
       </c>
-      <c r="G5" s="728"/>
+      <c r="G5" s="696"/>
       <c r="H5" s="46" t="s">
         <v>76</v>
       </c>
-      <c r="K5" s="706" t="s">
+      <c r="K5" s="713" t="s">
         <v>217</v>
       </c>
-      <c r="L5" s="721"/>
+      <c r="L5" s="728"/>
       <c r="M5" s="2" t="s">
         <v>215</v>
       </c>
       <c r="N5" s="61" t="s">
         <v>214</v>
       </c>
-      <c r="O5" s="738"/>
+      <c r="O5" s="706"/>
       <c r="P5" s="108" t="s">
         <v>216</v>
       </c>
@@ -13248,11 +13256,11 @@
       <c r="U5" s="19" t="s">
         <v>99</v>
       </c>
-      <c r="Y5" s="709" t="s">
+      <c r="Y5" s="716" t="s">
         <v>287</v>
       </c>
-      <c r="Z5" s="710"/>
-      <c r="AD5" s="701"/>
+      <c r="Z5" s="717"/>
+      <c r="AD5" s="708"/>
     </row>
     <row r="6" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C6" s="109"/>
@@ -13262,16 +13270,16 @@
       <c r="E6" s="45" t="s">
         <v>86</v>
       </c>
-      <c r="G6" s="728"/>
+      <c r="G6" s="696"/>
       <c r="H6" s="46" t="s">
         <v>81</v>
       </c>
       <c r="I6" s="23">
         <v>15</v>
       </c>
-      <c r="K6" s="707"/>
-      <c r="L6" s="721"/>
-      <c r="O6" s="738"/>
+      <c r="K6" s="714"/>
+      <c r="L6" s="728"/>
+      <c r="O6" s="706"/>
       <c r="T6" s="2" t="s">
         <v>101</v>
       </c>
@@ -13281,23 +13289,23 @@
       <c r="V6" s="21">
         <v>-1</v>
       </c>
-      <c r="AD6" s="701"/>
+      <c r="AD6" s="708"/>
     </row>
     <row r="7" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C7" s="110"/>
-      <c r="G7" s="728"/>
+      <c r="G7" s="696"/>
       <c r="H7" s="6"/>
-      <c r="K7" s="707"/>
-      <c r="L7" s="721"/>
+      <c r="K7" s="714"/>
+      <c r="L7" s="728"/>
       <c r="N7" s="21" t="s">
         <v>120</v>
       </c>
-      <c r="O7" s="738"/>
+      <c r="O7" s="706"/>
       <c r="P7" s="73"/>
       <c r="U7" s="104" t="s">
         <v>20</v>
       </c>
-      <c r="AD7" s="701"/>
+      <c r="AD7" s="708"/>
     </row>
     <row r="8" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C8" s="130"/>
@@ -13310,7 +13318,7 @@
       <c r="F8" s="66" t="s">
         <v>87</v>
       </c>
-      <c r="G8" s="728"/>
+      <c r="G8" s="696"/>
       <c r="H8" s="50" t="s">
         <v>76</v>
       </c>
@@ -13320,41 +13328,41 @@
       <c r="J8" s="111">
         <v>115</v>
       </c>
-      <c r="K8" s="707"/>
-      <c r="L8" s="721"/>
-      <c r="O8" s="738"/>
+      <c r="K8" s="714"/>
+      <c r="L8" s="728"/>
+      <c r="O8" s="706"/>
       <c r="P8" s="49"/>
-      <c r="S8" s="703" t="s">
+      <c r="S8" s="710" t="s">
         <v>212</v>
       </c>
-      <c r="T8" s="704"/>
-      <c r="U8" s="704"/>
-      <c r="V8" s="704"/>
-      <c r="W8" s="704"/>
-      <c r="X8" s="704"/>
-      <c r="Y8" s="704"/>
-      <c r="Z8" s="704"/>
-      <c r="AA8" s="704"/>
-      <c r="AB8" s="704"/>
-      <c r="AC8" s="705"/>
-      <c r="AD8" s="701"/>
+      <c r="T8" s="711"/>
+      <c r="U8" s="711"/>
+      <c r="V8" s="711"/>
+      <c r="W8" s="711"/>
+      <c r="X8" s="711"/>
+      <c r="Y8" s="711"/>
+      <c r="Z8" s="711"/>
+      <c r="AA8" s="711"/>
+      <c r="AB8" s="711"/>
+      <c r="AC8" s="712"/>
+      <c r="AD8" s="708"/>
     </row>
     <row r="9" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C9" s="693"/>
-      <c r="G9" s="728"/>
+      <c r="C9" s="732"/>
+      <c r="G9" s="696"/>
       <c r="H9" s="6"/>
-      <c r="K9" s="707"/>
-      <c r="L9" s="731" t="s">
+      <c r="K9" s="714"/>
+      <c r="L9" s="699" t="s">
         <v>218</v>
       </c>
-      <c r="M9" s="732"/>
-      <c r="N9" s="733"/>
-      <c r="O9" s="738"/>
+      <c r="M9" s="700"/>
+      <c r="N9" s="701"/>
+      <c r="O9" s="706"/>
       <c r="P9" s="75"/>
-      <c r="AD9" s="701"/>
+      <c r="AD9" s="708"/>
     </row>
     <row r="10" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C10" s="694"/>
+      <c r="C10" s="733"/>
       <c r="D10" s="23"/>
       <c r="E10" s="45" t="s">
         <v>88</v>
@@ -13362,7 +13370,7 @@
       <c r="F10" s="66" t="s">
         <v>89</v>
       </c>
-      <c r="G10" s="728"/>
+      <c r="G10" s="696"/>
       <c r="H10" s="51"/>
       <c r="I10" s="21" t="s">
         <v>81</v>
@@ -13370,33 +13378,33 @@
       <c r="J10" s="3">
         <v>15</v>
       </c>
-      <c r="K10" s="707"/>
-      <c r="M10" s="696" t="s">
+      <c r="K10" s="714"/>
+      <c r="M10" s="735" t="s">
         <v>90</v>
       </c>
-      <c r="N10" s="697"/>
-      <c r="O10" s="697"/>
-      <c r="P10" s="697"/>
-      <c r="Q10" s="697"/>
-      <c r="R10" s="697"/>
-      <c r="S10" s="697"/>
-      <c r="T10" s="697"/>
-      <c r="U10" s="697"/>
-      <c r="V10" s="697"/>
-      <c r="W10" s="697"/>
-      <c r="X10" s="697"/>
-      <c r="Y10" s="697"/>
-      <c r="Z10" s="697"/>
-      <c r="AA10" s="697"/>
-      <c r="AB10" s="697"/>
-      <c r="AC10" s="698"/>
-      <c r="AD10" s="701"/>
+      <c r="N10" s="736"/>
+      <c r="O10" s="736"/>
+      <c r="P10" s="736"/>
+      <c r="Q10" s="736"/>
+      <c r="R10" s="736"/>
+      <c r="S10" s="736"/>
+      <c r="T10" s="736"/>
+      <c r="U10" s="736"/>
+      <c r="V10" s="736"/>
+      <c r="W10" s="736"/>
+      <c r="X10" s="736"/>
+      <c r="Y10" s="736"/>
+      <c r="Z10" s="736"/>
+      <c r="AA10" s="736"/>
+      <c r="AB10" s="736"/>
+      <c r="AC10" s="737"/>
+      <c r="AD10" s="708"/>
     </row>
     <row r="11" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C11" s="695"/>
-      <c r="G11" s="728"/>
+      <c r="C11" s="734"/>
+      <c r="G11" s="696"/>
       <c r="H11" s="6"/>
-      <c r="K11" s="707"/>
+      <c r="K11" s="714"/>
       <c r="R11" s="52" t="s">
         <v>44</v>
       </c>
@@ -13404,17 +13412,17 @@
       <c r="Y11" s="68" t="s">
         <v>121</v>
       </c>
-      <c r="Z11" s="717" t="s">
+      <c r="Z11" s="724" t="s">
         <v>121</v>
       </c>
-      <c r="AA11" s="718"/>
+      <c r="AA11" s="725"/>
       <c r="AB11" s="52" t="s">
         <v>44</v>
       </c>
       <c r="AC11" s="118" t="s">
         <v>121</v>
       </c>
-      <c r="AD11" s="701"/>
+      <c r="AD11" s="708"/>
     </row>
     <row r="12" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C12" s="129"/>
@@ -13427,7 +13435,7 @@
       <c r="F12" s="66" t="s">
         <v>92</v>
       </c>
-      <c r="G12" s="728"/>
+      <c r="G12" s="696"/>
       <c r="H12" s="128"/>
       <c r="I12" s="19" t="s">
         <v>81</v>
@@ -13435,8 +13443,8 @@
       <c r="J12" s="3">
         <v>15</v>
       </c>
-      <c r="K12" s="707"/>
-      <c r="L12" s="722" t="s">
+      <c r="K12" s="714"/>
+      <c r="L12" s="729" t="s">
         <v>93</v>
       </c>
       <c r="M12" s="21" t="s">
@@ -13467,25 +13475,25 @@
         <v>116</v>
       </c>
       <c r="Y12" s="6"/>
-      <c r="AA12" s="711" t="s">
+      <c r="AA12" s="718" t="s">
         <v>126</v>
       </c>
-      <c r="AB12" s="712"/>
+      <c r="AB12" s="719"/>
       <c r="AC12" s="21" t="s">
         <v>233</v>
       </c>
-      <c r="AD12" s="701"/>
+      <c r="AD12" s="708"/>
     </row>
     <row r="13" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C13" s="693"/>
-      <c r="G13" s="728"/>
-      <c r="K13" s="707"/>
-      <c r="L13" s="723"/>
+      <c r="C13" s="732"/>
+      <c r="G13" s="696"/>
+      <c r="K13" s="714"/>
+      <c r="L13" s="730"/>
       <c r="M13" s="47"/>
-      <c r="Q13" s="730" t="s">
+      <c r="Q13" s="698" t="s">
         <v>210</v>
       </c>
-      <c r="R13" s="627"/>
+      <c r="R13" s="624"/>
       <c r="S13" s="557"/>
       <c r="T13" s="6"/>
       <c r="U13" s="96" t="s">
@@ -13494,17 +13502,17 @@
       <c r="X13" s="2" t="s">
         <v>123</v>
       </c>
-      <c r="AA13" s="713"/>
-      <c r="AB13" s="714"/>
-      <c r="AD13" s="701"/>
+      <c r="AA13" s="720"/>
+      <c r="AB13" s="721"/>
+      <c r="AD13" s="708"/>
     </row>
     <row r="14" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B14" s="2" t="s">
         <v>339</v>
       </c>
-      <c r="C14" s="695"/>
+      <c r="C14" s="734"/>
       <c r="D14" s="23"/>
-      <c r="G14" s="728"/>
+      <c r="G14" s="696"/>
       <c r="H14" s="125"/>
       <c r="I14" s="99" t="s">
         <v>44</v>
@@ -13512,8 +13520,8 @@
       <c r="J14" s="111">
         <v>115</v>
       </c>
-      <c r="K14" s="707"/>
-      <c r="L14" s="723"/>
+      <c r="K14" s="714"/>
+      <c r="L14" s="730"/>
       <c r="M14" s="21" t="s">
         <v>111</v>
       </c>
@@ -13534,9 +13542,9 @@
       <c r="Y14" s="21" t="s">
         <v>73</v>
       </c>
-      <c r="AA14" s="713"/>
-      <c r="AB14" s="714"/>
-      <c r="AD14" s="701"/>
+      <c r="AA14" s="720"/>
+      <c r="AB14" s="721"/>
+      <c r="AD14" s="708"/>
     </row>
     <row r="15" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C15" s="130" t="s">
@@ -13551,19 +13559,19 @@
       <c r="F15" s="66" t="s">
         <v>94</v>
       </c>
-      <c r="G15" s="728"/>
+      <c r="G15" s="696"/>
       <c r="H15" s="2" t="s">
         <v>81</v>
       </c>
       <c r="I15" s="53" t="s">
         <v>81</v>
       </c>
-      <c r="K15" s="707"/>
-      <c r="L15" s="724"/>
-      <c r="Q15" s="730" t="s">
+      <c r="K15" s="714"/>
+      <c r="L15" s="731"/>
+      <c r="Q15" s="698" t="s">
         <v>211</v>
       </c>
-      <c r="R15" s="627"/>
+      <c r="R15" s="624"/>
       <c r="S15" s="557"/>
       <c r="T15" s="6"/>
       <c r="V15" s="68" t="s">
@@ -13572,14 +13580,14 @@
       <c r="X15" s="2" t="s">
         <v>128</v>
       </c>
-      <c r="AA15" s="713"/>
-      <c r="AB15" s="714"/>
-      <c r="AD15" s="701"/>
+      <c r="AA15" s="720"/>
+      <c r="AB15" s="721"/>
+      <c r="AD15" s="708"/>
     </row>
     <row r="16" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C16" s="132"/>
-      <c r="G16" s="728"/>
-      <c r="K16" s="707"/>
+      <c r="G16" s="696"/>
+      <c r="K16" s="714"/>
       <c r="N16" s="47"/>
       <c r="O16" s="61" t="s">
         <v>109</v>
@@ -13598,24 +13606,24 @@
       <c r="Z16" s="76" t="s">
         <v>127</v>
       </c>
-      <c r="AA16" s="713"/>
-      <c r="AB16" s="714"/>
-      <c r="AD16" s="701"/>
+      <c r="AA16" s="720"/>
+      <c r="AB16" s="721"/>
+      <c r="AD16" s="708"/>
     </row>
     <row r="17" spans="3:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C17" s="109"/>
       <c r="E17" s="6" t="s">
         <v>95</v>
       </c>
-      <c r="F17" s="725" t="s">
+      <c r="F17" s="693" t="s">
         <v>96</v>
       </c>
-      <c r="G17" s="728"/>
+      <c r="G17" s="696"/>
       <c r="H17" s="54"/>
       <c r="I17" s="133" t="s">
         <v>81</v>
       </c>
-      <c r="K17" s="707"/>
+      <c r="K17" s="714"/>
       <c r="S17" s="557"/>
       <c r="V17" s="68" t="s">
         <v>44</v>
@@ -13623,9 +13631,9 @@
       <c r="X17" s="2" t="s">
         <v>118</v>
       </c>
-      <c r="AA17" s="713"/>
-      <c r="AB17" s="714"/>
-      <c r="AD17" s="701"/>
+      <c r="AA17" s="720"/>
+      <c r="AB17" s="721"/>
+      <c r="AD17" s="708"/>
     </row>
     <row r="18" spans="3:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C18" s="130"/>
@@ -13635,15 +13643,15 @@
       <c r="E18" s="6" t="s">
         <v>97</v>
       </c>
-      <c r="F18" s="726"/>
-      <c r="G18" s="728"/>
+      <c r="F18" s="694"/>
+      <c r="G18" s="696"/>
       <c r="H18" s="108" t="s">
         <v>76</v>
       </c>
       <c r="I18" s="21" t="s">
         <v>81</v>
       </c>
-      <c r="K18" s="707"/>
+      <c r="K18" s="714"/>
       <c r="O18" s="64" t="s">
         <v>115</v>
       </c>
@@ -13654,42 +13662,39 @@
       <c r="X18" s="2" t="s">
         <v>117</v>
       </c>
-      <c r="AA18" s="715"/>
-      <c r="AB18" s="716"/>
-      <c r="AD18" s="701"/>
+      <c r="AA18" s="722"/>
+      <c r="AB18" s="723"/>
+      <c r="AD18" s="708"/>
     </row>
     <row r="19" spans="3:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="F19" s="64" t="s">
         <v>209</v>
       </c>
-      <c r="G19" s="729"/>
-      <c r="K19" s="708"/>
+      <c r="G19" s="697"/>
+      <c r="K19" s="715"/>
       <c r="Q19" s="68" t="s">
         <v>44</v>
       </c>
-      <c r="R19" s="734" t="s">
+      <c r="R19" s="702" t="s">
         <v>124</v>
       </c>
-      <c r="S19" s="735"/>
-      <c r="T19" s="736"/>
+      <c r="S19" s="703"/>
+      <c r="T19" s="704"/>
       <c r="V19" s="77" t="s">
         <v>115</v>
       </c>
       <c r="Y19" s="19" t="s">
         <v>125</v>
       </c>
-      <c r="AD19" s="702"/>
+      <c r="AD19" s="709"/>
     </row>
   </sheetData>
   <mergeCells count="24">
-    <mergeCell ref="F17:F18"/>
-    <mergeCell ref="G2:G19"/>
-    <mergeCell ref="Q13:R13"/>
-    <mergeCell ref="Q15:R15"/>
-    <mergeCell ref="L9:N9"/>
-    <mergeCell ref="R19:T19"/>
-    <mergeCell ref="S12:S18"/>
-    <mergeCell ref="O3:O9"/>
+    <mergeCell ref="C9:C11"/>
+    <mergeCell ref="C13:C14"/>
+    <mergeCell ref="V2:W2"/>
+    <mergeCell ref="M10:AC10"/>
+    <mergeCell ref="F2:F3"/>
     <mergeCell ref="AD1:AD19"/>
     <mergeCell ref="S8:AC8"/>
     <mergeCell ref="K5:K19"/>
@@ -13701,11 +13706,14 @@
     <mergeCell ref="P3:Q3"/>
     <mergeCell ref="L4:L8"/>
     <mergeCell ref="L12:L15"/>
-    <mergeCell ref="C9:C11"/>
-    <mergeCell ref="C13:C14"/>
-    <mergeCell ref="V2:W2"/>
-    <mergeCell ref="M10:AC10"/>
-    <mergeCell ref="F2:F3"/>
+    <mergeCell ref="F17:F18"/>
+    <mergeCell ref="G2:G19"/>
+    <mergeCell ref="Q13:R13"/>
+    <mergeCell ref="Q15:R15"/>
+    <mergeCell ref="L9:N9"/>
+    <mergeCell ref="R19:T19"/>
+    <mergeCell ref="S12:S18"/>
+    <mergeCell ref="O3:O9"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Boat ReConfigured - India TV
Boat Enabled - India TV
ShieldW Enabled
</commit_message>
<xml_diff>
--- a/System_2.1.5.xlsx
+++ b/System_2.1.5.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Work\Work_For_\Work\Running AppS\System_Work_RW\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8648B577-ADCB-4E82-AE5D-CD5FE002C98D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{939C31B8-1EAC-4512-BB70-4DB4DB3D90FE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -5653,7 +5653,7 @@
   <dimension ref="B1:W28"/>
   <sheetViews>
     <sheetView topLeftCell="B9" workbookViewId="0">
-      <selection activeCell="X19" sqref="X19"/>
+      <selection activeCell="X3" sqref="X3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5842,7 +5842,7 @@
         <v>228</v>
       </c>
       <c r="V5" s="19">
-        <v>6000</v>
+        <v>6060</v>
       </c>
     </row>
     <row r="6" spans="2:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -6052,7 +6052,7 @@
         <v>227</v>
       </c>
       <c r="V11" s="64">
-        <v>100</v>
+        <v>101</v>
       </c>
     </row>
     <row r="12" spans="2:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -9440,8 +9440,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2029A93E-B53C-4201-9F17-439C144F3CF1}">
   <dimension ref="A1:AN37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A23" workbookViewId="0">
-      <selection activeCell="I37" sqref="I37"/>
+    <sheetView tabSelected="1" topLeftCell="N1" workbookViewId="0">
+      <selection activeCell="J34" sqref="J34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -11501,7 +11501,12 @@
         <v>294</v>
       </c>
       <c r="F23" s="184"/>
-      <c r="H23" s="274"/>
+      <c r="H23" s="42">
+        <v>-1</v>
+      </c>
+      <c r="I23" s="221" t="s">
+        <v>330</v>
+      </c>
       <c r="K23" s="403" t="s">
         <v>263</v>
       </c>
@@ -12065,12 +12070,6 @@
     </row>
     <row r="30" spans="1:40" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="G30" s="274"/>
-      <c r="H30" s="42">
-        <v>-1</v>
-      </c>
-      <c r="I30" s="221" t="s">
-        <v>330</v>
-      </c>
       <c r="K30" s="406"/>
       <c r="L30" s="344"/>
       <c r="M30" s="250"/>

</xml_diff>

<commit_message>
Boat Enabled - Zee N , ND TV
Boat Enabled - Zee N
ShieldW Enabled - Zee24 Taas

ShieldW Enabled - ND TV India
</commit_message>
<xml_diff>
--- a/System_2.1.5.xlsx
+++ b/System_2.1.5.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Work\Work_For_\Work\Running AppS\System_Work_RW\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{939C31B8-1EAC-4512-BB70-4DB4DB3D90FE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD520114-03BD-4AC2-91D9-3F9BD42E2B38}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1096" uniqueCount="616">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1097" uniqueCount="616">
   <si>
     <t>Zone</t>
   </si>
@@ -3473,7 +3473,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="741">
+  <cellXfs count="742">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
@@ -4845,6 +4845,63 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="255" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="32" fillId="27" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="27" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="27" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="13" fillId="27" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="13" fillId="27" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="27" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="27" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="27" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="27" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="19" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="19" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="36" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="36" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="39" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -4875,62 +4932,167 @@
     <xf numFmtId="0" fontId="6" fillId="18" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="255"/>
     </xf>
-    <xf numFmtId="0" fontId="32" fillId="27" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="73" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="57" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="11" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="11" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="13" fillId="27" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="13" fillId="27" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="27" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="27" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="27" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="27" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="36" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="36" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="3" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="18" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="18" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="18" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="32" fillId="27" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="32" fillId="27" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="14" fontId="13" fillId="27" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="49" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="49" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="49" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="14" fontId="13" fillId="27" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="32" fillId="27" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="27" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="27" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="27" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="19" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="19" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="36" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="36" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="52" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="54" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="16" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="16" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="19" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -4956,12 +5118,6 @@
     <xf numFmtId="0" fontId="38" fillId="7" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255"/>
-    </xf>
     <xf numFmtId="0" fontId="17" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="255"/>
     </xf>
@@ -4983,161 +5139,14 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="52" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="54" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="16" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="16" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="3" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="18" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="18" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="18" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="49" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="49" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="49" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="73" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="57" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="11" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="11" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="13" fillId="27" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="13" fillId="27" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="27" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="27" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="27" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="27" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="36" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="36" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="11" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="3" fillId="35" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="35" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="35" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="43" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -5196,15 +5205,6 @@
     <xf numFmtId="0" fontId="6" fillId="52" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="35" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="35" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="35" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -5223,25 +5223,46 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="30" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="30" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="30" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="24" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="24" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="24" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="18" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -5319,47 +5340,29 @@
     <xf numFmtId="0" fontId="3" fillId="21" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="30" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="30" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="30" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="24" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="24" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="24" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="53" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -5653,7 +5656,7 @@
   <dimension ref="B1:W28"/>
   <sheetViews>
     <sheetView topLeftCell="B9" workbookViewId="0">
-      <selection activeCell="X3" sqref="X3"/>
+      <selection activeCell="V16" sqref="V16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6726,7 +6729,7 @@
       <c r="P1" s="422" t="s">
         <v>407</v>
       </c>
-      <c r="Q1" s="569" t="s">
+      <c r="Q1" s="588" t="s">
         <v>181</v>
       </c>
       <c r="R1" s="100" t="s">
@@ -6746,32 +6749,32 @@
       </c>
     </row>
     <row r="2" spans="1:27" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="582">
+      <c r="A2" s="572">
         <f ca="1">TODAY()</f>
         <v>45279</v>
       </c>
-      <c r="B2" s="584" t="s">
+      <c r="B2" s="574" t="s">
         <v>388</v>
       </c>
-      <c r="C2" s="596" t="s">
+      <c r="C2" s="586" t="s">
         <v>364</v>
       </c>
-      <c r="D2" s="586" t="s">
+      <c r="D2" s="576" t="s">
         <v>103</v>
       </c>
-      <c r="E2" s="588" t="s">
+      <c r="E2" s="578" t="s">
         <v>65</v>
       </c>
       <c r="F2" s="196" t="s">
         <v>220</v>
       </c>
-      <c r="G2" s="594" t="s">
+      <c r="G2" s="584" t="s">
         <v>380</v>
       </c>
       <c r="H2" s="211" t="s">
         <v>220</v>
       </c>
-      <c r="I2" s="576" t="s">
+      <c r="I2" s="595" t="s">
         <v>103</v>
       </c>
       <c r="J2" s="420" t="s">
@@ -6795,7 +6798,7 @@
       <c r="P2" s="423">
         <v>40</v>
       </c>
-      <c r="Q2" s="570"/>
+      <c r="Q2" s="589"/>
       <c r="R2" s="21">
         <f>R7+R18</f>
         <v>5</v>
@@ -6821,14 +6824,14 @@
       </c>
     </row>
     <row r="3" spans="1:27" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="583"/>
-      <c r="B3" s="585"/>
-      <c r="C3" s="597"/>
-      <c r="D3" s="587"/>
-      <c r="E3" s="589"/>
-      <c r="G3" s="595"/>
+      <c r="A3" s="573"/>
+      <c r="B3" s="575"/>
+      <c r="C3" s="587"/>
+      <c r="D3" s="577"/>
+      <c r="E3" s="579"/>
+      <c r="G3" s="585"/>
       <c r="H3" s="6"/>
-      <c r="I3" s="577"/>
+      <c r="I3" s="596"/>
       <c r="K3" s="24">
         <v>2</v>
       </c>
@@ -6853,10 +6856,10 @@
         <v>389</v>
       </c>
       <c r="B4" s="248"/>
-      <c r="C4" s="590" t="s">
+      <c r="C4" s="580" t="s">
         <v>178</v>
       </c>
-      <c r="I4" s="577"/>
+      <c r="I4" s="596"/>
       <c r="R4" s="498" t="s">
         <v>578</v>
       </c>
@@ -6880,7 +6883,7 @@
       <c r="B5" s="100" t="s">
         <v>364</v>
       </c>
-      <c r="C5" s="591"/>
+      <c r="C5" s="581"/>
       <c r="D5" s="227" t="s">
         <v>103</v>
       </c>
@@ -6896,7 +6899,7 @@
       <c r="H5" s="211" t="s">
         <v>220</v>
       </c>
-      <c r="I5" s="577"/>
+      <c r="I5" s="596"/>
       <c r="J5" s="421" t="s">
         <v>273</v>
       </c>
@@ -6927,22 +6930,22 @@
       <c r="X5" s="494"/>
     </row>
     <row r="6" spans="1:27" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="579" t="s">
+      <c r="A6" s="569" t="s">
         <v>290</v>
       </c>
       <c r="B6" s="105" t="s">
         <v>199</v>
       </c>
-      <c r="C6" s="592"/>
-      <c r="D6" s="593"/>
+      <c r="C6" s="582"/>
+      <c r="D6" s="583"/>
       <c r="E6" s="96">
         <v>1</v>
       </c>
       <c r="G6" s="559"/>
-      <c r="I6" s="577"/>
+      <c r="I6" s="596"/>
     </row>
     <row r="7" spans="1:27" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="580"/>
+      <c r="A7" s="570"/>
       <c r="B7" s="100" t="s">
         <v>155</v>
       </c>
@@ -6953,7 +6956,7 @@
         <v>136</v>
       </c>
       <c r="G7" s="559"/>
-      <c r="I7" s="577"/>
+      <c r="I7" s="596"/>
       <c r="M7" s="16" t="s">
         <v>354</v>
       </c>
@@ -6991,7 +6994,7 @@
       </c>
     </row>
     <row r="8" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="581"/>
+      <c r="A8" s="571"/>
       <c r="B8" s="217" t="s">
         <v>28</v>
       </c>
@@ -7000,7 +7003,7 @@
         <v>3</v>
       </c>
       <c r="G8" s="559"/>
-      <c r="I8" s="577"/>
+      <c r="I8" s="596"/>
       <c r="N8" s="80"/>
       <c r="U8" s="6" t="s">
         <v>465</v>
@@ -7024,7 +7027,7 @@
       </c>
       <c r="G9" s="559"/>
       <c r="H9" s="6"/>
-      <c r="I9" s="577"/>
+      <c r="I9" s="596"/>
       <c r="M9" s="19" t="s">
         <v>546</v>
       </c>
@@ -7046,10 +7049,10 @@
       <c r="D10" s="108"/>
       <c r="E10" s="68">
         <f>Boat!U8</f>
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="G10" s="559"/>
-      <c r="I10" s="577"/>
+      <c r="I10" s="596"/>
       <c r="J10" s="24" t="s">
         <v>380</v>
       </c>
@@ -7081,7 +7084,7 @@
         <v>270</v>
       </c>
       <c r="G11" s="559"/>
-      <c r="I11" s="577"/>
+      <c r="I11" s="596"/>
       <c r="J11" s="24" t="s">
         <v>195</v>
       </c>
@@ -7107,12 +7110,12 @@
       <c r="S11" s="24">
         <v>1</v>
       </c>
-      <c r="U11" s="571" t="s">
+      <c r="U11" s="590" t="s">
         <v>581</v>
       </c>
-      <c r="V11" s="572"/>
-      <c r="W11" s="572"/>
-      <c r="X11" s="573"/>
+      <c r="V11" s="591"/>
+      <c r="W11" s="591"/>
+      <c r="X11" s="592"/>
     </row>
     <row r="12" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="232" t="s">
@@ -7123,7 +7126,7 @@
         <v>3</v>
       </c>
       <c r="G12" s="559"/>
-      <c r="I12" s="577"/>
+      <c r="I12" s="596"/>
       <c r="J12" s="24" t="s">
         <v>537</v>
       </c>
@@ -7156,7 +7159,7 @@
       </c>
       <c r="D13" s="20"/>
       <c r="G13" s="559"/>
-      <c r="I13" s="577"/>
+      <c r="I13" s="596"/>
       <c r="J13" s="108" t="s">
         <v>570</v>
       </c>
@@ -7197,7 +7200,7 @@
       <c r="H14" s="211" t="s">
         <v>220</v>
       </c>
-      <c r="I14" s="577"/>
+      <c r="I14" s="596"/>
       <c r="U14" s="6"/>
       <c r="V14" s="112"/>
       <c r="W14" s="6"/>
@@ -7215,7 +7218,7 @@
       <c r="H15" s="277">
         <v>0</v>
       </c>
-      <c r="I15" s="577"/>
+      <c r="I15" s="596"/>
       <c r="J15" s="108" t="s">
         <v>154</v>
       </c>
@@ -7246,7 +7249,7 @@
       <c r="D16" s="2" t="s">
         <v>509</v>
       </c>
-      <c r="I16" s="577"/>
+      <c r="I16" s="596"/>
       <c r="K16" s="100" t="s">
         <v>44</v>
       </c>
@@ -7280,7 +7283,7 @@
       <c r="G17" s="2" t="s">
         <v>440</v>
       </c>
-      <c r="I17" s="577"/>
+      <c r="I17" s="596"/>
       <c r="L17" s="2" t="s">
         <v>443</v>
       </c>
@@ -7292,13 +7295,13 @@
     </row>
     <row r="18" spans="1:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="G18" s="16"/>
-      <c r="I18" s="577"/>
+      <c r="I18" s="596"/>
       <c r="L18" s="16"/>
       <c r="M18" s="21"/>
-      <c r="O18" s="574" t="s">
+      <c r="O18" s="593" t="s">
         <v>538</v>
       </c>
-      <c r="P18" s="575"/>
+      <c r="P18" s="594"/>
       <c r="Q18" s="127" t="s">
         <v>44</v>
       </c>
@@ -7324,7 +7327,7 @@
       </c>
     </row>
     <row r="19" spans="1:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="I19" s="577"/>
+      <c r="I19" s="596"/>
       <c r="M19" s="21" t="s">
         <v>442</v>
       </c>
@@ -7356,7 +7359,7 @@
       <c r="G20" s="2" t="s">
         <v>440</v>
       </c>
-      <c r="I20" s="577"/>
+      <c r="I20" s="596"/>
       <c r="K20" s="19" t="s">
         <v>439</v>
       </c>
@@ -7381,7 +7384,7 @@
       <c r="Z20" s="112"/>
     </row>
     <row r="21" spans="1:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="I21" s="577"/>
+      <c r="I21" s="596"/>
       <c r="M21" s="221" t="s">
         <v>421</v>
       </c>
@@ -7417,7 +7420,7 @@
       <c r="G22" s="2" t="s">
         <v>440</v>
       </c>
-      <c r="I22" s="577"/>
+      <c r="I22" s="596"/>
       <c r="U22" s="6"/>
       <c r="V22" s="494"/>
       <c r="W22" s="6" t="s">
@@ -7437,13 +7440,13 @@
       <c r="E23" s="289" t="s">
         <v>44</v>
       </c>
-      <c r="I23" s="577"/>
+      <c r="I23" s="596"/>
       <c r="U23" s="6"/>
       <c r="V23" s="24"/>
       <c r="W23" s="6"/>
     </row>
     <row r="24" spans="1:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="I24" s="577"/>
+      <c r="I24" s="596"/>
       <c r="U24" s="354"/>
       <c r="V24" s="497">
         <v>0</v>
@@ -7471,7 +7474,7 @@
       <c r="H25" s="196" t="s">
         <v>271</v>
       </c>
-      <c r="I25" s="577"/>
+      <c r="I25" s="596"/>
       <c r="J25" s="421" t="s">
         <v>274</v>
       </c>
@@ -7516,7 +7519,7 @@
       <c r="H26" s="19" t="s">
         <v>220</v>
       </c>
-      <c r="I26" s="577"/>
+      <c r="I26" s="596"/>
       <c r="K26" s="24">
         <v>15</v>
       </c>
@@ -7551,7 +7554,7 @@
       </c>
     </row>
     <row r="27" spans="1:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="I27" s="577"/>
+      <c r="I27" s="596"/>
       <c r="O27" s="2" t="s">
         <v>99</v>
       </c>
@@ -7578,7 +7581,7 @@
       <c r="E28" s="220">
         <v>2</v>
       </c>
-      <c r="I28" s="577"/>
+      <c r="I28" s="596"/>
       <c r="Q28" s="6"/>
       <c r="R28" s="112"/>
       <c r="T28" s="142"/>
@@ -7600,7 +7603,7 @@
       <c r="H29" s="196" t="s">
         <v>272</v>
       </c>
-      <c r="I29" s="578"/>
+      <c r="I29" s="597"/>
       <c r="J29" s="333"/>
       <c r="L29" s="96" t="s">
         <v>278</v>
@@ -7670,6 +7673,11 @@
     </row>
   </sheetData>
   <mergeCells count="16">
+    <mergeCell ref="Q1:Q2"/>
+    <mergeCell ref="U11:X11"/>
+    <mergeCell ref="O18:P18"/>
+    <mergeCell ref="I2:I29"/>
+    <mergeCell ref="C13:C14"/>
     <mergeCell ref="A6:A8"/>
     <mergeCell ref="G5:G14"/>
     <mergeCell ref="A2:A3"/>
@@ -7681,11 +7689,6 @@
     <mergeCell ref="B11:B12"/>
     <mergeCell ref="G2:G3"/>
     <mergeCell ref="C2:C3"/>
-    <mergeCell ref="Q1:Q2"/>
-    <mergeCell ref="U11:X11"/>
-    <mergeCell ref="O18:P18"/>
-    <mergeCell ref="I2:I29"/>
-    <mergeCell ref="C13:C14"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -7761,7 +7764,7 @@
       <c r="H1" s="97" t="s">
         <v>350</v>
       </c>
-      <c r="I1" s="594" t="s">
+      <c r="I1" s="584" t="s">
         <v>377</v>
       </c>
       <c r="J1" s="2" t="s">
@@ -7822,7 +7825,7 @@
         <v>516</v>
       </c>
       <c r="AM1" s="426"/>
-      <c r="AN1" s="625"/>
+      <c r="AN1" s="622"/>
       <c r="AO1" s="350" t="s">
         <v>486</v>
       </c>
@@ -7831,23 +7834,23 @@
       </c>
     </row>
     <row r="2" spans="1:43" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="649">
+      <c r="A2" s="604">
         <f ca="1">TODAY()</f>
         <v>45279</v>
       </c>
-      <c r="B2" s="651" t="s">
+      <c r="B2" s="606" t="s">
         <v>378</v>
       </c>
-      <c r="C2" s="596" t="s">
+      <c r="C2" s="586" t="s">
         <v>364</v>
       </c>
-      <c r="D2" s="653" t="s">
+      <c r="D2" s="608" t="s">
         <v>362</v>
       </c>
-      <c r="E2" s="598" t="s">
+      <c r="E2" s="652" t="s">
         <v>65</v>
       </c>
-      <c r="F2" s="606" t="s">
+      <c r="F2" s="627" t="s">
         <v>103</v>
       </c>
       <c r="G2" s="417" t="s">
@@ -7856,31 +7859,31 @@
       <c r="H2" s="80" t="s">
         <v>33</v>
       </c>
-      <c r="I2" s="595"/>
+      <c r="I2" s="585"/>
       <c r="J2" s="81" t="s">
         <v>77</v>
       </c>
-      <c r="K2" s="600" t="s">
+      <c r="K2" s="654" t="s">
         <v>349</v>
       </c>
-      <c r="L2" s="601"/>
-      <c r="M2" s="606" t="s">
+      <c r="L2" s="655"/>
+      <c r="M2" s="627" t="s">
         <v>103</v>
       </c>
       <c r="N2" s="69" t="s">
         <v>28</v>
       </c>
-      <c r="O2" s="632" t="s">
+      <c r="O2" s="631" t="s">
         <v>103</v>
       </c>
       <c r="P2" s="85" t="s">
         <v>148</v>
       </c>
-      <c r="Q2" s="596" t="s">
+      <c r="Q2" s="586" t="s">
         <v>144</v>
       </c>
       <c r="R2" s="558"/>
-      <c r="S2" s="619" t="s">
+      <c r="S2" s="644" t="s">
         <v>149</v>
       </c>
       <c r="T2" s="89"/>
@@ -7913,15 +7916,15 @@
         <v>480</v>
       </c>
       <c r="AM2" s="452"/>
-      <c r="AN2" s="626"/>
+      <c r="AN2" s="623"/>
     </row>
     <row r="3" spans="1:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="650"/>
-      <c r="B3" s="652"/>
-      <c r="C3" s="597"/>
-      <c r="D3" s="654"/>
-      <c r="E3" s="599"/>
-      <c r="F3" s="607"/>
+      <c r="A3" s="605"/>
+      <c r="B3" s="607"/>
+      <c r="C3" s="587"/>
+      <c r="D3" s="609"/>
+      <c r="E3" s="653"/>
+      <c r="F3" s="628"/>
       <c r="G3" s="418" t="s">
         <v>28</v>
       </c>
@@ -7940,17 +7943,17 @@
       <c r="L3" s="206" t="s">
         <v>108</v>
       </c>
-      <c r="M3" s="607"/>
+      <c r="M3" s="628"/>
       <c r="N3" s="69" t="s">
         <v>147</v>
       </c>
-      <c r="O3" s="633"/>
+      <c r="O3" s="632"/>
       <c r="P3" s="2" t="s">
         <v>155</v>
       </c>
-      <c r="Q3" s="597"/>
+      <c r="Q3" s="587"/>
       <c r="R3" s="560"/>
-      <c r="S3" s="621"/>
+      <c r="S3" s="645"/>
       <c r="T3" s="89"/>
       <c r="U3" s="124"/>
       <c r="V3" s="120"/>
@@ -7967,7 +7970,7 @@
       <c r="AC3" s="100" t="s">
         <v>497</v>
       </c>
-      <c r="AD3" s="616" t="s">
+      <c r="AD3" s="643" t="s">
         <v>472</v>
       </c>
       <c r="AE3" s="262"/>
@@ -7979,16 +7982,16 @@
       <c r="AK3" s="262"/>
       <c r="AL3" s="16"/>
       <c r="AM3" s="452"/>
-      <c r="AN3" s="626"/>
+      <c r="AN3" s="623"/>
     </row>
     <row r="4" spans="1:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="243" t="s">
         <v>184</v>
       </c>
-      <c r="B4" s="665" t="s">
+      <c r="B4" s="620" t="s">
         <v>381</v>
       </c>
-      <c r="C4" s="596" t="s">
+      <c r="C4" s="586" t="s">
         <v>155</v>
       </c>
       <c r="D4" s="359" t="s">
@@ -7997,7 +8000,7 @@
       <c r="E4" s="396">
         <v>2</v>
       </c>
-      <c r="F4" s="607"/>
+      <c r="F4" s="628"/>
       <c r="G4" s="400" t="s">
         <v>203</v>
       </c>
@@ -8014,11 +8017,11 @@
         <v>151</v>
       </c>
       <c r="L4" s="209"/>
-      <c r="M4" s="607"/>
+      <c r="M4" s="628"/>
       <c r="N4" s="178" t="s">
         <v>70</v>
       </c>
-      <c r="O4" s="633"/>
+      <c r="O4" s="632"/>
       <c r="P4" s="2" t="s">
         <v>192</v>
       </c>
@@ -8045,7 +8048,7 @@
       <c r="AA4" s="313"/>
       <c r="AB4" s="214"/>
       <c r="AC4" s="16"/>
-      <c r="AD4" s="616"/>
+      <c r="AD4" s="643"/>
       <c r="AE4" s="262"/>
       <c r="AF4" s="262"/>
       <c r="AG4" s="16"/>
@@ -8055,37 +8058,37 @@
       <c r="AK4" s="262"/>
       <c r="AL4" s="16"/>
       <c r="AM4" s="452"/>
-      <c r="AN4" s="626"/>
+      <c r="AN4" s="623"/>
       <c r="AO4" s="350" t="s">
         <v>91</v>
       </c>
     </row>
     <row r="5" spans="1:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="594" t="s">
+      <c r="A5" s="584" t="s">
         <v>434</v>
       </c>
-      <c r="B5" s="666"/>
-      <c r="C5" s="597"/>
+      <c r="B5" s="621"/>
+      <c r="C5" s="587"/>
       <c r="D5" s="61" t="s">
         <v>154</v>
       </c>
       <c r="E5" s="397">
         <v>1</v>
       </c>
-      <c r="F5" s="607"/>
-      <c r="G5" s="657" t="s">
+      <c r="F5" s="628"/>
+      <c r="G5" s="612" t="s">
         <v>193</v>
       </c>
-      <c r="H5" s="657"/>
-      <c r="I5" s="657"/>
-      <c r="J5" s="657"/>
-      <c r="K5" s="657"/>
-      <c r="L5" s="658"/>
-      <c r="M5" s="607"/>
+      <c r="H5" s="612"/>
+      <c r="I5" s="612"/>
+      <c r="J5" s="612"/>
+      <c r="K5" s="612"/>
+      <c r="L5" s="613"/>
+      <c r="M5" s="628"/>
       <c r="N5" s="21">
         <v>8</v>
       </c>
-      <c r="O5" s="633"/>
+      <c r="O5" s="632"/>
       <c r="T5" s="89"/>
       <c r="U5" s="124"/>
       <c r="V5" s="120"/>
@@ -8116,24 +8119,24 @@
       <c r="AK5" s="262"/>
       <c r="AL5" s="80"/>
       <c r="AM5" s="452"/>
-      <c r="AN5" s="626"/>
+      <c r="AN5" s="623"/>
     </row>
     <row r="6" spans="1:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="595"/>
-      <c r="B6" s="663" t="s">
+      <c r="A6" s="585"/>
+      <c r="B6" s="618" t="s">
         <v>178</v>
       </c>
-      <c r="C6" s="592"/>
-      <c r="D6" s="593"/>
-      <c r="F6" s="607"/>
-      <c r="G6" s="659"/>
-      <c r="H6" s="659"/>
-      <c r="I6" s="659"/>
-      <c r="J6" s="659"/>
-      <c r="K6" s="659"/>
-      <c r="L6" s="660"/>
-      <c r="M6" s="607"/>
-      <c r="O6" s="633"/>
+      <c r="C6" s="582"/>
+      <c r="D6" s="583"/>
+      <c r="F6" s="628"/>
+      <c r="G6" s="614"/>
+      <c r="H6" s="614"/>
+      <c r="I6" s="614"/>
+      <c r="J6" s="614"/>
+      <c r="K6" s="614"/>
+      <c r="L6" s="615"/>
+      <c r="M6" s="628"/>
+      <c r="O6" s="632"/>
       <c r="T6" s="89"/>
       <c r="U6" s="124"/>
       <c r="V6" s="98" t="s">
@@ -8157,16 +8160,16 @@
       <c r="AF6" s="262"/>
       <c r="AG6" s="262"/>
       <c r="AH6" s="262"/>
-      <c r="AI6" s="615"/>
+      <c r="AI6" s="637"/>
       <c r="AJ6" s="465" t="s">
         <v>475</v>
       </c>
-      <c r="AK6" s="615" t="s">
+      <c r="AK6" s="637" t="s">
         <v>256</v>
       </c>
       <c r="AL6" s="262"/>
       <c r="AM6" s="452"/>
-      <c r="AN6" s="626"/>
+      <c r="AN6" s="623"/>
       <c r="AO6" s="350" t="s">
         <v>487</v>
       </c>
@@ -8175,7 +8178,7 @@
       <c r="A7" s="237" t="s">
         <v>596</v>
       </c>
-      <c r="B7" s="664"/>
+      <c r="B7" s="619"/>
       <c r="C7" s="207" t="s">
         <v>382</v>
       </c>
@@ -8185,7 +8188,7 @@
       <c r="E7" s="271">
         <v>3</v>
       </c>
-      <c r="F7" s="607"/>
+      <c r="F7" s="628"/>
       <c r="G7" s="419">
         <v>0</v>
       </c>
@@ -8204,8 +8207,8 @@
       <c r="L7" s="217">
         <v>0</v>
       </c>
-      <c r="M7" s="607"/>
-      <c r="O7" s="633"/>
+      <c r="M7" s="628"/>
+      <c r="O7" s="632"/>
       <c r="R7" s="99" t="s">
         <v>44</v>
       </c>
@@ -8229,18 +8232,18 @@
       <c r="AD7" s="16"/>
       <c r="AE7" s="262"/>
       <c r="AF7" s="262"/>
-      <c r="AG7" s="616" t="s">
+      <c r="AG7" s="643" t="s">
         <v>471</v>
       </c>
       <c r="AH7" s="262"/>
-      <c r="AI7" s="615"/>
+      <c r="AI7" s="637"/>
       <c r="AJ7" s="262"/>
-      <c r="AK7" s="615"/>
+      <c r="AK7" s="637"/>
       <c r="AL7" s="80" t="s">
         <v>514</v>
       </c>
       <c r="AM7" s="452"/>
-      <c r="AN7" s="626"/>
+      <c r="AN7" s="623"/>
       <c r="AP7" s="76" t="s">
         <v>488</v>
       </c>
@@ -8257,27 +8260,27 @@
         <f>SUM(G7:N9)</f>
         <v>15</v>
       </c>
-      <c r="F8" s="607"/>
-      <c r="G8" s="658">
-        <v>0</v>
-      </c>
-      <c r="H8" s="655" t="s">
+      <c r="F8" s="628"/>
+      <c r="G8" s="613">
+        <v>0</v>
+      </c>
+      <c r="H8" s="610" t="s">
         <v>105</v>
       </c>
       <c r="I8" s="558">
         <v>0</v>
       </c>
-      <c r="J8" s="655" t="s">
+      <c r="J8" s="610" t="s">
         <v>105</v>
       </c>
-      <c r="K8" s="661"/>
-      <c r="L8" s="617"/>
-      <c r="M8" s="630"/>
-      <c r="N8" s="622">
+      <c r="K8" s="616"/>
+      <c r="L8" s="646"/>
+      <c r="M8" s="629"/>
+      <c r="N8" s="649">
         <f>N5+N11</f>
         <v>15</v>
       </c>
-      <c r="O8" s="633"/>
+      <c r="O8" s="632"/>
       <c r="T8" s="103" t="s">
         <v>44</v>
       </c>
@@ -8295,14 +8298,14 @@
       <c r="AD8" s="16"/>
       <c r="AE8" s="262"/>
       <c r="AF8" s="262"/>
-      <c r="AG8" s="616"/>
+      <c r="AG8" s="643"/>
       <c r="AH8" s="262"/>
-      <c r="AI8" s="615"/>
+      <c r="AI8" s="637"/>
       <c r="AJ8" s="262"/>
       <c r="AK8" s="262"/>
       <c r="AL8" s="262"/>
       <c r="AM8" s="452"/>
-      <c r="AN8" s="626"/>
+      <c r="AN8" s="623"/>
     </row>
     <row r="9" spans="1:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="237" t="s">
@@ -8317,17 +8320,17 @@
       <c r="D9" s="360" t="s">
         <v>286</v>
       </c>
-      <c r="F9" s="607"/>
-      <c r="G9" s="660"/>
-      <c r="H9" s="656"/>
+      <c r="F9" s="628"/>
+      <c r="G9" s="615"/>
+      <c r="H9" s="611"/>
       <c r="I9" s="560"/>
-      <c r="J9" s="656"/>
-      <c r="K9" s="662"/>
-      <c r="L9" s="618"/>
-      <c r="M9" s="631"/>
-      <c r="N9" s="623"/>
-      <c r="O9" s="634"/>
-      <c r="S9" s="619" t="s">
+      <c r="J9" s="611"/>
+      <c r="K9" s="617"/>
+      <c r="L9" s="647"/>
+      <c r="M9" s="630"/>
+      <c r="N9" s="650"/>
+      <c r="O9" s="633"/>
+      <c r="S9" s="644" t="s">
         <v>62</v>
       </c>
       <c r="T9" s="89"/>
@@ -8349,16 +8352,16 @@
       </c>
       <c r="AE9" s="262"/>
       <c r="AF9" s="262"/>
-      <c r="AG9" s="616"/>
+      <c r="AG9" s="643"/>
       <c r="AH9" s="262"/>
-      <c r="AI9" s="615"/>
+      <c r="AI9" s="637"/>
       <c r="AJ9" s="80"/>
-      <c r="AK9" s="615" t="s">
+      <c r="AK9" s="637" t="s">
         <v>256</v>
       </c>
       <c r="AL9" s="262"/>
       <c r="AM9" s="452"/>
-      <c r="AN9" s="626"/>
+      <c r="AN9" s="623"/>
       <c r="AP9" s="2" t="s">
         <v>526</v>
       </c>
@@ -8373,22 +8376,22 @@
       <c r="D10" s="142"/>
       <c r="E10" s="242">
         <f>Boat!U8</f>
-        <v>37</v>
-      </c>
-      <c r="F10" s="607"/>
+        <v>36</v>
+      </c>
+      <c r="F10" s="628"/>
       <c r="N10" s="442" t="s">
         <v>406</v>
       </c>
-      <c r="O10" s="609" t="s">
+      <c r="O10" s="661" t="s">
         <v>103</v>
       </c>
-      <c r="P10" s="635" t="s">
+      <c r="P10" s="634" t="s">
         <v>410</v>
       </c>
       <c r="R10" s="74" t="s">
         <v>44</v>
       </c>
-      <c r="S10" s="620"/>
+      <c r="S10" s="648"/>
       <c r="T10" s="89"/>
       <c r="U10" s="123" t="s">
         <v>177</v>
@@ -8418,16 +8421,16 @@
       <c r="AF10" s="243" t="s">
         <v>318</v>
       </c>
-      <c r="AG10" s="616"/>
+      <c r="AG10" s="643"/>
       <c r="AH10" s="80"/>
-      <c r="AI10" s="615"/>
+      <c r="AI10" s="637"/>
       <c r="AJ10" s="262"/>
-      <c r="AK10" s="615"/>
+      <c r="AK10" s="637"/>
       <c r="AL10" s="262"/>
       <c r="AM10" s="466" t="s">
         <v>325</v>
       </c>
-      <c r="AN10" s="626"/>
+      <c r="AN10" s="623"/>
       <c r="AO10" s="209" t="s">
         <v>95</v>
       </c>
@@ -8445,18 +8448,18 @@
       <c r="D11" s="174" t="s">
         <v>362</v>
       </c>
-      <c r="F11" s="607"/>
+      <c r="F11" s="628"/>
       <c r="M11" s="6"/>
       <c r="N11" s="117">
         <v>7</v>
       </c>
-      <c r="O11" s="610"/>
-      <c r="P11" s="636"/>
+      <c r="O11" s="662"/>
+      <c r="P11" s="635"/>
       <c r="Q11" s="65"/>
       <c r="R11" s="120" t="s">
         <v>222</v>
       </c>
-      <c r="S11" s="620"/>
+      <c r="S11" s="648"/>
       <c r="T11" s="102" t="s">
         <v>44</v>
       </c>
@@ -8480,14 +8483,14 @@
       <c r="AF11" s="262" t="s">
         <v>493</v>
       </c>
-      <c r="AG11" s="616"/>
+      <c r="AG11" s="643"/>
       <c r="AH11" s="262"/>
       <c r="AI11" s="70"/>
       <c r="AJ11" s="262"/>
       <c r="AK11" s="262"/>
       <c r="AL11" s="262"/>
       <c r="AM11" s="452"/>
-      <c r="AN11" s="626"/>
+      <c r="AN11" s="623"/>
       <c r="AP11" s="76" t="s">
         <v>501</v>
       </c>
@@ -8506,7 +8509,7 @@
       <c r="E12" s="229">
         <v>3</v>
       </c>
-      <c r="F12" s="607"/>
+      <c r="F12" s="628"/>
       <c r="G12" s="349" t="s">
         <v>410</v>
       </c>
@@ -8515,16 +8518,16 @@
       </c>
       <c r="I12" s="565"/>
       <c r="J12" s="565"/>
-      <c r="K12" s="614"/>
+      <c r="K12" s="666"/>
       <c r="L12" s="208"/>
       <c r="M12" s="208"/>
       <c r="N12" s="208"/>
-      <c r="O12" s="610"/>
-      <c r="P12" s="636"/>
+      <c r="O12" s="662"/>
+      <c r="P12" s="635"/>
       <c r="R12" s="122" t="s">
         <v>181</v>
       </c>
-      <c r="S12" s="621"/>
+      <c r="S12" s="645"/>
       <c r="T12" s="101" t="s">
         <v>44</v>
       </c>
@@ -8545,16 +8548,16 @@
       <c r="AC12" s="100" t="s">
         <v>498</v>
       </c>
-      <c r="AD12" s="624" t="s">
+      <c r="AD12" s="651" t="s">
         <v>245</v>
       </c>
       <c r="AE12" s="465" t="s">
         <v>244</v>
       </c>
-      <c r="AF12" s="616" t="s">
+      <c r="AF12" s="643" t="s">
         <v>231</v>
       </c>
-      <c r="AG12" s="616"/>
+      <c r="AG12" s="643"/>
       <c r="AH12" s="243" t="s">
         <v>264</v>
       </c>
@@ -8567,7 +8570,7 @@
       <c r="AM12" s="638" t="s">
         <v>254</v>
       </c>
-      <c r="AN12" s="626"/>
+      <c r="AN12" s="623"/>
       <c r="AO12" s="350" t="s">
         <v>97</v>
       </c>
@@ -8579,17 +8582,17 @@
       <c r="E13" s="472">
         <v>-3</v>
       </c>
-      <c r="F13" s="607"/>
+      <c r="F13" s="628"/>
       <c r="G13" s="565" t="s">
         <v>447</v>
       </c>
       <c r="H13" s="565"/>
       <c r="I13" s="565"/>
-      <c r="J13" s="614"/>
+      <c r="J13" s="666"/>
       <c r="M13" s="6"/>
       <c r="N13" s="6"/>
-      <c r="O13" s="610"/>
-      <c r="P13" s="637"/>
+      <c r="O13" s="662"/>
+      <c r="P13" s="636"/>
       <c r="T13" s="105" t="s">
         <v>44</v>
       </c>
@@ -8610,8 +8613,8 @@
         <v>518</v>
       </c>
       <c r="AC13" s="16"/>
-      <c r="AD13" s="624"/>
-      <c r="AF13" s="616"/>
+      <c r="AD13" s="651"/>
+      <c r="AF13" s="643"/>
       <c r="AG13" s="80"/>
       <c r="AH13" s="243" t="s">
         <v>314</v>
@@ -8623,7 +8626,7 @@
       <c r="AK13" s="262"/>
       <c r="AL13" s="262"/>
       <c r="AM13" s="638"/>
-      <c r="AN13" s="626"/>
+      <c r="AN13" s="623"/>
     </row>
     <row r="14" spans="1:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="474"/>
@@ -8631,18 +8634,18 @@
       <c r="C14" s="483"/>
       <c r="D14" s="476"/>
       <c r="E14" s="477"/>
-      <c r="F14" s="607"/>
+      <c r="F14" s="628"/>
       <c r="G14" s="565" t="s">
         <v>446</v>
       </c>
       <c r="H14" s="565"/>
       <c r="I14" s="565"/>
-      <c r="J14" s="614"/>
+      <c r="J14" s="666"/>
       <c r="K14" s="2">
         <v>12</v>
       </c>
       <c r="N14" s="6"/>
-      <c r="O14" s="610"/>
+      <c r="O14" s="662"/>
       <c r="Q14" s="61" t="s">
         <v>554</v>
       </c>
@@ -8663,9 +8666,9 @@
       <c r="AA14" s="313"/>
       <c r="AB14" s="214"/>
       <c r="AC14" s="16"/>
-      <c r="AD14" s="624"/>
+      <c r="AD14" s="651"/>
       <c r="AE14" s="262"/>
-      <c r="AF14" s="616"/>
+      <c r="AF14" s="643"/>
       <c r="AG14" s="262"/>
       <c r="AH14" s="262"/>
       <c r="AI14" s="70"/>
@@ -8673,7 +8676,7 @@
       <c r="AK14" s="262"/>
       <c r="AL14" s="262"/>
       <c r="AM14" s="638"/>
-      <c r="AN14" s="626"/>
+      <c r="AN14" s="623"/>
     </row>
     <row r="15" spans="1:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="473" t="s">
@@ -8682,8 +8685,8 @@
       <c r="C15" s="558" t="s">
         <v>381</v>
       </c>
-      <c r="F15" s="607"/>
-      <c r="O15" s="610"/>
+      <c r="F15" s="628"/>
+      <c r="O15" s="662"/>
       <c r="R15" s="99" t="s">
         <v>44</v>
       </c>
@@ -8705,8 +8708,8 @@
       <c r="AC15" s="76" t="s">
         <v>496</v>
       </c>
-      <c r="AD15" s="624"/>
-      <c r="AF15" s="616"/>
+      <c r="AD15" s="651"/>
+      <c r="AF15" s="643"/>
       <c r="AG15" s="80"/>
       <c r="AH15" s="243" t="s">
         <v>465</v>
@@ -8720,7 +8723,7 @@
       <c r="AK15" s="262"/>
       <c r="AL15" s="262"/>
       <c r="AM15" s="638"/>
-      <c r="AN15" s="626"/>
+      <c r="AN15" s="623"/>
       <c r="AP15" s="76" t="s">
         <v>74</v>
       </c>
@@ -8742,13 +8745,13 @@
       <c r="E16" s="229">
         <v>1</v>
       </c>
-      <c r="F16" s="607"/>
+      <c r="F16" s="628"/>
       <c r="G16" s="349" t="s">
         <v>505</v>
       </c>
       <c r="I16" s="495"/>
       <c r="J16" s="20"/>
-      <c r="O16" s="610"/>
+      <c r="O16" s="662"/>
       <c r="R16" s="459" t="s">
         <v>185</v>
       </c>
@@ -8780,18 +8783,18 @@
       <c r="AM16" s="452" t="s">
         <v>324</v>
       </c>
-      <c r="AN16" s="626"/>
+      <c r="AN16" s="623"/>
       <c r="AP16" s="76" t="s">
         <v>235</v>
       </c>
     </row>
     <row r="17" spans="1:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B17" s="80"/>
-      <c r="F17" s="607"/>
+      <c r="F17" s="628"/>
       <c r="I17" s="496"/>
       <c r="J17" s="20"/>
       <c r="N17" s="6"/>
-      <c r="O17" s="610"/>
+      <c r="O17" s="662"/>
       <c r="Q17" s="21" t="s">
         <v>552</v>
       </c>
@@ -8836,7 +8839,7 @@
       <c r="AK17" s="262"/>
       <c r="AL17" s="80"/>
       <c r="AM17" s="452"/>
-      <c r="AN17" s="626"/>
+      <c r="AN17" s="623"/>
       <c r="AO17" s="209" t="s">
         <v>515</v>
       </c>
@@ -8860,21 +8863,21 @@
       <c r="E18" s="99" t="s">
         <v>44</v>
       </c>
-      <c r="F18" s="607"/>
+      <c r="F18" s="628"/>
       <c r="G18" s="349" t="s">
         <v>549</v>
       </c>
       <c r="I18" s="24"/>
       <c r="J18" s="20"/>
-      <c r="O18" s="610"/>
+      <c r="O18" s="662"/>
       <c r="Q18" s="112"/>
-      <c r="R18" s="602" t="s">
+      <c r="R18" s="656" t="s">
         <v>557</v>
       </c>
       <c r="T18" s="100" t="s">
         <v>44</v>
       </c>
-      <c r="U18" s="646" t="s">
+      <c r="U18" s="601" t="s">
         <v>44</v>
       </c>
       <c r="V18" s="120"/>
@@ -8895,7 +8898,7 @@
       <c r="AC18" s="16"/>
       <c r="AD18" s="16"/>
       <c r="AE18" s="262"/>
-      <c r="AF18" s="615" t="s">
+      <c r="AF18" s="637" t="s">
         <v>492</v>
       </c>
       <c r="AG18" s="262"/>
@@ -8907,20 +8910,20 @@
       <c r="AK18" s="262"/>
       <c r="AL18" s="80"/>
       <c r="AM18" s="452"/>
-      <c r="AN18" s="626"/>
+      <c r="AN18" s="623"/>
       <c r="AP18" s="76" t="s">
         <v>88</v>
       </c>
     </row>
     <row r="19" spans="1:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="F19" s="607"/>
+      <c r="F19" s="628"/>
       <c r="I19" s="224"/>
-      <c r="O19" s="610"/>
-      <c r="R19" s="603"/>
+      <c r="O19" s="662"/>
+      <c r="R19" s="657"/>
       <c r="S19" s="30" t="s">
         <v>555</v>
       </c>
-      <c r="U19" s="647"/>
+      <c r="U19" s="602"/>
       <c r="V19" s="146"/>
       <c r="W19" s="146"/>
       <c r="X19" s="455" t="s">
@@ -8935,7 +8938,7 @@
       <c r="AC19" s="16"/>
       <c r="AD19" s="16"/>
       <c r="AE19" s="262"/>
-      <c r="AF19" s="615"/>
+      <c r="AF19" s="637"/>
       <c r="AG19" s="262"/>
       <c r="AH19" s="262"/>
       <c r="AI19" s="70"/>
@@ -8945,7 +8948,7 @@
       </c>
       <c r="AL19" s="80"/>
       <c r="AM19" s="452"/>
-      <c r="AN19" s="626"/>
+      <c r="AN19" s="623"/>
       <c r="AP19" s="76" t="s">
         <v>485</v>
       </c>
@@ -8966,19 +8969,19 @@
       <c r="E20" s="461">
         <v>-1</v>
       </c>
-      <c r="F20" s="607"/>
+      <c r="F20" s="628"/>
       <c r="G20" s="349" t="s">
         <v>508</v>
       </c>
       <c r="I20" s="224"/>
-      <c r="O20" s="610"/>
-      <c r="Q20" s="612" t="s">
+      <c r="O20" s="662"/>
+      <c r="Q20" s="664" t="s">
         <v>48</v>
       </c>
       <c r="T20" s="428" t="s">
         <v>44</v>
       </c>
-      <c r="U20" s="648"/>
+      <c r="U20" s="603"/>
       <c r="W20" s="429"/>
       <c r="X20" s="456" t="s">
         <v>175</v>
@@ -9008,7 +9011,7 @@
       <c r="AM20" s="400" t="s">
         <v>254</v>
       </c>
-      <c r="AN20" s="626"/>
+      <c r="AN20" s="623"/>
       <c r="AO20" s="350" t="s">
         <v>477</v>
       </c>
@@ -9029,13 +9032,13 @@
       <c r="E21" s="271">
         <v>0</v>
       </c>
-      <c r="F21" s="607"/>
+      <c r="F21" s="628"/>
       <c r="I21" s="224"/>
-      <c r="O21" s="610"/>
-      <c r="Q21" s="613"/>
+      <c r="O21" s="662"/>
+      <c r="Q21" s="665"/>
       <c r="T21" s="446"/>
       <c r="U21" s="14"/>
-      <c r="V21" s="643"/>
+      <c r="V21" s="598"/>
       <c r="W21" s="450" t="s">
         <v>176</v>
       </c>
@@ -9073,15 +9076,15 @@
       <c r="AM21" s="452" t="s">
         <v>566</v>
       </c>
-      <c r="AN21" s="626"/>
+      <c r="AN21" s="623"/>
     </row>
     <row r="22" spans="1:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="F22" s="607"/>
+      <c r="F22" s="628"/>
       <c r="G22" s="349" t="s">
         <v>506</v>
       </c>
       <c r="I22" s="224"/>
-      <c r="O22" s="610"/>
+      <c r="O22" s="662"/>
       <c r="R22" s="458" t="s">
         <v>44</v>
       </c>
@@ -9089,7 +9092,7 @@
         <v>44</v>
       </c>
       <c r="U22" s="15"/>
-      <c r="V22" s="644"/>
+      <c r="V22" s="599"/>
       <c r="W22" s="450" t="s">
         <v>176</v>
       </c>
@@ -9107,7 +9110,7 @@
       <c r="AG22" s="6"/>
       <c r="AH22" s="6"/>
       <c r="AI22" s="6"/>
-      <c r="AJ22" s="615" t="s">
+      <c r="AJ22" s="637" t="s">
         <v>489</v>
       </c>
       <c r="AK22" s="262"/>
@@ -9115,7 +9118,7 @@
         <v>495</v>
       </c>
       <c r="AM22" s="306"/>
-      <c r="AN22" s="626"/>
+      <c r="AN22" s="623"/>
     </row>
     <row r="23" spans="1:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="236" t="s">
@@ -9133,17 +9136,17 @@
       <c r="E23" s="230">
         <v>1</v>
       </c>
-      <c r="F23" s="607"/>
+      <c r="F23" s="628"/>
       <c r="I23" s="224"/>
-      <c r="O23" s="610"/>
-      <c r="Q23" s="612" t="s">
+      <c r="O23" s="662"/>
+      <c r="Q23" s="664" t="s">
         <v>145</v>
       </c>
       <c r="T23" s="17"/>
       <c r="U23" s="444" t="s">
         <v>44</v>
       </c>
-      <c r="V23" s="644"/>
+      <c r="V23" s="599"/>
       <c r="W23" s="148"/>
       <c r="X23" s="453" t="s">
         <v>189</v>
@@ -9159,13 +9162,13 @@
       <c r="AG23" s="6"/>
       <c r="AH23" s="6"/>
       <c r="AI23" s="6"/>
-      <c r="AJ23" s="615"/>
+      <c r="AJ23" s="637"/>
       <c r="AK23" s="262"/>
       <c r="AL23" s="80" t="s">
         <v>525</v>
       </c>
       <c r="AM23" s="306"/>
-      <c r="AN23" s="626"/>
+      <c r="AN23" s="623"/>
     </row>
     <row r="24" spans="1:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="464" t="s">
@@ -9183,18 +9186,18 @@
       <c r="E24" s="460">
         <v>1</v>
       </c>
-      <c r="F24" s="607"/>
+      <c r="F24" s="628"/>
       <c r="G24" s="61" t="s">
         <v>507</v>
       </c>
       <c r="I24" s="224"/>
-      <c r="O24" s="610"/>
-      <c r="Q24" s="613"/>
+      <c r="O24" s="662"/>
+      <c r="Q24" s="665"/>
       <c r="T24" s="17"/>
       <c r="U24" s="232" t="s">
         <v>44</v>
       </c>
-      <c r="V24" s="644"/>
+      <c r="V24" s="599"/>
       <c r="W24" s="148"/>
       <c r="X24" s="453" t="s">
         <v>186</v>
@@ -9218,12 +9221,12 @@
         <v>480</v>
       </c>
       <c r="AM24" s="306"/>
-      <c r="AN24" s="626"/>
+      <c r="AN24" s="623"/>
     </row>
     <row r="25" spans="1:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="F25" s="607"/>
+      <c r="F25" s="628"/>
       <c r="I25" s="224"/>
-      <c r="O25" s="610"/>
+      <c r="O25" s="662"/>
       <c r="P25" s="209" t="s">
         <v>285</v>
       </c>
@@ -9236,7 +9239,7 @@
       <c r="U25" s="424" t="s">
         <v>44</v>
       </c>
-      <c r="V25" s="645"/>
+      <c r="V25" s="600"/>
       <c r="W25" s="148"/>
       <c r="X25" s="453" t="s">
         <v>190</v>
@@ -9258,7 +9261,7 @@
       <c r="AK25" s="142"/>
       <c r="AL25" s="6"/>
       <c r="AM25" s="306"/>
-      <c r="AN25" s="626"/>
+      <c r="AN25" s="623"/>
     </row>
     <row r="26" spans="1:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="236" t="s">
@@ -9276,17 +9279,17 @@
       <c r="E26" s="398">
         <v>1</v>
       </c>
-      <c r="F26" s="607"/>
+      <c r="F26" s="628"/>
       <c r="G26" s="349" t="s">
         <v>504</v>
       </c>
       <c r="I26" s="224"/>
-      <c r="O26" s="610"/>
-      <c r="P26" s="628" t="s">
+      <c r="O26" s="662"/>
+      <c r="P26" s="625" t="s">
         <v>547</v>
       </c>
-      <c r="Q26" s="629"/>
-      <c r="R26" s="604" t="s">
+      <c r="Q26" s="626"/>
+      <c r="R26" s="658" t="s">
         <v>556</v>
       </c>
       <c r="T26" s="182"/>
@@ -9325,7 +9328,7 @@
       <c r="AM26" s="466" t="s">
         <v>473</v>
       </c>
-      <c r="AN26" s="626"/>
+      <c r="AN26" s="623"/>
     </row>
     <row r="27" spans="1:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B27" s="21" t="s">
@@ -9337,13 +9340,13 @@
       <c r="E27" s="271" t="s">
         <v>44</v>
       </c>
-      <c r="F27" s="608"/>
+      <c r="F27" s="660"/>
       <c r="G27" s="61" t="s">
         <v>565</v>
       </c>
       <c r="I27" s="225"/>
-      <c r="O27" s="611"/>
-      <c r="R27" s="605"/>
+      <c r="O27" s="663"/>
+      <c r="R27" s="659"/>
       <c r="S27" s="445" t="s">
         <v>54</v>
       </c>
@@ -9373,10 +9376,48 @@
       <c r="AM27" s="400" t="s">
         <v>326</v>
       </c>
-      <c r="AN27" s="627"/>
+      <c r="AN27" s="624"/>
     </row>
   </sheetData>
   <mergeCells count="54">
+    <mergeCell ref="E2:E3"/>
+    <mergeCell ref="K2:L2"/>
+    <mergeCell ref="I1:I2"/>
+    <mergeCell ref="R18:R19"/>
+    <mergeCell ref="R26:R27"/>
+    <mergeCell ref="F2:F27"/>
+    <mergeCell ref="O10:O27"/>
+    <mergeCell ref="Q20:Q21"/>
+    <mergeCell ref="Q23:Q24"/>
+    <mergeCell ref="G14:J14"/>
+    <mergeCell ref="G13:J13"/>
+    <mergeCell ref="H12:K12"/>
+    <mergeCell ref="A5:A6"/>
+    <mergeCell ref="C6:D6"/>
+    <mergeCell ref="AI6:AI10"/>
+    <mergeCell ref="AF12:AF15"/>
+    <mergeCell ref="AG7:AG12"/>
+    <mergeCell ref="L8:L9"/>
+    <mergeCell ref="S9:S12"/>
+    <mergeCell ref="N8:N9"/>
+    <mergeCell ref="AD12:AD15"/>
+    <mergeCell ref="C15:C16"/>
+    <mergeCell ref="AN1:AN27"/>
+    <mergeCell ref="P26:Q26"/>
+    <mergeCell ref="Q2:Q3"/>
+    <mergeCell ref="M2:M9"/>
+    <mergeCell ref="O2:O9"/>
+    <mergeCell ref="P10:P13"/>
+    <mergeCell ref="AK6:AK7"/>
+    <mergeCell ref="AM12:AM15"/>
+    <mergeCell ref="AF18:AF19"/>
+    <mergeCell ref="AJ18:AJ19"/>
+    <mergeCell ref="Y1:Y27"/>
+    <mergeCell ref="AJ22:AJ23"/>
+    <mergeCell ref="AK9:AK10"/>
+    <mergeCell ref="AD3:AD4"/>
+    <mergeCell ref="S2:S3"/>
+    <mergeCell ref="R2:R3"/>
     <mergeCell ref="V21:V25"/>
     <mergeCell ref="U18:U20"/>
     <mergeCell ref="C2:C3"/>
@@ -9393,44 +9434,6 @@
     <mergeCell ref="B11:B12"/>
     <mergeCell ref="B6:B7"/>
     <mergeCell ref="B4:B5"/>
-    <mergeCell ref="AN1:AN27"/>
-    <mergeCell ref="P26:Q26"/>
-    <mergeCell ref="Q2:Q3"/>
-    <mergeCell ref="M2:M9"/>
-    <mergeCell ref="O2:O9"/>
-    <mergeCell ref="P10:P13"/>
-    <mergeCell ref="AK6:AK7"/>
-    <mergeCell ref="AM12:AM15"/>
-    <mergeCell ref="AF18:AF19"/>
-    <mergeCell ref="AJ18:AJ19"/>
-    <mergeCell ref="Y1:Y27"/>
-    <mergeCell ref="AJ22:AJ23"/>
-    <mergeCell ref="AK9:AK10"/>
-    <mergeCell ref="AD3:AD4"/>
-    <mergeCell ref="S2:S3"/>
-    <mergeCell ref="R2:R3"/>
-    <mergeCell ref="A5:A6"/>
-    <mergeCell ref="C6:D6"/>
-    <mergeCell ref="AI6:AI10"/>
-    <mergeCell ref="AF12:AF15"/>
-    <mergeCell ref="AG7:AG12"/>
-    <mergeCell ref="L8:L9"/>
-    <mergeCell ref="S9:S12"/>
-    <mergeCell ref="N8:N9"/>
-    <mergeCell ref="AD12:AD15"/>
-    <mergeCell ref="C15:C16"/>
-    <mergeCell ref="E2:E3"/>
-    <mergeCell ref="K2:L2"/>
-    <mergeCell ref="I1:I2"/>
-    <mergeCell ref="R18:R19"/>
-    <mergeCell ref="R26:R27"/>
-    <mergeCell ref="F2:F27"/>
-    <mergeCell ref="O10:O27"/>
-    <mergeCell ref="Q20:Q21"/>
-    <mergeCell ref="Q23:Q24"/>
-    <mergeCell ref="G14:J14"/>
-    <mergeCell ref="G13:J13"/>
-    <mergeCell ref="H12:K12"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -9440,8 +9443,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2029A93E-B53C-4201-9F17-439C144F3CF1}">
   <dimension ref="A1:AN37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="N1" workbookViewId="0">
-      <selection activeCell="J34" sqref="J34"/>
+    <sheetView tabSelected="1" topLeftCell="M18" workbookViewId="0">
+      <selection activeCell="AL30" sqref="AL30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9536,10 +9539,10 @@
       <c r="S1" s="142"/>
       <c r="T1" s="142"/>
       <c r="U1" s="6"/>
-      <c r="V1" s="670" t="s">
+      <c r="V1" s="673" t="s">
         <v>458</v>
       </c>
-      <c r="W1" s="671"/>
+      <c r="W1" s="674"/>
       <c r="X1" s="312">
         <f>68-(U8+W3+V3+S3)</f>
         <v>0</v>
@@ -9555,21 +9558,21 @@
       <c r="AB1" s="308" t="s">
         <v>44</v>
       </c>
-      <c r="AC1" s="672" t="s">
+      <c r="AC1" s="675" t="s">
         <v>191</v>
       </c>
-      <c r="AD1" s="673"/>
-      <c r="AE1" s="674"/>
-      <c r="AF1" s="675" t="s">
+      <c r="AD1" s="676"/>
+      <c r="AE1" s="677"/>
+      <c r="AF1" s="678" t="s">
         <v>298</v>
       </c>
-      <c r="AG1" s="676"/>
-      <c r="AH1" s="677"/>
-      <c r="AI1" s="667" t="s">
+      <c r="AG1" s="679"/>
+      <c r="AH1" s="680"/>
+      <c r="AI1" s="670" t="s">
         <v>461</v>
       </c>
-      <c r="AJ1" s="668"/>
-      <c r="AK1" s="669"/>
+      <c r="AJ1" s="671"/>
+      <c r="AK1" s="672"/>
       <c r="AN1" s="142"/>
     </row>
     <row r="2" spans="1:40" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -9586,19 +9589,19 @@
       <c r="K2" s="327">
         <v>-3</v>
       </c>
-      <c r="L2" s="678">
+      <c r="L2" s="681">
         <f>SUM(L5:L30)</f>
         <v>3</v>
       </c>
-      <c r="M2" s="680">
+      <c r="M2" s="683">
         <f>SUM(M4:M29)</f>
-        <v>9</v>
-      </c>
-      <c r="N2" s="682">
+        <v>10</v>
+      </c>
+      <c r="N2" s="685">
         <f>SUM(N4:N29)</f>
         <v>11</v>
       </c>
-      <c r="O2" s="622">
+      <c r="O2" s="649">
         <f>SUM(M30:M37)* (-1)</f>
         <v>-3</v>
       </c>
@@ -9617,7 +9620,7 @@
       <c r="T2" s="515" t="s">
         <v>221</v>
       </c>
-      <c r="U2" s="684" t="s">
+      <c r="U2" s="687" t="s">
         <v>239</v>
       </c>
       <c r="V2" s="516" t="s">
@@ -9686,10 +9689,10 @@
         <f>T3+V3+W3+S3</f>
         <v>68</v>
       </c>
-      <c r="L3" s="679"/>
-      <c r="M3" s="681"/>
-      <c r="N3" s="683"/>
-      <c r="O3" s="623"/>
+      <c r="L3" s="682"/>
+      <c r="M3" s="684"/>
+      <c r="N3" s="686"/>
+      <c r="O3" s="650"/>
       <c r="P3" s="176">
         <f>(L2+M2)-W3</f>
         <v>0</v>
@@ -9703,16 +9706,16 @@
       </c>
       <c r="T3" s="518">
         <f>SUM(T4:T29)</f>
-        <v>37</v>
-      </c>
-      <c r="U3" s="685"/>
+        <v>36</v>
+      </c>
+      <c r="U3" s="688"/>
       <c r="V3" s="519">
         <f t="shared" ref="V3:AA3" si="0">SUM(V4:V29)</f>
         <v>7</v>
       </c>
       <c r="W3" s="519">
         <f t="shared" si="0"/>
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="X3" s="59">
         <f t="shared" si="0"/>
@@ -9724,7 +9727,7 @@
       </c>
       <c r="Z3" s="66">
         <f t="shared" si="0"/>
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="AA3" s="66">
         <f t="shared" si="0"/>
@@ -9804,7 +9807,7 @@
         <f>AA4</f>
         <v>0</v>
       </c>
-      <c r="O4" s="686" t="s">
+      <c r="O4" s="667" t="s">
         <v>200</v>
       </c>
       <c r="P4" s="20"/>
@@ -9883,7 +9886,7 @@
         <f>AA5</f>
         <v>0</v>
       </c>
-      <c r="O5" s="687"/>
+      <c r="O5" s="668"/>
       <c r="P5" s="20"/>
       <c r="Q5" s="2" t="s">
         <v>347</v>
@@ -9970,7 +9973,7 @@
         <f>AA6</f>
         <v>0</v>
       </c>
-      <c r="O6" s="687"/>
+      <c r="O6" s="668"/>
       <c r="P6" s="19" t="s">
         <v>342</v>
       </c>
@@ -10062,7 +10065,7 @@
         <f t="shared" ref="N7:N37" si="10">AA7</f>
         <v>0</v>
       </c>
-      <c r="O7" s="687"/>
+      <c r="O7" s="668"/>
       <c r="P7" s="20"/>
       <c r="Q7" s="2" t="s">
         <v>342</v>
@@ -10168,7 +10171,7 @@
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
-      <c r="O8" s="687"/>
+      <c r="O8" s="668"/>
       <c r="P8" s="21" t="s">
         <v>238</v>
       </c>
@@ -10186,7 +10189,7 @@
       </c>
       <c r="U8" s="29">
         <f>T3</f>
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="V8" s="531">
         <v>0</v>
@@ -10252,7 +10255,7 @@
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
-      <c r="O9" s="687"/>
+      <c r="O9" s="668"/>
       <c r="P9" s="21" t="s">
         <v>342</v>
       </c>
@@ -10350,7 +10353,7 @@
         <f t="shared" si="10"/>
         <v>2</v>
       </c>
-      <c r="O10" s="687"/>
+      <c r="O10" s="668"/>
       <c r="P10" s="20"/>
       <c r="Q10" s="2" t="s">
         <v>347</v>
@@ -10433,7 +10436,7 @@
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
-      <c r="O11" s="687"/>
+      <c r="O11" s="668"/>
       <c r="P11" s="21" t="s">
         <v>342</v>
       </c>
@@ -10493,7 +10496,7 @@
       <c r="AN11" s="142"/>
     </row>
     <row r="12" spans="1:40" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="658" t="s">
+      <c r="A12" s="613" t="s">
         <v>55</v>
       </c>
       <c r="B12" s="30">
@@ -10502,7 +10505,7 @@
       <c r="C12" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="E12" s="612" t="s">
+      <c r="E12" s="664" t="s">
         <v>57</v>
       </c>
       <c r="G12" s="267"/>
@@ -10523,7 +10526,7 @@
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
-      <c r="O12" s="687"/>
+      <c r="O12" s="668"/>
       <c r="P12" s="21" t="s">
         <v>342</v>
       </c>
@@ -10595,14 +10598,14 @@
       </c>
     </row>
     <row r="13" spans="1:40" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="660"/>
+      <c r="A13" s="615"/>
       <c r="B13" s="153">
         <v>12</v>
       </c>
       <c r="C13" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="E13" s="613"/>
+      <c r="E13" s="665"/>
       <c r="F13" s="176">
         <v>0</v>
       </c>
@@ -10625,7 +10628,7 @@
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
-      <c r="O13" s="687"/>
+      <c r="O13" s="668"/>
       <c r="P13" s="21" t="s">
         <v>342</v>
       </c>
@@ -10701,7 +10704,7 @@
         <f t="shared" si="10"/>
         <v>2</v>
       </c>
-      <c r="O14" s="687"/>
+      <c r="O14" s="668"/>
       <c r="P14" s="20"/>
       <c r="Q14" s="205" t="s">
         <v>346</v>
@@ -10796,7 +10799,7 @@
         <f t="shared" si="10"/>
         <v>1</v>
       </c>
-      <c r="O15" s="687"/>
+      <c r="O15" s="668"/>
       <c r="P15" s="20"/>
       <c r="Q15" s="205" t="s">
         <v>346</v>
@@ -10883,7 +10886,7 @@
         <f t="shared" si="10"/>
         <v>1</v>
       </c>
-      <c r="O16" s="687"/>
+      <c r="O16" s="668"/>
       <c r="P16" s="21" t="s">
         <v>342</v>
       </c>
@@ -10981,7 +10984,7 @@
         <f t="shared" si="10"/>
         <v>1</v>
       </c>
-      <c r="O17" s="687"/>
+      <c r="O17" s="668"/>
       <c r="P17" s="20"/>
       <c r="Q17" s="2" t="s">
         <v>348</v>
@@ -11076,7 +11079,7 @@
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
-      <c r="O18" s="687"/>
+      <c r="O18" s="668"/>
       <c r="P18" s="21" t="s">
         <v>342</v>
       </c>
@@ -11159,7 +11162,7 @@
         <f t="shared" si="10"/>
         <v>1</v>
       </c>
-      <c r="O19" s="687"/>
+      <c r="O19" s="668"/>
       <c r="P19" s="20"/>
       <c r="Q19" s="2" t="s">
         <v>341</v>
@@ -11257,11 +11260,11 @@
         <f t="shared" si="10"/>
         <v>1</v>
       </c>
-      <c r="O20" s="688"/>
+      <c r="O20" s="669"/>
       <c r="P20" s="563" t="s">
         <v>342</v>
       </c>
-      <c r="Q20" s="614"/>
+      <c r="Q20" s="666"/>
       <c r="R20" s="321" t="s">
         <v>86</v>
       </c>
@@ -11497,7 +11500,7 @@
       <c r="AN22" s="142"/>
     </row>
     <row r="23" spans="1:40" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E23" s="665" t="s">
+      <c r="E23" s="620" t="s">
         <v>294</v>
       </c>
       <c r="F23" s="184"/>
@@ -11593,10 +11596,10 @@
       <c r="C24" s="2" t="s">
         <v>260</v>
       </c>
-      <c r="E24" s="666"/>
+      <c r="E24" s="621"/>
       <c r="F24" s="176"/>
       <c r="H24" s="42">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="K24" s="403" t="s">
         <v>301</v>
@@ -11605,7 +11608,7 @@
         <v>0</v>
       </c>
       <c r="M24" s="107">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N24" s="299">
         <f t="shared" si="10"/>
@@ -11614,7 +11617,7 @@
       <c r="P24" s="563" t="s">
         <v>342</v>
       </c>
-      <c r="Q24" s="614"/>
+      <c r="Q24" s="666"/>
       <c r="R24" s="321" t="s">
         <v>254</v>
       </c>
@@ -11622,7 +11625,7 @@
         <v>2</v>
       </c>
       <c r="T24" s="526">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="U24" s="527">
         <v>-2</v>
@@ -11630,7 +11633,7 @@
       <c r="V24" s="538"/>
       <c r="W24" s="524">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="X24" s="302"/>
       <c r="Y24" s="117">
@@ -11639,7 +11642,7 @@
       </c>
       <c r="Z24" s="296">
         <f t="shared" si="6"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AA24" s="296">
         <v>1</v>
@@ -11678,7 +11681,9 @@
       <c r="AL24" s="6" t="s">
         <v>527</v>
       </c>
-      <c r="AM24" s="546"/>
+      <c r="AM24" s="741" t="s">
+        <v>342</v>
+      </c>
       <c r="AN24" s="142" t="s">
         <v>254</v>
       </c>
@@ -12136,7 +12141,7 @@
         <v>-1</v>
       </c>
       <c r="H31" s="42">
-        <v>-5</v>
+        <v>-3</v>
       </c>
       <c r="I31" s="21" t="s">
         <v>435</v>
@@ -12358,6 +12363,9 @@
       <c r="E34" s="19" t="s">
         <v>304</v>
       </c>
+      <c r="H34" s="42">
+        <v>-1</v>
+      </c>
       <c r="K34" s="403" t="s">
         <v>305</v>
       </c>
@@ -12367,7 +12375,7 @@
       </c>
       <c r="N34" s="299">
         <f t="shared" si="10"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="P34" s="21" t="s">
         <v>342</v>
@@ -12392,41 +12400,41 @@
       <c r="X34" s="65"/>
       <c r="Y34" s="117">
         <f t="shared" si="3"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="Z34" s="64">
         <f t="shared" si="6"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AA34" s="64">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AB34" s="307">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="AC34" s="362">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AD34" s="366"/>
       <c r="AE34" s="367"/>
       <c r="AF34" s="325">
         <f t="shared" si="5"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AG34" s="348"/>
       <c r="AH34" s="326"/>
       <c r="AI34" s="347">
         <f t="shared" si="7"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AJ34" s="315">
         <f t="shared" si="8"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AK34" s="316">
         <f t="shared" si="9"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AL34" s="6"/>
       <c r="AM34" s="546" t="s">
@@ -12681,12 +12689,6 @@
     </row>
   </sheetData>
   <mergeCells count="15">
-    <mergeCell ref="A12:A13"/>
-    <mergeCell ref="E12:E13"/>
-    <mergeCell ref="P20:Q20"/>
-    <mergeCell ref="E23:E24"/>
-    <mergeCell ref="P24:Q24"/>
-    <mergeCell ref="O4:O20"/>
     <mergeCell ref="AI1:AK1"/>
     <mergeCell ref="V1:W1"/>
     <mergeCell ref="AC1:AE1"/>
@@ -12696,6 +12698,12 @@
     <mergeCell ref="N2:N3"/>
     <mergeCell ref="O2:O3"/>
     <mergeCell ref="U2:U3"/>
+    <mergeCell ref="A12:A13"/>
+    <mergeCell ref="E12:E13"/>
+    <mergeCell ref="P20:Q20"/>
+    <mergeCell ref="E23:E24"/>
+    <mergeCell ref="P24:Q24"/>
+    <mergeCell ref="O4:O20"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -12733,12 +12741,12 @@
       <c r="B1" s="563" t="s">
         <v>317</v>
       </c>
-      <c r="C1" s="614"/>
+      <c r="C1" s="666"/>
       <c r="D1" s="209"/>
       <c r="J1" s="563" t="s">
         <v>70</v>
       </c>
-      <c r="K1" s="614"/>
+      <c r="K1" s="666"/>
       <c r="L1" s="200" t="s">
         <v>337</v>
       </c>
@@ -13129,7 +13137,7 @@
       <c r="V1" s="563" t="s">
         <v>71</v>
       </c>
-      <c r="W1" s="614"/>
+      <c r="W1" s="666"/>
       <c r="X1" s="62" t="s">
         <v>102</v>
       </c>
@@ -13148,7 +13156,7 @@
       <c r="AC1" s="116" t="s">
         <v>191</v>
       </c>
-      <c r="AD1" s="702" t="s">
+      <c r="AD1" s="709" t="s">
         <v>213</v>
       </c>
       <c r="AE1" s="116" t="s">
@@ -13165,10 +13173,10 @@
       <c r="E2" s="39" t="s">
         <v>74</v>
       </c>
-      <c r="F2" s="701" t="s">
+      <c r="F2" s="740" t="s">
         <v>75</v>
       </c>
-      <c r="G2" s="729" t="s">
+      <c r="G2" s="697" t="s">
         <v>44</v>
       </c>
       <c r="H2" s="40" t="s">
@@ -13196,10 +13204,10 @@
       <c r="U2" s="60" t="s">
         <v>106</v>
       </c>
-      <c r="V2" s="670" t="s">
+      <c r="V2" s="673" t="s">
         <v>121</v>
       </c>
-      <c r="W2" s="671"/>
+      <c r="W2" s="674"/>
       <c r="X2" s="64" t="s">
         <v>110</v>
       </c>
@@ -13218,7 +13226,7 @@
       <c r="AC2" s="117" t="s">
         <v>99</v>
       </c>
-      <c r="AD2" s="703"/>
+      <c r="AD2" s="710"/>
       <c r="AE2" s="64" t="s">
         <v>99</v>
       </c>
@@ -13237,8 +13245,8 @@
       <c r="E3" s="39" t="s">
         <v>80</v>
       </c>
-      <c r="F3" s="662"/>
-      <c r="G3" s="730"/>
+      <c r="F3" s="617"/>
+      <c r="G3" s="698"/>
       <c r="H3" s="40" t="s">
         <v>81</v>
       </c>
@@ -13249,13 +13257,13 @@
         <v>82</v>
       </c>
       <c r="N3" s="44"/>
-      <c r="O3" s="739" t="s">
+      <c r="O3" s="707" t="s">
         <v>44</v>
       </c>
-      <c r="P3" s="721" t="s">
+      <c r="P3" s="728" t="s">
         <v>219</v>
       </c>
-      <c r="Q3" s="722"/>
+      <c r="Q3" s="729"/>
       <c r="S3" s="57" t="s">
         <v>220</v>
       </c>
@@ -13265,15 +13273,15 @@
       <c r="W3" s="59" t="s">
         <v>105</v>
       </c>
-      <c r="AD3" s="703"/>
+      <c r="AD3" s="710"/>
     </row>
     <row r="4" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="G4" s="730"/>
+      <c r="G4" s="698"/>
       <c r="H4" s="6"/>
       <c r="L4" s="692" t="s">
         <v>83</v>
       </c>
-      <c r="O4" s="740"/>
+      <c r="O4" s="708"/>
       <c r="T4" s="55" t="s">
         <v>98</v>
       </c>
@@ -13287,8 +13295,8 @@
         <v>195</v>
       </c>
       <c r="Z4" s="565"/>
-      <c r="AA4" s="614"/>
-      <c r="AD4" s="703"/>
+      <c r="AA4" s="666"/>
+      <c r="AD4" s="710"/>
     </row>
     <row r="5" spans="1:31" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C5" s="52" t="s">
@@ -13303,21 +13311,21 @@
       <c r="F5" s="66" t="s">
         <v>85</v>
       </c>
-      <c r="G5" s="730"/>
+      <c r="G5" s="698"/>
       <c r="H5" s="46" t="s">
         <v>76</v>
       </c>
-      <c r="K5" s="708" t="s">
+      <c r="K5" s="715" t="s">
         <v>217</v>
       </c>
-      <c r="L5" s="723"/>
+      <c r="L5" s="730"/>
       <c r="M5" s="2" t="s">
         <v>215</v>
       </c>
       <c r="N5" s="61" t="s">
         <v>214</v>
       </c>
-      <c r="O5" s="740"/>
+      <c r="O5" s="708"/>
       <c r="P5" s="108" t="s">
         <v>216</v>
       </c>
@@ -13333,11 +13341,11 @@
       <c r="U5" s="19" t="s">
         <v>99</v>
       </c>
-      <c r="Y5" s="711" t="s">
+      <c r="Y5" s="718" t="s">
         <v>287</v>
       </c>
-      <c r="Z5" s="712"/>
-      <c r="AD5" s="703"/>
+      <c r="Z5" s="719"/>
+      <c r="AD5" s="710"/>
     </row>
     <row r="6" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C6" s="109"/>
@@ -13347,16 +13355,16 @@
       <c r="E6" s="45" t="s">
         <v>86</v>
       </c>
-      <c r="G6" s="730"/>
+      <c r="G6" s="698"/>
       <c r="H6" s="46" t="s">
         <v>81</v>
       </c>
       <c r="I6" s="23">
         <v>15</v>
       </c>
-      <c r="K6" s="709"/>
-      <c r="L6" s="723"/>
-      <c r="O6" s="740"/>
+      <c r="K6" s="716"/>
+      <c r="L6" s="730"/>
+      <c r="O6" s="708"/>
       <c r="T6" s="2" t="s">
         <v>101</v>
       </c>
@@ -13366,23 +13374,23 @@
       <c r="V6" s="21">
         <v>-1</v>
       </c>
-      <c r="AD6" s="703"/>
+      <c r="AD6" s="710"/>
     </row>
     <row r="7" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C7" s="110"/>
-      <c r="G7" s="730"/>
+      <c r="G7" s="698"/>
       <c r="H7" s="6"/>
-      <c r="K7" s="709"/>
-      <c r="L7" s="723"/>
+      <c r="K7" s="716"/>
+      <c r="L7" s="730"/>
       <c r="N7" s="21" t="s">
         <v>120</v>
       </c>
-      <c r="O7" s="740"/>
+      <c r="O7" s="708"/>
       <c r="P7" s="73"/>
       <c r="U7" s="104" t="s">
         <v>20</v>
       </c>
-      <c r="AD7" s="703"/>
+      <c r="AD7" s="710"/>
     </row>
     <row r="8" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C8" s="130"/>
@@ -13395,7 +13403,7 @@
       <c r="F8" s="66" t="s">
         <v>87</v>
       </c>
-      <c r="G8" s="730"/>
+      <c r="G8" s="698"/>
       <c r="H8" s="50" t="s">
         <v>76</v>
       </c>
@@ -13405,41 +13413,41 @@
       <c r="J8" s="111">
         <v>115</v>
       </c>
-      <c r="K8" s="709"/>
-      <c r="L8" s="723"/>
-      <c r="O8" s="740"/>
+      <c r="K8" s="716"/>
+      <c r="L8" s="730"/>
+      <c r="O8" s="708"/>
       <c r="P8" s="49"/>
-      <c r="S8" s="705" t="s">
+      <c r="S8" s="712" t="s">
         <v>212</v>
       </c>
-      <c r="T8" s="706"/>
-      <c r="U8" s="706"/>
-      <c r="V8" s="706"/>
-      <c r="W8" s="706"/>
-      <c r="X8" s="706"/>
-      <c r="Y8" s="706"/>
-      <c r="Z8" s="706"/>
-      <c r="AA8" s="706"/>
-      <c r="AB8" s="706"/>
-      <c r="AC8" s="707"/>
-      <c r="AD8" s="703"/>
+      <c r="T8" s="713"/>
+      <c r="U8" s="713"/>
+      <c r="V8" s="713"/>
+      <c r="W8" s="713"/>
+      <c r="X8" s="713"/>
+      <c r="Y8" s="713"/>
+      <c r="Z8" s="713"/>
+      <c r="AA8" s="713"/>
+      <c r="AB8" s="713"/>
+      <c r="AC8" s="714"/>
+      <c r="AD8" s="710"/>
     </row>
     <row r="9" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C9" s="695"/>
-      <c r="G9" s="730"/>
+      <c r="C9" s="734"/>
+      <c r="G9" s="698"/>
       <c r="H9" s="6"/>
-      <c r="K9" s="709"/>
-      <c r="L9" s="733" t="s">
+      <c r="K9" s="716"/>
+      <c r="L9" s="701" t="s">
         <v>218</v>
       </c>
-      <c r="M9" s="734"/>
-      <c r="N9" s="735"/>
-      <c r="O9" s="740"/>
+      <c r="M9" s="702"/>
+      <c r="N9" s="703"/>
+      <c r="O9" s="708"/>
       <c r="P9" s="75"/>
-      <c r="AD9" s="703"/>
+      <c r="AD9" s="710"/>
     </row>
     <row r="10" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C10" s="696"/>
+      <c r="C10" s="735"/>
       <c r="D10" s="23"/>
       <c r="E10" s="45" t="s">
         <v>88</v>
@@ -13447,7 +13455,7 @@
       <c r="F10" s="66" t="s">
         <v>89</v>
       </c>
-      <c r="G10" s="730"/>
+      <c r="G10" s="698"/>
       <c r="H10" s="51"/>
       <c r="I10" s="21" t="s">
         <v>81</v>
@@ -13455,33 +13463,33 @@
       <c r="J10" s="3">
         <v>15</v>
       </c>
-      <c r="K10" s="709"/>
-      <c r="M10" s="698" t="s">
+      <c r="K10" s="716"/>
+      <c r="M10" s="737" t="s">
         <v>90</v>
       </c>
-      <c r="N10" s="699"/>
-      <c r="O10" s="699"/>
-      <c r="P10" s="699"/>
-      <c r="Q10" s="699"/>
-      <c r="R10" s="699"/>
-      <c r="S10" s="699"/>
-      <c r="T10" s="699"/>
-      <c r="U10" s="699"/>
-      <c r="V10" s="699"/>
-      <c r="W10" s="699"/>
-      <c r="X10" s="699"/>
-      <c r="Y10" s="699"/>
-      <c r="Z10" s="699"/>
-      <c r="AA10" s="699"/>
-      <c r="AB10" s="699"/>
-      <c r="AC10" s="700"/>
-      <c r="AD10" s="703"/>
+      <c r="N10" s="738"/>
+      <c r="O10" s="738"/>
+      <c r="P10" s="738"/>
+      <c r="Q10" s="738"/>
+      <c r="R10" s="738"/>
+      <c r="S10" s="738"/>
+      <c r="T10" s="738"/>
+      <c r="U10" s="738"/>
+      <c r="V10" s="738"/>
+      <c r="W10" s="738"/>
+      <c r="X10" s="738"/>
+      <c r="Y10" s="738"/>
+      <c r="Z10" s="738"/>
+      <c r="AA10" s="738"/>
+      <c r="AB10" s="738"/>
+      <c r="AC10" s="739"/>
+      <c r="AD10" s="710"/>
     </row>
     <row r="11" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C11" s="697"/>
-      <c r="G11" s="730"/>
+      <c r="C11" s="736"/>
+      <c r="G11" s="698"/>
       <c r="H11" s="6"/>
-      <c r="K11" s="709"/>
+      <c r="K11" s="716"/>
       <c r="R11" s="52" t="s">
         <v>44</v>
       </c>
@@ -13489,17 +13497,17 @@
       <c r="Y11" s="68" t="s">
         <v>121</v>
       </c>
-      <c r="Z11" s="719" t="s">
+      <c r="Z11" s="726" t="s">
         <v>121</v>
       </c>
-      <c r="AA11" s="720"/>
+      <c r="AA11" s="727"/>
       <c r="AB11" s="52" t="s">
         <v>44</v>
       </c>
       <c r="AC11" s="118" t="s">
         <v>121</v>
       </c>
-      <c r="AD11" s="703"/>
+      <c r="AD11" s="710"/>
     </row>
     <row r="12" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C12" s="129"/>
@@ -13512,7 +13520,7 @@
       <c r="F12" s="66" t="s">
         <v>92</v>
       </c>
-      <c r="G12" s="730"/>
+      <c r="G12" s="698"/>
       <c r="H12" s="128"/>
       <c r="I12" s="19" t="s">
         <v>81</v>
@@ -13520,8 +13528,8 @@
       <c r="J12" s="3">
         <v>15</v>
       </c>
-      <c r="K12" s="709"/>
-      <c r="L12" s="724" t="s">
+      <c r="K12" s="716"/>
+      <c r="L12" s="731" t="s">
         <v>93</v>
       </c>
       <c r="M12" s="21" t="s">
@@ -13552,25 +13560,25 @@
         <v>116</v>
       </c>
       <c r="Y12" s="6"/>
-      <c r="AA12" s="713" t="s">
+      <c r="AA12" s="720" t="s">
         <v>126</v>
       </c>
-      <c r="AB12" s="714"/>
+      <c r="AB12" s="721"/>
       <c r="AC12" s="21" t="s">
         <v>233</v>
       </c>
-      <c r="AD12" s="703"/>
+      <c r="AD12" s="710"/>
     </row>
     <row r="13" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C13" s="695"/>
-      <c r="G13" s="730"/>
-      <c r="K13" s="709"/>
-      <c r="L13" s="725"/>
+      <c r="C13" s="734"/>
+      <c r="G13" s="698"/>
+      <c r="K13" s="716"/>
+      <c r="L13" s="732"/>
       <c r="M13" s="47"/>
-      <c r="Q13" s="732" t="s">
+      <c r="Q13" s="700" t="s">
         <v>210</v>
       </c>
-      <c r="R13" s="629"/>
+      <c r="R13" s="626"/>
       <c r="S13" s="559"/>
       <c r="T13" s="6"/>
       <c r="U13" s="96" t="s">
@@ -13579,17 +13587,17 @@
       <c r="X13" s="2" t="s">
         <v>123</v>
       </c>
-      <c r="AA13" s="715"/>
-      <c r="AB13" s="716"/>
-      <c r="AD13" s="703"/>
+      <c r="AA13" s="722"/>
+      <c r="AB13" s="723"/>
+      <c r="AD13" s="710"/>
     </row>
     <row r="14" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B14" s="2" t="s">
         <v>339</v>
       </c>
-      <c r="C14" s="697"/>
+      <c r="C14" s="736"/>
       <c r="D14" s="23"/>
-      <c r="G14" s="730"/>
+      <c r="G14" s="698"/>
       <c r="H14" s="125"/>
       <c r="I14" s="99" t="s">
         <v>44</v>
@@ -13597,8 +13605,8 @@
       <c r="J14" s="111">
         <v>115</v>
       </c>
-      <c r="K14" s="709"/>
-      <c r="L14" s="725"/>
+      <c r="K14" s="716"/>
+      <c r="L14" s="732"/>
       <c r="M14" s="21" t="s">
         <v>111</v>
       </c>
@@ -13619,9 +13627,9 @@
       <c r="Y14" s="21" t="s">
         <v>73</v>
       </c>
-      <c r="AA14" s="715"/>
-      <c r="AB14" s="716"/>
-      <c r="AD14" s="703"/>
+      <c r="AA14" s="722"/>
+      <c r="AB14" s="723"/>
+      <c r="AD14" s="710"/>
     </row>
     <row r="15" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C15" s="130" t="s">
@@ -13636,19 +13644,19 @@
       <c r="F15" s="66" t="s">
         <v>94</v>
       </c>
-      <c r="G15" s="730"/>
+      <c r="G15" s="698"/>
       <c r="H15" s="2" t="s">
         <v>81</v>
       </c>
       <c r="I15" s="53" t="s">
         <v>81</v>
       </c>
-      <c r="K15" s="709"/>
-      <c r="L15" s="726"/>
-      <c r="Q15" s="732" t="s">
+      <c r="K15" s="716"/>
+      <c r="L15" s="733"/>
+      <c r="Q15" s="700" t="s">
         <v>211</v>
       </c>
-      <c r="R15" s="629"/>
+      <c r="R15" s="626"/>
       <c r="S15" s="559"/>
       <c r="T15" s="6"/>
       <c r="V15" s="68" t="s">
@@ -13657,14 +13665,14 @@
       <c r="X15" s="2" t="s">
         <v>128</v>
       </c>
-      <c r="AA15" s="715"/>
-      <c r="AB15" s="716"/>
-      <c r="AD15" s="703"/>
+      <c r="AA15" s="722"/>
+      <c r="AB15" s="723"/>
+      <c r="AD15" s="710"/>
     </row>
     <row r="16" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C16" s="132"/>
-      <c r="G16" s="730"/>
-      <c r="K16" s="709"/>
+      <c r="G16" s="698"/>
+      <c r="K16" s="716"/>
       <c r="N16" s="47"/>
       <c r="O16" s="61" t="s">
         <v>109</v>
@@ -13683,24 +13691,24 @@
       <c r="Z16" s="76" t="s">
         <v>127</v>
       </c>
-      <c r="AA16" s="715"/>
-      <c r="AB16" s="716"/>
-      <c r="AD16" s="703"/>
+      <c r="AA16" s="722"/>
+      <c r="AB16" s="723"/>
+      <c r="AD16" s="710"/>
     </row>
     <row r="17" spans="3:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C17" s="109"/>
       <c r="E17" s="6" t="s">
         <v>95</v>
       </c>
-      <c r="F17" s="727" t="s">
+      <c r="F17" s="695" t="s">
         <v>96</v>
       </c>
-      <c r="G17" s="730"/>
+      <c r="G17" s="698"/>
       <c r="H17" s="54"/>
       <c r="I17" s="133" t="s">
         <v>81</v>
       </c>
-      <c r="K17" s="709"/>
+      <c r="K17" s="716"/>
       <c r="S17" s="559"/>
       <c r="V17" s="68" t="s">
         <v>44</v>
@@ -13708,9 +13716,9 @@
       <c r="X17" s="2" t="s">
         <v>118</v>
       </c>
-      <c r="AA17" s="715"/>
-      <c r="AB17" s="716"/>
-      <c r="AD17" s="703"/>
+      <c r="AA17" s="722"/>
+      <c r="AB17" s="723"/>
+      <c r="AD17" s="710"/>
     </row>
     <row r="18" spans="3:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C18" s="130"/>
@@ -13720,15 +13728,15 @@
       <c r="E18" s="6" t="s">
         <v>97</v>
       </c>
-      <c r="F18" s="728"/>
-      <c r="G18" s="730"/>
+      <c r="F18" s="696"/>
+      <c r="G18" s="698"/>
       <c r="H18" s="108" t="s">
         <v>76</v>
       </c>
       <c r="I18" s="21" t="s">
         <v>81</v>
       </c>
-      <c r="K18" s="709"/>
+      <c r="K18" s="716"/>
       <c r="O18" s="64" t="s">
         <v>115</v>
       </c>
@@ -13739,42 +13747,39 @@
       <c r="X18" s="2" t="s">
         <v>117</v>
       </c>
-      <c r="AA18" s="717"/>
-      <c r="AB18" s="718"/>
-      <c r="AD18" s="703"/>
+      <c r="AA18" s="724"/>
+      <c r="AB18" s="725"/>
+      <c r="AD18" s="710"/>
     </row>
     <row r="19" spans="3:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="F19" s="64" t="s">
         <v>209</v>
       </c>
-      <c r="G19" s="731"/>
-      <c r="K19" s="710"/>
+      <c r="G19" s="699"/>
+      <c r="K19" s="717"/>
       <c r="Q19" s="68" t="s">
         <v>44</v>
       </c>
-      <c r="R19" s="736" t="s">
+      <c r="R19" s="704" t="s">
         <v>124</v>
       </c>
-      <c r="S19" s="737"/>
-      <c r="T19" s="738"/>
+      <c r="S19" s="705"/>
+      <c r="T19" s="706"/>
       <c r="V19" s="77" t="s">
         <v>115</v>
       </c>
       <c r="Y19" s="19" t="s">
         <v>125</v>
       </c>
-      <c r="AD19" s="704"/>
+      <c r="AD19" s="711"/>
     </row>
   </sheetData>
   <mergeCells count="24">
-    <mergeCell ref="F17:F18"/>
-    <mergeCell ref="G2:G19"/>
-    <mergeCell ref="Q13:R13"/>
-    <mergeCell ref="Q15:R15"/>
-    <mergeCell ref="L9:N9"/>
-    <mergeCell ref="R19:T19"/>
-    <mergeCell ref="S12:S18"/>
-    <mergeCell ref="O3:O9"/>
+    <mergeCell ref="C9:C11"/>
+    <mergeCell ref="C13:C14"/>
+    <mergeCell ref="V2:W2"/>
+    <mergeCell ref="M10:AC10"/>
+    <mergeCell ref="F2:F3"/>
     <mergeCell ref="AD1:AD19"/>
     <mergeCell ref="S8:AC8"/>
     <mergeCell ref="K5:K19"/>
@@ -13786,11 +13791,14 @@
     <mergeCell ref="P3:Q3"/>
     <mergeCell ref="L4:L8"/>
     <mergeCell ref="L12:L15"/>
-    <mergeCell ref="C9:C11"/>
-    <mergeCell ref="C13:C14"/>
-    <mergeCell ref="V2:W2"/>
-    <mergeCell ref="M10:AC10"/>
-    <mergeCell ref="F2:F3"/>
+    <mergeCell ref="F17:F18"/>
+    <mergeCell ref="G2:G19"/>
+    <mergeCell ref="Q13:R13"/>
+    <mergeCell ref="Q15:R15"/>
+    <mergeCell ref="L9:N9"/>
+    <mergeCell ref="R19:T19"/>
+    <mergeCell ref="S12:S18"/>
+    <mergeCell ref="O3:O9"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Boat Enabled - TimesNow NB , IndiaToday
Boat Enabled - Times Now NB

ShieldW - ND TV India

Boat Enabled - IndiaToday - WPJ
</commit_message>
<xml_diff>
--- a/System_2.1.5.xlsx
+++ b/System_2.1.5.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Work\Work_For_\Work\Running AppS\System_Work_RW\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD520114-03BD-4AC2-91D9-3F9BD42E2B38}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5037B8F0-3D26-4A07-A5C5-65F2BA75F3DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1097" uniqueCount="616">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1104" uniqueCount="621">
   <si>
     <t>Zone</t>
   </si>
@@ -1887,6 +1887,21 @@
   </si>
   <si>
     <t>Wbt_X_5F</t>
+  </si>
+  <si>
+    <t>Times Now NB</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> WLFIT_X_N-17_X_Left_UnTagged</t>
+  </si>
+  <si>
+    <t>5F</t>
+  </si>
+  <si>
+    <t>9F Reserverd</t>
+  </si>
+  <si>
+    <t>Only Use For WPJ , No WBt</t>
   </si>
 </sst>
 </file>
@@ -3473,7 +3488,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="742">
+  <cellXfs count="744">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
@@ -4797,6 +4812,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="53" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -4845,6 +4863,36 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="255" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="39" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="39" fillId="6" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="18" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="18" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="18" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255"/>
+    </xf>
     <xf numFmtId="0" fontId="32" fillId="27" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -4902,34 +4950,139 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="39" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="39" fillId="6" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="18" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="19" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="19" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="3" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="19" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="19" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="38" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="38" fillId="7" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="255"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="18" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="255"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="18" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="33" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="33" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="33" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="52" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="54" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="16" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="16" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="3" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="18" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="18" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="18" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="49" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="49" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="49" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="255"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
@@ -5004,140 +5157,62 @@
     <xf numFmtId="0" fontId="3" fillId="11" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="3" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="18" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="18" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="18" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="49" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="49" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="49" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="52" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="54" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="16" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="16" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="19" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="19" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="3" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="19" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="19" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="38" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="38" fillId="7" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="33" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="33" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="33" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="3" fillId="43" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="43" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="43" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="18" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="18" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="18" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="40" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="40" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="40" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="7" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="32" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="32" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="52" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="52" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="35" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="255" wrapText="1"/>
@@ -5148,63 +5223,6 @@
     <xf numFmtId="0" fontId="3" fillId="35" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="255" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="43" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="43" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="43" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="18" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="18" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="18" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="40" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="40" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="40" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="7" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="32" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="32" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="52" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="52" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -5223,46 +5241,25 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="30" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="30" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="30" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="24" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="24" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="24" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="18" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -5340,28 +5337,52 @@
     <xf numFmtId="0" fontId="3" fillId="21" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="53" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="30" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="30" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="30" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="24" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="24" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="24" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="14" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -5653,10 +5674,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B1:W28"/>
+  <dimension ref="B1:X28"/>
   <sheetViews>
     <sheetView topLeftCell="B9" workbookViewId="0">
-      <selection activeCell="V16" sqref="V16"/>
+      <selection activeCell="X20" sqref="X20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5709,10 +5730,10 @@
       <c r="I2" s="415" t="s">
         <v>6</v>
       </c>
-      <c r="J2" s="561" t="s">
+      <c r="J2" s="562" t="s">
         <v>7</v>
       </c>
-      <c r="K2" s="562"/>
+      <c r="K2" s="563"/>
       <c r="L2" s="1" t="s">
         <v>8</v>
       </c>
@@ -5722,14 +5743,14 @@
       <c r="N2" s="361" t="s">
         <v>10</v>
       </c>
-      <c r="O2" s="563" t="s">
+      <c r="O2" s="564" t="s">
         <v>384</v>
       </c>
-      <c r="P2" s="564"/>
-      <c r="Q2" s="565"/>
-      <c r="R2" s="565"/>
-      <c r="S2" s="565"/>
-      <c r="T2" s="566" t="s">
+      <c r="P2" s="565"/>
+      <c r="Q2" s="566"/>
+      <c r="R2" s="566"/>
+      <c r="S2" s="566"/>
+      <c r="T2" s="567" t="s">
         <v>385</v>
       </c>
       <c r="V2" s="2" t="s">
@@ -5743,7 +5764,7 @@
       <c r="C3" s="168" t="s">
         <v>11</v>
       </c>
-      <c r="D3" s="558"/>
+      <c r="D3" s="559"/>
       <c r="E3" s="349"/>
       <c r="F3" s="271" t="s">
         <v>69</v>
@@ -5779,7 +5800,7 @@
       <c r="S3" s="24">
         <v>0</v>
       </c>
-      <c r="T3" s="567"/>
+      <c r="T3" s="568"/>
       <c r="U3" s="19" t="s">
         <v>589</v>
       </c>
@@ -5795,7 +5816,7 @@
       <c r="C4" s="168" t="s">
         <v>361</v>
       </c>
-      <c r="D4" s="559"/>
+      <c r="D4" s="560"/>
       <c r="E4" s="61"/>
       <c r="F4" s="371" t="s">
         <v>42</v>
@@ -5812,7 +5833,7 @@
       </c>
       <c r="O4" s="6"/>
       <c r="P4" s="321"/>
-      <c r="T4" s="567"/>
+      <c r="T4" s="568"/>
     </row>
     <row r="5" spans="2:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B5" s="2" t="s">
@@ -5821,7 +5842,7 @@
       <c r="C5" s="168" t="s">
         <v>16</v>
       </c>
-      <c r="D5" s="560"/>
+      <c r="D5" s="561"/>
       <c r="F5" s="375" t="s">
         <v>42</v>
       </c>
@@ -5840,7 +5861,7 @@
         <v>521</v>
       </c>
       <c r="P5" s="504"/>
-      <c r="T5" s="567"/>
+      <c r="T5" s="568"/>
       <c r="U5" s="209" t="s">
         <v>228</v>
       </c>
@@ -5879,7 +5900,7 @@
       <c r="P6" s="504"/>
       <c r="Q6" s="16"/>
       <c r="R6" s="6"/>
-      <c r="T6" s="567"/>
+      <c r="T6" s="568"/>
     </row>
     <row r="7" spans="2:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B7" s="214" t="s">
@@ -5917,7 +5938,7 @@
       <c r="S7" s="24">
         <v>1</v>
       </c>
-      <c r="T7" s="567"/>
+      <c r="T7" s="568"/>
     </row>
     <row r="8" spans="2:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B8" s="2" t="s">
@@ -5946,7 +5967,7 @@
       <c r="P8" s="504"/>
       <c r="Q8" s="16"/>
       <c r="R8" s="6"/>
-      <c r="T8" s="567"/>
+      <c r="T8" s="568"/>
     </row>
     <row r="9" spans="2:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B9" s="3" t="s">
@@ -5980,7 +6001,7 @@
         <v>44</v>
       </c>
       <c r="P9" s="504"/>
-      <c r="T9" s="567"/>
+      <c r="T9" s="568"/>
     </row>
     <row r="10" spans="2:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B10" s="2" t="s">
@@ -6010,7 +6031,7 @@
         <v>521</v>
       </c>
       <c r="P10" s="504"/>
-      <c r="T10" s="567"/>
+      <c r="T10" s="568"/>
     </row>
     <row r="11" spans="2:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B11" s="2" t="s">
@@ -6050,7 +6071,7 @@
       <c r="S11" s="24">
         <v>1</v>
       </c>
-      <c r="T11" s="567"/>
+      <c r="T11" s="568"/>
       <c r="U11" s="209" t="s">
         <v>227</v>
       </c>
@@ -6083,7 +6104,7 @@
       <c r="P12" s="504"/>
       <c r="Q12" s="16"/>
       <c r="R12" s="142"/>
-      <c r="T12" s="567"/>
+      <c r="T12" s="568"/>
     </row>
     <row r="13" spans="2:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B13" s="261" t="s">
@@ -6115,7 +6136,7 @@
       </c>
       <c r="P13" s="504"/>
       <c r="R13" s="142"/>
-      <c r="T13" s="567"/>
+      <c r="T13" s="568"/>
       <c r="U13" s="2" t="s">
         <v>610</v>
       </c>
@@ -6125,7 +6146,7 @@
     </row>
     <row r="14" spans="2:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="P14" s="504"/>
-      <c r="T14" s="567"/>
+      <c r="T14" s="568"/>
     </row>
     <row r="15" spans="2:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B15" s="2" t="s">
@@ -6151,10 +6172,10 @@
       <c r="L15" s="137" t="s">
         <v>15</v>
       </c>
-      <c r="M15" s="555">
+      <c r="M15" s="556">
         <v>45275</v>
       </c>
-      <c r="N15" s="558" t="s">
+      <c r="N15" s="559" t="s">
         <v>22</v>
       </c>
       <c r="O15" s="502" t="s">
@@ -6170,7 +6191,7 @@
       <c r="S15" s="24">
         <v>1</v>
       </c>
-      <c r="T15" s="567"/>
+      <c r="T15" s="568"/>
     </row>
     <row r="16" spans="2:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B16" s="486" t="s">
@@ -6196,8 +6217,8 @@
       <c r="L16" s="199" t="s">
         <v>15</v>
       </c>
-      <c r="M16" s="556"/>
-      <c r="N16" s="559"/>
+      <c r="M16" s="557"/>
+      <c r="N16" s="560"/>
       <c r="P16" s="504"/>
       <c r="Q16" s="19" t="s">
         <v>612</v>
@@ -6208,9 +6229,9 @@
       <c r="S16" s="112">
         <v>1</v>
       </c>
-      <c r="T16" s="567"/>
-    </row>
-    <row r="17" spans="2:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="T16" s="568"/>
+    </row>
+    <row r="17" spans="2:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B17" s="2" t="s">
         <v>224</v>
       </c>
@@ -6236,8 +6257,8 @@
       <c r="L17" s="135" t="s">
         <v>15</v>
       </c>
-      <c r="M17" s="557"/>
-      <c r="N17" s="560"/>
+      <c r="M17" s="558"/>
+      <c r="N17" s="561"/>
       <c r="O17" s="502" t="s">
         <v>44</v>
       </c>
@@ -6253,13 +6274,13 @@
       <c r="S17" s="24">
         <v>0</v>
       </c>
-      <c r="T17" s="567"/>
-    </row>
-    <row r="18" spans="2:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="T17" s="568"/>
+    </row>
+    <row r="18" spans="2:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="P18" s="504"/>
-      <c r="T18" s="567"/>
-    </row>
-    <row r="19" spans="2:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="T18" s="568"/>
+    </row>
+    <row r="19" spans="2:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B19" s="2" t="s">
         <v>404</v>
       </c>
@@ -6285,16 +6306,16 @@
       <c r="L19" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="M19" s="555">
+      <c r="M19" s="556">
         <v>45275</v>
       </c>
       <c r="N19" s="414" t="s">
         <v>521</v>
       </c>
       <c r="P19" s="504"/>
-      <c r="T19" s="567"/>
-    </row>
-    <row r="20" spans="2:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="T19" s="568"/>
+    </row>
+    <row r="20" spans="2:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B20" s="246" t="s">
         <v>532</v>
       </c>
@@ -6318,7 +6339,7 @@
       <c r="L20" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="M20" s="556"/>
+      <c r="M20" s="557"/>
       <c r="N20" s="404" t="s">
         <v>26</v>
       </c>
@@ -6332,9 +6353,9 @@
       <c r="S20" s="24">
         <v>1</v>
       </c>
-      <c r="T20" s="567"/>
-    </row>
-    <row r="21" spans="2:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="T20" s="568"/>
+    </row>
+    <row r="21" spans="2:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B21" s="246" t="s">
         <v>27</v>
       </c>
@@ -6358,7 +6379,7 @@
       <c r="L21" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="M21" s="556"/>
+      <c r="M21" s="557"/>
       <c r="N21" s="404" t="s">
         <v>18</v>
       </c>
@@ -6372,13 +6393,13 @@
       <c r="S21" s="24">
         <v>1</v>
       </c>
-      <c r="T21" s="567"/>
-      <c r="U21" s="553" t="s">
+      <c r="T21" s="568"/>
+      <c r="U21" s="554" t="s">
         <v>226</v>
       </c>
-      <c r="V21" s="554"/>
-    </row>
-    <row r="22" spans="2:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="V21" s="555"/>
+    </row>
+    <row r="22" spans="2:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B22" s="276" t="s">
         <v>400</v>
       </c>
@@ -6402,14 +6423,17 @@
       <c r="L22" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="M22" s="556"/>
+      <c r="M22" s="557"/>
       <c r="N22" s="384" t="s">
         <v>26</v>
       </c>
       <c r="P22" s="504"/>
-      <c r="T22" s="567"/>
-    </row>
-    <row r="23" spans="2:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="T22" s="568"/>
+      <c r="X22" s="19" t="s">
+        <v>619</v>
+      </c>
+    </row>
+    <row r="23" spans="2:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B23" s="2" t="s">
         <v>433</v>
       </c>
@@ -6433,12 +6457,12 @@
       <c r="L23" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="M23" s="556"/>
+      <c r="M23" s="557"/>
       <c r="N23" s="61" t="s">
         <v>522</v>
       </c>
       <c r="P23" s="504"/>
-      <c r="T23" s="567"/>
+      <c r="T23" s="568"/>
       <c r="U23" s="2" t="s">
         <v>615</v>
       </c>
@@ -6449,7 +6473,7 @@
         <v>614</v>
       </c>
     </row>
-    <row r="24" spans="2:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="2:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B24" s="3" t="s">
         <v>533</v>
       </c>
@@ -6473,7 +6497,7 @@
       <c r="L24" s="135" t="s">
         <v>32</v>
       </c>
-      <c r="M24" s="556"/>
+      <c r="M24" s="557"/>
       <c r="N24" s="61" t="s">
         <v>26</v>
       </c>
@@ -6482,12 +6506,12 @@
       </c>
       <c r="P24" s="505"/>
       <c r="S24" s="80"/>
-      <c r="T24" s="567"/>
+      <c r="T24" s="568"/>
       <c r="W24" s="23" t="s">
         <v>613</v>
       </c>
     </row>
-    <row r="25" spans="2:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="2:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B25" s="3" t="s">
         <v>34</v>
       </c>
@@ -6513,7 +6537,7 @@
       <c r="L25" s="135" t="s">
         <v>35</v>
       </c>
-      <c r="M25" s="556"/>
+      <c r="M25" s="557"/>
       <c r="N25" s="61" t="s">
         <v>26</v>
       </c>
@@ -6529,12 +6553,12 @@
       <c r="S25" s="21">
         <v>0</v>
       </c>
-      <c r="T25" s="567"/>
+      <c r="T25" s="568"/>
       <c r="V25" s="23" t="s">
         <v>604</v>
       </c>
     </row>
-    <row r="26" spans="2:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="2:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B26" s="2" t="s">
         <v>428</v>
       </c>
@@ -6558,17 +6582,20 @@
       <c r="L26" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="M26" s="556"/>
+      <c r="M26" s="557"/>
       <c r="N26" s="61" t="s">
         <v>523</v>
       </c>
       <c r="P26" s="504"/>
-      <c r="T26" s="567"/>
+      <c r="T26" s="568"/>
+      <c r="V26" s="552" t="s">
+        <v>618</v>
+      </c>
       <c r="W26" s="2" t="s">
         <v>605</v>
       </c>
     </row>
-    <row r="27" spans="2:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="2:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B27" s="261" t="s">
         <v>405</v>
       </c>
@@ -6588,7 +6615,7 @@
       <c r="J27" s="411"/>
       <c r="K27" s="412"/>
       <c r="L27" s="413"/>
-      <c r="M27" s="556"/>
+      <c r="M27" s="557"/>
       <c r="N27" s="61"/>
       <c r="P27" s="321">
         <v>1</v>
@@ -6602,12 +6629,12 @@
       <c r="S27" s="24">
         <v>0</v>
       </c>
-      <c r="T27" s="567"/>
+      <c r="T27" s="568"/>
       <c r="W27" s="2" t="s">
         <v>606</v>
       </c>
     </row>
-    <row r="28" spans="2:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="2:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B28" s="261" t="s">
         <v>405</v>
       </c>
@@ -6633,7 +6660,7 @@
       <c r="L28" s="11" t="s">
         <v>37</v>
       </c>
-      <c r="M28" s="557"/>
+      <c r="M28" s="558"/>
       <c r="N28" s="61" t="s">
         <v>523</v>
       </c>
@@ -6649,7 +6676,7 @@
       <c r="S28" s="21">
         <v>0</v>
       </c>
-      <c r="T28" s="568"/>
+      <c r="T28" s="569"/>
     </row>
   </sheetData>
   <mergeCells count="8">
@@ -6671,8 +6698,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AB54FD83-008D-4F8B-87AC-83E7F70047CB}">
   <dimension ref="A1:AA32"/>
   <sheetViews>
-    <sheetView topLeftCell="H13" workbookViewId="0">
-      <selection activeCell="Z28" sqref="Z28"/>
+    <sheetView topLeftCell="H1" workbookViewId="0">
+      <selection activeCell="W14" sqref="W14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6729,7 +6756,7 @@
       <c r="P1" s="422" t="s">
         <v>407</v>
       </c>
-      <c r="Q1" s="588" t="s">
+      <c r="Q1" s="570" t="s">
         <v>181</v>
       </c>
       <c r="R1" s="100" t="s">
@@ -6749,32 +6776,32 @@
       </c>
     </row>
     <row r="2" spans="1:27" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="572">
+      <c r="A2" s="583">
         <f ca="1">TODAY()</f>
         <v>45279</v>
       </c>
-      <c r="B2" s="574" t="s">
+      <c r="B2" s="585" t="s">
         <v>388</v>
       </c>
-      <c r="C2" s="586" t="s">
+      <c r="C2" s="597" t="s">
         <v>364</v>
       </c>
-      <c r="D2" s="576" t="s">
+      <c r="D2" s="587" t="s">
         <v>103</v>
       </c>
-      <c r="E2" s="578" t="s">
+      <c r="E2" s="589" t="s">
         <v>65</v>
       </c>
       <c r="F2" s="196" t="s">
         <v>220</v>
       </c>
-      <c r="G2" s="584" t="s">
+      <c r="G2" s="595" t="s">
         <v>380</v>
       </c>
       <c r="H2" s="211" t="s">
         <v>220</v>
       </c>
-      <c r="I2" s="595" t="s">
+      <c r="I2" s="577" t="s">
         <v>103</v>
       </c>
       <c r="J2" s="420" t="s">
@@ -6798,14 +6825,14 @@
       <c r="P2" s="423">
         <v>40</v>
       </c>
-      <c r="Q2" s="589"/>
+      <c r="Q2" s="571"/>
       <c r="R2" s="21">
         <f>R7+R18</f>
         <v>5</v>
       </c>
       <c r="S2" s="21">
         <f>S7+S18</f>
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="T2" s="176">
         <f>SUM(T4:T16)</f>
@@ -6813,7 +6840,12 @@
       </c>
       <c r="U2" s="6"/>
       <c r="V2" s="495"/>
-      <c r="X2" s="495"/>
+      <c r="W2" s="6" t="s">
+        <v>469</v>
+      </c>
+      <c r="X2" s="495">
+        <v>1</v>
+      </c>
       <c r="Z2" s="24">
         <f>BoardRW!V3</f>
         <v>5</v>
@@ -6824,14 +6856,14 @@
       </c>
     </row>
     <row r="3" spans="1:27" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="573"/>
-      <c r="B3" s="575"/>
-      <c r="C3" s="587"/>
-      <c r="D3" s="577"/>
-      <c r="E3" s="579"/>
-      <c r="G3" s="585"/>
+      <c r="A3" s="584"/>
+      <c r="B3" s="586"/>
+      <c r="C3" s="598"/>
+      <c r="D3" s="588"/>
+      <c r="E3" s="590"/>
+      <c r="G3" s="596"/>
       <c r="H3" s="6"/>
-      <c r="I3" s="596"/>
+      <c r="I3" s="578"/>
       <c r="K3" s="24">
         <v>2</v>
       </c>
@@ -6856,10 +6888,10 @@
         <v>389</v>
       </c>
       <c r="B4" s="248"/>
-      <c r="C4" s="580" t="s">
+      <c r="C4" s="591" t="s">
         <v>178</v>
       </c>
-      <c r="I4" s="596"/>
+      <c r="I4" s="578"/>
       <c r="R4" s="498" t="s">
         <v>578</v>
       </c>
@@ -6883,7 +6915,7 @@
       <c r="B5" s="100" t="s">
         <v>364</v>
       </c>
-      <c r="C5" s="581"/>
+      <c r="C5" s="592"/>
       <c r="D5" s="227" t="s">
         <v>103</v>
       </c>
@@ -6893,13 +6925,13 @@
       <c r="F5" s="211" t="s">
         <v>220</v>
       </c>
-      <c r="G5" s="558" t="s">
+      <c r="G5" s="559" t="s">
         <v>276</v>
       </c>
       <c r="H5" s="211" t="s">
         <v>220</v>
       </c>
-      <c r="I5" s="596"/>
+      <c r="I5" s="578"/>
       <c r="J5" s="421" t="s">
         <v>273</v>
       </c>
@@ -6930,22 +6962,22 @@
       <c r="X5" s="494"/>
     </row>
     <row r="6" spans="1:27" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="569" t="s">
+      <c r="A6" s="580" t="s">
         <v>290</v>
       </c>
       <c r="B6" s="105" t="s">
         <v>199</v>
       </c>
-      <c r="C6" s="582"/>
-      <c r="D6" s="583"/>
+      <c r="C6" s="593"/>
+      <c r="D6" s="594"/>
       <c r="E6" s="96">
         <v>1</v>
       </c>
-      <c r="G6" s="559"/>
-      <c r="I6" s="596"/>
+      <c r="G6" s="560"/>
+      <c r="I6" s="578"/>
     </row>
     <row r="7" spans="1:27" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="570"/>
+      <c r="A7" s="581"/>
       <c r="B7" s="100" t="s">
         <v>155</v>
       </c>
@@ -6955,8 +6987,8 @@
       <c r="D7" s="30" t="s">
         <v>136</v>
       </c>
-      <c r="G7" s="559"/>
-      <c r="I7" s="596"/>
+      <c r="G7" s="560"/>
+      <c r="I7" s="578"/>
       <c r="M7" s="16" t="s">
         <v>354</v>
       </c>
@@ -6978,7 +7010,7 @@
       </c>
       <c r="S7" s="24">
         <f>3-S11</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="U7" s="6" t="s">
         <v>527</v>
@@ -6994,7 +7026,7 @@
       </c>
     </row>
     <row r="8" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="571"/>
+      <c r="A8" s="582"/>
       <c r="B8" s="217" t="s">
         <v>28</v>
       </c>
@@ -7002,8 +7034,8 @@
       <c r="E8" s="30">
         <v>3</v>
       </c>
-      <c r="G8" s="559"/>
-      <c r="I8" s="596"/>
+      <c r="G8" s="560"/>
+      <c r="I8" s="578"/>
       <c r="N8" s="80"/>
       <c r="U8" s="6" t="s">
         <v>465</v>
@@ -7025,9 +7057,9 @@
       <c r="D9" s="2" t="s">
         <v>142</v>
       </c>
-      <c r="G9" s="559"/>
+      <c r="G9" s="560"/>
       <c r="H9" s="6"/>
-      <c r="I9" s="596"/>
+      <c r="I9" s="578"/>
       <c r="M9" s="19" t="s">
         <v>546</v>
       </c>
@@ -7049,10 +7081,10 @@
       <c r="D10" s="108"/>
       <c r="E10" s="68">
         <f>Boat!U8</f>
-        <v>36</v>
-      </c>
-      <c r="G10" s="559"/>
-      <c r="I10" s="596"/>
+        <v>35</v>
+      </c>
+      <c r="G10" s="560"/>
+      <c r="I10" s="578"/>
       <c r="J10" s="24" t="s">
         <v>380</v>
       </c>
@@ -7074,7 +7106,7 @@
       <c r="A11" s="99" t="s">
         <v>184</v>
       </c>
-      <c r="B11" s="558" t="s">
+      <c r="B11" s="559" t="s">
         <v>391</v>
       </c>
       <c r="C11" s="175" t="s">
@@ -7083,8 +7115,8 @@
       <c r="D11" s="222" t="s">
         <v>270</v>
       </c>
-      <c r="G11" s="559"/>
-      <c r="I11" s="596"/>
+      <c r="G11" s="560"/>
+      <c r="I11" s="578"/>
       <c r="J11" s="24" t="s">
         <v>195</v>
       </c>
@@ -7108,25 +7140,25 @@
         <v>1</v>
       </c>
       <c r="S11" s="24">
-        <v>1</v>
-      </c>
-      <c r="U11" s="590" t="s">
+        <v>0</v>
+      </c>
+      <c r="U11" s="572" t="s">
         <v>581</v>
       </c>
-      <c r="V11" s="591"/>
-      <c r="W11" s="591"/>
-      <c r="X11" s="592"/>
+      <c r="V11" s="573"/>
+      <c r="W11" s="573"/>
+      <c r="X11" s="574"/>
     </row>
     <row r="12" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="232" t="s">
         <v>392</v>
       </c>
-      <c r="B12" s="560"/>
+      <c r="B12" s="561"/>
       <c r="E12" s="234">
         <v>3</v>
       </c>
-      <c r="G12" s="559"/>
-      <c r="I12" s="596"/>
+      <c r="G12" s="560"/>
+      <c r="I12" s="578"/>
       <c r="J12" s="24" t="s">
         <v>537</v>
       </c>
@@ -7154,12 +7186,12 @@
       <c r="B13" s="221" t="s">
         <v>330</v>
       </c>
-      <c r="C13" s="558" t="s">
+      <c r="C13" s="559" t="s">
         <v>195</v>
       </c>
       <c r="D13" s="20"/>
-      <c r="G13" s="559"/>
-      <c r="I13" s="596"/>
+      <c r="G13" s="560"/>
+      <c r="I13" s="578"/>
       <c r="J13" s="108" t="s">
         <v>570</v>
       </c>
@@ -7186,7 +7218,7 @@
       <c r="B14" s="177" t="s">
         <v>150</v>
       </c>
-      <c r="C14" s="560"/>
+      <c r="C14" s="561"/>
       <c r="D14" s="209" t="s">
         <v>154</v>
       </c>
@@ -7196,11 +7228,11 @@
       <c r="F14" s="211" t="s">
         <v>220</v>
       </c>
-      <c r="G14" s="560"/>
+      <c r="G14" s="561"/>
       <c r="H14" s="211" t="s">
         <v>220</v>
       </c>
-      <c r="I14" s="596"/>
+      <c r="I14" s="578"/>
       <c r="U14" s="6"/>
       <c r="V14" s="112"/>
       <c r="W14" s="6"/>
@@ -7218,7 +7250,7 @@
       <c r="H15" s="277">
         <v>0</v>
       </c>
-      <c r="I15" s="596"/>
+      <c r="I15" s="578"/>
       <c r="J15" s="108" t="s">
         <v>154</v>
       </c>
@@ -7249,7 +7281,7 @@
       <c r="D16" s="2" t="s">
         <v>509</v>
       </c>
-      <c r="I16" s="596"/>
+      <c r="I16" s="578"/>
       <c r="K16" s="100" t="s">
         <v>44</v>
       </c>
@@ -7283,7 +7315,7 @@
       <c r="G17" s="2" t="s">
         <v>440</v>
       </c>
-      <c r="I17" s="596"/>
+      <c r="I17" s="578"/>
       <c r="L17" s="2" t="s">
         <v>443</v>
       </c>
@@ -7295,13 +7327,13 @@
     </row>
     <row r="18" spans="1:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="G18" s="16"/>
-      <c r="I18" s="596"/>
+      <c r="I18" s="578"/>
       <c r="L18" s="16"/>
       <c r="M18" s="21"/>
-      <c r="O18" s="593" t="s">
+      <c r="O18" s="575" t="s">
         <v>538</v>
       </c>
-      <c r="P18" s="594"/>
+      <c r="P18" s="576"/>
       <c r="Q18" s="127" t="s">
         <v>44</v>
       </c>
@@ -7327,7 +7359,7 @@
       </c>
     </row>
     <row r="19" spans="1:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="I19" s="596"/>
+      <c r="I19" s="578"/>
       <c r="M19" s="21" t="s">
         <v>442</v>
       </c>
@@ -7359,7 +7391,7 @@
       <c r="G20" s="2" t="s">
         <v>440</v>
       </c>
-      <c r="I20" s="596"/>
+      <c r="I20" s="578"/>
       <c r="K20" s="19" t="s">
         <v>439</v>
       </c>
@@ -7384,7 +7416,7 @@
       <c r="Z20" s="112"/>
     </row>
     <row r="21" spans="1:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="I21" s="596"/>
+      <c r="I21" s="578"/>
       <c r="M21" s="221" t="s">
         <v>421</v>
       </c>
@@ -7420,7 +7452,7 @@
       <c r="G22" s="2" t="s">
         <v>440</v>
       </c>
-      <c r="I22" s="596"/>
+      <c r="I22" s="578"/>
       <c r="U22" s="6"/>
       <c r="V22" s="494"/>
       <c r="W22" s="6" t="s">
@@ -7440,13 +7472,13 @@
       <c r="E23" s="289" t="s">
         <v>44</v>
       </c>
-      <c r="I23" s="596"/>
+      <c r="I23" s="578"/>
       <c r="U23" s="6"/>
       <c r="V23" s="24"/>
       <c r="W23" s="6"/>
     </row>
     <row r="24" spans="1:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="I24" s="596"/>
+      <c r="I24" s="578"/>
       <c r="U24" s="354"/>
       <c r="V24" s="497">
         <v>0</v>
@@ -7474,7 +7506,7 @@
       <c r="H25" s="196" t="s">
         <v>271</v>
       </c>
-      <c r="I25" s="596"/>
+      <c r="I25" s="578"/>
       <c r="J25" s="421" t="s">
         <v>274</v>
       </c>
@@ -7519,7 +7551,7 @@
       <c r="H26" s="19" t="s">
         <v>220</v>
       </c>
-      <c r="I26" s="596"/>
+      <c r="I26" s="578"/>
       <c r="K26" s="24">
         <v>15</v>
       </c>
@@ -7554,7 +7586,7 @@
       </c>
     </row>
     <row r="27" spans="1:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="I27" s="596"/>
+      <c r="I27" s="578"/>
       <c r="O27" s="2" t="s">
         <v>99</v>
       </c>
@@ -7581,7 +7613,7 @@
       <c r="E28" s="220">
         <v>2</v>
       </c>
-      <c r="I28" s="596"/>
+      <c r="I28" s="578"/>
       <c r="Q28" s="6"/>
       <c r="R28" s="112"/>
       <c r="T28" s="142"/>
@@ -7603,7 +7635,7 @@
       <c r="H29" s="196" t="s">
         <v>272</v>
       </c>
-      <c r="I29" s="597"/>
+      <c r="I29" s="579"/>
       <c r="J29" s="333"/>
       <c r="L29" s="96" t="s">
         <v>278</v>
@@ -7673,11 +7705,6 @@
     </row>
   </sheetData>
   <mergeCells count="16">
-    <mergeCell ref="Q1:Q2"/>
-    <mergeCell ref="U11:X11"/>
-    <mergeCell ref="O18:P18"/>
-    <mergeCell ref="I2:I29"/>
-    <mergeCell ref="C13:C14"/>
     <mergeCell ref="A6:A8"/>
     <mergeCell ref="G5:G14"/>
     <mergeCell ref="A2:A3"/>
@@ -7689,6 +7716,11 @@
     <mergeCell ref="B11:B12"/>
     <mergeCell ref="G2:G3"/>
     <mergeCell ref="C2:C3"/>
+    <mergeCell ref="Q1:Q2"/>
+    <mergeCell ref="U11:X11"/>
+    <mergeCell ref="O18:P18"/>
+    <mergeCell ref="I2:I29"/>
+    <mergeCell ref="C13:C14"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -7764,7 +7796,7 @@
       <c r="H1" s="97" t="s">
         <v>350</v>
       </c>
-      <c r="I1" s="584" t="s">
+      <c r="I1" s="595" t="s">
         <v>377</v>
       </c>
       <c r="J1" s="2" t="s">
@@ -7800,7 +7832,7 @@
       <c r="X1" s="454" t="s">
         <v>156</v>
       </c>
-      <c r="Y1" s="640" t="s">
+      <c r="Y1" s="641" t="s">
         <v>550</v>
       </c>
       <c r="Z1" s="430">
@@ -7825,7 +7857,7 @@
         <v>516</v>
       </c>
       <c r="AM1" s="426"/>
-      <c r="AN1" s="622"/>
+      <c r="AN1" s="626"/>
       <c r="AO1" s="350" t="s">
         <v>486</v>
       </c>
@@ -7834,23 +7866,23 @@
       </c>
     </row>
     <row r="2" spans="1:43" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="604">
+      <c r="A2" s="650">
         <f ca="1">TODAY()</f>
         <v>45279</v>
       </c>
-      <c r="B2" s="606" t="s">
+      <c r="B2" s="652" t="s">
         <v>378</v>
       </c>
-      <c r="C2" s="586" t="s">
+      <c r="C2" s="597" t="s">
         <v>364</v>
       </c>
-      <c r="D2" s="608" t="s">
+      <c r="D2" s="654" t="s">
         <v>362</v>
       </c>
-      <c r="E2" s="652" t="s">
+      <c r="E2" s="599" t="s">
         <v>65</v>
       </c>
-      <c r="F2" s="627" t="s">
+      <c r="F2" s="607" t="s">
         <v>103</v>
       </c>
       <c r="G2" s="417" t="s">
@@ -7859,31 +7891,31 @@
       <c r="H2" s="80" t="s">
         <v>33</v>
       </c>
-      <c r="I2" s="585"/>
+      <c r="I2" s="596"/>
       <c r="J2" s="81" t="s">
         <v>77</v>
       </c>
-      <c r="K2" s="654" t="s">
+      <c r="K2" s="601" t="s">
         <v>349</v>
       </c>
-      <c r="L2" s="655"/>
-      <c r="M2" s="627" t="s">
+      <c r="L2" s="602"/>
+      <c r="M2" s="607" t="s">
         <v>103</v>
       </c>
       <c r="N2" s="69" t="s">
         <v>28</v>
       </c>
-      <c r="O2" s="631" t="s">
+      <c r="O2" s="633" t="s">
         <v>103</v>
       </c>
       <c r="P2" s="85" t="s">
         <v>148</v>
       </c>
-      <c r="Q2" s="586" t="s">
+      <c r="Q2" s="597" t="s">
         <v>144</v>
       </c>
-      <c r="R2" s="558"/>
-      <c r="S2" s="644" t="s">
+      <c r="R2" s="559"/>
+      <c r="S2" s="620" t="s">
         <v>149</v>
       </c>
       <c r="T2" s="89"/>
@@ -7893,7 +7925,7 @@
       <c r="X2" s="455" t="s">
         <v>157</v>
       </c>
-      <c r="Y2" s="641"/>
+      <c r="Y2" s="642"/>
       <c r="Z2" s="431">
         <v>1</v>
       </c>
@@ -7916,15 +7948,15 @@
         <v>480</v>
       </c>
       <c r="AM2" s="452"/>
-      <c r="AN2" s="623"/>
+      <c r="AN2" s="627"/>
     </row>
     <row r="3" spans="1:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="605"/>
-      <c r="B3" s="607"/>
-      <c r="C3" s="587"/>
-      <c r="D3" s="609"/>
-      <c r="E3" s="653"/>
-      <c r="F3" s="628"/>
+      <c r="A3" s="651"/>
+      <c r="B3" s="653"/>
+      <c r="C3" s="598"/>
+      <c r="D3" s="655"/>
+      <c r="E3" s="600"/>
+      <c r="F3" s="608"/>
       <c r="G3" s="418" t="s">
         <v>28</v>
       </c>
@@ -7943,17 +7975,17 @@
       <c r="L3" s="206" t="s">
         <v>108</v>
       </c>
-      <c r="M3" s="628"/>
+      <c r="M3" s="608"/>
       <c r="N3" s="69" t="s">
         <v>147</v>
       </c>
-      <c r="O3" s="632"/>
+      <c r="O3" s="634"/>
       <c r="P3" s="2" t="s">
         <v>155</v>
       </c>
-      <c r="Q3" s="587"/>
-      <c r="R3" s="560"/>
-      <c r="S3" s="645"/>
+      <c r="Q3" s="598"/>
+      <c r="R3" s="561"/>
+      <c r="S3" s="622"/>
       <c r="T3" s="89"/>
       <c r="U3" s="124"/>
       <c r="V3" s="120"/>
@@ -7961,7 +7993,7 @@
       <c r="X3" s="455" t="s">
         <v>158</v>
       </c>
-      <c r="Y3" s="641"/>
+      <c r="Y3" s="642"/>
       <c r="Z3" s="432">
         <v>1</v>
       </c>
@@ -7970,7 +8002,7 @@
       <c r="AC3" s="100" t="s">
         <v>497</v>
       </c>
-      <c r="AD3" s="643" t="s">
+      <c r="AD3" s="617" t="s">
         <v>472</v>
       </c>
       <c r="AE3" s="262"/>
@@ -7982,16 +8014,16 @@
       <c r="AK3" s="262"/>
       <c r="AL3" s="16"/>
       <c r="AM3" s="452"/>
-      <c r="AN3" s="623"/>
+      <c r="AN3" s="627"/>
     </row>
     <row r="4" spans="1:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="243" t="s">
         <v>184</v>
       </c>
-      <c r="B4" s="620" t="s">
+      <c r="B4" s="666" t="s">
         <v>381</v>
       </c>
-      <c r="C4" s="586" t="s">
+      <c r="C4" s="597" t="s">
         <v>155</v>
       </c>
       <c r="D4" s="359" t="s">
@@ -8000,7 +8032,7 @@
       <c r="E4" s="396">
         <v>2</v>
       </c>
-      <c r="F4" s="628"/>
+      <c r="F4" s="608"/>
       <c r="G4" s="400" t="s">
         <v>203</v>
       </c>
@@ -8017,11 +8049,11 @@
         <v>151</v>
       </c>
       <c r="L4" s="209"/>
-      <c r="M4" s="628"/>
+      <c r="M4" s="608"/>
       <c r="N4" s="178" t="s">
         <v>70</v>
       </c>
-      <c r="O4" s="632"/>
+      <c r="O4" s="634"/>
       <c r="P4" s="2" t="s">
         <v>192</v>
       </c>
@@ -8043,12 +8075,12 @@
       <c r="X4" s="455" t="s">
         <v>159</v>
       </c>
-      <c r="Y4" s="641"/>
+      <c r="Y4" s="642"/>
       <c r="Z4" s="433"/>
       <c r="AA4" s="313"/>
       <c r="AB4" s="214"/>
       <c r="AC4" s="16"/>
-      <c r="AD4" s="643"/>
+      <c r="AD4" s="617"/>
       <c r="AE4" s="262"/>
       <c r="AF4" s="262"/>
       <c r="AG4" s="16"/>
@@ -8058,37 +8090,37 @@
       <c r="AK4" s="262"/>
       <c r="AL4" s="16"/>
       <c r="AM4" s="452"/>
-      <c r="AN4" s="623"/>
+      <c r="AN4" s="627"/>
       <c r="AO4" s="350" t="s">
         <v>91</v>
       </c>
     </row>
     <row r="5" spans="1:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="584" t="s">
+      <c r="A5" s="595" t="s">
         <v>434</v>
       </c>
-      <c r="B5" s="621"/>
-      <c r="C5" s="587"/>
+      <c r="B5" s="667"/>
+      <c r="C5" s="598"/>
       <c r="D5" s="61" t="s">
         <v>154</v>
       </c>
       <c r="E5" s="397">
         <v>1</v>
       </c>
-      <c r="F5" s="628"/>
-      <c r="G5" s="612" t="s">
+      <c r="F5" s="608"/>
+      <c r="G5" s="658" t="s">
         <v>193</v>
       </c>
-      <c r="H5" s="612"/>
-      <c r="I5" s="612"/>
-      <c r="J5" s="612"/>
-      <c r="K5" s="612"/>
-      <c r="L5" s="613"/>
-      <c r="M5" s="628"/>
+      <c r="H5" s="658"/>
+      <c r="I5" s="658"/>
+      <c r="J5" s="658"/>
+      <c r="K5" s="658"/>
+      <c r="L5" s="659"/>
+      <c r="M5" s="608"/>
       <c r="N5" s="21">
         <v>8</v>
       </c>
-      <c r="O5" s="632"/>
+      <c r="O5" s="634"/>
       <c r="T5" s="89"/>
       <c r="U5" s="124"/>
       <c r="V5" s="120"/>
@@ -8096,7 +8128,7 @@
       <c r="X5" s="455" t="s">
         <v>160</v>
       </c>
-      <c r="Y5" s="641"/>
+      <c r="Y5" s="642"/>
       <c r="Z5" s="433">
         <v>1</v>
       </c>
@@ -8119,24 +8151,24 @@
       <c r="AK5" s="262"/>
       <c r="AL5" s="80"/>
       <c r="AM5" s="452"/>
-      <c r="AN5" s="623"/>
+      <c r="AN5" s="627"/>
     </row>
     <row r="6" spans="1:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="585"/>
-      <c r="B6" s="618" t="s">
+      <c r="A6" s="596"/>
+      <c r="B6" s="664" t="s">
         <v>178</v>
       </c>
-      <c r="C6" s="582"/>
-      <c r="D6" s="583"/>
-      <c r="F6" s="628"/>
-      <c r="G6" s="614"/>
-      <c r="H6" s="614"/>
-      <c r="I6" s="614"/>
-      <c r="J6" s="614"/>
-      <c r="K6" s="614"/>
-      <c r="L6" s="615"/>
-      <c r="M6" s="628"/>
-      <c r="O6" s="632"/>
+      <c r="C6" s="593"/>
+      <c r="D6" s="594"/>
+      <c r="F6" s="608"/>
+      <c r="G6" s="660"/>
+      <c r="H6" s="660"/>
+      <c r="I6" s="660"/>
+      <c r="J6" s="660"/>
+      <c r="K6" s="660"/>
+      <c r="L6" s="661"/>
+      <c r="M6" s="608"/>
+      <c r="O6" s="634"/>
       <c r="T6" s="89"/>
       <c r="U6" s="124"/>
       <c r="V6" s="98" t="s">
@@ -8146,7 +8178,7 @@
       <c r="X6" s="455" t="s">
         <v>161</v>
       </c>
-      <c r="Y6" s="641"/>
+      <c r="Y6" s="642"/>
       <c r="Z6" s="431">
         <v>1</v>
       </c>
@@ -8160,16 +8192,16 @@
       <c r="AF6" s="262"/>
       <c r="AG6" s="262"/>
       <c r="AH6" s="262"/>
-      <c r="AI6" s="637"/>
+      <c r="AI6" s="616"/>
       <c r="AJ6" s="465" t="s">
         <v>475</v>
       </c>
-      <c r="AK6" s="637" t="s">
+      <c r="AK6" s="616" t="s">
         <v>256</v>
       </c>
       <c r="AL6" s="262"/>
       <c r="AM6" s="452"/>
-      <c r="AN6" s="623"/>
+      <c r="AN6" s="627"/>
       <c r="AO6" s="350" t="s">
         <v>487</v>
       </c>
@@ -8178,7 +8210,7 @@
       <c r="A7" s="237" t="s">
         <v>596</v>
       </c>
-      <c r="B7" s="619"/>
+      <c r="B7" s="665"/>
       <c r="C7" s="207" t="s">
         <v>382</v>
       </c>
@@ -8188,7 +8220,7 @@
       <c r="E7" s="271">
         <v>3</v>
       </c>
-      <c r="F7" s="628"/>
+      <c r="F7" s="608"/>
       <c r="G7" s="419">
         <v>0</v>
       </c>
@@ -8201,14 +8233,14 @@
       <c r="J7" s="30">
         <v>0</v>
       </c>
-      <c r="K7" s="558">
+      <c r="K7" s="559">
         <v>0</v>
       </c>
       <c r="L7" s="217">
         <v>0</v>
       </c>
-      <c r="M7" s="628"/>
-      <c r="O7" s="632"/>
+      <c r="M7" s="608"/>
+      <c r="O7" s="634"/>
       <c r="R7" s="99" t="s">
         <v>44</v>
       </c>
@@ -8222,7 +8254,7 @@
       <c r="X7" s="455" t="s">
         <v>162</v>
       </c>
-      <c r="Y7" s="641"/>
+      <c r="Y7" s="642"/>
       <c r="Z7" s="431">
         <v>1</v>
       </c>
@@ -8232,18 +8264,18 @@
       <c r="AD7" s="16"/>
       <c r="AE7" s="262"/>
       <c r="AF7" s="262"/>
-      <c r="AG7" s="643" t="s">
+      <c r="AG7" s="617" t="s">
         <v>471</v>
       </c>
       <c r="AH7" s="262"/>
-      <c r="AI7" s="637"/>
+      <c r="AI7" s="616"/>
       <c r="AJ7" s="262"/>
-      <c r="AK7" s="637"/>
+      <c r="AK7" s="616"/>
       <c r="AL7" s="80" t="s">
         <v>514</v>
       </c>
       <c r="AM7" s="452"/>
-      <c r="AN7" s="623"/>
+      <c r="AN7" s="627"/>
       <c r="AP7" s="76" t="s">
         <v>488</v>
       </c>
@@ -8260,27 +8292,27 @@
         <f>SUM(G7:N9)</f>
         <v>15</v>
       </c>
-      <c r="F8" s="628"/>
-      <c r="G8" s="613">
-        <v>0</v>
-      </c>
-      <c r="H8" s="610" t="s">
+      <c r="F8" s="608"/>
+      <c r="G8" s="659">
+        <v>0</v>
+      </c>
+      <c r="H8" s="656" t="s">
         <v>105</v>
       </c>
-      <c r="I8" s="558">
-        <v>0</v>
-      </c>
-      <c r="J8" s="610" t="s">
+      <c r="I8" s="559">
+        <v>0</v>
+      </c>
+      <c r="J8" s="656" t="s">
         <v>105</v>
       </c>
-      <c r="K8" s="616"/>
-      <c r="L8" s="646"/>
-      <c r="M8" s="629"/>
-      <c r="N8" s="649">
+      <c r="K8" s="662"/>
+      <c r="L8" s="618"/>
+      <c r="M8" s="631"/>
+      <c r="N8" s="623">
         <f>N5+N11</f>
         <v>15</v>
       </c>
-      <c r="O8" s="632"/>
+      <c r="O8" s="634"/>
       <c r="T8" s="103" t="s">
         <v>44</v>
       </c>
@@ -8290,7 +8322,7 @@
       <c r="X8" s="455" t="s">
         <v>163</v>
       </c>
-      <c r="Y8" s="641"/>
+      <c r="Y8" s="642"/>
       <c r="Z8" s="433"/>
       <c r="AA8" s="313"/>
       <c r="AB8" s="214"/>
@@ -8298,14 +8330,14 @@
       <c r="AD8" s="16"/>
       <c r="AE8" s="262"/>
       <c r="AF8" s="262"/>
-      <c r="AG8" s="643"/>
+      <c r="AG8" s="617"/>
       <c r="AH8" s="262"/>
-      <c r="AI8" s="637"/>
+      <c r="AI8" s="616"/>
       <c r="AJ8" s="262"/>
       <c r="AK8" s="262"/>
       <c r="AL8" s="262"/>
       <c r="AM8" s="452"/>
-      <c r="AN8" s="623"/>
+      <c r="AN8" s="627"/>
     </row>
     <row r="9" spans="1:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="237" t="s">
@@ -8320,17 +8352,17 @@
       <c r="D9" s="360" t="s">
         <v>286</v>
       </c>
-      <c r="F9" s="628"/>
-      <c r="G9" s="615"/>
-      <c r="H9" s="611"/>
-      <c r="I9" s="560"/>
-      <c r="J9" s="611"/>
-      <c r="K9" s="617"/>
-      <c r="L9" s="647"/>
-      <c r="M9" s="630"/>
-      <c r="N9" s="650"/>
-      <c r="O9" s="633"/>
-      <c r="S9" s="644" t="s">
+      <c r="F9" s="608"/>
+      <c r="G9" s="661"/>
+      <c r="H9" s="657"/>
+      <c r="I9" s="561"/>
+      <c r="J9" s="657"/>
+      <c r="K9" s="663"/>
+      <c r="L9" s="619"/>
+      <c r="M9" s="632"/>
+      <c r="N9" s="624"/>
+      <c r="O9" s="635"/>
+      <c r="S9" s="620" t="s">
         <v>62</v>
       </c>
       <c r="T9" s="89"/>
@@ -8342,7 +8374,7 @@
       <c r="X9" s="455" t="s">
         <v>164</v>
       </c>
-      <c r="Y9" s="641"/>
+      <c r="Y9" s="642"/>
       <c r="Z9" s="434"/>
       <c r="AA9" s="313"/>
       <c r="AB9" s="214"/>
@@ -8352,16 +8384,16 @@
       </c>
       <c r="AE9" s="262"/>
       <c r="AF9" s="262"/>
-      <c r="AG9" s="643"/>
+      <c r="AG9" s="617"/>
       <c r="AH9" s="262"/>
-      <c r="AI9" s="637"/>
+      <c r="AI9" s="616"/>
       <c r="AJ9" s="80"/>
-      <c r="AK9" s="637" t="s">
+      <c r="AK9" s="616" t="s">
         <v>256</v>
       </c>
       <c r="AL9" s="262"/>
       <c r="AM9" s="452"/>
-      <c r="AN9" s="623"/>
+      <c r="AN9" s="627"/>
       <c r="AP9" s="2" t="s">
         <v>526</v>
       </c>
@@ -8376,22 +8408,22 @@
       <c r="D10" s="142"/>
       <c r="E10" s="242">
         <f>Boat!U8</f>
-        <v>36</v>
-      </c>
-      <c r="F10" s="628"/>
+        <v>35</v>
+      </c>
+      <c r="F10" s="608"/>
       <c r="N10" s="442" t="s">
         <v>406</v>
       </c>
-      <c r="O10" s="661" t="s">
+      <c r="O10" s="610" t="s">
         <v>103</v>
       </c>
-      <c r="P10" s="634" t="s">
+      <c r="P10" s="636" t="s">
         <v>410</v>
       </c>
       <c r="R10" s="74" t="s">
         <v>44</v>
       </c>
-      <c r="S10" s="648"/>
+      <c r="S10" s="621"/>
       <c r="T10" s="89"/>
       <c r="U10" s="123" t="s">
         <v>177</v>
@@ -8403,7 +8435,7 @@
       <c r="X10" s="455" t="s">
         <v>165</v>
       </c>
-      <c r="Y10" s="641"/>
+      <c r="Y10" s="642"/>
       <c r="Z10" s="433">
         <v>0</v>
       </c>
@@ -8421,16 +8453,16 @@
       <c r="AF10" s="243" t="s">
         <v>318</v>
       </c>
-      <c r="AG10" s="643"/>
+      <c r="AG10" s="617"/>
       <c r="AH10" s="80"/>
-      <c r="AI10" s="637"/>
+      <c r="AI10" s="616"/>
       <c r="AJ10" s="262"/>
-      <c r="AK10" s="637"/>
+      <c r="AK10" s="616"/>
       <c r="AL10" s="262"/>
       <c r="AM10" s="466" t="s">
         <v>325</v>
       </c>
-      <c r="AN10" s="623"/>
+      <c r="AN10" s="627"/>
       <c r="AO10" s="209" t="s">
         <v>95</v>
       </c>
@@ -8439,7 +8471,7 @@
       <c r="A11" s="228" t="s">
         <v>290</v>
       </c>
-      <c r="B11" s="558" t="s">
+      <c r="B11" s="559" t="s">
         <v>288</v>
       </c>
       <c r="C11" s="481" t="s">
@@ -8448,18 +8480,18 @@
       <c r="D11" s="174" t="s">
         <v>362</v>
       </c>
-      <c r="F11" s="628"/>
+      <c r="F11" s="608"/>
       <c r="M11" s="6"/>
       <c r="N11" s="117">
         <v>7</v>
       </c>
-      <c r="O11" s="662"/>
-      <c r="P11" s="635"/>
+      <c r="O11" s="611"/>
+      <c r="P11" s="637"/>
       <c r="Q11" s="65"/>
       <c r="R11" s="120" t="s">
         <v>222</v>
       </c>
-      <c r="S11" s="648"/>
+      <c r="S11" s="621"/>
       <c r="T11" s="102" t="s">
         <v>44</v>
       </c>
@@ -8469,7 +8501,7 @@
       <c r="X11" s="455" t="s">
         <v>166</v>
       </c>
-      <c r="Y11" s="641"/>
+      <c r="Y11" s="642"/>
       <c r="Z11" s="433"/>
       <c r="AA11" s="313">
         <v>1</v>
@@ -8483,14 +8515,14 @@
       <c r="AF11" s="262" t="s">
         <v>493</v>
       </c>
-      <c r="AG11" s="643"/>
+      <c r="AG11" s="617"/>
       <c r="AH11" s="262"/>
       <c r="AI11" s="70"/>
       <c r="AJ11" s="262"/>
       <c r="AK11" s="262"/>
       <c r="AL11" s="262"/>
       <c r="AM11" s="452"/>
-      <c r="AN11" s="623"/>
+      <c r="AN11" s="627"/>
       <c r="AP11" s="76" t="s">
         <v>501</v>
       </c>
@@ -8499,7 +8531,7 @@
       <c r="A12" s="232" t="s">
         <v>392</v>
       </c>
-      <c r="B12" s="560"/>
+      <c r="B12" s="561"/>
       <c r="C12" s="482" t="s">
         <v>393</v>
       </c>
@@ -8509,25 +8541,25 @@
       <c r="E12" s="229">
         <v>3</v>
       </c>
-      <c r="F12" s="628"/>
+      <c r="F12" s="608"/>
       <c r="G12" s="349" t="s">
         <v>410</v>
       </c>
-      <c r="H12" s="563" t="s">
+      <c r="H12" s="564" t="s">
         <v>446</v>
       </c>
-      <c r="I12" s="565"/>
-      <c r="J12" s="565"/>
-      <c r="K12" s="666"/>
+      <c r="I12" s="566"/>
+      <c r="J12" s="566"/>
+      <c r="K12" s="615"/>
       <c r="L12" s="208"/>
       <c r="M12" s="208"/>
       <c r="N12" s="208"/>
-      <c r="O12" s="662"/>
-      <c r="P12" s="635"/>
+      <c r="O12" s="611"/>
+      <c r="P12" s="637"/>
       <c r="R12" s="122" t="s">
         <v>181</v>
       </c>
-      <c r="S12" s="645"/>
+      <c r="S12" s="622"/>
       <c r="T12" s="101" t="s">
         <v>44</v>
       </c>
@@ -8537,7 +8569,7 @@
       <c r="X12" s="455" t="s">
         <v>167</v>
       </c>
-      <c r="Y12" s="641"/>
+      <c r="Y12" s="642"/>
       <c r="Z12" s="431">
         <v>1</v>
       </c>
@@ -8548,16 +8580,16 @@
       <c r="AC12" s="100" t="s">
         <v>498</v>
       </c>
-      <c r="AD12" s="651" t="s">
+      <c r="AD12" s="625" t="s">
         <v>245</v>
       </c>
       <c r="AE12" s="465" t="s">
         <v>244</v>
       </c>
-      <c r="AF12" s="643" t="s">
+      <c r="AF12" s="617" t="s">
         <v>231</v>
       </c>
-      <c r="AG12" s="643"/>
+      <c r="AG12" s="617"/>
       <c r="AH12" s="243" t="s">
         <v>264</v>
       </c>
@@ -8567,10 +8599,10 @@
       <c r="AJ12" s="262"/>
       <c r="AK12" s="262"/>
       <c r="AL12" s="262"/>
-      <c r="AM12" s="638" t="s">
+      <c r="AM12" s="639" t="s">
         <v>254</v>
       </c>
-      <c r="AN12" s="623"/>
+      <c r="AN12" s="627"/>
       <c r="AO12" s="350" t="s">
         <v>97</v>
       </c>
@@ -8582,17 +8614,17 @@
       <c r="E13" s="472">
         <v>-3</v>
       </c>
-      <c r="F13" s="628"/>
-      <c r="G13" s="565" t="s">
+      <c r="F13" s="608"/>
+      <c r="G13" s="566" t="s">
         <v>447</v>
       </c>
-      <c r="H13" s="565"/>
-      <c r="I13" s="565"/>
-      <c r="J13" s="666"/>
+      <c r="H13" s="566"/>
+      <c r="I13" s="566"/>
+      <c r="J13" s="615"/>
       <c r="M13" s="6"/>
       <c r="N13" s="6"/>
-      <c r="O13" s="662"/>
-      <c r="P13" s="636"/>
+      <c r="O13" s="611"/>
+      <c r="P13" s="638"/>
       <c r="T13" s="105" t="s">
         <v>44</v>
       </c>
@@ -8602,7 +8634,7 @@
       <c r="X13" s="455" t="s">
         <v>168</v>
       </c>
-      <c r="Y13" s="641"/>
+      <c r="Y13" s="642"/>
       <c r="Z13" s="431">
         <v>1</v>
       </c>
@@ -8613,8 +8645,8 @@
         <v>518</v>
       </c>
       <c r="AC13" s="16"/>
-      <c r="AD13" s="651"/>
-      <c r="AF13" s="643"/>
+      <c r="AD13" s="625"/>
+      <c r="AF13" s="617"/>
       <c r="AG13" s="80"/>
       <c r="AH13" s="243" t="s">
         <v>314</v>
@@ -8625,8 +8657,8 @@
       <c r="AJ13" s="80"/>
       <c r="AK13" s="262"/>
       <c r="AL13" s="262"/>
-      <c r="AM13" s="638"/>
-      <c r="AN13" s="623"/>
+      <c r="AM13" s="639"/>
+      <c r="AN13" s="627"/>
     </row>
     <row r="14" spans="1:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="474"/>
@@ -8634,18 +8666,18 @@
       <c r="C14" s="483"/>
       <c r="D14" s="476"/>
       <c r="E14" s="477"/>
-      <c r="F14" s="628"/>
-      <c r="G14" s="565" t="s">
+      <c r="F14" s="608"/>
+      <c r="G14" s="566" t="s">
         <v>446</v>
       </c>
-      <c r="H14" s="565"/>
-      <c r="I14" s="565"/>
-      <c r="J14" s="666"/>
+      <c r="H14" s="566"/>
+      <c r="I14" s="566"/>
+      <c r="J14" s="615"/>
       <c r="K14" s="2">
         <v>12</v>
       </c>
       <c r="N14" s="6"/>
-      <c r="O14" s="662"/>
+      <c r="O14" s="611"/>
       <c r="Q14" s="61" t="s">
         <v>554</v>
       </c>
@@ -8659,34 +8691,34 @@
       <c r="X14" s="455" t="s">
         <v>169</v>
       </c>
-      <c r="Y14" s="641"/>
+      <c r="Y14" s="642"/>
       <c r="Z14" s="431">
         <v>1</v>
       </c>
       <c r="AA14" s="313"/>
       <c r="AB14" s="214"/>
       <c r="AC14" s="16"/>
-      <c r="AD14" s="651"/>
+      <c r="AD14" s="625"/>
       <c r="AE14" s="262"/>
-      <c r="AF14" s="643"/>
+      <c r="AF14" s="617"/>
       <c r="AG14" s="262"/>
       <c r="AH14" s="262"/>
       <c r="AI14" s="70"/>
       <c r="AJ14" s="262"/>
       <c r="AK14" s="262"/>
       <c r="AL14" s="262"/>
-      <c r="AM14" s="638"/>
-      <c r="AN14" s="623"/>
+      <c r="AM14" s="639"/>
+      <c r="AN14" s="627"/>
     </row>
     <row r="15" spans="1:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="473" t="s">
         <v>524</v>
       </c>
-      <c r="C15" s="558" t="s">
+      <c r="C15" s="559" t="s">
         <v>381</v>
       </c>
-      <c r="F15" s="628"/>
-      <c r="O15" s="662"/>
+      <c r="F15" s="608"/>
+      <c r="O15" s="611"/>
       <c r="R15" s="99" t="s">
         <v>44</v>
       </c>
@@ -8699,7 +8731,7 @@
       <c r="X15" s="455" t="s">
         <v>170</v>
       </c>
-      <c r="Y15" s="641"/>
+      <c r="Y15" s="642"/>
       <c r="Z15" s="433">
         <v>1</v>
       </c>
@@ -8708,8 +8740,8 @@
       <c r="AC15" s="76" t="s">
         <v>496</v>
       </c>
-      <c r="AD15" s="651"/>
-      <c r="AF15" s="643"/>
+      <c r="AD15" s="625"/>
+      <c r="AF15" s="617"/>
       <c r="AG15" s="80"/>
       <c r="AH15" s="243" t="s">
         <v>465</v>
@@ -8722,8 +8754,8 @@
       </c>
       <c r="AK15" s="262"/>
       <c r="AL15" s="262"/>
-      <c r="AM15" s="638"/>
-      <c r="AN15" s="623"/>
+      <c r="AM15" s="639"/>
+      <c r="AN15" s="627"/>
       <c r="AP15" s="76" t="s">
         <v>74</v>
       </c>
@@ -8738,20 +8770,20 @@
       <c r="B16" s="21" t="s">
         <v>416</v>
       </c>
-      <c r="C16" s="560"/>
+      <c r="C16" s="561"/>
       <c r="D16" s="61" t="s">
         <v>510</v>
       </c>
       <c r="E16" s="229">
         <v>1</v>
       </c>
-      <c r="F16" s="628"/>
+      <c r="F16" s="608"/>
       <c r="G16" s="349" t="s">
         <v>505</v>
       </c>
       <c r="I16" s="495"/>
       <c r="J16" s="20"/>
-      <c r="O16" s="662"/>
+      <c r="O16" s="611"/>
       <c r="R16" s="459" t="s">
         <v>185</v>
       </c>
@@ -8762,7 +8794,7 @@
       <c r="X16" s="455" t="s">
         <v>171</v>
       </c>
-      <c r="Y16" s="641"/>
+      <c r="Y16" s="642"/>
       <c r="Z16" s="431">
         <v>1</v>
       </c>
@@ -8783,18 +8815,18 @@
       <c r="AM16" s="452" t="s">
         <v>324</v>
       </c>
-      <c r="AN16" s="623"/>
+      <c r="AN16" s="627"/>
       <c r="AP16" s="76" t="s">
         <v>235</v>
       </c>
     </row>
     <row r="17" spans="1:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B17" s="80"/>
-      <c r="F17" s="628"/>
+      <c r="F17" s="608"/>
       <c r="I17" s="496"/>
       <c r="J17" s="20"/>
       <c r="N17" s="6"/>
-      <c r="O17" s="662"/>
+      <c r="O17" s="611"/>
       <c r="Q17" s="21" t="s">
         <v>552</v>
       </c>
@@ -8814,7 +8846,7 @@
       <c r="X17" s="455" t="s">
         <v>172</v>
       </c>
-      <c r="Y17" s="641"/>
+      <c r="Y17" s="642"/>
       <c r="Z17" s="433"/>
       <c r="AA17" s="313"/>
       <c r="AB17" s="214"/>
@@ -8839,7 +8871,7 @@
       <c r="AK17" s="262"/>
       <c r="AL17" s="80"/>
       <c r="AM17" s="452"/>
-      <c r="AN17" s="623"/>
+      <c r="AN17" s="627"/>
       <c r="AO17" s="209" t="s">
         <v>515</v>
       </c>
@@ -8863,21 +8895,21 @@
       <c r="E18" s="99" t="s">
         <v>44</v>
       </c>
-      <c r="F18" s="628"/>
+      <c r="F18" s="608"/>
       <c r="G18" s="349" t="s">
         <v>549</v>
       </c>
       <c r="I18" s="24"/>
       <c r="J18" s="20"/>
-      <c r="O18" s="662"/>
+      <c r="O18" s="611"/>
       <c r="Q18" s="112"/>
-      <c r="R18" s="656" t="s">
+      <c r="R18" s="603" t="s">
         <v>557</v>
       </c>
       <c r="T18" s="100" t="s">
         <v>44</v>
       </c>
-      <c r="U18" s="601" t="s">
+      <c r="U18" s="647" t="s">
         <v>44</v>
       </c>
       <c r="V18" s="120"/>
@@ -8887,7 +8919,7 @@
       <c r="X18" s="455" t="s">
         <v>173</v>
       </c>
-      <c r="Y18" s="641"/>
+      <c r="Y18" s="642"/>
       <c r="Z18" s="433">
         <v>1</v>
       </c>
@@ -8898,38 +8930,38 @@
       <c r="AC18" s="16"/>
       <c r="AD18" s="16"/>
       <c r="AE18" s="262"/>
-      <c r="AF18" s="637" t="s">
+      <c r="AF18" s="616" t="s">
         <v>492</v>
       </c>
       <c r="AG18" s="262"/>
       <c r="AH18" s="70"/>
       <c r="AI18" s="70"/>
-      <c r="AJ18" s="639" t="s">
+      <c r="AJ18" s="640" t="s">
         <v>322</v>
       </c>
       <c r="AK18" s="262"/>
       <c r="AL18" s="80"/>
       <c r="AM18" s="452"/>
-      <c r="AN18" s="623"/>
+      <c r="AN18" s="627"/>
       <c r="AP18" s="76" t="s">
         <v>88</v>
       </c>
     </row>
     <row r="19" spans="1:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="F19" s="628"/>
+      <c r="F19" s="608"/>
       <c r="I19" s="224"/>
-      <c r="O19" s="662"/>
-      <c r="R19" s="657"/>
+      <c r="O19" s="611"/>
+      <c r="R19" s="604"/>
       <c r="S19" s="30" t="s">
         <v>555</v>
       </c>
-      <c r="U19" s="602"/>
+      <c r="U19" s="648"/>
       <c r="V19" s="146"/>
       <c r="W19" s="146"/>
       <c r="X19" s="455" t="s">
         <v>174</v>
       </c>
-      <c r="Y19" s="641"/>
+      <c r="Y19" s="642"/>
       <c r="Z19" s="431">
         <v>1</v>
       </c>
@@ -8938,17 +8970,17 @@
       <c r="AC19" s="16"/>
       <c r="AD19" s="16"/>
       <c r="AE19" s="262"/>
-      <c r="AF19" s="637"/>
+      <c r="AF19" s="616"/>
       <c r="AG19" s="262"/>
       <c r="AH19" s="262"/>
       <c r="AI19" s="70"/>
-      <c r="AJ19" s="639"/>
+      <c r="AJ19" s="640"/>
       <c r="AK19" s="484" t="s">
         <v>256</v>
       </c>
       <c r="AL19" s="80"/>
       <c r="AM19" s="452"/>
-      <c r="AN19" s="623"/>
+      <c r="AN19" s="627"/>
       <c r="AP19" s="76" t="s">
         <v>485</v>
       </c>
@@ -8969,24 +9001,24 @@
       <c r="E20" s="461">
         <v>-1</v>
       </c>
-      <c r="F20" s="628"/>
+      <c r="F20" s="608"/>
       <c r="G20" s="349" t="s">
         <v>508</v>
       </c>
       <c r="I20" s="224"/>
-      <c r="O20" s="662"/>
-      <c r="Q20" s="664" t="s">
+      <c r="O20" s="611"/>
+      <c r="Q20" s="613" t="s">
         <v>48</v>
       </c>
       <c r="T20" s="428" t="s">
         <v>44</v>
       </c>
-      <c r="U20" s="603"/>
+      <c r="U20" s="649"/>
       <c r="W20" s="429"/>
       <c r="X20" s="456" t="s">
         <v>175</v>
       </c>
-      <c r="Y20" s="641"/>
+      <c r="Y20" s="642"/>
       <c r="Z20" s="435">
         <v>1</v>
       </c>
@@ -9011,7 +9043,7 @@
       <c r="AM20" s="400" t="s">
         <v>254</v>
       </c>
-      <c r="AN20" s="623"/>
+      <c r="AN20" s="627"/>
       <c r="AO20" s="350" t="s">
         <v>477</v>
       </c>
@@ -9032,20 +9064,20 @@
       <c r="E21" s="271">
         <v>0</v>
       </c>
-      <c r="F21" s="628"/>
+      <c r="F21" s="608"/>
       <c r="I21" s="224"/>
-      <c r="O21" s="662"/>
-      <c r="Q21" s="665"/>
+      <c r="O21" s="611"/>
+      <c r="Q21" s="614"/>
       <c r="T21" s="446"/>
       <c r="U21" s="14"/>
-      <c r="V21" s="598"/>
+      <c r="V21" s="644"/>
       <c r="W21" s="450" t="s">
         <v>176</v>
       </c>
       <c r="X21" s="453" t="s">
         <v>187</v>
       </c>
-      <c r="Y21" s="641"/>
+      <c r="Y21" s="642"/>
       <c r="Z21" s="469">
         <v>3</v>
       </c>
@@ -9076,15 +9108,15 @@
       <c r="AM21" s="452" t="s">
         <v>566</v>
       </c>
-      <c r="AN21" s="623"/>
+      <c r="AN21" s="627"/>
     </row>
     <row r="22" spans="1:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="F22" s="628"/>
+      <c r="F22" s="608"/>
       <c r="G22" s="349" t="s">
         <v>506</v>
       </c>
       <c r="I22" s="224"/>
-      <c r="O22" s="662"/>
+      <c r="O22" s="611"/>
       <c r="R22" s="458" t="s">
         <v>44</v>
       </c>
@@ -9092,14 +9124,14 @@
         <v>44</v>
       </c>
       <c r="U22" s="15"/>
-      <c r="V22" s="599"/>
+      <c r="V22" s="645"/>
       <c r="W22" s="450" t="s">
         <v>176</v>
       </c>
       <c r="X22" s="453" t="s">
         <v>188</v>
       </c>
-      <c r="Y22" s="641"/>
+      <c r="Y22" s="642"/>
       <c r="Z22" s="439"/>
       <c r="AA22" s="10"/>
       <c r="AB22" s="439"/>
@@ -9110,7 +9142,7 @@
       <c r="AG22" s="6"/>
       <c r="AH22" s="6"/>
       <c r="AI22" s="6"/>
-      <c r="AJ22" s="637" t="s">
+      <c r="AJ22" s="616" t="s">
         <v>489</v>
       </c>
       <c r="AK22" s="262"/>
@@ -9118,7 +9150,7 @@
         <v>495</v>
       </c>
       <c r="AM22" s="306"/>
-      <c r="AN22" s="623"/>
+      <c r="AN22" s="627"/>
     </row>
     <row r="23" spans="1:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="236" t="s">
@@ -9136,22 +9168,22 @@
       <c r="E23" s="230">
         <v>1</v>
       </c>
-      <c r="F23" s="628"/>
+      <c r="F23" s="608"/>
       <c r="I23" s="224"/>
-      <c r="O23" s="662"/>
-      <c r="Q23" s="664" t="s">
+      <c r="O23" s="611"/>
+      <c r="Q23" s="613" t="s">
         <v>145</v>
       </c>
       <c r="T23" s="17"/>
       <c r="U23" s="444" t="s">
         <v>44</v>
       </c>
-      <c r="V23" s="599"/>
+      <c r="V23" s="645"/>
       <c r="W23" s="148"/>
       <c r="X23" s="453" t="s">
         <v>189</v>
       </c>
-      <c r="Y23" s="641"/>
+      <c r="Y23" s="642"/>
       <c r="Z23" s="17"/>
       <c r="AA23" s="10"/>
       <c r="AB23" s="439"/>
@@ -9162,13 +9194,13 @@
       <c r="AG23" s="6"/>
       <c r="AH23" s="6"/>
       <c r="AI23" s="6"/>
-      <c r="AJ23" s="637"/>
+      <c r="AJ23" s="616"/>
       <c r="AK23" s="262"/>
       <c r="AL23" s="80" t="s">
         <v>525</v>
       </c>
       <c r="AM23" s="306"/>
-      <c r="AN23" s="623"/>
+      <c r="AN23" s="627"/>
     </row>
     <row r="24" spans="1:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="464" t="s">
@@ -9186,23 +9218,23 @@
       <c r="E24" s="460">
         <v>1</v>
       </c>
-      <c r="F24" s="628"/>
+      <c r="F24" s="608"/>
       <c r="G24" s="61" t="s">
         <v>507</v>
       </c>
       <c r="I24" s="224"/>
-      <c r="O24" s="662"/>
-      <c r="Q24" s="665"/>
+      <c r="O24" s="611"/>
+      <c r="Q24" s="614"/>
       <c r="T24" s="17"/>
       <c r="U24" s="232" t="s">
         <v>44</v>
       </c>
-      <c r="V24" s="599"/>
+      <c r="V24" s="645"/>
       <c r="W24" s="148"/>
       <c r="X24" s="453" t="s">
         <v>186</v>
       </c>
-      <c r="Y24" s="641"/>
+      <c r="Y24" s="642"/>
       <c r="Z24" s="17"/>
       <c r="AA24" s="10"/>
       <c r="AB24" s="439"/>
@@ -9221,12 +9253,12 @@
         <v>480</v>
       </c>
       <c r="AM24" s="306"/>
-      <c r="AN24" s="623"/>
+      <c r="AN24" s="627"/>
     </row>
     <row r="25" spans="1:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="F25" s="628"/>
+      <c r="F25" s="608"/>
       <c r="I25" s="224"/>
-      <c r="O25" s="662"/>
+      <c r="O25" s="611"/>
       <c r="P25" s="209" t="s">
         <v>285</v>
       </c>
@@ -9239,12 +9271,12 @@
       <c r="U25" s="424" t="s">
         <v>44</v>
       </c>
-      <c r="V25" s="600"/>
+      <c r="V25" s="646"/>
       <c r="W25" s="148"/>
       <c r="X25" s="453" t="s">
         <v>190</v>
       </c>
-      <c r="Y25" s="641"/>
+      <c r="Y25" s="642"/>
       <c r="Z25" s="17"/>
       <c r="AA25" s="10"/>
       <c r="AB25" s="439"/>
@@ -9261,7 +9293,7 @@
       <c r="AK25" s="142"/>
       <c r="AL25" s="6"/>
       <c r="AM25" s="306"/>
-      <c r="AN25" s="623"/>
+      <c r="AN25" s="627"/>
     </row>
     <row r="26" spans="1:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="236" t="s">
@@ -9279,17 +9311,17 @@
       <c r="E26" s="398">
         <v>1</v>
       </c>
-      <c r="F26" s="628"/>
+      <c r="F26" s="608"/>
       <c r="G26" s="349" t="s">
         <v>504</v>
       </c>
       <c r="I26" s="224"/>
-      <c r="O26" s="662"/>
-      <c r="P26" s="625" t="s">
+      <c r="O26" s="611"/>
+      <c r="P26" s="629" t="s">
         <v>547</v>
       </c>
-      <c r="Q26" s="626"/>
-      <c r="R26" s="658" t="s">
+      <c r="Q26" s="630"/>
+      <c r="R26" s="605" t="s">
         <v>556</v>
       </c>
       <c r="T26" s="182"/>
@@ -9301,7 +9333,7 @@
       <c r="X26" s="453" t="s">
         <v>182</v>
       </c>
-      <c r="Y26" s="641"/>
+      <c r="Y26" s="642"/>
       <c r="Z26" s="17"/>
       <c r="AA26" s="10"/>
       <c r="AB26" s="439"/>
@@ -9328,7 +9360,7 @@
       <c r="AM26" s="466" t="s">
         <v>473</v>
       </c>
-      <c r="AN26" s="623"/>
+      <c r="AN26" s="627"/>
     </row>
     <row r="27" spans="1:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B27" s="21" t="s">
@@ -9340,13 +9372,13 @@
       <c r="E27" s="271" t="s">
         <v>44</v>
       </c>
-      <c r="F27" s="660"/>
+      <c r="F27" s="609"/>
       <c r="G27" s="61" t="s">
         <v>565</v>
       </c>
       <c r="I27" s="225"/>
-      <c r="O27" s="663"/>
-      <c r="R27" s="659"/>
+      <c r="O27" s="612"/>
+      <c r="R27" s="606"/>
       <c r="S27" s="445" t="s">
         <v>54</v>
       </c>
@@ -9359,7 +9391,7 @@
       <c r="X27" s="453" t="s">
         <v>551</v>
       </c>
-      <c r="Y27" s="642"/>
+      <c r="Y27" s="643"/>
       <c r="Z27" s="163"/>
       <c r="AA27" s="13"/>
       <c r="AB27" s="440"/>
@@ -9376,32 +9408,26 @@
       <c r="AM27" s="400" t="s">
         <v>326</v>
       </c>
-      <c r="AN27" s="624"/>
+      <c r="AN27" s="628"/>
     </row>
   </sheetData>
   <mergeCells count="54">
-    <mergeCell ref="E2:E3"/>
-    <mergeCell ref="K2:L2"/>
-    <mergeCell ref="I1:I2"/>
-    <mergeCell ref="R18:R19"/>
-    <mergeCell ref="R26:R27"/>
-    <mergeCell ref="F2:F27"/>
-    <mergeCell ref="O10:O27"/>
-    <mergeCell ref="Q20:Q21"/>
-    <mergeCell ref="Q23:Q24"/>
-    <mergeCell ref="G14:J14"/>
-    <mergeCell ref="G13:J13"/>
-    <mergeCell ref="H12:K12"/>
-    <mergeCell ref="A5:A6"/>
-    <mergeCell ref="C6:D6"/>
-    <mergeCell ref="AI6:AI10"/>
-    <mergeCell ref="AF12:AF15"/>
-    <mergeCell ref="AG7:AG12"/>
-    <mergeCell ref="L8:L9"/>
-    <mergeCell ref="S9:S12"/>
-    <mergeCell ref="N8:N9"/>
-    <mergeCell ref="AD12:AD15"/>
-    <mergeCell ref="C15:C16"/>
+    <mergeCell ref="V21:V25"/>
+    <mergeCell ref="U18:U20"/>
+    <mergeCell ref="C2:C3"/>
+    <mergeCell ref="C4:C5"/>
+    <mergeCell ref="A2:A3"/>
+    <mergeCell ref="B2:B3"/>
+    <mergeCell ref="D2:D3"/>
+    <mergeCell ref="J8:J9"/>
+    <mergeCell ref="G5:L6"/>
+    <mergeCell ref="I8:I9"/>
+    <mergeCell ref="K7:K9"/>
+    <mergeCell ref="H8:H9"/>
+    <mergeCell ref="G8:G9"/>
+    <mergeCell ref="B11:B12"/>
+    <mergeCell ref="B6:B7"/>
+    <mergeCell ref="B4:B5"/>
     <mergeCell ref="AN1:AN27"/>
     <mergeCell ref="P26:Q26"/>
     <mergeCell ref="Q2:Q3"/>
@@ -9418,22 +9444,28 @@
     <mergeCell ref="AD3:AD4"/>
     <mergeCell ref="S2:S3"/>
     <mergeCell ref="R2:R3"/>
-    <mergeCell ref="V21:V25"/>
-    <mergeCell ref="U18:U20"/>
-    <mergeCell ref="C2:C3"/>
-    <mergeCell ref="C4:C5"/>
-    <mergeCell ref="A2:A3"/>
-    <mergeCell ref="B2:B3"/>
-    <mergeCell ref="D2:D3"/>
-    <mergeCell ref="J8:J9"/>
-    <mergeCell ref="G5:L6"/>
-    <mergeCell ref="I8:I9"/>
-    <mergeCell ref="K7:K9"/>
-    <mergeCell ref="H8:H9"/>
-    <mergeCell ref="G8:G9"/>
-    <mergeCell ref="B11:B12"/>
-    <mergeCell ref="B6:B7"/>
-    <mergeCell ref="B4:B5"/>
+    <mergeCell ref="A5:A6"/>
+    <mergeCell ref="C6:D6"/>
+    <mergeCell ref="AI6:AI10"/>
+    <mergeCell ref="AF12:AF15"/>
+    <mergeCell ref="AG7:AG12"/>
+    <mergeCell ref="L8:L9"/>
+    <mergeCell ref="S9:S12"/>
+    <mergeCell ref="N8:N9"/>
+    <mergeCell ref="AD12:AD15"/>
+    <mergeCell ref="C15:C16"/>
+    <mergeCell ref="E2:E3"/>
+    <mergeCell ref="K2:L2"/>
+    <mergeCell ref="I1:I2"/>
+    <mergeCell ref="R18:R19"/>
+    <mergeCell ref="R26:R27"/>
+    <mergeCell ref="F2:F27"/>
+    <mergeCell ref="O10:O27"/>
+    <mergeCell ref="Q20:Q21"/>
+    <mergeCell ref="Q23:Q24"/>
+    <mergeCell ref="G14:J14"/>
+    <mergeCell ref="G13:J13"/>
+    <mergeCell ref="H12:K12"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -9443,8 +9475,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2029A93E-B53C-4201-9F17-439C144F3CF1}">
   <dimension ref="A1:AN37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="M18" workbookViewId="0">
-      <selection activeCell="AL30" sqref="AL30"/>
+    <sheetView tabSelected="1" topLeftCell="N1" workbookViewId="0">
+      <selection activeCell="AN25" sqref="AN25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9454,7 +9486,7 @@
     <col min="4" max="4" width="3" customWidth="1"/>
     <col min="6" max="7" width="2.28515625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="5.42578125" style="112" customWidth="1"/>
-    <col min="9" max="9" width="17.7109375" customWidth="1"/>
+    <col min="9" max="9" width="18.5703125" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="15.7109375" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="27.140625" style="391" customWidth="1"/>
     <col min="12" max="12" width="3.85546875" bestFit="1" customWidth="1"/>
@@ -9539,10 +9571,10 @@
       <c r="S1" s="142"/>
       <c r="T1" s="142"/>
       <c r="U1" s="6"/>
-      <c r="V1" s="673" t="s">
+      <c r="V1" s="671" t="s">
         <v>458</v>
       </c>
-      <c r="W1" s="674"/>
+      <c r="W1" s="672"/>
       <c r="X1" s="312">
         <f>68-(U8+W3+V3+S3)</f>
         <v>0</v>
@@ -9558,21 +9590,21 @@
       <c r="AB1" s="308" t="s">
         <v>44</v>
       </c>
-      <c r="AC1" s="675" t="s">
+      <c r="AC1" s="673" t="s">
         <v>191</v>
       </c>
-      <c r="AD1" s="676"/>
-      <c r="AE1" s="677"/>
-      <c r="AF1" s="678" t="s">
+      <c r="AD1" s="674"/>
+      <c r="AE1" s="675"/>
+      <c r="AF1" s="676" t="s">
         <v>298</v>
       </c>
-      <c r="AG1" s="679"/>
-      <c r="AH1" s="680"/>
-      <c r="AI1" s="670" t="s">
+      <c r="AG1" s="677"/>
+      <c r="AH1" s="678"/>
+      <c r="AI1" s="668" t="s">
         <v>461</v>
       </c>
-      <c r="AJ1" s="671"/>
-      <c r="AK1" s="672"/>
+      <c r="AJ1" s="669"/>
+      <c r="AK1" s="670"/>
       <c r="AN1" s="142"/>
     </row>
     <row r="2" spans="1:40" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -9589,21 +9621,21 @@
       <c r="K2" s="327">
         <v>-3</v>
       </c>
-      <c r="L2" s="681">
+      <c r="L2" s="679">
         <f>SUM(L5:L30)</f>
         <v>3</v>
       </c>
-      <c r="M2" s="683">
+      <c r="M2" s="681">
         <f>SUM(M4:M29)</f>
-        <v>10</v>
-      </c>
-      <c r="N2" s="685">
+        <v>11</v>
+      </c>
+      <c r="N2" s="683">
         <f>SUM(N4:N29)</f>
         <v>11</v>
       </c>
-      <c r="O2" s="649">
+      <c r="O2" s="623">
         <f>SUM(M30:M37)* (-1)</f>
-        <v>-3</v>
+        <v>-4</v>
       </c>
       <c r="P2" s="275" t="s">
         <v>243</v>
@@ -9620,7 +9652,7 @@
       <c r="T2" s="515" t="s">
         <v>221</v>
       </c>
-      <c r="U2" s="687" t="s">
+      <c r="U2" s="685" t="s">
         <v>239</v>
       </c>
       <c r="V2" s="516" t="s">
@@ -9689,10 +9721,10 @@
         <f>T3+V3+W3+S3</f>
         <v>68</v>
       </c>
-      <c r="L3" s="682"/>
-      <c r="M3" s="684"/>
-      <c r="N3" s="686"/>
-      <c r="O3" s="650"/>
+      <c r="L3" s="680"/>
+      <c r="M3" s="682"/>
+      <c r="N3" s="684"/>
+      <c r="O3" s="624"/>
       <c r="P3" s="176">
         <f>(L2+M2)-W3</f>
         <v>0</v>
@@ -9706,16 +9738,16 @@
       </c>
       <c r="T3" s="518">
         <f>SUM(T4:T29)</f>
-        <v>36</v>
-      </c>
-      <c r="U3" s="688"/>
+        <v>35</v>
+      </c>
+      <c r="U3" s="686"/>
       <c r="V3" s="519">
         <f t="shared" ref="V3:AA3" si="0">SUM(V4:V29)</f>
         <v>7</v>
       </c>
       <c r="W3" s="519">
         <f t="shared" si="0"/>
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="X3" s="59">
         <f t="shared" si="0"/>
@@ -9727,7 +9759,7 @@
       </c>
       <c r="Z3" s="66">
         <f t="shared" si="0"/>
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="AA3" s="66">
         <f t="shared" si="0"/>
@@ -9807,7 +9839,7 @@
         <f>AA4</f>
         <v>0</v>
       </c>
-      <c r="O4" s="667" t="s">
+      <c r="O4" s="687" t="s">
         <v>200</v>
       </c>
       <c r="P4" s="20"/>
@@ -9886,7 +9918,7 @@
         <f>AA5</f>
         <v>0</v>
       </c>
-      <c r="O5" s="668"/>
+      <c r="O5" s="688"/>
       <c r="P5" s="20"/>
       <c r="Q5" s="2" t="s">
         <v>347</v>
@@ -9973,7 +10005,7 @@
         <f>AA6</f>
         <v>0</v>
       </c>
-      <c r="O6" s="668"/>
+      <c r="O6" s="688"/>
       <c r="P6" s="19" t="s">
         <v>342</v>
       </c>
@@ -10065,7 +10097,7 @@
         <f t="shared" ref="N7:N37" si="10">AA7</f>
         <v>0</v>
       </c>
-      <c r="O7" s="668"/>
+      <c r="O7" s="688"/>
       <c r="P7" s="20"/>
       <c r="Q7" s="2" t="s">
         <v>342</v>
@@ -10132,7 +10164,9 @@
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
-      <c r="AL7" s="6"/>
+      <c r="AL7" s="6" t="s">
+        <v>245</v>
+      </c>
       <c r="AM7" s="546"/>
       <c r="AN7" s="262"/>
     </row>
@@ -10171,7 +10205,7 @@
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
-      <c r="O8" s="668"/>
+      <c r="O8" s="688"/>
       <c r="P8" s="21" t="s">
         <v>238</v>
       </c>
@@ -10189,7 +10223,7 @@
       </c>
       <c r="U8" s="29">
         <f>T3</f>
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="V8" s="531">
         <v>0</v>
@@ -10255,7 +10289,7 @@
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
-      <c r="O9" s="668"/>
+      <c r="O9" s="688"/>
       <c r="P9" s="21" t="s">
         <v>342</v>
       </c>
@@ -10353,7 +10387,7 @@
         <f t="shared" si="10"/>
         <v>2</v>
       </c>
-      <c r="O10" s="668"/>
+      <c r="O10" s="688"/>
       <c r="P10" s="20"/>
       <c r="Q10" s="2" t="s">
         <v>347</v>
@@ -10436,7 +10470,7 @@
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
-      <c r="O11" s="668"/>
+      <c r="O11" s="688"/>
       <c r="P11" s="21" t="s">
         <v>342</v>
       </c>
@@ -10496,7 +10530,7 @@
       <c r="AN11" s="142"/>
     </row>
     <row r="12" spans="1:40" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="613" t="s">
+      <c r="A12" s="659" t="s">
         <v>55</v>
       </c>
       <c r="B12" s="30">
@@ -10505,11 +10539,11 @@
       <c r="C12" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="E12" s="664" t="s">
+      <c r="E12" s="613" t="s">
         <v>57</v>
       </c>
       <c r="G12" s="267"/>
-      <c r="H12" s="544">
+      <c r="H12" s="743">
         <v>-1</v>
       </c>
       <c r="I12" s="61" t="s">
@@ -10526,7 +10560,7 @@
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
-      <c r="O12" s="668"/>
+      <c r="O12" s="688"/>
       <c r="P12" s="21" t="s">
         <v>342</v>
       </c>
@@ -10598,14 +10632,14 @@
       </c>
     </row>
     <row r="13" spans="1:40" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="615"/>
+      <c r="A13" s="661"/>
       <c r="B13" s="153">
         <v>12</v>
       </c>
       <c r="C13" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="E13" s="665"/>
+      <c r="E13" s="614"/>
       <c r="F13" s="176">
         <v>0</v>
       </c>
@@ -10628,7 +10662,7 @@
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
-      <c r="O13" s="668"/>
+      <c r="O13" s="688"/>
       <c r="P13" s="21" t="s">
         <v>342</v>
       </c>
@@ -10704,7 +10738,7 @@
         <f t="shared" si="10"/>
         <v>2</v>
       </c>
-      <c r="O14" s="668"/>
+      <c r="O14" s="688"/>
       <c r="P14" s="20"/>
       <c r="Q14" s="205" t="s">
         <v>346</v>
@@ -10799,7 +10833,7 @@
         <f t="shared" si="10"/>
         <v>1</v>
       </c>
-      <c r="O15" s="668"/>
+      <c r="O15" s="688"/>
       <c r="P15" s="20"/>
       <c r="Q15" s="205" t="s">
         <v>346</v>
@@ -10886,7 +10920,7 @@
         <f t="shared" si="10"/>
         <v>1</v>
       </c>
-      <c r="O16" s="668"/>
+      <c r="O16" s="688"/>
       <c r="P16" s="21" t="s">
         <v>342</v>
       </c>
@@ -10984,7 +11018,7 @@
         <f t="shared" si="10"/>
         <v>1</v>
       </c>
-      <c r="O17" s="668"/>
+      <c r="O17" s="688"/>
       <c r="P17" s="20"/>
       <c r="Q17" s="2" t="s">
         <v>348</v>
@@ -11079,7 +11113,7 @@
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
-      <c r="O18" s="668"/>
+      <c r="O18" s="688"/>
       <c r="P18" s="21" t="s">
         <v>342</v>
       </c>
@@ -11162,7 +11196,7 @@
         <f t="shared" si="10"/>
         <v>1</v>
       </c>
-      <c r="O19" s="668"/>
+      <c r="O19" s="688"/>
       <c r="P19" s="20"/>
       <c r="Q19" s="2" t="s">
         <v>341</v>
@@ -11260,11 +11294,11 @@
         <f t="shared" si="10"/>
         <v>1</v>
       </c>
-      <c r="O20" s="669"/>
-      <c r="P20" s="563" t="s">
+      <c r="O20" s="689"/>
+      <c r="P20" s="564" t="s">
         <v>342</v>
       </c>
-      <c r="Q20" s="666"/>
+      <c r="Q20" s="615"/>
       <c r="R20" s="321" t="s">
         <v>86</v>
       </c>
@@ -11500,7 +11534,7 @@
       <c r="AN22" s="142"/>
     </row>
     <row r="23" spans="1:40" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E23" s="620" t="s">
+      <c r="E23" s="666" t="s">
         <v>294</v>
       </c>
       <c r="F23" s="184"/>
@@ -11596,7 +11630,7 @@
       <c r="C24" s="2" t="s">
         <v>260</v>
       </c>
-      <c r="E24" s="621"/>
+      <c r="E24" s="667"/>
       <c r="F24" s="176"/>
       <c r="H24" s="42">
         <v>-1</v>
@@ -11614,10 +11648,10 @@
         <f t="shared" si="10"/>
         <v>1</v>
       </c>
-      <c r="P24" s="563" t="s">
+      <c r="P24" s="564" t="s">
         <v>342</v>
       </c>
-      <c r="Q24" s="666"/>
+      <c r="Q24" s="615"/>
       <c r="R24" s="321" t="s">
         <v>254</v>
       </c>
@@ -11681,7 +11715,7 @@
       <c r="AL24" s="6" t="s">
         <v>527</v>
       </c>
-      <c r="AM24" s="741" t="s">
+      <c r="AM24" s="553" t="s">
         <v>342</v>
       </c>
       <c r="AN24" s="142" t="s">
@@ -11689,13 +11723,19 @@
       </c>
     </row>
     <row r="25" spans="1:40" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="H25" s="42">
+        <v>-1</v>
+      </c>
+      <c r="I25" s="2" t="s">
+        <v>620</v>
+      </c>
       <c r="J25" s="334"/>
       <c r="K25" s="403" t="s">
         <v>300</v>
       </c>
       <c r="L25" s="342"/>
       <c r="M25" s="107">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N25" s="299">
         <f t="shared" si="10"/>
@@ -11711,7 +11751,7 @@
         <v>2</v>
       </c>
       <c r="T25" s="526">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="U25" s="527">
         <v>-2</v>
@@ -11719,7 +11759,7 @@
       <c r="V25" s="540"/>
       <c r="W25" s="524">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="X25" s="302"/>
       <c r="Y25" s="117">
@@ -11728,7 +11768,7 @@
       </c>
       <c r="Z25" s="296">
         <f t="shared" si="6"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AA25" s="296">
         <v>0</v>
@@ -11758,7 +11798,9 @@
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
-      <c r="AL25" s="16"/>
+      <c r="AL25" s="16" t="s">
+        <v>469</v>
+      </c>
       <c r="AM25" s="546" t="s">
         <v>470</v>
       </c>
@@ -12140,8 +12182,8 @@
       <c r="F31" s="100">
         <v>-1</v>
       </c>
-      <c r="H31" s="42">
-        <v>-3</v>
+      <c r="H31" s="743">
+        <v>-1</v>
       </c>
       <c r="I31" s="21" t="s">
         <v>435</v>
@@ -12205,9 +12247,10 @@
       <c r="H32" s="42">
         <v>-1</v>
       </c>
-      <c r="I32" s="61" t="s">
-        <v>510</v>
-      </c>
+      <c r="I32" s="662" t="s">
+        <v>617</v>
+      </c>
+      <c r="J32" s="742"/>
       <c r="K32" s="406"/>
       <c r="L32" s="550">
         <v>0</v>
@@ -12364,14 +12407,14 @@
         <v>304</v>
       </c>
       <c r="H34" s="42">
-        <v>-1</v>
+        <v>-2</v>
       </c>
       <c r="K34" s="403" t="s">
         <v>305</v>
       </c>
       <c r="L34" s="345"/>
       <c r="M34" s="253">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N34" s="299">
         <f t="shared" si="10"/>
@@ -12387,7 +12430,7 @@
         <v>2</v>
       </c>
       <c r="T34" s="194">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="U34" s="195">
         <v>-2</v>
@@ -12395,7 +12438,7 @@
       <c r="V34" s="216"/>
       <c r="W34" s="188">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="X34" s="65"/>
       <c r="Y34" s="117">
@@ -12404,7 +12447,7 @@
       </c>
       <c r="Z34" s="64">
         <f t="shared" si="6"/>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="AA34" s="64">
         <v>2</v>
@@ -12436,7 +12479,9 @@
         <f t="shared" si="9"/>
         <v>2</v>
       </c>
-      <c r="AL34" s="6"/>
+      <c r="AL34" s="6" t="s">
+        <v>616</v>
+      </c>
       <c r="AM34" s="546" t="s">
         <v>588</v>
       </c>
@@ -12602,7 +12647,7 @@
       </c>
     </row>
     <row r="37" spans="3:40" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="H37" s="544">
+      <c r="H37" s="743">
         <v>-1</v>
       </c>
       <c r="K37" s="405" t="s">
@@ -12688,7 +12733,14 @@
       </c>
     </row>
   </sheetData>
-  <mergeCells count="15">
+  <mergeCells count="16">
+    <mergeCell ref="I32:J32"/>
+    <mergeCell ref="A12:A13"/>
+    <mergeCell ref="E12:E13"/>
+    <mergeCell ref="P20:Q20"/>
+    <mergeCell ref="E23:E24"/>
+    <mergeCell ref="P24:Q24"/>
+    <mergeCell ref="O4:O20"/>
     <mergeCell ref="AI1:AK1"/>
     <mergeCell ref="V1:W1"/>
     <mergeCell ref="AC1:AE1"/>
@@ -12698,12 +12750,6 @@
     <mergeCell ref="N2:N3"/>
     <mergeCell ref="O2:O3"/>
     <mergeCell ref="U2:U3"/>
-    <mergeCell ref="A12:A13"/>
-    <mergeCell ref="E12:E13"/>
-    <mergeCell ref="P20:Q20"/>
-    <mergeCell ref="E23:E24"/>
-    <mergeCell ref="P24:Q24"/>
-    <mergeCell ref="O4:O20"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -12738,15 +12784,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B1" s="563" t="s">
+      <c r="B1" s="564" t="s">
         <v>317</v>
       </c>
-      <c r="C1" s="666"/>
+      <c r="C1" s="615"/>
       <c r="D1" s="209"/>
-      <c r="J1" s="563" t="s">
+      <c r="J1" s="564" t="s">
         <v>70</v>
       </c>
-      <c r="K1" s="666"/>
+      <c r="K1" s="615"/>
       <c r="L1" s="200" t="s">
         <v>337</v>
       </c>
@@ -12784,13 +12830,13 @@
         <v>34</v>
       </c>
       <c r="L2" s="201"/>
-      <c r="M2" s="689"/>
+      <c r="M2" s="690"/>
       <c r="N2" s="154">
         <v>2</v>
       </c>
       <c r="O2" s="155"/>
       <c r="P2" s="5"/>
-      <c r="Q2" s="692" t="s">
+      <c r="Q2" s="693" t="s">
         <v>44</v>
       </c>
       <c r="R2" s="19">
@@ -12813,13 +12859,13 @@
       <c r="K3" s="6" t="s">
         <v>334</v>
       </c>
-      <c r="M3" s="690"/>
+      <c r="M3" s="691"/>
       <c r="N3" s="17">
         <v>1</v>
       </c>
       <c r="O3" s="15"/>
       <c r="P3" s="10"/>
-      <c r="Q3" s="693"/>
+      <c r="Q3" s="694"/>
       <c r="R3" s="224"/>
     </row>
     <row r="4" spans="2:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -12838,13 +12884,13 @@
       <c r="K4" s="6" t="s">
         <v>335</v>
       </c>
-      <c r="M4" s="690"/>
+      <c r="M4" s="691"/>
       <c r="N4" s="17"/>
       <c r="O4" s="15">
         <v>1</v>
       </c>
       <c r="P4" s="10"/>
-      <c r="Q4" s="693"/>
+      <c r="Q4" s="694"/>
       <c r="R4" s="224"/>
     </row>
     <row r="5" spans="2:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -12864,13 +12910,13 @@
         <v>13</v>
       </c>
       <c r="L5" s="201"/>
-      <c r="M5" s="690"/>
+      <c r="M5" s="691"/>
       <c r="N5" s="17">
         <v>1</v>
       </c>
       <c r="O5" s="15"/>
       <c r="P5" s="10"/>
-      <c r="Q5" s="693"/>
+      <c r="Q5" s="694"/>
       <c r="R5" s="19">
         <v>-1</v>
       </c>
@@ -12891,13 +12937,13 @@
       <c r="K6" s="6" t="s">
         <v>333</v>
       </c>
-      <c r="M6" s="690"/>
+      <c r="M6" s="691"/>
       <c r="N6" s="17">
         <v>1</v>
       </c>
       <c r="O6" s="15"/>
       <c r="P6" s="10"/>
-      <c r="Q6" s="693"/>
+      <c r="Q6" s="694"/>
       <c r="R6" s="224"/>
     </row>
     <row r="7" spans="2:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -12917,13 +12963,13 @@
         <v>334</v>
       </c>
       <c r="L7" s="203"/>
-      <c r="M7" s="690"/>
+      <c r="M7" s="691"/>
       <c r="N7" s="17">
         <v>1</v>
       </c>
       <c r="O7" s="15"/>
       <c r="P7" s="10"/>
-      <c r="Q7" s="693"/>
+      <c r="Q7" s="694"/>
       <c r="R7" s="19">
         <v>-1</v>
       </c>
@@ -12944,13 +12990,13 @@
       <c r="K8" s="6" t="s">
         <v>332</v>
       </c>
-      <c r="M8" s="690"/>
+      <c r="M8" s="691"/>
       <c r="N8" s="17">
         <v>1</v>
       </c>
       <c r="O8" s="15"/>
       <c r="P8" s="10"/>
-      <c r="Q8" s="693"/>
+      <c r="Q8" s="694"/>
       <c r="R8" s="224"/>
     </row>
     <row r="9" spans="2:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -12970,13 +13016,13 @@
         <v>336</v>
       </c>
       <c r="L9" s="185"/>
-      <c r="M9" s="691"/>
+      <c r="M9" s="692"/>
       <c r="N9" s="163"/>
       <c r="O9" s="18"/>
       <c r="P9" s="13">
         <v>1</v>
       </c>
-      <c r="Q9" s="694"/>
+      <c r="Q9" s="695"/>
       <c r="R9" s="225"/>
     </row>
     <row r="10" spans="2:18" x14ac:dyDescent="0.25">
@@ -13134,10 +13180,10 @@
         <f ca="1">TODAY()</f>
         <v>45279</v>
       </c>
-      <c r="V1" s="563" t="s">
+      <c r="V1" s="564" t="s">
         <v>71</v>
       </c>
-      <c r="W1" s="666"/>
+      <c r="W1" s="615"/>
       <c r="X1" s="62" t="s">
         <v>102</v>
       </c>
@@ -13156,7 +13202,7 @@
       <c r="AC1" s="116" t="s">
         <v>191</v>
       </c>
-      <c r="AD1" s="709" t="s">
+      <c r="AD1" s="703" t="s">
         <v>213</v>
       </c>
       <c r="AE1" s="116" t="s">
@@ -13173,10 +13219,10 @@
       <c r="E2" s="39" t="s">
         <v>74</v>
       </c>
-      <c r="F2" s="740" t="s">
+      <c r="F2" s="702" t="s">
         <v>75</v>
       </c>
-      <c r="G2" s="697" t="s">
+      <c r="G2" s="730" t="s">
         <v>44</v>
       </c>
       <c r="H2" s="40" t="s">
@@ -13204,10 +13250,10 @@
       <c r="U2" s="60" t="s">
         <v>106</v>
       </c>
-      <c r="V2" s="673" t="s">
+      <c r="V2" s="671" t="s">
         <v>121</v>
       </c>
-      <c r="W2" s="674"/>
+      <c r="W2" s="672"/>
       <c r="X2" s="64" t="s">
         <v>110</v>
       </c>
@@ -13226,7 +13272,7 @@
       <c r="AC2" s="117" t="s">
         <v>99</v>
       </c>
-      <c r="AD2" s="710"/>
+      <c r="AD2" s="704"/>
       <c r="AE2" s="64" t="s">
         <v>99</v>
       </c>
@@ -13245,8 +13291,8 @@
       <c r="E3" s="39" t="s">
         <v>80</v>
       </c>
-      <c r="F3" s="617"/>
-      <c r="G3" s="698"/>
+      <c r="F3" s="663"/>
+      <c r="G3" s="731"/>
       <c r="H3" s="40" t="s">
         <v>81</v>
       </c>
@@ -13257,13 +13303,13 @@
         <v>82</v>
       </c>
       <c r="N3" s="44"/>
-      <c r="O3" s="707" t="s">
+      <c r="O3" s="740" t="s">
         <v>44</v>
       </c>
-      <c r="P3" s="728" t="s">
+      <c r="P3" s="722" t="s">
         <v>219</v>
       </c>
-      <c r="Q3" s="729"/>
+      <c r="Q3" s="723"/>
       <c r="S3" s="57" t="s">
         <v>220</v>
       </c>
@@ -13273,15 +13319,15 @@
       <c r="W3" s="59" t="s">
         <v>105</v>
       </c>
-      <c r="AD3" s="710"/>
+      <c r="AD3" s="704"/>
     </row>
     <row r="4" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="G4" s="698"/>
+      <c r="G4" s="731"/>
       <c r="H4" s="6"/>
-      <c r="L4" s="692" t="s">
+      <c r="L4" s="693" t="s">
         <v>83</v>
       </c>
-      <c r="O4" s="708"/>
+      <c r="O4" s="741"/>
       <c r="T4" s="55" t="s">
         <v>98</v>
       </c>
@@ -13291,12 +13337,12 @@
       <c r="X4" s="67" t="s">
         <v>223</v>
       </c>
-      <c r="Y4" s="563" t="s">
+      <c r="Y4" s="564" t="s">
         <v>195</v>
       </c>
-      <c r="Z4" s="565"/>
-      <c r="AA4" s="666"/>
-      <c r="AD4" s="710"/>
+      <c r="Z4" s="566"/>
+      <c r="AA4" s="615"/>
+      <c r="AD4" s="704"/>
     </row>
     <row r="5" spans="1:31" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C5" s="52" t="s">
@@ -13311,21 +13357,21 @@
       <c r="F5" s="66" t="s">
         <v>85</v>
       </c>
-      <c r="G5" s="698"/>
+      <c r="G5" s="731"/>
       <c r="H5" s="46" t="s">
         <v>76</v>
       </c>
-      <c r="K5" s="715" t="s">
+      <c r="K5" s="709" t="s">
         <v>217</v>
       </c>
-      <c r="L5" s="730"/>
+      <c r="L5" s="724"/>
       <c r="M5" s="2" t="s">
         <v>215</v>
       </c>
       <c r="N5" s="61" t="s">
         <v>214</v>
       </c>
-      <c r="O5" s="708"/>
+      <c r="O5" s="741"/>
       <c r="P5" s="108" t="s">
         <v>216</v>
       </c>
@@ -13341,11 +13387,11 @@
       <c r="U5" s="19" t="s">
         <v>99</v>
       </c>
-      <c r="Y5" s="718" t="s">
+      <c r="Y5" s="712" t="s">
         <v>287</v>
       </c>
-      <c r="Z5" s="719"/>
-      <c r="AD5" s="710"/>
+      <c r="Z5" s="713"/>
+      <c r="AD5" s="704"/>
     </row>
     <row r="6" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C6" s="109"/>
@@ -13355,16 +13401,16 @@
       <c r="E6" s="45" t="s">
         <v>86</v>
       </c>
-      <c r="G6" s="698"/>
+      <c r="G6" s="731"/>
       <c r="H6" s="46" t="s">
         <v>81</v>
       </c>
       <c r="I6" s="23">
         <v>15</v>
       </c>
-      <c r="K6" s="716"/>
-      <c r="L6" s="730"/>
-      <c r="O6" s="708"/>
+      <c r="K6" s="710"/>
+      <c r="L6" s="724"/>
+      <c r="O6" s="741"/>
       <c r="T6" s="2" t="s">
         <v>101</v>
       </c>
@@ -13374,23 +13420,23 @@
       <c r="V6" s="21">
         <v>-1</v>
       </c>
-      <c r="AD6" s="710"/>
+      <c r="AD6" s="704"/>
     </row>
     <row r="7" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C7" s="110"/>
-      <c r="G7" s="698"/>
+      <c r="G7" s="731"/>
       <c r="H7" s="6"/>
-      <c r="K7" s="716"/>
-      <c r="L7" s="730"/>
+      <c r="K7" s="710"/>
+      <c r="L7" s="724"/>
       <c r="N7" s="21" t="s">
         <v>120</v>
       </c>
-      <c r="O7" s="708"/>
+      <c r="O7" s="741"/>
       <c r="P7" s="73"/>
       <c r="U7" s="104" t="s">
         <v>20</v>
       </c>
-      <c r="AD7" s="710"/>
+      <c r="AD7" s="704"/>
     </row>
     <row r="8" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C8" s="130"/>
@@ -13403,7 +13449,7 @@
       <c r="F8" s="66" t="s">
         <v>87</v>
       </c>
-      <c r="G8" s="698"/>
+      <c r="G8" s="731"/>
       <c r="H8" s="50" t="s">
         <v>76</v>
       </c>
@@ -13413,41 +13459,41 @@
       <c r="J8" s="111">
         <v>115</v>
       </c>
-      <c r="K8" s="716"/>
-      <c r="L8" s="730"/>
-      <c r="O8" s="708"/>
+      <c r="K8" s="710"/>
+      <c r="L8" s="724"/>
+      <c r="O8" s="741"/>
       <c r="P8" s="49"/>
-      <c r="S8" s="712" t="s">
+      <c r="S8" s="706" t="s">
         <v>212</v>
       </c>
-      <c r="T8" s="713"/>
-      <c r="U8" s="713"/>
-      <c r="V8" s="713"/>
-      <c r="W8" s="713"/>
-      <c r="X8" s="713"/>
-      <c r="Y8" s="713"/>
-      <c r="Z8" s="713"/>
-      <c r="AA8" s="713"/>
-      <c r="AB8" s="713"/>
-      <c r="AC8" s="714"/>
-      <c r="AD8" s="710"/>
+      <c r="T8" s="707"/>
+      <c r="U8" s="707"/>
+      <c r="V8" s="707"/>
+      <c r="W8" s="707"/>
+      <c r="X8" s="707"/>
+      <c r="Y8" s="707"/>
+      <c r="Z8" s="707"/>
+      <c r="AA8" s="707"/>
+      <c r="AB8" s="707"/>
+      <c r="AC8" s="708"/>
+      <c r="AD8" s="704"/>
     </row>
     <row r="9" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C9" s="734"/>
-      <c r="G9" s="698"/>
+      <c r="C9" s="696"/>
+      <c r="G9" s="731"/>
       <c r="H9" s="6"/>
-      <c r="K9" s="716"/>
-      <c r="L9" s="701" t="s">
+      <c r="K9" s="710"/>
+      <c r="L9" s="734" t="s">
         <v>218</v>
       </c>
-      <c r="M9" s="702"/>
-      <c r="N9" s="703"/>
-      <c r="O9" s="708"/>
+      <c r="M9" s="735"/>
+      <c r="N9" s="736"/>
+      <c r="O9" s="741"/>
       <c r="P9" s="75"/>
-      <c r="AD9" s="710"/>
+      <c r="AD9" s="704"/>
     </row>
     <row r="10" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C10" s="735"/>
+      <c r="C10" s="697"/>
       <c r="D10" s="23"/>
       <c r="E10" s="45" t="s">
         <v>88</v>
@@ -13455,7 +13501,7 @@
       <c r="F10" s="66" t="s">
         <v>89</v>
       </c>
-      <c r="G10" s="698"/>
+      <c r="G10" s="731"/>
       <c r="H10" s="51"/>
       <c r="I10" s="21" t="s">
         <v>81</v>
@@ -13463,33 +13509,33 @@
       <c r="J10" s="3">
         <v>15</v>
       </c>
-      <c r="K10" s="716"/>
-      <c r="M10" s="737" t="s">
+      <c r="K10" s="710"/>
+      <c r="M10" s="699" t="s">
         <v>90</v>
       </c>
-      <c r="N10" s="738"/>
-      <c r="O10" s="738"/>
-      <c r="P10" s="738"/>
-      <c r="Q10" s="738"/>
-      <c r="R10" s="738"/>
-      <c r="S10" s="738"/>
-      <c r="T10" s="738"/>
-      <c r="U10" s="738"/>
-      <c r="V10" s="738"/>
-      <c r="W10" s="738"/>
-      <c r="X10" s="738"/>
-      <c r="Y10" s="738"/>
-      <c r="Z10" s="738"/>
-      <c r="AA10" s="738"/>
-      <c r="AB10" s="738"/>
-      <c r="AC10" s="739"/>
-      <c r="AD10" s="710"/>
+      <c r="N10" s="700"/>
+      <c r="O10" s="700"/>
+      <c r="P10" s="700"/>
+      <c r="Q10" s="700"/>
+      <c r="R10" s="700"/>
+      <c r="S10" s="700"/>
+      <c r="T10" s="700"/>
+      <c r="U10" s="700"/>
+      <c r="V10" s="700"/>
+      <c r="W10" s="700"/>
+      <c r="X10" s="700"/>
+      <c r="Y10" s="700"/>
+      <c r="Z10" s="700"/>
+      <c r="AA10" s="700"/>
+      <c r="AB10" s="700"/>
+      <c r="AC10" s="701"/>
+      <c r="AD10" s="704"/>
     </row>
     <row r="11" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C11" s="736"/>
-      <c r="G11" s="698"/>
+      <c r="C11" s="698"/>
+      <c r="G11" s="731"/>
       <c r="H11" s="6"/>
-      <c r="K11" s="716"/>
+      <c r="K11" s="710"/>
       <c r="R11" s="52" t="s">
         <v>44</v>
       </c>
@@ -13497,17 +13543,17 @@
       <c r="Y11" s="68" t="s">
         <v>121</v>
       </c>
-      <c r="Z11" s="726" t="s">
+      <c r="Z11" s="720" t="s">
         <v>121</v>
       </c>
-      <c r="AA11" s="727"/>
+      <c r="AA11" s="721"/>
       <c r="AB11" s="52" t="s">
         <v>44</v>
       </c>
       <c r="AC11" s="118" t="s">
         <v>121</v>
       </c>
-      <c r="AD11" s="710"/>
+      <c r="AD11" s="704"/>
     </row>
     <row r="12" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C12" s="129"/>
@@ -13520,7 +13566,7 @@
       <c r="F12" s="66" t="s">
         <v>92</v>
       </c>
-      <c r="G12" s="698"/>
+      <c r="G12" s="731"/>
       <c r="H12" s="128"/>
       <c r="I12" s="19" t="s">
         <v>81</v>
@@ -13528,8 +13574,8 @@
       <c r="J12" s="3">
         <v>15</v>
       </c>
-      <c r="K12" s="716"/>
-      <c r="L12" s="731" t="s">
+      <c r="K12" s="710"/>
+      <c r="L12" s="725" t="s">
         <v>93</v>
       </c>
       <c r="M12" s="21" t="s">
@@ -13544,7 +13590,7 @@
       <c r="Q12" s="113" t="s">
         <v>44</v>
       </c>
-      <c r="S12" s="558" t="s">
+      <c r="S12" s="559" t="s">
         <v>107</v>
       </c>
       <c r="T12" s="2" t="s">
@@ -13560,26 +13606,26 @@
         <v>116</v>
       </c>
       <c r="Y12" s="6"/>
-      <c r="AA12" s="720" t="s">
+      <c r="AA12" s="714" t="s">
         <v>126</v>
       </c>
-      <c r="AB12" s="721"/>
+      <c r="AB12" s="715"/>
       <c r="AC12" s="21" t="s">
         <v>233</v>
       </c>
-      <c r="AD12" s="710"/>
+      <c r="AD12" s="704"/>
     </row>
     <row r="13" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C13" s="734"/>
-      <c r="G13" s="698"/>
-      <c r="K13" s="716"/>
-      <c r="L13" s="732"/>
+      <c r="C13" s="696"/>
+      <c r="G13" s="731"/>
+      <c r="K13" s="710"/>
+      <c r="L13" s="726"/>
       <c r="M13" s="47"/>
-      <c r="Q13" s="700" t="s">
+      <c r="Q13" s="733" t="s">
         <v>210</v>
       </c>
-      <c r="R13" s="626"/>
-      <c r="S13" s="559"/>
+      <c r="R13" s="630"/>
+      <c r="S13" s="560"/>
       <c r="T13" s="6"/>
       <c r="U13" s="96" t="s">
         <v>132</v>
@@ -13587,17 +13633,17 @@
       <c r="X13" s="2" t="s">
         <v>123</v>
       </c>
-      <c r="AA13" s="722"/>
-      <c r="AB13" s="723"/>
-      <c r="AD13" s="710"/>
+      <c r="AA13" s="716"/>
+      <c r="AB13" s="717"/>
+      <c r="AD13" s="704"/>
     </row>
     <row r="14" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B14" s="2" t="s">
         <v>339</v>
       </c>
-      <c r="C14" s="736"/>
+      <c r="C14" s="698"/>
       <c r="D14" s="23"/>
-      <c r="G14" s="698"/>
+      <c r="G14" s="731"/>
       <c r="H14" s="125"/>
       <c r="I14" s="99" t="s">
         <v>44</v>
@@ -13605,8 +13651,8 @@
       <c r="J14" s="111">
         <v>115</v>
       </c>
-      <c r="K14" s="716"/>
-      <c r="L14" s="732"/>
+      <c r="K14" s="710"/>
+      <c r="L14" s="726"/>
       <c r="M14" s="21" t="s">
         <v>111</v>
       </c>
@@ -13616,7 +13662,7 @@
       <c r="R14" s="115" t="s">
         <v>44</v>
       </c>
-      <c r="S14" s="559"/>
+      <c r="S14" s="560"/>
       <c r="T14" s="77" t="s">
         <v>130</v>
       </c>
@@ -13627,9 +13673,9 @@
       <c r="Y14" s="21" t="s">
         <v>73</v>
       </c>
-      <c r="AA14" s="722"/>
-      <c r="AB14" s="723"/>
-      <c r="AD14" s="710"/>
+      <c r="AA14" s="716"/>
+      <c r="AB14" s="717"/>
+      <c r="AD14" s="704"/>
     </row>
     <row r="15" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C15" s="130" t="s">
@@ -13644,20 +13690,20 @@
       <c r="F15" s="66" t="s">
         <v>94</v>
       </c>
-      <c r="G15" s="698"/>
+      <c r="G15" s="731"/>
       <c r="H15" s="2" t="s">
         <v>81</v>
       </c>
       <c r="I15" s="53" t="s">
         <v>81</v>
       </c>
-      <c r="K15" s="716"/>
-      <c r="L15" s="733"/>
-      <c r="Q15" s="700" t="s">
+      <c r="K15" s="710"/>
+      <c r="L15" s="727"/>
+      <c r="Q15" s="733" t="s">
         <v>211</v>
       </c>
-      <c r="R15" s="626"/>
-      <c r="S15" s="559"/>
+      <c r="R15" s="630"/>
+      <c r="S15" s="560"/>
       <c r="T15" s="6"/>
       <c r="V15" s="68" t="s">
         <v>44</v>
@@ -13665,14 +13711,14 @@
       <c r="X15" s="2" t="s">
         <v>128</v>
       </c>
-      <c r="AA15" s="722"/>
-      <c r="AB15" s="723"/>
-      <c r="AD15" s="710"/>
+      <c r="AA15" s="716"/>
+      <c r="AB15" s="717"/>
+      <c r="AD15" s="704"/>
     </row>
     <row r="16" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C16" s="132"/>
-      <c r="G16" s="698"/>
-      <c r="K16" s="716"/>
+      <c r="G16" s="731"/>
+      <c r="K16" s="710"/>
       <c r="N16" s="47"/>
       <c r="O16" s="61" t="s">
         <v>109</v>
@@ -13680,7 +13726,7 @@
       <c r="R16" s="114" t="s">
         <v>44</v>
       </c>
-      <c r="S16" s="559"/>
+      <c r="S16" s="560"/>
       <c r="T16" s="76" t="s">
         <v>129</v>
       </c>
@@ -13691,34 +13737,34 @@
       <c r="Z16" s="76" t="s">
         <v>127</v>
       </c>
-      <c r="AA16" s="722"/>
-      <c r="AB16" s="723"/>
-      <c r="AD16" s="710"/>
+      <c r="AA16" s="716"/>
+      <c r="AB16" s="717"/>
+      <c r="AD16" s="704"/>
     </row>
     <row r="17" spans="3:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C17" s="109"/>
       <c r="E17" s="6" t="s">
         <v>95</v>
       </c>
-      <c r="F17" s="695" t="s">
+      <c r="F17" s="728" t="s">
         <v>96</v>
       </c>
-      <c r="G17" s="698"/>
+      <c r="G17" s="731"/>
       <c r="H17" s="54"/>
       <c r="I17" s="133" t="s">
         <v>81</v>
       </c>
-      <c r="K17" s="716"/>
-      <c r="S17" s="559"/>
+      <c r="K17" s="710"/>
+      <c r="S17" s="560"/>
       <c r="V17" s="68" t="s">
         <v>44</v>
       </c>
       <c r="X17" s="2" t="s">
         <v>118</v>
       </c>
-      <c r="AA17" s="722"/>
-      <c r="AB17" s="723"/>
-      <c r="AD17" s="710"/>
+      <c r="AA17" s="716"/>
+      <c r="AB17" s="717"/>
+      <c r="AD17" s="704"/>
     </row>
     <row r="18" spans="3:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C18" s="130"/>
@@ -13728,58 +13774,61 @@
       <c r="E18" s="6" t="s">
         <v>97</v>
       </c>
-      <c r="F18" s="696"/>
-      <c r="G18" s="698"/>
+      <c r="F18" s="729"/>
+      <c r="G18" s="731"/>
       <c r="H18" s="108" t="s">
         <v>76</v>
       </c>
       <c r="I18" s="21" t="s">
         <v>81</v>
       </c>
-      <c r="K18" s="716"/>
+      <c r="K18" s="710"/>
       <c r="O18" s="64" t="s">
         <v>115</v>
       </c>
-      <c r="S18" s="559"/>
+      <c r="S18" s="560"/>
       <c r="U18" s="76" t="s">
         <v>133</v>
       </c>
       <c r="X18" s="2" t="s">
         <v>117</v>
       </c>
-      <c r="AA18" s="724"/>
-      <c r="AB18" s="725"/>
-      <c r="AD18" s="710"/>
+      <c r="AA18" s="718"/>
+      <c r="AB18" s="719"/>
+      <c r="AD18" s="704"/>
     </row>
     <row r="19" spans="3:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="F19" s="64" t="s">
         <v>209</v>
       </c>
-      <c r="G19" s="699"/>
-      <c r="K19" s="717"/>
+      <c r="G19" s="732"/>
+      <c r="K19" s="711"/>
       <c r="Q19" s="68" t="s">
         <v>44</v>
       </c>
-      <c r="R19" s="704" t="s">
+      <c r="R19" s="737" t="s">
         <v>124</v>
       </c>
-      <c r="S19" s="705"/>
-      <c r="T19" s="706"/>
+      <c r="S19" s="738"/>
+      <c r="T19" s="739"/>
       <c r="V19" s="77" t="s">
         <v>115</v>
       </c>
       <c r="Y19" s="19" t="s">
         <v>125</v>
       </c>
-      <c r="AD19" s="711"/>
+      <c r="AD19" s="705"/>
     </row>
   </sheetData>
   <mergeCells count="24">
-    <mergeCell ref="C9:C11"/>
-    <mergeCell ref="C13:C14"/>
-    <mergeCell ref="V2:W2"/>
-    <mergeCell ref="M10:AC10"/>
-    <mergeCell ref="F2:F3"/>
+    <mergeCell ref="F17:F18"/>
+    <mergeCell ref="G2:G19"/>
+    <mergeCell ref="Q13:R13"/>
+    <mergeCell ref="Q15:R15"/>
+    <mergeCell ref="L9:N9"/>
+    <mergeCell ref="R19:T19"/>
+    <mergeCell ref="S12:S18"/>
+    <mergeCell ref="O3:O9"/>
     <mergeCell ref="AD1:AD19"/>
     <mergeCell ref="S8:AC8"/>
     <mergeCell ref="K5:K19"/>
@@ -13791,14 +13840,11 @@
     <mergeCell ref="P3:Q3"/>
     <mergeCell ref="L4:L8"/>
     <mergeCell ref="L12:L15"/>
-    <mergeCell ref="F17:F18"/>
-    <mergeCell ref="G2:G19"/>
-    <mergeCell ref="Q13:R13"/>
-    <mergeCell ref="Q15:R15"/>
-    <mergeCell ref="L9:N9"/>
-    <mergeCell ref="R19:T19"/>
-    <mergeCell ref="S12:S18"/>
-    <mergeCell ref="O3:O9"/>
+    <mergeCell ref="C9:C11"/>
+    <mergeCell ref="C13:C14"/>
+    <mergeCell ref="V2:W2"/>
+    <mergeCell ref="M10:AC10"/>
+    <mergeCell ref="F2:F3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>